<commit_message>
got way to add dynamic strings to excel file, implementing exportAgreement doc creation
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -5,139 +5,35 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\iCloud\ТАМОЖНЯ\2023\ВЛД2023\07_Фрио Севастополис\Реализация\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B27C24-CDCC-4B01-885C-B1F18C09C6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7E6D34-7D75-4075-8AD3-CBDEEBA491F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2152" yWindow="1950" windowWidth="20161" windowHeight="13380" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
-    <sheet name="146 доп" sheetId="2" r:id="rId1"/>
+    <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
     <sheet name="32" sheetId="1" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="Agr_No_EXP" localSheetId="1">'[1]Доп Экспорт'!$D$2</definedName>
-    <definedName name="Agr_No_EXP">'146 доп'!$D$2</definedName>
-    <definedName name="BL_Key" localSheetId="1">[1]BL!$J$14</definedName>
-    <definedName name="BL_Key">[2]BL!$J$14</definedName>
-    <definedName name="BL_List" localSheetId="1">[1]Сертификаты!$Q$1</definedName>
-    <definedName name="BL_List">[2]Сертификаты!$Q$1</definedName>
-    <definedName name="Dop_EXP" localSheetId="1">[1]Экспорт!$U$27</definedName>
-    <definedName name="Dop_EXP">[2]Экспорт!$U$27</definedName>
-    <definedName name="ID_AGR_STR" localSheetId="1">'[1]Договор Хранение'!$N$8</definedName>
-    <definedName name="ID_AGR_STR">'[2]Договор Хранение'!$N$8</definedName>
-    <definedName name="ID_EKSPORT" localSheetId="1">'[1]Доп Экспорт'!#REF!</definedName>
-    <definedName name="ID_EKSPORT">'146 доп'!#REF!</definedName>
-    <definedName name="ID_Эксп_ДОП" localSheetId="1">'[1]Доп Экспорт'!$U$17</definedName>
-    <definedName name="ID_Эксп_ДОП">'146 доп'!$U$17</definedName>
-    <definedName name="Konosament_EXP" localSheetId="1">[1]Экспорт!$B$28</definedName>
-    <definedName name="Konosament_EXP">[2]Экспорт!$B$28</definedName>
-    <definedName name="logo" localSheetId="0">INDEX([2]Б!$A$1:$A$2,MATCH(Порт_Компания,[2]Б!$B$1:$B$2,0))</definedName>
-    <definedName name="logo" localSheetId="1">INDEX([1]Б!$A$1:$A$2,MATCH('32'!Порт_Компания,[1]Б!$B$1:$B$2,0))</definedName>
-    <definedName name="logo">INDEX([2]Б!$A$1:$A$2,MATCH(Порт_Компания,[2]Б!$B$1:$B$2,0))</definedName>
-    <definedName name="nonComNo" localSheetId="1">[1]InvoiceNonCom!$O$4</definedName>
-    <definedName name="nonComNo">[2]InvoiceNonCom!$O$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'146 доп'!$A$1:$B$48</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'32'!$A$1:$G$85</definedName>
-    <definedName name="Product_VR" localSheetId="1">'[1]Внутренний рынок'!$P$2</definedName>
-    <definedName name="Product_VR">'[2]Внутренний рынок'!$P$2</definedName>
-    <definedName name="Product_VR_Spisok" localSheetId="1">'[1]Внутренний рынок'!$B$1</definedName>
-    <definedName name="Product_VR_Spisok">'[2]Внутренний рынок'!$B$1</definedName>
-    <definedName name="Svod_EXP" localSheetId="1">[1]Экспорт!$O$28</definedName>
-    <definedName name="Svod_EXP">[2]Экспорт!$O$28</definedName>
-    <definedName name="Vessel_EXP" localSheetId="1">[1]Экспорт!$AC$1</definedName>
-    <definedName name="Vessel_EXP">[2]Экспорт!$AC$1</definedName>
-    <definedName name="Vessel_VR" localSheetId="1">'[1]Внутренний рынок'!$N$2</definedName>
-    <definedName name="Vessel_VR">'[2]Внутренний рынок'!$N$2</definedName>
-    <definedName name="Vessel_VV" localSheetId="1">'[1]Внутренний рынок'!$A$1</definedName>
-    <definedName name="Vessel_VV">'[2]Внутренний рынок'!$A$1</definedName>
-    <definedName name="ВМРП" localSheetId="1">#REF!</definedName>
-    <definedName name="ВМРП">#REF!</definedName>
-    <definedName name="ДалькомХолод" localSheetId="1">#REF!</definedName>
-    <definedName name="ДалькомХолод">#REF!</definedName>
-    <definedName name="ДВ_Порт" localSheetId="1">#REF!</definedName>
-    <definedName name="ДВ_Порт">#REF!</definedName>
-    <definedName name="ДоговорНомер" localSheetId="1">'[1]Заявки на договора'!$L$3</definedName>
-    <definedName name="ДоговорНомер">'[2]Заявки на договора'!$L$3</definedName>
-    <definedName name="Допы_Хранение" localSheetId="1">'[1]Договор Хранение'!$R$1</definedName>
-    <definedName name="Допы_Хранение">'[2]Договор Хранение'!$R$1</definedName>
-    <definedName name="Заявка" localSheetId="1">'[1]Заявки на договора'!$J$1</definedName>
-    <definedName name="Заявка">'[2]Заявки на договора'!$J$1</definedName>
-    <definedName name="Заявка_Изготовитель" localSheetId="1">'[1]Заявки на договора'!$B$9</definedName>
-    <definedName name="Заявка_Изготовитель">'[2]Заявки на договора'!$B$9</definedName>
-    <definedName name="Заявка_наименование" localSheetId="1">'[1]Заявки на договора'!$C$9</definedName>
-    <definedName name="Заявка_наименование">'[2]Заявки на договора'!$C$9</definedName>
-    <definedName name="Заявка_Сорт" localSheetId="1">'[1]Заявки на договора'!$D$9</definedName>
-    <definedName name="Заявка_Сорт">'[2]Заявки на договора'!$D$9</definedName>
-    <definedName name="Заявка_Упаковка" localSheetId="1">'[1]Заявки на договора'!$E$9</definedName>
-    <definedName name="Заявка_Упаковка">'[2]Заявки на договора'!$E$9</definedName>
-    <definedName name="Инвойс_Заявка" localSheetId="1">[1]InvoiceNonCom!$V$3</definedName>
-    <definedName name="Инвойс_Заявка">[2]InvoiceNonCom!$V$3</definedName>
-    <definedName name="Клиенты" localSheetId="1">#REF!</definedName>
-    <definedName name="Клиенты">#REF!</definedName>
-    <definedName name="КОЛ_ВО_ЭКС" localSheetId="1">'[1]Доп Экспорт'!$R$17</definedName>
-    <definedName name="КОЛ_ВО_ЭКС">'146 доп'!$R$17</definedName>
-    <definedName name="Коносамент_ВР" localSheetId="1">'[1]Внутренний рынок'!$M$2</definedName>
-    <definedName name="Коносамент_ВР">'[2]Внутренний рынок'!$M$2</definedName>
-    <definedName name="Краткое_наименование" localSheetId="1">#REF!</definedName>
-    <definedName name="Краткое_наименование">#REF!</definedName>
-    <definedName name="Полное_наименование" localSheetId="1">#REF!</definedName>
-    <definedName name="Полное_наименование">#REF!</definedName>
-    <definedName name="Порт_Договор" localSheetId="1">'[1]Письмо в порт'!$H$17</definedName>
-    <definedName name="Порт_Договор">'[2]Письмо в порт'!$H$17</definedName>
-    <definedName name="Порт_Договор_Фильтр" localSheetId="1">'[1]Письмо в порт'!$H$9</definedName>
-    <definedName name="Порт_Договор_Фильтр">'[2]Письмо в порт'!$H$9</definedName>
-    <definedName name="Порт_Компания" localSheetId="1">'[1]Письмо в порт'!$H$10</definedName>
-    <definedName name="Порт_Компания">'[2]Письмо в порт'!$H$10</definedName>
-    <definedName name="Порт_Магадан">[2]!SPTamozhnya[Порт]</definedName>
-    <definedName name="Прод_тест" localSheetId="1">[1]Коносаменты!#REF!</definedName>
-    <definedName name="Прод_тест">[2]Коносаменты!#REF!</definedName>
-    <definedName name="ПРОД_ЭКС" localSheetId="1">'[1]Доп Экспорт'!$P$17</definedName>
-    <definedName name="ПРОД_ЭКС">'146 доп'!$P$17</definedName>
-    <definedName name="ПРОД_ЭКС_1" localSheetId="1">'[1]Доп Экспорт'!$O$17</definedName>
-    <definedName name="ПРОД_ЭКС_1">'146 доп'!$O$17</definedName>
-    <definedName name="ПРОД_ЭКС_2">'146 доп'!$P$17</definedName>
-    <definedName name="ПРОД_ЭКС2">'146 доп'!$P$17</definedName>
-    <definedName name="Рейс_ЭХ" localSheetId="1">'[1]Экспорт Хранение'!$A$29</definedName>
-    <definedName name="Рейс_ЭХ">'[2]Экспорт Хранение'!$A$29</definedName>
-    <definedName name="СОРТ_ЭКСП" localSheetId="1">'[1]Доп Экспорт'!$Q$17</definedName>
-    <definedName name="СОРТ_ЭКСП">'146 доп'!$Q$17</definedName>
-    <definedName name="СУММ_ЭКСП" localSheetId="1">'[1]Доп Экспорт'!$T$17:$T$18</definedName>
-    <definedName name="СУММ_ЭКСП">'146 доп'!$T$17:$T$18</definedName>
-    <definedName name="Сумма_Тов">'146 доп'!$T$17</definedName>
-    <definedName name="Телефон" localSheetId="1">#REF!</definedName>
-    <definedName name="Телефон">#REF!</definedName>
-    <definedName name="ТОВ_1" localSheetId="1">'[1]Доп Экспорт'!$N$17</definedName>
-    <definedName name="ТОВ_1">'146 доп'!$N$17</definedName>
-    <definedName name="ХР_BL" localSheetId="1">[1]InvoiceNonCom!$P$14</definedName>
-    <definedName name="ХР_BL">[2]InvoiceNonCom!$P$14</definedName>
-    <definedName name="ХР_ID" localSheetId="1">[1]InvoiceNonCom!$Y$14</definedName>
-    <definedName name="ХР_ID">[2]InvoiceNonCom!$Y$14</definedName>
-    <definedName name="ХР_Product" localSheetId="1">[1]InvoiceNonCom!$R$14</definedName>
-    <definedName name="ХР_Product">[2]InvoiceNonCom!$R$14</definedName>
-    <definedName name="ХР_Колво" localSheetId="1">[1]InvoiceNonCom!$T$14</definedName>
-    <definedName name="ХР_Колво">[2]InvoiceNonCom!$T$14</definedName>
-    <definedName name="ХР_Объем" localSheetId="1">[1]InvoiceNonCom!$U$14</definedName>
-    <definedName name="ХР_Объем">[2]InvoiceNonCom!$U$14</definedName>
-    <definedName name="ХР_Продукция" localSheetId="1">[1]InvoiceNonCom!$Q$14</definedName>
-    <definedName name="ХР_Продукция">[2]InvoiceNonCom!$Q$14</definedName>
-    <definedName name="ХР_Сумма" localSheetId="1">[1]InvoiceNonCom!$X$14</definedName>
-    <definedName name="ХР_Сумма">[2]InvoiceNonCom!$X$14</definedName>
-    <definedName name="ХР_Упаковка" localSheetId="1">[1]InvoiceNonCom!$S$14</definedName>
-    <definedName name="ХР_Упаковка">[2]InvoiceNonCom!$S$14</definedName>
-    <definedName name="ХР_Цена" localSheetId="1">[1]InvoiceNonCom!$W$14</definedName>
-    <definedName name="ХР_Цена">[2]InvoiceNonCom!$W$14</definedName>
-    <definedName name="Хранение_продукция" localSheetId="1">'[1]Экспорт Хранение'!$AH$1</definedName>
-    <definedName name="Хранение_продукция">'[2]Экспорт Хранение'!$AH$1</definedName>
-    <definedName name="Хранение_Суда" localSheetId="1">'[1]Экспорт Хранение'!$AG$1</definedName>
-    <definedName name="Хранение_Суда">'[2]Экспорт Хранение'!$AG$1</definedName>
-    <definedName name="ЦЕНА_ЭКСП" localSheetId="1">'[1]Доп Экспорт'!$S$17</definedName>
-    <definedName name="ЦЕНА_ЭКСП">'146 доп'!$S$17</definedName>
+    <definedName name="Контракт">Export_Contract!$A$2</definedName>
+    <definedName name="Контракт_дата">Export_Contract!$A$3</definedName>
+    <definedName name="Покупатель">Export_Contract!$A$11</definedName>
+    <definedName name="Покупатель_адрес">Export_Contract!$A$12</definedName>
+    <definedName name="Покупатель_заголовок">Export_Contract!$A$10</definedName>
+    <definedName name="Покупатель_представитель">Export_Contract!$A$13</definedName>
+    <definedName name="Покупатель_представитель_подробно">Export_Contract!$A$14</definedName>
+    <definedName name="Предмет_заголовок">Export_Contract!$A$15</definedName>
+    <definedName name="Предмет_массив">Export_Contract!$A$17</definedName>
+    <definedName name="Предмет_описание">Export_Contract!$A$16</definedName>
+    <definedName name="Продавец">Export_Contract!$A$6</definedName>
+    <definedName name="Продавец_адрес">Export_Contract!$A$7</definedName>
+    <definedName name="Продавец_заголовок">Export_Contract!$A$5</definedName>
+    <definedName name="Продавец_подписант">Export_Contract!$A$9</definedName>
+    <definedName name="Продавец_представитель">Export_Contract!$A$8</definedName>
+    <definedName name="Соглашение">Export_Contract!$A$1</definedName>
+    <definedName name="Стороны_заголовок">Export_Contract!$A$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -160,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="165">
   <si>
     <t>COMMERCIAL INVOICE</t>
   </si>
@@ -462,9 +358,6 @@
     <t>в пользу  ООО "Тихоокеанская рыбопромышленная компания"</t>
   </si>
   <si>
-    <t>AGREEMENT No. 146 dated March 10, 2023</t>
-  </si>
-  <si>
     <t>ДОПОЛНЕНИЕ № 146 от 10 марта 2023г.</t>
   </si>
   <si>
@@ -477,9 +370,6 @@
     <t>278-145</t>
   </si>
   <si>
-    <t>Magadan, dated July 10, 2019</t>
-  </si>
-  <si>
     <t>Магадан от 10 июля 2019г.</t>
   </si>
   <si>
@@ -501,15 +391,9 @@
     <t xml:space="preserve">Продавец:  </t>
   </si>
   <si>
-    <t>Represented by Deputy General Director </t>
-  </si>
-  <si>
     <t xml:space="preserve">В лице и.о. генерального директора </t>
   </si>
   <si>
-    <t>N.M. Kotov and</t>
-  </si>
-  <si>
     <t>Котова Н.М. и</t>
   </si>
   <si>
@@ -519,9 +403,6 @@
     <t>Покупатель:</t>
   </si>
   <si>
-    <t>Represented by president SE JI YOUNG</t>
-  </si>
-  <si>
     <t>в лице президента SE JI YOUNG</t>
   </si>
   <si>
@@ -537,13 +418,7 @@
     <t>1. Предмет Дополнения</t>
   </si>
   <si>
-    <t>1.1. Seller is obliged to deliver the commodity, and   Buyer  is obligated to receive and pay lot of the cargo,  produced by f/v "Morskoy Volk":</t>
-  </si>
-  <si>
     <t>1.1. Продавец обязуется поставить Покупателю, а Покупатель обязуется принять и оплатить партию продукции, изготовленную на МФТ "Морской Волк":</t>
-  </si>
-  <si>
-    <t>* MSC Frozen Alaska Pollock Milts  - 9,585 tn (net weight)</t>
   </si>
   <si>
     <t>* MSC Молоки минтая мороженые  - 9,585 тн (нетто)</t>
@@ -679,6 +554,9 @@
   <si>
     <t>2.2. Total amount of this Agreement is 
 USD 33 547,50 (Thirty three thousand five hundred forty eight US Dollars 50 Cents)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1150,6 +1028,27 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1161,6 +1060,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1170,12 +1108,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1200,65 +1132,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1275,533 +1153,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="SP_Consignee (2)"/>
-      <sheetName val="Коносаменты"/>
-      <sheetName val="№рейса_справочник"/>
-      <sheetName val="Образцы"/>
-      <sheetName val="Транспорта"/>
-      <sheetName val="Внутренний рынок"/>
-      <sheetName val="Заявки на договора"/>
-      <sheetName val="Письмо в порт"/>
-      <sheetName val="Экспорт"/>
-      <sheetName val="Сертификаты"/>
-      <sheetName val="Доп Экспорт"/>
-      <sheetName val="Инвойс Экспорт"/>
-      <sheetName val="SP_Consignee"/>
-      <sheetName val="BL"/>
-      <sheetName val="Экспорт Хранение"/>
-      <sheetName val="Договор Хранение"/>
-      <sheetName val="InvoiceNonCom"/>
-      <sheetName val="SPContract"/>
-      <sheetName val="SPAgent"/>
-      <sheetName val="SPBankProdavec"/>
-      <sheetName val="SPPortZarubezh"/>
-      <sheetName val="SPRekvizitBankProdavec"/>
-      <sheetName val="SPTamozhnya"/>
-      <sheetName val="SPPodpisant"/>
-      <sheetName val="SPPort"/>
-      <sheetName val="SPClientsSell"/>
-      <sheetName val="Б"/>
-      <sheetName val="Суда"/>
-      <sheetName val="Продавец"/>
-      <sheetName val="Вид операции"/>
-      <sheetName val="Продукция"/>
-      <sheetName val="e00eb4de3c8a421cba9b8f4cb8546ec"/>
-      <sheetName val="Движение продукции"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v/>
-          </cell>
-          <cell r="B1" t="str">
-            <v/>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="M2" t="str">
-            <v/>
-          </cell>
-          <cell r="N2" t="str">
-            <v/>
-          </cell>
-          <cell r="P2" t="str">
-            <v/>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="1">
-          <cell r="J1">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="L3">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="C9" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="D9" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="E9" t="e">
-            <v>#VALUE!</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="9">
-          <cell r="H9">
-            <v>360</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="H10" t="str">
-            <v/>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="H17">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8">
-        <row r="1">
-          <cell r="AC1" t="str">
-            <v>СРТМ "Си Хантер"</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="U27">
-            <v>144</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28" t="str">
-            <v>07_Фрио Севастополис.</v>
-          </cell>
-          <cell r="O28" t="str">
-            <v>СРТМ "Си Хантер"</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9">
-        <row r="1">
-          <cell r="Q1" t="str">
-            <v>FRSH-30T</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10">
-        <row r="2">
-          <cell r="D2" t="str">
-            <v>278-147</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="N17" t="str">
-            <v>Молоки минтая</v>
-          </cell>
-          <cell r="O17" t="str">
-            <v>MSC Молоки минтая мороженые</v>
-          </cell>
-          <cell r="P17" t="str">
-            <v>MSC Frozen Alaska Pollock Milts</v>
-          </cell>
-          <cell r="Q17" t="str">
-            <v/>
-          </cell>
-          <cell r="R17">
-            <v>22.364999999999998</v>
-          </cell>
-          <cell r="S17">
-            <v>3500</v>
-          </cell>
-          <cell r="T17">
-            <v>78277.5</v>
-          </cell>
-          <cell r="U17" t="str">
-            <v>Молоки минтая-</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13">
-        <row r="14">
-          <cell r="J14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="14">
-        <row r="1">
-          <cell r="AG1" t="str">
-            <v>СРТМ "Си Хантер"</v>
-          </cell>
-          <cell r="AH1" t="str">
-            <v xml:space="preserve">Икра Минтая </v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>07_Фрио Севастополис.</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="15">
-        <row r="1">
-          <cell r="R1" t="str">
-            <v>12-28</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="N8" t="str">
-            <v>MSCИкра Минтая СРТМ "Си Хантер"
-f/v "Sea Hunter"KTI</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="16">
-        <row r="3">
-          <cell r="V3">
-            <v>27</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="O4">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="P14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="Q14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="R14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="S14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="T14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="U14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="W14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="X14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="Y14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>ТРК</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>МСИ</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="SP_Consignee (2)"/>
-      <sheetName val="Коносаменты"/>
-      <sheetName val="№рейса_справочник"/>
-      <sheetName val="Образцы"/>
-      <sheetName val="Транспорта"/>
-      <sheetName val="Внутренний рынок"/>
-      <sheetName val="Заявки на договора"/>
-      <sheetName val="Письмо в порт"/>
-      <sheetName val="Экспорт"/>
-      <sheetName val="Сертификаты"/>
-      <sheetName val="Доп Экспорт"/>
-      <sheetName val="Инвойс Экспорт"/>
-      <sheetName val="SP_Consignee"/>
-      <sheetName val="BL"/>
-      <sheetName val="Экспорт Хранение"/>
-      <sheetName val="Договор Хранение"/>
-      <sheetName val="InvoiceNonCom"/>
-      <sheetName val="SPContract"/>
-      <sheetName val="SPAgent"/>
-      <sheetName val="SPBankProdavec"/>
-      <sheetName val="SPPortZarubezh"/>
-      <sheetName val="SPRekvizitBankProdavec"/>
-      <sheetName val="SPTamozhnya"/>
-      <sheetName val="SPPodpisant"/>
-      <sheetName val="SPPort"/>
-      <sheetName val="SPClientsSell"/>
-      <sheetName val="Б"/>
-      <sheetName val="Суда"/>
-      <sheetName val="Продавец"/>
-      <sheetName val="Вид операции"/>
-      <sheetName val="Продукция"/>
-      <sheetName val="e00eb4de3c8a421cba9b8f4cb8546ec"/>
-      <sheetName val="Движение продукции"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v/>
-          </cell>
-          <cell r="B1" t="str">
-            <v/>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="M2" t="str">
-            <v/>
-          </cell>
-          <cell r="N2" t="str">
-            <v/>
-          </cell>
-          <cell r="P2" t="str">
-            <v/>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="1">
-          <cell r="J1">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="L3">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="C9" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="D9" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="E9" t="e">
-            <v>#VALUE!</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="9">
-          <cell r="H9">
-            <v>360</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="H10" t="str">
-            <v/>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="H17">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8">
-        <row r="1">
-          <cell r="AC1" t="str">
-            <v>СРТМ "Си Хантер"</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="U27">
-            <v>144</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28" t="str">
-            <v>07_Фрио Севастополис.</v>
-          </cell>
-          <cell r="O28" t="str">
-            <v>СРТМ "Си Хантер"</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9">
-        <row r="1">
-          <cell r="Q1" t="str">
-            <v>FRSH-30T</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13">
-        <row r="14">
-          <cell r="J14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="14">
-        <row r="1">
-          <cell r="AG1" t="str">
-            <v>СРТМ "Си Хантер"</v>
-          </cell>
-          <cell r="AH1" t="str">
-            <v xml:space="preserve">Икра Минтая </v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>07_Фрио Севастополис.</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="15">
-        <row r="1">
-          <cell r="R1" t="str">
-            <v>12-28</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="N8" t="str">
-            <v>MSCИкра Минтая СРТМ "Си Хантер"
-f/v "Sea Hunter"KTI</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="16">
-        <row r="3">
-          <cell r="V3">
-            <v>27</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="O4">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="P14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="Q14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="R14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="S14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="T14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="U14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="W14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="X14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-          <cell r="Y14" t="e">
-            <v>#VALUE!</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>ТРК</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>МСИ</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2106,8 +1457,8 @@
   </sheetPr>
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A29" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="151" zoomScaleNormal="100" zoomScaleSheetLayoutView="151" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2130,63 +1481,63 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>101</v>
       </c>
       <c r="D1" s="3"/>
       <c r="N1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="47" t="s">
-        <v>25</v>
+        <v>164</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="3"/>
       <c r="N2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="47" t="s">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H3" s="49"/>
       <c r="N3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="N4" t="s">
         <v>108</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="N4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="51" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>6</v>
+        <v>164</v>
       </c>
       <c r="B6" s="53" t="s">
         <v>64</v>
@@ -2194,7 +1545,7 @@
     </row>
     <row r="7" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>164</v>
       </c>
       <c r="B7" s="50" t="s">
         <v>66</v>
@@ -2202,31 +1553,31 @@
     </row>
     <row r="8" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>113</v>
+        <v>164</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="51" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
-        <v>13</v>
+        <v>164</v>
       </c>
       <c r="B11" s="53" t="s">
         <v>13</v>
@@ -2234,7 +1585,7 @@
     </row>
     <row r="12" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
-        <v>15</v>
+        <v>164</v>
       </c>
       <c r="B12" s="50" t="s">
         <v>15</v>
@@ -2242,49 +1593,49 @@
     </row>
     <row r="13" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="54" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B15" s="55" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="B17" s="56" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="M17" s="57"/>
       <c r="N17" t="s">
         <v>38</v>
       </c>
       <c r="O17" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="P17" t="s">
         <v>39</v>
@@ -2302,111 +1653,111 @@
         <v>33547.5</v>
       </c>
       <c r="U17" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="54" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B18" s="55" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="26.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="26.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B20" s="56" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="45.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="59" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B22" s="60" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="41.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="61" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B25" s="61" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="56.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="54" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B27" s="55" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="54" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B29" s="55" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B30" s="53" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -2427,10 +1778,10 @@
     </row>
     <row r="33" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -2454,23 +1805,23 @@
         <v>59</v>
       </c>
       <c r="B36" s="50" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B38" s="50" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -2491,58 +1842,58 @@
     </row>
     <row r="41" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B41" s="50" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B45" s="50" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="19" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B46" s="62" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="63" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B47" s="63" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2580,8 +1931,8 @@
   </sheetPr>
   <dimension ref="A1:Z85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A57" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView view="pageBreakPreview" zoomScale="160" zoomScaleNormal="70" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2603,26 +1954,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="99" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="100"/>
+      <c r="E2" s="70"/>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2637,15 +1988,15 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="64" t="s">
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="65"/>
+      <c r="E3" s="72"/>
       <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
@@ -2660,13 +2011,13 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="72"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2674,46 +2025,46 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="86" t="s">
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="88"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="78"/>
       <c r="Q5">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="81" t="s">
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="83"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="79"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="81" t="s">
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="83"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="79"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2723,12 +2074,12 @@
         <v>18</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="86" t="s">
+      <c r="D8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="88"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="78"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
@@ -2738,12 +2089,12 @@
         <v>21</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="89" t="s">
+      <c r="D9" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="91"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="84"/>
     </row>
     <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
@@ -2753,50 +2104,50 @@
         <v>24</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="81" t="s">
+      <c r="D10" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="83"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="79"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="18"/>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="92"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="75"/>
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="20"/>
-      <c r="D12" s="86" t="s">
+      <c r="D12" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="88"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="66" t="s">
+      <c r="D13" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="92"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="75"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="24" t="s">
@@ -2808,10 +2159,10 @@
       <c r="C14" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="93" t="s">
+      <c r="D14" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="93"/>
+      <c r="E14" s="87"/>
       <c r="F14" s="25" t="s">
         <v>35</v>
       </c>
@@ -3053,37 +2404,37 @@
       <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="68" t="s">
+      <c r="A33" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="70"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="90"/>
     </row>
     <row r="34" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="68" t="s">
+      <c r="A34" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="70"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="89"/>
+      <c r="F34" s="89"/>
+      <c r="G34" s="90"/>
     </row>
     <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="71" t="s">
+      <c r="A35" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="73"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="67"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="91"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="33"/>
@@ -3102,62 +2453,62 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="74" t="s">
+      <c r="A37" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="93"/>
+      <c r="D37" s="93"/>
+      <c r="E37" s="93"/>
       <c r="F37" s="36"/>
       <c r="G37" s="15"/>
     </row>
     <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="76" t="s">
+      <c r="A38" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="78" t="s">
+      <c r="B38" s="95"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="79"/>
-      <c r="F38" s="79"/>
-      <c r="G38" s="80"/>
+      <c r="E38" s="97"/>
+      <c r="F38" s="97"/>
+      <c r="G38" s="98"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="64" t="s">
+      <c r="A39" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="65"/>
-      <c r="C39" s="65"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="72"/>
       <c r="D39" s="8"/>
       <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="64" t="s">
+      <c r="A40" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="72"/>
       <c r="D40" s="8"/>
       <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="64" t="s">
+      <c r="A41" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="65"/>
-      <c r="C41" s="65"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="72"/>
       <c r="D41" s="8"/>
       <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="67"/>
-      <c r="C42" s="67"/>
+      <c r="B42" s="74"/>
+      <c r="C42" s="74"/>
       <c r="D42" s="21"/>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
@@ -3165,26 +2516,26 @@
     </row>
     <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="44" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A44" s="98" t="s">
+      <c r="A44" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="98"/>
-      <c r="C44" s="98"/>
-      <c r="D44" s="98"/>
-      <c r="E44" s="98"/>
-      <c r="F44" s="98"/>
-      <c r="G44" s="98"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="68"/>
     </row>
     <row r="45" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="96" t="s">
+      <c r="A45" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="97"/>
-      <c r="C45" s="97"/>
-      <c r="D45" s="96" t="s">
+      <c r="B45" s="86"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="97"/>
+      <c r="E45" s="86"/>
       <c r="F45" s="1" t="s">
         <v>3</v>
       </c>
@@ -3193,15 +2544,15 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="81" t="s">
+      <c r="A46" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="82"/>
-      <c r="C46" s="82"/>
-      <c r="D46" s="64" t="s">
+      <c r="B46" s="65"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="65"/>
+      <c r="E46" s="72"/>
       <c r="F46" s="6" t="s">
         <v>8</v>
       </c>
@@ -3210,54 +2561,54 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="92"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="72"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="67"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A48" s="94" t="s">
+      <c r="A48" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="95"/>
-      <c r="C48" s="95"/>
-      <c r="D48" s="86" t="s">
+      <c r="B48" s="100"/>
+      <c r="C48" s="100"/>
+      <c r="D48" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="87"/>
-      <c r="F48" s="87"/>
-      <c r="G48" s="88"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="77"/>
+      <c r="G48" s="78"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A49" s="64" t="s">
+      <c r="A49" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="65"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="81" t="s">
+      <c r="B49" s="72"/>
+      <c r="C49" s="72"/>
+      <c r="D49" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="82"/>
-      <c r="F49" s="82"/>
-      <c r="G49" s="83"/>
+      <c r="E49" s="65"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="79"/>
     </row>
     <row r="50" spans="1:16" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="84" t="s">
+      <c r="A50" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="85"/>
-      <c r="C50" s="85"/>
-      <c r="D50" s="81" t="s">
+      <c r="B50" s="81"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="82"/>
-      <c r="F50" s="82"/>
-      <c r="G50" s="83"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="65"/>
+      <c r="G50" s="79"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" s="38" t="s">
@@ -3267,12 +2618,12 @@
         <v>70</v>
       </c>
       <c r="C51" s="9"/>
-      <c r="D51" s="86" t="s">
+      <c r="D51" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="E51" s="87"/>
-      <c r="F51" s="87"/>
-      <c r="G51" s="88"/>
+      <c r="E51" s="77"/>
+      <c r="F51" s="77"/>
+      <c r="G51" s="78"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" s="12" t="s">
@@ -3282,12 +2633,12 @@
         <v>73</v>
       </c>
       <c r="C52" s="9"/>
-      <c r="D52" s="89" t="s">
+      <c r="D52" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="E52" s="90"/>
-      <c r="F52" s="90"/>
-      <c r="G52" s="91"/>
+      <c r="E52" s="83"/>
+      <c r="F52" s="83"/>
+      <c r="G52" s="84"/>
     </row>
     <row r="53" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="38" t="s">
@@ -3297,50 +2648,50 @@
         <v>76</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="D53" s="81" t="s">
+      <c r="D53" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="E53" s="82"/>
-      <c r="F53" s="82"/>
-      <c r="G53" s="83"/>
+      <c r="E53" s="65"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="79"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A54" s="16" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B54" s="17" t="s">
         <v>78</v>
       </c>
       <c r="C54" s="18"/>
-      <c r="D54" s="66" t="s">
+      <c r="D54" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="E54" s="67"/>
-      <c r="F54" s="67"/>
-      <c r="G54" s="92"/>
+      <c r="E54" s="74"/>
+      <c r="F54" s="74"/>
+      <c r="G54" s="75"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C55" s="20"/>
-      <c r="D55" s="86" t="s">
+      <c r="D55" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="E55" s="87"/>
-      <c r="F55" s="87"/>
-      <c r="G55" s="88"/>
+      <c r="E55" s="77"/>
+      <c r="F55" s="77"/>
+      <c r="G55" s="78"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A56" s="21"/>
       <c r="B56" s="22"/>
       <c r="C56" s="23"/>
-      <c r="D56" s="66" t="s">
+      <c r="D56" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="E56" s="67"/>
-      <c r="F56" s="67"/>
-      <c r="G56" s="92"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="74"/>
+      <c r="G56" s="75"/>
     </row>
     <row r="57" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="24" t="s">
@@ -3352,10 +2703,10 @@
       <c r="C57" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="D57" s="93" t="s">
+      <c r="D57" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="E57" s="93"/>
+      <c r="E57" s="87"/>
       <c r="F57" s="25" t="s">
         <v>85</v>
       </c>
@@ -3536,37 +2887,37 @@
       <c r="G75" s="15"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A76" s="68" t="s">
+      <c r="A76" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="B76" s="69"/>
-      <c r="C76" s="69"/>
-      <c r="D76" s="69"/>
-      <c r="E76" s="69"/>
-      <c r="F76" s="69"/>
-      <c r="G76" s="70"/>
+      <c r="B76" s="89"/>
+      <c r="C76" s="89"/>
+      <c r="D76" s="89"/>
+      <c r="E76" s="89"/>
+      <c r="F76" s="89"/>
+      <c r="G76" s="90"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A77" s="68" t="s">
+      <c r="A77" s="88" t="s">
         <v>93</v>
       </c>
-      <c r="B77" s="69"/>
-      <c r="C77" s="69"/>
-      <c r="D77" s="69"/>
-      <c r="E77" s="69"/>
-      <c r="F77" s="69"/>
-      <c r="G77" s="70"/>
+      <c r="B77" s="89"/>
+      <c r="C77" s="89"/>
+      <c r="D77" s="89"/>
+      <c r="E77" s="89"/>
+      <c r="F77" s="89"/>
+      <c r="G77" s="90"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A78" s="71" t="s">
+      <c r="A78" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B78" s="72"/>
-      <c r="C78" s="72"/>
-      <c r="D78" s="72"/>
-      <c r="E78" s="72"/>
-      <c r="F78" s="72"/>
-      <c r="G78" s="73"/>
+      <c r="B78" s="67"/>
+      <c r="C78" s="67"/>
+      <c r="D78" s="67"/>
+      <c r="E78" s="67"/>
+      <c r="F78" s="67"/>
+      <c r="G78" s="91"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" s="33"/>
@@ -3585,62 +2936,62 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A80" s="74" t="s">
+      <c r="A80" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="B80" s="75"/>
-      <c r="C80" s="75"/>
-      <c r="D80" s="75"/>
-      <c r="E80" s="75"/>
+      <c r="B80" s="93"/>
+      <c r="C80" s="93"/>
+      <c r="D80" s="93"/>
+      <c r="E80" s="93"/>
       <c r="F80" s="36"/>
       <c r="G80" s="15"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A81" s="76" t="s">
+      <c r="A81" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="B81" s="77"/>
-      <c r="C81" s="77"/>
-      <c r="D81" s="78" t="s">
+      <c r="B81" s="95"/>
+      <c r="C81" s="95"/>
+      <c r="D81" s="96" t="s">
         <v>98</v>
       </c>
-      <c r="E81" s="79"/>
-      <c r="F81" s="79"/>
-      <c r="G81" s="80"/>
+      <c r="E81" s="97"/>
+      <c r="F81" s="97"/>
+      <c r="G81" s="98"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A82" s="64" t="s">
+      <c r="A82" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="B82" s="65"/>
-      <c r="C82" s="65"/>
+      <c r="B82" s="72"/>
+      <c r="C82" s="72"/>
       <c r="D82" s="8"/>
       <c r="G82" s="9"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A83" s="64" t="s">
+      <c r="A83" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="B83" s="65"/>
-      <c r="C83" s="65"/>
+      <c r="B83" s="72"/>
+      <c r="C83" s="72"/>
       <c r="D83" s="8"/>
       <c r="G83" s="9"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A84" s="64" t="s">
+      <c r="A84" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B84" s="65"/>
-      <c r="C84" s="65"/>
+      <c r="B84" s="72"/>
+      <c r="C84" s="72"/>
       <c r="D84" s="8"/>
       <c r="G84" s="9"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A85" s="66" t="s">
+      <c r="A85" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="B85" s="67"/>
-      <c r="C85" s="67"/>
+      <c r="B85" s="74"/>
+      <c r="C85" s="74"/>
       <c r="D85" s="21"/>
       <c r="E85" s="22"/>
       <c r="F85" s="22"/>
@@ -3648,25 +2999,33 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="A83:C83"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A77:G77"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:G48"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="D14:E14"/>
@@ -3681,33 +3040,25 @@
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A77:G77"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3" xr:uid="{6D6CA36A-C765-4458-8A8E-A06DE7CFDD36}">

</xml_diff>

<commit_message>
initExcel logic store init separated
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7E6D34-7D75-4075-8AD3-CBDEEBA491F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D27FE3D-CC52-43AB-B9C4-003CE4731E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-14497" yWindow="16103" windowWidth="28994" windowHeight="15794" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="172">
   <si>
     <t>COMMERCIAL INVOICE</t>
   </si>
@@ -556,7 +556,28 @@
 USD 33 547,50 (Thirty three thousand five hundred forty eight US Dollars 50 Cents)</t>
   </si>
   <si>
-    <t>-</t>
+    <t>AGREEMENT No. 146 dated March 10, 2023</t>
+  </si>
+  <si>
+    <t>Magadan, dated July 10, 2019</t>
+  </si>
+  <si>
+    <t>Tikhrybcom Co., LTD</t>
+  </si>
+  <si>
+    <t>Represented by Deputy General Director </t>
+  </si>
+  <si>
+    <t>N.M. Kotov and</t>
+  </si>
+  <si>
+    <t>Represented by president SE JI YOUNG</t>
+  </si>
+  <si>
+    <t>1.1. Seller is obliged to deliver the commodity, and   Buyer  is obligated to receive and pay lot of the cargo,  produced by f/v "Morskoy Volk":</t>
+  </si>
+  <si>
+    <t>* MSC Frozen Alaska Pollock Milts  - 9,585 tn (net weight)</t>
   </si>
 </sst>
 </file>
@@ -1028,16 +1049,106 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1047,96 +1158,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1457,8 +1478,8 @@
   </sheetPr>
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="151" zoomScaleNormal="100" zoomScaleSheetLayoutView="151" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="151" zoomScaleNormal="100" zoomScaleSheetLayoutView="151" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1493,7 +1514,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="47" t="s">
-        <v>164</v>
+        <v>25</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>102</v>
@@ -1505,7 +1526,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="47" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>104</v>
@@ -1537,7 +1558,7 @@
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B6" s="53" t="s">
         <v>64</v>
@@ -1545,7 +1566,7 @@
     </row>
     <row r="7" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="B7" s="50" t="s">
         <v>66</v>
@@ -1553,7 +1574,7 @@
     </row>
     <row r="8" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B8" s="50" t="s">
         <v>111</v>
@@ -1561,7 +1582,7 @@
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B9" s="50" t="s">
         <v>112</v>
@@ -1577,7 +1598,7 @@
     </row>
     <row r="11" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
-        <v>164</v>
+        <v>13</v>
       </c>
       <c r="B11" s="53" t="s">
         <v>13</v>
@@ -1585,7 +1606,7 @@
     </row>
     <row r="12" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
-        <v>164</v>
+        <v>15</v>
       </c>
       <c r="B12" s="50" t="s">
         <v>15</v>
@@ -1593,7 +1614,7 @@
     </row>
     <row r="13" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B13" s="50" t="s">
         <v>115</v>
@@ -1617,7 +1638,7 @@
     </row>
     <row r="16" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B16" s="50" t="s">
         <v>120</v>
@@ -1625,7 +1646,7 @@
     </row>
     <row r="17" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B17" s="56" t="s">
         <v>121</v>
@@ -1954,26 +1975,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="69" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="70"/>
+      <c r="E2" s="100"/>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1988,15 +2009,15 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="71" t="s">
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="72"/>
+      <c r="E3" s="65"/>
       <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
@@ -2011,13 +2032,13 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="67"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="72"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2025,46 +2046,46 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="76" t="s">
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="78"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="88"/>
       <c r="Q5">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="64" t="s">
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="79"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="83"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="64" t="s">
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="79"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="83"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2074,12 +2095,12 @@
         <v>18</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="76" t="s">
+      <c r="D8" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="78"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="88"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
@@ -2089,12 +2110,12 @@
         <v>21</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="82" t="s">
+      <c r="D9" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="84"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="91"/>
     </row>
     <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
@@ -2104,12 +2125,12 @@
         <v>24</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="79"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="83"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
@@ -2119,35 +2140,35 @@
         <v>26</v>
       </c>
       <c r="C11" s="18"/>
-      <c r="D11" s="73" t="s">
+      <c r="D11" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="92"/>
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="20"/>
-      <c r="D12" s="76" t="s">
+      <c r="D12" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="88"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="73" t="s">
+      <c r="D13" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="75"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="92"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="24" t="s">
@@ -2159,10 +2180,10 @@
       <c r="C14" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="87" t="s">
+      <c r="D14" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="87"/>
+      <c r="E14" s="93"/>
       <c r="F14" s="25" t="s">
         <v>35</v>
       </c>
@@ -2404,37 +2425,37 @@
       <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="88" t="s">
+      <c r="A33" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="89"/>
-      <c r="C33" s="89"/>
-      <c r="D33" s="89"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="89"/>
-      <c r="G33" s="90"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="70"/>
     </row>
     <row r="34" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="88" t="s">
+      <c r="A34" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="89"/>
-      <c r="C34" s="89"/>
-      <c r="D34" s="89"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="89"/>
-      <c r="G34" s="90"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="70"/>
     </row>
     <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="91"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="73"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="33"/>
@@ -2453,62 +2474,62 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="92" t="s">
+      <c r="A37" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="93"/>
-      <c r="C37" s="93"/>
-      <c r="D37" s="93"/>
-      <c r="E37" s="93"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
       <c r="F37" s="36"/>
       <c r="G37" s="15"/>
     </row>
     <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="94" t="s">
+      <c r="A38" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="95"/>
-      <c r="C38" s="95"/>
-      <c r="D38" s="96" t="s">
+      <c r="B38" s="77"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="97"/>
-      <c r="F38" s="97"/>
-      <c r="G38" s="98"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="80"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="71" t="s">
+      <c r="A39" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="72"/>
-      <c r="C39" s="72"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="65"/>
       <c r="D39" s="8"/>
       <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="71" t="s">
+      <c r="A40" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="72"/>
-      <c r="C40" s="72"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
       <c r="D40" s="8"/>
       <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="71" t="s">
+      <c r="A41" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="72"/>
-      <c r="C41" s="72"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="65"/>
       <c r="D41" s="8"/>
       <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="73" t="s">
+      <c r="A42" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="74"/>
-      <c r="C42" s="74"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="67"/>
       <c r="D42" s="21"/>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
@@ -2516,26 +2537,26 @@
     </row>
     <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="44" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A44" s="68" t="s">
+      <c r="A44" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="68"/>
-      <c r="C44" s="68"/>
-      <c r="D44" s="68"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="68"/>
-      <c r="G44" s="68"/>
+      <c r="B44" s="98"/>
+      <c r="C44" s="98"/>
+      <c r="D44" s="98"/>
+      <c r="E44" s="98"/>
+      <c r="F44" s="98"/>
+      <c r="G44" s="98"/>
     </row>
     <row r="45" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="85" t="s">
+      <c r="A45" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="86"/>
-      <c r="C45" s="86"/>
-      <c r="D45" s="85" t="s">
+      <c r="B45" s="97"/>
+      <c r="C45" s="97"/>
+      <c r="D45" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="86"/>
+      <c r="E45" s="97"/>
       <c r="F45" s="1" t="s">
         <v>3</v>
       </c>
@@ -2544,15 +2565,15 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="65"/>
-      <c r="C46" s="65"/>
-      <c r="D46" s="71" t="s">
+      <c r="B46" s="82"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="72"/>
+      <c r="E46" s="65"/>
       <c r="F46" s="6" t="s">
         <v>8</v>
       </c>
@@ -2561,54 +2582,54 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A47" s="73" t="s">
+      <c r="A47" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="75"/>
-      <c r="C47" s="65"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="67"/>
+      <c r="B47" s="92"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="72"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A48" s="99" t="s">
+      <c r="A48" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="100"/>
-      <c r="C48" s="100"/>
-      <c r="D48" s="76" t="s">
+      <c r="B48" s="95"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="77"/>
-      <c r="F48" s="77"/>
-      <c r="G48" s="78"/>
+      <c r="E48" s="87"/>
+      <c r="F48" s="87"/>
+      <c r="G48" s="88"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A49" s="71" t="s">
+      <c r="A49" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="72"/>
-      <c r="C49" s="72"/>
-      <c r="D49" s="64" t="s">
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="65"/>
-      <c r="F49" s="65"/>
-      <c r="G49" s="79"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="83"/>
     </row>
     <row r="50" spans="1:16" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="80" t="s">
+      <c r="A50" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="81"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="64" t="s">
+      <c r="B50" s="85"/>
+      <c r="C50" s="85"/>
+      <c r="D50" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="65"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="79"/>
+      <c r="E50" s="82"/>
+      <c r="F50" s="82"/>
+      <c r="G50" s="83"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" s="38" t="s">
@@ -2618,12 +2639,12 @@
         <v>70</v>
       </c>
       <c r="C51" s="9"/>
-      <c r="D51" s="76" t="s">
+      <c r="D51" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="E51" s="77"/>
-      <c r="F51" s="77"/>
-      <c r="G51" s="78"/>
+      <c r="E51" s="87"/>
+      <c r="F51" s="87"/>
+      <c r="G51" s="88"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" s="12" t="s">
@@ -2633,12 +2654,12 @@
         <v>73</v>
       </c>
       <c r="C52" s="9"/>
-      <c r="D52" s="82" t="s">
+      <c r="D52" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="E52" s="83"/>
-      <c r="F52" s="83"/>
-      <c r="G52" s="84"/>
+      <c r="E52" s="90"/>
+      <c r="F52" s="90"/>
+      <c r="G52" s="91"/>
     </row>
     <row r="53" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="38" t="s">
@@ -2648,12 +2669,12 @@
         <v>76</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="D53" s="64" t="s">
+      <c r="D53" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="E53" s="65"/>
-      <c r="F53" s="65"/>
-      <c r="G53" s="79"/>
+      <c r="E53" s="82"/>
+      <c r="F53" s="82"/>
+      <c r="G53" s="83"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A54" s="16" t="s">
@@ -2663,35 +2684,35 @@
         <v>78</v>
       </c>
       <c r="C54" s="18"/>
-      <c r="D54" s="73" t="s">
+      <c r="D54" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="E54" s="74"/>
-      <c r="F54" s="74"/>
-      <c r="G54" s="75"/>
+      <c r="E54" s="67"/>
+      <c r="F54" s="67"/>
+      <c r="G54" s="92"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C55" s="20"/>
-      <c r="D55" s="76" t="s">
+      <c r="D55" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="E55" s="77"/>
-      <c r="F55" s="77"/>
-      <c r="G55" s="78"/>
+      <c r="E55" s="87"/>
+      <c r="F55" s="87"/>
+      <c r="G55" s="88"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A56" s="21"/>
       <c r="B56" s="22"/>
       <c r="C56" s="23"/>
-      <c r="D56" s="73" t="s">
+      <c r="D56" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="E56" s="74"/>
-      <c r="F56" s="74"/>
-      <c r="G56" s="75"/>
+      <c r="E56" s="67"/>
+      <c r="F56" s="67"/>
+      <c r="G56" s="92"/>
     </row>
     <row r="57" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="24" t="s">
@@ -2703,10 +2724,10 @@
       <c r="C57" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="D57" s="87" t="s">
+      <c r="D57" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="E57" s="87"/>
+      <c r="E57" s="93"/>
       <c r="F57" s="25" t="s">
         <v>85</v>
       </c>
@@ -2887,37 +2908,37 @@
       <c r="G75" s="15"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A76" s="88" t="s">
+      <c r="A76" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="B76" s="89"/>
-      <c r="C76" s="89"/>
-      <c r="D76" s="89"/>
-      <c r="E76" s="89"/>
-      <c r="F76" s="89"/>
-      <c r="G76" s="90"/>
+      <c r="B76" s="69"/>
+      <c r="C76" s="69"/>
+      <c r="D76" s="69"/>
+      <c r="E76" s="69"/>
+      <c r="F76" s="69"/>
+      <c r="G76" s="70"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A77" s="88" t="s">
+      <c r="A77" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="B77" s="89"/>
-      <c r="C77" s="89"/>
-      <c r="D77" s="89"/>
-      <c r="E77" s="89"/>
-      <c r="F77" s="89"/>
-      <c r="G77" s="90"/>
+      <c r="B77" s="69"/>
+      <c r="C77" s="69"/>
+      <c r="D77" s="69"/>
+      <c r="E77" s="69"/>
+      <c r="F77" s="69"/>
+      <c r="G77" s="70"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A78" s="66" t="s">
+      <c r="A78" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="B78" s="67"/>
-      <c r="C78" s="67"/>
-      <c r="D78" s="67"/>
-      <c r="E78" s="67"/>
-      <c r="F78" s="67"/>
-      <c r="G78" s="91"/>
+      <c r="B78" s="72"/>
+      <c r="C78" s="72"/>
+      <c r="D78" s="72"/>
+      <c r="E78" s="72"/>
+      <c r="F78" s="72"/>
+      <c r="G78" s="73"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" s="33"/>
@@ -2936,62 +2957,62 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A80" s="92" t="s">
+      <c r="A80" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="B80" s="93"/>
-      <c r="C80" s="93"/>
-      <c r="D80" s="93"/>
-      <c r="E80" s="93"/>
+      <c r="B80" s="75"/>
+      <c r="C80" s="75"/>
+      <c r="D80" s="75"/>
+      <c r="E80" s="75"/>
       <c r="F80" s="36"/>
       <c r="G80" s="15"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A81" s="94" t="s">
+      <c r="A81" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="B81" s="95"/>
-      <c r="C81" s="95"/>
-      <c r="D81" s="96" t="s">
+      <c r="B81" s="77"/>
+      <c r="C81" s="77"/>
+      <c r="D81" s="78" t="s">
         <v>98</v>
       </c>
-      <c r="E81" s="97"/>
-      <c r="F81" s="97"/>
-      <c r="G81" s="98"/>
+      <c r="E81" s="79"/>
+      <c r="F81" s="79"/>
+      <c r="G81" s="80"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A82" s="71" t="s">
+      <c r="A82" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="B82" s="72"/>
-      <c r="C82" s="72"/>
+      <c r="B82" s="65"/>
+      <c r="C82" s="65"/>
       <c r="D82" s="8"/>
       <c r="G82" s="9"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A83" s="71" t="s">
+      <c r="A83" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="B83" s="72"/>
-      <c r="C83" s="72"/>
+      <c r="B83" s="65"/>
+      <c r="C83" s="65"/>
       <c r="D83" s="8"/>
       <c r="G83" s="9"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A84" s="71" t="s">
+      <c r="A84" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="B84" s="72"/>
-      <c r="C84" s="72"/>
+      <c r="B84" s="65"/>
+      <c r="C84" s="65"/>
       <c r="D84" s="8"/>
       <c r="G84" s="9"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A85" s="73" t="s">
+      <c r="A85" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="B85" s="74"/>
-      <c r="C85" s="74"/>
+      <c r="B85" s="67"/>
+      <c r="C85" s="67"/>
       <c r="D85" s="21"/>
       <c r="E85" s="22"/>
       <c r="F85" s="22"/>
@@ -2999,33 +3020,25 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A77:G77"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="A82:C82"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="D14:E14"/>
@@ -3040,25 +3053,33 @@
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="A44:G44"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A83:C83"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A77:G77"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="A82:C82"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3" xr:uid="{6D6CA36A-C765-4458-8A8E-A06DE7CFDD36}">

</xml_diff>

<commit_message>
contract cost tmp section added, format function cost added, format counts functions updated
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,15 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D27FE3D-CC52-43AB-B9C4-003CE4731E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DE9312-048F-45F8-8C30-50485F0B1F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14497" yWindow="16103" windowWidth="28994" windowHeight="15794" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-23828" yWindow="570" windowWidth="18953" windowHeight="11040" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
     <sheet name="32" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Адрес_покупатель_банк_свифт">Export_Contract!$A$44</definedName>
+    <definedName name="Адреса_банк_получателя">Export_Contract!$A$33</definedName>
+    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$A$34</definedName>
+    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$A$35</definedName>
+    <definedName name="Адреса_покупатель">Export_Contract!$A$39</definedName>
+    <definedName name="Адреса_покупатель_адрес">Export_Contract!$A$40</definedName>
+    <definedName name="Адреса_покупатель_банк">Export_Contract!$A$41</definedName>
+    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$A$43</definedName>
+    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$A$42</definedName>
+    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$A$45</definedName>
+    <definedName name="Адреса_покупатель_заголовок">Export_Contract!$A$38</definedName>
+    <definedName name="Адреса_покупатель_счет">Export_Contract!$A$46</definedName>
+    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$A$36</definedName>
+    <definedName name="Адреса_получатель_счет">Export_Contract!$A$37</definedName>
+    <definedName name="Адреса_продавец">Export_Contract!$A$31</definedName>
+    <definedName name="Адреса_продавец_адрес">Export_Contract!$A$32</definedName>
+    <definedName name="Адреса_продавец_заголовок">Export_Contract!$A$30</definedName>
+    <definedName name="Адреса_сторон_заголовок">Export_Contract!$A$29</definedName>
+    <definedName name="Доставка_заголовок">Export_Contract!$A$22</definedName>
+    <definedName name="Доставка_порт">Export_Contract!$A$24</definedName>
+    <definedName name="Доставка_условия">Export_Contract!$A$23</definedName>
     <definedName name="Контракт">Export_Contract!$A$2</definedName>
     <definedName name="Контракт_дата">Export_Contract!$A$3</definedName>
     <definedName name="Покупатель">Export_Contract!$A$11</definedName>
@@ -32,8 +53,16 @@
     <definedName name="Продавец_заголовок">Export_Contract!$A$5</definedName>
     <definedName name="Продавец_подписант">Export_Contract!$A$9</definedName>
     <definedName name="Продавец_представитель">Export_Contract!$A$8</definedName>
+    <definedName name="Прочие_условия_заголовок">Export_Contract!$A$27</definedName>
+    <definedName name="Прочие_условия_описание">Export_Contract!$A$28</definedName>
+    <definedName name="Сертификаты_массив">Export_Contract!$A$26</definedName>
+    <definedName name="Сертификаты_описание">Export_Contract!$A$25</definedName>
     <definedName name="Соглашение">Export_Contract!$A$1</definedName>
     <definedName name="Стороны_заголовок">Export_Contract!$A$4</definedName>
+    <definedName name="Цена_всего">Export_Contract!$A$21</definedName>
+    <definedName name="Цена_заголовок">Export_Contract!$A$18</definedName>
+    <definedName name="Цена_массив">Export_Contract!$A$20</definedName>
+    <definedName name="Цена_описание">Export_Contract!$A$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1049,6 +1078,27 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1060,6 +1110,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1069,12 +1158,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1099,65 +1182,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1478,8 +1507,8 @@
   </sheetPr>
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="151" zoomScaleNormal="100" zoomScaleSheetLayoutView="151" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A12" zoomScale="151" zoomScaleNormal="100" zoomScaleSheetLayoutView="151" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1975,26 +2004,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="99" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="100"/>
+      <c r="E2" s="70"/>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2009,15 +2038,15 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="64" t="s">
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="65"/>
+      <c r="E3" s="72"/>
       <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
@@ -2032,13 +2061,13 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="72"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2046,46 +2075,46 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="86" t="s">
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="88"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="78"/>
       <c r="Q5">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="81" t="s">
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="83"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="79"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="81" t="s">
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="83"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="79"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2095,12 +2124,12 @@
         <v>18</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="86" t="s">
+      <c r="D8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="88"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="78"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
@@ -2110,12 +2139,12 @@
         <v>21</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="89" t="s">
+      <c r="D9" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="91"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="84"/>
     </row>
     <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
@@ -2125,12 +2154,12 @@
         <v>24</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="81" t="s">
+      <c r="D10" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="83"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="79"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
@@ -2140,35 +2169,35 @@
         <v>26</v>
       </c>
       <c r="C11" s="18"/>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="92"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="75"/>
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="20"/>
-      <c r="D12" s="86" t="s">
+      <c r="D12" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="88"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="66" t="s">
+      <c r="D13" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="92"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="75"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="24" t="s">
@@ -2180,10 +2209,10 @@
       <c r="C14" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="93" t="s">
+      <c r="D14" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="93"/>
+      <c r="E14" s="87"/>
       <c r="F14" s="25" t="s">
         <v>35</v>
       </c>
@@ -2425,37 +2454,37 @@
       <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="68" t="s">
+      <c r="A33" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="70"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="90"/>
     </row>
     <row r="34" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="68" t="s">
+      <c r="A34" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="70"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="89"/>
+      <c r="F34" s="89"/>
+      <c r="G34" s="90"/>
     </row>
     <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="71" t="s">
+      <c r="A35" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="73"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="67"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="91"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="33"/>
@@ -2474,62 +2503,62 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="74" t="s">
+      <c r="A37" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="93"/>
+      <c r="D37" s="93"/>
+      <c r="E37" s="93"/>
       <c r="F37" s="36"/>
       <c r="G37" s="15"/>
     </row>
     <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="76" t="s">
+      <c r="A38" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="78" t="s">
+      <c r="B38" s="95"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="79"/>
-      <c r="F38" s="79"/>
-      <c r="G38" s="80"/>
+      <c r="E38" s="97"/>
+      <c r="F38" s="97"/>
+      <c r="G38" s="98"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="64" t="s">
+      <c r="A39" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="65"/>
-      <c r="C39" s="65"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="72"/>
       <c r="D39" s="8"/>
       <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="64" t="s">
+      <c r="A40" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="72"/>
       <c r="D40" s="8"/>
       <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="64" t="s">
+      <c r="A41" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="65"/>
-      <c r="C41" s="65"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="72"/>
       <c r="D41" s="8"/>
       <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="67"/>
-      <c r="C42" s="67"/>
+      <c r="B42" s="74"/>
+      <c r="C42" s="74"/>
       <c r="D42" s="21"/>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
@@ -2537,26 +2566,26 @@
     </row>
     <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="44" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A44" s="98" t="s">
+      <c r="A44" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="98"/>
-      <c r="C44" s="98"/>
-      <c r="D44" s="98"/>
-      <c r="E44" s="98"/>
-      <c r="F44" s="98"/>
-      <c r="G44" s="98"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="68"/>
     </row>
     <row r="45" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="96" t="s">
+      <c r="A45" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="97"/>
-      <c r="C45" s="97"/>
-      <c r="D45" s="96" t="s">
+      <c r="B45" s="86"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="97"/>
+      <c r="E45" s="86"/>
       <c r="F45" s="1" t="s">
         <v>3</v>
       </c>
@@ -2565,15 +2594,15 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="81" t="s">
+      <c r="A46" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="82"/>
-      <c r="C46" s="82"/>
-      <c r="D46" s="64" t="s">
+      <c r="B46" s="65"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="65"/>
+      <c r="E46" s="72"/>
       <c r="F46" s="6" t="s">
         <v>8</v>
       </c>
@@ -2582,54 +2611,54 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="92"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="72"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="67"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A48" s="94" t="s">
+      <c r="A48" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="95"/>
-      <c r="C48" s="95"/>
-      <c r="D48" s="86" t="s">
+      <c r="B48" s="100"/>
+      <c r="C48" s="100"/>
+      <c r="D48" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="87"/>
-      <c r="F48" s="87"/>
-      <c r="G48" s="88"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="77"/>
+      <c r="G48" s="78"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A49" s="64" t="s">
+      <c r="A49" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="65"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="81" t="s">
+      <c r="B49" s="72"/>
+      <c r="C49" s="72"/>
+      <c r="D49" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="82"/>
-      <c r="F49" s="82"/>
-      <c r="G49" s="83"/>
+      <c r="E49" s="65"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="79"/>
     </row>
     <row r="50" spans="1:16" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="84" t="s">
+      <c r="A50" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="85"/>
-      <c r="C50" s="85"/>
-      <c r="D50" s="81" t="s">
+      <c r="B50" s="81"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="82"/>
-      <c r="F50" s="82"/>
-      <c r="G50" s="83"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="65"/>
+      <c r="G50" s="79"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" s="38" t="s">
@@ -2639,12 +2668,12 @@
         <v>70</v>
       </c>
       <c r="C51" s="9"/>
-      <c r="D51" s="86" t="s">
+      <c r="D51" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="E51" s="87"/>
-      <c r="F51" s="87"/>
-      <c r="G51" s="88"/>
+      <c r="E51" s="77"/>
+      <c r="F51" s="77"/>
+      <c r="G51" s="78"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" s="12" t="s">
@@ -2654,12 +2683,12 @@
         <v>73</v>
       </c>
       <c r="C52" s="9"/>
-      <c r="D52" s="89" t="s">
+      <c r="D52" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="E52" s="90"/>
-      <c r="F52" s="90"/>
-      <c r="G52" s="91"/>
+      <c r="E52" s="83"/>
+      <c r="F52" s="83"/>
+      <c r="G52" s="84"/>
     </row>
     <row r="53" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="38" t="s">
@@ -2669,12 +2698,12 @@
         <v>76</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="D53" s="81" t="s">
+      <c r="D53" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="E53" s="82"/>
-      <c r="F53" s="82"/>
-      <c r="G53" s="83"/>
+      <c r="E53" s="65"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="79"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A54" s="16" t="s">
@@ -2684,35 +2713,35 @@
         <v>78</v>
       </c>
       <c r="C54" s="18"/>
-      <c r="D54" s="66" t="s">
+      <c r="D54" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="E54" s="67"/>
-      <c r="F54" s="67"/>
-      <c r="G54" s="92"/>
+      <c r="E54" s="74"/>
+      <c r="F54" s="74"/>
+      <c r="G54" s="75"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C55" s="20"/>
-      <c r="D55" s="86" t="s">
+      <c r="D55" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="E55" s="87"/>
-      <c r="F55" s="87"/>
-      <c r="G55" s="88"/>
+      <c r="E55" s="77"/>
+      <c r="F55" s="77"/>
+      <c r="G55" s="78"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A56" s="21"/>
       <c r="B56" s="22"/>
       <c r="C56" s="23"/>
-      <c r="D56" s="66" t="s">
+      <c r="D56" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="E56" s="67"/>
-      <c r="F56" s="67"/>
-      <c r="G56" s="92"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="74"/>
+      <c r="G56" s="75"/>
     </row>
     <row r="57" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="24" t="s">
@@ -2724,10 +2753,10 @@
       <c r="C57" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="D57" s="93" t="s">
+      <c r="D57" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="E57" s="93"/>
+      <c r="E57" s="87"/>
       <c r="F57" s="25" t="s">
         <v>85</v>
       </c>
@@ -2908,37 +2937,37 @@
       <c r="G75" s="15"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A76" s="68" t="s">
+      <c r="A76" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="B76" s="69"/>
-      <c r="C76" s="69"/>
-      <c r="D76" s="69"/>
-      <c r="E76" s="69"/>
-      <c r="F76" s="69"/>
-      <c r="G76" s="70"/>
+      <c r="B76" s="89"/>
+      <c r="C76" s="89"/>
+      <c r="D76" s="89"/>
+      <c r="E76" s="89"/>
+      <c r="F76" s="89"/>
+      <c r="G76" s="90"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A77" s="68" t="s">
+      <c r="A77" s="88" t="s">
         <v>93</v>
       </c>
-      <c r="B77" s="69"/>
-      <c r="C77" s="69"/>
-      <c r="D77" s="69"/>
-      <c r="E77" s="69"/>
-      <c r="F77" s="69"/>
-      <c r="G77" s="70"/>
+      <c r="B77" s="89"/>
+      <c r="C77" s="89"/>
+      <c r="D77" s="89"/>
+      <c r="E77" s="89"/>
+      <c r="F77" s="89"/>
+      <c r="G77" s="90"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A78" s="71" t="s">
+      <c r="A78" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B78" s="72"/>
-      <c r="C78" s="72"/>
-      <c r="D78" s="72"/>
-      <c r="E78" s="72"/>
-      <c r="F78" s="72"/>
-      <c r="G78" s="73"/>
+      <c r="B78" s="67"/>
+      <c r="C78" s="67"/>
+      <c r="D78" s="67"/>
+      <c r="E78" s="67"/>
+      <c r="F78" s="67"/>
+      <c r="G78" s="91"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" s="33"/>
@@ -2957,62 +2986,62 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A80" s="74" t="s">
+      <c r="A80" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="B80" s="75"/>
-      <c r="C80" s="75"/>
-      <c r="D80" s="75"/>
-      <c r="E80" s="75"/>
+      <c r="B80" s="93"/>
+      <c r="C80" s="93"/>
+      <c r="D80" s="93"/>
+      <c r="E80" s="93"/>
       <c r="F80" s="36"/>
       <c r="G80" s="15"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A81" s="76" t="s">
+      <c r="A81" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="B81" s="77"/>
-      <c r="C81" s="77"/>
-      <c r="D81" s="78" t="s">
+      <c r="B81" s="95"/>
+      <c r="C81" s="95"/>
+      <c r="D81" s="96" t="s">
         <v>98</v>
       </c>
-      <c r="E81" s="79"/>
-      <c r="F81" s="79"/>
-      <c r="G81" s="80"/>
+      <c r="E81" s="97"/>
+      <c r="F81" s="97"/>
+      <c r="G81" s="98"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A82" s="64" t="s">
+      <c r="A82" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="B82" s="65"/>
-      <c r="C82" s="65"/>
+      <c r="B82" s="72"/>
+      <c r="C82" s="72"/>
       <c r="D82" s="8"/>
       <c r="G82" s="9"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A83" s="64" t="s">
+      <c r="A83" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="B83" s="65"/>
-      <c r="C83" s="65"/>
+      <c r="B83" s="72"/>
+      <c r="C83" s="72"/>
       <c r="D83" s="8"/>
       <c r="G83" s="9"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A84" s="64" t="s">
+      <c r="A84" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B84" s="65"/>
-      <c r="C84" s="65"/>
+      <c r="B84" s="72"/>
+      <c r="C84" s="72"/>
       <c r="D84" s="8"/>
       <c r="G84" s="9"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A85" s="66" t="s">
+      <c r="A85" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="B85" s="67"/>
-      <c r="C85" s="67"/>
+      <c r="B85" s="74"/>
+      <c r="C85" s="74"/>
       <c r="D85" s="21"/>
       <c r="E85" s="22"/>
       <c r="F85" s="22"/>
@@ -3020,25 +3049,33 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="A83:C83"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A77:G77"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:G48"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="D14:E14"/>
@@ -3053,33 +3090,25 @@
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A77:G77"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3" xr:uid="{6D6CA36A-C765-4458-8A8E-A06DE7CFDD36}">

</xml_diff>

<commit_message>
template contract export ready, implementing front
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DE9312-048F-45F8-8C30-50485F0B1F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479505CF-7B1C-43D6-B02E-9AA317A444E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23828" yWindow="570" windowWidth="18953" windowHeight="11040" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-28898" yWindow="-907" windowWidth="28996" windowHeight="15795" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -908,7 +908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1068,9 +1068,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1078,16 +1075,106 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1098,95 +1185,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1507,14 +1513,13 @@
   </sheetPr>
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A12" zoomScale="151" zoomScaleNormal="100" zoomScaleSheetLayoutView="151" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScale="151" zoomScaleNormal="100" zoomScaleSheetLayoutView="151" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" customWidth="1"/>
-    <col min="2" max="2" width="49.6640625" customWidth="1"/>
+    <col min="1" max="2" width="50.19921875" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.796875" customWidth="1"/>
@@ -1763,18 +1768,18 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="61" t="s">
+      <c r="A25" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="100" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="56.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:21" ht="55.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="101" t="s">
         <v>138</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="102" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1934,15 +1939,15 @@
       <c r="A46" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="B46" s="62" t="s">
+      <c r="B46" s="61" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="63" t="s">
+      <c r="A47" s="62" t="s">
         <v>158</v>
       </c>
-      <c r="B47" s="63" t="s">
+      <c r="B47" s="62" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2004,26 +2009,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="69" t="s">
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="70"/>
+      <c r="E2" s="99"/>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2038,15 +2043,15 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="71" t="s">
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="72"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
@@ -2061,13 +2066,13 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="67"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="71"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2075,46 +2080,46 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="76" t="s">
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="78"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="87"/>
       <c r="Q5">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="64" t="s">
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="79"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="82"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="64" t="s">
+      <c r="B7" s="84"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="79"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="82"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2124,12 +2129,12 @@
         <v>18</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="76" t="s">
+      <c r="D8" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="78"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="87"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
@@ -2139,12 +2144,12 @@
         <v>21</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="82" t="s">
+      <c r="D9" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="84"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="90"/>
     </row>
     <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
@@ -2154,12 +2159,12 @@
         <v>24</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="79"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="82"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
@@ -2169,35 +2174,35 @@
         <v>26</v>
       </c>
       <c r="C11" s="18"/>
-      <c r="D11" s="73" t="s">
+      <c r="D11" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="91"/>
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="20"/>
-      <c r="D12" s="76" t="s">
+      <c r="D12" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="87"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="73" t="s">
+      <c r="D13" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="75"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="91"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="24" t="s">
@@ -2209,10 +2214,10 @@
       <c r="C14" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="87" t="s">
+      <c r="D14" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="87"/>
+      <c r="E14" s="92"/>
       <c r="F14" s="25" t="s">
         <v>35</v>
       </c>
@@ -2454,37 +2459,37 @@
       <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="88" t="s">
+      <c r="A33" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="89"/>
-      <c r="C33" s="89"/>
-      <c r="D33" s="89"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="89"/>
-      <c r="G33" s="90"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="69"/>
     </row>
     <row r="34" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="88" t="s">
+      <c r="A34" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="89"/>
-      <c r="C34" s="89"/>
-      <c r="D34" s="89"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="89"/>
-      <c r="G34" s="90"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="69"/>
     </row>
     <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="91"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="72"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="33"/>
@@ -2503,62 +2508,62 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="92" t="s">
+      <c r="A37" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="93"/>
-      <c r="C37" s="93"/>
-      <c r="D37" s="93"/>
-      <c r="E37" s="93"/>
+      <c r="B37" s="74"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
       <c r="F37" s="36"/>
       <c r="G37" s="15"/>
     </row>
     <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="94" t="s">
+      <c r="A38" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="95"/>
-      <c r="C38" s="95"/>
-      <c r="D38" s="96" t="s">
+      <c r="B38" s="76"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="97"/>
-      <c r="F38" s="97"/>
-      <c r="G38" s="98"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="79"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="71" t="s">
+      <c r="A39" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="72"/>
-      <c r="C39" s="72"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="64"/>
       <c r="D39" s="8"/>
       <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="71" t="s">
+      <c r="A40" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="72"/>
-      <c r="C40" s="72"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="64"/>
       <c r="D40" s="8"/>
       <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="71" t="s">
+      <c r="A41" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="72"/>
-      <c r="C41" s="72"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="64"/>
       <c r="D41" s="8"/>
       <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="73" t="s">
+      <c r="A42" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="74"/>
-      <c r="C42" s="74"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
       <c r="D42" s="21"/>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
@@ -2566,26 +2571,26 @@
     </row>
     <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="44" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A44" s="68" t="s">
+      <c r="A44" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="68"/>
-      <c r="C44" s="68"/>
-      <c r="D44" s="68"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="68"/>
-      <c r="G44" s="68"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="97"/>
+      <c r="D44" s="97"/>
+      <c r="E44" s="97"/>
+      <c r="F44" s="97"/>
+      <c r="G44" s="97"/>
     </row>
     <row r="45" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="85" t="s">
+      <c r="A45" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="86"/>
-      <c r="C45" s="86"/>
-      <c r="D45" s="85" t="s">
+      <c r="B45" s="96"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="86"/>
+      <c r="E45" s="96"/>
       <c r="F45" s="1" t="s">
         <v>3</v>
       </c>
@@ -2594,15 +2599,15 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="65"/>
-      <c r="C46" s="65"/>
-      <c r="D46" s="71" t="s">
+      <c r="B46" s="81"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="72"/>
+      <c r="E46" s="64"/>
       <c r="F46" s="6" t="s">
         <v>8</v>
       </c>
@@ -2611,54 +2616,54 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A47" s="73" t="s">
+      <c r="A47" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="75"/>
-      <c r="C47" s="65"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="67"/>
+      <c r="B47" s="91"/>
+      <c r="C47" s="81"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="71"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A48" s="99" t="s">
+      <c r="A48" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="100"/>
-      <c r="C48" s="100"/>
-      <c r="D48" s="76" t="s">
+      <c r="B48" s="94"/>
+      <c r="C48" s="94"/>
+      <c r="D48" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="77"/>
-      <c r="F48" s="77"/>
-      <c r="G48" s="78"/>
+      <c r="E48" s="86"/>
+      <c r="F48" s="86"/>
+      <c r="G48" s="87"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A49" s="71" t="s">
+      <c r="A49" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="72"/>
-      <c r="C49" s="72"/>
-      <c r="D49" s="64" t="s">
+      <c r="B49" s="64"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="65"/>
-      <c r="F49" s="65"/>
-      <c r="G49" s="79"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="82"/>
     </row>
     <row r="50" spans="1:16" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="80" t="s">
+      <c r="A50" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="81"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="64" t="s">
+      <c r="B50" s="84"/>
+      <c r="C50" s="84"/>
+      <c r="D50" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="65"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="79"/>
+      <c r="E50" s="81"/>
+      <c r="F50" s="81"/>
+      <c r="G50" s="82"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" s="38" t="s">
@@ -2668,12 +2673,12 @@
         <v>70</v>
       </c>
       <c r="C51" s="9"/>
-      <c r="D51" s="76" t="s">
+      <c r="D51" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="E51" s="77"/>
-      <c r="F51" s="77"/>
-      <c r="G51" s="78"/>
+      <c r="E51" s="86"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="87"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" s="12" t="s">
@@ -2683,12 +2688,12 @@
         <v>73</v>
       </c>
       <c r="C52" s="9"/>
-      <c r="D52" s="82" t="s">
+      <c r="D52" s="88" t="s">
         <v>74</v>
       </c>
-      <c r="E52" s="83"/>
-      <c r="F52" s="83"/>
-      <c r="G52" s="84"/>
+      <c r="E52" s="89"/>
+      <c r="F52" s="89"/>
+      <c r="G52" s="90"/>
     </row>
     <row r="53" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="38" t="s">
@@ -2698,12 +2703,12 @@
         <v>76</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="D53" s="64" t="s">
+      <c r="D53" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="E53" s="65"/>
-      <c r="F53" s="65"/>
-      <c r="G53" s="79"/>
+      <c r="E53" s="81"/>
+      <c r="F53" s="81"/>
+      <c r="G53" s="82"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A54" s="16" t="s">
@@ -2713,35 +2718,35 @@
         <v>78</v>
       </c>
       <c r="C54" s="18"/>
-      <c r="D54" s="73" t="s">
+      <c r="D54" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="E54" s="74"/>
-      <c r="F54" s="74"/>
-      <c r="G54" s="75"/>
+      <c r="E54" s="66"/>
+      <c r="F54" s="66"/>
+      <c r="G54" s="91"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C55" s="20"/>
-      <c r="D55" s="76" t="s">
+      <c r="D55" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="E55" s="77"/>
-      <c r="F55" s="77"/>
-      <c r="G55" s="78"/>
+      <c r="E55" s="86"/>
+      <c r="F55" s="86"/>
+      <c r="G55" s="87"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A56" s="21"/>
       <c r="B56" s="22"/>
       <c r="C56" s="23"/>
-      <c r="D56" s="73" t="s">
+      <c r="D56" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="E56" s="74"/>
-      <c r="F56" s="74"/>
-      <c r="G56" s="75"/>
+      <c r="E56" s="66"/>
+      <c r="F56" s="66"/>
+      <c r="G56" s="91"/>
     </row>
     <row r="57" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="24" t="s">
@@ -2753,10 +2758,10 @@
       <c r="C57" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="D57" s="87" t="s">
+      <c r="D57" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="E57" s="87"/>
+      <c r="E57" s="92"/>
       <c r="F57" s="25" t="s">
         <v>85</v>
       </c>
@@ -2937,37 +2942,37 @@
       <c r="G75" s="15"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A76" s="88" t="s">
+      <c r="A76" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="B76" s="89"/>
-      <c r="C76" s="89"/>
-      <c r="D76" s="89"/>
-      <c r="E76" s="89"/>
-      <c r="F76" s="89"/>
-      <c r="G76" s="90"/>
+      <c r="B76" s="68"/>
+      <c r="C76" s="68"/>
+      <c r="D76" s="68"/>
+      <c r="E76" s="68"/>
+      <c r="F76" s="68"/>
+      <c r="G76" s="69"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A77" s="88" t="s">
+      <c r="A77" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="B77" s="89"/>
-      <c r="C77" s="89"/>
-      <c r="D77" s="89"/>
-      <c r="E77" s="89"/>
-      <c r="F77" s="89"/>
-      <c r="G77" s="90"/>
+      <c r="B77" s="68"/>
+      <c r="C77" s="68"/>
+      <c r="D77" s="68"/>
+      <c r="E77" s="68"/>
+      <c r="F77" s="68"/>
+      <c r="G77" s="69"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A78" s="66" t="s">
+      <c r="A78" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="B78" s="67"/>
-      <c r="C78" s="67"/>
-      <c r="D78" s="67"/>
-      <c r="E78" s="67"/>
-      <c r="F78" s="67"/>
-      <c r="G78" s="91"/>
+      <c r="B78" s="71"/>
+      <c r="C78" s="71"/>
+      <c r="D78" s="71"/>
+      <c r="E78" s="71"/>
+      <c r="F78" s="71"/>
+      <c r="G78" s="72"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" s="33"/>
@@ -2986,62 +2991,62 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A80" s="92" t="s">
+      <c r="A80" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="B80" s="93"/>
-      <c r="C80" s="93"/>
-      <c r="D80" s="93"/>
-      <c r="E80" s="93"/>
+      <c r="B80" s="74"/>
+      <c r="C80" s="74"/>
+      <c r="D80" s="74"/>
+      <c r="E80" s="74"/>
       <c r="F80" s="36"/>
       <c r="G80" s="15"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A81" s="94" t="s">
+      <c r="A81" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="B81" s="95"/>
-      <c r="C81" s="95"/>
-      <c r="D81" s="96" t="s">
+      <c r="B81" s="76"/>
+      <c r="C81" s="76"/>
+      <c r="D81" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="E81" s="97"/>
-      <c r="F81" s="97"/>
-      <c r="G81" s="98"/>
+      <c r="E81" s="78"/>
+      <c r="F81" s="78"/>
+      <c r="G81" s="79"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A82" s="71" t="s">
+      <c r="A82" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="B82" s="72"/>
-      <c r="C82" s="72"/>
+      <c r="B82" s="64"/>
+      <c r="C82" s="64"/>
       <c r="D82" s="8"/>
       <c r="G82" s="9"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A83" s="71" t="s">
+      <c r="A83" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="B83" s="72"/>
-      <c r="C83" s="72"/>
+      <c r="B83" s="64"/>
+      <c r="C83" s="64"/>
       <c r="D83" s="8"/>
       <c r="G83" s="9"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A84" s="71" t="s">
+      <c r="A84" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="B84" s="72"/>
-      <c r="C84" s="72"/>
+      <c r="B84" s="64"/>
+      <c r="C84" s="64"/>
       <c r="D84" s="8"/>
       <c r="G84" s="9"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A85" s="73" t="s">
+      <c r="A85" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="B85" s="74"/>
-      <c r="C85" s="74"/>
+      <c r="B85" s="66"/>
+      <c r="C85" s="66"/>
       <c r="D85" s="21"/>
       <c r="E85" s="22"/>
       <c r="F85" s="22"/>
@@ -3049,33 +3054,25 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A77:G77"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="A82:C82"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="D14:E14"/>
@@ -3090,25 +3087,33 @@
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="A44:G44"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A83:C83"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A77:G77"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="A82:C82"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3" xr:uid="{6D6CA36A-C765-4458-8A8E-A06DE7CFDD36}">

</xml_diff>

<commit_message>
com invoice template names cells implemented + minor fixes in formatCount and contract template
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6032F0C-DC7D-4BFF-B02A-A7742E41B891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649204C6-553B-4D39-9E7E-EB86F06FA21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34388" yWindow="3593" windowWidth="14242" windowHeight="10409" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="26783" yWindow="-98" windowWidth="28995" windowHeight="15796" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -40,11 +40,75 @@
     <definedName name="Доставка_порт">Export_Contract!$A$24</definedName>
     <definedName name="Доставка_условия">Export_Contract!$A$23</definedName>
     <definedName name="Инвойс">Com_Invoice!$D$3</definedName>
+    <definedName name="Инвойс_Bl">Com_Invoice!$A$15</definedName>
+    <definedName name="Инвойс_Bl_п">Com_Invoice!$A$58</definedName>
+    <definedName name="Инвойс_банк_получателя">Com_Invoice!$A$38</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес">Com_Invoice!$A$39</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес_п">Com_Invoice!$A$82</definedName>
+    <definedName name="Инвойс_банк_получателя_п">Com_Invoice!$A$81</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт">Com_Invoice!$A$40</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт_п">Com_Invoice!$A$83</definedName>
+    <definedName name="Инвойс_всего">Com_Invoice!$E$15</definedName>
+    <definedName name="Инвойс_всего_п">Com_Invoice!$E$58</definedName>
+    <definedName name="Инвойс_дата_п">Com_Invoice!$A$52</definedName>
+    <definedName name="Инвойс_контракт">Com_Invoice!$D$10</definedName>
+    <definedName name="Инвойс_контракт_дата">Com_Invoice!$D$11</definedName>
+    <definedName name="Инвойс_контракт_дата_п">Com_Invoice!$D$54</definedName>
+    <definedName name="Инвойс_контракт_п">Com_Invoice!$D$53</definedName>
+    <definedName name="Инвойс_куда">Com_Invoice!$A$11</definedName>
+    <definedName name="Инвойс_куда_п">Com_Invoice!$A$54</definedName>
+    <definedName name="Инвойс_места">Com_Invoice!$D$15</definedName>
+    <definedName name="Инвойс_места_п">Com_Invoice!$D$58</definedName>
+    <definedName name="Инвойс_откуда">Com_Invoice!$B$11</definedName>
+    <definedName name="Инвойс_откуда_п">Com_Invoice!$B$54</definedName>
+    <definedName name="Инвойс_п">Com_Invoice!$D$46</definedName>
+    <definedName name="Инвойс_подвал_всего">Com_Invoice!$D$36</definedName>
+    <definedName name="Инвойс_подвал_всего_п">Com_Invoice!$D$79</definedName>
+    <definedName name="Инвойс_подвал_места">Com_Invoice!$C$36</definedName>
+    <definedName name="Инвойс_подвал_места_п">Com_Invoice!$C$79</definedName>
+    <definedName name="Инвойс_подвал_сумма">Com_Invoice!$G$36</definedName>
+    <definedName name="Инвойс_подвал_сумма_п">Com_Invoice!$G$79</definedName>
+    <definedName name="Инвойс_подписант">Com_Invoice!$D$38</definedName>
+    <definedName name="Инвойс_подписант_п">Com_Invoice!$D$81</definedName>
+    <definedName name="Инвойс_покупатель">Com_Invoice!$D$6</definedName>
+    <definedName name="Инвойс_покупатель_адрес">Com_Invoice!$D$7</definedName>
+    <definedName name="Инвойс_покупатель_адрес_п">Com_Invoice!$D$50</definedName>
+    <definedName name="Инвойс_покупатель_п">Com_Invoice!$D$49</definedName>
+    <definedName name="Инвойс_получатель">Com_Invoice!$A$6</definedName>
+    <definedName name="Инвойс_получатель_адрес">Com_Invoice!$A$7</definedName>
+    <definedName name="Инвойс_получатель_адрес_п">Com_Invoice!$A$50</definedName>
+    <definedName name="Инвойс_получатель_в_пользу">Com_Invoice!$A$41</definedName>
+    <definedName name="Инвойс_получатель_в_пользу_п">Com_Invoice!$A$84</definedName>
+    <definedName name="Инвойс_получатель_п">Com_Invoice!$A$49</definedName>
+    <definedName name="Инвойс_получатель_счет">Com_Invoice!$A$42</definedName>
+    <definedName name="Инвойс_получатель_счет_п">Com_Invoice!$A$85</definedName>
     <definedName name="Инвойс_продавец">Com_Invoice!$A$3</definedName>
+    <definedName name="Инвойс_продавец_адрес">Com_Invoice!$A$4</definedName>
+    <definedName name="Инвойс_продавец_адрес_п">Com_Invoice!$A$47</definedName>
+    <definedName name="Инвойс_продавец_п">Com_Invoice!$A$46</definedName>
+    <definedName name="Инвойс_продукт">Com_Invoice!$B$15</definedName>
+    <definedName name="Инвойс_продукт_п">Com_Invoice!$B$58</definedName>
+    <definedName name="Инвойс_соглашение">Com_Invoice!$D$9</definedName>
+    <definedName name="Инвойс_соглашение_п">Com_Invoice!$D$52</definedName>
+    <definedName name="Инвойс_судно">Com_Invoice!$A$33</definedName>
+    <definedName name="Инвойс_судно_п">Com_Invoice!$A$76</definedName>
+    <definedName name="Инвойс_сумма">Com_Invoice!$G$15</definedName>
+    <definedName name="Инвойс_сумма_п">Com_Invoice!$G$58</definedName>
+    <definedName name="Инвойс_транспорт">Com_Invoice!$B$9</definedName>
+    <definedName name="Инвойс_транспорт_п">Com_Invoice!$B$52</definedName>
+    <definedName name="Инвойс_упаковка">Com_Invoice!$C$15</definedName>
+    <definedName name="Инвойс_упаковка_п">Com_Invoice!$C$58</definedName>
+    <definedName name="Инвойс_условия">Com_Invoice!$D$13</definedName>
+    <definedName name="Инвойс_условия_п">Com_Invoice!$D$56</definedName>
+    <definedName name="Инвойс_цена">Com_Invoice!$F$15</definedName>
+    <definedName name="Инвойс_цена_п">Com_Invoice!$F$58</definedName>
+    <definedName name="Иновйс_дата">Com_Invoice!$A$9</definedName>
     <definedName name="Контракт">Export_Contract!$A$2</definedName>
     <definedName name="Контракт_дата">Export_Contract!$A$3</definedName>
     <definedName name="МСЦ">Com_Invoice!$F$3</definedName>
+    <definedName name="МСЦ_п">Com_Invoice!$F$46</definedName>
     <definedName name="МСЦ_сертификат">Com_Invoice!$G$3</definedName>
+    <definedName name="МСЦ_сертификат_п">Com_Invoice!$G$46</definedName>
     <definedName name="Покупатель">Export_Contract!$A$11</definedName>
     <definedName name="Покупатель_адрес">Export_Contract!$A$12</definedName>
     <definedName name="Покупатель_заголовок">Export_Contract!$A$10</definedName>
@@ -90,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="170">
   <si>
     <t>COMMERCIAL INVOICE</t>
   </si>
@@ -706,7 +770,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -716,12 +780,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBFBFBF"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -907,7 +965,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1061,12 +1119,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1083,16 +1135,106 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1102,96 +1244,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1512,8 +1564,8 @@
   </sheetPr>
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="151" zoomScaleNormal="100" zoomScaleSheetLayoutView="151" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="151" zoomScaleNormal="100" zoomScaleSheetLayoutView="151" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1661,7 +1713,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="54" t="s">
         <v>116</v>
       </c>
@@ -1710,7 +1762,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="54" t="s">
         <v>122</v>
       </c>
@@ -1742,11 +1794,11 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="59" t="s">
+    <row r="22" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="54" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1767,22 +1819,22 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="63" t="s">
+      <c r="A25" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="61" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="55.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="65" t="s">
+      <c r="B26" s="63" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="54" t="s">
         <v>138</v>
       </c>
@@ -1798,7 +1850,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="54" t="s">
         <v>142</v>
       </c>
@@ -1938,15 +1990,15 @@
       <c r="A46" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="B46" s="61" t="s">
+      <c r="B46" s="59" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="62" t="s">
+      <c r="A47" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="B47" s="62" t="s">
+      <c r="B47" s="60" t="s">
         <v>157</v>
       </c>
     </row>
@@ -1985,8 +2037,8 @@
   </sheetPr>
   <dimension ref="A1:Z85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A31" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2008,26 +2060,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="71" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="72"/>
+      <c r="E2" s="100"/>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2039,15 +2091,15 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="73" t="s">
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="74"/>
+      <c r="E3" s="65"/>
       <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
@@ -2059,13 +2111,13 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="69"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="72"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2073,46 +2125,46 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="78" t="s">
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="80"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="88"/>
       <c r="Q5">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="66" t="s">
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="81"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="83"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="66" t="s">
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="81"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="83"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2122,12 +2174,12 @@
         <v>17</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="80"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="88"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
@@ -2137,12 +2189,12 @@
         <v>20</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="86"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="91"/>
     </row>
     <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
@@ -2152,12 +2204,12 @@
         <v>23</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="81"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="83"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
@@ -2167,35 +2219,35 @@
         <v>25</v>
       </c>
       <c r="C11" s="18"/>
-      <c r="D11" s="75" t="s">
+      <c r="D11" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="77"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="92"/>
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="20"/>
-      <c r="D12" s="78" t="s">
+      <c r="D12" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="79"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="80"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="88"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="75" t="s">
+      <c r="D13" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="77"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="92"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="24" t="s">
@@ -2207,10 +2259,10 @@
       <c r="C14" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="89" t="s">
+      <c r="D14" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="89"/>
+      <c r="E14" s="93"/>
       <c r="F14" s="25" t="s">
         <v>34</v>
       </c>
@@ -2449,37 +2501,37 @@
       <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="90" t="s">
+      <c r="A33" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="91"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="92"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="70"/>
     </row>
     <row r="34" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="91"/>
-      <c r="C34" s="91"/>
-      <c r="D34" s="91"/>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="92"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="70"/>
     </row>
     <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="68" t="s">
+      <c r="A35" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="69"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="93"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="73"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="33"/>
@@ -2498,62 +2550,62 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="94" t="s">
+      <c r="A37" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="95"/>
-      <c r="C37" s="95"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="95"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
       <c r="F37" s="36"/>
       <c r="G37" s="15"/>
     </row>
     <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="96" t="s">
+      <c r="A38" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="97"/>
-      <c r="C38" s="97"/>
-      <c r="D38" s="98" t="s">
+      <c r="B38" s="77"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="99"/>
-      <c r="F38" s="99"/>
-      <c r="G38" s="100"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="80"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="73" t="s">
+      <c r="A39" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="74"/>
-      <c r="C39" s="74"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="65"/>
       <c r="D39" s="8"/>
       <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="73" t="s">
+      <c r="A40" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="74"/>
-      <c r="C40" s="74"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
       <c r="D40" s="8"/>
       <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="73" t="s">
+      <c r="A41" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="74"/>
-      <c r="C41" s="74"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="65"/>
       <c r="D41" s="8"/>
       <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="75" t="s">
+      <c r="A42" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="76"/>
-      <c r="C42" s="76"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="67"/>
       <c r="D42" s="21"/>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
@@ -2561,26 +2613,26 @@
     </row>
     <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="44" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A44" s="70" t="s">
+      <c r="A44" s="98" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="70"/>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="70"/>
+      <c r="B44" s="98"/>
+      <c r="C44" s="98"/>
+      <c r="D44" s="98"/>
+      <c r="E44" s="98"/>
+      <c r="F44" s="98"/>
+      <c r="G44" s="98"/>
     </row>
     <row r="45" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="87" t="s">
+      <c r="A45" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="B45" s="88"/>
-      <c r="C45" s="88"/>
-      <c r="D45" s="87" t="s">
+      <c r="B45" s="97"/>
+      <c r="C45" s="97"/>
+      <c r="D45" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="E45" s="88"/>
+      <c r="E45" s="97"/>
       <c r="F45" s="1" t="s">
         <v>3</v>
       </c>
@@ -2589,15 +2641,15 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="66" t="s">
+      <c r="A46" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="67"/>
-      <c r="C46" s="67"/>
-      <c r="D46" s="73" t="s">
+      <c r="B46" s="82"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="E46" s="74"/>
+      <c r="E46" s="65"/>
       <c r="F46" s="6" t="s">
         <v>7</v>
       </c>
@@ -2606,54 +2658,54 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A47" s="75" t="s">
+      <c r="A47" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="77"/>
-      <c r="C47" s="67"/>
-      <c r="D47" s="68"/>
-      <c r="E47" s="69"/>
+      <c r="B47" s="92"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="72"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A48" s="101" t="s">
+      <c r="A48" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="102"/>
-      <c r="C48" s="102"/>
-      <c r="D48" s="78" t="s">
+      <c r="B48" s="95"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="E48" s="79"/>
-      <c r="F48" s="79"/>
-      <c r="G48" s="80"/>
+      <c r="E48" s="87"/>
+      <c r="F48" s="87"/>
+      <c r="G48" s="88"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A49" s="73" t="s">
+      <c r="A49" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B49" s="74"/>
-      <c r="C49" s="74"/>
-      <c r="D49" s="66" t="s">
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E49" s="67"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="81"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="83"/>
     </row>
     <row r="50" spans="1:16" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="82" t="s">
+      <c r="A50" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="83"/>
-      <c r="C50" s="83"/>
-      <c r="D50" s="66" t="s">
+      <c r="B50" s="85"/>
+      <c r="C50" s="85"/>
+      <c r="D50" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="E50" s="67"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="81"/>
+      <c r="E50" s="82"/>
+      <c r="F50" s="82"/>
+      <c r="G50" s="83"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" s="38" t="s">
@@ -2663,12 +2715,12 @@
         <v>68</v>
       </c>
       <c r="C51" s="9"/>
-      <c r="D51" s="78" t="s">
+      <c r="D51" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="E51" s="79"/>
-      <c r="F51" s="79"/>
-      <c r="G51" s="80"/>
+      <c r="E51" s="87"/>
+      <c r="F51" s="87"/>
+      <c r="G51" s="88"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" s="12" t="s">
@@ -2678,12 +2730,12 @@
         <v>71</v>
       </c>
       <c r="C52" s="9"/>
-      <c r="D52" s="84" t="s">
+      <c r="D52" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="E52" s="85"/>
-      <c r="F52" s="85"/>
-      <c r="G52" s="86"/>
+      <c r="E52" s="90"/>
+      <c r="F52" s="90"/>
+      <c r="G52" s="91"/>
     </row>
     <row r="53" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="38" t="s">
@@ -2693,12 +2745,12 @@
         <v>74</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="D53" s="66" t="s">
+      <c r="D53" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="E53" s="67"/>
-      <c r="F53" s="67"/>
-      <c r="G53" s="81"/>
+      <c r="E53" s="82"/>
+      <c r="F53" s="82"/>
+      <c r="G53" s="83"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A54" s="16" t="s">
@@ -2708,35 +2760,35 @@
         <v>76</v>
       </c>
       <c r="C54" s="18"/>
-      <c r="D54" s="75" t="s">
+      <c r="D54" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="E54" s="76"/>
-      <c r="F54" s="76"/>
-      <c r="G54" s="77"/>
+      <c r="E54" s="67"/>
+      <c r="F54" s="67"/>
+      <c r="G54" s="92"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C55" s="20"/>
-      <c r="D55" s="78" t="s">
+      <c r="D55" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="E55" s="79"/>
-      <c r="F55" s="79"/>
-      <c r="G55" s="80"/>
+      <c r="E55" s="87"/>
+      <c r="F55" s="87"/>
+      <c r="G55" s="88"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A56" s="21"/>
       <c r="B56" s="22"/>
       <c r="C56" s="23"/>
-      <c r="D56" s="75" t="s">
+      <c r="D56" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="E56" s="76"/>
-      <c r="F56" s="76"/>
-      <c r="G56" s="77"/>
+      <c r="E56" s="67"/>
+      <c r="F56" s="67"/>
+      <c r="G56" s="92"/>
     </row>
     <row r="57" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="24" t="s">
@@ -2748,10 +2800,10 @@
       <c r="C57" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="D57" s="89" t="s">
+      <c r="D57" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="E57" s="89"/>
+      <c r="E57" s="93"/>
       <c r="F57" s="25" t="s">
         <v>83</v>
       </c>
@@ -2932,37 +2984,37 @@
       <c r="G75" s="15"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A76" s="90" t="s">
+      <c r="A76" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="B76" s="91"/>
-      <c r="C76" s="91"/>
-      <c r="D76" s="91"/>
-      <c r="E76" s="91"/>
-      <c r="F76" s="91"/>
-      <c r="G76" s="92"/>
+      <c r="B76" s="69"/>
+      <c r="C76" s="69"/>
+      <c r="D76" s="69"/>
+      <c r="E76" s="69"/>
+      <c r="F76" s="69"/>
+      <c r="G76" s="70"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A77" s="90" t="s">
+      <c r="A77" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="B77" s="91"/>
-      <c r="C77" s="91"/>
-      <c r="D77" s="91"/>
-      <c r="E77" s="91"/>
-      <c r="F77" s="91"/>
-      <c r="G77" s="92"/>
+      <c r="B77" s="69"/>
+      <c r="C77" s="69"/>
+      <c r="D77" s="69"/>
+      <c r="E77" s="69"/>
+      <c r="F77" s="69"/>
+      <c r="G77" s="70"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A78" s="68" t="s">
+      <c r="A78" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="B78" s="69"/>
-      <c r="C78" s="69"/>
-      <c r="D78" s="69"/>
-      <c r="E78" s="69"/>
-      <c r="F78" s="69"/>
-      <c r="G78" s="93"/>
+      <c r="B78" s="72"/>
+      <c r="C78" s="72"/>
+      <c r="D78" s="72"/>
+      <c r="E78" s="72"/>
+      <c r="F78" s="72"/>
+      <c r="G78" s="73"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" s="33"/>
@@ -2981,62 +3033,62 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A80" s="94" t="s">
+      <c r="A80" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="B80" s="95"/>
-      <c r="C80" s="95"/>
-      <c r="D80" s="95"/>
-      <c r="E80" s="95"/>
+      <c r="B80" s="75"/>
+      <c r="C80" s="75"/>
+      <c r="D80" s="75"/>
+      <c r="E80" s="75"/>
       <c r="F80" s="36"/>
       <c r="G80" s="15"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A81" s="96" t="s">
+      <c r="A81" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="B81" s="97"/>
-      <c r="C81" s="97"/>
-      <c r="D81" s="98" t="s">
+      <c r="B81" s="77"/>
+      <c r="C81" s="77"/>
+      <c r="D81" s="78" t="s">
         <v>96</v>
       </c>
-      <c r="E81" s="99"/>
-      <c r="F81" s="99"/>
-      <c r="G81" s="100"/>
+      <c r="E81" s="79"/>
+      <c r="F81" s="79"/>
+      <c r="G81" s="80"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A82" s="73" t="s">
+      <c r="A82" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="B82" s="74"/>
-      <c r="C82" s="74"/>
+      <c r="B82" s="65"/>
+      <c r="C82" s="65"/>
       <c r="D82" s="8"/>
       <c r="G82" s="9"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A83" s="73" t="s">
+      <c r="A83" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="B83" s="74"/>
-      <c r="C83" s="74"/>
+      <c r="B83" s="65"/>
+      <c r="C83" s="65"/>
       <c r="D83" s="8"/>
       <c r="G83" s="9"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A84" s="73" t="s">
+      <c r="A84" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="B84" s="74"/>
-      <c r="C84" s="74"/>
+      <c r="B84" s="65"/>
+      <c r="C84" s="65"/>
       <c r="D84" s="8"/>
       <c r="G84" s="9"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A85" s="75" t="s">
+      <c r="A85" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="B85" s="76"/>
-      <c r="C85" s="76"/>
+      <c r="B85" s="67"/>
+      <c r="C85" s="67"/>
       <c r="D85" s="21"/>
       <c r="E85" s="22"/>
       <c r="F85" s="22"/>
@@ -3044,33 +3096,25 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A77:G77"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="A82:C82"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="D14:E14"/>
@@ -3085,25 +3129,33 @@
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="A44:G44"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A83:C83"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A77:G77"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="A82:C82"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>

</xml_diff>

<commit_message>
template fixes added, page print area fixed
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649204C6-553B-4D39-9E7E-EB86F06FA21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BEB227-A8F4-4C33-985D-237AA6D2C722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26783" yWindow="-98" windowWidth="28995" windowHeight="15796" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-28898" yWindow="1853" windowWidth="28996" windowHeight="15794" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -41,74 +41,74 @@
     <definedName name="Доставка_условия">Export_Contract!$A$23</definedName>
     <definedName name="Инвойс">Com_Invoice!$D$3</definedName>
     <definedName name="Инвойс_Bl">Com_Invoice!$A$15</definedName>
-    <definedName name="Инвойс_Bl_п">Com_Invoice!$A$58</definedName>
-    <definedName name="Инвойс_банк_получателя">Com_Invoice!$A$38</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес">Com_Invoice!$A$39</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес_п">Com_Invoice!$A$82</definedName>
-    <definedName name="Инвойс_банк_получателя_п">Com_Invoice!$A$81</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт">Com_Invoice!$A$40</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт_п">Com_Invoice!$A$83</definedName>
+    <definedName name="Инвойс_Bl_п">Com_Invoice!$A$80</definedName>
+    <definedName name="Инвойс_банк_получателя">Com_Invoice!$A$44</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес">Com_Invoice!$A$45</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес_п">Com_Invoice!$A$109</definedName>
+    <definedName name="Инвойс_банк_получателя_п">Com_Invoice!$A$108</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт">Com_Invoice!$A$46</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт_п">Com_Invoice!$A$110</definedName>
     <definedName name="Инвойс_всего">Com_Invoice!$E$15</definedName>
-    <definedName name="Инвойс_всего_п">Com_Invoice!$E$58</definedName>
-    <definedName name="Инвойс_дата_п">Com_Invoice!$A$52</definedName>
+    <definedName name="Инвойс_всего_п">Com_Invoice!$E$80</definedName>
+    <definedName name="Инвойс_дата_п">Com_Invoice!$A$74</definedName>
     <definedName name="Инвойс_контракт">Com_Invoice!$D$10</definedName>
     <definedName name="Инвойс_контракт_дата">Com_Invoice!$D$11</definedName>
-    <definedName name="Инвойс_контракт_дата_п">Com_Invoice!$D$54</definedName>
-    <definedName name="Инвойс_контракт_п">Com_Invoice!$D$53</definedName>
+    <definedName name="Инвойс_контракт_дата_п">Com_Invoice!$D$76</definedName>
+    <definedName name="Инвойс_контракт_п">Com_Invoice!$D$75</definedName>
     <definedName name="Инвойс_куда">Com_Invoice!$A$11</definedName>
-    <definedName name="Инвойс_куда_п">Com_Invoice!$A$54</definedName>
+    <definedName name="Инвойс_куда_п">Com_Invoice!$A$76</definedName>
     <definedName name="Инвойс_места">Com_Invoice!$D$15</definedName>
-    <definedName name="Инвойс_места_п">Com_Invoice!$D$58</definedName>
+    <definedName name="Инвойс_места_п">Com_Invoice!$D$80</definedName>
     <definedName name="Инвойс_откуда">Com_Invoice!$B$11</definedName>
-    <definedName name="Инвойс_откуда_п">Com_Invoice!$B$54</definedName>
-    <definedName name="Инвойс_п">Com_Invoice!$D$46</definedName>
-    <definedName name="Инвойс_подвал_всего">Com_Invoice!$D$36</definedName>
-    <definedName name="Инвойс_подвал_всего_п">Com_Invoice!$D$79</definedName>
-    <definedName name="Инвойс_подвал_места">Com_Invoice!$C$36</definedName>
-    <definedName name="Инвойс_подвал_места_п">Com_Invoice!$C$79</definedName>
-    <definedName name="Инвойс_подвал_сумма">Com_Invoice!$G$36</definedName>
-    <definedName name="Инвойс_подвал_сумма_п">Com_Invoice!$G$79</definedName>
-    <definedName name="Инвойс_подписант">Com_Invoice!$D$38</definedName>
-    <definedName name="Инвойс_подписант_п">Com_Invoice!$D$81</definedName>
+    <definedName name="Инвойс_откуда_п">Com_Invoice!$B$76</definedName>
+    <definedName name="Инвойс_п">Com_Invoice!$D$68</definedName>
+    <definedName name="Инвойс_подвал_всего">Com_Invoice!$D$42</definedName>
+    <definedName name="Инвойс_подвал_всего_п">Com_Invoice!$D$106</definedName>
+    <definedName name="Инвойс_подвал_места">Com_Invoice!$C$42</definedName>
+    <definedName name="Инвойс_подвал_места_п">Com_Invoice!$C$106</definedName>
+    <definedName name="Инвойс_подвал_сумма">Com_Invoice!$G$42</definedName>
+    <definedName name="Инвойс_подвал_сумма_п">Com_Invoice!$G$106</definedName>
+    <definedName name="Инвойс_подписант">Com_Invoice!$D$44</definedName>
+    <definedName name="Инвойс_подписант_п">Com_Invoice!$D$108</definedName>
     <definedName name="Инвойс_покупатель">Com_Invoice!$D$6</definedName>
     <definedName name="Инвойс_покупатель_адрес">Com_Invoice!$D$7</definedName>
-    <definedName name="Инвойс_покупатель_адрес_п">Com_Invoice!$D$50</definedName>
-    <definedName name="Инвойс_покупатель_п">Com_Invoice!$D$49</definedName>
+    <definedName name="Инвойс_покупатель_адрес_п">Com_Invoice!$D$72</definedName>
+    <definedName name="Инвойс_покупатель_п">Com_Invoice!$D$71</definedName>
     <definedName name="Инвойс_получатель">Com_Invoice!$A$6</definedName>
     <definedName name="Инвойс_получатель_адрес">Com_Invoice!$A$7</definedName>
-    <definedName name="Инвойс_получатель_адрес_п">Com_Invoice!$A$50</definedName>
-    <definedName name="Инвойс_получатель_в_пользу">Com_Invoice!$A$41</definedName>
-    <definedName name="Инвойс_получатель_в_пользу_п">Com_Invoice!$A$84</definedName>
-    <definedName name="Инвойс_получатель_п">Com_Invoice!$A$49</definedName>
-    <definedName name="Инвойс_получатель_счет">Com_Invoice!$A$42</definedName>
-    <definedName name="Инвойс_получатель_счет_п">Com_Invoice!$A$85</definedName>
+    <definedName name="Инвойс_получатель_адрес_п">Com_Invoice!$A$72</definedName>
+    <definedName name="Инвойс_получатель_в_пользу">Com_Invoice!$A$47</definedName>
+    <definedName name="Инвойс_получатель_в_пользу_п">Com_Invoice!$A$111</definedName>
+    <definedName name="Инвойс_получатель_п">Com_Invoice!$A$71</definedName>
+    <definedName name="Инвойс_получатель_счет">Com_Invoice!$A$48</definedName>
+    <definedName name="Инвойс_получатель_счет_п">Com_Invoice!$A$112</definedName>
     <definedName name="Инвойс_продавец">Com_Invoice!$A$3</definedName>
     <definedName name="Инвойс_продавец_адрес">Com_Invoice!$A$4</definedName>
-    <definedName name="Инвойс_продавец_адрес_п">Com_Invoice!$A$47</definedName>
-    <definedName name="Инвойс_продавец_п">Com_Invoice!$A$46</definedName>
+    <definedName name="Инвойс_продавец_адрес_п">Com_Invoice!$A$69</definedName>
+    <definedName name="Инвойс_продавец_п">Com_Invoice!$A$68</definedName>
     <definedName name="Инвойс_продукт">Com_Invoice!$B$15</definedName>
-    <definedName name="Инвойс_продукт_п">Com_Invoice!$B$58</definedName>
+    <definedName name="Инвойс_продукт_п">Com_Invoice!$B$80</definedName>
     <definedName name="Инвойс_соглашение">Com_Invoice!$D$9</definedName>
-    <definedName name="Инвойс_соглашение_п">Com_Invoice!$D$52</definedName>
-    <definedName name="Инвойс_судно">Com_Invoice!$A$33</definedName>
-    <definedName name="Инвойс_судно_п">Com_Invoice!$A$76</definedName>
+    <definedName name="Инвойс_соглашение_п">Com_Invoice!$D$74</definedName>
+    <definedName name="Инвойс_судно">Com_Invoice!$A$39</definedName>
+    <definedName name="Инвойс_судно_п">Com_Invoice!$A$103</definedName>
     <definedName name="Инвойс_сумма">Com_Invoice!$G$15</definedName>
-    <definedName name="Инвойс_сумма_п">Com_Invoice!$G$58</definedName>
+    <definedName name="Инвойс_сумма_п">Com_Invoice!$G$80</definedName>
     <definedName name="Инвойс_транспорт">Com_Invoice!$B$9</definedName>
-    <definedName name="Инвойс_транспорт_п">Com_Invoice!$B$52</definedName>
+    <definedName name="Инвойс_транспорт_п">Com_Invoice!$B$74</definedName>
     <definedName name="Инвойс_упаковка">Com_Invoice!$C$15</definedName>
-    <definedName name="Инвойс_упаковка_п">Com_Invoice!$C$58</definedName>
+    <definedName name="Инвойс_упаковка_п">Com_Invoice!$C$80</definedName>
     <definedName name="Инвойс_условия">Com_Invoice!$D$13</definedName>
-    <definedName name="Инвойс_условия_п">Com_Invoice!$D$56</definedName>
+    <definedName name="Инвойс_условия_п">Com_Invoice!$D$78</definedName>
     <definedName name="Инвойс_цена">Com_Invoice!$F$15</definedName>
-    <definedName name="Инвойс_цена_п">Com_Invoice!$F$58</definedName>
+    <definedName name="Инвойс_цена_п">Com_Invoice!$F$80</definedName>
     <definedName name="Иновйс_дата">Com_Invoice!$A$9</definedName>
     <definedName name="Контракт">Export_Contract!$A$2</definedName>
     <definedName name="Контракт_дата">Export_Contract!$A$3</definedName>
     <definedName name="МСЦ">Com_Invoice!$F$3</definedName>
-    <definedName name="МСЦ_п">Com_Invoice!$F$46</definedName>
+    <definedName name="МСЦ_п">Com_Invoice!$F$68</definedName>
     <definedName name="МСЦ_сертификат">Com_Invoice!$G$3</definedName>
-    <definedName name="МСЦ_сертификат_п">Com_Invoice!$G$46</definedName>
+    <definedName name="МСЦ_сертификат_п">Com_Invoice!$G$68</definedName>
     <definedName name="Покупатель">Export_Contract!$A$11</definedName>
     <definedName name="Покупатель_адрес">Export_Contract!$A$12</definedName>
     <definedName name="Покупатель_заголовок">Export_Contract!$A$10</definedName>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="171">
   <si>
     <t>COMMERCIAL INVOICE</t>
   </si>
@@ -670,16 +670,20 @@
   </si>
   <si>
     <t>* MSC Frozen Alaska Pollock Milts  - 9,585 tn (net weight)</t>
+  </si>
+  <si>
+    <t>ROOM 1105, NOBLIAN 2, 80, JUNGANG-DAERO, JUNG-GU, BUSAN, KOREA Manysdfjsdlfjkalsdfsad;fjskldafj;sdlfakldfksa;flksdklf;js</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="[$-FC19]d\ mmmm\ yyyy\ &quot;г.&quot;"/>
     <numFmt numFmtId="166" formatCode="#,##0.000#"/>
+    <numFmt numFmtId="167" formatCode="\ &quot;@* &quot;\ "/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -763,7 +767,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -965,7 +969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1060,12 +1064,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1125,125 +1123,198 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1561,11 +1632,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B05EB69-7436-401E-967C-BE559ABF33B1}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="151" zoomScaleNormal="100" zoomScaleSheetLayoutView="151" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="81" zoomScaleNormal="100" zoomScaleSheetLayoutView="81" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1586,10 +1658,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="44" t="s">
         <v>98</v>
       </c>
       <c r="D1" s="3"/>
@@ -1598,10 +1670,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="46" t="s">
         <v>100</v>
       </c>
       <c r="D2" s="3"/>
@@ -1610,13 +1682,13 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="H3" s="49"/>
+      <c r="H3" s="47"/>
       <c r="N3" t="s">
         <v>103</v>
       </c>
@@ -1625,7 +1697,7 @@
       <c r="A4" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="48" t="s">
         <v>105</v>
       </c>
       <c r="N4" t="s">
@@ -1633,10 +1705,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="50" t="s">
         <v>108</v>
       </c>
       <c r="D5" s="3"/>
@@ -1645,7 +1717,7 @@
       <c r="A6" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="51" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1653,7 +1725,7 @@
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="48" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1661,7 +1733,7 @@
       <c r="A8" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="48" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1669,15 +1741,15 @@
       <c r="A9" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="48" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="50" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1685,7 +1757,7 @@
       <c r="A11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="51" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1693,7 +1765,7 @@
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="48" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1701,7 +1773,7 @@
       <c r="A13" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="48" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1709,15 +1781,15 @@
       <c r="A14" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="48" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="54" t="s">
+    <row r="15" spans="1:14" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="53" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1725,7 +1797,7 @@
       <c r="A16" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="48" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1733,10 +1805,10 @@
       <c r="A17" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="M17" s="57"/>
+      <c r="M17" s="55"/>
       <c r="N17" t="s">
         <v>37</v>
       </c>
@@ -1749,7 +1821,7 @@
       <c r="Q17" t="s">
         <v>27</v>
       </c>
-      <c r="R17" s="58">
+      <c r="R17" s="56">
         <v>9.5850000000000009</v>
       </c>
       <c r="S17">
@@ -1762,11 +1834,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="54" t="s">
+    <row r="18" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="B18" s="55" t="s">
+      <c r="B18" s="53" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1774,7 +1846,7 @@
       <c r="A19" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="48" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1782,7 +1854,7 @@
       <c r="A20" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="54" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1790,15 +1862,15 @@
       <c r="A21" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="48" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="54" t="s">
+    <row r="22" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="52" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1806,7 +1878,7 @@
       <c r="A23" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="48" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1814,31 +1886,31 @@
       <c r="A24" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="48" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="61" t="s">
+      <c r="A25" s="123" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="123" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="55.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="62" t="s">
+      <c r="A26" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="63" t="s">
+      <c r="B26" s="60" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="54" t="s">
+    <row r="27" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="52" t="s">
         <v>138</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="53" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1846,15 +1918,15 @@
       <c r="A28" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="48" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="54" t="s">
+    <row r="29" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="53" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1862,7 +1934,7 @@
       <c r="A30" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B30" s="53" t="s">
+      <c r="B30" s="51" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1870,7 +1942,7 @@
       <c r="A31" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="53" t="s">
+      <c r="B31" s="51" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1878,7 +1950,7 @@
       <c r="A32" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="50" t="s">
+      <c r="B32" s="48" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1886,7 +1958,7 @@
       <c r="A33" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="48" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1894,7 +1966,7 @@
       <c r="A34" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="48" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1902,7 +1974,7 @@
       <c r="A35" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="48" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1910,7 +1982,7 @@
       <c r="A36" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="50" t="s">
+      <c r="B36" s="48" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1918,7 +1990,7 @@
       <c r="A37" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B37" s="50" t="s">
+      <c r="B37" s="48" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1926,7 +1998,7 @@
       <c r="A38" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="48" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1934,7 +2006,7 @@
       <c r="A39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="50" t="s">
+      <c r="B39" s="48" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1942,7 +2014,7 @@
       <c r="A40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="48" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1950,7 +2022,7 @@
       <c r="A41" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="48" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1958,7 +2030,7 @@
       <c r="A42" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B42" s="50" t="s">
+      <c r="B42" s="48" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1966,7 +2038,7 @@
       <c r="A43" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B43" s="50" t="s">
+      <c r="B43" s="48" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1974,7 +2046,7 @@
       <c r="A44" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="48" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1982,7 +2054,7 @@
       <c r="A45" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="48" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1990,15 +2062,15 @@
       <c r="A46" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="B46" s="59" t="s">
+      <c r="B46" s="57" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="60" t="s">
+      <c r="A47" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="B47" s="60" t="s">
+      <c r="B47" s="58" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2023,7 +2095,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.11811023622047245" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="84" orientation="portrait" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="2" max="1048575" man="1"/>
   </colBreaks>
@@ -2034,11 +2106,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F42404-E30B-43BB-827E-C2B73C5861E4}">
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z85"/>
+  <dimension ref="A1:Z112"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A31" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView view="pageBreakPreview" zoomScale="78" zoomScaleNormal="70" zoomScaleSheetLayoutView="78" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2059,27 +2132,27 @@
     <col min="24" max="27" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="98" t="s">
+    <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="99" t="s">
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="100"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2091,15 +2164,15 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="64" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="65"/>
+      <c r="E3" s="76"/>
       <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
@@ -2111,13 +2184,13 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="72"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="113"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2125,46 +2198,46 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="86" t="s">
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="88"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="68"/>
       <c r="Q5">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="81" t="s">
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="83"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="69"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="84" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="81" t="s">
+      <c r="A7" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="107"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="109" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="83"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="111"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2174,12 +2247,12 @@
         <v>17</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="86" t="s">
+      <c r="D8" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="88"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="68"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
@@ -2189,12 +2262,12 @@
         <v>20</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="89" t="s">
+      <c r="D9" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="91"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="75"/>
     </row>
     <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
@@ -2204,12 +2277,12 @@
         <v>23</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="81" t="s">
+      <c r="D10" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="83"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="69"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
@@ -2219,35 +2292,35 @@
         <v>25</v>
       </c>
       <c r="C11" s="18"/>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="92"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="72"/>
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="20"/>
-      <c r="D12" s="86" t="s">
+      <c r="D12" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="88"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="68"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="66" t="s">
+      <c r="D13" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="92"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="105"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="24" t="s">
@@ -2259,10 +2332,10 @@
       <c r="C14" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="93" t="s">
+      <c r="D14" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="93"/>
+      <c r="E14" s="99"/>
       <c r="F14" s="25" t="s">
         <v>34</v>
       </c>
@@ -2424,9 +2497,6 @@
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
       <c r="G24" s="7"/>
-      <c r="Q24">
-        <v>33547.5</v>
-      </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A25" s="6"/>
@@ -2481,6 +2551,9 @@
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
       <c r="G30" s="7"/>
+      <c r="Q30">
+        <v>33547.5</v>
+      </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A31" s="6"/>
@@ -2497,671 +2570,861 @@
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="32"/>
-    </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="68" t="s">
+      <c r="F32" s="27"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="6"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="6"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="6"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" s="6"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="6"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="6"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="32"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="70"/>
-    </row>
-    <row r="34" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="68" t="s">
+      <c r="B39" s="97"/>
+      <c r="C39" s="97"/>
+      <c r="D39" s="97"/>
+      <c r="E39" s="97"/>
+      <c r="F39" s="97"/>
+      <c r="G39" s="98"/>
+    </row>
+    <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="96" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="70"/>
-    </row>
-    <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="71" t="s">
+      <c r="B40" s="97"/>
+      <c r="C40" s="97"/>
+      <c r="D40" s="97"/>
+      <c r="E40" s="97"/>
+      <c r="F40" s="97"/>
+      <c r="G40" s="98"/>
+    </row>
+    <row r="41" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="73"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" s="33"/>
-      <c r="B36" s="34" t="s">
+      <c r="B41" s="94"/>
+      <c r="C41" s="94"/>
+      <c r="D41" s="94"/>
+      <c r="E41" s="94"/>
+      <c r="F41" s="94"/>
+      <c r="G41" s="95"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="33"/>
+      <c r="B42" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C42" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D42" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F36" s="36"/>
-      <c r="G36" s="37" t="s">
+      <c r="F42" s="36"/>
+      <c r="G42" s="37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="74" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="15"/>
-    </row>
-    <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="76" t="s">
+      <c r="B43" s="117"/>
+      <c r="C43" s="117"/>
+      <c r="D43" s="117"/>
+      <c r="E43" s="117"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="15"/>
+    </row>
+    <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="78" t="s">
+      <c r="B44" s="78"/>
+      <c r="C44" s="78"/>
+      <c r="D44" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="79"/>
-      <c r="F38" s="79"/>
-      <c r="G38" s="80"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="64" t="s">
+      <c r="E44" s="80"/>
+      <c r="F44" s="80"/>
+      <c r="G44" s="81"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="65"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="8"/>
-      <c r="G39" s="9"/>
-    </row>
-    <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="64" t="s">
+      <c r="B45" s="76"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="8"/>
+      <c r="G45" s="9"/>
+    </row>
+    <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="8"/>
-      <c r="G40" s="9"/>
-    </row>
-    <row r="41" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="64" t="s">
+      <c r="B46" s="76"/>
+      <c r="C46" s="76"/>
+      <c r="D46" s="8"/>
+      <c r="G46" s="9"/>
+    </row>
+    <row r="47" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="65"/>
-      <c r="C41" s="65"/>
-      <c r="D41" s="8"/>
-      <c r="G41" s="9"/>
-    </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="66" t="s">
+      <c r="B47" s="76"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="8"/>
+      <c r="G47" s="9"/>
+    </row>
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="67"/>
-      <c r="C42" s="67"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="18"/>
-    </row>
-    <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="44" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A44" s="98" t="s">
+      <c r="B48" s="71"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="18"/>
+    </row>
+    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="121"/>
+      <c r="B49" s="121"/>
+      <c r="C49" s="121"/>
+      <c r="D49" s="122"/>
+      <c r="E49" s="122"/>
+      <c r="F49" s="122"/>
+      <c r="G49" s="122"/>
+    </row>
+    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="121"/>
+      <c r="B50" s="121"/>
+      <c r="C50" s="121"/>
+      <c r="D50" s="122"/>
+      <c r="E50" s="122"/>
+      <c r="F50" s="122"/>
+      <c r="G50" s="122"/>
+    </row>
+    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="121"/>
+      <c r="B51" s="121"/>
+      <c r="C51" s="121"/>
+      <c r="D51" s="122"/>
+      <c r="E51" s="122"/>
+      <c r="F51" s="122"/>
+      <c r="G51" s="122"/>
+    </row>
+    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="121"/>
+      <c r="B52" s="121"/>
+      <c r="C52" s="121"/>
+      <c r="D52" s="122"/>
+      <c r="E52" s="122"/>
+      <c r="F52" s="122"/>
+      <c r="G52" s="122"/>
+    </row>
+    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="121"/>
+      <c r="B53" s="121"/>
+      <c r="C53" s="121"/>
+      <c r="D53" s="122"/>
+      <c r="E53" s="122"/>
+      <c r="F53" s="122"/>
+      <c r="G53" s="122"/>
+    </row>
+    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="121"/>
+      <c r="B54" s="121"/>
+      <c r="C54" s="121"/>
+      <c r="D54" s="122"/>
+      <c r="E54" s="122"/>
+      <c r="F54" s="122"/>
+      <c r="G54" s="122"/>
+    </row>
+    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="121"/>
+      <c r="B55" s="121"/>
+      <c r="C55" s="121"/>
+      <c r="D55" s="122"/>
+      <c r="E55" s="122"/>
+      <c r="F55" s="122"/>
+      <c r="G55" s="122"/>
+    </row>
+    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="121"/>
+      <c r="B56" s="121"/>
+      <c r="C56" s="121"/>
+      <c r="D56" s="122"/>
+      <c r="E56" s="122"/>
+      <c r="F56" s="122"/>
+      <c r="G56" s="122"/>
+    </row>
+    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="121"/>
+      <c r="B57" s="121"/>
+      <c r="C57" s="121"/>
+      <c r="D57" s="122"/>
+      <c r="E57" s="122"/>
+      <c r="F57" s="122"/>
+      <c r="G57" s="122"/>
+    </row>
+    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="121"/>
+      <c r="B58" s="121"/>
+      <c r="C58" s="121"/>
+      <c r="D58" s="122"/>
+      <c r="E58" s="122"/>
+      <c r="F58" s="122"/>
+      <c r="G58" s="122"/>
+    </row>
+    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="121"/>
+      <c r="B59" s="121"/>
+      <c r="C59" s="121"/>
+      <c r="D59" s="122"/>
+      <c r="E59" s="122"/>
+      <c r="F59" s="122"/>
+      <c r="G59" s="122"/>
+    </row>
+    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="121"/>
+      <c r="B60" s="121"/>
+      <c r="C60" s="121"/>
+      <c r="D60" s="122"/>
+      <c r="E60" s="122"/>
+      <c r="F60" s="122"/>
+      <c r="G60" s="122"/>
+    </row>
+    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="121"/>
+      <c r="B61" s="121"/>
+      <c r="C61" s="121"/>
+      <c r="D61" s="122"/>
+      <c r="E61" s="122"/>
+      <c r="F61" s="122"/>
+      <c r="G61" s="122"/>
+    </row>
+    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="121"/>
+      <c r="B62" s="121"/>
+      <c r="C62" s="121"/>
+      <c r="D62" s="122"/>
+      <c r="E62" s="122"/>
+      <c r="F62" s="122"/>
+      <c r="G62" s="122"/>
+    </row>
+    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="121"/>
+      <c r="B63" s="121"/>
+      <c r="C63" s="121"/>
+      <c r="D63" s="122"/>
+      <c r="E63" s="122"/>
+      <c r="F63" s="122"/>
+      <c r="G63" s="122"/>
+    </row>
+    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="121"/>
+      <c r="B64" s="121"/>
+      <c r="C64" s="121"/>
+      <c r="D64" s="122"/>
+      <c r="E64" s="122"/>
+      <c r="F64" s="122"/>
+      <c r="G64" s="122"/>
+    </row>
+    <row r="65" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="66" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A66" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="98"/>
-      <c r="C44" s="98"/>
-      <c r="D44" s="98"/>
-      <c r="E44" s="98"/>
-      <c r="F44" s="98"/>
-      <c r="G44" s="98"/>
-    </row>
-    <row r="45" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="96" t="s">
+      <c r="B66" s="83"/>
+      <c r="C66" s="83"/>
+      <c r="D66" s="83"/>
+      <c r="E66" s="83"/>
+      <c r="F66" s="83"/>
+      <c r="G66" s="83"/>
+    </row>
+    <row r="67" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A67" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="B45" s="97"/>
-      <c r="C45" s="97"/>
-      <c r="D45" s="96" t="s">
+      <c r="B67" s="85"/>
+      <c r="C67" s="85"/>
+      <c r="D67" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="E45" s="97"/>
-      <c r="F45" s="1" t="s">
+      <c r="E67" s="85"/>
+      <c r="F67" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="81" t="s">
+    <row r="68" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A68" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="82"/>
-      <c r="C46" s="82"/>
-      <c r="D46" s="64" t="s">
+      <c r="B68" s="62"/>
+      <c r="C68" s="62"/>
+      <c r="D68" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="E46" s="65"/>
-      <c r="F46" s="6" t="s">
+      <c r="E68" s="76"/>
+      <c r="F68" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G46" s="7" t="s">
+      <c r="G68" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A47" s="66" t="s">
+    <row r="69" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="92"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="9"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A48" s="94" t="s">
+      <c r="B69" s="71"/>
+      <c r="C69" s="62"/>
+      <c r="D69" s="112"/>
+      <c r="E69" s="113"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="9"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A70" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="95"/>
-      <c r="C48" s="95"/>
-      <c r="D48" s="86" t="s">
+      <c r="B70" s="85"/>
+      <c r="C70" s="87"/>
+      <c r="D70" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="E48" s="87"/>
-      <c r="F48" s="87"/>
-      <c r="G48" s="88"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A49" s="64" t="s">
+      <c r="E70" s="67"/>
+      <c r="F70" s="67"/>
+      <c r="G70" s="68"/>
+    </row>
+    <row r="71" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A71" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B49" s="65"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="81" t="s">
+      <c r="B71" s="76"/>
+      <c r="C71" s="76"/>
+      <c r="D71" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="E49" s="82"/>
-      <c r="F49" s="82"/>
-      <c r="G49" s="83"/>
-    </row>
-    <row r="50" spans="1:16" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="84" t="s">
+      <c r="E71" s="62"/>
+      <c r="F71" s="62"/>
+      <c r="G71" s="69"/>
+    </row>
+    <row r="72" spans="1:7" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A72" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="85"/>
-      <c r="C50" s="85"/>
-      <c r="D50" s="81" t="s">
+      <c r="B72" s="110"/>
+      <c r="C72" s="110"/>
+      <c r="D72" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="E50" s="82"/>
-      <c r="F50" s="82"/>
-      <c r="G50" s="83"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A51" s="38" t="s">
+      <c r="E72" s="119"/>
+      <c r="F72" s="119"/>
+      <c r="G72" s="120"/>
+    </row>
+    <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A73" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B73" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="86" t="s">
+      <c r="C73" s="9"/>
+      <c r="D73" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="E51" s="87"/>
-      <c r="F51" s="87"/>
-      <c r="G51" s="88"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A52" s="12" t="s">
+      <c r="E73" s="67"/>
+      <c r="F73" s="67"/>
+      <c r="G73" s="68"/>
+    </row>
+    <row r="74" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A74" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B74" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="89" t="s">
+      <c r="C74" s="9"/>
+      <c r="D74" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="E52" s="90"/>
-      <c r="F52" s="90"/>
-      <c r="G52" s="91"/>
-    </row>
-    <row r="53" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="38" t="s">
+      <c r="E74" s="74"/>
+      <c r="F74" s="74"/>
+      <c r="G74" s="75"/>
+    </row>
+    <row r="75" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A75" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="39" t="s">
+      <c r="B75" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="81" t="s">
+      <c r="C75" s="15"/>
+      <c r="D75" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="E53" s="82"/>
-      <c r="F53" s="82"/>
-      <c r="G53" s="83"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A54" s="16" t="s">
+      <c r="E75" s="62"/>
+      <c r="F75" s="62"/>
+      <c r="G75" s="69"/>
+    </row>
+    <row r="76" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A76" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B76" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="C54" s="18"/>
-      <c r="D54" s="66" t="s">
+      <c r="C76" s="18"/>
+      <c r="D76" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="E54" s="67"/>
-      <c r="F54" s="67"/>
-      <c r="G54" s="92"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A55" s="8" t="s">
+      <c r="E76" s="71"/>
+      <c r="F76" s="71"/>
+      <c r="G76" s="72"/>
+    </row>
+    <row r="77" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A77" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="20"/>
-      <c r="D55" s="86" t="s">
+      <c r="C77" s="20"/>
+      <c r="D77" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="E55" s="87"/>
-      <c r="F55" s="87"/>
-      <c r="G55" s="88"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A56" s="21"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="66" t="s">
+      <c r="E77" s="67"/>
+      <c r="F77" s="67"/>
+      <c r="G77" s="68"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A78" s="21"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="23"/>
+      <c r="D78" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="E56" s="67"/>
-      <c r="F56" s="67"/>
-      <c r="G56" s="92"/>
-    </row>
-    <row r="57" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="24" t="s">
+      <c r="E78" s="71"/>
+      <c r="F78" s="71"/>
+      <c r="G78" s="72"/>
+    </row>
+    <row r="79" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A79" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B57" s="25" t="s">
+      <c r="B79" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="C57" s="40" t="s">
+      <c r="C79" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D57" s="93" t="s">
+      <c r="D79" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="E57" s="93"/>
-      <c r="F57" s="25" t="s">
+      <c r="E79" s="92"/>
+      <c r="F79" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="G57" s="26" t="s">
+      <c r="G79" s="26" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A58" s="6" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A80" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B58" s="27" t="s">
+      <c r="B80" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C58" s="27" t="s">
+      <c r="C80" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="D58" s="27" t="s">
+      <c r="D80" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="E58" s="27" t="s">
+      <c r="E80" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="F58" s="27" t="s">
+      <c r="F80" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G58" s="7" t="s">
+      <c r="G80" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A59" s="41"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="42"/>
-    </row>
-    <row r="60" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="6"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
-      <c r="G60" s="7"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A61" s="6"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="7"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A62" s="6"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="7"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="7"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A64" s="6"/>
-      <c r="B64" s="27"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="7"/>
-      <c r="P64" s="43"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A65" s="6"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="7"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A66" s="6"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="7"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A67" s="6"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="7"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A68" s="6"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="7"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A69" s="6"/>
-      <c r="B69" s="27"/>
-      <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="27"/>
-      <c r="G69" s="7"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A70" s="6"/>
-      <c r="B70" s="27"/>
-      <c r="C70" s="27"/>
-      <c r="D70" s="27"/>
-      <c r="F70" s="27"/>
-      <c r="G70" s="7"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A71" s="6"/>
-      <c r="B71" s="27"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="27"/>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="7"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A72" s="6"/>
-      <c r="B72" s="27"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="7"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A73" s="6"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="7"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A74" s="6"/>
-      <c r="B74" s="27"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="27"/>
-      <c r="F74" s="27"/>
-      <c r="G74" s="7"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A75" s="12"/>
-      <c r="B75" s="44"/>
-      <c r="C75" s="44"/>
-      <c r="D75" s="44"/>
-      <c r="E75" s="44"/>
-      <c r="F75" s="36"/>
-      <c r="G75" s="15"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A76" s="68" t="s">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A81" s="39"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="40"/>
+    </row>
+    <row r="82" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A82" s="6"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="27"/>
+      <c r="E82" s="27"/>
+      <c r="F82" s="27"/>
+      <c r="G82" s="7"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A83" s="6"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
+      <c r="E83" s="27"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="7"/>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A84" s="6"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="27"/>
+      <c r="D84" s="27"/>
+      <c r="E84" s="27"/>
+      <c r="F84" s="27"/>
+      <c r="G84" s="7"/>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="E85" s="27"/>
+      <c r="F85" s="27"/>
+      <c r="G85" s="7"/>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A86" s="6"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="27"/>
+      <c r="D86" s="27"/>
+      <c r="E86" s="27"/>
+      <c r="F86" s="27"/>
+      <c r="G86" s="7"/>
+      <c r="P86" s="41"/>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A87" s="6"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="27"/>
+      <c r="D87" s="27"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="7"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A88" s="6"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="27"/>
+      <c r="G88" s="7"/>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A89" s="6"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
+      <c r="E89" s="27"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="7"/>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A90" s="6"/>
+      <c r="B90" s="27"/>
+      <c r="C90" s="27"/>
+      <c r="D90" s="27"/>
+      <c r="E90" s="27"/>
+      <c r="F90" s="27"/>
+      <c r="G90" s="7"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A91" s="6"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
+      <c r="E91" s="27"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="7"/>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A92" s="6"/>
+      <c r="B92" s="27"/>
+      <c r="C92" s="27"/>
+      <c r="D92" s="27"/>
+      <c r="E92" s="27"/>
+      <c r="F92" s="27"/>
+      <c r="G92" s="7"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A93" s="6"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
+      <c r="E93" s="27"/>
+      <c r="F93" s="27"/>
+      <c r="G93" s="7"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A94" s="6"/>
+      <c r="B94" s="27"/>
+      <c r="C94" s="27"/>
+      <c r="D94" s="27"/>
+      <c r="E94" s="27"/>
+      <c r="F94" s="27"/>
+      <c r="G94" s="7"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A95" s="6"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="27"/>
+      <c r="D95" s="27"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="27"/>
+      <c r="G95" s="7"/>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A96" s="6"/>
+      <c r="B96" s="27"/>
+      <c r="C96" s="27"/>
+      <c r="D96" s="27"/>
+      <c r="E96" s="27"/>
+      <c r="F96" s="27"/>
+      <c r="G96" s="7"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A97" s="6"/>
+      <c r="B97" s="27"/>
+      <c r="C97" s="27"/>
+      <c r="D97" s="27"/>
+      <c r="F97" s="27"/>
+      <c r="G97" s="7"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A98" s="6"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="27"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="27"/>
+      <c r="G98" s="7"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A99" s="6"/>
+      <c r="B99" s="27"/>
+      <c r="C99" s="27"/>
+      <c r="D99" s="27"/>
+      <c r="E99" s="27"/>
+      <c r="F99" s="27"/>
+      <c r="G99" s="7"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A100" s="6"/>
+      <c r="B100" s="27"/>
+      <c r="C100" s="27"/>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="7"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A101" s="6"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
+      <c r="D101" s="27"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="27"/>
+      <c r="G101" s="7"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A102" s="12"/>
+      <c r="B102" s="42"/>
+      <c r="C102" s="42"/>
+      <c r="D102" s="42"/>
+      <c r="E102" s="42"/>
+      <c r="F102" s="36"/>
+      <c r="G102" s="15"/>
+    </row>
+    <row r="103" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A103" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="B76" s="69"/>
-      <c r="C76" s="69"/>
-      <c r="D76" s="69"/>
-      <c r="E76" s="69"/>
-      <c r="F76" s="69"/>
-      <c r="G76" s="70"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A77" s="68" t="s">
+      <c r="B103" s="101"/>
+      <c r="C103" s="101"/>
+      <c r="D103" s="101"/>
+      <c r="E103" s="101"/>
+      <c r="F103" s="101"/>
+      <c r="G103" s="102"/>
+    </row>
+    <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A104" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="B77" s="69"/>
-      <c r="C77" s="69"/>
-      <c r="D77" s="69"/>
-      <c r="E77" s="69"/>
-      <c r="F77" s="69"/>
-      <c r="G77" s="70"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A78" s="71" t="s">
+      <c r="B104" s="101"/>
+      <c r="C104" s="101"/>
+      <c r="D104" s="101"/>
+      <c r="E104" s="101"/>
+      <c r="F104" s="101"/>
+      <c r="G104" s="102"/>
+    </row>
+    <row r="105" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A105" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B78" s="72"/>
-      <c r="C78" s="72"/>
-      <c r="D78" s="72"/>
-      <c r="E78" s="72"/>
-      <c r="F78" s="72"/>
-      <c r="G78" s="73"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A79" s="33"/>
-      <c r="B79" s="34" t="s">
+      <c r="B105" s="94"/>
+      <c r="C105" s="94"/>
+      <c r="D105" s="94"/>
+      <c r="E105" s="94"/>
+      <c r="F105" s="94"/>
+      <c r="G105" s="95"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A106" s="33"/>
+      <c r="B106" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="C79" s="34" t="s">
+      <c r="C106" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="D79" s="35" t="s">
+      <c r="D106" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="F79" s="36"/>
-      <c r="G79" s="37" t="s">
+      <c r="F106" s="36"/>
+      <c r="G106" s="37" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A80" s="74" t="s">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A107" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="B80" s="75"/>
-      <c r="C80" s="75"/>
-      <c r="D80" s="75"/>
-      <c r="E80" s="75"/>
-      <c r="F80" s="36"/>
-      <c r="G80" s="15"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A81" s="76" t="s">
+      <c r="B107" s="117"/>
+      <c r="C107" s="117"/>
+      <c r="D107" s="117"/>
+      <c r="E107" s="117"/>
+      <c r="F107" s="36"/>
+      <c r="G107" s="15"/>
+    </row>
+    <row r="108" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A108" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="B81" s="77"/>
-      <c r="C81" s="77"/>
-      <c r="D81" s="78" t="s">
+      <c r="B108" s="78"/>
+      <c r="C108" s="78"/>
+      <c r="D108" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="E81" s="79"/>
-      <c r="F81" s="79"/>
-      <c r="G81" s="80"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A82" s="64" t="s">
+      <c r="E108" s="80"/>
+      <c r="F108" s="80"/>
+      <c r="G108" s="81"/>
+    </row>
+    <row r="109" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A109" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B82" s="65"/>
-      <c r="C82" s="65"/>
-      <c r="D82" s="8"/>
-      <c r="G82" s="9"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A83" s="64" t="s">
+      <c r="B109" s="76"/>
+      <c r="C109" s="76"/>
+      <c r="D109" s="8"/>
+      <c r="G109" s="9"/>
+    </row>
+    <row r="110" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A110" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="B83" s="65"/>
-      <c r="C83" s="65"/>
-      <c r="D83" s="8"/>
-      <c r="G83" s="9"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A84" s="64" t="s">
+      <c r="B110" s="76"/>
+      <c r="C110" s="76"/>
+      <c r="D110" s="8"/>
+      <c r="G110" s="9"/>
+    </row>
+    <row r="111" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A111" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="B84" s="65"/>
-      <c r="C84" s="65"/>
-      <c r="D84" s="8"/>
-      <c r="G84" s="9"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A85" s="66" t="s">
+      <c r="B111" s="76"/>
+      <c r="C111" s="76"/>
+      <c r="D111" s="8"/>
+      <c r="G111" s="9"/>
+    </row>
+    <row r="112" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A112" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="B85" s="67"/>
-      <c r="C85" s="67"/>
-      <c r="D85" s="21"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="22"/>
-      <c r="G85" s="18"/>
+      <c r="B112" s="71"/>
+      <c r="C112" s="71"/>
+      <c r="D112" s="21"/>
+      <c r="E112" s="22"/>
+      <c r="F112" s="22"/>
+      <c r="G112" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:E3"/>
+  <mergeCells count="10">
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="D13:G13"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:G6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A77:G77"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="82" fitToHeight="2" orientation="portrait" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="43" max="6" man="1"/>
-  </rowBreaks>
+  <pageSetup paperSize="9" scale="82" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
invoices groupping added, cellUtils refactored, types refactored
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BEB227-A8F4-4C33-985D-237AA6D2C722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79EC959-3BB4-499B-B09E-660A41F1DBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="1853" windowWidth="28996" windowHeight="15794" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-14497" yWindow="16103" windowWidth="28994" windowHeight="15794" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="172">
   <si>
     <t>COMMERCIAL INVOICE</t>
   </si>
@@ -442,9 +442,6 @@
   </si>
   <si>
     <t>33 547,50$</t>
-  </si>
-  <si>
-    <t>Подписанно Котова Н.М.</t>
   </si>
   <si>
     <t>в пользу  ООО "Тихоокеанская рыбопромышленная компания"</t>
@@ -673,6 +670,12 @@
   </si>
   <si>
     <t>ROOM 1105, NOBLIAN 2, 80, JUNGANG-DAERO, JUNG-GU, BUSAN, KOREA Manysdfjsdlfjkalsdfsad;fjskldafj;sdlfakldfksa;flksdklf;js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Продавец тут будет </t>
+  </si>
+  <si>
+    <t>Подписано Котова Н.М.</t>
   </si>
 </sst>
 </file>
@@ -969,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1255,6 +1258,36 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1273,48 +1306,17 @@
     <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1636,8 +1638,8 @@
   </sheetPr>
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="81" zoomScaleNormal="100" zoomScaleSheetLayoutView="81" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScale="81" zoomScaleNormal="100" zoomScaleSheetLayoutView="81" workbookViewId="0">
+      <selection activeCell="B26" sqref="A23:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1659,14 +1661,14 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="3"/>
       <c r="N1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
@@ -1674,48 +1676,48 @@
         <v>24</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="3"/>
       <c r="N2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="45" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H3" s="47"/>
       <c r="N3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="N4" t="s">
         <v>105</v>
-      </c>
-      <c r="N4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="50" t="s">
         <v>107</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>108</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="51" t="s">
         <v>62</v>
@@ -1731,26 +1733,26 @@
     </row>
     <row r="8" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="50" t="s">
         <v>111</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -1771,49 +1773,49 @@
     </row>
     <row r="13" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="48" t="s">
         <v>114</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="B15" s="53" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M17" s="55"/>
       <c r="N17" t="s">
         <v>37</v>
       </c>
       <c r="O17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P17" t="s">
         <v>38</v>
@@ -1831,111 +1833,111 @@
         <v>33547.5</v>
       </c>
       <c r="U17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="53" t="s">
         <v>122</v>
-      </c>
-      <c r="B18" s="53" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="26.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="48" t="s">
         <v>124</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="26.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="54" t="s">
         <v>126</v>
-      </c>
-      <c r="B20" s="54" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="45.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="52" t="s">
         <v>128</v>
-      </c>
-      <c r="B22" s="52" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="48" t="s">
         <v>130</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="41.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="48" t="s">
+    </row>
+    <row r="25" spans="1:21" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="103" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="123" t="s">
+      <c r="B25" s="103" t="s">
         <v>134</v>
-      </c>
-      <c r="B25" s="123" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="55.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="60" t="s">
         <v>136</v>
-      </c>
-      <c r="B26" s="60" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="53" t="s">
         <v>138</v>
-      </c>
-      <c r="B27" s="53" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="48" t="s">
         <v>140</v>
-      </c>
-      <c r="B28" s="48" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="B29" s="53" t="s">
         <v>142</v>
-      </c>
-      <c r="B29" s="53" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -1956,10 +1958,10 @@
     </row>
     <row r="33" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="48" t="s">
         <v>145</v>
-      </c>
-      <c r="B33" s="48" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -1983,34 +1985,34 @@
         <v>57</v>
       </c>
       <c r="B36" s="48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="B37" s="48" t="s">
-        <v>149</v>
-      </c>
     </row>
     <row r="38" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="48" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="39" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="48" t="s">
+      <c r="B39" s="51" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" ht="28.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
         <v>14</v>
       </c>
@@ -2020,58 +2022,58 @@
     </row>
     <row r="41" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B41" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B42" s="48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B43" s="48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B44" s="48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B45" s="48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B46" s="57" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="58" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" s="58" t="s">
         <v>156</v>
-      </c>
-      <c r="B47" s="58" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2085,7 +2087,7 @@
     <row r="71" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="78" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{13E4E285-FA5D-41CC-AC7F-578EA8AF8279}">
       <formula1>_xlfn.ANCHORARRAY($N$1)</formula1>
     </dataValidation>
@@ -2095,7 +2097,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.11811023622047245" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="84" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="2" max="1048575" man="1"/>
   </colBreaks>
@@ -2110,8 +2112,8 @@
   </sheetPr>
   <dimension ref="A1:Z112"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="78" zoomScaleNormal="70" zoomScaleSheetLayoutView="78" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2144,12 +2146,12 @@
       <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="122" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="11"/>
@@ -2165,7 +2167,7 @@
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="61" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="B3" s="62"/>
       <c r="C3" s="42"/>
@@ -2189,8 +2191,8 @@
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="113"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="112"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2227,17 +2229,17 @@
       <c r="G6" s="69"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="106" t="s">
-        <v>170</v>
-      </c>
-      <c r="B7" s="107"/>
-      <c r="C7" s="108"/>
-      <c r="D7" s="109" t="s">
+      <c r="A7" s="116" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="117"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="111"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="119"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2286,7 +2288,7 @@
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>25</v>
@@ -2315,12 +2317,12 @@
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="103" t="s">
+      <c r="D13" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="105"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="115"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="24" t="s">
@@ -2677,13 +2679,13 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="116" t="s">
+      <c r="A43" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="117"/>
-      <c r="C43" s="117"/>
-      <c r="D43" s="117"/>
-      <c r="E43" s="117"/>
+      <c r="B43" s="105"/>
+      <c r="C43" s="105"/>
+      <c r="D43" s="105"/>
+      <c r="E43" s="105"/>
       <c r="F43" s="36"/>
       <c r="G43" s="15"/>
     </row>
@@ -2738,149 +2740,85 @@
       <c r="F48" s="22"/>
       <c r="G48" s="18"/>
     </row>
-    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="121"/>
-      <c r="B49" s="121"/>
-      <c r="C49" s="121"/>
-      <c r="D49" s="122"/>
-      <c r="E49" s="122"/>
-      <c r="F49" s="122"/>
-      <c r="G49" s="122"/>
-    </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="121"/>
-      <c r="B50" s="121"/>
-      <c r="C50" s="121"/>
-      <c r="D50" s="122"/>
-      <c r="E50" s="122"/>
-      <c r="F50" s="122"/>
-      <c r="G50" s="122"/>
-    </row>
-    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="121"/>
-      <c r="B51" s="121"/>
-      <c r="C51" s="121"/>
-      <c r="D51" s="122"/>
-      <c r="E51" s="122"/>
-      <c r="F51" s="122"/>
-      <c r="G51" s="122"/>
-    </row>
-    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="121"/>
-      <c r="B52" s="121"/>
-      <c r="C52" s="121"/>
-      <c r="D52" s="122"/>
-      <c r="E52" s="122"/>
-      <c r="F52" s="122"/>
-      <c r="G52" s="122"/>
-    </row>
-    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="121"/>
-      <c r="B53" s="121"/>
-      <c r="C53" s="121"/>
-      <c r="D53" s="122"/>
-      <c r="E53" s="122"/>
-      <c r="F53" s="122"/>
-      <c r="G53" s="122"/>
-    </row>
-    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="121"/>
-      <c r="B54" s="121"/>
-      <c r="C54" s="121"/>
-      <c r="D54" s="122"/>
-      <c r="E54" s="122"/>
-      <c r="F54" s="122"/>
-      <c r="G54" s="122"/>
-    </row>
-    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="121"/>
-      <c r="B55" s="121"/>
-      <c r="C55" s="121"/>
-      <c r="D55" s="122"/>
-      <c r="E55" s="122"/>
-      <c r="F55" s="122"/>
-      <c r="G55" s="122"/>
-    </row>
-    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="121"/>
-      <c r="B56" s="121"/>
-      <c r="C56" s="121"/>
-      <c r="D56" s="122"/>
-      <c r="E56" s="122"/>
-      <c r="F56" s="122"/>
-      <c r="G56" s="122"/>
-    </row>
-    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="121"/>
-      <c r="B57" s="121"/>
-      <c r="C57" s="121"/>
-      <c r="D57" s="122"/>
-      <c r="E57" s="122"/>
-      <c r="F57" s="122"/>
-      <c r="G57" s="122"/>
-    </row>
-    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="121"/>
-      <c r="B58" s="121"/>
-      <c r="C58" s="121"/>
-      <c r="D58" s="122"/>
-      <c r="E58" s="122"/>
-      <c r="F58" s="122"/>
-      <c r="G58" s="122"/>
-    </row>
-    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="121"/>
-      <c r="B59" s="121"/>
-      <c r="C59" s="121"/>
-      <c r="D59" s="122"/>
-      <c r="E59" s="122"/>
-      <c r="F59" s="122"/>
-      <c r="G59" s="122"/>
-    </row>
-    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="121"/>
-      <c r="B60" s="121"/>
-      <c r="C60" s="121"/>
-      <c r="D60" s="122"/>
-      <c r="E60" s="122"/>
-      <c r="F60" s="122"/>
-      <c r="G60" s="122"/>
-    </row>
-    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="121"/>
-      <c r="B61" s="121"/>
-      <c r="C61" s="121"/>
-      <c r="D61" s="122"/>
-      <c r="E61" s="122"/>
-      <c r="F61" s="122"/>
-      <c r="G61" s="122"/>
-    </row>
-    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="121"/>
-      <c r="B62" s="121"/>
-      <c r="C62" s="121"/>
-      <c r="D62" s="122"/>
-      <c r="E62" s="122"/>
-      <c r="F62" s="122"/>
-      <c r="G62" s="122"/>
-    </row>
-    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="121"/>
-      <c r="B63" s="121"/>
-      <c r="C63" s="121"/>
-      <c r="D63" s="122"/>
-      <c r="E63" s="122"/>
-      <c r="F63" s="122"/>
-      <c r="G63" s="122"/>
-    </row>
-    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="121"/>
-      <c r="B64" s="121"/>
-      <c r="C64" s="121"/>
-      <c r="D64" s="122"/>
-      <c r="E64" s="122"/>
-      <c r="F64" s="122"/>
-      <c r="G64" s="122"/>
+    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="62"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="62"/>
+    </row>
+    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="62"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="62"/>
+    </row>
+    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="62"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="62"/>
+    </row>
+    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="62"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="62"/>
+    </row>
+    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="62"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="62"/>
+    </row>
+    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="62"/>
+      <c r="B54" s="62"/>
+      <c r="C54" s="62"/>
+    </row>
+    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="62"/>
+      <c r="B55" s="62"/>
+      <c r="C55" s="62"/>
+    </row>
+    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="62"/>
+      <c r="B56" s="62"/>
+      <c r="C56" s="62"/>
+    </row>
+    <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="62"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="62"/>
+    </row>
+    <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="62"/>
+      <c r="B58" s="62"/>
+      <c r="C58" s="62"/>
+    </row>
+    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="62"/>
+      <c r="B59" s="62"/>
+      <c r="C59" s="62"/>
+    </row>
+    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="62"/>
+      <c r="B60" s="62"/>
+      <c r="C60" s="62"/>
+    </row>
+    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="62"/>
+      <c r="B61" s="62"/>
+      <c r="C61" s="62"/>
+    </row>
+    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="62"/>
+      <c r="B62" s="62"/>
+      <c r="C62" s="62"/>
+    </row>
+    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="62"/>
+      <c r="B63" s="62"/>
+      <c r="C63" s="62"/>
+    </row>
+    <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="62"/>
+      <c r="B64" s="62"/>
+      <c r="C64" s="62"/>
     </row>
     <row r="65" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="66" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.75">
@@ -2934,8 +2872,8 @@
       </c>
       <c r="B69" s="71"/>
       <c r="C69" s="62"/>
-      <c r="D69" s="112"/>
-      <c r="E69" s="113"/>
+      <c r="D69" s="111"/>
+      <c r="E69" s="112"/>
       <c r="F69" s="8"/>
       <c r="G69" s="9"/>
     </row>
@@ -2966,17 +2904,17 @@
       <c r="G71" s="69"/>
     </row>
     <row r="72" spans="1:7" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="109" t="s">
+      <c r="A72" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="110"/>
-      <c r="C72" s="110"/>
-      <c r="D72" s="118" t="s">
+      <c r="B72" s="107"/>
+      <c r="C72" s="107"/>
+      <c r="D72" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="E72" s="119"/>
-      <c r="F72" s="119"/>
-      <c r="G72" s="120"/>
+      <c r="E72" s="109"/>
+      <c r="F72" s="109"/>
+      <c r="G72" s="110"/>
     </row>
     <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="88" t="s">
@@ -3025,7 +2963,7 @@
     </row>
     <row r="76" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B76" s="71" t="s">
         <v>76</v>
@@ -3349,13 +3287,13 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A107" s="116" t="s">
+      <c r="A107" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="117"/>
-      <c r="C107" s="117"/>
-      <c r="D107" s="117"/>
-      <c r="E107" s="117"/>
+      <c r="B107" s="105"/>
+      <c r="C107" s="105"/>
+      <c r="D107" s="105"/>
+      <c r="E107" s="105"/>
       <c r="F107" s="36"/>
       <c r="G107" s="15"/>
     </row>
@@ -3366,7 +3304,7 @@
       <c r="B108" s="78"/>
       <c r="C108" s="78"/>
       <c r="D108" s="79" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="E108" s="80"/>
       <c r="F108" s="80"/>
@@ -3392,7 +3330,7 @@
     </row>
     <row r="111" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="66" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B111" s="76"/>
       <c r="C111" s="76"/>
@@ -3412,16 +3350,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A2:C2"/>
     <mergeCell ref="A107:E107"/>
     <mergeCell ref="A72:C72"/>
     <mergeCell ref="D72:G72"/>
     <mergeCell ref="D69:E69"/>
     <mergeCell ref="A43:E43"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>

</xml_diff>

<commit_message>
implementing excel utils object
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79EC959-3BB4-499B-B09E-660A41F1DBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951D20CB-1093-4FF8-AEAC-1C406DC64C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14497" yWindow="16103" windowWidth="28994" windowHeight="15794" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15796" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <definedName name="Доставка_порт">Export_Contract!$A$24</definedName>
     <definedName name="Доставка_условия">Export_Contract!$A$23</definedName>
     <definedName name="Инвойс">Com_Invoice!$D$3</definedName>
-    <definedName name="Инвойс_Bl">Com_Invoice!$A$15</definedName>
+    <definedName name="Инвойс_Bl_массив">Com_Invoice!$A$15</definedName>
     <definedName name="Инвойс_Bl_п">Com_Invoice!$A$80</definedName>
     <definedName name="Инвойс_банк_получателя">Com_Invoice!$A$44</definedName>
     <definedName name="Инвойс_банк_получателя_адрес">Com_Invoice!$A$45</definedName>
@@ -50,6 +50,7 @@
     <definedName name="Инвойс_банк_получателя_свифт_п">Com_Invoice!$A$110</definedName>
     <definedName name="Инвойс_всего">Com_Invoice!$E$15</definedName>
     <definedName name="Инвойс_всего_п">Com_Invoice!$E$80</definedName>
+    <definedName name="Инвойс_дата">Com_Invoice!$A$9</definedName>
     <definedName name="Инвойс_дата_п">Com_Invoice!$A$74</definedName>
     <definedName name="Инвойс_контракт">Com_Invoice!$D$10</definedName>
     <definedName name="Инвойс_контракт_дата">Com_Invoice!$D$11</definedName>
@@ -102,7 +103,6 @@
     <definedName name="Инвойс_условия_п">Com_Invoice!$D$78</definedName>
     <definedName name="Инвойс_цена">Com_Invoice!$F$15</definedName>
     <definedName name="Инвойс_цена_п">Com_Invoice!$F$80</definedName>
-    <definedName name="Иновйс_дата">Com_Invoice!$A$9</definedName>
     <definedName name="Контракт">Export_Contract!$A$2</definedName>
     <definedName name="Контракт_дата">Export_Contract!$A$3</definedName>
     <definedName name="МСЦ">Com_Invoice!$F$3</definedName>
@@ -1261,18 +1261,54 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1281,42 +1317,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1639,7 +1639,7 @@
   <dimension ref="A1:W78"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScale="81" zoomScaleNormal="100" zoomScaleSheetLayoutView="81" workbookViewId="0">
-      <selection activeCell="B26" sqref="A23:B26"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2113,7 +2113,7 @@
   <dimension ref="A1:Z112"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2146,12 +2146,12 @@
       <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="122" t="s">
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="104" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="11"/>
@@ -2191,8 +2191,8 @@
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="112"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="115"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2229,17 +2229,17 @@
       <c r="G6" s="69"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="108" t="s">
         <v>169</v>
       </c>
-      <c r="B7" s="117"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="106" t="s">
+      <c r="B7" s="109"/>
+      <c r="C7" s="110"/>
+      <c r="D7" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="119"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="112"/>
+      <c r="G7" s="113"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2317,12 +2317,12 @@
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="113" t="s">
+      <c r="D13" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="114"/>
-      <c r="F13" s="114"/>
-      <c r="G13" s="115"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="107"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="24" t="s">
@@ -2679,13 +2679,13 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="104" t="s">
+      <c r="A43" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="105"/>
-      <c r="C43" s="105"/>
-      <c r="D43" s="105"/>
-      <c r="E43" s="105"/>
+      <c r="B43" s="119"/>
+      <c r="C43" s="119"/>
+      <c r="D43" s="119"/>
+      <c r="E43" s="119"/>
       <c r="F43" s="36"/>
       <c r="G43" s="15"/>
     </row>
@@ -2872,8 +2872,8 @@
       </c>
       <c r="B69" s="71"/>
       <c r="C69" s="62"/>
-      <c r="D69" s="111"/>
-      <c r="E69" s="112"/>
+      <c r="D69" s="114"/>
+      <c r="E69" s="115"/>
       <c r="F69" s="8"/>
       <c r="G69" s="9"/>
     </row>
@@ -2904,17 +2904,17 @@
       <c r="G71" s="69"/>
     </row>
     <row r="72" spans="1:7" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="106" t="s">
+      <c r="A72" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="107"/>
-      <c r="C72" s="107"/>
-      <c r="D72" s="108" t="s">
+      <c r="B72" s="112"/>
+      <c r="C72" s="112"/>
+      <c r="D72" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="E72" s="109"/>
-      <c r="F72" s="109"/>
-      <c r="G72" s="110"/>
+      <c r="E72" s="121"/>
+      <c r="F72" s="121"/>
+      <c r="G72" s="122"/>
     </row>
     <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="88" t="s">
@@ -3287,13 +3287,13 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A107" s="104" t="s">
+      <c r="A107" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="105"/>
-      <c r="C107" s="105"/>
-      <c r="D107" s="105"/>
-      <c r="E107" s="105"/>
+      <c r="B107" s="119"/>
+      <c r="C107" s="119"/>
+      <c r="D107" s="119"/>
+      <c r="E107" s="119"/>
       <c r="F107" s="36"/>
       <c r="G107" s="15"/>
     </row>
@@ -3350,16 +3350,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A107:E107"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="A43:E43"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>

</xml_diff>

<commit_message>
stylization invoice rows bl added, refactoring formatting numnbers
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951D20CB-1093-4FF8-AEAC-1C406DC64C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91D97DB-571C-4C6C-8DF3-D306A1E44DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15796" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-55778" yWindow="-907" windowWidth="28995" windowHeight="15795" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -791,7 +791,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -968,11 +968,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1246,9 +1283,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
@@ -1264,14 +1298,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1282,41 +1334,30 @@
     <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1893,10 +1934,10 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="103" t="s">
+      <c r="A25" s="102" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="103" t="s">
+      <c r="B25" s="102" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2112,8 +2153,8 @@
   </sheetPr>
   <dimension ref="A1:Z112"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2146,12 +2187,12 @@
       <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="104" t="s">
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="103" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="11"/>
@@ -2191,8 +2232,8 @@
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
-      <c r="D4" s="114"/>
-      <c r="E4" s="115"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="112"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2229,17 +2270,17 @@
       <c r="G6" s="69"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="108" t="s">
+      <c r="A7" s="113" t="s">
         <v>169</v>
       </c>
-      <c r="B7" s="109"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="111" t="s">
+      <c r="B7" s="114"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="113"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="116"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2313,35 +2354,35 @@
       <c r="F12" s="67"/>
       <c r="G12" s="68"/>
     </row>
-    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="105" t="s">
+    <row r="13" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="8"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="108" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="106"/>
-      <c r="F13" s="106"/>
-      <c r="G13" s="107"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A14" s="24" t="s">
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
+      <c r="G13" s="110"/>
+    </row>
+    <row r="14" spans="1:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="121" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="99" t="s">
+      <c r="D14" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="99"/>
-      <c r="F14" s="25" t="s">
+      <c r="E14" s="123"/>
+      <c r="F14" s="122" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="124" t="s">
         <v>35</v>
       </c>
       <c r="Q14" t="s">
@@ -2679,13 +2720,13 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="118" t="s">
+      <c r="A43" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="119"/>
-      <c r="C43" s="119"/>
-      <c r="D43" s="119"/>
-      <c r="E43" s="119"/>
+      <c r="B43" s="105"/>
+      <c r="C43" s="105"/>
+      <c r="D43" s="105"/>
+      <c r="E43" s="105"/>
       <c r="F43" s="36"/>
       <c r="G43" s="15"/>
     </row>
@@ -2872,8 +2913,8 @@
       </c>
       <c r="B69" s="71"/>
       <c r="C69" s="62"/>
-      <c r="D69" s="114"/>
-      <c r="E69" s="115"/>
+      <c r="D69" s="111"/>
+      <c r="E69" s="112"/>
       <c r="F69" s="8"/>
       <c r="G69" s="9"/>
     </row>
@@ -2904,17 +2945,17 @@
       <c r="G71" s="69"/>
     </row>
     <row r="72" spans="1:7" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="111" t="s">
+      <c r="A72" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="112"/>
-      <c r="C72" s="112"/>
-      <c r="D72" s="120" t="s">
+      <c r="B72" s="107"/>
+      <c r="C72" s="107"/>
+      <c r="D72" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="E72" s="121"/>
-      <c r="F72" s="121"/>
-      <c r="G72" s="122"/>
+      <c r="E72" s="109"/>
+      <c r="F72" s="109"/>
+      <c r="G72" s="110"/>
     </row>
     <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="88" t="s">
@@ -3238,26 +3279,26 @@
       <c r="G102" s="15"/>
     </row>
     <row r="103" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A103" s="100" t="s">
+      <c r="A103" s="99" t="s">
         <v>90</v>
       </c>
-      <c r="B103" s="101"/>
-      <c r="C103" s="101"/>
-      <c r="D103" s="101"/>
-      <c r="E103" s="101"/>
-      <c r="F103" s="101"/>
-      <c r="G103" s="102"/>
+      <c r="B103" s="100"/>
+      <c r="C103" s="100"/>
+      <c r="D103" s="100"/>
+      <c r="E103" s="100"/>
+      <c r="F103" s="100"/>
+      <c r="G103" s="101"/>
     </row>
     <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="100" t="s">
+      <c r="A104" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="B104" s="101"/>
-      <c r="C104" s="101"/>
-      <c r="D104" s="101"/>
-      <c r="E104" s="101"/>
-      <c r="F104" s="101"/>
-      <c r="G104" s="102"/>
+      <c r="B104" s="100"/>
+      <c r="C104" s="100"/>
+      <c r="D104" s="100"/>
+      <c r="E104" s="100"/>
+      <c r="F104" s="100"/>
+      <c r="G104" s="101"/>
     </row>
     <row r="105" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="93" t="s">
@@ -3287,13 +3328,13 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A107" s="118" t="s">
+      <c r="A107" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="119"/>
-      <c r="C107" s="119"/>
-      <c r="D107" s="119"/>
-      <c r="E107" s="119"/>
+      <c r="B107" s="105"/>
+      <c r="C107" s="105"/>
+      <c r="D107" s="105"/>
+      <c r="E107" s="105"/>
       <c r="F107" s="36"/>
       <c r="G107" s="15"/>
     </row>
@@ -3350,16 +3391,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A2:C2"/>
     <mergeCell ref="A107:E107"/>
     <mergeCell ref="A72:C72"/>
     <mergeCell ref="D72:G72"/>
     <mergeCell ref="D69:E69"/>
     <mergeCell ref="A43:E43"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>

</xml_diff>

<commit_message>
merge cells fn added, implementing translation template
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91D97DB-571C-4C6C-8DF3-D306A1E44DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F253FB-5BB1-492F-BCDC-FD58B62EAB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-907" windowWidth="28995" windowHeight="15795" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-14497" yWindow="16103" windowWidth="28994" windowHeight="15794" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -52,6 +52,8 @@
     <definedName name="Инвойс_всего_п">Com_Invoice!$E$80</definedName>
     <definedName name="Инвойс_дата">Com_Invoice!$A$9</definedName>
     <definedName name="Инвойс_дата_п">Com_Invoice!$A$74</definedName>
+    <definedName name="Инвойс_декларация">Com_Invoice!$A$12</definedName>
+    <definedName name="Инвойс_декларация_п">Com_Invoice!$A$77</definedName>
     <definedName name="Инвойс_контракт">Com_Invoice!$D$10</definedName>
     <definedName name="Инвойс_контракт_дата">Com_Invoice!$D$11</definedName>
     <definedName name="Инвойс_контракт_дата_п">Com_Invoice!$D$76</definedName>
@@ -154,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="174">
   <si>
     <t>COMMERCIAL INVOICE</t>
   </si>
@@ -631,9 +633,6 @@
     <t>Покупатель/Buyer ________________________SE JI YOUNG</t>
   </si>
   <si>
-    <t>Busan, Korea</t>
-  </si>
-  <si>
     <t>Пусан, Корея</t>
   </si>
   <si>
@@ -676,6 +675,15 @@
   </si>
   <si>
     <t>Подписано Котова Н.М.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Декларация хуекларация </t>
+  </si>
+  <si>
+    <t>Декларация хуекларация по русски</t>
+  </si>
+  <si>
+    <t>7, Chungjang-daero, Jung-gu, Busan, Republic of Korea (Jungang-dong-4</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1175,9 +1183,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1298,66 +1303,83 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1679,7 +1701,7 @@
   </sheetPr>
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScale="81" zoomScaleNormal="100" zoomScaleSheetLayoutView="81" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="81" zoomScaleNormal="100" zoomScaleSheetLayoutView="81" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -1702,7 +1724,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>97</v>
@@ -1726,7 +1748,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>101</v>
@@ -1758,7 +1780,7 @@
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B6" s="51" t="s">
         <v>62</v>
@@ -1774,7 +1796,7 @@
     </row>
     <row r="8" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>108</v>
@@ -1782,7 +1804,7 @@
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9" s="48" t="s">
         <v>109</v>
@@ -1814,7 +1836,7 @@
     </row>
     <row r="13" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B13" s="48" t="s">
         <v>112</v>
@@ -1838,7 +1860,7 @@
     </row>
     <row r="16" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B16" s="48" t="s">
         <v>117</v>
@@ -1846,7 +1868,7 @@
     </row>
     <row r="17" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B17" s="54" t="s">
         <v>118</v>
@@ -1903,10 +1925,10 @@
     </row>
     <row r="21" spans="1:21" ht="45.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
@@ -1934,10 +1956,10 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="102" t="s">
+      <c r="A25" s="101" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="102" t="s">
+      <c r="B25" s="101" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2153,8 +2175,8 @@
   </sheetPr>
   <dimension ref="A1:Z112"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2176,23 +2198,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="103" t="s">
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="102" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="11"/>
@@ -2208,14 +2230,14 @@
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" s="62"/>
       <c r="C3" s="42"/>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="76"/>
+      <c r="E3" s="75"/>
       <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
@@ -2232,8 +2254,8 @@
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="112"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="117"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2241,46 +2263,46 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="65" t="s">
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="68"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="67"/>
       <c r="Q5">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="127"/>
       <c r="D6" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="69"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="68"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="113" t="s">
-        <v>169</v>
-      </c>
-      <c r="B7" s="114"/>
-      <c r="C7" s="115"/>
-      <c r="D7" s="106" t="s">
+      <c r="A7" s="110" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="111"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="116"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="115"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2290,12 +2312,12 @@
         <v>17</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="68"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="67"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
@@ -2305,12 +2327,12 @@
         <v>20</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="73" t="s">
+      <c r="D9" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="75"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="74"/>
     </row>
     <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
@@ -2325,64 +2347,63 @@
       </c>
       <c r="E10" s="62"/>
       <c r="F10" s="62"/>
-      <c r="G10" s="69"/>
+      <c r="G10" s="68"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
-        <v>157</v>
+        <v>1</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="18"/>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="72"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="71"/>
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
-        <v>27</v>
+        <v>171</v>
       </c>
       <c r="C12" s="20"/>
-      <c r="D12" s="65" t="s">
+      <c r="D12" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="68"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="8"/>
-      <c r="B13" s="119"/>
       <c r="C13" s="15"/>
-      <c r="D13" s="108" t="s">
+      <c r="D13" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="110"/>
+      <c r="E13" s="108"/>
+      <c r="F13" s="108"/>
+      <c r="G13" s="109"/>
     </row>
     <row r="14" spans="1:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="122" t="s">
+      <c r="B14" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="123" t="s">
+      <c r="D14" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="123"/>
-      <c r="F14" s="122" t="s">
+      <c r="E14" s="105"/>
+      <c r="F14" s="104" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="124" t="s">
+      <c r="G14" s="106" t="s">
         <v>35</v>
       </c>
       <c r="Q14" t="s">
@@ -2671,37 +2692,37 @@
       <c r="G38" s="32"/>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="96" t="s">
+      <c r="A39" s="95" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="97"/>
-      <c r="C39" s="97"/>
-      <c r="D39" s="97"/>
-      <c r="E39" s="97"/>
-      <c r="F39" s="97"/>
-      <c r="G39" s="98"/>
+      <c r="B39" s="96"/>
+      <c r="C39" s="96"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="96"/>
+      <c r="F39" s="96"/>
+      <c r="G39" s="97"/>
     </row>
     <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="96" t="s">
+      <c r="A40" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="97"/>
-      <c r="C40" s="97"/>
-      <c r="D40" s="97"/>
-      <c r="E40" s="97"/>
-      <c r="F40" s="97"/>
-      <c r="G40" s="98"/>
+      <c r="B40" s="96"/>
+      <c r="C40" s="96"/>
+      <c r="D40" s="96"/>
+      <c r="E40" s="96"/>
+      <c r="F40" s="96"/>
+      <c r="G40" s="97"/>
     </row>
     <row r="41" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="93" t="s">
+      <c r="A41" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="94"/>
-      <c r="C41" s="94"/>
-      <c r="D41" s="94"/>
-      <c r="E41" s="94"/>
-      <c r="F41" s="94"/>
-      <c r="G41" s="95"/>
+      <c r="B41" s="93"/>
+      <c r="C41" s="93"/>
+      <c r="D41" s="93"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="93"/>
+      <c r="G41" s="94"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="33"/>
@@ -2711,7 +2732,7 @@
       <c r="C42" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="35" t="s">
+      <c r="D42" s="122" t="s">
         <v>43</v>
       </c>
       <c r="F42" s="36"/>
@@ -2720,61 +2741,61 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="104" t="s">
+      <c r="A43" s="120" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="105"/>
-      <c r="C43" s="105"/>
-      <c r="D43" s="105"/>
-      <c r="E43" s="105"/>
+      <c r="B43" s="121"/>
+      <c r="C43" s="121"/>
+      <c r="D43" s="121"/>
+      <c r="E43" s="121"/>
       <c r="F43" s="36"/>
       <c r="G43" s="15"/>
     </row>
     <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="77" t="s">
+      <c r="A44" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="78"/>
-      <c r="C44" s="78"/>
-      <c r="D44" s="79" t="s">
+      <c r="B44" s="77"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="80"/>
-      <c r="F44" s="80"/>
-      <c r="G44" s="81"/>
+      <c r="E44" s="79"/>
+      <c r="F44" s="79"/>
+      <c r="G44" s="80"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="76"/>
-      <c r="C45" s="76"/>
+      <c r="B45" s="75"/>
+      <c r="C45" s="75"/>
       <c r="D45" s="8"/>
       <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="66" t="s">
+      <c r="A46" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="76"/>
-      <c r="C46" s="76"/>
+      <c r="B46" s="75"/>
+      <c r="C46" s="75"/>
       <c r="D46" s="8"/>
       <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="B47" s="76"/>
-      <c r="C47" s="76"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="75"/>
       <c r="D47" s="8"/>
       <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="70" t="s">
+      <c r="A48" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="71"/>
+      <c r="B48" s="70"/>
       <c r="C48" s="71"/>
       <c r="D48" s="21"/>
       <c r="E48" s="22"/>
@@ -2863,30 +2884,30 @@
     </row>
     <row r="65" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="66" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A66" s="83" t="s">
+      <c r="A66" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="83"/>
-      <c r="C66" s="83"/>
-      <c r="D66" s="83"/>
-      <c r="E66" s="83"/>
-      <c r="F66" s="83"/>
-      <c r="G66" s="83"/>
+      <c r="B66" s="82"/>
+      <c r="C66" s="82"/>
+      <c r="D66" s="82"/>
+      <c r="E66" s="82"/>
+      <c r="F66" s="82"/>
+      <c r="G66" s="82"/>
     </row>
     <row r="67" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="84" t="s">
+      <c r="A67" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="85"/>
-      <c r="C67" s="85"/>
-      <c r="D67" s="84" t="s">
+      <c r="B67" s="84"/>
+      <c r="C67" s="84"/>
+      <c r="D67" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="E67" s="85"/>
-      <c r="F67" s="1" t="s">
+      <c r="E67" s="84"/>
+      <c r="F67" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G67" s="124" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2896,102 +2917,102 @@
       </c>
       <c r="B68" s="62"/>
       <c r="C68" s="62"/>
-      <c r="D68" s="66" t="s">
+      <c r="D68" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="E68" s="76"/>
-      <c r="F68" s="6" t="s">
+      <c r="E68" s="75"/>
+      <c r="F68" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="G68" s="7" t="s">
+      <c r="G68" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="70" t="s">
+      <c r="A69" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="71"/>
+      <c r="B69" s="70"/>
       <c r="C69" s="62"/>
-      <c r="D69" s="111"/>
-      <c r="E69" s="112"/>
+      <c r="D69" s="61"/>
+      <c r="E69" s="62"/>
       <c r="F69" s="8"/>
       <c r="G69" s="9"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A70" s="86" t="s">
+      <c r="A70" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="85"/>
-      <c r="C70" s="87"/>
-      <c r="D70" s="65" t="s">
+      <c r="B70" s="84"/>
+      <c r="C70" s="86"/>
+      <c r="D70" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="E70" s="67"/>
-      <c r="F70" s="67"/>
-      <c r="G70" s="68"/>
+      <c r="E70" s="66"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="67"/>
     </row>
     <row r="71" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="66" t="s">
+      <c r="A71" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="B71" s="76"/>
-      <c r="C71" s="76"/>
+      <c r="B71" s="75"/>
+      <c r="C71" s="75"/>
       <c r="D71" s="61" t="s">
         <v>12</v>
       </c>
       <c r="E71" s="62"/>
       <c r="F71" s="62"/>
-      <c r="G71" s="69"/>
+      <c r="G71" s="68"/>
     </row>
     <row r="72" spans="1:7" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="106" t="s">
+      <c r="A72" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="107"/>
-      <c r="C72" s="107"/>
-      <c r="D72" s="108" t="s">
-        <v>14</v>
-      </c>
-      <c r="E72" s="109"/>
-      <c r="F72" s="109"/>
-      <c r="G72" s="110"/>
+      <c r="B72" s="114"/>
+      <c r="C72" s="115"/>
+      <c r="D72" s="113" t="s">
+        <v>173</v>
+      </c>
+      <c r="E72" s="114"/>
+      <c r="F72" s="114"/>
+      <c r="G72" s="115"/>
     </row>
     <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="88" t="s">
+      <c r="A73" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="B73" s="89" t="s">
+      <c r="B73" s="88" t="s">
         <v>68</v>
       </c>
       <c r="C73" s="9"/>
-      <c r="D73" s="65" t="s">
+      <c r="D73" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="E73" s="67"/>
-      <c r="F73" s="67"/>
-      <c r="G73" s="68"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="67"/>
     </row>
     <row r="74" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="90" t="s">
+      <c r="B74" s="89" t="s">
         <v>71</v>
       </c>
       <c r="C74" s="9"/>
-      <c r="D74" s="73" t="s">
+      <c r="D74" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="75"/>
+      <c r="E74" s="73"/>
+      <c r="F74" s="73"/>
+      <c r="G74" s="74"/>
     </row>
     <row r="75" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="88" t="s">
+      <c r="A75" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="B75" s="91" t="s">
+      <c r="B75" s="90" t="s">
         <v>74</v>
       </c>
       <c r="C75" s="15"/>
@@ -3000,45 +3021,45 @@
       </c>
       <c r="E75" s="62"/>
       <c r="F75" s="62"/>
-      <c r="G75" s="69"/>
+      <c r="G75" s="68"/>
     </row>
     <row r="76" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="70" t="s">
-        <v>158</v>
-      </c>
-      <c r="B76" s="71" t="s">
+      <c r="A76" s="69" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" s="70" t="s">
         <v>76</v>
       </c>
       <c r="C76" s="18"/>
-      <c r="D76" s="70" t="s">
+      <c r="D76" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="E76" s="71"/>
-      <c r="F76" s="71"/>
-      <c r="G76" s="72"/>
+      <c r="E76" s="70"/>
+      <c r="F76" s="70"/>
+      <c r="G76" s="71"/>
     </row>
     <row r="77" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="8" t="s">
-        <v>27</v>
+        <v>172</v>
       </c>
       <c r="C77" s="20"/>
-      <c r="D77" s="65" t="s">
+      <c r="D77" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="E77" s="67"/>
-      <c r="F77" s="67"/>
-      <c r="G77" s="68"/>
+      <c r="E77" s="66"/>
+      <c r="F77" s="66"/>
+      <c r="G77" s="67"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" s="21"/>
       <c r="B78" s="22"/>
       <c r="C78" s="23"/>
-      <c r="D78" s="70" t="s">
+      <c r="D78" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="E78" s="71"/>
-      <c r="F78" s="71"/>
-      <c r="G78" s="72"/>
+      <c r="E78" s="70"/>
+      <c r="F78" s="70"/>
+      <c r="G78" s="71"/>
     </row>
     <row r="79" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="24" t="s">
@@ -3050,10 +3071,10 @@
       <c r="C79" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D79" s="92" t="s">
+      <c r="D79" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="E79" s="92"/>
+      <c r="E79" s="91"/>
       <c r="F79" s="25" t="s">
         <v>83</v>
       </c>
@@ -3279,37 +3300,37 @@
       <c r="G102" s="15"/>
     </row>
     <row r="103" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A103" s="99" t="s">
+      <c r="A103" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="B103" s="100"/>
-      <c r="C103" s="100"/>
-      <c r="D103" s="100"/>
-      <c r="E103" s="100"/>
-      <c r="F103" s="100"/>
-      <c r="G103" s="101"/>
+      <c r="B103" s="99"/>
+      <c r="C103" s="99"/>
+      <c r="D103" s="99"/>
+      <c r="E103" s="99"/>
+      <c r="F103" s="99"/>
+      <c r="G103" s="100"/>
     </row>
     <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="99" t="s">
+      <c r="A104" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="B104" s="100"/>
-      <c r="C104" s="100"/>
-      <c r="D104" s="100"/>
-      <c r="E104" s="100"/>
-      <c r="F104" s="100"/>
-      <c r="G104" s="101"/>
+      <c r="B104" s="99"/>
+      <c r="C104" s="99"/>
+      <c r="D104" s="99"/>
+      <c r="E104" s="99"/>
+      <c r="F104" s="99"/>
+      <c r="G104" s="100"/>
     </row>
     <row r="105" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A105" s="93" t="s">
+      <c r="A105" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="B105" s="94"/>
-      <c r="C105" s="94"/>
-      <c r="D105" s="94"/>
-      <c r="E105" s="94"/>
-      <c r="F105" s="94"/>
-      <c r="G105" s="95"/>
+      <c r="B105" s="93"/>
+      <c r="C105" s="93"/>
+      <c r="D105" s="93"/>
+      <c r="E105" s="93"/>
+      <c r="F105" s="93"/>
+      <c r="G105" s="94"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A106" s="33"/>
@@ -3328,79 +3349,78 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A107" s="104" t="s">
+      <c r="A107" s="120" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="105"/>
-      <c r="C107" s="105"/>
-      <c r="D107" s="105"/>
-      <c r="E107" s="105"/>
+      <c r="B107" s="121"/>
+      <c r="C107" s="121"/>
+      <c r="D107" s="121"/>
+      <c r="E107" s="121"/>
       <c r="F107" s="36"/>
       <c r="G107" s="15"/>
     </row>
     <row r="108" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A108" s="77" t="s">
+      <c r="A108" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="B108" s="78"/>
-      <c r="C108" s="78"/>
-      <c r="D108" s="79" t="s">
-        <v>171</v>
-      </c>
-      <c r="E108" s="80"/>
-      <c r="F108" s="80"/>
-      <c r="G108" s="81"/>
+      <c r="B108" s="77"/>
+      <c r="C108" s="77"/>
+      <c r="D108" s="78" t="s">
+        <v>170</v>
+      </c>
+      <c r="E108" s="79"/>
+      <c r="F108" s="79"/>
+      <c r="G108" s="80"/>
     </row>
     <row r="109" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A109" s="66" t="s">
+      <c r="A109" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="B109" s="76"/>
-      <c r="C109" s="76"/>
+      <c r="B109" s="75"/>
+      <c r="C109" s="75"/>
       <c r="D109" s="8"/>
       <c r="G109" s="9"/>
     </row>
     <row r="110" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A110" s="66" t="s">
+      <c r="A110" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="B110" s="76"/>
-      <c r="C110" s="76"/>
+      <c r="B110" s="75"/>
+      <c r="C110" s="75"/>
       <c r="D110" s="8"/>
       <c r="G110" s="9"/>
     </row>
     <row r="111" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A111" s="66" t="s">
+      <c r="A111" s="65" t="s">
         <v>96</v>
       </c>
-      <c r="B111" s="76"/>
-      <c r="C111" s="76"/>
+      <c r="B111" s="75"/>
+      <c r="C111" s="75"/>
       <c r="D111" s="8"/>
       <c r="G111" s="9"/>
     </row>
     <row r="112" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A112" s="70" t="s">
+      <c r="A112" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="B112" s="71"/>
-      <c r="C112" s="71"/>
+      <c r="B112" s="70"/>
+      <c r="C112" s="70"/>
       <c r="D112" s="21"/>
       <c r="E112" s="22"/>
       <c r="F112" s="22"/>
       <c r="G112" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A107:E107"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="A43:E43"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>

</xml_diff>

<commit_message>
file namings and folder directory in invoices refactored
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F253FB-5BB1-492F-BCDC-FD58B62EAB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE10A4B-1A54-4575-8FD9-5B7E89259853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14497" yWindow="16103" windowWidth="28994" windowHeight="15794" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <definedName name="Доставка_условия">Export_Contract!$A$23</definedName>
     <definedName name="Инвойс">Com_Invoice!$D$3</definedName>
     <definedName name="Инвойс_Bl_массив">Com_Invoice!$A$15</definedName>
-    <definedName name="Инвойс_Bl_п">Com_Invoice!$A$80</definedName>
+    <definedName name="Инвойс_Bl_массив_п">Com_Invoice!$A$80</definedName>
     <definedName name="Инвойс_банк_получателя">Com_Invoice!$A$44</definedName>
     <definedName name="Инвойс_банк_получателя_адрес">Com_Invoice!$A$45</definedName>
     <definedName name="Инвойс_банк_получателя_адрес_п">Com_Invoice!$A$109</definedName>
@@ -1017,7 +1017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1315,6 +1315,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1333,15 +1366,6 @@
     <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1353,33 +1377,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2175,8 +2172,8 @@
   </sheetPr>
   <dimension ref="A1:Z112"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A74" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2209,11 +2206,11 @@
       <c r="G1" s="81"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
       <c r="D2" s="102" t="s">
         <v>2</v>
       </c>
@@ -2254,8 +2251,8 @@
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="117"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="125"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2282,27 +2279,27 @@
       <c r="A6" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="126"/>
-      <c r="C6" s="127"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="112"/>
       <c r="D6" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
       <c r="G6" s="68"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="121" t="s">
         <v>168</v>
       </c>
-      <c r="B7" s="111"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="113" t="s">
+      <c r="B7" s="122"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="114"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="115"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="117"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2379,12 +2376,12 @@
     <row r="13" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="8"/>
       <c r="C13" s="15"/>
-      <c r="D13" s="107" t="s">
+      <c r="D13" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="108"/>
-      <c r="F13" s="108"/>
-      <c r="G13" s="109"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="120"/>
     </row>
     <row r="14" spans="1:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="103" t="s">
@@ -2732,7 +2729,7 @@
       <c r="C42" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="122" t="s">
+      <c r="D42" s="107" t="s">
         <v>43</v>
       </c>
       <c r="F42" s="36"/>
@@ -2741,13 +2738,13 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="120" t="s">
+      <c r="A43" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="121"/>
-      <c r="C43" s="121"/>
-      <c r="D43" s="121"/>
-      <c r="E43" s="121"/>
+      <c r="B43" s="114"/>
+      <c r="C43" s="114"/>
+      <c r="D43" s="114"/>
+      <c r="E43" s="114"/>
       <c r="F43" s="36"/>
       <c r="G43" s="15"/>
     </row>
@@ -2904,10 +2901,10 @@
         <v>61</v>
       </c>
       <c r="E67" s="84"/>
-      <c r="F67" s="123" t="s">
+      <c r="F67" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="G67" s="124" t="s">
+      <c r="G67" s="109" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2921,7 +2918,7 @@
         <v>63</v>
       </c>
       <c r="E68" s="75"/>
-      <c r="F68" s="125" t="s">
+      <c r="F68" s="110" t="s">
         <v>7</v>
       </c>
       <c r="G68" s="32" t="s">
@@ -2966,17 +2963,17 @@
       <c r="G71" s="68"/>
     </row>
     <row r="72" spans="1:7" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="113" t="s">
+      <c r="A72" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="114"/>
-      <c r="C72" s="115"/>
-      <c r="D72" s="113" t="s">
+      <c r="B72" s="116"/>
+      <c r="C72" s="117"/>
+      <c r="D72" s="115" t="s">
         <v>173</v>
       </c>
-      <c r="E72" s="114"/>
-      <c r="F72" s="114"/>
-      <c r="G72" s="115"/>
+      <c r="E72" s="116"/>
+      <c r="F72" s="116"/>
+      <c r="G72" s="117"/>
     </row>
     <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="87" t="s">
@@ -3349,13 +3346,13 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A107" s="120" t="s">
+      <c r="A107" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="121"/>
-      <c r="C107" s="121"/>
-      <c r="D107" s="121"/>
-      <c r="E107" s="121"/>
+      <c r="B107" s="114"/>
+      <c r="C107" s="114"/>
+      <c r="D107" s="114"/>
+      <c r="E107" s="114"/>
       <c r="F107" s="36"/>
       <c r="G107" s="15"/>
     </row>
@@ -3412,15 +3409,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A2:C2"/>
     <mergeCell ref="A107:E107"/>
     <mergeCell ref="A72:C72"/>
     <mergeCell ref="D72:G72"/>
     <mergeCell ref="A43:E43"/>
     <mergeCell ref="D13:G13"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>

</xml_diff>

<commit_message>
beta export contract template ready
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE10A4B-1A54-4575-8FD9-5B7E89259853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378BE253-AEE2-4FE3-8CF9-8F2572D5ED9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14497" yWindow="16103" windowWidth="28994" windowHeight="15794" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="5520" yWindow="3180" windowWidth="14400" windowHeight="8100" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="175">
   <si>
     <t>COMMERCIAL INVOICE</t>
   </si>
@@ -429,9 +429,6 @@
   </si>
   <si>
     <t>МФТ "Морской Волк"</t>
-  </si>
-  <si>
-    <t>Страна происхождения России</t>
   </si>
   <si>
     <t>ИТОГ:</t>
@@ -633,9 +630,6 @@
     <t>Покупатель/Buyer ________________________SE JI YOUNG</t>
   </si>
   <si>
-    <t>Пусан, Корея</t>
-  </si>
-  <si>
     <t>2.2. Общая сумма настоящего Дополнения составляет 
 $33 547,50 Тридцать три тысячи пятьсот сорок восемь долларов 50 центов</t>
   </si>
@@ -684,6 +678,15 @@
   </si>
   <si>
     <t>7, Chungjang-daero, Jung-gu, Busan, Republic of Korea (Jungang-dong-4</t>
+  </si>
+  <si>
+    <t>Страна происхождения Россия</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Порт тут быть большой может </t>
+  </si>
+  <si>
+    <t>Пусан, Корея Южная</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1020,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1333,21 +1336,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1357,26 +1381,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1721,14 +1727,14 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" s="3"/>
       <c r="N1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
@@ -1736,48 +1742,48 @@
         <v>24</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="3"/>
       <c r="N2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="45" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H3" s="47"/>
       <c r="N3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="N4" t="s">
         <v>104</v>
-      </c>
-      <c r="N4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="50" t="s">
         <v>106</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>107</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B6" s="51" t="s">
         <v>62</v>
@@ -1793,26 +1799,26 @@
     </row>
     <row r="8" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="50" t="s">
         <v>110</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -1833,49 +1839,49 @@
     </row>
     <row r="13" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="48" t="s">
         <v>113</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="53" t="s">
         <v>115</v>
-      </c>
-      <c r="B15" s="53" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M17" s="55"/>
       <c r="N17" t="s">
         <v>37</v>
       </c>
       <c r="O17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P17" t="s">
         <v>38</v>
@@ -1893,111 +1899,111 @@
         <v>33547.5</v>
       </c>
       <c r="U17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="53" t="s">
         <v>121</v>
-      </c>
-      <c r="B18" s="53" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="26.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="48" t="s">
         <v>123</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="26.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="54" t="s">
         <v>125</v>
-      </c>
-      <c r="B20" s="54" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="45.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="52" t="s">
         <v>127</v>
-      </c>
-      <c r="B22" s="52" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="48" t="s">
         <v>129</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="41.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="48" t="s">
         <v>131</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="101" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="101" t="s">
         <v>133</v>
-      </c>
-      <c r="B25" s="101" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="55.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="60" t="s">
         <v>135</v>
-      </c>
-      <c r="B26" s="60" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="53" t="s">
         <v>137</v>
-      </c>
-      <c r="B27" s="53" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="48" t="s">
         <v>139</v>
-      </c>
-      <c r="B28" s="48" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="53" t="s">
         <v>141</v>
-      </c>
-      <c r="B29" s="53" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -2018,10 +2024,10 @@
     </row>
     <row r="33" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" s="48" t="s">
         <v>144</v>
-      </c>
-      <c r="B33" s="48" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -2045,23 +2051,23 @@
         <v>57</v>
       </c>
       <c r="B36" s="48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="48" t="s">
         <v>147</v>
-      </c>
-      <c r="B37" s="48" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="51" t="s">
         <v>110</v>
-      </c>
-      <c r="B38" s="51" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -2082,58 +2088,58 @@
     </row>
     <row r="41" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B41" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B42" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B43" s="48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B44" s="48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B45" s="48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B46" s="57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="58" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="58" t="s">
         <v>155</v>
-      </c>
-      <c r="B47" s="58" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2172,8 +2178,8 @@
   </sheetPr>
   <dimension ref="A1:Z112"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A74" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A69" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2206,11 +2212,11 @@
       <c r="G1" s="81"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
       <c r="D2" s="102" t="s">
         <v>2</v>
       </c>
@@ -2226,8 +2232,8 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="61" t="s">
-        <v>169</v>
+      <c r="A3" s="128" t="s">
+        <v>167</v>
       </c>
       <c r="B3" s="62"/>
       <c r="C3" s="42"/>
@@ -2246,13 +2252,13 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="128" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="125"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="120"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2289,17 +2295,17 @@
       <c r="G6" s="68"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="121" t="s">
-        <v>168</v>
-      </c>
-      <c r="B7" s="122"/>
-      <c r="C7" s="123"/>
-      <c r="D7" s="115" t="s">
+      <c r="A7" s="113" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="114"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="117"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="117"/>
+      <c r="G7" s="118"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2346,9 +2352,9 @@
       <c r="F10" s="62"/>
       <c r="G10" s="68"/>
     </row>
-    <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:26" ht="34.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
-        <v>1</v>
+        <v>173</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>25</v>
@@ -2363,7 +2369,7 @@
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="64" t="s">
@@ -2376,12 +2382,12 @@
     <row r="13" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="8"/>
       <c r="C13" s="15"/>
-      <c r="D13" s="118" t="s">
+      <c r="D13" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="119"/>
-      <c r="F13" s="119"/>
-      <c r="G13" s="120"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
+      <c r="G13" s="127"/>
     </row>
     <row r="14" spans="1:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="103" t="s">
@@ -2738,13 +2744,13 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="113" t="s">
+      <c r="A43" s="123" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="114"/>
-      <c r="C43" s="114"/>
-      <c r="D43" s="114"/>
-      <c r="E43" s="114"/>
+      <c r="B43" s="124"/>
+      <c r="C43" s="124"/>
+      <c r="D43" s="124"/>
+      <c r="E43" s="124"/>
       <c r="F43" s="36"/>
       <c r="G43" s="15"/>
     </row>
@@ -2963,17 +2969,17 @@
       <c r="G71" s="68"/>
     </row>
     <row r="72" spans="1:7" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="115" t="s">
+      <c r="A72" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="116"/>
-      <c r="C72" s="117"/>
-      <c r="D72" s="115" t="s">
-        <v>173</v>
-      </c>
-      <c r="E72" s="116"/>
-      <c r="F72" s="116"/>
-      <c r="G72" s="117"/>
+      <c r="B72" s="117"/>
+      <c r="C72" s="118"/>
+      <c r="D72" s="116" t="s">
+        <v>171</v>
+      </c>
+      <c r="E72" s="117"/>
+      <c r="F72" s="117"/>
+      <c r="G72" s="118"/>
     </row>
     <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="87" t="s">
@@ -3020,9 +3026,9 @@
       <c r="F75" s="62"/>
       <c r="G75" s="68"/>
     </row>
-    <row r="76" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="69" t="s">
-        <v>157</v>
+    <row r="76" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A76" s="16" t="s">
+        <v>174</v>
       </c>
       <c r="B76" s="70" t="s">
         <v>76</v>
@@ -3037,7 +3043,7 @@
     </row>
     <row r="77" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C77" s="20"/>
       <c r="D77" s="64" t="s">
@@ -3309,7 +3315,7 @@
     </row>
     <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="98" t="s">
-        <v>91</v>
+        <v>172</v>
       </c>
       <c r="B104" s="99"/>
       <c r="C104" s="99"/>
@@ -3332,27 +3338,27 @@
     <row r="106" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A106" s="33"/>
       <c r="B106" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C106" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="C106" s="34" t="s">
+      <c r="D106" s="35" t="s">
         <v>93</v>
-      </c>
-      <c r="D106" s="35" t="s">
-        <v>94</v>
       </c>
       <c r="F106" s="36"/>
       <c r="G106" s="37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A107" s="113" t="s">
+      <c r="A107" s="123" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="114"/>
-      <c r="C107" s="114"/>
-      <c r="D107" s="114"/>
-      <c r="E107" s="114"/>
+      <c r="B107" s="124"/>
+      <c r="C107" s="124"/>
+      <c r="D107" s="124"/>
+      <c r="E107" s="124"/>
       <c r="F107" s="36"/>
       <c r="G107" s="15"/>
     </row>
@@ -3363,7 +3369,7 @@
       <c r="B108" s="77"/>
       <c r="C108" s="77"/>
       <c r="D108" s="78" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E108" s="79"/>
       <c r="F108" s="79"/>
@@ -3389,7 +3395,7 @@
     </row>
     <row r="111" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B111" s="75"/>
       <c r="C111" s="75"/>

</xml_diff>

<commit_message>
refactoring application (now sps initializing directly in rows) + tostr object in row implementation working on
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378BE253-AEE2-4FE3-8CF9-8F2572D5ED9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61012236-15B3-4B18-821E-B11E3C097FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="3180" windowWidth="14400" windowHeight="8100" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="21345" yWindow="16755" windowWidth="15488" windowHeight="15007" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -686,7 +686,7 @@
     <t xml:space="preserve">Порт тут быть большой может </t>
   </si>
   <si>
-    <t>Пусан, Корея Южная</t>
+    <t>Пусан, Корея Южная(хуюжная)</t>
   </si>
 </sst>
 </file>
@@ -1336,6 +1336,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1380,9 +1383,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2178,13 +2178,13 @@
   </sheetPr>
   <dimension ref="A1:Z112"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A69" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.53125" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
@@ -2212,11 +2212,11 @@
       <c r="G1" s="81"/>
     </row>
     <row r="2" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
       <c r="D2" s="102" t="s">
         <v>2</v>
       </c>
@@ -2232,7 +2232,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="113" t="s">
         <v>167</v>
       </c>
       <c r="B3" s="62"/>
@@ -2252,13 +2252,13 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="128" t="s">
+      <c r="A4" s="113" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="121"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="Q4">
@@ -2295,17 +2295,17 @@
       <c r="G6" s="68"/>
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="114" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="114"/>
-      <c r="C7" s="115"/>
-      <c r="D7" s="116" t="s">
+      <c r="B7" s="115"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="118"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="119"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
@@ -2382,12 +2382,12 @@
     <row r="13" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="8"/>
       <c r="C13" s="15"/>
-      <c r="D13" s="125" t="s">
+      <c r="D13" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="126"/>
-      <c r="F13" s="126"/>
-      <c r="G13" s="127"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
+      <c r="G13" s="128"/>
     </row>
     <row r="14" spans="1:26" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="103" t="s">
@@ -2744,13 +2744,13 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="123" t="s">
+      <c r="A43" s="124" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="124"/>
-      <c r="C43" s="124"/>
-      <c r="D43" s="124"/>
-      <c r="E43" s="124"/>
+      <c r="B43" s="125"/>
+      <c r="C43" s="125"/>
+      <c r="D43" s="125"/>
+      <c r="E43" s="125"/>
       <c r="F43" s="36"/>
       <c r="G43" s="15"/>
     </row>
@@ -2969,17 +2969,17 @@
       <c r="G71" s="68"/>
     </row>
     <row r="72" spans="1:7" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="116" t="s">
+      <c r="A72" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="117"/>
-      <c r="C72" s="118"/>
-      <c r="D72" s="116" t="s">
+      <c r="B72" s="118"/>
+      <c r="C72" s="119"/>
+      <c r="D72" s="117" t="s">
         <v>171</v>
       </c>
-      <c r="E72" s="117"/>
-      <c r="F72" s="117"/>
-      <c r="G72" s="118"/>
+      <c r="E72" s="118"/>
+      <c r="F72" s="118"/>
+      <c r="G72" s="119"/>
     </row>
     <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="87" t="s">
@@ -3352,13 +3352,13 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A107" s="123" t="s">
+      <c r="A107" s="124" t="s">
         <v>52</v>
       </c>
-      <c r="B107" s="124"/>
-      <c r="C107" s="124"/>
-      <c r="D107" s="124"/>
-      <c r="E107" s="124"/>
+      <c r="B107" s="125"/>
+      <c r="C107" s="125"/>
+      <c r="D107" s="125"/>
+      <c r="E107" s="125"/>
       <c r="F107" s="36"/>
       <c r="G107" s="15"/>
     </row>

</xml_diff>

<commit_message>
to str obj canceled, now com invoice initializing in setcominvoices.ts file
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61012236-15B3-4B18-821E-B11E3C097FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA44FD19-DD0B-4DB8-A68C-CC5CCFF996B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21345" yWindow="16755" windowWidth="15488" windowHeight="15007" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="41183" yWindow="2663" windowWidth="28995" windowHeight="15794" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -2178,14 +2178,14 @@
   </sheetPr>
   <dimension ref="A1:Z112"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.53125" customWidth="1"/>
-    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="1" max="1" width="14.06640625" customWidth="1"/>
+    <col min="2" max="2" width="37.46484375" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>

</xml_diff>

<commit_message>
template Request Contract Ru added, work on inner Route in progress
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA44FD19-DD0B-4DB8-A68C-CC5CCFF996B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03849501-4B72-4140-BD5A-D19D387DB474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41183" yWindow="2663" windowWidth="28995" windowHeight="15794" activeTab="1" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="-35123" yWindow="3195" windowWidth="11400" windowHeight="6000" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -446,9 +446,6 @@
     <t>в пользу  ООО "Тихоокеанская рыбопромышленная компания"</t>
   </si>
   <si>
-    <t>ДОПОЛНЕНИЕ № 146 от 10 марта 2023г.</t>
-  </si>
-  <si>
     <t>278-144</t>
   </si>
   <si>
@@ -638,9 +635,6 @@
 USD 33 547,50 (Thirty three thousand five hundred forty eight US Dollars 50 Cents)</t>
   </si>
   <si>
-    <t>AGREEMENT No. 146 dated March 10, 2023</t>
-  </si>
-  <si>
     <t>Magadan, dated July 10, 2019</t>
   </si>
   <si>
@@ -687,6 +681,12 @@
   </si>
   <si>
     <t>Пусан, Корея Южная(хуюжная)</t>
+  </si>
+  <si>
+    <t>Supplementary Agreement No. 146 dated March 10, 2023</t>
+  </si>
+  <si>
+    <t>Дополнительное соглашение № 146 от 10 марта 2023г.</t>
   </si>
 </sst>
 </file>
@@ -1704,8 +1704,8 @@
   </sheetPr>
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="81" zoomScaleNormal="100" zoomScaleSheetLayoutView="81" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="81" zoomScaleNormal="100" zoomScaleSheetLayoutView="81" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1727,14 +1727,14 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="43" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>96</v>
+        <v>174</v>
       </c>
       <c r="D1" s="3"/>
       <c r="N1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
@@ -1742,48 +1742,48 @@
         <v>24</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="3"/>
       <c r="N2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="45" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H3" s="47"/>
       <c r="N3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="N4" t="s">
         <v>103</v>
-      </c>
-      <c r="N4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="50" t="s">
         <v>105</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>106</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B6" s="51" t="s">
         <v>62</v>
@@ -1799,26 +1799,26 @@
     </row>
     <row r="8" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="50" t="s">
         <v>109</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -1839,49 +1839,49 @@
     </row>
     <row r="13" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="48" t="s">
         <v>112</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="53" t="s">
         <v>114</v>
-      </c>
-      <c r="B15" s="53" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M17" s="55"/>
       <c r="N17" t="s">
         <v>37</v>
       </c>
       <c r="O17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P17" t="s">
         <v>38</v>
@@ -1899,111 +1899,111 @@
         <v>33547.5</v>
       </c>
       <c r="U17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="53" t="s">
         <v>120</v>
-      </c>
-      <c r="B18" s="53" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="26.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="48" t="s">
         <v>122</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="26.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="54" t="s">
         <v>124</v>
-      </c>
-      <c r="B20" s="54" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="45.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="52" t="s">
         <v>126</v>
-      </c>
-      <c r="B22" s="52" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="48" t="s">
         <v>128</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="41.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="48" t="s">
         <v>130</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="101" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="101" t="s">
         <v>132</v>
-      </c>
-      <c r="B25" s="101" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="55.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="60" t="s">
         <v>134</v>
-      </c>
-      <c r="B26" s="60" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="53" t="s">
         <v>136</v>
-      </c>
-      <c r="B27" s="53" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="48" t="s">
         <v>138</v>
-      </c>
-      <c r="B28" s="48" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="21.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="53" t="s">
         <v>140</v>
-      </c>
-      <c r="B29" s="53" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -2024,10 +2024,10 @@
     </row>
     <row r="33" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="48" t="s">
         <v>143</v>
-      </c>
-      <c r="B33" s="48" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -2051,23 +2051,23 @@
         <v>57</v>
       </c>
       <c r="B36" s="48" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" s="48" t="s">
         <v>146</v>
-      </c>
-      <c r="B37" s="48" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="51" t="s">
         <v>109</v>
-      </c>
-      <c r="B38" s="51" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
@@ -2088,58 +2088,58 @@
     </row>
     <row r="41" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B41" s="48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B42" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B43" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B44" s="48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B45" s="48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B46" s="57" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="B47" s="58" t="s">
         <v>154</v>
-      </c>
-      <c r="B47" s="58" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="13.05" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2178,7 +2178,7 @@
   </sheetPr>
   <dimension ref="A1:Z112"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="113" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B3" s="62"/>
       <c r="C3" s="42"/>
@@ -2296,7 +2296,7 @@
     </row>
     <row r="7" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="114" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B7" s="115"/>
       <c r="C7" s="116"/>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="11" spans="1:26" ht="34.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>25</v>
@@ -2369,7 +2369,7 @@
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="64" t="s">
@@ -2975,7 +2975,7 @@
       <c r="B72" s="118"/>
       <c r="C72" s="119"/>
       <c r="D72" s="117" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E72" s="118"/>
       <c r="F72" s="118"/>
@@ -3028,7 +3028,7 @@
     </row>
     <row r="76" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B76" s="70" t="s">
         <v>76</v>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="77" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C77" s="20"/>
       <c r="D77" s="64" t="s">
@@ -3315,7 +3315,7 @@
     </row>
     <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="98" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B104" s="99"/>
       <c r="C104" s="99"/>
@@ -3369,7 +3369,7 @@
       <c r="B108" s="77"/>
       <c r="C108" s="77"/>
       <c r="D108" s="78" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E108" s="79"/>
       <c r="F108" s="79"/>

</xml_diff>

<commit_message>
refactored export contract tmp structure, cells comonized in getExportContractCells fn
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AD6ED3-6C6E-4378-995F-C33915FF81D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBB16FF-9A6B-492A-B55F-AD2D67B62AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="16395" xr2:uid="{ABD52FE1-B0FA-4F1F-8DD6-2BC65DEFB27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="2" r:id="rId1"/>
@@ -1656,8 +1656,8 @@
   </sheetPr>
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A27" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="140" zoomScaleNormal="100" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2379,8 +2379,8 @@
   </sheetPr>
   <dimension ref="A2:AB129"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A61" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A18" zoomScale="106" zoomScaleNormal="70" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
mergeCoppiedCells (if worksheet is coppied multiple times) mechanism implementation beta ready
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A033E5-9E46-410A-A5C9-4475A0AE1F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74233516-7D8C-4510-91E9-6F74BBE52C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16995" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Com_Invoice" sheetId="3" r:id="rId1"/>
-    <sheet name="Export_Contract" sheetId="1" r:id="rId2"/>
+    <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
+    <sheet name="Invoice" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Com_Invoice!$A$2:$M$52</definedName>
     <definedName name="Seal_agent_end">Export_Contract!$H$51</definedName>
     <definedName name="Seal_agent_start">Export_Contract!$G$41</definedName>
     <definedName name="Seal_seller_end">Export_Contract!$C$51</definedName>
@@ -43,103 +42,33 @@
     <definedName name="Адреса_продавец_адрес">Export_Contract!$B$32</definedName>
     <definedName name="Доставка_порт">Export_Contract!$B$25</definedName>
     <definedName name="Доставка_условия">Export_Contract!$B$24</definedName>
-    <definedName name="Инвойс" localSheetId="0">Com_Invoice!$B$2</definedName>
-    <definedName name="Инвойс">#REF!</definedName>
-    <definedName name="Инвойс_Bl_массив" localSheetId="0">Com_Invoice!$B$23</definedName>
-    <definedName name="Инвойс_Bl_массив">#REF!</definedName>
-    <definedName name="Инвойс_Bl_массив_п">#REF!</definedName>
-    <definedName name="Инвойс_банк_получателя" localSheetId="0">Com_Invoice!$B$38</definedName>
-    <definedName name="Инвойс_банк_получателя">#REF!</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес" localSheetId="0">Com_Invoice!$B$39</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес">#REF!</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес_п">#REF!</definedName>
-    <definedName name="Инвойс_банк_получателя_п">#REF!</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт" localSheetId="0">Com_Invoice!$B$40</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт">#REF!</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт_п">#REF!</definedName>
-    <definedName name="Инвойс_всего">#REF!</definedName>
-    <definedName name="Инвойс_всего_п">#REF!</definedName>
-    <definedName name="Инвойс_дата" localSheetId="0">Com_Invoice!$B$5</definedName>
-    <definedName name="Инвойс_дата">#REF!</definedName>
-    <definedName name="Инвойс_дата_отправки">Com_Invoice!$F$20</definedName>
-    <definedName name="Инвойс_дата_п">#REF!</definedName>
-    <definedName name="Инвойс_декларация" localSheetId="0">Com_Invoice!$D$20</definedName>
-    <definedName name="Инвойс_декларация">#REF!</definedName>
-    <definedName name="Инвойс_декларация_п">#REF!</definedName>
-    <definedName name="Инвойс_изготовитель">Com_Invoice!$B$16</definedName>
-    <definedName name="Инвойс_контракт" localSheetId="0">Com_Invoice!$B$4</definedName>
-    <definedName name="Инвойс_контракт">#REF!</definedName>
-    <definedName name="Инвойс_контракт_дата">#REF!</definedName>
-    <definedName name="Инвойс_контракт_дата_п">#REF!</definedName>
-    <definedName name="Инвойс_контракт_п">#REF!</definedName>
-    <definedName name="Инвойс_куда" localSheetId="0">Com_Invoice!$D$18</definedName>
-    <definedName name="Инвойс_куда">#REF!</definedName>
-    <definedName name="Инвойс_куда_п">#REF!</definedName>
-    <definedName name="Инвойс_места">#REF!</definedName>
-    <definedName name="Инвойс_места_п">#REF!</definedName>
-    <definedName name="Инвойс_МСЦ">Com_Invoice!$D$16</definedName>
-    <definedName name="Инвойс_откуда" localSheetId="0">Com_Invoice!$F$18</definedName>
-    <definedName name="Инвойс_откуда">#REF!</definedName>
-    <definedName name="Инвойс_откуда_п">#REF!</definedName>
-    <definedName name="Инвойс_п">#REF!</definedName>
-    <definedName name="Инвойс_подвал_всего">#REF!</definedName>
-    <definedName name="Инвойс_подвал_всего_п">#REF!</definedName>
-    <definedName name="Инвойс_подвал_места">#REF!</definedName>
-    <definedName name="Инвойс_подвал_места_п">#REF!</definedName>
-    <definedName name="Инвойс_подвал_сумма">#REF!</definedName>
-    <definedName name="Инвойс_подвал_сумма_п">#REF!</definedName>
-    <definedName name="Инвойс_подписант" localSheetId="0">Com_Invoice!$H$38</definedName>
-    <definedName name="Инвойс_подписант">#REF!</definedName>
-    <definedName name="Инвойс_подписант_п">#REF!</definedName>
-    <definedName name="Инвойс_покупатель" localSheetId="0">Com_Invoice!$B$10</definedName>
-    <definedName name="Инвойс_покупатель">#REF!</definedName>
-    <definedName name="Инвойс_покупатель_адрес" localSheetId="0">Com_Invoice!$B$11</definedName>
-    <definedName name="Инвойс_покупатель_адрес">#REF!</definedName>
-    <definedName name="Инвойс_покупатель_адрес_п">#REF!</definedName>
-    <definedName name="Инвойс_покупатель_п">#REF!</definedName>
-    <definedName name="Инвойс_получатель" localSheetId="0">Com_Invoice!$B$13</definedName>
-    <definedName name="Инвойс_получатель">#REF!</definedName>
-    <definedName name="Инвойс_получатель_адрес" localSheetId="0">Com_Invoice!$B$14</definedName>
-    <definedName name="Инвойс_получатель_адрес">#REF!</definedName>
-    <definedName name="Инвойс_получатель_адрес_п">#REF!</definedName>
-    <definedName name="Инвойс_получатель_в_пользу" localSheetId="0">Com_Invoice!$B$41</definedName>
-    <definedName name="Инвойс_получатель_в_пользу">#REF!</definedName>
-    <definedName name="Инвойс_получатель_в_пользу_п">#REF!</definedName>
-    <definedName name="Инвойс_получатель_п">#REF!</definedName>
-    <definedName name="Инвойс_получатель_счет" localSheetId="0">Com_Invoice!$B$42</definedName>
-    <definedName name="Инвойс_получатель_счет">#REF!</definedName>
-    <definedName name="Инвойс_получатель_счет_п">#REF!</definedName>
-    <definedName name="Инвойс_продавец" localSheetId="0">Com_Invoice!$B$7</definedName>
-    <definedName name="Инвойс_продавец">#REF!</definedName>
-    <definedName name="Инвойс_продавец_адрес" localSheetId="0">Com_Invoice!$B$8</definedName>
-    <definedName name="Инвойс_продавец_адрес">#REF!</definedName>
-    <definedName name="Инвойс_продавец_адрес_п">#REF!</definedName>
-    <definedName name="Инвойс_продавец_п">#REF!</definedName>
-    <definedName name="Инвойс_продукт">#REF!</definedName>
-    <definedName name="Инвойс_продукт_п">#REF!</definedName>
-    <definedName name="Инвойс_соглашение" localSheetId="0">Com_Invoice!$B$3</definedName>
-    <definedName name="Инвойс_соглашение">#REF!</definedName>
-    <definedName name="Инвойс_соглашение_п">#REF!</definedName>
-    <definedName name="Инвойс_судно">#REF!</definedName>
-    <definedName name="Инвойс_судно_п">#REF!</definedName>
-    <definedName name="Инвойс_сумма">#REF!</definedName>
-    <definedName name="Инвойс_сумма_п">#REF!</definedName>
-    <definedName name="Инвойс_транспорт" localSheetId="0">Com_Invoice!$B$18</definedName>
-    <definedName name="Инвойс_транспорт">#REF!</definedName>
-    <definedName name="Инвойс_транспорт_п">#REF!</definedName>
-    <definedName name="Инвойс_упаковка">#REF!</definedName>
-    <definedName name="Инвойс_упаковка_п">#REF!</definedName>
-    <definedName name="Инвойс_условия" localSheetId="0">Com_Invoice!$B$20</definedName>
-    <definedName name="Инвойс_условия">#REF!</definedName>
-    <definedName name="Инвойс_условия_п">#REF!</definedName>
-    <definedName name="Инвойс_цена">#REF!</definedName>
-    <definedName name="Инвойс_цена_п">#REF!</definedName>
+    <definedName name="Инвойс">Invoice!$B$2</definedName>
+    <definedName name="Инвойс_Bl_массив">Invoice!$B$23</definedName>
+    <definedName name="Инвойс_банк_получателя">Invoice!$B$38</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес">Invoice!$B$39</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт">Invoice!$B$40</definedName>
+    <definedName name="Инвойс_дата">Invoice!$B$5</definedName>
+    <definedName name="Инвойс_дата_отправки">Invoice!$F$20</definedName>
+    <definedName name="Инвойс_декларация">Invoice!$D$20</definedName>
+    <definedName name="Инвойс_изготовитель">Invoice!$B$16</definedName>
+    <definedName name="Инвойс_контракт">Invoice!$B$4</definedName>
+    <definedName name="Инвойс_куда">Invoice!$D$18</definedName>
+    <definedName name="Инвойс_МСЦ">Invoice!$D$16</definedName>
+    <definedName name="Инвойс_откуда">Invoice!$F$18</definedName>
+    <definedName name="Инвойс_подписант">Invoice!$I$38</definedName>
+    <definedName name="Инвойс_покупатель">Invoice!$B$10</definedName>
+    <definedName name="Инвойс_покупатель_адрес">Invoice!$B$11</definedName>
+    <definedName name="Инвойс_получатель">Invoice!$B$13</definedName>
+    <definedName name="Инвойс_получатель_адрес">Invoice!$B$14</definedName>
+    <definedName name="Инвойс_получатель_в_пользу">Invoice!$B$41</definedName>
+    <definedName name="Инвойс_получатель_счет">Invoice!$B$42</definedName>
+    <definedName name="Инвойс_продавец">Invoice!$B$7</definedName>
+    <definedName name="Инвойс_продавец_адрес">Invoice!$B$8</definedName>
+    <definedName name="Инвойс_соглашение">Invoice!$B$3</definedName>
+    <definedName name="Инвойс_транспорт">Invoice!$B$18</definedName>
+    <definedName name="Инвойс_условия">Invoice!$B$20</definedName>
     <definedName name="Контракт">Export_Contract!$B$2</definedName>
     <definedName name="Контракт_дата">Export_Contract!$B$3</definedName>
-    <definedName name="МСЦ">#REF!</definedName>
-    <definedName name="МСЦ_п">#REF!</definedName>
-    <definedName name="МСЦ_сертификат">#REF!</definedName>
-    <definedName name="МСЦ_сертификат_п">#REF!</definedName>
     <definedName name="Покупатель">Export_Contract!$B$11</definedName>
     <definedName name="Покупатель_адрес">Export_Contract!$B$12</definedName>
     <definedName name="Покупатель_представитель">Export_Contract!$B$13</definedName>
@@ -514,9 +443,6 @@
     <t>10702070/180923/3382666</t>
   </si>
   <si>
-    <t>Условия доставки и оплаты</t>
-  </si>
-  <si>
     <t>№ временной декларации на товары:</t>
   </si>
   <si>
@@ -623,6 +549,9 @@
   </si>
   <si>
     <t>Покупатель:</t>
+  </si>
+  <si>
+    <t>Условия доставки и оплаты:</t>
   </si>
 </sst>
 </file>
@@ -927,7 +856,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="207">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1088,9 +1017,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1147,9 +1073,6 @@
     <xf numFmtId="3" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1162,40 +1085,10 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1206,286 +1099,14 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1494,14 +1115,292 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1862,888 +1761,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBB9FB0-5253-4E0F-9002-2C89C8553DAA}">
-  <sheetPr>
-    <tabColor theme="8" tint="-0.249977111117893"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:AB52"/>
-  <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:F23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="1" customWidth="1"/>
-    <col min="2" max="2" width="11.73046875" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="14.3984375" customWidth="1"/>
-    <col min="5" max="5" width="8.46484375" customWidth="1"/>
-    <col min="6" max="6" width="19.86328125" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.19921875" customWidth="1"/>
-    <col min="10" max="10" width="5.59765625" customWidth="1"/>
-    <col min="11" max="11" width="7.1328125" customWidth="1"/>
-    <col min="12" max="12" width="15.53125" customWidth="1"/>
-    <col min="13" max="13" width="0.59765625" customWidth="1"/>
-    <col min="14" max="17" width="9.1328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="0.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="56"/>
-      <c r="M1" s="58"/>
-    </row>
-    <row r="2" spans="1:13" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="103"/>
-      <c r="B2" s="108" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="107" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="58"/>
-    </row>
-    <row r="3" spans="1:13" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="103"/>
-      <c r="B3" s="195" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="114" t="s">
-        <v>138</v>
-      </c>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="58"/>
-    </row>
-    <row r="4" spans="1:13" s="100" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="102"/>
-      <c r="B4" s="109" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="111" t="s">
-        <v>136</v>
-      </c>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="90"/>
-    </row>
-    <row r="5" spans="1:13" s="100" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="101"/>
-      <c r="B5" s="112" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="113" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="90"/>
-    </row>
-    <row r="6" spans="1:13" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="56"/>
-      <c r="B6" s="104" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="96" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="58"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="56"/>
-      <c r="B7" s="105" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="58"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="56"/>
-      <c r="B8" s="106" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="106"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="106"/>
-      <c r="G8" s="99" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="58"/>
-    </row>
-    <row r="9" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="56"/>
-      <c r="B9" s="104" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="104"/>
-      <c r="D9" s="104"/>
-      <c r="E9" s="104"/>
-      <c r="F9" s="104"/>
-      <c r="G9" s="97" t="s">
-        <v>142</v>
-      </c>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="93"/>
-      <c r="L9" s="93"/>
-      <c r="M9" s="58"/>
-    </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="56"/>
-      <c r="B10" s="105" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="93"/>
-      <c r="L10" s="93"/>
-      <c r="M10" s="58"/>
-    </row>
-    <row r="11" spans="1:13" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="56"/>
-      <c r="B11" s="106" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="106"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="117" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="106"/>
-      <c r="I11" s="106"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="106"/>
-      <c r="L11" s="106"/>
-      <c r="M11" s="58"/>
-    </row>
-    <row r="12" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="56"/>
-      <c r="B12" s="104" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="104"/>
-      <c r="D12" s="104"/>
-      <c r="E12" s="104"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="96" t="s">
-        <v>131</v>
-      </c>
-      <c r="H12" s="95"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="95"/>
-      <c r="K12" s="93"/>
-      <c r="L12" s="93"/>
-      <c r="M12" s="58"/>
-    </row>
-    <row r="13" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="56"/>
-      <c r="B13" s="105" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="94"/>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="93"/>
-      <c r="M13" s="58"/>
-    </row>
-    <row r="14" spans="1:13" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="56"/>
-      <c r="B14" s="106" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="106"/>
-      <c r="D14" s="106"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="106"/>
-      <c r="G14" s="117" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="106"/>
-      <c r="I14" s="106"/>
-      <c r="J14" s="106"/>
-      <c r="K14" s="106"/>
-      <c r="L14" s="106"/>
-      <c r="M14" s="58"/>
-    </row>
-    <row r="15" spans="1:13" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="92"/>
-      <c r="B15" s="177" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" s="177"/>
-      <c r="D15" s="178" t="s">
-        <v>115</v>
-      </c>
-      <c r="E15" s="178"/>
-      <c r="F15" s="178" t="s">
-        <v>118</v>
-      </c>
-      <c r="G15" s="176" t="s">
-        <v>117</v>
-      </c>
-      <c r="H15" s="178"/>
-      <c r="I15" s="179" t="s">
-        <v>115</v>
-      </c>
-      <c r="J15" s="179"/>
-      <c r="K15" s="180" t="s">
-        <v>116</v>
-      </c>
-      <c r="L15" s="180"/>
-      <c r="M15" s="58"/>
-    </row>
-    <row r="16" spans="1:13" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="56"/>
-      <c r="B16" s="193" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="193"/>
-      <c r="D16" s="87" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="89"/>
-      <c r="F16" s="89" t="s">
-        <v>114</v>
-      </c>
-      <c r="G16" s="91" t="s">
-        <v>112</v>
-      </c>
-      <c r="H16" s="89"/>
-      <c r="I16" s="168" t="s">
-        <v>110</v>
-      </c>
-      <c r="J16" s="168"/>
-      <c r="K16" s="167" t="s">
-        <v>111</v>
-      </c>
-      <c r="L16" s="167"/>
-      <c r="M16" s="58"/>
-    </row>
-    <row r="17" spans="1:28" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="56"/>
-      <c r="B17" s="170" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" s="171"/>
-      <c r="D17" s="171" t="s">
-        <v>129</v>
-      </c>
-      <c r="E17" s="169"/>
-      <c r="F17" s="187" t="s">
-        <v>128</v>
-      </c>
-      <c r="G17" s="172" t="s">
-        <v>127</v>
-      </c>
-      <c r="H17" s="173"/>
-      <c r="I17" s="172" t="s">
-        <v>126</v>
-      </c>
-      <c r="J17" s="173"/>
-      <c r="K17" s="174" t="s">
-        <v>125</v>
-      </c>
-      <c r="L17" s="175"/>
-      <c r="M17" s="58"/>
-    </row>
-    <row r="18" spans="1:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="56"/>
-      <c r="B18" s="194" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="194"/>
-      <c r="D18" s="185" t="s">
-        <v>123</v>
-      </c>
-      <c r="E18" s="185"/>
-      <c r="F18" s="188" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="185" t="s">
-        <v>122</v>
-      </c>
-      <c r="H18" s="128"/>
-      <c r="I18" s="118" t="s">
-        <v>121</v>
-      </c>
-      <c r="J18" s="118"/>
-      <c r="K18" s="127" t="s">
-        <v>120</v>
-      </c>
-      <c r="L18" s="127"/>
-      <c r="M18" s="58"/>
-    </row>
-    <row r="19" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="56"/>
-      <c r="B19" s="123" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" s="123"/>
-      <c r="D19" s="182" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="182"/>
-      <c r="F19" s="189"/>
-      <c r="G19" s="182" t="s">
-        <v>106</v>
-      </c>
-      <c r="H19" s="182"/>
-      <c r="I19" s="181" t="s">
-        <v>107</v>
-      </c>
-      <c r="J19" s="181"/>
-      <c r="K19" s="181"/>
-      <c r="L19" s="181"/>
-      <c r="M19" s="58"/>
-    </row>
-    <row r="20" spans="1:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="56"/>
-      <c r="B20" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="88"/>
-      <c r="D20" s="183" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="183"/>
-      <c r="F20" s="190"/>
-      <c r="G20" s="184" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" s="206"/>
-      <c r="I20" s="184" t="s">
-        <v>105</v>
-      </c>
-      <c r="J20" s="204"/>
-      <c r="K20" s="205"/>
-      <c r="L20" s="205"/>
-      <c r="M20" s="58"/>
-    </row>
-    <row r="21" spans="1:28" s="84" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="203"/>
-      <c r="B21" s="191"/>
-      <c r="C21" s="191"/>
-      <c r="D21" s="191"/>
-      <c r="E21" s="191"/>
-      <c r="F21" s="192"/>
-      <c r="G21" s="186"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="86"/>
-      <c r="J21" s="86"/>
-      <c r="K21" s="86"/>
-      <c r="M21" s="85"/>
-      <c r="R21"/>
-      <c r="S21"/>
-      <c r="T21"/>
-      <c r="U21"/>
-      <c r="V21"/>
-      <c r="W21"/>
-      <c r="X21"/>
-      <c r="Y21"/>
-      <c r="Z21"/>
-      <c r="AA21"/>
-      <c r="AB21"/>
-    </row>
-    <row r="22" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="56"/>
-      <c r="B22" s="61" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="126" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="126"/>
-      <c r="E22" s="126"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="61" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22" s="83" t="s">
-        <v>101</v>
-      </c>
-      <c r="I22" s="82" t="s">
-        <v>100</v>
-      </c>
-      <c r="J22" s="126" t="s">
-        <v>99</v>
-      </c>
-      <c r="K22" s="126"/>
-      <c r="L22" s="61" t="s">
-        <v>98</v>
-      </c>
-      <c r="M22" s="58"/>
-    </row>
-    <row r="23" spans="1:28" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="56"/>
-      <c r="B23" s="78" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="129" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="129"/>
-      <c r="E23" s="129"/>
-      <c r="F23" s="129"/>
-      <c r="G23" s="81" t="s">
-        <v>95</v>
-      </c>
-      <c r="H23" s="80" t="s">
-        <v>92</v>
-      </c>
-      <c r="I23" s="79">
-        <v>14</v>
-      </c>
-      <c r="J23" s="130" t="s">
-        <v>94</v>
-      </c>
-      <c r="K23" s="130"/>
-      <c r="L23" s="78" t="s">
-        <v>91</v>
-      </c>
-      <c r="M23" s="58"/>
-    </row>
-    <row r="24" spans="1:28" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="56"/>
-      <c r="B24" s="119" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="119"/>
-      <c r="D24" s="119"/>
-      <c r="E24" s="119"/>
-      <c r="F24" s="119"/>
-      <c r="G24" s="119"/>
-      <c r="H24" s="77" t="s">
-        <v>92</v>
-      </c>
-      <c r="I24" s="76">
-        <v>14</v>
-      </c>
-      <c r="J24" s="120" t="s">
-        <v>50</v>
-      </c>
-      <c r="K24" s="120"/>
-      <c r="L24" s="196" t="s">
-        <v>91</v>
-      </c>
-      <c r="M24" s="58"/>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A25" s="56"/>
-      <c r="B25" s="70"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="75"/>
-      <c r="I25" s="70"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="70"/>
-      <c r="L25" s="75"/>
-      <c r="M25" s="58"/>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A26" s="56"/>
-      <c r="B26" s="70"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="75"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="75"/>
-      <c r="M26" s="58"/>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A27" s="56"/>
-      <c r="B27" s="70"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="70"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="75"/>
-      <c r="M27" s="58"/>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A28" s="56"/>
-      <c r="B28" s="70"/>
-      <c r="C28" s="70"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="70"/>
-      <c r="J28" s="70"/>
-      <c r="K28" s="70"/>
-      <c r="L28" s="75"/>
-      <c r="M28" s="58"/>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A29" s="56"/>
-      <c r="B29" s="70"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="70"/>
-      <c r="J29" s="70"/>
-      <c r="K29" s="70"/>
-      <c r="L29" s="75"/>
-      <c r="M29" s="58"/>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A30" s="56"/>
-      <c r="B30" s="70"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="70"/>
-      <c r="J30" s="70"/>
-      <c r="K30" s="70"/>
-      <c r="L30" s="75"/>
-      <c r="M30" s="58"/>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A31" s="56"/>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="70"/>
-      <c r="J31" s="70"/>
-      <c r="K31" s="70"/>
-      <c r="L31" s="75"/>
-      <c r="M31" s="58"/>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A32" s="56"/>
-      <c r="B32" s="70"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="75"/>
-      <c r="I32" s="70"/>
-      <c r="J32" s="70"/>
-      <c r="K32" s="70"/>
-      <c r="L32" s="75"/>
-      <c r="M32" s="58"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A33" s="56"/>
-      <c r="B33" s="70"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="70"/>
-      <c r="J33" s="70"/>
-      <c r="K33" s="70"/>
-      <c r="L33" s="75"/>
-      <c r="M33" s="58"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A34" s="56"/>
-      <c r="B34" s="70"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="75"/>
-      <c r="M34" s="58"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A35" s="56"/>
-      <c r="B35" s="70"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="70"/>
-      <c r="L35" s="197"/>
-      <c r="M35" s="58"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A36" s="56"/>
-      <c r="B36" s="70"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="70"/>
-      <c r="J36" s="70"/>
-      <c r="K36" s="70"/>
-      <c r="L36" s="197"/>
-      <c r="M36" s="58"/>
-    </row>
-    <row r="37" spans="1:13" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="56"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="62"/>
-      <c r="I37" s="57"/>
-      <c r="J37" s="57"/>
-      <c r="K37" s="70"/>
-      <c r="L37" s="198"/>
-      <c r="M37" s="58"/>
-    </row>
-    <row r="38" spans="1:13" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="56"/>
-      <c r="B38" s="200" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="72"/>
-      <c r="H38" s="124" t="s">
-        <v>90</v>
-      </c>
-      <c r="I38" s="125"/>
-      <c r="J38" s="125"/>
-      <c r="K38" s="125"/>
-      <c r="L38" s="125"/>
-      <c r="M38" s="58"/>
-    </row>
-    <row r="39" spans="1:13" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="56"/>
-      <c r="B39" s="201" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" s="70"/>
-      <c r="D39" s="70"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="62"/>
-      <c r="H39" s="71"/>
-      <c r="I39" s="57"/>
-      <c r="J39" s="57"/>
-      <c r="K39" s="70"/>
-      <c r="L39" s="198"/>
-      <c r="M39" s="58"/>
-    </row>
-    <row r="40" spans="1:13" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="56"/>
-      <c r="B40" s="201" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="70"/>
-      <c r="D40" s="70"/>
-      <c r="E40" s="70"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="62"/>
-      <c r="H40" s="71"/>
-      <c r="I40" s="57"/>
-      <c r="J40" s="57"/>
-      <c r="K40" s="70"/>
-      <c r="L40" s="198"/>
-      <c r="M40" s="58"/>
-    </row>
-    <row r="41" spans="1:13" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="56"/>
-      <c r="B41" s="201" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="62"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="57"/>
-      <c r="J41" s="57"/>
-      <c r="K41" s="70"/>
-      <c r="L41" s="198"/>
-      <c r="M41" s="58"/>
-    </row>
-    <row r="42" spans="1:13" s="65" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="69"/>
-      <c r="B42" s="202" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="68"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="67"/>
-      <c r="G42" s="66"/>
-      <c r="H42" s="121"/>
-      <c r="I42" s="122"/>
-      <c r="J42" s="122"/>
-      <c r="K42" s="122"/>
-      <c r="L42" s="122"/>
-      <c r="M42" s="199"/>
-    </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="49" customFormat="1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="50" customFormat="1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="51" customFormat="1" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="52" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.45"/>
-  </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="G14:L14"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:L4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-  </mergeCells>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="71" fitToHeight="2" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BF4CFE-C418-488F-8DFD-13F601FB1BC8}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2791,18 +1808,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="161" t="s">
+      <c r="B1" s="186" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="161" t="s">
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="186" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="162"/>
-      <c r="H1" s="162"/>
-      <c r="I1" s="162"/>
+      <c r="G1" s="187"/>
+      <c r="H1" s="187"/>
+      <c r="I1" s="187"/>
       <c r="J1" s="9"/>
       <c r="L1" s="11"/>
       <c r="O1" s="10"/>
@@ -2819,18 +1836,18 @@
       <c r="Z1" s="10"/>
     </row>
     <row r="2" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="189" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="164" t="s">
+      <c r="C2" s="190"/>
+      <c r="D2" s="190"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="189" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="165"/>
+      <c r="G2" s="190"/>
+      <c r="H2" s="190"/>
+      <c r="I2" s="190"/>
       <c r="J2" s="9"/>
       <c r="L2" s="11"/>
       <c r="O2" s="10"/>
@@ -2847,18 +1864,18 @@
       <c r="Z2" s="10"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="164" t="s">
+      <c r="B3" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="165"/>
-      <c r="D3" s="165"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="164" t="s">
+      <c r="C3" s="190"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="191"/>
+      <c r="F3" s="189" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="165"/>
-      <c r="H3" s="165"/>
-      <c r="I3" s="165"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="190"/>
+      <c r="I3" s="190"/>
       <c r="J3" s="9"/>
       <c r="N3" s="13"/>
       <c r="O3" s="14"/>
@@ -2879,18 +1896,18 @@
       <c r="AD3" s="13"/>
     </row>
     <row r="4" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="158" t="s">
+      <c r="B4" s="183" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="159"/>
-      <c r="D4" s="159"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="158" t="s">
+      <c r="C4" s="184"/>
+      <c r="D4" s="184"/>
+      <c r="E4" s="185"/>
+      <c r="F4" s="183" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="159"/>
-      <c r="H4" s="159"/>
-      <c r="I4" s="159"/>
+      <c r="G4" s="184"/>
+      <c r="H4" s="184"/>
+      <c r="I4" s="184"/>
       <c r="J4" s="16"/>
       <c r="N4" s="18"/>
       <c r="AA4" s="18"/>
@@ -2899,18 +1916,18 @@
       <c r="AD4" s="18"/>
     </row>
     <row r="5" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="138" t="s">
+      <c r="B5" s="163" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="140"/>
-      <c r="F5" s="138" t="s">
+      <c r="C5" s="164"/>
+      <c r="D5" s="164"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="163" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="139"/>
-      <c r="H5" s="139"/>
-      <c r="I5" s="139"/>
+      <c r="G5" s="164"/>
+      <c r="H5" s="164"/>
+      <c r="I5" s="164"/>
       <c r="J5" s="54"/>
       <c r="L5" s="55"/>
       <c r="O5" s="10"/>
@@ -2955,48 +1972,48 @@
       <c r="Z6" s="10"/>
     </row>
     <row r="7" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="147" t="s">
+      <c r="B7" s="172" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="148"/>
-      <c r="D7" s="148"/>
-      <c r="E7" s="149"/>
-      <c r="F7" s="131" t="s">
+      <c r="C7" s="173"/>
+      <c r="D7" s="173"/>
+      <c r="E7" s="174"/>
+      <c r="F7" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="132"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="132"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="157"/>
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="156" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="131" t="s">
+      <c r="C8" s="157"/>
+      <c r="D8" s="157"/>
+      <c r="E8" s="158"/>
+      <c r="F8" s="156" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="132"/>
-      <c r="H8" s="132"/>
-      <c r="I8" s="132"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="157"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="131" t="s">
+      <c r="B9" s="156" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="132"/>
-      <c r="D9" s="132"/>
-      <c r="E9" s="133"/>
-      <c r="F9" s="131" t="s">
+      <c r="C9" s="157"/>
+      <c r="D9" s="157"/>
+      <c r="E9" s="158"/>
+      <c r="F9" s="156" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="132"/>
-      <c r="H9" s="132"/>
-      <c r="I9" s="132"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="157"/>
       <c r="J9" s="22"/>
       <c r="N9" s="18"/>
       <c r="O9" s="10"/>
@@ -3017,18 +2034,18 @@
       <c r="AD9" s="18"/>
     </row>
     <row r="10" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="138" t="s">
+      <c r="B10" s="163" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="139"/>
-      <c r="D10" s="139"/>
-      <c r="E10" s="140"/>
-      <c r="F10" s="138" t="s">
+      <c r="C10" s="164"/>
+      <c r="D10" s="164"/>
+      <c r="E10" s="165"/>
+      <c r="F10" s="163" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="139"/>
-      <c r="H10" s="139"/>
-      <c r="I10" s="139"/>
+      <c r="G10" s="164"/>
+      <c r="H10" s="164"/>
+      <c r="I10" s="164"/>
       <c r="J10" s="54"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
@@ -3071,18 +2088,18 @@
       <c r="Z11" s="10"/>
     </row>
     <row r="12" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="131" t="s">
+      <c r="B12" s="156" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="132"/>
-      <c r="D12" s="132"/>
-      <c r="E12" s="133"/>
-      <c r="F12" s="131" t="s">
+      <c r="C12" s="157"/>
+      <c r="D12" s="157"/>
+      <c r="E12" s="158"/>
+      <c r="F12" s="156" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="132"/>
-      <c r="H12" s="132"/>
-      <c r="I12" s="132"/>
+      <c r="G12" s="157"/>
+      <c r="H12" s="157"/>
+      <c r="I12" s="157"/>
       <c r="J12" s="22"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
@@ -3100,18 +2117,18 @@
       <c r="AA12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="131" t="s">
+      <c r="B13" s="156" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="132"/>
-      <c r="D13" s="132"/>
-      <c r="E13" s="133"/>
-      <c r="F13" s="131" t="s">
+      <c r="C13" s="157"/>
+      <c r="D13" s="157"/>
+      <c r="E13" s="158"/>
+      <c r="F13" s="156" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="132"/>
-      <c r="H13" s="132"/>
-      <c r="I13" s="132"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="157"/>
+      <c r="I13" s="157"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -3129,18 +2146,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="131" t="s">
+      <c r="B14" s="156" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="132"/>
-      <c r="D14" s="132"/>
-      <c r="E14" s="133"/>
-      <c r="F14" s="131" t="s">
+      <c r="C14" s="157"/>
+      <c r="D14" s="157"/>
+      <c r="E14" s="158"/>
+      <c r="F14" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="132"/>
-      <c r="H14" s="132"/>
-      <c r="I14" s="132"/>
+      <c r="G14" s="157"/>
+      <c r="H14" s="157"/>
+      <c r="I14" s="157"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -3158,18 +2175,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="150" t="s">
+      <c r="B15" s="175" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="151"/>
-      <c r="D15" s="151"/>
+      <c r="C15" s="176"/>
+      <c r="D15" s="176"/>
       <c r="E15" s="21"/>
-      <c r="F15" s="150" t="s">
+      <c r="F15" s="175" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="151"/>
-      <c r="H15" s="151"/>
-      <c r="I15" s="152"/>
+      <c r="G15" s="176"/>
+      <c r="H15" s="176"/>
+      <c r="I15" s="177"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -3187,18 +2204,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="131" t="s">
+      <c r="B16" s="156" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="155" t="s">
+      <c r="C16" s="178"/>
+      <c r="D16" s="178"/>
+      <c r="E16" s="179"/>
+      <c r="F16" s="180" t="s">
         <v>80</v>
       </c>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
+      <c r="G16" s="178"/>
+      <c r="H16" s="178"/>
+      <c r="I16" s="178"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -3216,18 +2233,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="156" t="s">
+      <c r="B17" s="181" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="157"/>
+      <c r="C17" s="182"/>
       <c r="D17" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="157" t="s">
+      <c r="E17" s="182" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="157"/>
-      <c r="G17" s="157"/>
+      <c r="F17" s="182"/>
+      <c r="G17" s="182"/>
       <c r="H17" s="23" t="s">
         <v>81</v>
       </c>
@@ -3251,18 +2268,18 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="141" t="s">
+      <c r="B18" s="166" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="142"/>
+      <c r="C18" s="167"/>
       <c r="D18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="143" t="s">
+      <c r="E18" s="168" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
+      <c r="F18" s="168"/>
+      <c r="G18" s="168"/>
       <c r="H18" s="1" t="s">
         <v>26</v>
       </c>
@@ -3411,18 +2428,18 @@
       <c r="AD23" s="10"/>
     </row>
     <row r="24" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="144" t="s">
+      <c r="B24" s="169" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="145"/>
-      <c r="D24" s="145"/>
-      <c r="E24" s="146"/>
-      <c r="F24" s="144" t="s">
+      <c r="C24" s="170"/>
+      <c r="D24" s="170"/>
+      <c r="E24" s="171"/>
+      <c r="F24" s="169" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="145"/>
-      <c r="H24" s="145"/>
-      <c r="I24" s="145"/>
+      <c r="G24" s="170"/>
+      <c r="H24" s="170"/>
+      <c r="I24" s="170"/>
       <c r="J24" s="22"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
@@ -3443,48 +2460,48 @@
       <c r="AD24" s="10"/>
     </row>
     <row r="25" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="131" t="s">
+      <c r="B25" s="156" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="132"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="133"/>
-      <c r="F25" s="131" t="s">
+      <c r="C25" s="157"/>
+      <c r="D25" s="157"/>
+      <c r="E25" s="158"/>
+      <c r="F25" s="156" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="132"/>
-      <c r="H25" s="132"/>
-      <c r="I25" s="132"/>
+      <c r="G25" s="157"/>
+      <c r="H25" s="157"/>
+      <c r="I25" s="157"/>
       <c r="J25" s="19"/>
     </row>
     <row r="26" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="147" t="s">
+      <c r="B26" s="172" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="148"/>
-      <c r="D26" s="148"/>
-      <c r="E26" s="149"/>
-      <c r="F26" s="131" t="s">
+      <c r="C26" s="173"/>
+      <c r="D26" s="173"/>
+      <c r="E26" s="174"/>
+      <c r="F26" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="G26" s="132"/>
-      <c r="H26" s="132"/>
-      <c r="I26" s="133"/>
+      <c r="G26" s="157"/>
+      <c r="H26" s="157"/>
+      <c r="I26" s="158"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="138" t="s">
+      <c r="B27" s="163" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="139"/>
-      <c r="D27" s="139"/>
+      <c r="C27" s="164"/>
+      <c r="D27" s="164"/>
       <c r="E27" s="32"/>
-      <c r="F27" s="138" t="s">
+      <c r="F27" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="139"/>
-      <c r="H27" s="139"/>
-      <c r="I27" s="140"/>
+      <c r="G27" s="164"/>
+      <c r="H27" s="164"/>
+      <c r="I27" s="165"/>
       <c r="J27" s="22"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
@@ -3505,33 +2522,33 @@
       <c r="AD27" s="10"/>
     </row>
     <row r="28" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="131" t="s">
+      <c r="B28" s="156" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="132"/>
-      <c r="D28" s="132"/>
-      <c r="E28" s="133"/>
-      <c r="F28" s="131" t="s">
+      <c r="C28" s="157"/>
+      <c r="D28" s="157"/>
+      <c r="E28" s="158"/>
+      <c r="F28" s="156" t="s">
         <v>38</v>
       </c>
-      <c r="G28" s="132"/>
-      <c r="H28" s="132"/>
-      <c r="I28" s="132"/>
+      <c r="G28" s="157"/>
+      <c r="H28" s="157"/>
+      <c r="I28" s="157"/>
       <c r="J28" s="9"/>
     </row>
     <row r="29" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="138" t="s">
+      <c r="B29" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="139"/>
-      <c r="D29" s="139"/>
+      <c r="C29" s="164"/>
+      <c r="D29" s="164"/>
       <c r="E29" s="21"/>
-      <c r="F29" s="138" t="s">
+      <c r="F29" s="163" t="s">
         <v>40</v>
       </c>
-      <c r="G29" s="139"/>
-      <c r="H29" s="139"/>
-      <c r="I29" s="140"/>
+      <c r="G29" s="164"/>
+      <c r="H29" s="164"/>
+      <c r="I29" s="165"/>
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -3550,18 +2567,18 @@
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="134" t="s">
+      <c r="B31" s="159" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="135"/>
-      <c r="D31" s="135"/>
-      <c r="E31" s="136"/>
-      <c r="F31" s="134" t="s">
+      <c r="C31" s="160"/>
+      <c r="D31" s="160"/>
+      <c r="E31" s="161"/>
+      <c r="F31" s="159" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="135"/>
-      <c r="H31" s="135"/>
-      <c r="I31" s="135"/>
+      <c r="G31" s="160"/>
+      <c r="H31" s="160"/>
+      <c r="I31" s="160"/>
       <c r="J31" s="34"/>
       <c r="N31" s="36"/>
       <c r="O31" s="36"/>
@@ -3582,103 +2599,103 @@
       <c r="AD31" s="36"/>
     </row>
     <row r="32" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="131" t="s">
+      <c r="B32" s="156" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="132"/>
-      <c r="D32" s="132"/>
-      <c r="E32" s="133"/>
-      <c r="F32" s="131" t="s">
+      <c r="C32" s="157"/>
+      <c r="D32" s="157"/>
+      <c r="E32" s="158"/>
+      <c r="F32" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="132"/>
-      <c r="H32" s="132"/>
-      <c r="I32" s="132"/>
+      <c r="G32" s="157"/>
+      <c r="H32" s="157"/>
+      <c r="I32" s="157"/>
       <c r="J32" s="19"/>
     </row>
     <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="131" t="s">
+      <c r="B33" s="156" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="132"/>
-      <c r="D33" s="132"/>
-      <c r="E33" s="133"/>
-      <c r="F33" s="131" t="s">
+      <c r="C33" s="157"/>
+      <c r="D33" s="157"/>
+      <c r="E33" s="158"/>
+      <c r="F33" s="156" t="s">
         <v>43</v>
       </c>
-      <c r="G33" s="132"/>
-      <c r="H33" s="132"/>
-      <c r="I33" s="132"/>
+      <c r="G33" s="157"/>
+      <c r="H33" s="157"/>
+      <c r="I33" s="157"/>
       <c r="J33" s="19"/>
     </row>
     <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="131" t="s">
+      <c r="B34" s="156" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="132"/>
-      <c r="D34" s="132"/>
-      <c r="E34" s="133"/>
-      <c r="F34" s="131" t="s">
+      <c r="C34" s="157"/>
+      <c r="D34" s="157"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="156" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="132"/>
-      <c r="H34" s="132"/>
-      <c r="I34" s="132"/>
+      <c r="G34" s="157"/>
+      <c r="H34" s="157"/>
+      <c r="I34" s="157"/>
       <c r="J34" s="19"/>
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="131" t="s">
+      <c r="B35" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="132"/>
-      <c r="D35" s="132"/>
-      <c r="E35" s="133"/>
-      <c r="F35" s="131" t="s">
+      <c r="C35" s="157"/>
+      <c r="D35" s="157"/>
+      <c r="E35" s="158"/>
+      <c r="F35" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="G35" s="132"/>
-      <c r="H35" s="132"/>
-      <c r="I35" s="132"/>
+      <c r="G35" s="157"/>
+      <c r="H35" s="157"/>
+      <c r="I35" s="157"/>
       <c r="J35" s="19"/>
     </row>
     <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="131" t="s">
+      <c r="B36" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="132"/>
-      <c r="D36" s="132"/>
-      <c r="E36" s="133"/>
-      <c r="F36" s="131" t="s">
+      <c r="C36" s="157"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="158"/>
+      <c r="F36" s="156" t="s">
         <v>47</v>
       </c>
-      <c r="G36" s="132"/>
-      <c r="H36" s="132"/>
-      <c r="I36" s="132"/>
+      <c r="G36" s="157"/>
+      <c r="H36" s="157"/>
+      <c r="I36" s="157"/>
       <c r="J36" s="19"/>
     </row>
     <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="131" t="s">
+      <c r="B37" s="156" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="132"/>
-      <c r="D37" s="132"/>
-      <c r="E37" s="133"/>
-      <c r="F37" s="131" t="s">
+      <c r="C37" s="157"/>
+      <c r="D37" s="157"/>
+      <c r="E37" s="158"/>
+      <c r="F37" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="G37" s="132"/>
-      <c r="H37" s="132"/>
-      <c r="I37" s="132"/>
+      <c r="G37" s="157"/>
+      <c r="H37" s="157"/>
+      <c r="I37" s="157"/>
       <c r="J37" s="19"/>
     </row>
     <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="63" t="s">
+      <c r="B38" s="62" t="s">
         <v>74</v>
       </c>
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
       <c r="E38" s="21"/>
-      <c r="F38" s="63" t="s">
+      <c r="F38" s="62" t="s">
         <v>75</v>
       </c>
       <c r="G38" s="20"/>
@@ -3687,18 +2704,18 @@
       <c r="J38" s="19"/>
     </row>
     <row r="39" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="134" t="s">
+      <c r="B39" s="159" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="135"/>
-      <c r="D39" s="135"/>
-      <c r="E39" s="136"/>
-      <c r="F39" s="134" t="s">
+      <c r="C39" s="160"/>
+      <c r="D39" s="160"/>
+      <c r="E39" s="161"/>
+      <c r="F39" s="159" t="s">
         <v>15</v>
       </c>
-      <c r="G39" s="137"/>
-      <c r="H39" s="137"/>
-      <c r="I39" s="137"/>
+      <c r="G39" s="162"/>
+      <c r="H39" s="162"/>
+      <c r="I39" s="162"/>
       <c r="J39" s="34"/>
       <c r="N39" s="36"/>
       <c r="O39" s="36"/>
@@ -3719,18 +2736,18 @@
       <c r="AD39" s="36"/>
     </row>
     <row r="40" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="131" t="s">
+      <c r="B40" s="156" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="132"/>
-      <c r="D40" s="132"/>
-      <c r="E40" s="133"/>
-      <c r="F40" s="131" t="s">
+      <c r="C40" s="157"/>
+      <c r="D40" s="157"/>
+      <c r="E40" s="158"/>
+      <c r="F40" s="156" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="132"/>
-      <c r="H40" s="132"/>
-      <c r="I40" s="132"/>
+      <c r="G40" s="157"/>
+      <c r="H40" s="157"/>
+      <c r="I40" s="157"/>
       <c r="J40" s="19"/>
     </row>
     <row r="41" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -4110,4 +3127,889 @@
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.35433070866141736" bottom="0.15748031496062992" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="76" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBB9FB0-5253-4E0F-9002-2C89C8553DAA}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AC52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="1" customWidth="1"/>
+    <col min="2" max="2" width="11.73046875" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="14.3984375" customWidth="1"/>
+    <col min="5" max="5" width="8.46484375" customWidth="1"/>
+    <col min="6" max="6" width="19.86328125" customWidth="1"/>
+    <col min="7" max="7" width="0.9296875" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="14.19921875" customWidth="1"/>
+    <col min="11" max="11" width="5.59765625" customWidth="1"/>
+    <col min="12" max="12" width="7.1328125" customWidth="1"/>
+    <col min="13" max="13" width="15.53125" customWidth="1"/>
+    <col min="14" max="14" width="0.59765625" customWidth="1"/>
+    <col min="15" max="18" width="9.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="0.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="56"/>
+      <c r="N1" s="58"/>
+    </row>
+    <row r="2" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="89"/>
+      <c r="B2" s="119" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="122" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="58"/>
+    </row>
+    <row r="3" spans="1:14" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="89"/>
+      <c r="B3" s="120" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="123" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="58"/>
+    </row>
+    <row r="4" spans="1:14" s="86" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="88"/>
+      <c r="B4" s="120" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="123" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="84"/>
+    </row>
+    <row r="5" spans="1:14" s="86" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="87"/>
+      <c r="B5" s="120" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="120"/>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="123" t="s">
+        <v>133</v>
+      </c>
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="84"/>
+    </row>
+    <row r="6" spans="1:14" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="56"/>
+      <c r="B6" s="110" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="110"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="96" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="58"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="56"/>
+      <c r="B7" s="113" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="99" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="58"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="56"/>
+      <c r="B8" s="125" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="125"/>
+      <c r="F8" s="125"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="101" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="98"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="58"/>
+    </row>
+    <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="56"/>
+      <c r="B9" s="126" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="126"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="103" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" s="98"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="98"/>
+      <c r="L9" s="98"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="58"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="56"/>
+      <c r="B10" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="113"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+      <c r="L10" s="98"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="58"/>
+    </row>
+    <row r="11" spans="1:14" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="56"/>
+      <c r="B11" s="102" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="155" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="102"/>
+      <c r="N11" s="58"/>
+    </row>
+    <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="56"/>
+      <c r="B12" s="126" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="126"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="126"/>
+      <c r="H12" s="96" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="97"/>
+      <c r="J12" s="97"/>
+      <c r="K12" s="97"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="58"/>
+    </row>
+    <row r="13" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="56"/>
+      <c r="B13" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="100"/>
+      <c r="J13" s="100"/>
+      <c r="K13" s="100"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="58"/>
+    </row>
+    <row r="14" spans="1:14" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="56"/>
+      <c r="B14" s="102" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="118"/>
+      <c r="H14" s="155" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="102"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="58"/>
+    </row>
+    <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="85"/>
+      <c r="B15" s="104" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="104"/>
+      <c r="D15" s="105" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="105"/>
+      <c r="H15" s="106" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="105"/>
+      <c r="J15" s="127" t="s">
+        <v>114</v>
+      </c>
+      <c r="K15" s="127"/>
+      <c r="L15" s="151" t="s">
+        <v>115</v>
+      </c>
+      <c r="M15" s="151"/>
+      <c r="N15" s="58"/>
+    </row>
+    <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="56"/>
+      <c r="B16" s="118" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="107"/>
+      <c r="D16" s="194" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="108"/>
+      <c r="F16" s="144" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" s="108"/>
+      <c r="H16" s="197" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="108"/>
+      <c r="J16" s="109" t="s">
+        <v>109</v>
+      </c>
+      <c r="K16" s="109"/>
+      <c r="L16" s="152" t="s">
+        <v>110</v>
+      </c>
+      <c r="M16" s="152"/>
+      <c r="N16" s="58"/>
+    </row>
+    <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="56"/>
+      <c r="B17" s="126" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="126"/>
+      <c r="D17" s="126" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" s="130"/>
+      <c r="F17" s="143" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" s="143"/>
+      <c r="H17" s="103" t="s">
+        <v>126</v>
+      </c>
+      <c r="I17" s="98"/>
+      <c r="J17" s="111" t="s">
+        <v>125</v>
+      </c>
+      <c r="K17" s="98"/>
+      <c r="L17" s="153" t="s">
+        <v>124</v>
+      </c>
+      <c r="M17" s="154"/>
+      <c r="N17" s="58"/>
+    </row>
+    <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="56"/>
+      <c r="B18" s="102" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="125"/>
+      <c r="D18" s="195" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="109"/>
+      <c r="F18" s="196" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="144"/>
+      <c r="H18" s="197" t="s">
+        <v>121</v>
+      </c>
+      <c r="I18" s="109"/>
+      <c r="J18" s="195" t="s">
+        <v>120</v>
+      </c>
+      <c r="K18" s="109"/>
+      <c r="L18" s="152" t="s">
+        <v>119</v>
+      </c>
+      <c r="M18" s="152"/>
+      <c r="N18" s="58"/>
+    </row>
+    <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="56"/>
+      <c r="B19" s="131" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="131"/>
+      <c r="D19" s="131" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="131"/>
+      <c r="F19" s="145"/>
+      <c r="G19" s="145"/>
+      <c r="H19" s="148" t="s">
+        <v>142</v>
+      </c>
+      <c r="I19" s="128"/>
+      <c r="J19" s="126" t="s">
+        <v>106</v>
+      </c>
+      <c r="K19" s="126"/>
+      <c r="L19" s="126"/>
+      <c r="M19" s="126"/>
+      <c r="N19" s="58"/>
+    </row>
+    <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="56"/>
+      <c r="B20" s="194" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="112"/>
+      <c r="D20" s="129" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="129"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="146"/>
+      <c r="H20" s="198" t="s">
+        <v>65</v>
+      </c>
+      <c r="I20" s="108"/>
+      <c r="J20" s="113" t="s">
+        <v>105</v>
+      </c>
+      <c r="K20" s="114"/>
+      <c r="L20" s="109"/>
+      <c r="M20" s="109"/>
+      <c r="N20" s="58"/>
+    </row>
+    <row r="21" spans="1:29" s="82" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="95"/>
+      <c r="B21" s="115"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="115"/>
+      <c r="F21" s="115"/>
+      <c r="G21" s="147"/>
+      <c r="H21" s="149"/>
+      <c r="I21" s="116"/>
+      <c r="J21" s="116"/>
+      <c r="K21" s="116"/>
+      <c r="L21" s="116"/>
+      <c r="M21" s="117"/>
+      <c r="N21" s="83"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+      <c r="AB21"/>
+      <c r="AC21"/>
+    </row>
+    <row r="22" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="56"/>
+      <c r="B22" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="132" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="132"/>
+      <c r="E22" s="132"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="132"/>
+      <c r="H22" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="I22" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="J22" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="K22" s="132" t="s">
+        <v>99</v>
+      </c>
+      <c r="L22" s="132"/>
+      <c r="M22" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="N22" s="58"/>
+    </row>
+    <row r="23" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="56"/>
+      <c r="B23" s="139" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="192" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="192"/>
+      <c r="E23" s="192"/>
+      <c r="F23" s="192"/>
+      <c r="G23" s="140"/>
+      <c r="H23" s="141" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="J23" s="78">
+        <v>14</v>
+      </c>
+      <c r="K23" s="193" t="s">
+        <v>94</v>
+      </c>
+      <c r="L23" s="193"/>
+      <c r="M23" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="N23" s="58"/>
+    </row>
+    <row r="24" spans="1:29" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="56"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="137"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="137"/>
+      <c r="G24" s="137"/>
+      <c r="H24" s="138" t="s">
+        <v>93</v>
+      </c>
+      <c r="I24" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="J24" s="75">
+        <v>14</v>
+      </c>
+      <c r="K24" s="142" t="s">
+        <v>50</v>
+      </c>
+      <c r="L24" s="142"/>
+      <c r="M24" s="90" t="s">
+        <v>91</v>
+      </c>
+      <c r="N24" s="58"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A25" s="56"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="69"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="58"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A26" s="56"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="69"/>
+      <c r="K26" s="69"/>
+      <c r="L26" s="69"/>
+      <c r="M26" s="74"/>
+      <c r="N26" s="58"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A27" s="56"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="69"/>
+      <c r="K27" s="69"/>
+      <c r="L27" s="69"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="58"/>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A28" s="56"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="69"/>
+      <c r="L28" s="69"/>
+      <c r="M28" s="74"/>
+      <c r="N28" s="58"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A29" s="56"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="69"/>
+      <c r="K29" s="69"/>
+      <c r="L29" s="69"/>
+      <c r="M29" s="74"/>
+      <c r="N29" s="58"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A30" s="56"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="69"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="74"/>
+      <c r="N30" s="58"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A31" s="56"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="69"/>
+      <c r="K31" s="69"/>
+      <c r="L31" s="69"/>
+      <c r="M31" s="74"/>
+      <c r="N31" s="58"/>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A32" s="56"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="74"/>
+      <c r="N32" s="58"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A33" s="56"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="69"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="69"/>
+      <c r="M33" s="74"/>
+      <c r="N33" s="58"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A34" s="56"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
+      <c r="L34" s="69"/>
+      <c r="M34" s="74"/>
+      <c r="N34" s="58"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A35" s="56"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="74"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="69"/>
+      <c r="M35" s="74"/>
+      <c r="N35" s="58"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A36" s="56"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="69"/>
+      <c r="K36" s="69"/>
+      <c r="L36" s="69"/>
+      <c r="M36" s="74"/>
+      <c r="N36" s="58"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="56"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="61"/>
+      <c r="J37" s="57"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="69"/>
+      <c r="M37" s="61"/>
+      <c r="N37" s="58"/>
+    </row>
+    <row r="38" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="56"/>
+      <c r="B38" s="92" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="72"/>
+      <c r="G38" s="72"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="134" t="s">
+        <v>90</v>
+      </c>
+      <c r="J38" s="133"/>
+      <c r="K38" s="133"/>
+      <c r="L38" s="133"/>
+      <c r="M38" s="133"/>
+      <c r="N38" s="58"/>
+    </row>
+    <row r="39" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="56"/>
+      <c r="B39" s="93" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="57"/>
+      <c r="K39" s="57"/>
+      <c r="L39" s="69"/>
+      <c r="M39" s="61"/>
+      <c r="N39" s="58"/>
+    </row>
+    <row r="40" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="56"/>
+      <c r="B40" s="93" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="70"/>
+      <c r="J40" s="57"/>
+      <c r="K40" s="57"/>
+      <c r="L40" s="69"/>
+      <c r="M40" s="61"/>
+      <c r="N40" s="58"/>
+    </row>
+    <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="56"/>
+      <c r="B41" s="93" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="69"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="59"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="70"/>
+      <c r="J41" s="57"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="69"/>
+      <c r="M41" s="61"/>
+      <c r="N41" s="58"/>
+    </row>
+    <row r="42" spans="1:14" s="64" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="68"/>
+      <c r="B42" s="94" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="135"/>
+      <c r="J42" s="136"/>
+      <c r="K42" s="136"/>
+      <c r="L42" s="136"/>
+      <c r="M42" s="136"/>
+      <c r="N42" s="91"/>
+    </row>
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="49" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="50" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="51" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="52" ht="2.25" customHeight="1" x14ac:dyDescent="0.45"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="K23:L23"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="70" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
excel utils api refactored, middle string in tmps with double utils added + empty title declaration in setsell obj added
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,40 +8,42 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74233516-7D8C-4510-91E9-6F74BBE52C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4772B29-DF2C-47FD-991C-571D2DD65396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="2370" yWindow="1875" windowWidth="14385" windowHeight="8085" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
     <sheet name="Invoice" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Seal_agent_end">Export_Contract!$H$51</definedName>
-    <definedName name="Seal_agent_start">Export_Contract!$G$41</definedName>
-    <definedName name="Seal_seller_end">Export_Contract!$C$51</definedName>
-    <definedName name="Seal_seller_start">Export_Contract!$C$43</definedName>
-    <definedName name="Sign_agent_end">Export_Contract!$G$51</definedName>
-    <definedName name="Sign_agent_start">Export_Contract!$G$49</definedName>
-    <definedName name="Sign_seller_start">Export_Contract!$C$49</definedName>
-    <definedName name="Адреса_банк_получателя">Export_Contract!$B$33</definedName>
-    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$34</definedName>
-    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$35</definedName>
-    <definedName name="Адреса_подпись">Export_Contract!$B$50</definedName>
-    <definedName name="Адреса_покупатель">Export_Contract!$B$39</definedName>
-    <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$40</definedName>
-    <definedName name="Адреса_покупатель_банк">Export_Contract!$B$42</definedName>
-    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$B$45</definedName>
-    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$B$44</definedName>
-    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$B$46</definedName>
-    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$B$47</definedName>
-    <definedName name="Адреса_покупатель_счет">Export_Contract!$B$48</definedName>
-    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$B$36</definedName>
-    <definedName name="Адреса_получатель_счет">Export_Contract!$B$37</definedName>
-    <definedName name="Адреса_продавец">Export_Contract!$B$31</definedName>
-    <definedName name="Адреса_продавец_адрес">Export_Contract!$B$32</definedName>
-    <definedName name="Доставка_порт">Export_Contract!$B$25</definedName>
-    <definedName name="Доставка_условия">Export_Contract!$B$24</definedName>
+    <definedName name="MID_Contract">Export_Contract!$E$1</definedName>
+    <definedName name="MID_Invoice">Invoice!$G$1</definedName>
+    <definedName name="Seal_agent_end">Export_Contract!$H$52</definedName>
+    <definedName name="Seal_agent_start">Export_Contract!$G$42</definedName>
+    <definedName name="Seal_seller_end">Export_Contract!$C$52</definedName>
+    <definedName name="Seal_seller_start">Export_Contract!$C$44</definedName>
+    <definedName name="Sign_agent_end">Export_Contract!$G$52</definedName>
+    <definedName name="Sign_agent_start">Export_Contract!$G$50</definedName>
+    <definedName name="Sign_seller_start">Export_Contract!$C$50</definedName>
+    <definedName name="Адреса_банк_получателя">Export_Contract!$B$34</definedName>
+    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$35</definedName>
+    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$36</definedName>
+    <definedName name="Адреса_подпись">Export_Contract!$B$51</definedName>
+    <definedName name="Адреса_покупатель">Export_Contract!$B$40</definedName>
+    <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$41</definedName>
+    <definedName name="Адреса_покупатель_банк">Export_Contract!$B$43</definedName>
+    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$B$46</definedName>
+    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$B$45</definedName>
+    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$B$47</definedName>
+    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$B$48</definedName>
+    <definedName name="Адреса_покупатель_счет">Export_Contract!$B$49</definedName>
+    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$B$37</definedName>
+    <definedName name="Адреса_получатель_счет">Export_Contract!$B$38</definedName>
+    <definedName name="Адреса_продавец">Export_Contract!$B$32</definedName>
+    <definedName name="Адреса_продавец_адрес">Export_Contract!$B$33</definedName>
+    <definedName name="Доставка_порт">Export_Contract!$B$26</definedName>
+    <definedName name="Доставка_условия">Export_Contract!$B$25</definedName>
     <definedName name="Инвойс">Invoice!$B$2</definedName>
     <definedName name="Инвойс_Bl_массив">Invoice!$B$23</definedName>
     <definedName name="Инвойс_банк_получателя">Invoice!$B$38</definedName>
@@ -67,20 +69,20 @@
     <definedName name="Инвойс_соглашение">Invoice!$B$3</definedName>
     <definedName name="Инвойс_транспорт">Invoice!$B$18</definedName>
     <definedName name="Инвойс_условия">Invoice!$B$20</definedName>
-    <definedName name="Контракт">Export_Contract!$B$2</definedName>
-    <definedName name="Контракт_дата">Export_Contract!$B$3</definedName>
-    <definedName name="Покупатель">Export_Contract!$B$11</definedName>
-    <definedName name="Покупатель_адрес">Export_Contract!$B$12</definedName>
-    <definedName name="Покупатель_представитель">Export_Contract!$B$13</definedName>
-    <definedName name="Покупатель_представитель_подробно">Export_Contract!$B$14</definedName>
-    <definedName name="Предмет_массив">Export_Contract!$B$18</definedName>
-    <definedName name="Продавец">Export_Contract!$B$6</definedName>
-    <definedName name="Продавец_адрес">Export_Contract!$B$7</definedName>
-    <definedName name="Продавец_подписант">Export_Contract!$B$9</definedName>
-    <definedName name="Продавец_представитель">Export_Contract!$B$8</definedName>
-    <definedName name="Прочие_условия_описание">Export_Contract!$B$28</definedName>
-    <definedName name="Соглашение">Export_Contract!$B$1</definedName>
-    <definedName name="Цена_всего">Export_Contract!$B$22</definedName>
+    <definedName name="Контракт">Export_Contract!$B$3</definedName>
+    <definedName name="Контракт_дата">Export_Contract!$B$4</definedName>
+    <definedName name="Покупатель">Export_Contract!$B$12</definedName>
+    <definedName name="Покупатель_адрес">Export_Contract!$B$13</definedName>
+    <definedName name="Покупатель_представитель">Export_Contract!$B$14</definedName>
+    <definedName name="Покупатель_представитель_подробно">Export_Contract!$B$15</definedName>
+    <definedName name="Предмет_массив">Export_Contract!$B$19</definedName>
+    <definedName name="Продавец">Export_Contract!$B$7</definedName>
+    <definedName name="Продавец_адрес">Export_Contract!$B$8</definedName>
+    <definedName name="Продавец_подписант">Export_Contract!$B$10</definedName>
+    <definedName name="Продавец_представитель">Export_Contract!$B$9</definedName>
+    <definedName name="Прочие_условия_описание">Export_Contract!$B$29</definedName>
+    <definedName name="Соглашение">Export_Contract!$B$2</definedName>
+    <definedName name="Цена_всего">Export_Contract!$B$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -103,10 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="143">
-  <si>
-    <t>Supplementary Agreement No. 146 dated March 10, 2023</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="143">
   <si>
     <t>Дополнительное соглашение № 146 от 10 марта 2023г.</t>
   </si>
@@ -552,6 +551,9 @@
   </si>
   <si>
     <t>Условия доставки и оплаты:</t>
+  </si>
+  <si>
+    <t>Agreement No. 146 dated March 10, 2023</t>
   </si>
 </sst>
 </file>
@@ -562,7 +564,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -718,6 +720,18 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -856,7 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1273,6 +1287,26 @@
     <xf numFmtId="9" fontId="18" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1363,14 +1397,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1386,21 +1420,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1765,10 +1784,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AF87"/>
+  <dimension ref="B1:AF88"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:E16"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1807,155 +1826,132 @@
     <col min="33" max="16384" width="8.796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="186" t="s">
+    <row r="1" spans="2:30" ht="2.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="162"/>
+      <c r="I1" s="162"/>
+    </row>
+    <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="194" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="194" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="186" t="s">
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="163"/>
+      <c r="L2" s="11"/>
+      <c r="N2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+    </row>
+    <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="197" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="187"/>
-      <c r="H1" s="187"/>
-      <c r="I1" s="187"/>
-      <c r="J1" s="9"/>
-      <c r="L1" s="11"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-    </row>
-    <row r="2" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="189" t="s">
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="199"/>
+      <c r="F3" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="191"/>
-      <c r="F2" s="189" t="s">
+      <c r="G3" s="198"/>
+      <c r="H3" s="198"/>
+      <c r="I3" s="198"/>
+      <c r="J3" s="9"/>
+      <c r="L3" s="11"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+    </row>
+    <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="190"/>
-      <c r="H2" s="190"/>
-      <c r="I2" s="190"/>
-      <c r="J2" s="9"/>
-      <c r="L2" s="11"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-    </row>
-    <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="189" t="s">
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="199"/>
+      <c r="F4" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="190"/>
-      <c r="D3" s="190"/>
-      <c r="E3" s="191"/>
-      <c r="F3" s="189" t="s">
+      <c r="G4" s="198"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198"/>
+      <c r="J4" s="9"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="13"/>
+      <c r="AC4" s="13"/>
+      <c r="AD4" s="13"/>
+    </row>
+    <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="191" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="190"/>
-      <c r="H3" s="190"/>
-      <c r="I3" s="190"/>
-      <c r="J3" s="9"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="13"/>
-      <c r="AB3" s="13"/>
-      <c r="AC3" s="13"/>
-      <c r="AD3" s="13"/>
-    </row>
-    <row r="4" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="183" t="s">
+      <c r="C5" s="192"/>
+      <c r="D5" s="192"/>
+      <c r="E5" s="193"/>
+      <c r="F5" s="191" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="185"/>
-      <c r="F4" s="183" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="184"/>
-      <c r="H4" s="184"/>
-      <c r="I4" s="184"/>
-      <c r="J4" s="16"/>
-      <c r="N4" s="18"/>
-      <c r="AA4" s="18"/>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="18"/>
-      <c r="AD4" s="18"/>
-    </row>
-    <row r="5" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="163" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="164"/>
-      <c r="D5" s="164"/>
-      <c r="E5" s="165"/>
-      <c r="F5" s="163" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="164"/>
-      <c r="H5" s="164"/>
-      <c r="I5" s="164"/>
-      <c r="J5" s="54"/>
-      <c r="L5" s="55"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="10"/>
+      <c r="G5" s="192"/>
+      <c r="H5" s="192"/>
+      <c r="I5" s="192"/>
+      <c r="J5" s="16"/>
+      <c r="N5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="171" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="171" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
+      <c r="G6" s="172"/>
+      <c r="H6" s="172"/>
+      <c r="I6" s="172"/>
       <c r="J6" s="54"/>
       <c r="L6" s="55"/>
       <c r="O6" s="10"/>
@@ -1971,82 +1967,79 @@
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
     </row>
-    <row r="7" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="172" t="s">
+    <row r="7" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="54"/>
+      <c r="L7" s="55"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+    </row>
+    <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="180" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="164" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="173"/>
-      <c r="D7" s="173"/>
-      <c r="E7" s="174"/>
-      <c r="F7" s="156" t="s">
+      <c r="G8" s="165"/>
+      <c r="H8" s="165"/>
+      <c r="I8" s="165"/>
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="164" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="157"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="157"/>
-      <c r="J7" s="22"/>
-    </row>
-    <row r="8" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="156" t="s">
+      <c r="C9" s="165"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="164" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="157"/>
-      <c r="D8" s="157"/>
-      <c r="E8" s="158"/>
-      <c r="F8" s="156" t="s">
+      <c r="G9" s="165"/>
+      <c r="H9" s="165"/>
+      <c r="I9" s="165"/>
+      <c r="J9" s="22"/>
+    </row>
+    <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="164" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="157"/>
-      <c r="H8" s="157"/>
-      <c r="I8" s="157"/>
-      <c r="J8" s="22"/>
-    </row>
-    <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="156" t="s">
+      <c r="C10" s="165"/>
+      <c r="D10" s="165"/>
+      <c r="E10" s="166"/>
+      <c r="F10" s="164" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="158"/>
-      <c r="F9" s="156" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="157"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="22"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="10"/>
-      <c r="AA9" s="18"/>
-      <c r="AB9" s="18"/>
-      <c r="AC9" s="18"/>
-      <c r="AD9" s="18"/>
-    </row>
-    <row r="10" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="163" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="164"/>
-      <c r="D10" s="164"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="163" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="164"/>
-      <c r="H10" s="164"/>
-      <c r="I10" s="164"/>
-      <c r="J10" s="54"/>
+      <c r="G10" s="165"/>
+      <c r="H10" s="165"/>
+      <c r="I10" s="165"/>
+      <c r="J10" s="22"/>
+      <c r="N10" s="18"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
@@ -2059,20 +2052,24 @@
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
-    </row>
-    <row r="11" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="18"/>
+      <c r="AC10" s="18"/>
+      <c r="AD10" s="18"/>
+    </row>
+    <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="171" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="172"/>
+      <c r="D11" s="172"/>
+      <c r="E11" s="173"/>
+      <c r="F11" s="171" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="172"/>
+      <c r="H11" s="172"/>
+      <c r="I11" s="172"/>
       <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -2087,21 +2084,20 @@
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
     </row>
-    <row r="12" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="156" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="157"/>
-      <c r="D12" s="157"/>
-      <c r="E12" s="158"/>
-      <c r="F12" s="156" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="157"/>
-      <c r="H12" s="157"/>
-      <c r="I12" s="157"/>
-      <c r="J12" s="22"/>
-      <c r="N12" s="10"/>
+    <row r="12" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="54"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
@@ -2114,21 +2110,20 @@
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
-      <c r="AA12" s="10"/>
-    </row>
-    <row r="13" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="156" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="157"/>
-      <c r="D13" s="157"/>
-      <c r="E13" s="158"/>
-      <c r="F13" s="156" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="157"/>
-      <c r="H13" s="157"/>
-      <c r="I13" s="157"/>
+    </row>
+    <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="164" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="165"/>
+      <c r="D13" s="165"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="164" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="165"/>
+      <c r="H13" s="165"/>
+      <c r="I13" s="165"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2145,19 +2140,19 @@
       <c r="Z13" s="10"/>
       <c r="AA13" s="10"/>
     </row>
-    <row r="14" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="156" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="157"/>
-      <c r="D14" s="157"/>
-      <c r="E14" s="158"/>
-      <c r="F14" s="156" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="157"/>
-      <c r="H14" s="157"/>
-      <c r="I14" s="157"/>
+    <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="164" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="165"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="164" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="165"/>
+      <c r="H14" s="165"/>
+      <c r="I14" s="165"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2174,19 +2169,19 @@
       <c r="Z14" s="10"/>
       <c r="AA14" s="10"/>
     </row>
-    <row r="15" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="175" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="176"/>
-      <c r="D15" s="176"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="175" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="176"/>
-      <c r="H15" s="176"/>
-      <c r="I15" s="177"/>
+    <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="164" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="165"/>
+      <c r="D15" s="165"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="164" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="165"/>
+      <c r="H15" s="165"/>
+      <c r="I15" s="165"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2203,19 +2198,19 @@
       <c r="Z15" s="10"/>
       <c r="AA15" s="10"/>
     </row>
-    <row r="16" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="156" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="178"/>
-      <c r="D16" s="178"/>
-      <c r="E16" s="179"/>
-      <c r="F16" s="180" t="s">
-        <v>80</v>
-      </c>
-      <c r="G16" s="178"/>
-      <c r="H16" s="178"/>
-      <c r="I16" s="178"/>
+    <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="183" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="184"/>
+      <c r="D16" s="184"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="183" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="184"/>
+      <c r="H16" s="184"/>
+      <c r="I16" s="185"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2232,26 +2227,20 @@
       <c r="Z16" s="10"/>
       <c r="AA16" s="10"/>
     </row>
-    <row r="17" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="181" t="s">
+    <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="164" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="182"/>
-      <c r="D17" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="182" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="182"/>
-      <c r="G17" s="182"/>
-      <c r="H17" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="I17" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="J17" s="24"/>
+      <c r="C17" s="186"/>
+      <c r="D17" s="186"/>
+      <c r="E17" s="187"/>
+      <c r="F17" s="188" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="186"/>
+      <c r="H17" s="186"/>
+      <c r="I17" s="186"/>
+      <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
@@ -2267,26 +2256,26 @@
       <c r="Z17" s="10"/>
       <c r="AA17" s="10"/>
     </row>
-    <row r="18" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="166" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="167"/>
-      <c r="D18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="168" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="168"/>
-      <c r="G18" s="168"/>
-      <c r="H18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18" s="2"/>
+    <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="189" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="190"/>
+      <c r="D18" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="190" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="190"/>
+      <c r="G18" s="190"/>
+      <c r="H18" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18" s="24"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
@@ -2301,19 +2290,26 @@
       <c r="Y18" s="10"/>
       <c r="Z18" s="10"/>
       <c r="AA18" s="10"/>
-      <c r="AB18" s="10"/>
-      <c r="AC18" s="10"/>
-      <c r="AD18" s="10"/>
-    </row>
-    <row r="19" spans="2:30" ht="6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="5"/>
+    </row>
+    <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="174" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="175"/>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="176" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="176"/>
+      <c r="G19" s="176"/>
+      <c r="H19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>26</v>
+      </c>
       <c r="J19" s="2"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
@@ -2333,17 +2329,13 @@
       <c r="AC19" s="10"/>
       <c r="AD19" s="10"/>
     </row>
-    <row r="20" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+    <row r="20" spans="2:30" ht="6" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="8"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="5"/>
       <c r="H20" s="26"/>
       <c r="I20" s="5"/>
       <c r="J20" s="2"/>
@@ -2365,81 +2357,81 @@
       <c r="AC20" s="10"/>
       <c r="AD20" s="10"/>
     </row>
-    <row r="21" spans="2:30" s="30" customFormat="1" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="27" t="s">
+    <row r="21" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="2"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10"/>
+      <c r="AD21" s="10"/>
+    </row>
+    <row r="22" spans="2:30" s="30" customFormat="1" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="19"/>
-    </row>
-    <row r="22" spans="2:30" s="30" customFormat="1" ht="23.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="19" t="s">
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="19"/>
+    </row>
+    <row r="23" spans="2:30" s="30" customFormat="1" ht="23.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="19" t="s">
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="19"/>
+    </row>
+    <row r="24" spans="2:30" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="19"/>
-    </row>
-    <row r="23" spans="2:30" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="6" t="s">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="22"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-      <c r="W23" s="10"/>
-      <c r="X23" s="10"/>
-      <c r="Y23" s="10"/>
-      <c r="Z23" s="10"/>
-      <c r="AA23" s="10"/>
-      <c r="AB23" s="10"/>
-      <c r="AC23" s="10"/>
-      <c r="AD23" s="10"/>
-    </row>
-    <row r="24" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="169" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="170"/>
-      <c r="D24" s="170"/>
-      <c r="E24" s="171"/>
-      <c r="F24" s="169" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" s="170"/>
-      <c r="H24" s="170"/>
-      <c r="I24" s="170"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
       <c r="J24" s="22"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
@@ -2459,362 +2451,379 @@
       <c r="AC24" s="10"/>
       <c r="AD24" s="10"/>
     </row>
-    <row r="25" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="156" t="s">
+    <row r="25" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="177" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="178"/>
+      <c r="D25" s="178"/>
+      <c r="E25" s="179"/>
+      <c r="F25" s="177" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="178"/>
+      <c r="H25" s="178"/>
+      <c r="I25" s="178"/>
+      <c r="J25" s="22"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="10"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="10"/>
+      <c r="AD25" s="10"/>
+    </row>
+    <row r="26" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="164" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="165"/>
+      <c r="D26" s="165"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="164" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="165"/>
+      <c r="H26" s="165"/>
+      <c r="I26" s="165"/>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="157"/>
-      <c r="D25" s="157"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="156" t="s">
+      <c r="C27" s="181"/>
+      <c r="D27" s="181"/>
+      <c r="E27" s="182"/>
+      <c r="F27" s="164" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="157"/>
-      <c r="H25" s="157"/>
-      <c r="I25" s="157"/>
-      <c r="J25" s="19"/>
-    </row>
-    <row r="26" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="172" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="173"/>
-      <c r="D26" s="173"/>
-      <c r="E26" s="174"/>
-      <c r="F26" s="156" t="s">
-        <v>86</v>
-      </c>
-      <c r="G26" s="157"/>
-      <c r="H26" s="157"/>
-      <c r="I26" s="158"/>
-      <c r="J26" s="19"/>
-    </row>
-    <row r="27" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="163" t="s">
+      <c r="G27" s="165"/>
+      <c r="H27" s="165"/>
+      <c r="I27" s="166"/>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="171" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="172"/>
+      <c r="D28" s="172"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="171" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="164"/>
-      <c r="D27" s="164"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="163" t="s">
+      <c r="G28" s="172"/>
+      <c r="H28" s="172"/>
+      <c r="I28" s="173"/>
+      <c r="J28" s="22"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
+      <c r="X28" s="10"/>
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="10"/>
+      <c r="AB28" s="10"/>
+      <c r="AC28" s="10"/>
+      <c r="AD28" s="10"/>
+    </row>
+    <row r="29" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="164" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="165"/>
+      <c r="D29" s="165"/>
+      <c r="E29" s="166"/>
+      <c r="F29" s="164" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="164"/>
-      <c r="H27" s="164"/>
-      <c r="I27" s="165"/>
-      <c r="J27" s="22"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
-      <c r="W27" s="10"/>
-      <c r="X27" s="10"/>
-      <c r="Y27" s="10"/>
-      <c r="Z27" s="10"/>
-      <c r="AA27" s="10"/>
-      <c r="AB27" s="10"/>
-      <c r="AC27" s="10"/>
-      <c r="AD27" s="10"/>
-    </row>
-    <row r="28" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="156" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="158"/>
-      <c r="F28" s="156" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="163" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="164"/>
-      <c r="D29" s="164"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="163" t="s">
-        <v>40</v>
-      </c>
-      <c r="G29" s="164"/>
-      <c r="H29" s="164"/>
+      <c r="G29" s="165"/>
+      <c r="H29" s="165"/>
       <c r="I29" s="165"/>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+    <row r="30" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="171" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="172"/>
+      <c r="D30" s="172"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="50" t="s">
+      <c r="F30" s="171" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="173"/>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="167" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="168"/>
+      <c r="D32" s="168"/>
+      <c r="E32" s="169"/>
+      <c r="F32" s="167" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="168"/>
+      <c r="H32" s="168"/>
+      <c r="I32" s="168"/>
+      <c r="J32" s="34"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="36"/>
+      <c r="T32" s="36"/>
+      <c r="U32" s="36"/>
+      <c r="V32" s="36"/>
+      <c r="W32" s="36"/>
+      <c r="X32" s="36"/>
+      <c r="Y32" s="36"/>
+      <c r="Z32" s="36"/>
+      <c r="AA32" s="36"/>
+      <c r="AB32" s="36"/>
+      <c r="AC32" s="36"/>
+      <c r="AD32" s="36"/>
+    </row>
+    <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="164" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="165"/>
+      <c r="D33" s="165"/>
+      <c r="E33" s="166"/>
+      <c r="F33" s="164" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="165"/>
+      <c r="H33" s="165"/>
+      <c r="I33" s="165"/>
+      <c r="J33" s="19"/>
+    </row>
+    <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="164" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="165"/>
+      <c r="D34" s="165"/>
+      <c r="E34" s="166"/>
+      <c r="F34" s="164" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" s="165"/>
+      <c r="H34" s="165"/>
+      <c r="I34" s="165"/>
+      <c r="J34" s="19"/>
+    </row>
+    <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="164" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="165"/>
+      <c r="D35" s="165"/>
+      <c r="E35" s="166"/>
+      <c r="F35" s="164" t="s">
+        <v>43</v>
+      </c>
+      <c r="G35" s="165"/>
+      <c r="H35" s="165"/>
+      <c r="I35" s="165"/>
+      <c r="J35" s="19"/>
+    </row>
+    <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="164" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="165"/>
+      <c r="D36" s="165"/>
+      <c r="E36" s="166"/>
+      <c r="F36" s="164" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" s="165"/>
+      <c r="H36" s="165"/>
+      <c r="I36" s="165"/>
+      <c r="J36" s="19"/>
+    </row>
+    <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="164" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="165"/>
+      <c r="D37" s="165"/>
+      <c r="E37" s="166"/>
+      <c r="F37" s="164" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="165"/>
+      <c r="H37" s="165"/>
+      <c r="I37" s="165"/>
+      <c r="J37" s="19"/>
+    </row>
+    <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="164" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="165"/>
+      <c r="D38" s="165"/>
+      <c r="E38" s="166"/>
+      <c r="F38" s="164" t="s">
+        <v>48</v>
+      </c>
+      <c r="G38" s="165"/>
+      <c r="H38" s="165"/>
+      <c r="I38" s="165"/>
+      <c r="J38" s="19"/>
+    </row>
+    <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="9"/>
-    </row>
-    <row r="31" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="159" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="160"/>
-      <c r="D31" s="160"/>
-      <c r="E31" s="161"/>
-      <c r="F31" s="159" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="160"/>
-      <c r="H31" s="160"/>
-      <c r="I31" s="160"/>
-      <c r="J31" s="34"/>
-      <c r="N31" s="36"/>
-      <c r="O31" s="36"/>
-      <c r="P31" s="36"/>
-      <c r="Q31" s="36"/>
-      <c r="R31" s="36"/>
-      <c r="S31" s="36"/>
-      <c r="T31" s="36"/>
-      <c r="U31" s="36"/>
-      <c r="V31" s="36"/>
-      <c r="W31" s="36"/>
-      <c r="X31" s="36"/>
-      <c r="Y31" s="36"/>
-      <c r="Z31" s="36"/>
-      <c r="AA31" s="36"/>
-      <c r="AB31" s="36"/>
-      <c r="AC31" s="36"/>
-      <c r="AD31" s="36"/>
-    </row>
-    <row r="32" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="156" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="157"/>
-      <c r="D32" s="157"/>
-      <c r="E32" s="158"/>
-      <c r="F32" s="156" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="157"/>
-      <c r="H32" s="157"/>
-      <c r="I32" s="157"/>
-      <c r="J32" s="19"/>
-    </row>
-    <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="156" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="157"/>
-      <c r="D33" s="157"/>
-      <c r="E33" s="158"/>
-      <c r="F33" s="156" t="s">
-        <v>43</v>
-      </c>
-      <c r="G33" s="157"/>
-      <c r="H33" s="157"/>
-      <c r="I33" s="157"/>
-      <c r="J33" s="19"/>
-    </row>
-    <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="156" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="157"/>
-      <c r="D34" s="157"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="156" t="s">
-        <v>44</v>
-      </c>
-      <c r="G34" s="157"/>
-      <c r="H34" s="157"/>
-      <c r="I34" s="157"/>
-      <c r="J34" s="19"/>
-    </row>
-    <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="156" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="157"/>
-      <c r="D35" s="157"/>
-      <c r="E35" s="158"/>
-      <c r="F35" s="156" t="s">
-        <v>45</v>
-      </c>
-      <c r="G35" s="157"/>
-      <c r="H35" s="157"/>
-      <c r="I35" s="157"/>
-      <c r="J35" s="19"/>
-    </row>
-    <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="156" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="157"/>
-      <c r="D36" s="157"/>
-      <c r="E36" s="158"/>
-      <c r="F36" s="156" t="s">
-        <v>47</v>
-      </c>
-      <c r="G36" s="157"/>
-      <c r="H36" s="157"/>
-      <c r="I36" s="157"/>
-      <c r="J36" s="19"/>
-    </row>
-    <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="156" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="157"/>
-      <c r="D37" s="157"/>
-      <c r="E37" s="158"/>
-      <c r="F37" s="156" t="s">
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="19"/>
+    </row>
+    <row r="40" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="167" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="168"/>
+      <c r="D40" s="168"/>
+      <c r="E40" s="169"/>
+      <c r="F40" s="167" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="170"/>
+      <c r="H40" s="170"/>
+      <c r="I40" s="170"/>
+      <c r="J40" s="34"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="36"/>
+      <c r="Q40" s="36"/>
+      <c r="R40" s="36"/>
+      <c r="S40" s="36"/>
+      <c r="T40" s="36"/>
+      <c r="U40" s="36"/>
+      <c r="V40" s="36"/>
+      <c r="W40" s="36"/>
+      <c r="X40" s="36"/>
+      <c r="Y40" s="36"/>
+      <c r="Z40" s="36"/>
+      <c r="AA40" s="36"/>
+      <c r="AB40" s="36"/>
+      <c r="AC40" s="36"/>
+      <c r="AD40" s="36"/>
+    </row>
+    <row r="41" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="164" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="165"/>
+      <c r="D41" s="165"/>
+      <c r="E41" s="166"/>
+      <c r="F41" s="164" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="165"/>
+      <c r="H41" s="165"/>
+      <c r="I41" s="165"/>
+      <c r="J41" s="19"/>
+    </row>
+    <row r="42" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="19"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="G37" s="157"/>
-      <c r="H37" s="157"/>
-      <c r="I37" s="157"/>
-      <c r="J37" s="19"/>
-    </row>
-    <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="19"/>
-    </row>
-    <row r="39" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="159" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="160"/>
-      <c r="D39" s="160"/>
-      <c r="E39" s="161"/>
-      <c r="F39" s="159" t="s">
-        <v>15</v>
-      </c>
-      <c r="G39" s="162"/>
-      <c r="H39" s="162"/>
-      <c r="I39" s="162"/>
-      <c r="J39" s="34"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="36"/>
-      <c r="R39" s="36"/>
-      <c r="S39" s="36"/>
-      <c r="T39" s="36"/>
-      <c r="U39" s="36"/>
-      <c r="V39" s="36"/>
-      <c r="W39" s="36"/>
-      <c r="X39" s="36"/>
-      <c r="Y39" s="36"/>
-      <c r="Z39" s="36"/>
-      <c r="AA39" s="36"/>
-      <c r="AB39" s="36"/>
-      <c r="AC39" s="36"/>
-      <c r="AD39" s="36"/>
-    </row>
-    <row r="40" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="156" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="157"/>
-      <c r="D40" s="157"/>
-      <c r="E40" s="158"/>
-      <c r="F40" s="156" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="157"/>
-      <c r="H40" s="157"/>
-      <c r="I40" s="157"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="41" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="19"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="20" t="s">
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="19"/>
+    </row>
+    <row r="43" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B43" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="19"/>
-    </row>
-    <row r="42" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="G42" s="28"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="39"/>
-      <c r="C43" s="31" t="s">
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="31"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="27"/>
       <c r="G43" s="28"/>
       <c r="H43" s="38"/>
       <c r="I43" s="38"/>
       <c r="J43" s="19"/>
     </row>
-    <row r="44" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="G44" s="38"/>
+    <row r="44" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B44" s="39"/>
+      <c r="C44" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="31"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="28"/>
       <c r="H44" s="38"/>
       <c r="I44" s="38"/>
       <c r="J44" s="19"/>
     </row>
     <row r="45" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B45" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C45" s="28"/>
       <c r="D45" s="28"/>
-      <c r="E45" s="29"/>
+      <c r="E45" s="37"/>
       <c r="F45" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G45" s="38"/>
       <c r="H45" s="38"/>
@@ -2823,13 +2832,13 @@
     </row>
     <row r="46" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B46" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="29"/>
-      <c r="F46" s="28" t="s">
-        <v>54</v>
+      <c r="F46" s="27" t="s">
+        <v>52</v>
       </c>
       <c r="G46" s="38"/>
       <c r="H46" s="38"/>
@@ -2838,13 +2847,13 @@
     </row>
     <row r="47" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B47" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C47" s="28"/>
       <c r="D47" s="28"/>
       <c r="E47" s="29"/>
       <c r="F47" s="28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G47" s="38"/>
       <c r="H47" s="38"/>
@@ -2853,78 +2862,82 @@
     </row>
     <row r="48" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C48" s="28"/>
       <c r="D48" s="28"/>
       <c r="E48" s="29"/>
       <c r="F48" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="19"/>
+    </row>
+    <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="19"/>
+    </row>
+    <row r="50" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="19"/>
+      <c r="C50" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="31"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H50" s="31"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="19"/>
+    </row>
+    <row r="51" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="19"/>
-    </row>
-    <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="19"/>
-      <c r="C49" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="D49" s="31"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H49" s="31"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="19"/>
-    </row>
-    <row r="50" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="40" t="s">
+      <c r="C51" s="41"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="G50" s="41"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="42"/>
-      <c r="J50" s="15"/>
-    </row>
-    <row r="51" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="43"/>
-      <c r="C51" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="D51" s="45"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="H51" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="I51" s="46"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="42"/>
       <c r="J51" s="15"/>
     </row>
-    <row r="52" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="15"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="48"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
+    <row r="52" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="43"/>
+      <c r="C52" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="45"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="H52" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="I52" s="46"/>
       <c r="J52" s="15"/>
     </row>
-    <row r="53" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="15"/>
       <c r="C53" s="48"/>
       <c r="D53" s="48"/>
@@ -3023,22 +3036,31 @@
       <c r="I61" s="15"/>
       <c r="J61" s="15"/>
     </row>
-    <row r="62" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="62" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B62" s="15"/>
+      <c r="C62" s="48"/>
+      <c r="D62" s="48"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+    </row>
     <row r="63" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="64" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="65" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="66" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="67" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="75" spans="6:7" x14ac:dyDescent="0.45">
-      <c r="F75" s="10"/>
-      <c r="G75" s="10"/>
-    </row>
-    <row r="80" spans="6:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="87" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="68" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="76" spans="6:7" x14ac:dyDescent="0.45">
+      <c r="F76" s="10"/>
+      <c r="G76" s="10"/>
+    </row>
+    <row r="81" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="88" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="B3:E3"/>
@@ -3047,80 +3069,82 @@
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="F10:I10"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:I11"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B15:E15"/>
     <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B16:D16"/>
     <mergeCell ref="F16:I16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="E18:G18"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:G19"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="F25:I25"/>
+    <mergeCell ref="B26:E26"/>
     <mergeCell ref="F26:I26"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:D27"/>
     <mergeCell ref="F27:I27"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:D28"/>
     <mergeCell ref="F28:I28"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="F41:I41"/>
     <mergeCell ref="B36:E36"/>
     <mergeCell ref="F36:I36"/>
     <mergeCell ref="B37:E37"/>
     <mergeCell ref="F37:I37"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:I40"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="F33:I33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
   </mergeCells>
-  <conditionalFormatting sqref="H18">
+  <conditionalFormatting sqref="H19">
     <cfRule type="notContainsBlanks" dxfId="3" priority="2">
-      <formula>LEN(TRIM(H18))&gt;0</formula>
+      <formula>LEN(TRIM(H19))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J17">
+  <conditionalFormatting sqref="J18">
     <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(J17))&gt;0</formula>
+      <formula>LEN(TRIM(J18))&gt;0</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="1" priority="4">
-      <formula>LEN(TRIM(J17))&gt;0</formula>
+      <formula>LEN(TRIM(J18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J18 D18:E19 B19:C19 I19:J20 B20 E20">
+  <conditionalFormatting sqref="J19 D19:E20 B20:C20 I20:J21 B21 E21">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B18))&gt;0</formula>
+      <formula>LEN(TRIM(B19))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{F8B8C03B-01BB-43AB-8211-944828195CE5}">
-      <formula1>_xlfn.ANCHORARRAY($V$1)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3" xr:uid="{F8B8C03B-01BB-43AB-8211-944828195CE5}">
+      <formula1>_xlfn.ANCHORARRAY($V$2)</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
@@ -3137,8 +3161,8 @@
   </sheetPr>
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3160,14 +3184,17 @@
     <col min="15" max="18" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="0.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="56"/>
+      <c r="G1" s="161" t="s">
+        <v>49</v>
+      </c>
       <c r="N1" s="58"/>
     </row>
     <row r="2" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="89"/>
       <c r="B2" s="119" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" s="119"/>
       <c r="D2" s="119"/>
@@ -3175,7 +3202,7 @@
       <c r="F2" s="119"/>
       <c r="G2" s="119"/>
       <c r="H2" s="122" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I2" s="119"/>
       <c r="J2" s="119"/>
@@ -3187,7 +3214,7 @@
     <row r="3" spans="1:14" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="89"/>
       <c r="B3" s="120" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C3" s="120"/>
       <c r="D3" s="120"/>
@@ -3195,7 +3222,7 @@
       <c r="F3" s="121"/>
       <c r="G3" s="121"/>
       <c r="H3" s="123" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I3" s="120"/>
       <c r="J3" s="120"/>
@@ -3207,7 +3234,7 @@
     <row r="4" spans="1:14" s="86" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="88"/>
       <c r="B4" s="120" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C4" s="120"/>
       <c r="D4" s="120"/>
@@ -3215,7 +3242,7 @@
       <c r="F4" s="120"/>
       <c r="G4" s="120"/>
       <c r="H4" s="123" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I4" s="120"/>
       <c r="J4" s="120"/>
@@ -3227,7 +3254,7 @@
     <row r="5" spans="1:14" s="86" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="87"/>
       <c r="B5" s="120" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" s="120"/>
       <c r="D5" s="120"/>
@@ -3235,7 +3262,7 @@
       <c r="F5" s="120"/>
       <c r="G5" s="120"/>
       <c r="H5" s="123" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I5" s="120"/>
       <c r="J5" s="120"/>
@@ -3247,7 +3274,7 @@
     <row r="6" spans="1:14" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="56"/>
       <c r="B6" s="110" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C6" s="110"/>
       <c r="D6" s="110"/>
@@ -3255,7 +3282,7 @@
       <c r="F6" s="110"/>
       <c r="G6" s="110"/>
       <c r="H6" s="96" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I6" s="97"/>
       <c r="J6" s="97"/>
@@ -3267,7 +3294,7 @@
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="56"/>
       <c r="B7" s="113" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="124"/>
       <c r="D7" s="124"/>
@@ -3275,7 +3302,7 @@
       <c r="F7" s="124"/>
       <c r="G7" s="124"/>
       <c r="H7" s="99" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" s="100"/>
       <c r="J7" s="100"/>
@@ -3287,7 +3314,7 @@
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="56"/>
       <c r="B8" s="125" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="125"/>
       <c r="D8" s="125"/>
@@ -3295,7 +3322,7 @@
       <c r="F8" s="125"/>
       <c r="G8" s="125"/>
       <c r="H8" s="101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I8" s="102"/>
       <c r="J8" s="102"/>
@@ -3307,7 +3334,7 @@
     <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="56"/>
       <c r="B9" s="126" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="126"/>
       <c r="D9" s="126"/>
@@ -3315,7 +3342,7 @@
       <c r="F9" s="126"/>
       <c r="G9" s="126"/>
       <c r="H9" s="103" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I9" s="98"/>
       <c r="J9" s="98"/>
@@ -3327,7 +3354,7 @@
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="56"/>
       <c r="B10" s="113" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="113"/>
       <c r="D10" s="113"/>
@@ -3335,7 +3362,7 @@
       <c r="F10" s="113"/>
       <c r="G10" s="113"/>
       <c r="H10" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" s="98"/>
       <c r="J10" s="98"/>
@@ -3347,7 +3374,7 @@
     <row r="11" spans="1:14" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="56"/>
       <c r="B11" s="102" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="102"/>
       <c r="D11" s="102"/>
@@ -3355,7 +3382,7 @@
       <c r="F11" s="102"/>
       <c r="G11" s="118"/>
       <c r="H11" s="155" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="102"/>
       <c r="J11" s="102"/>
@@ -3367,7 +3394,7 @@
     <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="56"/>
       <c r="B12" s="126" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C12" s="126"/>
       <c r="D12" s="126"/>
@@ -3375,7 +3402,7 @@
       <c r="F12" s="126"/>
       <c r="G12" s="126"/>
       <c r="H12" s="96" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I12" s="97"/>
       <c r="J12" s="97"/>
@@ -3387,7 +3414,7 @@
     <row r="13" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="56"/>
       <c r="B13" s="113" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="113"/>
       <c r="D13" s="113"/>
@@ -3395,7 +3422,7 @@
       <c r="F13" s="113"/>
       <c r="G13" s="113"/>
       <c r="H13" s="99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" s="100"/>
       <c r="J13" s="100"/>
@@ -3407,7 +3434,7 @@
     <row r="14" spans="1:14" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="56"/>
       <c r="B14" s="102" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="102"/>
       <c r="D14" s="102"/>
@@ -3415,7 +3442,7 @@
       <c r="F14" s="102"/>
       <c r="G14" s="118"/>
       <c r="H14" s="155" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I14" s="102"/>
       <c r="J14" s="102"/>
@@ -3427,27 +3454,27 @@
     <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="85"/>
       <c r="B15" s="104" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="104"/>
       <c r="D15" s="105" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E15" s="105"/>
       <c r="F15" s="105" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G15" s="105"/>
       <c r="H15" s="106" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I15" s="105"/>
       <c r="J15" s="127" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K15" s="127"/>
       <c r="L15" s="151" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M15" s="151"/>
       <c r="N15" s="58"/>
@@ -3455,27 +3482,27 @@
     <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="56"/>
       <c r="B16" s="118" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="107"/>
-      <c r="D16" s="194" t="s">
-        <v>112</v>
+      <c r="D16" s="156" t="s">
+        <v>111</v>
       </c>
       <c r="E16" s="108"/>
       <c r="F16" s="144" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G16" s="108"/>
-      <c r="H16" s="197" t="s">
-        <v>111</v>
+      <c r="H16" s="159" t="s">
+        <v>110</v>
       </c>
       <c r="I16" s="108"/>
       <c r="J16" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K16" s="109"/>
       <c r="L16" s="152" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M16" s="152"/>
       <c r="N16" s="58"/>
@@ -3483,27 +3510,27 @@
     <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="56"/>
       <c r="B17" s="126" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C17" s="126"/>
       <c r="D17" s="126" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E17" s="130"/>
       <c r="F17" s="143" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G17" s="143"/>
       <c r="H17" s="103" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I17" s="98"/>
       <c r="J17" s="111" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K17" s="98"/>
       <c r="L17" s="153" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M17" s="154"/>
       <c r="N17" s="58"/>
@@ -3511,27 +3538,27 @@
     <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="56"/>
       <c r="B18" s="102" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C18" s="125"/>
-      <c r="D18" s="195" t="s">
-        <v>122</v>
+      <c r="D18" s="157" t="s">
+        <v>121</v>
       </c>
       <c r="E18" s="109"/>
-      <c r="F18" s="196" t="s">
-        <v>61</v>
+      <c r="F18" s="158" t="s">
+        <v>60</v>
       </c>
       <c r="G18" s="144"/>
-      <c r="H18" s="197" t="s">
-        <v>121</v>
+      <c r="H18" s="159" t="s">
+        <v>120</v>
       </c>
       <c r="I18" s="109"/>
-      <c r="J18" s="195" t="s">
-        <v>120</v>
+      <c r="J18" s="157" t="s">
+        <v>119</v>
       </c>
       <c r="K18" s="109"/>
       <c r="L18" s="152" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M18" s="152"/>
       <c r="N18" s="58"/>
@@ -3539,21 +3566,21 @@
     <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="56"/>
       <c r="B19" s="131" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" s="131"/>
       <c r="D19" s="131" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E19" s="131"/>
       <c r="F19" s="145"/>
       <c r="G19" s="145"/>
       <c r="H19" s="148" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I19" s="128"/>
       <c r="J19" s="126" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K19" s="126"/>
       <c r="L19" s="126"/>
@@ -3562,22 +3589,22 @@
     </row>
     <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="56"/>
-      <c r="B20" s="194" t="s">
-        <v>62</v>
+      <c r="B20" s="156" t="s">
+        <v>61</v>
       </c>
       <c r="C20" s="112"/>
       <c r="D20" s="129" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E20" s="129"/>
       <c r="F20" s="146"/>
       <c r="G20" s="146"/>
-      <c r="H20" s="198" t="s">
-        <v>65</v>
+      <c r="H20" s="160" t="s">
+        <v>64</v>
       </c>
       <c r="I20" s="108"/>
       <c r="J20" s="113" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K20" s="114"/>
       <c r="L20" s="109"/>
@@ -3614,60 +3641,60 @@
     <row r="22" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="56"/>
       <c r="B22" s="60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" s="132" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D22" s="132"/>
       <c r="E22" s="132"/>
       <c r="F22" s="150"/>
       <c r="G22" s="132"/>
       <c r="H22" s="60" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I22" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J22" s="80" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K22" s="132" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L22" s="132"/>
       <c r="M22" s="60" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N22" s="58"/>
     </row>
     <row r="23" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="56"/>
       <c r="B23" s="139" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="192" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="192"/>
-      <c r="E23" s="192"/>
-      <c r="F23" s="192"/>
+      <c r="C23" s="200" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="200"/>
+      <c r="E23" s="200"/>
+      <c r="F23" s="200"/>
       <c r="G23" s="140"/>
       <c r="H23" s="141" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I23" s="79" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J23" s="78">
         <v>14</v>
       </c>
-      <c r="K23" s="193" t="s">
-        <v>94</v>
-      </c>
-      <c r="L23" s="193"/>
+      <c r="K23" s="201" t="s">
+        <v>93</v>
+      </c>
+      <c r="L23" s="201"/>
       <c r="M23" s="77" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N23" s="58"/>
     </row>
@@ -3679,20 +3706,20 @@
       <c r="F24" s="137"/>
       <c r="G24" s="137"/>
       <c r="H24" s="138" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I24" s="76" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J24" s="75">
         <v>14</v>
       </c>
       <c r="K24" s="142" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L24" s="142"/>
       <c r="M24" s="90" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N24" s="58"/>
     </row>
@@ -3904,7 +3931,7 @@
     <row r="38" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="56"/>
       <c r="B38" s="92" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="73"/>
       <c r="D38" s="73"/>
@@ -3913,7 +3940,7 @@
       <c r="G38" s="72"/>
       <c r="H38" s="71"/>
       <c r="I38" s="134" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J38" s="133"/>
       <c r="K38" s="133"/>
@@ -3924,7 +3951,7 @@
     <row r="39" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="56"/>
       <c r="B39" s="93" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" s="69"/>
       <c r="D39" s="69"/>
@@ -3942,7 +3969,7 @@
     <row r="40" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="56"/>
       <c r="B40" s="93" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" s="69"/>
       <c r="D40" s="69"/>
@@ -3960,7 +3987,7 @@
     <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="56"/>
       <c r="B41" s="93" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C41" s="69"/>
       <c r="D41" s="69"/>
@@ -3978,7 +4005,7 @@
     <row r="42" spans="1:14" s="64" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="68"/>
       <c r="B42" s="94" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C42" s="67"/>
       <c r="D42" s="67"/>

</xml_diff>

<commit_message>
assortiment fixed + grouping rows by pack in sales contract added
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4772B29-DF2C-47FD-991C-571D2DD65396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF72E3B-41EE-4F43-BCFF-2B4B42220B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="1875" windowWidth="14385" windowHeight="8085" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -1307,6 +1307,51 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1316,6 +1361,48 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1327,93 +1414,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1839,18 +1839,18 @@
       <c r="I1" s="162"/>
     </row>
     <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="194" t="s">
+      <c r="B2" s="164" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="194" t="s">
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
       <c r="J2" s="163"/>
       <c r="L2" s="11"/>
       <c r="N2" s="18"/>
@@ -1860,18 +1860,18 @@
       <c r="AD2" s="18"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="167" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="199"/>
-      <c r="F3" s="197" t="s">
+      <c r="C3" s="168"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="167" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="198"/>
-      <c r="H3" s="198"/>
-      <c r="I3" s="198"/>
+      <c r="G3" s="168"/>
+      <c r="H3" s="168"/>
+      <c r="I3" s="168"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1888,18 +1888,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="197" t="s">
+      <c r="B4" s="167" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="198"/>
-      <c r="D4" s="198"/>
-      <c r="E4" s="199"/>
-      <c r="F4" s="197" t="s">
+      <c r="C4" s="168"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="169"/>
+      <c r="F4" s="167" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="198"/>
-      <c r="H4" s="198"/>
-      <c r="I4" s="198"/>
+      <c r="G4" s="168"/>
+      <c r="H4" s="168"/>
+      <c r="I4" s="168"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1920,18 +1920,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="191" t="s">
+      <c r="B5" s="170" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="192"/>
-      <c r="D5" s="192"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="191" t="s">
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="170" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="192"/>
-      <c r="H5" s="192"/>
-      <c r="I5" s="192"/>
+      <c r="G5" s="171"/>
+      <c r="H5" s="171"/>
+      <c r="I5" s="171"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1940,18 +1940,18 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="171" t="s">
+      <c r="B6" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="172"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="171" t="s">
+      <c r="C6" s="174"/>
+      <c r="D6" s="174"/>
+      <c r="E6" s="175"/>
+      <c r="F6" s="173" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="172"/>
-      <c r="H6" s="172"/>
-      <c r="I6" s="172"/>
+      <c r="G6" s="174"/>
+      <c r="H6" s="174"/>
+      <c r="I6" s="174"/>
       <c r="J6" s="54"/>
       <c r="L6" s="55"/>
       <c r="O6" s="10"/>
@@ -1996,48 +1996,48 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="181"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="182"/>
-      <c r="F8" s="164" t="s">
+      <c r="C8" s="177"/>
+      <c r="D8" s="177"/>
+      <c r="E8" s="178"/>
+      <c r="F8" s="179" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="165"/>
-      <c r="H8" s="165"/>
-      <c r="I8" s="165"/>
+      <c r="G8" s="180"/>
+      <c r="H8" s="180"/>
+      <c r="I8" s="180"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="164" t="s">
+      <c r="B9" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="165"/>
-      <c r="D9" s="165"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="164" t="s">
+      <c r="C9" s="180"/>
+      <c r="D9" s="180"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="165"/>
-      <c r="H9" s="165"/>
-      <c r="I9" s="165"/>
+      <c r="G9" s="180"/>
+      <c r="H9" s="180"/>
+      <c r="I9" s="180"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="164" t="s">
+      <c r="B10" s="179" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="166"/>
-      <c r="F10" s="164" t="s">
+      <c r="C10" s="180"/>
+      <c r="D10" s="180"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="179" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="165"/>
-      <c r="H10" s="165"/>
-      <c r="I10" s="165"/>
+      <c r="G10" s="180"/>
+      <c r="H10" s="180"/>
+      <c r="I10" s="180"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -2058,18 +2058,18 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="171" t="s">
+      <c r="B11" s="173" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="172"/>
-      <c r="D11" s="172"/>
-      <c r="E11" s="173"/>
-      <c r="F11" s="171" t="s">
+      <c r="C11" s="174"/>
+      <c r="D11" s="174"/>
+      <c r="E11" s="175"/>
+      <c r="F11" s="173" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="172"/>
-      <c r="H11" s="172"/>
-      <c r="I11" s="172"/>
+      <c r="G11" s="174"/>
+      <c r="H11" s="174"/>
+      <c r="I11" s="174"/>
       <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -2112,18 +2112,18 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="164" t="s">
+      <c r="B13" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="165"/>
-      <c r="E13" s="166"/>
-      <c r="F13" s="164" t="s">
+      <c r="C13" s="180"/>
+      <c r="D13" s="180"/>
+      <c r="E13" s="181"/>
+      <c r="F13" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="165"/>
-      <c r="H13" s="165"/>
-      <c r="I13" s="165"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2141,18 +2141,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="165"/>
-      <c r="E14" s="166"/>
-      <c r="F14" s="164" t="s">
+      <c r="C14" s="180"/>
+      <c r="D14" s="180"/>
+      <c r="E14" s="181"/>
+      <c r="F14" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="165"/>
-      <c r="H14" s="165"/>
-      <c r="I14" s="165"/>
+      <c r="G14" s="180"/>
+      <c r="H14" s="180"/>
+      <c r="I14" s="180"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2170,18 +2170,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="164" t="s">
+      <c r="B15" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="165"/>
-      <c r="E15" s="166"/>
-      <c r="F15" s="164" t="s">
+      <c r="C15" s="180"/>
+      <c r="D15" s="180"/>
+      <c r="E15" s="181"/>
+      <c r="F15" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="165"/>
-      <c r="H15" s="165"/>
-      <c r="I15" s="165"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="180"/>
+      <c r="I15" s="180"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2199,18 +2199,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="183" t="s">
+      <c r="B16" s="182" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="184"/>
-      <c r="D16" s="184"/>
+      <c r="C16" s="183"/>
+      <c r="D16" s="183"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="183" t="s">
+      <c r="F16" s="182" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="184"/>
-      <c r="H16" s="184"/>
-      <c r="I16" s="185"/>
+      <c r="G16" s="183"/>
+      <c r="H16" s="183"/>
+      <c r="I16" s="184"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2228,18 +2228,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="164" t="s">
+      <c r="B17" s="179" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="186"/>
-      <c r="D17" s="186"/>
-      <c r="E17" s="187"/>
-      <c r="F17" s="188" t="s">
+      <c r="C17" s="185"/>
+      <c r="D17" s="185"/>
+      <c r="E17" s="186"/>
+      <c r="F17" s="187" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="186"/>
-      <c r="H17" s="186"/>
-      <c r="I17" s="186"/>
+      <c r="G17" s="185"/>
+      <c r="H17" s="185"/>
+      <c r="I17" s="185"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2257,18 +2257,18 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="189" t="s">
+      <c r="B18" s="188" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="190"/>
+      <c r="C18" s="189"/>
       <c r="D18" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="190" t="s">
+      <c r="E18" s="189" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="190"/>
-      <c r="G18" s="190"/>
+      <c r="F18" s="189"/>
+      <c r="G18" s="189"/>
       <c r="H18" s="23" t="s">
         <v>80</v>
       </c>
@@ -2292,18 +2292,18 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="174" t="s">
+      <c r="B19" s="190" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="175"/>
+      <c r="C19" s="191"/>
       <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="176" t="s">
+      <c r="E19" s="192" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="176"/>
-      <c r="G19" s="176"/>
+      <c r="F19" s="192"/>
+      <c r="G19" s="192"/>
       <c r="H19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2452,18 +2452,18 @@
       <c r="AD24" s="10"/>
     </row>
     <row r="25" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="177" t="s">
+      <c r="B25" s="193" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="178"/>
-      <c r="D25" s="178"/>
-      <c r="E25" s="179"/>
-      <c r="F25" s="177" t="s">
+      <c r="C25" s="194"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
+      <c r="F25" s="193" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="178"/>
-      <c r="H25" s="178"/>
-      <c r="I25" s="178"/>
+      <c r="G25" s="194"/>
+      <c r="H25" s="194"/>
+      <c r="I25" s="194"/>
       <c r="J25" s="22"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
@@ -2484,48 +2484,48 @@
       <c r="AD25" s="10"/>
     </row>
     <row r="26" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="164" t="s">
+      <c r="B26" s="179" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="165"/>
-      <c r="D26" s="165"/>
-      <c r="E26" s="166"/>
-      <c r="F26" s="164" t="s">
+      <c r="C26" s="180"/>
+      <c r="D26" s="180"/>
+      <c r="E26" s="181"/>
+      <c r="F26" s="179" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="165"/>
-      <c r="H26" s="165"/>
-      <c r="I26" s="165"/>
+      <c r="G26" s="180"/>
+      <c r="H26" s="180"/>
+      <c r="I26" s="180"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="180" t="s">
+      <c r="B27" s="176" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="181"/>
-      <c r="D27" s="181"/>
-      <c r="E27" s="182"/>
-      <c r="F27" s="164" t="s">
+      <c r="C27" s="177"/>
+      <c r="D27" s="177"/>
+      <c r="E27" s="178"/>
+      <c r="F27" s="179" t="s">
         <v>85</v>
       </c>
-      <c r="G27" s="165"/>
-      <c r="H27" s="165"/>
-      <c r="I27" s="166"/>
+      <c r="G27" s="180"/>
+      <c r="H27" s="180"/>
+      <c r="I27" s="181"/>
       <c r="J27" s="19"/>
     </row>
     <row r="28" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="171" t="s">
+      <c r="B28" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="172"/>
-      <c r="D28" s="172"/>
+      <c r="C28" s="174"/>
+      <c r="D28" s="174"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="171" t="s">
+      <c r="F28" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="172"/>
-      <c r="H28" s="172"/>
-      <c r="I28" s="173"/>
+      <c r="G28" s="174"/>
+      <c r="H28" s="174"/>
+      <c r="I28" s="175"/>
       <c r="J28" s="22"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
@@ -2546,33 +2546,33 @@
       <c r="AD28" s="10"/>
     </row>
     <row r="29" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="164" t="s">
+      <c r="B29" s="179" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="165"/>
-      <c r="D29" s="165"/>
-      <c r="E29" s="166"/>
-      <c r="F29" s="164" t="s">
+      <c r="C29" s="180"/>
+      <c r="D29" s="180"/>
+      <c r="E29" s="181"/>
+      <c r="F29" s="179" t="s">
         <v>37</v>
       </c>
-      <c r="G29" s="165"/>
-      <c r="H29" s="165"/>
-      <c r="I29" s="165"/>
+      <c r="G29" s="180"/>
+      <c r="H29" s="180"/>
+      <c r="I29" s="180"/>
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="171" t="s">
+      <c r="B30" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="172"/>
-      <c r="D30" s="172"/>
+      <c r="C30" s="174"/>
+      <c r="D30" s="174"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="171" t="s">
+      <c r="F30" s="173" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="172"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="173"/>
+      <c r="G30" s="174"/>
+      <c r="H30" s="174"/>
+      <c r="I30" s="175"/>
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -2591,18 +2591,18 @@
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="167" t="s">
+      <c r="B32" s="196" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="168"/>
-      <c r="D32" s="168"/>
-      <c r="E32" s="169"/>
-      <c r="F32" s="167" t="s">
+      <c r="C32" s="197"/>
+      <c r="D32" s="197"/>
+      <c r="E32" s="198"/>
+      <c r="F32" s="196" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="168"/>
-      <c r="H32" s="168"/>
-      <c r="I32" s="168"/>
+      <c r="G32" s="197"/>
+      <c r="H32" s="197"/>
+      <c r="I32" s="197"/>
       <c r="J32" s="34"/>
       <c r="N32" s="36"/>
       <c r="O32" s="36"/>
@@ -2623,93 +2623,93 @@
       <c r="AD32" s="36"/>
     </row>
     <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="164" t="s">
+      <c r="B33" s="179" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="165"/>
-      <c r="D33" s="165"/>
-      <c r="E33" s="166"/>
-      <c r="F33" s="164" t="s">
+      <c r="C33" s="180"/>
+      <c r="D33" s="180"/>
+      <c r="E33" s="181"/>
+      <c r="F33" s="179" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="165"/>
-      <c r="H33" s="165"/>
-      <c r="I33" s="165"/>
+      <c r="G33" s="180"/>
+      <c r="H33" s="180"/>
+      <c r="I33" s="180"/>
       <c r="J33" s="19"/>
     </row>
     <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="164" t="s">
+      <c r="B34" s="179" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="165"/>
-      <c r="D34" s="165"/>
-      <c r="E34" s="166"/>
-      <c r="F34" s="164" t="s">
+      <c r="C34" s="180"/>
+      <c r="D34" s="180"/>
+      <c r="E34" s="181"/>
+      <c r="F34" s="179" t="s">
         <v>42</v>
       </c>
-      <c r="G34" s="165"/>
-      <c r="H34" s="165"/>
-      <c r="I34" s="165"/>
+      <c r="G34" s="180"/>
+      <c r="H34" s="180"/>
+      <c r="I34" s="180"/>
       <c r="J34" s="19"/>
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="164" t="s">
+      <c r="B35" s="179" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="165"/>
-      <c r="D35" s="165"/>
-      <c r="E35" s="166"/>
-      <c r="F35" s="164" t="s">
+      <c r="C35" s="180"/>
+      <c r="D35" s="180"/>
+      <c r="E35" s="181"/>
+      <c r="F35" s="179" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="165"/>
-      <c r="H35" s="165"/>
-      <c r="I35" s="165"/>
+      <c r="G35" s="180"/>
+      <c r="H35" s="180"/>
+      <c r="I35" s="180"/>
       <c r="J35" s="19"/>
     </row>
     <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="164" t="s">
+      <c r="B36" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="165"/>
-      <c r="D36" s="165"/>
-      <c r="E36" s="166"/>
-      <c r="F36" s="164" t="s">
+      <c r="C36" s="180"/>
+      <c r="D36" s="180"/>
+      <c r="E36" s="181"/>
+      <c r="F36" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="165"/>
-      <c r="H36" s="165"/>
-      <c r="I36" s="165"/>
+      <c r="G36" s="180"/>
+      <c r="H36" s="180"/>
+      <c r="I36" s="180"/>
       <c r="J36" s="19"/>
     </row>
     <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="164" t="s">
+      <c r="B37" s="179" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="165"/>
-      <c r="D37" s="165"/>
-      <c r="E37" s="166"/>
-      <c r="F37" s="164" t="s">
+      <c r="C37" s="180"/>
+      <c r="D37" s="180"/>
+      <c r="E37" s="181"/>
+      <c r="F37" s="179" t="s">
         <v>46</v>
       </c>
-      <c r="G37" s="165"/>
-      <c r="H37" s="165"/>
-      <c r="I37" s="165"/>
+      <c r="G37" s="180"/>
+      <c r="H37" s="180"/>
+      <c r="I37" s="180"/>
       <c r="J37" s="19"/>
     </row>
     <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="164" t="s">
+      <c r="B38" s="179" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="165"/>
-      <c r="D38" s="165"/>
-      <c r="E38" s="166"/>
-      <c r="F38" s="164" t="s">
+      <c r="C38" s="180"/>
+      <c r="D38" s="180"/>
+      <c r="E38" s="181"/>
+      <c r="F38" s="179" t="s">
         <v>48</v>
       </c>
-      <c r="G38" s="165"/>
-      <c r="H38" s="165"/>
-      <c r="I38" s="165"/>
+      <c r="G38" s="180"/>
+      <c r="H38" s="180"/>
+      <c r="I38" s="180"/>
       <c r="J38" s="19"/>
     </row>
     <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2728,18 +2728,18 @@
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="167" t="s">
+      <c r="B40" s="196" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="168"/>
-      <c r="D40" s="168"/>
-      <c r="E40" s="169"/>
-      <c r="F40" s="167" t="s">
+      <c r="C40" s="197"/>
+      <c r="D40" s="197"/>
+      <c r="E40" s="198"/>
+      <c r="F40" s="196" t="s">
         <v>14</v>
       </c>
-      <c r="G40" s="170"/>
-      <c r="H40" s="170"/>
-      <c r="I40" s="170"/>
+      <c r="G40" s="199"/>
+      <c r="H40" s="199"/>
+      <c r="I40" s="199"/>
       <c r="J40" s="34"/>
       <c r="N40" s="36"/>
       <c r="O40" s="36"/>
@@ -2760,18 +2760,18 @@
       <c r="AD40" s="36"/>
     </row>
     <row r="41" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="164" t="s">
+      <c r="B41" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="165"/>
-      <c r="D41" s="165"/>
-      <c r="E41" s="166"/>
-      <c r="F41" s="164" t="s">
+      <c r="C41" s="180"/>
+      <c r="D41" s="180"/>
+      <c r="E41" s="181"/>
+      <c r="F41" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="G41" s="165"/>
-      <c r="H41" s="165"/>
-      <c r="I41" s="165"/>
+      <c r="G41" s="180"/>
+      <c r="H41" s="180"/>
+      <c r="I41" s="180"/>
       <c r="J41" s="19"/>
     </row>
     <row r="42" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3061,36 +3061,24 @@
     <row r="88" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="B19:C19"/>
@@ -3105,24 +3093,36 @@
     <mergeCell ref="F28:I28"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="notContainsBlanks" dxfId="3" priority="2">
@@ -3162,7 +3162,7 @@
   <dimension ref="A1:AC52"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
minor fixes to export templates added
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF72E3B-41EE-4F43-BCFF-2B4B42220B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D434E91-F94D-4AA5-A995-A418E846ABE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -870,7 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1307,6 +1307,96 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1325,102 +1415,13 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1839,18 +1840,18 @@
       <c r="I1" s="162"/>
     </row>
     <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="194" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="164" t="s">
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="194" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="165"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
       <c r="J2" s="163"/>
       <c r="L2" s="11"/>
       <c r="N2" s="18"/>
@@ -1860,18 +1861,18 @@
       <c r="AD2" s="18"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="167" t="s">
+      <c r="B3" s="197" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="167" t="s">
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="199"/>
+      <c r="F3" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="168"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="198"/>
+      <c r="I3" s="198"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1888,18 +1889,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="169"/>
-      <c r="F4" s="167" t="s">
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="199"/>
+      <c r="F4" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="168"/>
-      <c r="H4" s="168"/>
-      <c r="I4" s="168"/>
+      <c r="G4" s="198"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1920,18 +1921,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="170" t="s">
+      <c r="B5" s="191" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="171"/>
-      <c r="D5" s="171"/>
-      <c r="E5" s="172"/>
-      <c r="F5" s="170" t="s">
+      <c r="C5" s="192"/>
+      <c r="D5" s="192"/>
+      <c r="E5" s="193"/>
+      <c r="F5" s="191" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="171"/>
-      <c r="H5" s="171"/>
-      <c r="I5" s="171"/>
+      <c r="G5" s="192"/>
+      <c r="H5" s="192"/>
+      <c r="I5" s="192"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1940,18 +1941,18 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="173" t="s">
+      <c r="B6" s="171" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="174"/>
-      <c r="D6" s="174"/>
-      <c r="E6" s="175"/>
-      <c r="F6" s="173" t="s">
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="171" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="174"/>
-      <c r="H6" s="174"/>
-      <c r="I6" s="174"/>
+      <c r="G6" s="172"/>
+      <c r="H6" s="172"/>
+      <c r="I6" s="172"/>
       <c r="J6" s="54"/>
       <c r="L6" s="55"/>
       <c r="O6" s="10"/>
@@ -1996,48 +1997,48 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="176" t="s">
+      <c r="B8" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="177"/>
-      <c r="D8" s="177"/>
-      <c r="E8" s="178"/>
-      <c r="F8" s="179" t="s">
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="164" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="180"/>
-      <c r="H8" s="180"/>
-      <c r="I8" s="180"/>
+      <c r="G8" s="165"/>
+      <c r="H8" s="165"/>
+      <c r="I8" s="165"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="179" t="s">
+      <c r="B9" s="164" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="180"/>
-      <c r="D9" s="180"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="179" t="s">
+      <c r="C9" s="165"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="164" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="180"/>
-      <c r="H9" s="180"/>
-      <c r="I9" s="180"/>
+      <c r="G9" s="165"/>
+      <c r="H9" s="165"/>
+      <c r="I9" s="165"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="179" t="s">
+      <c r="B10" s="164" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="180"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="179" t="s">
+      <c r="C10" s="165"/>
+      <c r="D10" s="165"/>
+      <c r="E10" s="166"/>
+      <c r="F10" s="164" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="180"/>
-      <c r="H10" s="180"/>
-      <c r="I10" s="180"/>
+      <c r="G10" s="165"/>
+      <c r="H10" s="165"/>
+      <c r="I10" s="165"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -2058,18 +2059,18 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="173" t="s">
+      <c r="B11" s="171" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="174"/>
-      <c r="D11" s="174"/>
-      <c r="E11" s="175"/>
-      <c r="F11" s="173" t="s">
+      <c r="C11" s="172"/>
+      <c r="D11" s="172"/>
+      <c r="E11" s="173"/>
+      <c r="F11" s="171" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="174"/>
-      <c r="H11" s="174"/>
-      <c r="I11" s="174"/>
+      <c r="G11" s="172"/>
+      <c r="H11" s="172"/>
+      <c r="I11" s="172"/>
       <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -2112,18 +2113,18 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="179" t="s">
+      <c r="B13" s="164" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="180"/>
-      <c r="D13" s="180"/>
-      <c r="E13" s="181"/>
-      <c r="F13" s="179" t="s">
+      <c r="C13" s="165"/>
+      <c r="D13" s="165"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="164" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="180"/>
-      <c r="H13" s="180"/>
-      <c r="I13" s="180"/>
+      <c r="G13" s="165"/>
+      <c r="H13" s="165"/>
+      <c r="I13" s="165"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2141,18 +2142,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="179" t="s">
+      <c r="B14" s="164" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="180"/>
-      <c r="D14" s="180"/>
-      <c r="E14" s="181"/>
-      <c r="F14" s="179" t="s">
+      <c r="C14" s="165"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="180"/>
-      <c r="H14" s="180"/>
-      <c r="I14" s="180"/>
+      <c r="G14" s="165"/>
+      <c r="H14" s="165"/>
+      <c r="I14" s="165"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2170,18 +2171,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="179" t="s">
+      <c r="B15" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="180"/>
-      <c r="D15" s="180"/>
-      <c r="E15" s="181"/>
-      <c r="F15" s="179" t="s">
+      <c r="C15" s="165"/>
+      <c r="D15" s="165"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="180"/>
-      <c r="H15" s="180"/>
-      <c r="I15" s="180"/>
+      <c r="G15" s="165"/>
+      <c r="H15" s="165"/>
+      <c r="I15" s="165"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2199,18 +2200,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="182" t="s">
+      <c r="B16" s="183" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="183"/>
-      <c r="D16" s="183"/>
+      <c r="C16" s="184"/>
+      <c r="D16" s="184"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="182" t="s">
+      <c r="F16" s="183" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="183"/>
-      <c r="H16" s="183"/>
-      <c r="I16" s="184"/>
+      <c r="G16" s="184"/>
+      <c r="H16" s="184"/>
+      <c r="I16" s="185"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2228,18 +2229,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="179" t="s">
+      <c r="B17" s="164" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="185"/>
-      <c r="D17" s="185"/>
-      <c r="E17" s="186"/>
-      <c r="F17" s="187" t="s">
+      <c r="C17" s="186"/>
+      <c r="D17" s="186"/>
+      <c r="E17" s="187"/>
+      <c r="F17" s="188" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="185"/>
-      <c r="H17" s="185"/>
-      <c r="I17" s="185"/>
+      <c r="G17" s="186"/>
+      <c r="H17" s="186"/>
+      <c r="I17" s="186"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2257,18 +2258,18 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="188" t="s">
+      <c r="B18" s="189" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="189"/>
+      <c r="C18" s="190"/>
       <c r="D18" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="189" t="s">
+      <c r="E18" s="190" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="189"/>
-      <c r="G18" s="189"/>
+      <c r="F18" s="190"/>
+      <c r="G18" s="190"/>
       <c r="H18" s="23" t="s">
         <v>80</v>
       </c>
@@ -2292,18 +2293,18 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="190" t="s">
+      <c r="B19" s="174" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="191"/>
+      <c r="C19" s="175"/>
       <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="192" t="s">
+      <c r="E19" s="176" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="192"/>
-      <c r="G19" s="192"/>
+      <c r="F19" s="176"/>
+      <c r="G19" s="176"/>
       <c r="H19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2452,18 +2453,18 @@
       <c r="AD24" s="10"/>
     </row>
     <row r="25" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="193" t="s">
+      <c r="B25" s="177" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="194"/>
-      <c r="D25" s="194"/>
-      <c r="E25" s="195"/>
-      <c r="F25" s="193" t="s">
+      <c r="C25" s="178"/>
+      <c r="D25" s="178"/>
+      <c r="E25" s="179"/>
+      <c r="F25" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="194"/>
-      <c r="H25" s="194"/>
-      <c r="I25" s="194"/>
+      <c r="G25" s="178"/>
+      <c r="H25" s="178"/>
+      <c r="I25" s="178"/>
       <c r="J25" s="22"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
@@ -2484,48 +2485,48 @@
       <c r="AD25" s="10"/>
     </row>
     <row r="26" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="179" t="s">
+      <c r="B26" s="164" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="180"/>
-      <c r="D26" s="180"/>
-      <c r="E26" s="181"/>
-      <c r="F26" s="179" t="s">
+      <c r="C26" s="165"/>
+      <c r="D26" s="165"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="180"/>
-      <c r="H26" s="180"/>
-      <c r="I26" s="180"/>
+      <c r="G26" s="165"/>
+      <c r="H26" s="165"/>
+      <c r="I26" s="165"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="176" t="s">
+      <c r="B27" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="177"/>
-      <c r="D27" s="177"/>
-      <c r="E27" s="178"/>
-      <c r="F27" s="179" t="s">
+      <c r="C27" s="181"/>
+      <c r="D27" s="181"/>
+      <c r="E27" s="182"/>
+      <c r="F27" s="164" t="s">
         <v>85</v>
       </c>
-      <c r="G27" s="180"/>
-      <c r="H27" s="180"/>
-      <c r="I27" s="181"/>
+      <c r="G27" s="165"/>
+      <c r="H27" s="165"/>
+      <c r="I27" s="166"/>
       <c r="J27" s="19"/>
     </row>
     <row r="28" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="173" t="s">
+      <c r="B28" s="171" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="174"/>
-      <c r="D28" s="174"/>
+      <c r="C28" s="172"/>
+      <c r="D28" s="172"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="173" t="s">
+      <c r="F28" s="171" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="174"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="175"/>
+      <c r="G28" s="172"/>
+      <c r="H28" s="172"/>
+      <c r="I28" s="173"/>
       <c r="J28" s="22"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
@@ -2546,33 +2547,33 @@
       <c r="AD28" s="10"/>
     </row>
     <row r="29" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="179" t="s">
+      <c r="B29" s="164" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="180"/>
-      <c r="D29" s="180"/>
-      <c r="E29" s="181"/>
-      <c r="F29" s="179" t="s">
+      <c r="C29" s="165"/>
+      <c r="D29" s="165"/>
+      <c r="E29" s="166"/>
+      <c r="F29" s="164" t="s">
         <v>37</v>
       </c>
-      <c r="G29" s="180"/>
-      <c r="H29" s="180"/>
-      <c r="I29" s="180"/>
+      <c r="G29" s="165"/>
+      <c r="H29" s="165"/>
+      <c r="I29" s="165"/>
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="173" t="s">
+      <c r="B30" s="171" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="174"/>
-      <c r="D30" s="174"/>
+      <c r="C30" s="172"/>
+      <c r="D30" s="172"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="173" t="s">
+      <c r="F30" s="171" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="174"/>
-      <c r="H30" s="174"/>
-      <c r="I30" s="175"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="173"/>
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -2591,18 +2592,18 @@
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="196" t="s">
+      <c r="B32" s="167" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="197"/>
-      <c r="D32" s="197"/>
-      <c r="E32" s="198"/>
-      <c r="F32" s="196" t="s">
+      <c r="C32" s="168"/>
+      <c r="D32" s="168"/>
+      <c r="E32" s="169"/>
+      <c r="F32" s="167" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="197"/>
-      <c r="H32" s="197"/>
-      <c r="I32" s="197"/>
+      <c r="G32" s="168"/>
+      <c r="H32" s="168"/>
+      <c r="I32" s="168"/>
       <c r="J32" s="34"/>
       <c r="N32" s="36"/>
       <c r="O32" s="36"/>
@@ -2623,93 +2624,93 @@
       <c r="AD32" s="36"/>
     </row>
     <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="179" t="s">
+      <c r="B33" s="164" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="180"/>
-      <c r="D33" s="180"/>
-      <c r="E33" s="181"/>
-      <c r="F33" s="179" t="s">
+      <c r="C33" s="165"/>
+      <c r="D33" s="165"/>
+      <c r="E33" s="166"/>
+      <c r="F33" s="164" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="180"/>
-      <c r="H33" s="180"/>
-      <c r="I33" s="180"/>
+      <c r="G33" s="165"/>
+      <c r="H33" s="165"/>
+      <c r="I33" s="165"/>
       <c r="J33" s="19"/>
     </row>
     <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="179" t="s">
+      <c r="B34" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="180"/>
-      <c r="D34" s="180"/>
-      <c r="E34" s="181"/>
-      <c r="F34" s="179" t="s">
+      <c r="C34" s="165"/>
+      <c r="D34" s="165"/>
+      <c r="E34" s="166"/>
+      <c r="F34" s="164" t="s">
         <v>42</v>
       </c>
-      <c r="G34" s="180"/>
-      <c r="H34" s="180"/>
-      <c r="I34" s="180"/>
+      <c r="G34" s="165"/>
+      <c r="H34" s="165"/>
+      <c r="I34" s="165"/>
       <c r="J34" s="19"/>
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="179" t="s">
+      <c r="B35" s="164" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="180"/>
-      <c r="D35" s="180"/>
-      <c r="E35" s="181"/>
-      <c r="F35" s="179" t="s">
+      <c r="C35" s="165"/>
+      <c r="D35" s="165"/>
+      <c r="E35" s="166"/>
+      <c r="F35" s="164" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="180"/>
-      <c r="H35" s="180"/>
-      <c r="I35" s="180"/>
+      <c r="G35" s="165"/>
+      <c r="H35" s="165"/>
+      <c r="I35" s="165"/>
       <c r="J35" s="19"/>
     </row>
     <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="179" t="s">
+      <c r="B36" s="164" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="180"/>
-      <c r="D36" s="180"/>
-      <c r="E36" s="181"/>
-      <c r="F36" s="179" t="s">
+      <c r="C36" s="165"/>
+      <c r="D36" s="165"/>
+      <c r="E36" s="166"/>
+      <c r="F36" s="164" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="180"/>
-      <c r="H36" s="180"/>
-      <c r="I36" s="180"/>
+      <c r="G36" s="165"/>
+      <c r="H36" s="165"/>
+      <c r="I36" s="165"/>
       <c r="J36" s="19"/>
     </row>
     <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="179" t="s">
+      <c r="B37" s="164" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="180"/>
-      <c r="D37" s="180"/>
-      <c r="E37" s="181"/>
-      <c r="F37" s="179" t="s">
+      <c r="C37" s="165"/>
+      <c r="D37" s="165"/>
+      <c r="E37" s="166"/>
+      <c r="F37" s="164" t="s">
         <v>46</v>
       </c>
-      <c r="G37" s="180"/>
-      <c r="H37" s="180"/>
-      <c r="I37" s="180"/>
+      <c r="G37" s="165"/>
+      <c r="H37" s="165"/>
+      <c r="I37" s="165"/>
       <c r="J37" s="19"/>
     </row>
     <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="179" t="s">
+      <c r="B38" s="164" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="180"/>
-      <c r="D38" s="180"/>
-      <c r="E38" s="181"/>
-      <c r="F38" s="179" t="s">
+      <c r="C38" s="165"/>
+      <c r="D38" s="165"/>
+      <c r="E38" s="166"/>
+      <c r="F38" s="164" t="s">
         <v>48</v>
       </c>
-      <c r="G38" s="180"/>
-      <c r="H38" s="180"/>
-      <c r="I38" s="180"/>
+      <c r="G38" s="165"/>
+      <c r="H38" s="165"/>
+      <c r="I38" s="165"/>
       <c r="J38" s="19"/>
     </row>
     <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2728,18 +2729,18 @@
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="196" t="s">
+      <c r="B40" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="197"/>
-      <c r="D40" s="197"/>
-      <c r="E40" s="198"/>
-      <c r="F40" s="196" t="s">
+      <c r="C40" s="168"/>
+      <c r="D40" s="168"/>
+      <c r="E40" s="169"/>
+      <c r="F40" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="G40" s="199"/>
-      <c r="H40" s="199"/>
-      <c r="I40" s="199"/>
+      <c r="G40" s="170"/>
+      <c r="H40" s="170"/>
+      <c r="I40" s="170"/>
       <c r="J40" s="34"/>
       <c r="N40" s="36"/>
       <c r="O40" s="36"/>
@@ -2760,18 +2761,18 @@
       <c r="AD40" s="36"/>
     </row>
     <row r="41" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="179" t="s">
+      <c r="B41" s="164" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="180"/>
-      <c r="D41" s="180"/>
-      <c r="E41" s="181"/>
-      <c r="F41" s="179" t="s">
+      <c r="C41" s="165"/>
+      <c r="D41" s="165"/>
+      <c r="E41" s="166"/>
+      <c r="F41" s="164" t="s">
         <v>15</v>
       </c>
-      <c r="G41" s="180"/>
-      <c r="H41" s="180"/>
-      <c r="I41" s="180"/>
+      <c r="G41" s="165"/>
+      <c r="H41" s="165"/>
+      <c r="I41" s="165"/>
       <c r="J41" s="19"/>
     </row>
     <row r="42" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3061,24 +3062,36 @@
     <row r="88" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:G18"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="B19:C19"/>
@@ -3093,36 +3106,24 @@
     <mergeCell ref="F28:I28"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="notContainsBlanks" dxfId="3" priority="2">
@@ -3161,8 +3162,8 @@
   </sheetPr>
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="232" zoomScaleNormal="100" zoomScaleSheetLayoutView="232" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3185,11 +3186,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="56"/>
+      <c r="A1" s="202"/>
       <c r="G1" s="161" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="58"/>
+      <c r="N1" s="202"/>
     </row>
     <row r="2" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="89"/>

</xml_diff>

<commit_message>
pictures export contract tmp page implemented (only contract page)
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D434E91-F94D-4AA5-A995-A418E846ABE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8E9A10-9EB3-485A-9655-794264D30DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,17 @@
   <definedNames>
     <definedName name="MID_Contract">Export_Contract!$E$1</definedName>
     <definedName name="MID_Invoice">Invoice!$G$1</definedName>
-    <definedName name="Seal_agent_end">Export_Contract!$H$52</definedName>
+    <definedName name="Seal_agent_end">Export_Contract!$H$53</definedName>
     <definedName name="Seal_agent_start">Export_Contract!$G$42</definedName>
-    <definedName name="Seal_seller_end">Export_Contract!$C$52</definedName>
+    <definedName name="Seal_seller_end">Export_Contract!$C$53</definedName>
     <definedName name="Seal_seller_start">Export_Contract!$C$44</definedName>
-    <definedName name="Sign_agent_end">Export_Contract!$G$52</definedName>
-    <definedName name="Sign_agent_start">Export_Contract!$G$50</definedName>
-    <definedName name="Sign_seller_start">Export_Contract!$C$50</definedName>
+    <definedName name="Sign_agent_end">Export_Contract!$G$53</definedName>
+    <definedName name="Sign_agent_start">Export_Contract!$G$51</definedName>
+    <definedName name="Sign_seller_start">Export_Contract!$C$51</definedName>
     <definedName name="Адреса_банк_получателя">Export_Contract!$B$34</definedName>
     <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$35</definedName>
     <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$36</definedName>
-    <definedName name="Адреса_подпись">Export_Contract!$B$51</definedName>
+    <definedName name="Адреса_подпись">Export_Contract!$B$52</definedName>
     <definedName name="Адреса_покупатель">Export_Contract!$B$40</definedName>
     <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$41</definedName>
     <definedName name="Адреса_покупатель_банк">Export_Contract!$B$43</definedName>
@@ -280,12 +280,6 @@
     <t>A/C: 242-910002-68638</t>
   </si>
   <si>
-    <t xml:space="preserve">Продавец/Seller  _______________________N.M. Kotov </t>
-  </si>
-  <si>
-    <t>Покупатель/Buyer ________________________SE JI YOUNG</t>
-  </si>
-  <si>
     <t>2.2. Total amount of this Agreement is specified in US dollars and is the following:</t>
   </si>
   <si>
@@ -554,6 +548,12 @@
   </si>
   <si>
     <t>Agreement No. 146 dated March 10, 2023</t>
+  </si>
+  <si>
+    <t>Покупатель/Buyer _________________________________SE JI YOUNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Продавец/Seller  ___________________________________N.M. Kotov </t>
   </si>
 </sst>
 </file>
@@ -870,7 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -974,14 +974,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1308,6 +1302,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1421,7 +1418,31 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1785,24 +1806,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AF88"/>
+  <dimension ref="B1:AF89"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:E11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A18" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="1.06640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="23.59765625" style="49" customWidth="1"/>
-    <col min="4" max="4" width="18" style="49" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="49" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="49" customWidth="1"/>
-    <col min="7" max="7" width="21.53125" style="49" customWidth="1"/>
-    <col min="8" max="8" width="12.265625" style="49" customWidth="1"/>
-    <col min="9" max="9" width="15.06640625" style="49" customWidth="1"/>
-    <col min="10" max="10" width="1.06640625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" style="47" customWidth="1"/>
+    <col min="3" max="3" width="29" style="47" customWidth="1"/>
+    <col min="4" max="4" width="17.06640625" style="47" customWidth="1"/>
+    <col min="5" max="5" width="10.19921875" style="47" customWidth="1"/>
+    <col min="6" max="6" width="13.06640625" style="47" customWidth="1"/>
+    <col min="7" max="7" width="25.9296875" style="47" customWidth="1"/>
+    <col min="8" max="8" width="13.86328125" style="47" customWidth="1"/>
+    <col min="9" max="9" width="15.1328125" style="47" customWidth="1"/>
+    <col min="10" max="10" width="1.06640625" style="47" customWidth="1"/>
     <col min="11" max="11" width="8.796875" style="10"/>
     <col min="12" max="12" width="13" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.796875" style="10"/>
@@ -1828,31 +1849,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="2.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
-      <c r="H1" s="162"/>
-      <c r="I1" s="162"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
     </row>
     <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="194" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="194" t="s">
+      <c r="B2" s="193" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="194"/>
+      <c r="D2" s="194"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="193" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="163"/>
+      <c r="G2" s="194"/>
+      <c r="H2" s="194"/>
+      <c r="I2" s="194"/>
+      <c r="J2" s="161"/>
       <c r="L2" s="11"/>
       <c r="N2" s="18"/>
       <c r="AA2" s="18"/>
@@ -1861,18 +1882,18 @@
       <c r="AD2" s="18"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="196" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="199"/>
-      <c r="F3" s="197" t="s">
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="198"/>
+      <c r="F3" s="196" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="198"/>
-      <c r="H3" s="198"/>
-      <c r="I3" s="198"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="197"/>
+      <c r="I3" s="197"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1889,18 +1910,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="197" t="s">
+      <c r="B4" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="198"/>
-      <c r="D4" s="198"/>
-      <c r="E4" s="199"/>
-      <c r="F4" s="197" t="s">
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
+      <c r="F4" s="196" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="198"/>
-      <c r="H4" s="198"/>
-      <c r="I4" s="198"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="197"/>
+      <c r="I4" s="197"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1921,18 +1942,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="191" t="s">
+      <c r="B5" s="190" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="192"/>
-      <c r="D5" s="192"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="191" t="s">
+      <c r="C5" s="191"/>
+      <c r="D5" s="191"/>
+      <c r="E5" s="192"/>
+      <c r="F5" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="192"/>
-      <c r="H5" s="192"/>
-      <c r="I5" s="192"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="191"/>
+      <c r="I5" s="191"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1941,20 +1962,20 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="171" t="s">
+      <c r="B6" s="170" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="171"/>
+      <c r="D6" s="171"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="170" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="172"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="171" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="172"/>
-      <c r="H6" s="172"/>
-      <c r="I6" s="172"/>
-      <c r="J6" s="54"/>
-      <c r="L6" s="55"/>
+      <c r="G6" s="171"/>
+      <c r="H6" s="171"/>
+      <c r="I6" s="171"/>
+      <c r="J6" s="52"/>
+      <c r="L6" s="53"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
@@ -1970,19 +1991,19 @@
     </row>
     <row r="7" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="53"/>
+        <v>65</v>
+      </c>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="54"/>
-      <c r="L7" s="55"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="52"/>
+      <c r="L7" s="53"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
@@ -1997,48 +2018,48 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="181"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="182"/>
-      <c r="F8" s="164" t="s">
+      <c r="C8" s="180"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="163" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="165"/>
-      <c r="H8" s="165"/>
-      <c r="I8" s="165"/>
+      <c r="G8" s="164"/>
+      <c r="H8" s="164"/>
+      <c r="I8" s="164"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="164" t="s">
+      <c r="B9" s="163" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="165"/>
-      <c r="D9" s="165"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="164" t="s">
+      <c r="C9" s="164"/>
+      <c r="D9" s="164"/>
+      <c r="E9" s="165"/>
+      <c r="F9" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="165"/>
-      <c r="H9" s="165"/>
-      <c r="I9" s="165"/>
+      <c r="G9" s="164"/>
+      <c r="H9" s="164"/>
+      <c r="I9" s="164"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="164" t="s">
+      <c r="B10" s="163" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="166"/>
-      <c r="F10" s="164" t="s">
+      <c r="C10" s="164"/>
+      <c r="D10" s="164"/>
+      <c r="E10" s="165"/>
+      <c r="F10" s="163" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="165"/>
-      <c r="H10" s="165"/>
-      <c r="I10" s="165"/>
+      <c r="G10" s="164"/>
+      <c r="H10" s="164"/>
+      <c r="I10" s="164"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -2059,19 +2080,19 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="171" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="172"/>
-      <c r="D11" s="172"/>
-      <c r="E11" s="173"/>
-      <c r="F11" s="171" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="172"/>
-      <c r="H11" s="172"/>
-      <c r="I11" s="172"/>
-      <c r="J11" s="54"/>
+      <c r="B11" s="170" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="171"/>
+      <c r="D11" s="171"/>
+      <c r="E11" s="172"/>
+      <c r="F11" s="170" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="171"/>
+      <c r="H11" s="171"/>
+      <c r="I11" s="171"/>
+      <c r="J11" s="52"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
@@ -2091,14 +2112,14 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="51"/>
+      <c r="E12" s="49"/>
       <c r="F12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="8"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="54"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="52"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
@@ -2113,18 +2134,18 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="164" t="s">
+      <c r="B13" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="165"/>
-      <c r="E13" s="166"/>
-      <c r="F13" s="164" t="s">
+      <c r="C13" s="164"/>
+      <c r="D13" s="164"/>
+      <c r="E13" s="165"/>
+      <c r="F13" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="165"/>
-      <c r="H13" s="165"/>
-      <c r="I13" s="165"/>
+      <c r="G13" s="164"/>
+      <c r="H13" s="164"/>
+      <c r="I13" s="164"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2142,18 +2163,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="163" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="165"/>
-      <c r="E14" s="166"/>
-      <c r="F14" s="164" t="s">
+      <c r="C14" s="164"/>
+      <c r="D14" s="164"/>
+      <c r="E14" s="165"/>
+      <c r="F14" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="165"/>
-      <c r="H14" s="165"/>
-      <c r="I14" s="165"/>
+      <c r="G14" s="164"/>
+      <c r="H14" s="164"/>
+      <c r="I14" s="164"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2171,18 +2192,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="164" t="s">
+      <c r="B15" s="163" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="165"/>
-      <c r="E15" s="166"/>
-      <c r="F15" s="164" t="s">
+      <c r="C15" s="164"/>
+      <c r="D15" s="164"/>
+      <c r="E15" s="165"/>
+      <c r="F15" s="163" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="165"/>
-      <c r="H15" s="165"/>
-      <c r="I15" s="165"/>
+      <c r="G15" s="164"/>
+      <c r="H15" s="164"/>
+      <c r="I15" s="164"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2200,18 +2221,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="183" t="s">
+      <c r="B16" s="182" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="184"/>
-      <c r="D16" s="184"/>
+      <c r="C16" s="183"/>
+      <c r="D16" s="183"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="183" t="s">
+      <c r="F16" s="182" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="184"/>
-      <c r="H16" s="184"/>
-      <c r="I16" s="185"/>
+      <c r="G16" s="183"/>
+      <c r="H16" s="183"/>
+      <c r="I16" s="184"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2229,18 +2250,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="164" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="186"/>
-      <c r="D17" s="186"/>
-      <c r="E17" s="187"/>
-      <c r="F17" s="188" t="s">
-        <v>79</v>
-      </c>
-      <c r="G17" s="186"/>
-      <c r="H17" s="186"/>
-      <c r="I17" s="186"/>
+      <c r="B17" s="163" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="185"/>
+      <c r="D17" s="185"/>
+      <c r="E17" s="186"/>
+      <c r="F17" s="187" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="185"/>
+      <c r="H17" s="185"/>
+      <c r="I17" s="185"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2258,23 +2279,23 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="189" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="190"/>
+      <c r="B18" s="188" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="189"/>
       <c r="D18" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="190" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="190"/>
-      <c r="G18" s="190"/>
+        <v>74</v>
+      </c>
+      <c r="E18" s="189" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="189"/>
+      <c r="G18" s="189"/>
       <c r="H18" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J18" s="24"/>
       <c r="N18" s="10"/>
@@ -2293,18 +2314,18 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="174" t="s">
+      <c r="B19" s="173" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="175"/>
+      <c r="C19" s="174"/>
       <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="176" t="s">
+      <c r="E19" s="175" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="176"/>
-      <c r="G19" s="176"/>
+      <c r="F19" s="175"/>
+      <c r="G19" s="175"/>
       <c r="H19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2392,13 +2413,13 @@
     </row>
     <row r="22" spans="2:30" s="30" customFormat="1" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
       <c r="E22" s="29"/>
       <c r="F22" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
@@ -2453,18 +2474,18 @@
       <c r="AD24" s="10"/>
     </row>
     <row r="25" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="177" t="s">
+      <c r="B25" s="176" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="178"/>
-      <c r="D25" s="178"/>
-      <c r="E25" s="179"/>
-      <c r="F25" s="177" t="s">
+      <c r="C25" s="177"/>
+      <c r="D25" s="177"/>
+      <c r="E25" s="178"/>
+      <c r="F25" s="176" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="178"/>
-      <c r="H25" s="178"/>
-      <c r="I25" s="178"/>
+      <c r="G25" s="177"/>
+      <c r="H25" s="177"/>
+      <c r="I25" s="177"/>
       <c r="J25" s="22"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
@@ -2485,48 +2506,48 @@
       <c r="AD25" s="10"/>
     </row>
     <row r="26" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="164" t="s">
+      <c r="B26" s="163" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="164"/>
+      <c r="D26" s="164"/>
+      <c r="E26" s="165"/>
+      <c r="F26" s="163" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="165"/>
-      <c r="D26" s="165"/>
-      <c r="E26" s="166"/>
-      <c r="F26" s="164" t="s">
-        <v>84</v>
-      </c>
-      <c r="G26" s="165"/>
-      <c r="H26" s="165"/>
-      <c r="I26" s="165"/>
+      <c r="G26" s="164"/>
+      <c r="H26" s="164"/>
+      <c r="I26" s="164"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="180" t="s">
+      <c r="B27" s="179" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="180"/>
+      <c r="D27" s="180"/>
+      <c r="E27" s="181"/>
+      <c r="F27" s="163" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="181"/>
-      <c r="D27" s="181"/>
-      <c r="E27" s="182"/>
-      <c r="F27" s="164" t="s">
-        <v>85</v>
-      </c>
-      <c r="G27" s="165"/>
-      <c r="H27" s="165"/>
-      <c r="I27" s="166"/>
+      <c r="G27" s="164"/>
+      <c r="H27" s="164"/>
+      <c r="I27" s="165"/>
       <c r="J27" s="19"/>
     </row>
     <row r="28" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="171" t="s">
+      <c r="B28" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="172"/>
-      <c r="D28" s="172"/>
+      <c r="C28" s="171"/>
+      <c r="D28" s="171"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="171" t="s">
+      <c r="F28" s="170" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="172"/>
-      <c r="H28" s="172"/>
-      <c r="I28" s="173"/>
+      <c r="G28" s="171"/>
+      <c r="H28" s="171"/>
+      <c r="I28" s="172"/>
       <c r="J28" s="22"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
@@ -2547,44 +2568,44 @@
       <c r="AD28" s="10"/>
     </row>
     <row r="29" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="164" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="165"/>
-      <c r="D29" s="165"/>
-      <c r="E29" s="166"/>
-      <c r="F29" s="164" t="s">
+      <c r="B29" s="163" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="164"/>
+      <c r="D29" s="164"/>
+      <c r="E29" s="165"/>
+      <c r="F29" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="G29" s="165"/>
-      <c r="H29" s="165"/>
-      <c r="I29" s="165"/>
+      <c r="G29" s="164"/>
+      <c r="H29" s="164"/>
+      <c r="I29" s="164"/>
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="171" t="s">
+      <c r="B30" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="172"/>
-      <c r="D30" s="172"/>
+      <c r="C30" s="171"/>
+      <c r="D30" s="171"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="171" t="s">
+      <c r="F30" s="170" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="172"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="173"/>
+      <c r="G30" s="171"/>
+      <c r="H30" s="171"/>
+      <c r="I30" s="172"/>
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="50" t="s">
-        <v>66</v>
+      <c r="B31" s="48" t="s">
+        <v>64</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="21"/>
-      <c r="F31" s="50" t="s">
-        <v>72</v>
+      <c r="F31" s="48" t="s">
+        <v>70</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
@@ -2592,18 +2613,18 @@
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="167" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="168"/>
-      <c r="D32" s="168"/>
-      <c r="E32" s="169"/>
-      <c r="F32" s="167" t="s">
+      <c r="B32" s="166" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="167"/>
+      <c r="D32" s="167"/>
+      <c r="E32" s="168"/>
+      <c r="F32" s="166" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="168"/>
-      <c r="H32" s="168"/>
-      <c r="I32" s="168"/>
+      <c r="G32" s="167"/>
+      <c r="H32" s="167"/>
+      <c r="I32" s="167"/>
       <c r="J32" s="34"/>
       <c r="N32" s="36"/>
       <c r="O32" s="36"/>
@@ -2624,104 +2645,104 @@
       <c r="AD32" s="36"/>
     </row>
     <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="164" t="s">
+      <c r="B33" s="163" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="165"/>
-      <c r="D33" s="165"/>
-      <c r="E33" s="166"/>
-      <c r="F33" s="164" t="s">
+      <c r="C33" s="164"/>
+      <c r="D33" s="164"/>
+      <c r="E33" s="165"/>
+      <c r="F33" s="163" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="165"/>
-      <c r="H33" s="165"/>
-      <c r="I33" s="165"/>
+      <c r="G33" s="164"/>
+      <c r="H33" s="164"/>
+      <c r="I33" s="164"/>
       <c r="J33" s="19"/>
     </row>
     <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="164" t="s">
+      <c r="B34" s="163" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="165"/>
-      <c r="D34" s="165"/>
-      <c r="E34" s="166"/>
-      <c r="F34" s="164" t="s">
+      <c r="C34" s="164"/>
+      <c r="D34" s="164"/>
+      <c r="E34" s="165"/>
+      <c r="F34" s="163" t="s">
         <v>42</v>
       </c>
-      <c r="G34" s="165"/>
-      <c r="H34" s="165"/>
-      <c r="I34" s="165"/>
+      <c r="G34" s="164"/>
+      <c r="H34" s="164"/>
+      <c r="I34" s="164"/>
       <c r="J34" s="19"/>
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="164" t="s">
+      <c r="B35" s="163" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="165"/>
-      <c r="D35" s="165"/>
-      <c r="E35" s="166"/>
-      <c r="F35" s="164" t="s">
+      <c r="C35" s="164"/>
+      <c r="D35" s="164"/>
+      <c r="E35" s="165"/>
+      <c r="F35" s="163" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="165"/>
-      <c r="H35" s="165"/>
-      <c r="I35" s="165"/>
+      <c r="G35" s="164"/>
+      <c r="H35" s="164"/>
+      <c r="I35" s="164"/>
       <c r="J35" s="19"/>
     </row>
     <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="164" t="s">
+      <c r="B36" s="163" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="165"/>
-      <c r="D36" s="165"/>
-      <c r="E36" s="166"/>
-      <c r="F36" s="164" t="s">
+      <c r="C36" s="164"/>
+      <c r="D36" s="164"/>
+      <c r="E36" s="165"/>
+      <c r="F36" s="163" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="165"/>
-      <c r="H36" s="165"/>
-      <c r="I36" s="165"/>
+      <c r="G36" s="164"/>
+      <c r="H36" s="164"/>
+      <c r="I36" s="164"/>
       <c r="J36" s="19"/>
     </row>
     <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="164" t="s">
+      <c r="B37" s="163" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="165"/>
-      <c r="D37" s="165"/>
-      <c r="E37" s="166"/>
-      <c r="F37" s="164" t="s">
+      <c r="C37" s="164"/>
+      <c r="D37" s="164"/>
+      <c r="E37" s="165"/>
+      <c r="F37" s="163" t="s">
         <v>46</v>
       </c>
-      <c r="G37" s="165"/>
-      <c r="H37" s="165"/>
-      <c r="I37" s="165"/>
+      <c r="G37" s="164"/>
+      <c r="H37" s="164"/>
+      <c r="I37" s="164"/>
       <c r="J37" s="19"/>
     </row>
     <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="164" t="s">
+      <c r="B38" s="163" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="165"/>
-      <c r="D38" s="165"/>
-      <c r="E38" s="166"/>
-      <c r="F38" s="164" t="s">
+      <c r="C38" s="164"/>
+      <c r="D38" s="164"/>
+      <c r="E38" s="165"/>
+      <c r="F38" s="163" t="s">
         <v>48</v>
       </c>
-      <c r="G38" s="165"/>
-      <c r="H38" s="165"/>
-      <c r="I38" s="165"/>
+      <c r="G38" s="164"/>
+      <c r="H38" s="164"/>
+      <c r="I38" s="164"/>
       <c r="J38" s="19"/>
     </row>
     <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="62" t="s">
-        <v>73</v>
+      <c r="B39" s="60" t="s">
+        <v>71</v>
       </c>
       <c r="C39" s="20"/>
       <c r="D39" s="20"/>
       <c r="E39" s="21"/>
-      <c r="F39" s="62" t="s">
-        <v>74</v>
+      <c r="F39" s="60" t="s">
+        <v>72</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
@@ -2729,18 +2750,18 @@
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="167" t="s">
+      <c r="B40" s="166" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="168"/>
-      <c r="D40" s="168"/>
-      <c r="E40" s="169"/>
-      <c r="F40" s="167" t="s">
+      <c r="C40" s="167"/>
+      <c r="D40" s="167"/>
+      <c r="E40" s="168"/>
+      <c r="F40" s="166" t="s">
         <v>14</v>
       </c>
-      <c r="G40" s="170"/>
-      <c r="H40" s="170"/>
-      <c r="I40" s="170"/>
+      <c r="G40" s="169"/>
+      <c r="H40" s="169"/>
+      <c r="I40" s="169"/>
       <c r="J40" s="34"/>
       <c r="N40" s="36"/>
       <c r="O40" s="36"/>
@@ -2760,24 +2781,23 @@
       <c r="AC40" s="36"/>
       <c r="AD40" s="36"/>
     </row>
-    <row r="41" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="164" t="s">
+    <row r="41" spans="2:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="165"/>
-      <c r="D41" s="165"/>
-      <c r="E41" s="166"/>
-      <c r="F41" s="164" t="s">
+      <c r="C41" s="164"/>
+      <c r="D41" s="164"/>
+      <c r="E41" s="165"/>
+      <c r="F41" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="G41" s="165"/>
-      <c r="H41" s="165"/>
-      <c r="I41" s="165"/>
+      <c r="G41" s="164"/>
+      <c r="H41" s="164"/>
+      <c r="I41" s="164"/>
       <c r="J41" s="19"/>
     </row>
-    <row r="42" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:30" ht="1.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B42" s="19"/>
-      <c r="C42" s="31"/>
       <c r="D42" s="31"/>
       <c r="E42" s="21"/>
       <c r="F42" s="19"/>
@@ -2788,171 +2808,205 @@
       <c r="I42" s="20"/>
       <c r="J42" s="19"/>
     </row>
-    <row r="43" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="27" t="s">
+    <row r="43" spans="2:30" s="205" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B43" s="201" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="27" t="s">
+      <c r="C43" s="202"/>
+      <c r="D43" s="202"/>
+      <c r="E43" s="203"/>
+      <c r="F43" s="201" t="s">
         <v>50</v>
       </c>
-      <c r="G43" s="28"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="19"/>
-    </row>
-    <row r="44" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="39"/>
+      <c r="G43" s="202"/>
+      <c r="H43" s="204"/>
+      <c r="I43" s="204"/>
+      <c r="J43" s="162"/>
+      <c r="N43" s="206"/>
+      <c r="O43" s="206"/>
+      <c r="P43" s="206"/>
+      <c r="Q43" s="206"/>
+      <c r="R43" s="206"/>
+      <c r="S43" s="206"/>
+      <c r="T43" s="206"/>
+      <c r="U43" s="206"/>
+      <c r="V43" s="206"/>
+      <c r="W43" s="206"/>
+      <c r="X43" s="206"/>
+      <c r="Y43" s="206"/>
+      <c r="Z43" s="206"/>
+      <c r="AA43" s="206"/>
+      <c r="AB43" s="206"/>
+      <c r="AC43" s="206"/>
+      <c r="AD43" s="206"/>
+    </row>
+    <row r="44" spans="2:30" s="205" customFormat="1" ht="1.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B44" s="201"/>
       <c r="C44" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="31"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="38"/>
-      <c r="J44" s="19"/>
-    </row>
-    <row r="45" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="27" t="s">
+      <c r="D44" s="202"/>
+      <c r="E44" s="203"/>
+      <c r="F44" s="201"/>
+      <c r="G44" s="202"/>
+      <c r="H44" s="204"/>
+      <c r="I44" s="204"/>
+      <c r="J44" s="162"/>
+      <c r="N44" s="206"/>
+      <c r="O44" s="206"/>
+      <c r="P44" s="206"/>
+      <c r="Q44" s="206"/>
+      <c r="R44" s="206"/>
+      <c r="S44" s="206"/>
+      <c r="T44" s="206"/>
+      <c r="U44" s="206"/>
+      <c r="V44" s="206"/>
+      <c r="W44" s="206"/>
+      <c r="X44" s="206"/>
+      <c r="Y44" s="206"/>
+      <c r="Z44" s="206"/>
+      <c r="AA44" s="206"/>
+      <c r="AB44" s="206"/>
+      <c r="AC44" s="206"/>
+      <c r="AD44" s="206"/>
+    </row>
+    <row r="45" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="207" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="27" t="s">
+      <c r="C45" s="208"/>
+      <c r="D45" s="208"/>
+      <c r="E45" s="209"/>
+      <c r="F45" s="207" t="s">
         <v>51</v>
       </c>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
+      <c r="G45" s="210"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
       <c r="J45" s="19"/>
     </row>
-    <row r="46" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="27" t="s">
+    <row r="46" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="207" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="27" t="s">
+      <c r="C46" s="208"/>
+      <c r="D46" s="208"/>
+      <c r="E46" s="211"/>
+      <c r="F46" s="207" t="s">
         <v>52</v>
       </c>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
+      <c r="G46" s="210"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
       <c r="J46" s="19"/>
     </row>
-    <row r="47" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="27" t="s">
+    <row r="47" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B47" s="207" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="28" t="s">
+      <c r="C47" s="208"/>
+      <c r="D47" s="208"/>
+      <c r="E47" s="211"/>
+      <c r="F47" s="208" t="s">
         <v>53</v>
       </c>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="38"/>
+      <c r="G47" s="210"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="37"/>
       <c r="J47" s="19"/>
     </row>
-    <row r="48" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="27" t="s">
+    <row r="48" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B48" s="207" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="28" t="s">
+      <c r="C48" s="208"/>
+      <c r="D48" s="208"/>
+      <c r="E48" s="211"/>
+      <c r="F48" s="208" t="s">
         <v>54</v>
       </c>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
+      <c r="G48" s="210"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
       <c r="J48" s="19"/>
     </row>
-    <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="27" t="s">
+    <row r="49" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="207" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="28" t="s">
+      <c r="C49" s="208"/>
+      <c r="D49" s="208"/>
+      <c r="E49" s="211"/>
+      <c r="F49" s="208" t="s">
         <v>55</v>
       </c>
-      <c r="G49" s="28"/>
+      <c r="G49" s="208"/>
       <c r="H49" s="28"/>
       <c r="I49" s="28"/>
       <c r="J49" s="19"/>
     </row>
-    <row r="50" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="19"/>
-      <c r="C50" s="36" t="s">
+    <row r="50" spans="2:10" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="207"/>
+      <c r="C50" s="208"/>
+      <c r="D50" s="208"/>
+      <c r="E50" s="211"/>
+      <c r="F50" s="208"/>
+      <c r="G50" s="208"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="19"/>
+    </row>
+    <row r="51" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="19"/>
+      <c r="C51" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="D50" s="31"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="12" t="s">
+      <c r="D51" s="31"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="19"/>
-    </row>
-    <row r="51" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="G51" s="41"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="42"/>
-      <c r="J51" s="15"/>
-    </row>
-    <row r="52" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="43"/>
-      <c r="C52" s="44" t="s">
+      <c r="H51" s="31"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="19"/>
+    </row>
+    <row r="52" spans="2:10" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="G52" s="39"/>
+      <c r="H52" s="39"/>
+      <c r="I52" s="40"/>
+      <c r="J52" s="15"/>
+    </row>
+    <row r="53" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="41"/>
+      <c r="C53" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="D52" s="45"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="44" t="s">
+      <c r="D53" s="43"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="45"/>
+      <c r="G53" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="H52" s="44" t="s">
+      <c r="H53" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="I52" s="46"/>
-      <c r="J52" s="15"/>
-    </row>
-    <row r="53" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="15"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
+      <c r="I53" s="44"/>
       <c r="J53" s="15"/>
     </row>
-    <row r="54" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B54" s="15"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="48"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
       <c r="E54" s="15"/>
       <c r="F54" s="15"/>
       <c r="G54" s="15"/>
@@ -2962,8 +3016,8 @@
     </row>
     <row r="55" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B55" s="15"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="46"/>
       <c r="E55" s="15"/>
       <c r="F55" s="15"/>
       <c r="G55" s="15"/>
@@ -2973,8 +3027,8 @@
     </row>
     <row r="56" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B56" s="15"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="46"/>
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
@@ -2984,8 +3038,8 @@
     </row>
     <row r="57" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B57" s="15"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
       <c r="G57" s="15"/>
@@ -2995,8 +3049,8 @@
     </row>
     <row r="58" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B58" s="15"/>
-      <c r="C58" s="48"/>
-      <c r="D58" s="48"/>
+      <c r="C58" s="46"/>
+      <c r="D58" s="46"/>
       <c r="E58" s="15"/>
       <c r="F58" s="15"/>
       <c r="G58" s="15"/>
@@ -3006,8 +3060,8 @@
     </row>
     <row r="59" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B59" s="15"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="46"/>
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
       <c r="G59" s="15"/>
@@ -3017,8 +3071,8 @@
     </row>
     <row r="60" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B60" s="15"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="48"/>
+      <c r="C60" s="46"/>
+      <c r="D60" s="46"/>
       <c r="E60" s="15"/>
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
@@ -3028,8 +3082,8 @@
     </row>
     <row r="61" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B61" s="15"/>
-      <c r="C61" s="48"/>
-      <c r="D61" s="48"/>
+      <c r="C61" s="46"/>
+      <c r="D61" s="46"/>
       <c r="E61" s="15"/>
       <c r="F61" s="15"/>
       <c r="G61" s="15"/>
@@ -3039,8 +3093,8 @@
     </row>
     <row r="62" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B62" s="15"/>
-      <c r="C62" s="48"/>
-      <c r="D62" s="48"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="46"/>
       <c r="E62" s="15"/>
       <c r="F62" s="15"/>
       <c r="G62" s="15"/>
@@ -3048,18 +3102,29 @@
       <c r="I62" s="15"/>
       <c r="J62" s="15"/>
     </row>
-    <row r="63" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="63" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B63" s="15"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="46"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+    </row>
     <row r="64" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="65" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="66" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="67" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="68" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="76" spans="6:7" x14ac:dyDescent="0.45">
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
-    </row>
-    <row r="81" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="88" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="69" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="77" spans="6:7" x14ac:dyDescent="0.45">
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+    </row>
+    <row r="82" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="89" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="62">
     <mergeCell ref="B2:E2"/>
@@ -3150,7 +3215,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.35433070866141736" bottom="0.15748031496062992" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="76" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3162,7 +3227,7 @@
   </sheetPr>
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="232" zoomScaleNormal="100" zoomScaleSheetLayoutView="232" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="94" zoomScaleNormal="100" zoomScaleSheetLayoutView="94" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -3186,447 +3251,445 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="202"/>
-      <c r="G1" s="161" t="s">
+      <c r="G1" s="159" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="202"/>
     </row>
     <row r="2" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="89"/>
-      <c r="B2" s="119" t="s">
+      <c r="A2" s="87"/>
+      <c r="B2" s="117" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="120" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="56"/>
+    </row>
+    <row r="3" spans="1:14" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="87"/>
+      <c r="B3" s="118" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="121" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="56"/>
+    </row>
+    <row r="4" spans="1:14" s="84" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="86"/>
+      <c r="B4" s="118" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="121" t="s">
+        <v>132</v>
+      </c>
+      <c r="I4" s="118"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="118"/>
+      <c r="M4" s="118"/>
+      <c r="N4" s="82"/>
+    </row>
+    <row r="5" spans="1:14" s="84" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="85"/>
+      <c r="B5" s="118" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="121" t="s">
+        <v>130</v>
+      </c>
+      <c r="I5" s="118"/>
+      <c r="J5" s="118"/>
+      <c r="K5" s="118"/>
+      <c r="L5" s="118"/>
+      <c r="M5" s="118"/>
+      <c r="N5" s="82"/>
+    </row>
+    <row r="6" spans="1:14" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="54"/>
+      <c r="B6" s="108" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="94" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="56"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="54"/>
+      <c r="B7" s="111" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="97" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="56"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="54"/>
+      <c r="B8" s="123" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="56"/>
+    </row>
+    <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="54"/>
+      <c r="B9" s="124" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="124"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="124"/>
+      <c r="F9" s="124"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="101" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="96"/>
+      <c r="M9" s="96"/>
+      <c r="N9" s="56"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="54"/>
+      <c r="B10" s="111" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="111"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="97" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="96"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="96"/>
+      <c r="M10" s="96"/>
+      <c r="N10" s="56"/>
+    </row>
+    <row r="11" spans="1:14" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="54"/>
+      <c r="B11" s="100" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="100"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="100"/>
+      <c r="G11" s="116"/>
+      <c r="H11" s="153" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="100"/>
+      <c r="J11" s="100"/>
+      <c r="K11" s="100"/>
+      <c r="L11" s="100"/>
+      <c r="M11" s="100"/>
+      <c r="N11" s="56"/>
+    </row>
+    <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="54"/>
+      <c r="B12" s="124" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="124"/>
+      <c r="D12" s="124"/>
+      <c r="E12" s="124"/>
+      <c r="F12" s="124"/>
+      <c r="G12" s="124"/>
+      <c r="H12" s="94" t="s">
+        <v>127</v>
+      </c>
+      <c r="I12" s="95"/>
+      <c r="J12" s="95"/>
+      <c r="K12" s="95"/>
+      <c r="L12" s="96"/>
+      <c r="M12" s="96"/>
+      <c r="N12" s="56"/>
+    </row>
+    <row r="13" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="54"/>
+      <c r="B13" s="111" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="97" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="96"/>
+      <c r="M13" s="96"/>
+      <c r="N13" s="56"/>
+    </row>
+    <row r="14" spans="1:14" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="54"/>
+      <c r="B14" s="100" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="100"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="116"/>
+      <c r="H14" s="153" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="100"/>
+      <c r="J14" s="100"/>
+      <c r="K14" s="100"/>
+      <c r="L14" s="100"/>
+      <c r="M14" s="100"/>
+      <c r="N14" s="56"/>
+    </row>
+    <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="83"/>
+      <c r="B15" s="102" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="102"/>
+      <c r="D15" s="103" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="103"/>
+      <c r="F15" s="103" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" s="103"/>
+      <c r="H15" s="104" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" s="103"/>
+      <c r="J15" s="125" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" s="125"/>
+      <c r="L15" s="149" t="s">
+        <v>112</v>
+      </c>
+      <c r="M15" s="149"/>
+      <c r="N15" s="56"/>
+    </row>
+    <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="54"/>
+      <c r="B16" s="116" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="105"/>
+      <c r="D16" s="154" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="106"/>
+      <c r="F16" s="142" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" s="106"/>
+      <c r="H16" s="157" t="s">
+        <v>108</v>
+      </c>
+      <c r="I16" s="106"/>
+      <c r="J16" s="107" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" s="107"/>
+      <c r="L16" s="150" t="s">
+        <v>107</v>
+      </c>
+      <c r="M16" s="150"/>
+      <c r="N16" s="56"/>
+    </row>
+    <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="54"/>
+      <c r="B17" s="124" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="124"/>
+      <c r="D17" s="124" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="128"/>
+      <c r="F17" s="141" t="s">
+        <v>124</v>
+      </c>
+      <c r="G17" s="141"/>
+      <c r="H17" s="101" t="s">
+        <v>123</v>
+      </c>
+      <c r="I17" s="96"/>
+      <c r="J17" s="109" t="s">
+        <v>122</v>
+      </c>
+      <c r="K17" s="96"/>
+      <c r="L17" s="151" t="s">
+        <v>121</v>
+      </c>
+      <c r="M17" s="152"/>
+      <c r="N17" s="56"/>
+    </row>
+    <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="54"/>
+      <c r="B18" s="100" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="123"/>
+      <c r="D18" s="155" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" s="107"/>
+      <c r="F18" s="156" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="142"/>
+      <c r="H18" s="157" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="107"/>
+      <c r="J18" s="155" t="s">
+        <v>117</v>
+      </c>
+      <c r="K18" s="107"/>
+      <c r="L18" s="150" t="s">
+        <v>116</v>
+      </c>
+      <c r="M18" s="150"/>
+      <c r="N18" s="56"/>
+    </row>
+    <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="54"/>
+      <c r="B19" s="129" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="129"/>
+      <c r="D19" s="129" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="129"/>
+      <c r="F19" s="143"/>
+      <c r="G19" s="143"/>
+      <c r="H19" s="146" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="122" t="s">
-        <v>138</v>
-      </c>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="58"/>
-    </row>
-    <row r="3" spans="1:14" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="89"/>
-      <c r="B3" s="120" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="123" t="s">
-        <v>136</v>
-      </c>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-      <c r="N3" s="58"/>
-    </row>
-    <row r="4" spans="1:14" s="86" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="88"/>
-      <c r="B4" s="120" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="120"/>
-      <c r="H4" s="123" t="s">
-        <v>134</v>
-      </c>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="120"/>
-      <c r="N4" s="84"/>
-    </row>
-    <row r="5" spans="1:14" s="86" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="87"/>
-      <c r="B5" s="120" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="123" t="s">
-        <v>132</v>
-      </c>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="120"/>
-      <c r="N5" s="84"/>
-    </row>
-    <row r="6" spans="1:14" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="56"/>
-      <c r="B6" s="110" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="96" t="s">
-        <v>72</v>
-      </c>
-      <c r="I6" s="97"/>
-      <c r="J6" s="97"/>
-      <c r="K6" s="97"/>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
-      <c r="N6" s="58"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="56"/>
-      <c r="B7" s="113" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="124"/>
-      <c r="D7" s="124"/>
-      <c r="E7" s="124"/>
-      <c r="F7" s="124"/>
-      <c r="G7" s="124"/>
-      <c r="H7" s="99" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="58"/>
-    </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="56"/>
-      <c r="B8" s="125" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="125"/>
-      <c r="H8" s="101" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
-      <c r="N8" s="58"/>
-    </row>
-    <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="56"/>
-      <c r="B9" s="126" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="126"/>
-      <c r="D9" s="126"/>
-      <c r="E9" s="126"/>
-      <c r="F9" s="126"/>
-      <c r="G9" s="126"/>
-      <c r="H9" s="103" t="s">
-        <v>140</v>
-      </c>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="98"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="98"/>
-      <c r="N9" s="58"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="56"/>
-      <c r="B10" s="113" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="113"/>
-      <c r="G10" s="113"/>
-      <c r="H10" s="99" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="98"/>
-      <c r="J10" s="98"/>
-      <c r="K10" s="98"/>
-      <c r="L10" s="98"/>
-      <c r="M10" s="98"/>
-      <c r="N10" s="58"/>
-    </row>
-    <row r="11" spans="1:14" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="56"/>
-      <c r="B11" s="102" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="155" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="102"/>
-      <c r="J11" s="102"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="102"/>
-      <c r="M11" s="102"/>
-      <c r="N11" s="58"/>
-    </row>
-    <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="56"/>
-      <c r="B12" s="126" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="126"/>
-      <c r="D12" s="126"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="126"/>
-      <c r="H12" s="96" t="s">
-        <v>129</v>
-      </c>
-      <c r="I12" s="97"/>
-      <c r="J12" s="97"/>
-      <c r="K12" s="97"/>
-      <c r="L12" s="98"/>
-      <c r="M12" s="98"/>
-      <c r="N12" s="58"/>
-    </row>
-    <row r="13" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="56"/>
-      <c r="B13" s="113" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="113"/>
-      <c r="H13" s="99" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100"/>
-      <c r="K13" s="100"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="98"/>
-      <c r="N13" s="58"/>
-    </row>
-    <row r="14" spans="1:14" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="56"/>
-      <c r="B14" s="102" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="102"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="118"/>
-      <c r="H14" s="155" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="102"/>
-      <c r="J14" s="102"/>
-      <c r="K14" s="102"/>
-      <c r="L14" s="102"/>
-      <c r="M14" s="102"/>
-      <c r="N14" s="58"/>
-    </row>
-    <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="85"/>
-      <c r="B15" s="104" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="105" t="s">
-        <v>113</v>
-      </c>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105" t="s">
-        <v>116</v>
-      </c>
-      <c r="G15" s="105"/>
-      <c r="H15" s="106" t="s">
-        <v>115</v>
-      </c>
-      <c r="I15" s="105"/>
-      <c r="J15" s="127" t="s">
-        <v>113</v>
-      </c>
-      <c r="K15" s="127"/>
-      <c r="L15" s="151" t="s">
-        <v>114</v>
-      </c>
-      <c r="M15" s="151"/>
-      <c r="N15" s="58"/>
-    </row>
-    <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="56"/>
-      <c r="B16" s="118" t="s">
+      <c r="I19" s="126"/>
+      <c r="J19" s="124" t="s">
+        <v>103</v>
+      </c>
+      <c r="K19" s="124"/>
+      <c r="L19" s="124"/>
+      <c r="M19" s="124"/>
+      <c r="N19" s="56"/>
+    </row>
+    <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="54"/>
+      <c r="B20" s="154" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="110"/>
+      <c r="D20" s="127" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="127"/>
+      <c r="F20" s="144"/>
+      <c r="G20" s="144"/>
+      <c r="H20" s="158" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="107"/>
-      <c r="D16" s="156" t="s">
-        <v>111</v>
-      </c>
-      <c r="E16" s="108"/>
-      <c r="F16" s="144" t="s">
-        <v>112</v>
-      </c>
-      <c r="G16" s="108"/>
-      <c r="H16" s="159" t="s">
-        <v>110</v>
-      </c>
-      <c r="I16" s="108"/>
-      <c r="J16" s="109" t="s">
-        <v>108</v>
-      </c>
-      <c r="K16" s="109"/>
-      <c r="L16" s="152" t="s">
-        <v>109</v>
-      </c>
-      <c r="M16" s="152"/>
-      <c r="N16" s="58"/>
-    </row>
-    <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="56"/>
-      <c r="B17" s="126" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" s="126"/>
-      <c r="D17" s="126" t="s">
-        <v>127</v>
-      </c>
-      <c r="E17" s="130"/>
-      <c r="F17" s="143" t="s">
-        <v>126</v>
-      </c>
-      <c r="G17" s="143"/>
-      <c r="H17" s="103" t="s">
-        <v>125</v>
-      </c>
-      <c r="I17" s="98"/>
-      <c r="J17" s="111" t="s">
-        <v>124</v>
-      </c>
-      <c r="K17" s="98"/>
-      <c r="L17" s="153" t="s">
-        <v>123</v>
-      </c>
-      <c r="M17" s="154"/>
-      <c r="N17" s="58"/>
-    </row>
-    <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="56"/>
-      <c r="B18" s="102" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="125"/>
-      <c r="D18" s="157" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" s="109"/>
-      <c r="F18" s="158" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="144"/>
-      <c r="H18" s="159" t="s">
-        <v>120</v>
-      </c>
-      <c r="I18" s="109"/>
-      <c r="J18" s="157" t="s">
-        <v>119</v>
-      </c>
-      <c r="K18" s="109"/>
-      <c r="L18" s="152" t="s">
-        <v>118</v>
-      </c>
-      <c r="M18" s="152"/>
-      <c r="N18" s="58"/>
-    </row>
-    <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="56"/>
-      <c r="B19" s="131" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" s="131"/>
-      <c r="D19" s="131" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="131"/>
-      <c r="F19" s="145"/>
-      <c r="G19" s="145"/>
-      <c r="H19" s="148" t="s">
-        <v>141</v>
-      </c>
-      <c r="I19" s="128"/>
-      <c r="J19" s="126" t="s">
-        <v>105</v>
-      </c>
-      <c r="K19" s="126"/>
-      <c r="L19" s="126"/>
-      <c r="M19" s="126"/>
-      <c r="N19" s="58"/>
-    </row>
-    <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="56"/>
-      <c r="B20" s="156" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="112"/>
-      <c r="D20" s="129" t="s">
-        <v>104</v>
-      </c>
-      <c r="E20" s="129"/>
-      <c r="F20" s="146"/>
-      <c r="G20" s="146"/>
-      <c r="H20" s="160" t="s">
-        <v>64</v>
-      </c>
-      <c r="I20" s="108"/>
-      <c r="J20" s="113" t="s">
-        <v>104</v>
-      </c>
-      <c r="K20" s="114"/>
-      <c r="L20" s="109"/>
-      <c r="M20" s="109"/>
-      <c r="N20" s="58"/>
-    </row>
-    <row r="21" spans="1:29" s="82" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="95"/>
-      <c r="B21" s="115"/>
-      <c r="C21" s="115"/>
-      <c r="D21" s="115"/>
-      <c r="E21" s="115"/>
-      <c r="F21" s="115"/>
-      <c r="G21" s="147"/>
-      <c r="H21" s="149"/>
-      <c r="I21" s="116"/>
-      <c r="J21" s="116"/>
-      <c r="K21" s="116"/>
-      <c r="L21" s="116"/>
-      <c r="M21" s="117"/>
-      <c r="N21" s="83"/>
+      <c r="I20" s="106"/>
+      <c r="J20" s="111" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" s="112"/>
+      <c r="L20" s="107"/>
+      <c r="M20" s="107"/>
+      <c r="N20" s="56"/>
+    </row>
+    <row r="21" spans="1:29" s="80" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="93"/>
+      <c r="B21" s="113"/>
+      <c r="C21" s="113"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="113"/>
+      <c r="G21" s="145"/>
+      <c r="H21" s="147"/>
+      <c r="I21" s="114"/>
+      <c r="J21" s="114"/>
+      <c r="K21" s="114"/>
+      <c r="L21" s="114"/>
+      <c r="M21" s="115"/>
+      <c r="N21" s="81"/>
       <c r="S21"/>
       <c r="T21"/>
       <c r="U21"/>
@@ -3640,386 +3703,386 @@
       <c r="AC21"/>
     </row>
     <row r="22" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="56"/>
-      <c r="B22" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="132" t="s">
-        <v>102</v>
-      </c>
-      <c r="D22" s="132"/>
-      <c r="E22" s="132"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="132"/>
-      <c r="H22" s="60" t="s">
+      <c r="A22" s="54"/>
+      <c r="B22" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="I22" s="81" t="s">
+      <c r="C22" s="130" t="s">
         <v>100</v>
       </c>
-      <c r="J22" s="80" t="s">
+      <c r="D22" s="130"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="148"/>
+      <c r="G22" s="130"/>
+      <c r="H22" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="K22" s="132" t="s">
+      <c r="I22" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="L22" s="132"/>
-      <c r="M22" s="60" t="s">
+      <c r="J22" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="N22" s="58"/>
+      <c r="K22" s="130" t="s">
+        <v>96</v>
+      </c>
+      <c r="L22" s="130"/>
+      <c r="M22" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="N22" s="56"/>
     </row>
     <row r="23" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="56"/>
-      <c r="B23" s="139" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="200" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="200"/>
-      <c r="E23" s="200"/>
-      <c r="F23" s="200"/>
-      <c r="G23" s="140"/>
-      <c r="H23" s="141" t="s">
+      <c r="A23" s="54"/>
+      <c r="B23" s="137" t="s">
         <v>94</v>
       </c>
-      <c r="I23" s="79" t="s">
+      <c r="C23" s="199" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="199"/>
+      <c r="E23" s="199"/>
+      <c r="F23" s="199"/>
+      <c r="G23" s="138"/>
+      <c r="H23" s="139" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" s="77" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" s="76">
+        <v>14</v>
+      </c>
+      <c r="K23" s="200" t="s">
         <v>91</v>
       </c>
-      <c r="J23" s="78">
+      <c r="L23" s="200"/>
+      <c r="M23" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="N23" s="56"/>
+    </row>
+    <row r="24" spans="1:29" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="54"/>
+      <c r="C24" s="135"/>
+      <c r="D24" s="135"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="135"/>
+      <c r="G24" s="135"/>
+      <c r="H24" s="136" t="s">
+        <v>90</v>
+      </c>
+      <c r="I24" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" s="73">
         <v>14</v>
       </c>
-      <c r="K23" s="201" t="s">
-        <v>93</v>
-      </c>
-      <c r="L23" s="201"/>
-      <c r="M23" s="77" t="s">
-        <v>90</v>
-      </c>
-      <c r="N23" s="58"/>
-    </row>
-    <row r="24" spans="1:29" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="56"/>
-      <c r="C24" s="137"/>
-      <c r="D24" s="137"/>
-      <c r="E24" s="137"/>
-      <c r="F24" s="137"/>
-      <c r="G24" s="137"/>
-      <c r="H24" s="138" t="s">
-        <v>92</v>
-      </c>
-      <c r="I24" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="J24" s="75">
-        <v>14</v>
-      </c>
-      <c r="K24" s="142" t="s">
+      <c r="K24" s="140" t="s">
         <v>49</v>
       </c>
-      <c r="L24" s="142"/>
-      <c r="M24" s="90" t="s">
-        <v>90</v>
-      </c>
-      <c r="N24" s="58"/>
+      <c r="L24" s="140"/>
+      <c r="M24" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="N24" s="56"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A25" s="56"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="63"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="74"/>
-      <c r="N25" s="58"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="72"/>
+      <c r="N25" s="56"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A26" s="56"/>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="63"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="69"/>
-      <c r="M26" s="74"/>
-      <c r="N26" s="58"/>
+      <c r="A26" s="54"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="56"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A27" s="56"/>
-      <c r="B27" s="69"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="69"/>
-      <c r="L27" s="69"/>
-      <c r="M27" s="74"/>
-      <c r="N27" s="58"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="56"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A28" s="56"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="63"/>
-      <c r="I28" s="74"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="74"/>
-      <c r="N28" s="58"/>
+      <c r="A28" s="54"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="56"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A29" s="56"/>
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="63"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="69"/>
-      <c r="M29" s="74"/>
-      <c r="N29" s="58"/>
+      <c r="A29" s="54"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="56"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A30" s="56"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="63"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="69"/>
-      <c r="M30" s="74"/>
-      <c r="N30" s="58"/>
+      <c r="A30" s="54"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="72"/>
+      <c r="N30" s="56"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A31" s="56"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="63"/>
-      <c r="I31" s="74"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="74"/>
-      <c r="N31" s="58"/>
+      <c r="A31" s="54"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="72"/>
+      <c r="N31" s="56"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A32" s="56"/>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="74"/>
-      <c r="N32" s="58"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="67"/>
+      <c r="M32" s="72"/>
+      <c r="N32" s="56"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A33" s="56"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="58"/>
+      <c r="A33" s="54"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="67"/>
+      <c r="M33" s="72"/>
+      <c r="N33" s="56"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A34" s="56"/>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="63"/>
-      <c r="I34" s="74"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
-      <c r="L34" s="69"/>
-      <c r="M34" s="74"/>
-      <c r="N34" s="58"/>
+      <c r="A34" s="54"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="72"/>
+      <c r="N34" s="56"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A35" s="56"/>
-      <c r="B35" s="69"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="59"/>
-      <c r="H35" s="63"/>
-      <c r="I35" s="74"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="69"/>
-      <c r="L35" s="69"/>
-      <c r="M35" s="74"/>
-      <c r="N35" s="58"/>
+      <c r="A35" s="54"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="67"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="67"/>
+      <c r="M35" s="72"/>
+      <c r="N35" s="56"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A36" s="56"/>
-      <c r="B36" s="69"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="63"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="69"/>
-      <c r="K36" s="69"/>
-      <c r="L36" s="69"/>
-      <c r="M36" s="74"/>
-      <c r="N36" s="58"/>
+      <c r="A36" s="54"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="67"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="67"/>
+      <c r="M36" s="72"/>
+      <c r="N36" s="56"/>
     </row>
     <row r="37" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="56"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="61"/>
-      <c r="J37" s="57"/>
-      <c r="K37" s="57"/>
-      <c r="L37" s="69"/>
-      <c r="M37" s="61"/>
-      <c r="N37" s="58"/>
+      <c r="A37" s="54"/>
+      <c r="C37" s="67"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="59"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="55"/>
+      <c r="L37" s="67"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="56"/>
     </row>
     <row r="38" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="56"/>
-      <c r="B38" s="92" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="73"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="72"/>
-      <c r="G38" s="72"/>
-      <c r="H38" s="71"/>
-      <c r="I38" s="134" t="s">
-        <v>89</v>
-      </c>
-      <c r="J38" s="133"/>
-      <c r="K38" s="133"/>
-      <c r="L38" s="133"/>
-      <c r="M38" s="133"/>
-      <c r="N38" s="58"/>
+      <c r="A38" s="54"/>
+      <c r="B38" s="90" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="71"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="132" t="s">
+        <v>87</v>
+      </c>
+      <c r="J38" s="131"/>
+      <c r="K38" s="131"/>
+      <c r="L38" s="131"/>
+      <c r="M38" s="131"/>
+      <c r="N38" s="56"/>
     </row>
     <row r="39" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="56"/>
-      <c r="B39" s="93" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
-      <c r="H39" s="61"/>
-      <c r="I39" s="70"/>
-      <c r="J39" s="57"/>
-      <c r="K39" s="57"/>
-      <c r="L39" s="69"/>
-      <c r="M39" s="61"/>
-      <c r="N39" s="58"/>
+      <c r="A39" s="54"/>
+      <c r="B39" s="91" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="57"/>
+      <c r="H39" s="59"/>
+      <c r="I39" s="68"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="59"/>
+      <c r="N39" s="56"/>
     </row>
     <row r="40" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="56"/>
-      <c r="B40" s="93" t="s">
+      <c r="A40" s="54"/>
+      <c r="B40" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="69"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="59"/>
-      <c r="H40" s="61"/>
-      <c r="I40" s="70"/>
-      <c r="J40" s="57"/>
-      <c r="K40" s="57"/>
-      <c r="L40" s="69"/>
-      <c r="M40" s="61"/>
-      <c r="N40" s="58"/>
+      <c r="C40" s="67"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="57"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="68"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="67"/>
+      <c r="M40" s="59"/>
+      <c r="N40" s="56"/>
     </row>
     <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="56"/>
-      <c r="B41" s="93" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="57"/>
-      <c r="K41" s="57"/>
-      <c r="L41" s="69"/>
-      <c r="M41" s="61"/>
-      <c r="N41" s="58"/>
-    </row>
-    <row r="42" spans="1:14" s="64" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="68"/>
-      <c r="B42" s="94" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="67"/>
-      <c r="F42" s="66"/>
-      <c r="G42" s="66"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="135"/>
-      <c r="J42" s="136"/>
-      <c r="K42" s="136"/>
-      <c r="L42" s="136"/>
-      <c r="M42" s="136"/>
-      <c r="N42" s="91"/>
+      <c r="A41" s="54"/>
+      <c r="B41" s="91" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="67"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="67"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="59"/>
+      <c r="I41" s="68"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="55"/>
+      <c r="L41" s="67"/>
+      <c r="M41" s="59"/>
+      <c r="N41" s="56"/>
+    </row>
+    <row r="42" spans="1:14" s="62" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="66"/>
+      <c r="B42" s="92" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="64"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="133"/>
+      <c r="J42" s="134"/>
+      <c r="K42" s="134"/>
+      <c r="L42" s="134"/>
+      <c r="M42" s="134"/>
+      <c r="N42" s="89"/>
     </row>
     <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
merging new group api
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8E9A10-9EB3-485A-9655-794264D30DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC21CF9-6305-453A-AE4D-18CAC4D7A775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,17 @@
   <definedNames>
     <definedName name="MID_Contract">Export_Contract!$E$1</definedName>
     <definedName name="MID_Invoice">Invoice!$G$1</definedName>
-    <definedName name="Seal_agent_end">Export_Contract!$H$53</definedName>
+    <definedName name="Seal_agent_end">Export_Contract!$H$52</definedName>
     <definedName name="Seal_agent_start">Export_Contract!$G$42</definedName>
-    <definedName name="Seal_seller_end">Export_Contract!$C$53</definedName>
+    <definedName name="Seal_seller_end">Export_Contract!$C$52</definedName>
     <definedName name="Seal_seller_start">Export_Contract!$C$44</definedName>
-    <definedName name="Sign_agent_end">Export_Contract!$G$53</definedName>
-    <definedName name="Sign_agent_start">Export_Contract!$G$51</definedName>
-    <definedName name="Sign_seller_start">Export_Contract!$C$51</definedName>
+    <definedName name="Sign_agent_end">Export_Contract!$G$52</definedName>
+    <definedName name="Sign_agent_start">Export_Contract!$G$50</definedName>
+    <definedName name="Sign_seller_start">Export_Contract!$C$50</definedName>
     <definedName name="Адреса_банк_получателя">Export_Contract!$B$34</definedName>
     <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$35</definedName>
     <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$36</definedName>
-    <definedName name="Адреса_подпись">Export_Contract!$B$52</definedName>
+    <definedName name="Адреса_подпись">Export_Contract!$B$51</definedName>
     <definedName name="Адреса_покупатель">Export_Contract!$B$40</definedName>
     <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$41</definedName>
     <definedName name="Адреса_покупатель_банк">Export_Contract!$B$43</definedName>
@@ -280,6 +280,12 @@
     <t>A/C: 242-910002-68638</t>
   </si>
   <si>
+    <t xml:space="preserve">Продавец/Seller  _______________________N.M. Kotov </t>
+  </si>
+  <si>
+    <t>Покупатель/Buyer ________________________SE JI YOUNG</t>
+  </si>
+  <si>
     <t>2.2. Total amount of this Agreement is specified in US dollars and is the following:</t>
   </si>
   <si>
@@ -548,12 +554,6 @@
   </si>
   <si>
     <t>Agreement No. 146 dated March 10, 2023</t>
-  </si>
-  <si>
-    <t>Покупатель/Buyer _________________________________SE JI YOUNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Продавец/Seller  ___________________________________N.M. Kotov </t>
   </si>
 </sst>
 </file>
@@ -870,7 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -974,8 +974,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1302,9 +1308,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1417,31 +1420,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1806,24 +1784,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AF89"/>
+  <dimension ref="B1:AF88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A18" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27:I27"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="1.06640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="11.265625" style="47" customWidth="1"/>
-    <col min="3" max="3" width="29" style="47" customWidth="1"/>
-    <col min="4" max="4" width="17.06640625" style="47" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" style="47" customWidth="1"/>
-    <col min="6" max="6" width="13.06640625" style="47" customWidth="1"/>
-    <col min="7" max="7" width="25.9296875" style="47" customWidth="1"/>
-    <col min="8" max="8" width="13.86328125" style="47" customWidth="1"/>
-    <col min="9" max="9" width="15.1328125" style="47" customWidth="1"/>
-    <col min="10" max="10" width="1.06640625" style="47" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="49" customWidth="1"/>
+    <col min="3" max="3" width="23.59765625" style="49" customWidth="1"/>
+    <col min="4" max="4" width="18" style="49" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="49" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="49" customWidth="1"/>
+    <col min="7" max="7" width="21.53125" style="49" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" style="49" customWidth="1"/>
+    <col min="9" max="9" width="15.06640625" style="49" customWidth="1"/>
+    <col min="10" max="10" width="1.06640625" style="49" customWidth="1"/>
     <col min="11" max="11" width="8.796875" style="10"/>
     <col min="12" max="12" width="13" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.796875" style="10"/>
@@ -1849,31 +1827,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="2.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160" t="s">
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
-      <c r="I1" s="160"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="162"/>
+      <c r="I1" s="162"/>
     </row>
     <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="193" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" s="194"/>
-      <c r="D2" s="194"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="193" t="s">
+      <c r="B2" s="194" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="194" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="194"/>
-      <c r="H2" s="194"/>
-      <c r="I2" s="194"/>
-      <c r="J2" s="161"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="163"/>
       <c r="L2" s="11"/>
       <c r="N2" s="18"/>
       <c r="AA2" s="18"/>
@@ -1882,18 +1860,18 @@
       <c r="AD2" s="18"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="196" t="s">
+      <c r="B3" s="197" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="198"/>
-      <c r="F3" s="196" t="s">
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="199"/>
+      <c r="F3" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="197"/>
-      <c r="H3" s="197"/>
-      <c r="I3" s="197"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="198"/>
+      <c r="I3" s="198"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1910,18 +1888,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="197"/>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
-      <c r="F4" s="196" t="s">
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="199"/>
+      <c r="F4" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="197"/>
-      <c r="H4" s="197"/>
-      <c r="I4" s="197"/>
+      <c r="G4" s="198"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1942,18 +1920,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="191" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="191"/>
-      <c r="D5" s="191"/>
-      <c r="E5" s="192"/>
-      <c r="F5" s="190" t="s">
+      <c r="C5" s="192"/>
+      <c r="D5" s="192"/>
+      <c r="E5" s="193"/>
+      <c r="F5" s="191" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="191"/>
-      <c r="H5" s="191"/>
-      <c r="I5" s="191"/>
+      <c r="G5" s="192"/>
+      <c r="H5" s="192"/>
+      <c r="I5" s="192"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1962,20 +1940,20 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="170" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="171"/>
-      <c r="D6" s="171"/>
-      <c r="E6" s="172"/>
-      <c r="F6" s="170" t="s">
+      <c r="B6" s="171" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="171"/>
-      <c r="H6" s="171"/>
-      <c r="I6" s="171"/>
-      <c r="J6" s="52"/>
-      <c r="L6" s="53"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="171" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="172"/>
+      <c r="H6" s="172"/>
+      <c r="I6" s="172"/>
+      <c r="J6" s="54"/>
+      <c r="L6" s="55"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
@@ -1991,19 +1969,19 @@
     </row>
     <row r="7" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="51"/>
+        <v>67</v>
+      </c>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="53"/>
       <c r="F7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="52"/>
-      <c r="L7" s="53"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="54"/>
+      <c r="L7" s="55"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
@@ -2018,48 +1996,48 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="179" t="s">
+      <c r="B8" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="180"/>
-      <c r="D8" s="180"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="163" t="s">
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="164" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="164"/>
-      <c r="H8" s="164"/>
-      <c r="I8" s="164"/>
+      <c r="G8" s="165"/>
+      <c r="H8" s="165"/>
+      <c r="I8" s="165"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="163" t="s">
+      <c r="B9" s="164" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="164"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="165"/>
-      <c r="F9" s="163" t="s">
+      <c r="C9" s="165"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="164" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="164"/>
-      <c r="H9" s="164"/>
-      <c r="I9" s="164"/>
+      <c r="G9" s="165"/>
+      <c r="H9" s="165"/>
+      <c r="I9" s="165"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="163" t="s">
+      <c r="B10" s="164" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="164"/>
-      <c r="D10" s="164"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="163" t="s">
+      <c r="C10" s="165"/>
+      <c r="D10" s="165"/>
+      <c r="E10" s="166"/>
+      <c r="F10" s="164" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="164"/>
-      <c r="H10" s="164"/>
-      <c r="I10" s="164"/>
+      <c r="G10" s="165"/>
+      <c r="H10" s="165"/>
+      <c r="I10" s="165"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -2080,19 +2058,19 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="170" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="171"/>
-      <c r="D11" s="171"/>
-      <c r="E11" s="172"/>
-      <c r="F11" s="170" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="171"/>
-      <c r="H11" s="171"/>
-      <c r="I11" s="171"/>
-      <c r="J11" s="52"/>
+      <c r="B11" s="171" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="172"/>
+      <c r="D11" s="172"/>
+      <c r="E11" s="173"/>
+      <c r="F11" s="171" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="172"/>
+      <c r="H11" s="172"/>
+      <c r="I11" s="172"/>
+      <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
@@ -2112,14 +2090,14 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="49"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="8"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="54"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
@@ -2134,18 +2112,18 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="163" t="s">
+      <c r="B13" s="164" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="164"/>
-      <c r="D13" s="164"/>
-      <c r="E13" s="165"/>
-      <c r="F13" s="163" t="s">
+      <c r="C13" s="165"/>
+      <c r="D13" s="165"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="164" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="164"/>
-      <c r="H13" s="164"/>
-      <c r="I13" s="164"/>
+      <c r="G13" s="165"/>
+      <c r="H13" s="165"/>
+      <c r="I13" s="165"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2163,18 +2141,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="163" t="s">
+      <c r="B14" s="164" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="164"/>
-      <c r="D14" s="164"/>
-      <c r="E14" s="165"/>
-      <c r="F14" s="163" t="s">
+      <c r="C14" s="165"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="164"/>
-      <c r="H14" s="164"/>
-      <c r="I14" s="164"/>
+      <c r="G14" s="165"/>
+      <c r="H14" s="165"/>
+      <c r="I14" s="165"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2192,18 +2170,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="163" t="s">
+      <c r="B15" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="164"/>
-      <c r="D15" s="164"/>
-      <c r="E15" s="165"/>
-      <c r="F15" s="163" t="s">
+      <c r="C15" s="165"/>
+      <c r="D15" s="165"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="164"/>
-      <c r="H15" s="164"/>
-      <c r="I15" s="164"/>
+      <c r="G15" s="165"/>
+      <c r="H15" s="165"/>
+      <c r="I15" s="165"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2221,18 +2199,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="182" t="s">
+      <c r="B16" s="183" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="183"/>
-      <c r="D16" s="183"/>
+      <c r="C16" s="184"/>
+      <c r="D16" s="184"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="182" t="s">
+      <c r="F16" s="183" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="183"/>
-      <c r="H16" s="183"/>
-      <c r="I16" s="184"/>
+      <c r="G16" s="184"/>
+      <c r="H16" s="184"/>
+      <c r="I16" s="185"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2250,18 +2228,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="163" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="185"/>
-      <c r="D17" s="185"/>
-      <c r="E17" s="186"/>
-      <c r="F17" s="187" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" s="185"/>
-      <c r="H17" s="185"/>
-      <c r="I17" s="185"/>
+      <c r="B17" s="164" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="186"/>
+      <c r="D17" s="186"/>
+      <c r="E17" s="187"/>
+      <c r="F17" s="188" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="186"/>
+      <c r="H17" s="186"/>
+      <c r="I17" s="186"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2279,23 +2257,23 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="188" t="s">
+      <c r="B18" s="189" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="190"/>
+      <c r="D18" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="190" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="189"/>
-      <c r="D18" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="189" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="189"/>
-      <c r="G18" s="189"/>
+      <c r="F18" s="190"/>
+      <c r="G18" s="190"/>
       <c r="H18" s="23" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J18" s="24"/>
       <c r="N18" s="10"/>
@@ -2314,18 +2292,18 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="173" t="s">
+      <c r="B19" s="174" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="174"/>
+      <c r="C19" s="175"/>
       <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="175" t="s">
+      <c r="E19" s="176" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="175"/>
-      <c r="G19" s="175"/>
+      <c r="F19" s="176"/>
+      <c r="G19" s="176"/>
       <c r="H19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2413,13 +2391,13 @@
     </row>
     <row r="22" spans="2:30" s="30" customFormat="1" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="27" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
       <c r="E22" s="29"/>
       <c r="F22" s="27" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
@@ -2474,18 +2452,18 @@
       <c r="AD24" s="10"/>
     </row>
     <row r="25" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="176" t="s">
+      <c r="B25" s="177" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="177"/>
-      <c r="D25" s="177"/>
-      <c r="E25" s="178"/>
-      <c r="F25" s="176" t="s">
+      <c r="C25" s="178"/>
+      <c r="D25" s="178"/>
+      <c r="E25" s="179"/>
+      <c r="F25" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="177"/>
-      <c r="H25" s="177"/>
-      <c r="I25" s="177"/>
+      <c r="G25" s="178"/>
+      <c r="H25" s="178"/>
+      <c r="I25" s="178"/>
       <c r="J25" s="22"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
@@ -2506,48 +2484,48 @@
       <c r="AD25" s="10"/>
     </row>
     <row r="26" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="163" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="164"/>
-      <c r="D26" s="164"/>
-      <c r="E26" s="165"/>
-      <c r="F26" s="163" t="s">
+      <c r="B26" s="164" t="s">
         <v>82</v>
       </c>
-      <c r="G26" s="164"/>
-      <c r="H26" s="164"/>
-      <c r="I26" s="164"/>
+      <c r="C26" s="165"/>
+      <c r="D26" s="165"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="164" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="165"/>
+      <c r="H26" s="165"/>
+      <c r="I26" s="165"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="179" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="180"/>
-      <c r="D27" s="180"/>
-      <c r="E27" s="181"/>
-      <c r="F27" s="163" t="s">
+      <c r="B27" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="G27" s="164"/>
-      <c r="H27" s="164"/>
-      <c r="I27" s="165"/>
+      <c r="C27" s="181"/>
+      <c r="D27" s="181"/>
+      <c r="E27" s="182"/>
+      <c r="F27" s="164" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="165"/>
+      <c r="H27" s="165"/>
+      <c r="I27" s="166"/>
       <c r="J27" s="19"/>
     </row>
     <row r="28" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="170" t="s">
+      <c r="B28" s="171" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="171"/>
-      <c r="D28" s="171"/>
+      <c r="C28" s="172"/>
+      <c r="D28" s="172"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="170" t="s">
+      <c r="F28" s="171" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="171"/>
-      <c r="H28" s="171"/>
-      <c r="I28" s="172"/>
+      <c r="G28" s="172"/>
+      <c r="H28" s="172"/>
+      <c r="I28" s="173"/>
       <c r="J28" s="22"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
@@ -2568,44 +2546,44 @@
       <c r="AD28" s="10"/>
     </row>
     <row r="29" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="163" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="164"/>
-      <c r="D29" s="164"/>
-      <c r="E29" s="165"/>
-      <c r="F29" s="163" t="s">
+      <c r="B29" s="164" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="165"/>
+      <c r="D29" s="165"/>
+      <c r="E29" s="166"/>
+      <c r="F29" s="164" t="s">
         <v>37</v>
       </c>
-      <c r="G29" s="164"/>
-      <c r="H29" s="164"/>
-      <c r="I29" s="164"/>
+      <c r="G29" s="165"/>
+      <c r="H29" s="165"/>
+      <c r="I29" s="165"/>
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="170" t="s">
+      <c r="B30" s="171" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="171"/>
-      <c r="D30" s="171"/>
+      <c r="C30" s="172"/>
+      <c r="D30" s="172"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="170" t="s">
+      <c r="F30" s="171" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="171"/>
-      <c r="H30" s="171"/>
-      <c r="I30" s="172"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="173"/>
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="48" t="s">
-        <v>64</v>
+      <c r="B31" s="50" t="s">
+        <v>66</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="21"/>
-      <c r="F31" s="48" t="s">
-        <v>70</v>
+      <c r="F31" s="50" t="s">
+        <v>72</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
@@ -2613,18 +2591,18 @@
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="166" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="167"/>
-      <c r="D32" s="167"/>
-      <c r="E32" s="168"/>
-      <c r="F32" s="166" t="s">
+      <c r="B32" s="167" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="168"/>
+      <c r="D32" s="168"/>
+      <c r="E32" s="169"/>
+      <c r="F32" s="167" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="167"/>
-      <c r="H32" s="167"/>
-      <c r="I32" s="167"/>
+      <c r="G32" s="168"/>
+      <c r="H32" s="168"/>
+      <c r="I32" s="168"/>
       <c r="J32" s="34"/>
       <c r="N32" s="36"/>
       <c r="O32" s="36"/>
@@ -2645,104 +2623,104 @@
       <c r="AD32" s="36"/>
     </row>
     <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="163" t="s">
+      <c r="B33" s="164" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="164"/>
-      <c r="D33" s="164"/>
-      <c r="E33" s="165"/>
-      <c r="F33" s="163" t="s">
+      <c r="C33" s="165"/>
+      <c r="D33" s="165"/>
+      <c r="E33" s="166"/>
+      <c r="F33" s="164" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="164"/>
-      <c r="H33" s="164"/>
-      <c r="I33" s="164"/>
+      <c r="G33" s="165"/>
+      <c r="H33" s="165"/>
+      <c r="I33" s="165"/>
       <c r="J33" s="19"/>
     </row>
     <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="163" t="s">
+      <c r="B34" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="164"/>
-      <c r="D34" s="164"/>
-      <c r="E34" s="165"/>
-      <c r="F34" s="163" t="s">
+      <c r="C34" s="165"/>
+      <c r="D34" s="165"/>
+      <c r="E34" s="166"/>
+      <c r="F34" s="164" t="s">
         <v>42</v>
       </c>
-      <c r="G34" s="164"/>
-      <c r="H34" s="164"/>
-      <c r="I34" s="164"/>
+      <c r="G34" s="165"/>
+      <c r="H34" s="165"/>
+      <c r="I34" s="165"/>
       <c r="J34" s="19"/>
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="163" t="s">
+      <c r="B35" s="164" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="164"/>
-      <c r="D35" s="164"/>
-      <c r="E35" s="165"/>
-      <c r="F35" s="163" t="s">
+      <c r="C35" s="165"/>
+      <c r="D35" s="165"/>
+      <c r="E35" s="166"/>
+      <c r="F35" s="164" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="164"/>
-      <c r="H35" s="164"/>
-      <c r="I35" s="164"/>
+      <c r="G35" s="165"/>
+      <c r="H35" s="165"/>
+      <c r="I35" s="165"/>
       <c r="J35" s="19"/>
     </row>
     <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="163" t="s">
+      <c r="B36" s="164" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="164"/>
-      <c r="D36" s="164"/>
-      <c r="E36" s="165"/>
-      <c r="F36" s="163" t="s">
+      <c r="C36" s="165"/>
+      <c r="D36" s="165"/>
+      <c r="E36" s="166"/>
+      <c r="F36" s="164" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="164"/>
-      <c r="H36" s="164"/>
-      <c r="I36" s="164"/>
+      <c r="G36" s="165"/>
+      <c r="H36" s="165"/>
+      <c r="I36" s="165"/>
       <c r="J36" s="19"/>
     </row>
     <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="163" t="s">
+      <c r="B37" s="164" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="164"/>
-      <c r="D37" s="164"/>
-      <c r="E37" s="165"/>
-      <c r="F37" s="163" t="s">
+      <c r="C37" s="165"/>
+      <c r="D37" s="165"/>
+      <c r="E37" s="166"/>
+      <c r="F37" s="164" t="s">
         <v>46</v>
       </c>
-      <c r="G37" s="164"/>
-      <c r="H37" s="164"/>
-      <c r="I37" s="164"/>
+      <c r="G37" s="165"/>
+      <c r="H37" s="165"/>
+      <c r="I37" s="165"/>
       <c r="J37" s="19"/>
     </row>
     <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="163" t="s">
+      <c r="B38" s="164" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="164"/>
-      <c r="D38" s="164"/>
-      <c r="E38" s="165"/>
-      <c r="F38" s="163" t="s">
+      <c r="C38" s="165"/>
+      <c r="D38" s="165"/>
+      <c r="E38" s="166"/>
+      <c r="F38" s="164" t="s">
         <v>48</v>
       </c>
-      <c r="G38" s="164"/>
-      <c r="H38" s="164"/>
-      <c r="I38" s="164"/>
+      <c r="G38" s="165"/>
+      <c r="H38" s="165"/>
+      <c r="I38" s="165"/>
       <c r="J38" s="19"/>
     </row>
     <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="60" t="s">
-        <v>71</v>
+      <c r="B39" s="62" t="s">
+        <v>73</v>
       </c>
       <c r="C39" s="20"/>
       <c r="D39" s="20"/>
       <c r="E39" s="21"/>
-      <c r="F39" s="60" t="s">
-        <v>72</v>
+      <c r="F39" s="62" t="s">
+        <v>74</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
@@ -2750,18 +2728,18 @@
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="166" t="s">
+      <c r="B40" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="167"/>
-      <c r="D40" s="167"/>
-      <c r="E40" s="168"/>
-      <c r="F40" s="166" t="s">
+      <c r="C40" s="168"/>
+      <c r="D40" s="168"/>
+      <c r="E40" s="169"/>
+      <c r="F40" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="G40" s="169"/>
-      <c r="H40" s="169"/>
-      <c r="I40" s="169"/>
+      <c r="G40" s="170"/>
+      <c r="H40" s="170"/>
+      <c r="I40" s="170"/>
       <c r="J40" s="34"/>
       <c r="N40" s="36"/>
       <c r="O40" s="36"/>
@@ -2781,23 +2759,24 @@
       <c r="AC40" s="36"/>
       <c r="AD40" s="36"/>
     </row>
-    <row r="41" spans="2:30" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="163" t="s">
+    <row r="41" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="164" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="164"/>
-      <c r="D41" s="164"/>
-      <c r="E41" s="165"/>
-      <c r="F41" s="163" t="s">
+      <c r="C41" s="165"/>
+      <c r="D41" s="165"/>
+      <c r="E41" s="166"/>
+      <c r="F41" s="164" t="s">
         <v>15</v>
       </c>
-      <c r="G41" s="164"/>
-      <c r="H41" s="164"/>
-      <c r="I41" s="164"/>
+      <c r="G41" s="165"/>
+      <c r="H41" s="165"/>
+      <c r="I41" s="165"/>
       <c r="J41" s="19"/>
     </row>
-    <row r="42" spans="2:30" ht="1.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B42" s="19"/>
+      <c r="C42" s="31"/>
       <c r="D42" s="31"/>
       <c r="E42" s="21"/>
       <c r="F42" s="19"/>
@@ -2808,205 +2787,171 @@
       <c r="I42" s="20"/>
       <c r="J42" s="19"/>
     </row>
-    <row r="43" spans="2:30" s="205" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="201" t="s">
+    <row r="43" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B43" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="202"/>
-      <c r="D43" s="202"/>
-      <c r="E43" s="203"/>
-      <c r="F43" s="201" t="s">
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="G43" s="202"/>
-      <c r="H43" s="204"/>
-      <c r="I43" s="204"/>
-      <c r="J43" s="162"/>
-      <c r="N43" s="206"/>
-      <c r="O43" s="206"/>
-      <c r="P43" s="206"/>
-      <c r="Q43" s="206"/>
-      <c r="R43" s="206"/>
-      <c r="S43" s="206"/>
-      <c r="T43" s="206"/>
-      <c r="U43" s="206"/>
-      <c r="V43" s="206"/>
-      <c r="W43" s="206"/>
-      <c r="X43" s="206"/>
-      <c r="Y43" s="206"/>
-      <c r="Z43" s="206"/>
-      <c r="AA43" s="206"/>
-      <c r="AB43" s="206"/>
-      <c r="AC43" s="206"/>
-      <c r="AD43" s="206"/>
-    </row>
-    <row r="44" spans="2:30" s="205" customFormat="1" ht="1.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="201"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="19"/>
+    </row>
+    <row r="44" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B44" s="39"/>
       <c r="C44" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="202"/>
-      <c r="E44" s="203"/>
-      <c r="F44" s="201"/>
-      <c r="G44" s="202"/>
-      <c r="H44" s="204"/>
-      <c r="I44" s="204"/>
-      <c r="J44" s="162"/>
-      <c r="N44" s="206"/>
-      <c r="O44" s="206"/>
-      <c r="P44" s="206"/>
-      <c r="Q44" s="206"/>
-      <c r="R44" s="206"/>
-      <c r="S44" s="206"/>
-      <c r="T44" s="206"/>
-      <c r="U44" s="206"/>
-      <c r="V44" s="206"/>
-      <c r="W44" s="206"/>
-      <c r="X44" s="206"/>
-      <c r="Y44" s="206"/>
-      <c r="Z44" s="206"/>
-      <c r="AA44" s="206"/>
-      <c r="AB44" s="206"/>
-      <c r="AC44" s="206"/>
-      <c r="AD44" s="206"/>
-    </row>
-    <row r="45" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="207" t="s">
+      <c r="D44" s="31"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="19"/>
+    </row>
+    <row r="45" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="208"/>
-      <c r="D45" s="208"/>
-      <c r="E45" s="209"/>
-      <c r="F45" s="207" t="s">
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="G45" s="210"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="37"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
       <c r="J45" s="19"/>
     </row>
-    <row r="46" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="207" t="s">
+    <row r="46" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="208"/>
-      <c r="D46" s="208"/>
-      <c r="E46" s="211"/>
-      <c r="F46" s="207" t="s">
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="G46" s="210"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="37"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
       <c r="J46" s="19"/>
     </row>
-    <row r="47" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="207" t="s">
+    <row r="47" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B47" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="208"/>
-      <c r="D47" s="208"/>
-      <c r="E47" s="211"/>
-      <c r="F47" s="208" t="s">
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="G47" s="210"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="37"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
       <c r="J47" s="19"/>
     </row>
-    <row r="48" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="207" t="s">
+    <row r="48" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B48" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="208"/>
-      <c r="D48" s="208"/>
-      <c r="E48" s="211"/>
-      <c r="F48" s="208" t="s">
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="G48" s="210"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
       <c r="J48" s="19"/>
     </row>
-    <row r="49" spans="2:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="207" t="s">
+    <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="208"/>
-      <c r="D49" s="208"/>
-      <c r="E49" s="211"/>
-      <c r="F49" s="208" t="s">
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="G49" s="208"/>
+      <c r="G49" s="28"/>
       <c r="H49" s="28"/>
       <c r="I49" s="28"/>
       <c r="J49" s="19"/>
     </row>
-    <row r="50" spans="2:10" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="207"/>
-      <c r="C50" s="208"/>
-      <c r="D50" s="208"/>
-      <c r="E50" s="211"/>
-      <c r="F50" s="208"/>
-      <c r="G50" s="208"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="28"/>
+    <row r="50" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="19"/>
+      <c r="C50" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="31"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H50" s="31"/>
+      <c r="I50" s="31"/>
       <c r="J50" s="19"/>
     </row>
-    <row r="51" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="19"/>
-      <c r="C51" s="36" t="s">
+    <row r="51" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="41"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="42"/>
+      <c r="J51" s="15"/>
+    </row>
+    <row r="52" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="43"/>
+      <c r="C52" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="D51" s="31"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="12" t="s">
+      <c r="D52" s="45"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="H51" s="31"/>
-      <c r="I51" s="31"/>
-      <c r="J51" s="19"/>
-    </row>
-    <row r="52" spans="2:10" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="40"/>
-      <c r="F52" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="G52" s="39"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="40"/>
+      <c r="H52" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="I52" s="46"/>
       <c r="J52" s="15"/>
     </row>
-    <row r="53" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="41"/>
-      <c r="C53" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="D53" s="43"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="45"/>
-      <c r="G53" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="H53" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="I53" s="44"/>
+    <row r="53" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="15"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="48"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
       <c r="J53" s="15"/>
     </row>
-    <row r="54" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B54" s="15"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="46"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="48"/>
       <c r="E54" s="15"/>
       <c r="F54" s="15"/>
       <c r="G54" s="15"/>
@@ -3016,8 +2961,8 @@
     </row>
     <row r="55" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B55" s="15"/>
-      <c r="C55" s="46"/>
-      <c r="D55" s="46"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
       <c r="E55" s="15"/>
       <c r="F55" s="15"/>
       <c r="G55" s="15"/>
@@ -3027,8 +2972,8 @@
     </row>
     <row r="56" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B56" s="15"/>
-      <c r="C56" s="46"/>
-      <c r="D56" s="46"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="48"/>
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
@@ -3038,8 +2983,8 @@
     </row>
     <row r="57" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B57" s="15"/>
-      <c r="C57" s="46"/>
-      <c r="D57" s="46"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
       <c r="G57" s="15"/>
@@ -3049,8 +2994,8 @@
     </row>
     <row r="58" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B58" s="15"/>
-      <c r="C58" s="46"/>
-      <c r="D58" s="46"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="48"/>
       <c r="E58" s="15"/>
       <c r="F58" s="15"/>
       <c r="G58" s="15"/>
@@ -3060,8 +3005,8 @@
     </row>
     <row r="59" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B59" s="15"/>
-      <c r="C59" s="46"/>
-      <c r="D59" s="46"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="48"/>
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
       <c r="G59" s="15"/>
@@ -3071,8 +3016,8 @@
     </row>
     <row r="60" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B60" s="15"/>
-      <c r="C60" s="46"/>
-      <c r="D60" s="46"/>
+      <c r="C60" s="48"/>
+      <c r="D60" s="48"/>
       <c r="E60" s="15"/>
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
@@ -3082,8 +3027,8 @@
     </row>
     <row r="61" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B61" s="15"/>
-      <c r="C61" s="46"/>
-      <c r="D61" s="46"/>
+      <c r="C61" s="48"/>
+      <c r="D61" s="48"/>
       <c r="E61" s="15"/>
       <c r="F61" s="15"/>
       <c r="G61" s="15"/>
@@ -3093,8 +3038,8 @@
     </row>
     <row r="62" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B62" s="15"/>
-      <c r="C62" s="46"/>
-      <c r="D62" s="46"/>
+      <c r="C62" s="48"/>
+      <c r="D62" s="48"/>
       <c r="E62" s="15"/>
       <c r="F62" s="15"/>
       <c r="G62" s="15"/>
@@ -3102,29 +3047,18 @@
       <c r="I62" s="15"/>
       <c r="J62" s="15"/>
     </row>
-    <row r="63" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B63" s="15"/>
-      <c r="C63" s="46"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="15"/>
-      <c r="I63" s="15"/>
-      <c r="J63" s="15"/>
-    </row>
+    <row r="63" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="64" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="65" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="66" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="67" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="68" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="69" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="77" spans="6:7" x14ac:dyDescent="0.45">
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
-    </row>
-    <row r="82" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="89" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="76" spans="6:7" x14ac:dyDescent="0.45">
+      <c r="F76" s="10"/>
+      <c r="G76" s="10"/>
+    </row>
+    <row r="81" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="88" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="62">
     <mergeCell ref="B2:E2"/>
@@ -3215,7 +3149,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.35433070866141736" bottom="0.15748031496062992" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="76" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3227,8 +3161,8 @@
   </sheetPr>
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="94" zoomScaleNormal="100" zoomScaleSheetLayoutView="94" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3251,445 +3185,447 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G1" s="159" t="s">
+      <c r="A1" s="56"/>
+      <c r="G1" s="161" t="s">
         <v>49</v>
       </c>
+      <c r="N1" s="58"/>
     </row>
     <row r="2" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="87"/>
-      <c r="B2" s="117" t="s">
+      <c r="A2" s="89"/>
+      <c r="B2" s="119" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="122" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="58"/>
+    </row>
+    <row r="3" spans="1:14" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="89"/>
+      <c r="B3" s="120" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="120" t="s">
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="123" t="s">
         <v>136</v>
       </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="56"/>
-    </row>
-    <row r="3" spans="1:14" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="87"/>
-      <c r="B3" s="118" t="s">
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="58"/>
+    </row>
+    <row r="4" spans="1:14" s="86" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="88"/>
+      <c r="B4" s="120" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="121" t="s">
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="123" t="s">
         <v>134</v>
       </c>
-      <c r="I3" s="118"/>
-      <c r="J3" s="118"/>
-      <c r="K3" s="118"/>
-      <c r="L3" s="118"/>
-      <c r="M3" s="118"/>
-      <c r="N3" s="56"/>
-    </row>
-    <row r="4" spans="1:14" s="84" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="86"/>
-      <c r="B4" s="118" t="s">
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="84"/>
+    </row>
+    <row r="5" spans="1:14" s="86" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="87"/>
+      <c r="B5" s="120" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="118"/>
-      <c r="H4" s="121" t="s">
+      <c r="C5" s="120"/>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="123" t="s">
         <v>132</v>
       </c>
-      <c r="I4" s="118"/>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="118"/>
-      <c r="M4" s="118"/>
-      <c r="N4" s="82"/>
-    </row>
-    <row r="5" spans="1:14" s="84" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="85"/>
-      <c r="B5" s="118" t="s">
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="84"/>
+    </row>
+    <row r="6" spans="1:14" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="56"/>
+      <c r="B6" s="110" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="121" t="s">
+      <c r="C6" s="110"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="96" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="58"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="56"/>
+      <c r="B7" s="113" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="99" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="58"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="56"/>
+      <c r="B8" s="125" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="125"/>
+      <c r="F8" s="125"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="98"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="58"/>
+    </row>
+    <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="56"/>
+      <c r="B9" s="126" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="126"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="103" t="s">
+        <v>140</v>
+      </c>
+      <c r="I9" s="98"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="98"/>
+      <c r="L9" s="98"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="58"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="56"/>
+      <c r="B10" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="113"/>
+      <c r="D10" s="113"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+      <c r="L10" s="98"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="58"/>
+    </row>
+    <row r="11" spans="1:14" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="56"/>
+      <c r="B11" s="102" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="155" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="102"/>
+      <c r="N11" s="58"/>
+    </row>
+    <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="56"/>
+      <c r="B12" s="126" t="s">
         <v>130</v>
       </c>
-      <c r="I5" s="118"/>
-      <c r="J5" s="118"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="118"/>
-      <c r="M5" s="118"/>
-      <c r="N5" s="82"/>
-    </row>
-    <row r="6" spans="1:14" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="54"/>
-      <c r="B6" s="108" t="s">
+      <c r="C12" s="126"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="126"/>
+      <c r="H12" s="96" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="94" t="s">
-        <v>70</v>
-      </c>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="96"/>
-      <c r="M6" s="96"/>
-      <c r="N6" s="56"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="54"/>
-      <c r="B7" s="111" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="122"/>
-      <c r="F7" s="122"/>
-      <c r="G7" s="122"/>
-      <c r="H7" s="97" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="96"/>
-      <c r="M7" s="96"/>
-      <c r="N7" s="56"/>
-    </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="54"/>
-      <c r="B8" s="123" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="123"/>
-      <c r="G8" s="123"/>
-      <c r="H8" s="99" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="100"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="100"/>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96"/>
-      <c r="N8" s="56"/>
-    </row>
-    <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="54"/>
-      <c r="B9" s="124" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="124"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="101" t="s">
-        <v>138</v>
-      </c>
-      <c r="I9" s="96"/>
-      <c r="J9" s="96"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="96"/>
-      <c r="M9" s="96"/>
-      <c r="N9" s="56"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="54"/>
-      <c r="B10" s="111" t="s">
+      <c r="I12" s="97"/>
+      <c r="J12" s="97"/>
+      <c r="K12" s="97"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="58"/>
+    </row>
+    <row r="13" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="56"/>
+      <c r="B13" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="111"/>
-      <c r="F10" s="111"/>
-      <c r="G10" s="111"/>
-      <c r="H10" s="97" t="s">
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="96"/>
-      <c r="J10" s="96"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="96"/>
-      <c r="M10" s="96"/>
-      <c r="N10" s="56"/>
-    </row>
-    <row r="11" spans="1:14" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="54"/>
-      <c r="B11" s="100" t="s">
+      <c r="I13" s="100"/>
+      <c r="J13" s="100"/>
+      <c r="K13" s="100"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="58"/>
+    </row>
+    <row r="14" spans="1:14" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="56"/>
+      <c r="B14" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="116"/>
-      <c r="H11" s="153" t="s">
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="118"/>
+      <c r="H14" s="155" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="100"/>
-      <c r="J11" s="100"/>
-      <c r="K11" s="100"/>
-      <c r="L11" s="100"/>
-      <c r="M11" s="100"/>
-      <c r="N11" s="56"/>
-    </row>
-    <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="54"/>
-      <c r="B12" s="124" t="s">
+      <c r="I14" s="102"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="58"/>
+    </row>
+    <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="85"/>
+      <c r="B15" s="104" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="104"/>
+      <c r="D15" s="105" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="105"/>
+      <c r="H15" s="106" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="105"/>
+      <c r="J15" s="127" t="s">
+        <v>113</v>
+      </c>
+      <c r="K15" s="127"/>
+      <c r="L15" s="151" t="s">
+        <v>114</v>
+      </c>
+      <c r="M15" s="151"/>
+      <c r="N15" s="58"/>
+    </row>
+    <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="56"/>
+      <c r="B16" s="118" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="107"/>
+      <c r="D16" s="156" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="108"/>
+      <c r="F16" s="144" t="s">
+        <v>112</v>
+      </c>
+      <c r="G16" s="108"/>
+      <c r="H16" s="159" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" s="108"/>
+      <c r="J16" s="109" t="s">
+        <v>108</v>
+      </c>
+      <c r="K16" s="109"/>
+      <c r="L16" s="152" t="s">
+        <v>109</v>
+      </c>
+      <c r="M16" s="152"/>
+      <c r="N16" s="58"/>
+    </row>
+    <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="56"/>
+      <c r="B17" s="126" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="124"/>
-      <c r="D12" s="124"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="124"/>
-      <c r="G12" s="124"/>
-      <c r="H12" s="94" t="s">
+      <c r="C17" s="126"/>
+      <c r="D17" s="126" t="s">
         <v>127</v>
       </c>
-      <c r="I12" s="95"/>
-      <c r="J12" s="95"/>
-      <c r="K12" s="95"/>
-      <c r="L12" s="96"/>
-      <c r="M12" s="96"/>
-      <c r="N12" s="56"/>
-    </row>
-    <row r="13" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="54"/>
-      <c r="B13" s="111" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="97" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="98"/>
-      <c r="J13" s="98"/>
-      <c r="K13" s="98"/>
-      <c r="L13" s="96"/>
-      <c r="M13" s="96"/>
-      <c r="N13" s="56"/>
-    </row>
-    <row r="14" spans="1:14" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="54"/>
-      <c r="B14" s="100" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="116"/>
-      <c r="H14" s="153" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="100"/>
-      <c r="J14" s="100"/>
-      <c r="K14" s="100"/>
-      <c r="L14" s="100"/>
-      <c r="M14" s="100"/>
-      <c r="N14" s="56"/>
-    </row>
-    <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="83"/>
-      <c r="B15" s="102" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="103" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="103"/>
-      <c r="F15" s="103" t="s">
-        <v>114</v>
-      </c>
-      <c r="G15" s="103"/>
-      <c r="H15" s="104" t="s">
-        <v>113</v>
-      </c>
-      <c r="I15" s="103"/>
-      <c r="J15" s="125" t="s">
-        <v>111</v>
-      </c>
-      <c r="K15" s="125"/>
-      <c r="L15" s="149" t="s">
-        <v>112</v>
-      </c>
-      <c r="M15" s="149"/>
-      <c r="N15" s="56"/>
-    </row>
-    <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="54"/>
-      <c r="B16" s="116" t="s">
+      <c r="E17" s="130"/>
+      <c r="F17" s="143" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" s="143"/>
+      <c r="H17" s="103" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" s="98"/>
+      <c r="J17" s="111" t="s">
+        <v>124</v>
+      </c>
+      <c r="K17" s="98"/>
+      <c r="L17" s="153" t="s">
+        <v>123</v>
+      </c>
+      <c r="M17" s="154"/>
+      <c r="N17" s="58"/>
+    </row>
+    <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="56"/>
+      <c r="B18" s="102" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="125"/>
+      <c r="D18" s="157" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="109"/>
+      <c r="F18" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="154" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16" s="106"/>
-      <c r="F16" s="142" t="s">
-        <v>110</v>
-      </c>
-      <c r="G16" s="106"/>
-      <c r="H16" s="157" t="s">
-        <v>108</v>
-      </c>
-      <c r="I16" s="106"/>
-      <c r="J16" s="107" t="s">
+      <c r="G18" s="144"/>
+      <c r="H18" s="159" t="s">
+        <v>120</v>
+      </c>
+      <c r="I18" s="109"/>
+      <c r="J18" s="157" t="s">
+        <v>119</v>
+      </c>
+      <c r="K18" s="109"/>
+      <c r="L18" s="152" t="s">
+        <v>118</v>
+      </c>
+      <c r="M18" s="152"/>
+      <c r="N18" s="58"/>
+    </row>
+    <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="56"/>
+      <c r="B19" s="131" t="s">
         <v>106</v>
       </c>
-      <c r="K16" s="107"/>
-      <c r="L16" s="150" t="s">
+      <c r="C19" s="131"/>
+      <c r="D19" s="131" t="s">
         <v>107</v>
       </c>
-      <c r="M16" s="150"/>
-      <c r="N16" s="56"/>
-    </row>
-    <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="54"/>
-      <c r="B17" s="124" t="s">
-        <v>126</v>
-      </c>
-      <c r="C17" s="124"/>
-      <c r="D17" s="124" t="s">
-        <v>125</v>
-      </c>
-      <c r="E17" s="128"/>
-      <c r="F17" s="141" t="s">
-        <v>124</v>
-      </c>
-      <c r="G17" s="141"/>
-      <c r="H17" s="101" t="s">
-        <v>123</v>
-      </c>
-      <c r="I17" s="96"/>
-      <c r="J17" s="109" t="s">
-        <v>122</v>
-      </c>
-      <c r="K17" s="96"/>
-      <c r="L17" s="151" t="s">
-        <v>121</v>
-      </c>
-      <c r="M17" s="152"/>
-      <c r="N17" s="56"/>
-    </row>
-    <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="54"/>
-      <c r="B18" s="100" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="123"/>
-      <c r="D18" s="155" t="s">
-        <v>119</v>
-      </c>
-      <c r="E18" s="107"/>
-      <c r="F18" s="156" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="142"/>
-      <c r="H18" s="157" t="s">
-        <v>118</v>
-      </c>
-      <c r="I18" s="107"/>
-      <c r="J18" s="155" t="s">
-        <v>117</v>
-      </c>
-      <c r="K18" s="107"/>
-      <c r="L18" s="150" t="s">
-        <v>116</v>
-      </c>
-      <c r="M18" s="150"/>
-      <c r="N18" s="56"/>
-    </row>
-    <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="54"/>
-      <c r="B19" s="129" t="s">
+      <c r="E19" s="131"/>
+      <c r="F19" s="145"/>
+      <c r="G19" s="145"/>
+      <c r="H19" s="148" t="s">
+        <v>141</v>
+      </c>
+      <c r="I19" s="128"/>
+      <c r="J19" s="126" t="s">
+        <v>105</v>
+      </c>
+      <c r="K19" s="126"/>
+      <c r="L19" s="126"/>
+      <c r="M19" s="126"/>
+      <c r="N19" s="58"/>
+    </row>
+    <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="56"/>
+      <c r="B20" s="156" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="112"/>
+      <c r="D20" s="129" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="129"/>
-      <c r="D19" s="129" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" s="129"/>
-      <c r="F19" s="143"/>
-      <c r="G19" s="143"/>
-      <c r="H19" s="146" t="s">
-        <v>139</v>
-      </c>
-      <c r="I19" s="126"/>
-      <c r="J19" s="124" t="s">
-        <v>103</v>
-      </c>
-      <c r="K19" s="124"/>
-      <c r="L19" s="124"/>
-      <c r="M19" s="124"/>
-      <c r="N19" s="56"/>
-    </row>
-    <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="54"/>
-      <c r="B20" s="154" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="110"/>
-      <c r="D20" s="127" t="s">
-        <v>102</v>
-      </c>
-      <c r="E20" s="127"/>
-      <c r="F20" s="144"/>
-      <c r="G20" s="144"/>
-      <c r="H20" s="158" t="s">
-        <v>62</v>
-      </c>
-      <c r="I20" s="106"/>
-      <c r="J20" s="111" t="s">
-        <v>102</v>
-      </c>
-      <c r="K20" s="112"/>
-      <c r="L20" s="107"/>
-      <c r="M20" s="107"/>
-      <c r="N20" s="56"/>
-    </row>
-    <row r="21" spans="1:29" s="80" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="93"/>
-      <c r="B21" s="113"/>
-      <c r="C21" s="113"/>
-      <c r="D21" s="113"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="113"/>
-      <c r="G21" s="145"/>
-      <c r="H21" s="147"/>
-      <c r="I21" s="114"/>
-      <c r="J21" s="114"/>
-      <c r="K21" s="114"/>
-      <c r="L21" s="114"/>
-      <c r="M21" s="115"/>
-      <c r="N21" s="81"/>
+      <c r="E20" s="129"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="146"/>
+      <c r="H20" s="160" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="108"/>
+      <c r="J20" s="113" t="s">
+        <v>104</v>
+      </c>
+      <c r="K20" s="114"/>
+      <c r="L20" s="109"/>
+      <c r="M20" s="109"/>
+      <c r="N20" s="58"/>
+    </row>
+    <row r="21" spans="1:29" s="82" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="95"/>
+      <c r="B21" s="115"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="115"/>
+      <c r="F21" s="115"/>
+      <c r="G21" s="147"/>
+      <c r="H21" s="149"/>
+      <c r="I21" s="116"/>
+      <c r="J21" s="116"/>
+      <c r="K21" s="116"/>
+      <c r="L21" s="116"/>
+      <c r="M21" s="117"/>
+      <c r="N21" s="83"/>
       <c r="S21"/>
       <c r="T21"/>
       <c r="U21"/>
@@ -3703,386 +3639,386 @@
       <c r="AC21"/>
     </row>
     <row r="22" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="54"/>
-      <c r="B22" s="58" t="s">
+      <c r="A22" s="56"/>
+      <c r="B22" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="132" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="132"/>
+      <c r="E22" s="132"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="132"/>
+      <c r="H22" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="130" t="s">
+      <c r="I22" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="130"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="148"/>
-      <c r="G22" s="130"/>
-      <c r="H22" s="58" t="s">
+      <c r="J22" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="I22" s="79" t="s">
+      <c r="K22" s="132" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="78" t="s">
+      <c r="L22" s="132"/>
+      <c r="M22" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="K22" s="130" t="s">
+      <c r="N22" s="58"/>
+    </row>
+    <row r="23" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="56"/>
+      <c r="B23" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="L22" s="130"/>
-      <c r="M22" s="58" t="s">
+      <c r="C23" s="200" t="s">
         <v>95</v>
       </c>
-      <c r="N22" s="56"/>
-    </row>
-    <row r="23" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="54"/>
-      <c r="B23" s="137" t="s">
+      <c r="D23" s="200"/>
+      <c r="E23" s="200"/>
+      <c r="F23" s="200"/>
+      <c r="G23" s="140"/>
+      <c r="H23" s="141" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="199" t="s">
+      <c r="I23" s="79" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" s="78">
+        <v>14</v>
+      </c>
+      <c r="K23" s="201" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="199"/>
-      <c r="E23" s="199"/>
-      <c r="F23" s="199"/>
-      <c r="G23" s="138"/>
-      <c r="H23" s="139" t="s">
+      <c r="L23" s="201"/>
+      <c r="M23" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="N23" s="58"/>
+    </row>
+    <row r="24" spans="1:29" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="56"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="137"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="137"/>
+      <c r="G24" s="137"/>
+      <c r="H24" s="138" t="s">
         <v>92</v>
       </c>
-      <c r="I23" s="77" t="s">
+      <c r="I24" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="J24" s="75">
+        <v>14</v>
+      </c>
+      <c r="K24" s="142" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="142"/>
+      <c r="M24" s="90" t="s">
+        <v>90</v>
+      </c>
+      <c r="N24" s="58"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A25" s="56"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="69"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="58"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A26" s="56"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="69"/>
+      <c r="K26" s="69"/>
+      <c r="L26" s="69"/>
+      <c r="M26" s="74"/>
+      <c r="N26" s="58"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A27" s="56"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="69"/>
+      <c r="K27" s="69"/>
+      <c r="L27" s="69"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="58"/>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A28" s="56"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="69"/>
+      <c r="L28" s="69"/>
+      <c r="M28" s="74"/>
+      <c r="N28" s="58"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A29" s="56"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="69"/>
+      <c r="K29" s="69"/>
+      <c r="L29" s="69"/>
+      <c r="M29" s="74"/>
+      <c r="N29" s="58"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A30" s="56"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="69"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="74"/>
+      <c r="N30" s="58"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A31" s="56"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="69"/>
+      <c r="K31" s="69"/>
+      <c r="L31" s="69"/>
+      <c r="M31" s="74"/>
+      <c r="N31" s="58"/>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A32" s="56"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="74"/>
+      <c r="N32" s="58"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A33" s="56"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="69"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="69"/>
+      <c r="M33" s="74"/>
+      <c r="N33" s="58"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A34" s="56"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
+      <c r="L34" s="69"/>
+      <c r="M34" s="74"/>
+      <c r="N34" s="58"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A35" s="56"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="74"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="69"/>
+      <c r="M35" s="74"/>
+      <c r="N35" s="58"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A36" s="56"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="69"/>
+      <c r="K36" s="69"/>
+      <c r="L36" s="69"/>
+      <c r="M36" s="74"/>
+      <c r="N36" s="58"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="56"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="61"/>
+      <c r="J37" s="57"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="69"/>
+      <c r="M37" s="61"/>
+      <c r="N37" s="58"/>
+    </row>
+    <row r="38" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="56"/>
+      <c r="B38" s="92" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="72"/>
+      <c r="G38" s="72"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="134" t="s">
         <v>89</v>
       </c>
-      <c r="J23" s="76">
-        <v>14</v>
-      </c>
-      <c r="K23" s="200" t="s">
-        <v>91</v>
-      </c>
-      <c r="L23" s="200"/>
-      <c r="M23" s="75" t="s">
+      <c r="J38" s="133"/>
+      <c r="K38" s="133"/>
+      <c r="L38" s="133"/>
+      <c r="M38" s="133"/>
+      <c r="N38" s="58"/>
+    </row>
+    <row r="39" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="56"/>
+      <c r="B39" s="93" t="s">
         <v>88</v>
       </c>
-      <c r="N23" s="56"/>
-    </row>
-    <row r="24" spans="1:29" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="54"/>
-      <c r="C24" s="135"/>
-      <c r="D24" s="135"/>
-      <c r="E24" s="135"/>
-      <c r="F24" s="135"/>
-      <c r="G24" s="135"/>
-      <c r="H24" s="136" t="s">
-        <v>90</v>
-      </c>
-      <c r="I24" s="74" t="s">
-        <v>89</v>
-      </c>
-      <c r="J24" s="73">
-        <v>14</v>
-      </c>
-      <c r="K24" s="140" t="s">
-        <v>49</v>
-      </c>
-      <c r="L24" s="140"/>
-      <c r="M24" s="88" t="s">
-        <v>88</v>
-      </c>
-      <c r="N24" s="56"/>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A25" s="54"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
-      <c r="L25" s="67"/>
-      <c r="M25" s="72"/>
-      <c r="N25" s="56"/>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A26" s="54"/>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="67"/>
-      <c r="K26" s="67"/>
-      <c r="L26" s="67"/>
-      <c r="M26" s="72"/>
-      <c r="N26" s="56"/>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A27" s="54"/>
-      <c r="B27" s="67"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="67"/>
-      <c r="L27" s="67"/>
-      <c r="M27" s="72"/>
-      <c r="N27" s="56"/>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A28" s="54"/>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="67"/>
-      <c r="K28" s="67"/>
-      <c r="L28" s="67"/>
-      <c r="M28" s="72"/>
-      <c r="N28" s="56"/>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A29" s="54"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="67"/>
-      <c r="L29" s="67"/>
-      <c r="M29" s="72"/>
-      <c r="N29" s="56"/>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A30" s="54"/>
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="67"/>
-      <c r="L30" s="67"/>
-      <c r="M30" s="72"/>
-      <c r="N30" s="56"/>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A31" s="54"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="72"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="67"/>
-      <c r="L31" s="67"/>
-      <c r="M31" s="72"/>
-      <c r="N31" s="56"/>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A32" s="54"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="67"/>
-      <c r="L32" s="67"/>
-      <c r="M32" s="72"/>
-      <c r="N32" s="56"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A33" s="54"/>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="67"/>
-      <c r="K33" s="67"/>
-      <c r="L33" s="67"/>
-      <c r="M33" s="72"/>
-      <c r="N33" s="56"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A34" s="54"/>
-      <c r="B34" s="67"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="67"/>
-      <c r="K34" s="67"/>
-      <c r="L34" s="67"/>
-      <c r="M34" s="72"/>
-      <c r="N34" s="56"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A35" s="54"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="72"/>
-      <c r="N35" s="56"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A36" s="54"/>
-      <c r="B36" s="67"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="67"/>
-      <c r="K36" s="67"/>
-      <c r="L36" s="67"/>
-      <c r="M36" s="72"/>
-      <c r="N36" s="56"/>
-    </row>
-    <row r="37" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="54"/>
-      <c r="C37" s="67"/>
-      <c r="D37" s="67"/>
-      <c r="E37" s="67"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="55"/>
-      <c r="L37" s="67"/>
-      <c r="M37" s="59"/>
-      <c r="N37" s="56"/>
-    </row>
-    <row r="38" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="54"/>
-      <c r="B38" s="90" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="71"/>
-      <c r="D38" s="71"/>
-      <c r="E38" s="71"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="69"/>
-      <c r="I38" s="132" t="s">
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="57"/>
+      <c r="K39" s="57"/>
+      <c r="L39" s="69"/>
+      <c r="M39" s="61"/>
+      <c r="N39" s="58"/>
+    </row>
+    <row r="40" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="56"/>
+      <c r="B40" s="93" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="70"/>
+      <c r="J40" s="57"/>
+      <c r="K40" s="57"/>
+      <c r="L40" s="69"/>
+      <c r="M40" s="61"/>
+      <c r="N40" s="58"/>
+    </row>
+    <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="56"/>
+      <c r="B41" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="J38" s="131"/>
-      <c r="K38" s="131"/>
-      <c r="L38" s="131"/>
-      <c r="M38" s="131"/>
-      <c r="N38" s="56"/>
-    </row>
-    <row r="39" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="54"/>
-      <c r="B39" s="91" t="s">
+      <c r="C41" s="69"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="59"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="70"/>
+      <c r="J41" s="57"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="69"/>
+      <c r="M41" s="61"/>
+      <c r="N41" s="58"/>
+    </row>
+    <row r="42" spans="1:14" s="64" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="68"/>
+      <c r="B42" s="94" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="67"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="67"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="59"/>
-      <c r="I39" s="68"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="55"/>
-      <c r="L39" s="67"/>
-      <c r="M39" s="59"/>
-      <c r="N39" s="56"/>
-    </row>
-    <row r="40" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="54"/>
-      <c r="B40" s="91" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="67"/>
-      <c r="F40" s="57"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="68"/>
-      <c r="J40" s="55"/>
-      <c r="K40" s="55"/>
-      <c r="L40" s="67"/>
-      <c r="M40" s="59"/>
-      <c r="N40" s="56"/>
-    </row>
-    <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="54"/>
-      <c r="B41" s="91" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="67"/>
-      <c r="F41" s="57"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="59"/>
-      <c r="I41" s="68"/>
-      <c r="J41" s="55"/>
-      <c r="K41" s="55"/>
-      <c r="L41" s="67"/>
-      <c r="M41" s="59"/>
-      <c r="N41" s="56"/>
-    </row>
-    <row r="42" spans="1:14" s="62" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="66"/>
-      <c r="B42" s="92" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="64"/>
-      <c r="G42" s="64"/>
-      <c r="H42" s="63"/>
-      <c r="I42" s="133"/>
-      <c r="J42" s="134"/>
-      <c r="K42" s="134"/>
-      <c r="L42" s="134"/>
-      <c r="M42" s="134"/>
-      <c r="N42" s="89"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="135"/>
+      <c r="J42" s="136"/>
+      <c r="K42" s="136"/>
+      <c r="L42" s="136"/>
+      <c r="M42" s="136"/>
+      <c r="N42" s="91"/>
     </row>
     <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
minor export template fixes added
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC21CF9-6305-453A-AE4D-18CAC4D7A775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A99E0E-BC7D-4F86-832C-89CFED62CC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -870,7 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1307,6 +1307,51 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1316,6 +1361,48 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1328,98 +1415,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1485,9 +1488,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1525,7 +1528,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1631,7 +1634,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1773,7 +1776,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1786,8 +1789,8 @@
   </sheetPr>
   <dimension ref="B1:AF88"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:E11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A26" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1839,18 +1842,18 @@
       <c r="I1" s="162"/>
     </row>
     <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="194" t="s">
+      <c r="B2" s="164" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="194" t="s">
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
       <c r="J2" s="163"/>
       <c r="L2" s="11"/>
       <c r="N2" s="18"/>
@@ -1860,18 +1863,18 @@
       <c r="AD2" s="18"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="167" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="199"/>
-      <c r="F3" s="197" t="s">
+      <c r="C3" s="168"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="167" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="198"/>
-      <c r="H3" s="198"/>
-      <c r="I3" s="198"/>
+      <c r="G3" s="168"/>
+      <c r="H3" s="168"/>
+      <c r="I3" s="168"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1888,18 +1891,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="197" t="s">
+      <c r="B4" s="167" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="198"/>
-      <c r="D4" s="198"/>
-      <c r="E4" s="199"/>
-      <c r="F4" s="197" t="s">
+      <c r="C4" s="168"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="169"/>
+      <c r="F4" s="167" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="198"/>
-      <c r="H4" s="198"/>
-      <c r="I4" s="198"/>
+      <c r="G4" s="168"/>
+      <c r="H4" s="168"/>
+      <c r="I4" s="168"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1920,18 +1923,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="191" t="s">
+      <c r="B5" s="170" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="192"/>
-      <c r="D5" s="192"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="191" t="s">
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="170" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="192"/>
-      <c r="H5" s="192"/>
-      <c r="I5" s="192"/>
+      <c r="G5" s="171"/>
+      <c r="H5" s="171"/>
+      <c r="I5" s="171"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1940,18 +1943,18 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="171" t="s">
+      <c r="B6" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="172"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="171" t="s">
+      <c r="C6" s="174"/>
+      <c r="D6" s="174"/>
+      <c r="E6" s="175"/>
+      <c r="F6" s="173" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="172"/>
-      <c r="H6" s="172"/>
-      <c r="I6" s="172"/>
+      <c r="G6" s="174"/>
+      <c r="H6" s="174"/>
+      <c r="I6" s="174"/>
       <c r="J6" s="54"/>
       <c r="L6" s="55"/>
       <c r="O6" s="10"/>
@@ -1996,48 +1999,48 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="181"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="182"/>
-      <c r="F8" s="164" t="s">
+      <c r="C8" s="177"/>
+      <c r="D8" s="177"/>
+      <c r="E8" s="178"/>
+      <c r="F8" s="179" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="165"/>
-      <c r="H8" s="165"/>
-      <c r="I8" s="165"/>
+      <c r="G8" s="180"/>
+      <c r="H8" s="180"/>
+      <c r="I8" s="180"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="164" t="s">
+      <c r="B9" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="165"/>
-      <c r="D9" s="165"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="164" t="s">
+      <c r="C9" s="180"/>
+      <c r="D9" s="180"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="165"/>
-      <c r="H9" s="165"/>
-      <c r="I9" s="165"/>
+      <c r="G9" s="180"/>
+      <c r="H9" s="180"/>
+      <c r="I9" s="180"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="164" t="s">
+      <c r="B10" s="179" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="166"/>
-      <c r="F10" s="164" t="s">
+      <c r="C10" s="180"/>
+      <c r="D10" s="180"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="179" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="165"/>
-      <c r="H10" s="165"/>
-      <c r="I10" s="165"/>
+      <c r="G10" s="180"/>
+      <c r="H10" s="180"/>
+      <c r="I10" s="180"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -2058,18 +2061,18 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="171" t="s">
+      <c r="B11" s="173" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="172"/>
-      <c r="D11" s="172"/>
-      <c r="E11" s="173"/>
-      <c r="F11" s="171" t="s">
+      <c r="C11" s="174"/>
+      <c r="D11" s="174"/>
+      <c r="E11" s="175"/>
+      <c r="F11" s="173" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="172"/>
-      <c r="H11" s="172"/>
-      <c r="I11" s="172"/>
+      <c r="G11" s="174"/>
+      <c r="H11" s="174"/>
+      <c r="I11" s="174"/>
       <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -2112,18 +2115,18 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="164" t="s">
+      <c r="B13" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="165"/>
-      <c r="E13" s="166"/>
-      <c r="F13" s="164" t="s">
+      <c r="C13" s="180"/>
+      <c r="D13" s="180"/>
+      <c r="E13" s="181"/>
+      <c r="F13" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="165"/>
-      <c r="H13" s="165"/>
-      <c r="I13" s="165"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2141,18 +2144,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="165"/>
-      <c r="E14" s="166"/>
-      <c r="F14" s="164" t="s">
+      <c r="C14" s="180"/>
+      <c r="D14" s="180"/>
+      <c r="E14" s="181"/>
+      <c r="F14" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="165"/>
-      <c r="H14" s="165"/>
-      <c r="I14" s="165"/>
+      <c r="G14" s="180"/>
+      <c r="H14" s="180"/>
+      <c r="I14" s="180"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2170,18 +2173,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="164" t="s">
+      <c r="B15" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="165"/>
-      <c r="E15" s="166"/>
-      <c r="F15" s="164" t="s">
+      <c r="C15" s="180"/>
+      <c r="D15" s="180"/>
+      <c r="E15" s="181"/>
+      <c r="F15" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="165"/>
-      <c r="H15" s="165"/>
-      <c r="I15" s="165"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="180"/>
+      <c r="I15" s="180"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2199,18 +2202,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="183" t="s">
+      <c r="B16" s="182" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="184"/>
-      <c r="D16" s="184"/>
+      <c r="C16" s="183"/>
+      <c r="D16" s="183"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="183" t="s">
+      <c r="F16" s="182" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="184"/>
-      <c r="H16" s="184"/>
-      <c r="I16" s="185"/>
+      <c r="G16" s="183"/>
+      <c r="H16" s="183"/>
+      <c r="I16" s="184"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2228,18 +2231,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="164" t="s">
+      <c r="B17" s="179" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="186"/>
-      <c r="D17" s="186"/>
-      <c r="E17" s="187"/>
-      <c r="F17" s="188" t="s">
+      <c r="C17" s="185"/>
+      <c r="D17" s="185"/>
+      <c r="E17" s="186"/>
+      <c r="F17" s="187" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="186"/>
-      <c r="H17" s="186"/>
-      <c r="I17" s="186"/>
+      <c r="G17" s="185"/>
+      <c r="H17" s="185"/>
+      <c r="I17" s="185"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2257,18 +2260,18 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="189" t="s">
+      <c r="B18" s="188" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="190"/>
+      <c r="C18" s="189"/>
       <c r="D18" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="190" t="s">
+      <c r="E18" s="189" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="190"/>
-      <c r="G18" s="190"/>
+      <c r="F18" s="189"/>
+      <c r="G18" s="189"/>
       <c r="H18" s="23" t="s">
         <v>80</v>
       </c>
@@ -2292,18 +2295,18 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="174" t="s">
+      <c r="B19" s="190" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="175"/>
+      <c r="C19" s="191"/>
       <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="176" t="s">
+      <c r="E19" s="192" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="176"/>
-      <c r="G19" s="176"/>
+      <c r="F19" s="192"/>
+      <c r="G19" s="192"/>
       <c r="H19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2452,18 +2455,18 @@
       <c r="AD24" s="10"/>
     </row>
     <row r="25" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="177" t="s">
+      <c r="B25" s="193" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="178"/>
-      <c r="D25" s="178"/>
-      <c r="E25" s="179"/>
-      <c r="F25" s="177" t="s">
+      <c r="C25" s="194"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="195"/>
+      <c r="F25" s="193" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="178"/>
-      <c r="H25" s="178"/>
-      <c r="I25" s="178"/>
+      <c r="G25" s="194"/>
+      <c r="H25" s="194"/>
+      <c r="I25" s="194"/>
       <c r="J25" s="22"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
@@ -2484,48 +2487,48 @@
       <c r="AD25" s="10"/>
     </row>
     <row r="26" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="164" t="s">
+      <c r="B26" s="179" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="165"/>
-      <c r="D26" s="165"/>
-      <c r="E26" s="166"/>
-      <c r="F26" s="164" t="s">
+      <c r="C26" s="180"/>
+      <c r="D26" s="180"/>
+      <c r="E26" s="181"/>
+      <c r="F26" s="179" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="165"/>
-      <c r="H26" s="165"/>
-      <c r="I26" s="165"/>
+      <c r="G26" s="180"/>
+      <c r="H26" s="180"/>
+      <c r="I26" s="180"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="180" t="s">
+      <c r="B27" s="176" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="181"/>
-      <c r="D27" s="181"/>
-      <c r="E27" s="182"/>
-      <c r="F27" s="164" t="s">
+      <c r="C27" s="177"/>
+      <c r="D27" s="177"/>
+      <c r="E27" s="178"/>
+      <c r="F27" s="179" t="s">
         <v>85</v>
       </c>
-      <c r="G27" s="165"/>
-      <c r="H27" s="165"/>
-      <c r="I27" s="166"/>
+      <c r="G27" s="180"/>
+      <c r="H27" s="180"/>
+      <c r="I27" s="181"/>
       <c r="J27" s="19"/>
     </row>
     <row r="28" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="171" t="s">
+      <c r="B28" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="172"/>
-      <c r="D28" s="172"/>
+      <c r="C28" s="174"/>
+      <c r="D28" s="174"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="171" t="s">
+      <c r="F28" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="172"/>
-      <c r="H28" s="172"/>
-      <c r="I28" s="173"/>
+      <c r="G28" s="174"/>
+      <c r="H28" s="174"/>
+      <c r="I28" s="175"/>
       <c r="J28" s="22"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
@@ -2546,33 +2549,33 @@
       <c r="AD28" s="10"/>
     </row>
     <row r="29" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="164" t="s">
+      <c r="B29" s="179" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="165"/>
-      <c r="D29" s="165"/>
-      <c r="E29" s="166"/>
-      <c r="F29" s="164" t="s">
+      <c r="C29" s="180"/>
+      <c r="D29" s="180"/>
+      <c r="E29" s="181"/>
+      <c r="F29" s="179" t="s">
         <v>37</v>
       </c>
-      <c r="G29" s="165"/>
-      <c r="H29" s="165"/>
-      <c r="I29" s="165"/>
+      <c r="G29" s="180"/>
+      <c r="H29" s="180"/>
+      <c r="I29" s="180"/>
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="171" t="s">
+      <c r="B30" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="172"/>
-      <c r="D30" s="172"/>
+      <c r="C30" s="174"/>
+      <c r="D30" s="174"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="171" t="s">
+      <c r="F30" s="173" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="172"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="173"/>
+      <c r="G30" s="174"/>
+      <c r="H30" s="174"/>
+      <c r="I30" s="175"/>
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -2591,18 +2594,18 @@
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="167" t="s">
+      <c r="B32" s="196" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="168"/>
-      <c r="D32" s="168"/>
-      <c r="E32" s="169"/>
-      <c r="F32" s="167" t="s">
+      <c r="C32" s="197"/>
+      <c r="D32" s="197"/>
+      <c r="E32" s="198"/>
+      <c r="F32" s="196" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="168"/>
-      <c r="H32" s="168"/>
-      <c r="I32" s="168"/>
+      <c r="G32" s="197"/>
+      <c r="H32" s="197"/>
+      <c r="I32" s="197"/>
       <c r="J32" s="34"/>
       <c r="N32" s="36"/>
       <c r="O32" s="36"/>
@@ -2623,93 +2626,93 @@
       <c r="AD32" s="36"/>
     </row>
     <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="164" t="s">
+      <c r="B33" s="179" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="165"/>
-      <c r="D33" s="165"/>
-      <c r="E33" s="166"/>
-      <c r="F33" s="164" t="s">
+      <c r="C33" s="180"/>
+      <c r="D33" s="180"/>
+      <c r="E33" s="181"/>
+      <c r="F33" s="179" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="165"/>
-      <c r="H33" s="165"/>
-      <c r="I33" s="165"/>
+      <c r="G33" s="180"/>
+      <c r="H33" s="180"/>
+      <c r="I33" s="180"/>
       <c r="J33" s="19"/>
     </row>
     <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="164" t="s">
+      <c r="B34" s="179" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="165"/>
-      <c r="D34" s="165"/>
-      <c r="E34" s="166"/>
-      <c r="F34" s="164" t="s">
+      <c r="C34" s="180"/>
+      <c r="D34" s="180"/>
+      <c r="E34" s="181"/>
+      <c r="F34" s="179" t="s">
         <v>42</v>
       </c>
-      <c r="G34" s="165"/>
-      <c r="H34" s="165"/>
-      <c r="I34" s="165"/>
+      <c r="G34" s="180"/>
+      <c r="H34" s="180"/>
+      <c r="I34" s="180"/>
       <c r="J34" s="19"/>
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="164" t="s">
+      <c r="B35" s="179" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="165"/>
-      <c r="D35" s="165"/>
-      <c r="E35" s="166"/>
-      <c r="F35" s="164" t="s">
+      <c r="C35" s="180"/>
+      <c r="D35" s="180"/>
+      <c r="E35" s="181"/>
+      <c r="F35" s="179" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="165"/>
-      <c r="H35" s="165"/>
-      <c r="I35" s="165"/>
+      <c r="G35" s="180"/>
+      <c r="H35" s="180"/>
+      <c r="I35" s="180"/>
       <c r="J35" s="19"/>
     </row>
     <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="164" t="s">
+      <c r="B36" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="165"/>
-      <c r="D36" s="165"/>
-      <c r="E36" s="166"/>
-      <c r="F36" s="164" t="s">
+      <c r="C36" s="180"/>
+      <c r="D36" s="180"/>
+      <c r="E36" s="181"/>
+      <c r="F36" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="165"/>
-      <c r="H36" s="165"/>
-      <c r="I36" s="165"/>
+      <c r="G36" s="180"/>
+      <c r="H36" s="180"/>
+      <c r="I36" s="180"/>
       <c r="J36" s="19"/>
     </row>
     <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="164" t="s">
+      <c r="B37" s="179" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="165"/>
-      <c r="D37" s="165"/>
-      <c r="E37" s="166"/>
-      <c r="F37" s="164" t="s">
+      <c r="C37" s="180"/>
+      <c r="D37" s="180"/>
+      <c r="E37" s="181"/>
+      <c r="F37" s="179" t="s">
         <v>46</v>
       </c>
-      <c r="G37" s="165"/>
-      <c r="H37" s="165"/>
-      <c r="I37" s="165"/>
+      <c r="G37" s="180"/>
+      <c r="H37" s="180"/>
+      <c r="I37" s="180"/>
       <c r="J37" s="19"/>
     </row>
     <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="164" t="s">
+      <c r="B38" s="179" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="165"/>
-      <c r="D38" s="165"/>
-      <c r="E38" s="166"/>
-      <c r="F38" s="164" t="s">
+      <c r="C38" s="180"/>
+      <c r="D38" s="180"/>
+      <c r="E38" s="181"/>
+      <c r="F38" s="179" t="s">
         <v>48</v>
       </c>
-      <c r="G38" s="165"/>
-      <c r="H38" s="165"/>
-      <c r="I38" s="165"/>
+      <c r="G38" s="180"/>
+      <c r="H38" s="180"/>
+      <c r="I38" s="180"/>
       <c r="J38" s="19"/>
     </row>
     <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2728,18 +2731,18 @@
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="167" t="s">
+      <c r="B40" s="196" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="168"/>
-      <c r="D40" s="168"/>
-      <c r="E40" s="169"/>
-      <c r="F40" s="167" t="s">
+      <c r="C40" s="197"/>
+      <c r="D40" s="197"/>
+      <c r="E40" s="198"/>
+      <c r="F40" s="196" t="s">
         <v>14</v>
       </c>
-      <c r="G40" s="170"/>
-      <c r="H40" s="170"/>
-      <c r="I40" s="170"/>
+      <c r="G40" s="199"/>
+      <c r="H40" s="199"/>
+      <c r="I40" s="199"/>
       <c r="J40" s="34"/>
       <c r="N40" s="36"/>
       <c r="O40" s="36"/>
@@ -2760,18 +2763,18 @@
       <c r="AD40" s="36"/>
     </row>
     <row r="41" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="164" t="s">
+      <c r="B41" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="165"/>
-      <c r="D41" s="165"/>
-      <c r="E41" s="166"/>
-      <c r="F41" s="164" t="s">
+      <c r="C41" s="180"/>
+      <c r="D41" s="180"/>
+      <c r="E41" s="181"/>
+      <c r="F41" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="G41" s="165"/>
-      <c r="H41" s="165"/>
-      <c r="I41" s="165"/>
+      <c r="G41" s="180"/>
+      <c r="H41" s="180"/>
+      <c r="I41" s="180"/>
       <c r="J41" s="19"/>
     </row>
     <row r="42" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2830,19 +2833,19 @@
       <c r="I45" s="38"/>
       <c r="J45" s="19"/>
     </row>
-    <row r="46" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="27" t="s">
+    <row r="46" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="179" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="27" t="s">
+      <c r="C46" s="202"/>
+      <c r="D46" s="202"/>
+      <c r="E46" s="181"/>
+      <c r="F46" s="179" t="s">
         <v>52</v>
       </c>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
+      <c r="G46" s="202"/>
+      <c r="H46" s="202"/>
+      <c r="I46" s="181"/>
       <c r="J46" s="19"/>
     </row>
     <row r="47" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3060,37 +3063,27 @@
     <row r="81" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="88" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:G18"/>
+  <mergeCells count="64">
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="B19:C19"/>
@@ -3105,24 +3098,36 @@
     <mergeCell ref="F28:I28"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="notContainsBlanks" dxfId="3" priority="2">
@@ -3161,7 +3166,7 @@
   </sheetPr>
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed export contract tmp fields with face podpisant and org form + certificates exw field remove
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A99E0E-BC7D-4F86-832C-89CFED62CC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024EE776-F747-44D4-ADF4-1638BB5C3160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="2287" yWindow="3278" windowWidth="13425" windowHeight="7784" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -81,6 +81,7 @@
     <definedName name="Продавец_подписант">Export_Contract!$B$10</definedName>
     <definedName name="Продавец_представитель">Export_Contract!$B$9</definedName>
     <definedName name="Прочие_условия_описание">Export_Contract!$B$29</definedName>
+    <definedName name="Сертификаты_обязательства">Export_Contract!$B$27</definedName>
     <definedName name="Соглашение">Export_Contract!$B$2</definedName>
     <definedName name="Цена_всего">Export_Contract!$B$23</definedName>
   </definedNames>
@@ -105,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="141">
   <si>
     <t>Дополнительное соглашение № 146 от 10 марта 2023г.</t>
   </si>
@@ -141,12 +142,6 @@
   </si>
   <si>
     <t xml:space="preserve">В лице и.о. генерального директора </t>
-  </si>
-  <si>
-    <t>N.M. Kotov and</t>
-  </si>
-  <si>
-    <t>Котова Н.М. и</t>
   </si>
   <si>
     <t>KTI COMPANY LIMITED</t>
@@ -1789,8 +1784,8 @@
   </sheetPr>
   <dimension ref="B1:AF88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A26" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1834,7 +1829,7 @@
       <c r="C1" s="162"/>
       <c r="D1" s="162"/>
       <c r="E1" s="162" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F1" s="162"/>
       <c r="G1" s="162"/>
@@ -1843,7 +1838,7 @@
     </row>
     <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="164" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2" s="165"/>
       <c r="D2" s="165"/>
@@ -1944,13 +1939,13 @@
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="173" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" s="174"/>
       <c r="D6" s="174"/>
       <c r="E6" s="175"/>
       <c r="F6" s="173" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G6" s="174"/>
       <c r="H6" s="174"/>
@@ -1972,7 +1967,7 @@
     </row>
     <row r="7" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
@@ -2017,30 +2012,26 @@
       <c r="B9" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="180"/>
-      <c r="D9" s="180"/>
+      <c r="C9" s="202"/>
+      <c r="D9" s="202"/>
       <c r="E9" s="181"/>
       <c r="F9" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="180"/>
-      <c r="H9" s="180"/>
-      <c r="I9" s="180"/>
+      <c r="G9" s="202"/>
+      <c r="H9" s="202"/>
+      <c r="I9" s="181"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="179" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="180"/>
+      <c r="B10" s="179"/>
+      <c r="C10" s="202"/>
+      <c r="D10" s="202"/>
       <c r="E10" s="181"/>
-      <c r="F10" s="179" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="180"/>
-      <c r="H10" s="180"/>
-      <c r="I10" s="180"/>
+      <c r="F10" s="179"/>
+      <c r="G10" s="202"/>
+      <c r="H10" s="202"/>
+      <c r="I10" s="181"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -2062,13 +2053,13 @@
     </row>
     <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="173" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" s="174"/>
       <c r="D11" s="174"/>
       <c r="E11" s="175"/>
       <c r="F11" s="173" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G11" s="174"/>
       <c r="H11" s="174"/>
@@ -2089,13 +2080,13 @@
     </row>
     <row r="12" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="51"/>
       <c r="F12" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="52"/>
@@ -2116,13 +2107,13 @@
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="179" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" s="180"/>
       <c r="D13" s="180"/>
       <c r="E13" s="181"/>
       <c r="F13" s="179" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G13" s="180"/>
       <c r="H13" s="180"/>
@@ -2145,13 +2136,13 @@
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="179" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="180"/>
       <c r="D14" s="180"/>
       <c r="E14" s="181"/>
       <c r="F14" s="179" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G14" s="180"/>
       <c r="H14" s="180"/>
@@ -2174,13 +2165,13 @@
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="179" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" s="180"/>
       <c r="D15" s="180"/>
       <c r="E15" s="181"/>
       <c r="F15" s="179" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G15" s="180"/>
       <c r="H15" s="180"/>
@@ -2203,13 +2194,13 @@
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="182" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" s="183"/>
       <c r="D16" s="183"/>
       <c r="E16" s="21"/>
       <c r="F16" s="182" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G16" s="183"/>
       <c r="H16" s="183"/>
@@ -2232,13 +2223,13 @@
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="179" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C17" s="185"/>
       <c r="D17" s="185"/>
       <c r="E17" s="186"/>
       <c r="F17" s="187" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G17" s="185"/>
       <c r="H17" s="185"/>
@@ -2261,22 +2252,22 @@
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="188" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" s="189"/>
       <c r="D18" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E18" s="189" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F18" s="189"/>
       <c r="G18" s="189"/>
       <c r="H18" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J18" s="24"/>
       <c r="N18" s="10"/>
@@ -2296,22 +2287,22 @@
     </row>
     <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="190" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" s="191"/>
       <c r="D19" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E19" s="192" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F19" s="192"/>
       <c r="G19" s="192"/>
       <c r="H19" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J19" s="2"/>
       <c r="N19" s="10"/>
@@ -2362,13 +2353,13 @@
     </row>
     <row r="21" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="5"/>
       <c r="F21" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="26"/>
@@ -2394,13 +2385,13 @@
     </row>
     <row r="22" spans="2:30" s="30" customFormat="1" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
       <c r="E22" s="29"/>
       <c r="F22" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
@@ -2409,13 +2400,13 @@
     </row>
     <row r="23" spans="2:30" s="30" customFormat="1" ht="23.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
       <c r="E23" s="21"/>
       <c r="F23" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -2424,13 +2415,13 @@
     </row>
     <row r="24" spans="2:30" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="32"/>
       <c r="F24" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="33"/>
@@ -2456,13 +2447,13 @@
     </row>
     <row r="25" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="193" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" s="194"/>
       <c r="D25" s="194"/>
       <c r="E25" s="195"/>
       <c r="F25" s="193" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G25" s="194"/>
       <c r="H25" s="194"/>
@@ -2488,13 +2479,13 @@
     </row>
     <row r="26" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="179" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C26" s="180"/>
       <c r="D26" s="180"/>
       <c r="E26" s="181"/>
       <c r="F26" s="179" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G26" s="180"/>
       <c r="H26" s="180"/>
@@ -2503,13 +2494,13 @@
     </row>
     <row r="27" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="176" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C27" s="177"/>
       <c r="D27" s="177"/>
       <c r="E27" s="178"/>
       <c r="F27" s="179" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G27" s="180"/>
       <c r="H27" s="180"/>
@@ -2518,13 +2509,13 @@
     </row>
     <row r="28" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="173" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C28" s="174"/>
       <c r="D28" s="174"/>
       <c r="E28" s="32"/>
       <c r="F28" s="173" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G28" s="174"/>
       <c r="H28" s="174"/>
@@ -2550,13 +2541,13 @@
     </row>
     <row r="29" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B29" s="179" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29" s="180"/>
       <c r="D29" s="180"/>
       <c r="E29" s="181"/>
       <c r="F29" s="179" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G29" s="180"/>
       <c r="H29" s="180"/>
@@ -2565,13 +2556,13 @@
     </row>
     <row r="30" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B30" s="173" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="174"/>
       <c r="D30" s="174"/>
       <c r="E30" s="21"/>
       <c r="F30" s="173" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G30" s="174"/>
       <c r="H30" s="174"/>
@@ -2580,13 +2571,13 @@
     </row>
     <row r="31" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="21"/>
       <c r="F31" s="50" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
@@ -2595,7 +2586,7 @@
     </row>
     <row r="32" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="196" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C32" s="197"/>
       <c r="D32" s="197"/>
@@ -2627,7 +2618,7 @@
     </row>
     <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="179" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" s="180"/>
       <c r="D33" s="180"/>
@@ -2642,13 +2633,13 @@
     </row>
     <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="179" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" s="180"/>
       <c r="D34" s="180"/>
       <c r="E34" s="181"/>
       <c r="F34" s="179" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G34" s="180"/>
       <c r="H34" s="180"/>
@@ -2657,13 +2648,13 @@
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B35" s="179" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C35" s="180"/>
       <c r="D35" s="180"/>
       <c r="E35" s="181"/>
       <c r="F35" s="179" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G35" s="180"/>
       <c r="H35" s="180"/>
@@ -2672,13 +2663,13 @@
     </row>
     <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="179" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C36" s="180"/>
       <c r="D36" s="180"/>
       <c r="E36" s="181"/>
       <c r="F36" s="179" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G36" s="180"/>
       <c r="H36" s="180"/>
@@ -2687,13 +2678,13 @@
     </row>
     <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="179" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C37" s="180"/>
       <c r="D37" s="180"/>
       <c r="E37" s="181"/>
       <c r="F37" s="179" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G37" s="180"/>
       <c r="H37" s="180"/>
@@ -2702,13 +2693,13 @@
     </row>
     <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B38" s="179" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C38" s="180"/>
       <c r="D38" s="180"/>
       <c r="E38" s="181"/>
       <c r="F38" s="179" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G38" s="180"/>
       <c r="H38" s="180"/>
@@ -2717,13 +2708,13 @@
     </row>
     <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B39" s="62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C39" s="20"/>
       <c r="D39" s="20"/>
       <c r="E39" s="21"/>
       <c r="F39" s="62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
@@ -2732,13 +2723,13 @@
     </row>
     <row r="40" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B40" s="196" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C40" s="197"/>
       <c r="D40" s="197"/>
       <c r="E40" s="198"/>
       <c r="F40" s="196" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G40" s="199"/>
       <c r="H40" s="199"/>
@@ -2764,13 +2755,13 @@
     </row>
     <row r="41" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B41" s="179" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C41" s="180"/>
       <c r="D41" s="180"/>
       <c r="E41" s="181"/>
       <c r="F41" s="179" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G41" s="180"/>
       <c r="H41" s="180"/>
@@ -2784,7 +2775,7 @@
       <c r="E42" s="21"/>
       <c r="F42" s="19"/>
       <c r="G42" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
@@ -2792,13 +2783,13 @@
     </row>
     <row r="43" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B43" s="27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="37"/>
       <c r="F43" s="27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G43" s="28"/>
       <c r="H43" s="38"/>
@@ -2808,7 +2799,7 @@
     <row r="44" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B44" s="39"/>
       <c r="C44" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D44" s="31"/>
       <c r="E44" s="21"/>
@@ -2820,13 +2811,13 @@
     </row>
     <row r="45" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B45" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C45" s="28"/>
       <c r="D45" s="28"/>
       <c r="E45" s="37"/>
       <c r="F45" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G45" s="38"/>
       <c r="H45" s="38"/>
@@ -2835,28 +2826,28 @@
     </row>
     <row r="46" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B46" s="179" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" s="202"/>
-      <c r="D46" s="202"/>
+        <v>50</v>
+      </c>
+      <c r="C46" s="180"/>
+      <c r="D46" s="180"/>
       <c r="E46" s="181"/>
       <c r="F46" s="179" t="s">
-        <v>52</v>
-      </c>
-      <c r="G46" s="202"/>
-      <c r="H46" s="202"/>
+        <v>50</v>
+      </c>
+      <c r="G46" s="180"/>
+      <c r="H46" s="180"/>
       <c r="I46" s="181"/>
       <c r="J46" s="19"/>
     </row>
     <row r="47" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B47" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C47" s="28"/>
       <c r="D47" s="28"/>
       <c r="E47" s="29"/>
       <c r="F47" s="28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G47" s="38"/>
       <c r="H47" s="38"/>
@@ -2865,13 +2856,13 @@
     </row>
     <row r="48" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C48" s="28"/>
       <c r="D48" s="28"/>
       <c r="E48" s="29"/>
       <c r="F48" s="28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G48" s="38"/>
       <c r="H48" s="38"/>
@@ -2880,13 +2871,13 @@
     </row>
     <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C49" s="28"/>
       <c r="D49" s="28"/>
       <c r="E49" s="29"/>
       <c r="F49" s="28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
@@ -2896,13 +2887,13 @@
     <row r="50" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50" s="19"/>
       <c r="C50" s="36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D50" s="31"/>
       <c r="E50" s="21"/>
       <c r="F50" s="31"/>
       <c r="G50" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H50" s="31"/>
       <c r="I50" s="31"/>
@@ -2910,13 +2901,13 @@
     </row>
     <row r="51" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B51" s="40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C51" s="41"/>
       <c r="D51" s="41"/>
       <c r="E51" s="42"/>
       <c r="F51" s="41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G51" s="41"/>
       <c r="H51" s="41"/>
@@ -2926,16 +2917,16 @@
     <row r="52" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="43"/>
       <c r="C52" s="44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D52" s="45"/>
       <c r="E52" s="46"/>
       <c r="F52" s="47"/>
       <c r="G52" s="44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H52" s="44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I52" s="46"/>
       <c r="J52" s="15"/>
@@ -3063,19 +3054,13 @@
     <row r="81" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="88" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="64">
+  <mergeCells count="62">
     <mergeCell ref="B46:E46"/>
     <mergeCell ref="F46:I46"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="F35:I35"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
     <mergeCell ref="B41:E41"/>
     <mergeCell ref="F41:I41"/>
     <mergeCell ref="B36:E36"/>
@@ -3084,6 +3069,12 @@
     <mergeCell ref="F37:I37"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="F38:I38"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="B19:C19"/>
@@ -3110,12 +3101,10 @@
     <mergeCell ref="F14:I14"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:I10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="F11:I11"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="F9:I10"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="B6:E6"/>
@@ -3166,7 +3155,7 @@
   </sheetPr>
   <dimension ref="A1:AC52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -3192,14 +3181,14 @@
     <row r="1" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="56"/>
       <c r="G1" s="161" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N1" s="58"/>
     </row>
     <row r="2" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="89"/>
       <c r="B2" s="119" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C2" s="119"/>
       <c r="D2" s="119"/>
@@ -3207,7 +3196,7 @@
       <c r="F2" s="119"/>
       <c r="G2" s="119"/>
       <c r="H2" s="122" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I2" s="119"/>
       <c r="J2" s="119"/>
@@ -3219,7 +3208,7 @@
     <row r="3" spans="1:14" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="89"/>
       <c r="B3" s="120" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C3" s="120"/>
       <c r="D3" s="120"/>
@@ -3227,7 +3216,7 @@
       <c r="F3" s="121"/>
       <c r="G3" s="121"/>
       <c r="H3" s="123" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I3" s="120"/>
       <c r="J3" s="120"/>
@@ -3239,7 +3228,7 @@
     <row r="4" spans="1:14" s="86" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="88"/>
       <c r="B4" s="120" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" s="120"/>
       <c r="D4" s="120"/>
@@ -3247,7 +3236,7 @@
       <c r="F4" s="120"/>
       <c r="G4" s="120"/>
       <c r="H4" s="123" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I4" s="120"/>
       <c r="J4" s="120"/>
@@ -3259,7 +3248,7 @@
     <row r="5" spans="1:14" s="86" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="87"/>
       <c r="B5" s="120" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C5" s="120"/>
       <c r="D5" s="120"/>
@@ -3267,7 +3256,7 @@
       <c r="F5" s="120"/>
       <c r="G5" s="120"/>
       <c r="H5" s="123" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I5" s="120"/>
       <c r="J5" s="120"/>
@@ -3279,7 +3268,7 @@
     <row r="6" spans="1:14" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="56"/>
       <c r="B6" s="110" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C6" s="110"/>
       <c r="D6" s="110"/>
@@ -3287,7 +3276,7 @@
       <c r="F6" s="110"/>
       <c r="G6" s="110"/>
       <c r="H6" s="96" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I6" s="97"/>
       <c r="J6" s="97"/>
@@ -3299,7 +3288,7 @@
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="56"/>
       <c r="B7" s="113" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="124"/>
       <c r="D7" s="124"/>
@@ -3339,7 +3328,7 @@
     <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="56"/>
       <c r="B9" s="126" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" s="126"/>
       <c r="D9" s="126"/>
@@ -3347,7 +3336,7 @@
       <c r="F9" s="126"/>
       <c r="G9" s="126"/>
       <c r="H9" s="103" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I9" s="98"/>
       <c r="J9" s="98"/>
@@ -3359,7 +3348,7 @@
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="56"/>
       <c r="B10" s="113" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" s="113"/>
       <c r="D10" s="113"/>
@@ -3367,7 +3356,7 @@
       <c r="F10" s="113"/>
       <c r="G10" s="113"/>
       <c r="H10" s="99" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I10" s="98"/>
       <c r="J10" s="98"/>
@@ -3379,7 +3368,7 @@
     <row r="11" spans="1:14" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="56"/>
       <c r="B11" s="102" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="102"/>
       <c r="D11" s="102"/>
@@ -3387,7 +3376,7 @@
       <c r="F11" s="102"/>
       <c r="G11" s="118"/>
       <c r="H11" s="155" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I11" s="102"/>
       <c r="J11" s="102"/>
@@ -3399,7 +3388,7 @@
     <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="56"/>
       <c r="B12" s="126" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C12" s="126"/>
       <c r="D12" s="126"/>
@@ -3407,7 +3396,7 @@
       <c r="F12" s="126"/>
       <c r="G12" s="126"/>
       <c r="H12" s="96" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I12" s="97"/>
       <c r="J12" s="97"/>
@@ -3419,7 +3408,7 @@
     <row r="13" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="56"/>
       <c r="B13" s="113" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="113"/>
       <c r="D13" s="113"/>
@@ -3427,7 +3416,7 @@
       <c r="F13" s="113"/>
       <c r="G13" s="113"/>
       <c r="H13" s="99" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I13" s="100"/>
       <c r="J13" s="100"/>
@@ -3439,7 +3428,7 @@
     <row r="14" spans="1:14" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="56"/>
       <c r="B14" s="102" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="102"/>
       <c r="D14" s="102"/>
@@ -3447,7 +3436,7 @@
       <c r="F14" s="102"/>
       <c r="G14" s="118"/>
       <c r="H14" s="155" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I14" s="102"/>
       <c r="J14" s="102"/>
@@ -3459,27 +3448,27 @@
     <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="85"/>
       <c r="B15" s="104" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C15" s="104"/>
       <c r="D15" s="105" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E15" s="105"/>
       <c r="F15" s="105" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G15" s="105"/>
       <c r="H15" s="106" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I15" s="105"/>
       <c r="J15" s="127" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K15" s="127"/>
       <c r="L15" s="151" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M15" s="151"/>
       <c r="N15" s="58"/>
@@ -3487,27 +3476,27 @@
     <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="56"/>
       <c r="B16" s="118" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C16" s="107"/>
       <c r="D16" s="156" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E16" s="108"/>
       <c r="F16" s="144" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G16" s="108"/>
       <c r="H16" s="159" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I16" s="108"/>
       <c r="J16" s="109" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K16" s="109"/>
       <c r="L16" s="152" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M16" s="152"/>
       <c r="N16" s="58"/>
@@ -3515,27 +3504,27 @@
     <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="56"/>
       <c r="B17" s="126" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C17" s="126"/>
       <c r="D17" s="126" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E17" s="130"/>
       <c r="F17" s="143" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G17" s="143"/>
       <c r="H17" s="103" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I17" s="98"/>
       <c r="J17" s="111" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K17" s="98"/>
       <c r="L17" s="153" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M17" s="154"/>
       <c r="N17" s="58"/>
@@ -3543,27 +3532,27 @@
     <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="56"/>
       <c r="B18" s="102" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C18" s="125"/>
       <c r="D18" s="157" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E18" s="109"/>
       <c r="F18" s="158" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G18" s="144"/>
       <c r="H18" s="159" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I18" s="109"/>
       <c r="J18" s="157" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K18" s="109"/>
       <c r="L18" s="152" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M18" s="152"/>
       <c r="N18" s="58"/>
@@ -3571,21 +3560,21 @@
     <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="56"/>
       <c r="B19" s="131" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C19" s="131"/>
       <c r="D19" s="131" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E19" s="131"/>
       <c r="F19" s="145"/>
       <c r="G19" s="145"/>
       <c r="H19" s="148" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I19" s="128"/>
       <c r="J19" s="126" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K19" s="126"/>
       <c r="L19" s="126"/>
@@ -3595,21 +3584,21 @@
     <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="56"/>
       <c r="B20" s="156" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" s="112"/>
       <c r="D20" s="129" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E20" s="129"/>
       <c r="F20" s="146"/>
       <c r="G20" s="146"/>
       <c r="H20" s="160" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I20" s="108"/>
       <c r="J20" s="113" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K20" s="114"/>
       <c r="L20" s="109"/>
@@ -3646,60 +3635,60 @@
     <row r="22" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="56"/>
       <c r="B22" s="60" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C22" s="132" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D22" s="132"/>
       <c r="E22" s="132"/>
       <c r="F22" s="150"/>
       <c r="G22" s="132"/>
       <c r="H22" s="60" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I22" s="81" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J22" s="80" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K22" s="132" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L22" s="132"/>
       <c r="M22" s="60" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N22" s="58"/>
     </row>
     <row r="23" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="56"/>
       <c r="B23" s="139" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C23" s="200" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D23" s="200"/>
       <c r="E23" s="200"/>
       <c r="F23" s="200"/>
       <c r="G23" s="140"/>
       <c r="H23" s="141" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I23" s="79" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J23" s="78">
         <v>14</v>
       </c>
       <c r="K23" s="201" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L23" s="201"/>
       <c r="M23" s="77" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N23" s="58"/>
     </row>
@@ -3711,20 +3700,20 @@
       <c r="F24" s="137"/>
       <c r="G24" s="137"/>
       <c r="H24" s="138" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I24" s="76" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J24" s="75">
         <v>14</v>
       </c>
       <c r="K24" s="142" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L24" s="142"/>
       <c r="M24" s="90" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N24" s="58"/>
     </row>
@@ -3936,7 +3925,7 @@
     <row r="38" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="56"/>
       <c r="B38" s="92" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C38" s="73"/>
       <c r="D38" s="73"/>
@@ -3945,7 +3934,7 @@
       <c r="G38" s="72"/>
       <c r="H38" s="71"/>
       <c r="I38" s="134" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J38" s="133"/>
       <c r="K38" s="133"/>
@@ -3956,7 +3945,7 @@
     <row r="39" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="56"/>
       <c r="B39" s="93" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C39" s="69"/>
       <c r="D39" s="69"/>
@@ -3974,7 +3963,7 @@
     <row r="40" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="56"/>
       <c r="B40" s="93" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C40" s="69"/>
       <c r="D40" s="69"/>
@@ -3992,7 +3981,7 @@
     <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="56"/>
       <c r="B41" s="93" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41" s="69"/>
       <c r="D41" s="69"/>
@@ -4010,7 +3999,7 @@
     <row r="42" spans="1:14" s="64" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="68"/>
       <c r="B42" s="94" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C42" s="67"/>
       <c r="D42" s="67"/>

</xml_diff>

<commit_message>
added export tmp currency support
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024EE776-F747-44D4-ADF4-1638BB5C3160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCD2417-FEBF-4046-A164-E882B01BB09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2287" yWindow="3278" windowWidth="13425" windowHeight="7784" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -19,31 +19,31 @@
   <definedNames>
     <definedName name="MID_Contract">Export_Contract!$E$1</definedName>
     <definedName name="MID_Invoice">Invoice!$G$1</definedName>
-    <definedName name="Seal_agent_end">Export_Contract!$H$52</definedName>
-    <definedName name="Seal_agent_start">Export_Contract!$G$42</definedName>
-    <definedName name="Seal_seller_end">Export_Contract!$C$52</definedName>
-    <definedName name="Seal_seller_start">Export_Contract!$C$44</definedName>
-    <definedName name="Sign_agent_end">Export_Contract!$G$52</definedName>
-    <definedName name="Sign_agent_start">Export_Contract!$G$50</definedName>
-    <definedName name="Sign_seller_start">Export_Contract!$C$50</definedName>
-    <definedName name="Адреса_банк_получателя">Export_Contract!$B$34</definedName>
-    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$35</definedName>
-    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$36</definedName>
-    <definedName name="Адреса_подпись">Export_Contract!$B$51</definedName>
-    <definedName name="Адреса_покупатель">Export_Contract!$B$40</definedName>
-    <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$41</definedName>
-    <definedName name="Адреса_покупатель_банк">Export_Contract!$B$43</definedName>
-    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$B$46</definedName>
-    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$B$45</definedName>
-    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$B$47</definedName>
-    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$B$48</definedName>
-    <definedName name="Адреса_покупатель_счет">Export_Contract!$B$49</definedName>
-    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$B$37</definedName>
-    <definedName name="Адреса_получатель_счет">Export_Contract!$B$38</definedName>
-    <definedName name="Адреса_продавец">Export_Contract!$B$32</definedName>
-    <definedName name="Адреса_продавец_адрес">Export_Contract!$B$33</definedName>
-    <definedName name="Доставка_порт">Export_Contract!$B$26</definedName>
-    <definedName name="Доставка_условия">Export_Contract!$B$25</definedName>
+    <definedName name="Seal_agent_end">Export_Contract!$H$51</definedName>
+    <definedName name="Seal_agent_start">Export_Contract!$G$41</definedName>
+    <definedName name="Seal_seller_end">Export_Contract!$C$51</definedName>
+    <definedName name="Seal_seller_start">Export_Contract!$C$43</definedName>
+    <definedName name="Sign_agent_end">Export_Contract!$G$51</definedName>
+    <definedName name="Sign_agent_start">Export_Contract!$G$49</definedName>
+    <definedName name="Sign_seller_start">Export_Contract!$C$49</definedName>
+    <definedName name="Адреса_банк_получателя">Export_Contract!$B$33</definedName>
+    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$34</definedName>
+    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$35</definedName>
+    <definedName name="Адреса_подпись">Export_Contract!$B$50</definedName>
+    <definedName name="Адреса_покупатель">Export_Contract!$B$39</definedName>
+    <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$40</definedName>
+    <definedName name="Адреса_покупатель_банк">Export_Contract!$B$42</definedName>
+    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$B$45</definedName>
+    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$B$44</definedName>
+    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$B$46</definedName>
+    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$B$47</definedName>
+    <definedName name="Адреса_покупатель_счет">Export_Contract!$B$48</definedName>
+    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$B$36</definedName>
+    <definedName name="Адреса_получатель_счет">Export_Contract!$B$37</definedName>
+    <definedName name="Адреса_продавец">Export_Contract!$B$31</definedName>
+    <definedName name="Адреса_продавец_адрес">Export_Contract!$B$32</definedName>
+    <definedName name="Доставка_порт">Export_Contract!$B$25</definedName>
+    <definedName name="Доставка_условия">Export_Contract!$B$24</definedName>
     <definedName name="Инвойс">Invoice!$B$2</definedName>
     <definedName name="Инвойс_Bl_массив">Invoice!$B$23</definedName>
     <definedName name="Инвойс_банк_получателя">Invoice!$B$38</definedName>
@@ -80,10 +80,10 @@
     <definedName name="Продавец_адрес">Export_Contract!$B$8</definedName>
     <definedName name="Продавец_подписант">Export_Contract!$B$10</definedName>
     <definedName name="Продавец_представитель">Export_Contract!$B$9</definedName>
-    <definedName name="Прочие_условия_описание">Export_Contract!$B$29</definedName>
-    <definedName name="Сертификаты_обязательства">Export_Contract!$B$27</definedName>
+    <definedName name="Прочие_условия_описание">Export_Contract!$B$28</definedName>
+    <definedName name="Сертификаты_обязательства">Export_Contract!$B$26</definedName>
     <definedName name="Соглашение">Export_Contract!$B$2</definedName>
-    <definedName name="Цена_всего">Export_Contract!$B$23</definedName>
+    <definedName name="Цена_всего">Export_Contract!$B$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="139">
   <si>
     <t>Дополнительное соглашение № 146 от 10 марта 2023г.</t>
   </si>
@@ -279,13 +279,6 @@
   </si>
   <si>
     <t>Покупатель/Buyer ________________________SE JI YOUNG</t>
-  </si>
-  <si>
-    <t>2.2. Total amount of this Agreement is specified in US dollars and is the following:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.2. Общая сумма настоящего Дополнения указана в долларах США и составляет:
-</t>
   </si>
   <si>
     <t>VLADIVOSTOK, RUSSIA</t>
@@ -865,7 +858,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1302,6 +1295,96 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1320,104 +1403,11 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1782,10 +1772,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AF88"/>
+  <dimension ref="B1:AF87"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:E10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1837,18 +1827,18 @@
       <c r="I1" s="162"/>
     </row>
     <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="164" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="164" t="s">
+      <c r="B2" s="194" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="194" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="165"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
       <c r="J2" s="163"/>
       <c r="L2" s="11"/>
       <c r="N2" s="18"/>
@@ -1858,18 +1848,18 @@
       <c r="AD2" s="18"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="167" t="s">
+      <c r="B3" s="197" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="167" t="s">
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="199"/>
+      <c r="F3" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="168"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="198"/>
+      <c r="I3" s="198"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1886,18 +1876,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="169"/>
-      <c r="F4" s="167" t="s">
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="199"/>
+      <c r="F4" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="168"/>
-      <c r="H4" s="168"/>
-      <c r="I4" s="168"/>
+      <c r="G4" s="198"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1918,18 +1908,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="170" t="s">
+      <c r="B5" s="191" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="171"/>
-      <c r="D5" s="171"/>
-      <c r="E5" s="172"/>
-      <c r="F5" s="170" t="s">
+      <c r="C5" s="192"/>
+      <c r="D5" s="192"/>
+      <c r="E5" s="193"/>
+      <c r="F5" s="191" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="171"/>
-      <c r="H5" s="171"/>
-      <c r="I5" s="171"/>
+      <c r="G5" s="192"/>
+      <c r="H5" s="192"/>
+      <c r="I5" s="192"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1938,18 +1928,18 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="173" t="s">
+      <c r="B6" s="171" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="171" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="174"/>
-      <c r="D6" s="174"/>
-      <c r="E6" s="175"/>
-      <c r="F6" s="173" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="174"/>
-      <c r="H6" s="174"/>
-      <c r="I6" s="174"/>
+      <c r="G6" s="172"/>
+      <c r="H6" s="172"/>
+      <c r="I6" s="172"/>
       <c r="J6" s="54"/>
       <c r="L6" s="55"/>
       <c r="O6" s="10"/>
@@ -1967,7 +1957,7 @@
     </row>
     <row r="7" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
@@ -1994,44 +1984,44 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="176" t="s">
+      <c r="B8" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="177"/>
-      <c r="D8" s="177"/>
-      <c r="E8" s="178"/>
-      <c r="F8" s="179" t="s">
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="164" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="180"/>
-      <c r="H8" s="180"/>
-      <c r="I8" s="180"/>
+      <c r="G8" s="165"/>
+      <c r="H8" s="165"/>
+      <c r="I8" s="165"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="179" t="s">
+      <c r="B9" s="164" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="202"/>
-      <c r="D9" s="202"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="179" t="s">
+      <c r="C9" s="165"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="164" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="202"/>
-      <c r="H9" s="202"/>
-      <c r="I9" s="181"/>
+      <c r="G9" s="165"/>
+      <c r="H9" s="165"/>
+      <c r="I9" s="166"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="179"/>
-      <c r="C10" s="202"/>
-      <c r="D10" s="202"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="179"/>
-      <c r="G10" s="202"/>
-      <c r="H10" s="202"/>
-      <c r="I10" s="181"/>
+      <c r="B10" s="164"/>
+      <c r="C10" s="165"/>
+      <c r="D10" s="165"/>
+      <c r="E10" s="166"/>
+      <c r="F10" s="164"/>
+      <c r="G10" s="165"/>
+      <c r="H10" s="165"/>
+      <c r="I10" s="166"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -2052,18 +2042,18 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="173" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="174"/>
-      <c r="D11" s="174"/>
-      <c r="E11" s="175"/>
-      <c r="F11" s="173" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="174"/>
-      <c r="H11" s="174"/>
-      <c r="I11" s="174"/>
+      <c r="B11" s="171" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="172"/>
+      <c r="D11" s="172"/>
+      <c r="E11" s="173"/>
+      <c r="F11" s="171" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="172"/>
+      <c r="H11" s="172"/>
+      <c r="I11" s="172"/>
       <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -2106,18 +2096,18 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="179" t="s">
+      <c r="B13" s="164" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="180"/>
-      <c r="D13" s="180"/>
-      <c r="E13" s="181"/>
-      <c r="F13" s="179" t="s">
+      <c r="C13" s="165"/>
+      <c r="D13" s="165"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="164" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="180"/>
-      <c r="H13" s="180"/>
-      <c r="I13" s="180"/>
+      <c r="G13" s="165"/>
+      <c r="H13" s="165"/>
+      <c r="I13" s="165"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2135,18 +2125,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="179" t="s">
+      <c r="B14" s="164" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="180"/>
-      <c r="D14" s="180"/>
-      <c r="E14" s="181"/>
-      <c r="F14" s="179" t="s">
+      <c r="C14" s="165"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="164" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="180"/>
-      <c r="H14" s="180"/>
-      <c r="I14" s="180"/>
+      <c r="G14" s="165"/>
+      <c r="H14" s="165"/>
+      <c r="I14" s="165"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2164,18 +2154,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="179" t="s">
+      <c r="B15" s="164" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="180"/>
-      <c r="D15" s="180"/>
-      <c r="E15" s="181"/>
-      <c r="F15" s="179" t="s">
+      <c r="C15" s="165"/>
+      <c r="D15" s="165"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="180"/>
-      <c r="H15" s="180"/>
-      <c r="I15" s="180"/>
+      <c r="G15" s="165"/>
+      <c r="H15" s="165"/>
+      <c r="I15" s="165"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2193,18 +2183,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="182" t="s">
+      <c r="B16" s="183" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="183"/>
-      <c r="D16" s="183"/>
+      <c r="C16" s="184"/>
+      <c r="D16" s="184"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="182" t="s">
+      <c r="F16" s="183" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="183"/>
-      <c r="H16" s="183"/>
-      <c r="I16" s="184"/>
+      <c r="G16" s="184"/>
+      <c r="H16" s="184"/>
+      <c r="I16" s="185"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2222,18 +2212,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="179" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="185"/>
-      <c r="D17" s="185"/>
-      <c r="E17" s="186"/>
-      <c r="F17" s="187" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" s="185"/>
-      <c r="H17" s="185"/>
-      <c r="I17" s="185"/>
+      <c r="B17" s="164" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="186"/>
+      <c r="D17" s="186"/>
+      <c r="E17" s="187"/>
+      <c r="F17" s="188" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="186"/>
+      <c r="H17" s="186"/>
+      <c r="I17" s="186"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2251,23 +2241,23 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="188" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="189"/>
+      <c r="B18" s="189" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="190"/>
       <c r="D18" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="189" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="189"/>
-      <c r="G18" s="189"/>
+        <v>72</v>
+      </c>
+      <c r="E18" s="190" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="190"/>
+      <c r="G18" s="190"/>
       <c r="H18" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J18" s="24"/>
       <c r="N18" s="10"/>
@@ -2286,18 +2276,18 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="190" t="s">
+      <c r="B19" s="174" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="191"/>
+      <c r="C19" s="175"/>
       <c r="D19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="192" t="s">
+      <c r="E19" s="176" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="192"/>
-      <c r="G19" s="192"/>
+      <c r="F19" s="176"/>
+      <c r="G19" s="176"/>
       <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2383,49 +2373,66 @@
       <c r="AC21" s="10"/>
       <c r="AD21" s="10"/>
     </row>
-    <row r="22" spans="2:30" s="30" customFormat="1" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="29"/>
+    <row r="22" spans="2:30" s="30" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
       <c r="J22" s="19"/>
     </row>
-    <row r="23" spans="2:30" s="30" customFormat="1" ht="23.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="19"/>
-    </row>
-    <row r="24" spans="2:30" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="6" t="s">
+    <row r="23" spans="2:30" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="6" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="22"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="10"/>
+      <c r="AD23" s="10"/>
+    </row>
+    <row r="24" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="177" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="178"/>
+      <c r="D24" s="178"/>
+      <c r="E24" s="179"/>
+      <c r="F24" s="177" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="178"/>
+      <c r="H24" s="178"/>
+      <c r="I24" s="178"/>
       <c r="J24" s="22"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
@@ -2445,409 +2452,392 @@
       <c r="AC24" s="10"/>
       <c r="AD24" s="10"/>
     </row>
-    <row r="25" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="193" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="194"/>
-      <c r="D25" s="194"/>
-      <c r="E25" s="195"/>
-      <c r="F25" s="193" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="194"/>
-      <c r="H25" s="194"/>
-      <c r="I25" s="194"/>
-      <c r="J25" s="22"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
-      <c r="T25" s="10"/>
-      <c r="U25" s="10"/>
-      <c r="V25" s="10"/>
-      <c r="W25" s="10"/>
-      <c r="X25" s="10"/>
-      <c r="Y25" s="10"/>
-      <c r="Z25" s="10"/>
-      <c r="AA25" s="10"/>
-      <c r="AB25" s="10"/>
-      <c r="AC25" s="10"/>
-      <c r="AD25" s="10"/>
-    </row>
-    <row r="26" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="179" t="s">
+    <row r="25" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="164" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="165"/>
+      <c r="D25" s="165"/>
+      <c r="E25" s="166"/>
+      <c r="F25" s="164" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="180"/>
-      <c r="D26" s="180"/>
-      <c r="E26" s="181"/>
-      <c r="F26" s="179" t="s">
-        <v>82</v>
-      </c>
-      <c r="G26" s="180"/>
-      <c r="H26" s="180"/>
-      <c r="I26" s="180"/>
+      <c r="G25" s="165"/>
+      <c r="H25" s="165"/>
+      <c r="I25" s="165"/>
+      <c r="J25" s="19"/>
+    </row>
+    <row r="26" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="180" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="181"/>
+      <c r="D26" s="181"/>
+      <c r="E26" s="182"/>
+      <c r="F26" s="164" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="165"/>
+      <c r="H26" s="165"/>
+      <c r="I26" s="166"/>
       <c r="J26" s="19"/>
     </row>
-    <row r="27" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="176" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="177"/>
-      <c r="D27" s="177"/>
-      <c r="E27" s="178"/>
-      <c r="F27" s="179" t="s">
-        <v>83</v>
-      </c>
-      <c r="G27" s="180"/>
-      <c r="H27" s="180"/>
-      <c r="I27" s="181"/>
-      <c r="J27" s="19"/>
-    </row>
-    <row r="28" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="173" t="s">
+    <row r="27" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="171" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="174"/>
-      <c r="D28" s="174"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="173" t="s">
+      <c r="C27" s="172"/>
+      <c r="D27" s="172"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="171" t="s">
         <v>34</v>
       </c>
-      <c r="G28" s="174"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="175"/>
-      <c r="J28" s="22"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
-      <c r="T28" s="10"/>
-      <c r="U28" s="10"/>
-      <c r="V28" s="10"/>
-      <c r="W28" s="10"/>
-      <c r="X28" s="10"/>
-      <c r="Y28" s="10"/>
-      <c r="Z28" s="10"/>
-      <c r="AA28" s="10"/>
-      <c r="AB28" s="10"/>
-      <c r="AC28" s="10"/>
-      <c r="AD28" s="10"/>
-    </row>
-    <row r="29" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="179" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="180"/>
-      <c r="D29" s="180"/>
-      <c r="E29" s="181"/>
-      <c r="F29" s="179" t="s">
+      <c r="G27" s="172"/>
+      <c r="H27" s="172"/>
+      <c r="I27" s="173"/>
+      <c r="J27" s="22"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10"/>
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="10"/>
+      <c r="AD27" s="10"/>
+    </row>
+    <row r="28" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="164" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="165"/>
+      <c r="D28" s="165"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="164" t="s">
         <v>35</v>
       </c>
-      <c r="G29" s="180"/>
-      <c r="H29" s="180"/>
-      <c r="I29" s="180"/>
+      <c r="G28" s="165"/>
+      <c r="H28" s="165"/>
+      <c r="I28" s="165"/>
+      <c r="J28" s="9"/>
+    </row>
+    <row r="29" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="171" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="172"/>
+      <c r="D29" s="172"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="171" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="172"/>
+      <c r="H29" s="172"/>
+      <c r="I29" s="173"/>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="173" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="174"/>
-      <c r="D30" s="174"/>
+    <row r="30" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="173" t="s">
-        <v>37</v>
-      </c>
-      <c r="G30" s="174"/>
-      <c r="H30" s="174"/>
-      <c r="I30" s="175"/>
+      <c r="F30" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="50" t="s">
+    <row r="31" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="167" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="168"/>
+      <c r="D31" s="168"/>
+      <c r="E31" s="169"/>
+      <c r="F31" s="167" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="168"/>
+      <c r="H31" s="168"/>
+      <c r="I31" s="168"/>
+      <c r="J31" s="34"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="36"/>
+      <c r="U31" s="36"/>
+      <c r="V31" s="36"/>
+      <c r="W31" s="36"/>
+      <c r="X31" s="36"/>
+      <c r="Y31" s="36"/>
+      <c r="Z31" s="36"/>
+      <c r="AA31" s="36"/>
+      <c r="AB31" s="36"/>
+      <c r="AC31" s="36"/>
+      <c r="AD31" s="36"/>
+    </row>
+    <row r="32" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="164" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="165"/>
+      <c r="D32" s="165"/>
+      <c r="E32" s="166"/>
+      <c r="F32" s="164" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="165"/>
+      <c r="H32" s="165"/>
+      <c r="I32" s="165"/>
+      <c r="J32" s="19"/>
+    </row>
+    <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="164" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="165"/>
+      <c r="D33" s="165"/>
+      <c r="E33" s="166"/>
+      <c r="F33" s="164" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="165"/>
+      <c r="H33" s="165"/>
+      <c r="I33" s="165"/>
+      <c r="J33" s="19"/>
+    </row>
+    <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="164" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="165"/>
+      <c r="D34" s="165"/>
+      <c r="E34" s="166"/>
+      <c r="F34" s="164" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" s="165"/>
+      <c r="H34" s="165"/>
+      <c r="I34" s="165"/>
+      <c r="J34" s="19"/>
+    </row>
+    <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="164" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="165"/>
+      <c r="D35" s="165"/>
+      <c r="E35" s="166"/>
+      <c r="F35" s="164" t="s">
+        <v>42</v>
+      </c>
+      <c r="G35" s="165"/>
+      <c r="H35" s="165"/>
+      <c r="I35" s="165"/>
+      <c r="J35" s="19"/>
+    </row>
+    <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="164" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="165"/>
+      <c r="D36" s="165"/>
+      <c r="E36" s="166"/>
+      <c r="F36" s="164" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" s="165"/>
+      <c r="H36" s="165"/>
+      <c r="I36" s="165"/>
+      <c r="J36" s="19"/>
+    </row>
+    <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="164" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="165"/>
+      <c r="D37" s="165"/>
+      <c r="E37" s="166"/>
+      <c r="F37" s="164" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="165"/>
+      <c r="H37" s="165"/>
+      <c r="I37" s="165"/>
+      <c r="J37" s="19"/>
+    </row>
+    <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="196" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="197"/>
-      <c r="D32" s="197"/>
-      <c r="E32" s="198"/>
-      <c r="F32" s="196" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="197"/>
-      <c r="H32" s="197"/>
-      <c r="I32" s="197"/>
-      <c r="J32" s="34"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="36"/>
-      <c r="P32" s="36"/>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="36"/>
-      <c r="T32" s="36"/>
-      <c r="U32" s="36"/>
-      <c r="V32" s="36"/>
-      <c r="W32" s="36"/>
-      <c r="X32" s="36"/>
-      <c r="Y32" s="36"/>
-      <c r="Z32" s="36"/>
-      <c r="AA32" s="36"/>
-      <c r="AB32" s="36"/>
-      <c r="AC32" s="36"/>
-      <c r="AD32" s="36"/>
-    </row>
-    <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="179" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="180"/>
-      <c r="D33" s="180"/>
-      <c r="E33" s="181"/>
-      <c r="F33" s="179" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="180"/>
-      <c r="H33" s="180"/>
-      <c r="I33" s="180"/>
-      <c r="J33" s="19"/>
-    </row>
-    <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="179" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="180"/>
-      <c r="D34" s="180"/>
-      <c r="E34" s="181"/>
-      <c r="F34" s="179" t="s">
-        <v>40</v>
-      </c>
-      <c r="G34" s="180"/>
-      <c r="H34" s="180"/>
-      <c r="I34" s="180"/>
-      <c r="J34" s="19"/>
-    </row>
-    <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="179" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="180"/>
-      <c r="D35" s="180"/>
-      <c r="E35" s="181"/>
-      <c r="F35" s="179" t="s">
-        <v>41</v>
-      </c>
-      <c r="G35" s="180"/>
-      <c r="H35" s="180"/>
-      <c r="I35" s="180"/>
-      <c r="J35" s="19"/>
-    </row>
-    <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="179" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="180"/>
-      <c r="D36" s="180"/>
-      <c r="E36" s="181"/>
-      <c r="F36" s="179" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" s="180"/>
-      <c r="H36" s="180"/>
-      <c r="I36" s="180"/>
-      <c r="J36" s="19"/>
-    </row>
-    <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="179" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="180"/>
-      <c r="D37" s="180"/>
-      <c r="E37" s="181"/>
-      <c r="F37" s="179" t="s">
-        <v>44</v>
-      </c>
-      <c r="G37" s="180"/>
-      <c r="H37" s="180"/>
-      <c r="I37" s="180"/>
-      <c r="J37" s="19"/>
-    </row>
-    <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="179" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="180"/>
-      <c r="D38" s="180"/>
-      <c r="E38" s="181"/>
-      <c r="F38" s="179" t="s">
-        <v>46</v>
-      </c>
-      <c r="G38" s="180"/>
-      <c r="H38" s="180"/>
-      <c r="I38" s="180"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
       <c r="J38" s="19"/>
     </row>
-    <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="196" t="s">
+    <row r="39" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="167" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="197"/>
-      <c r="D40" s="197"/>
-      <c r="E40" s="198"/>
-      <c r="F40" s="196" t="s">
+      <c r="C39" s="168"/>
+      <c r="D39" s="168"/>
+      <c r="E39" s="169"/>
+      <c r="F39" s="167" t="s">
         <v>12</v>
       </c>
-      <c r="G40" s="199"/>
-      <c r="H40" s="199"/>
-      <c r="I40" s="199"/>
-      <c r="J40" s="34"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="36"/>
-      <c r="R40" s="36"/>
-      <c r="S40" s="36"/>
-      <c r="T40" s="36"/>
-      <c r="U40" s="36"/>
-      <c r="V40" s="36"/>
-      <c r="W40" s="36"/>
-      <c r="X40" s="36"/>
-      <c r="Y40" s="36"/>
-      <c r="Z40" s="36"/>
-      <c r="AA40" s="36"/>
-      <c r="AB40" s="36"/>
-      <c r="AC40" s="36"/>
-      <c r="AD40" s="36"/>
-    </row>
-    <row r="41" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="179" t="s">
+      <c r="G39" s="170"/>
+      <c r="H39" s="170"/>
+      <c r="I39" s="170"/>
+      <c r="J39" s="34"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="P39" s="36"/>
+      <c r="Q39" s="36"/>
+      <c r="R39" s="36"/>
+      <c r="S39" s="36"/>
+      <c r="T39" s="36"/>
+      <c r="U39" s="36"/>
+      <c r="V39" s="36"/>
+      <c r="W39" s="36"/>
+      <c r="X39" s="36"/>
+      <c r="Y39" s="36"/>
+      <c r="Z39" s="36"/>
+      <c r="AA39" s="36"/>
+      <c r="AB39" s="36"/>
+      <c r="AC39" s="36"/>
+      <c r="AD39" s="36"/>
+    </row>
+    <row r="40" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="164" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="180"/>
-      <c r="D41" s="180"/>
-      <c r="E41" s="181"/>
-      <c r="F41" s="179" t="s">
+      <c r="C40" s="165"/>
+      <c r="D40" s="165"/>
+      <c r="E40" s="166"/>
+      <c r="F40" s="164" t="s">
         <v>13</v>
       </c>
-      <c r="G41" s="180"/>
-      <c r="H41" s="180"/>
-      <c r="I41" s="180"/>
+      <c r="G40" s="165"/>
+      <c r="H40" s="165"/>
+      <c r="I40" s="165"/>
+      <c r="J40" s="19"/>
+    </row>
+    <row r="41" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="19"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
       <c r="J41" s="19"/>
     </row>
-    <row r="42" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="19"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="20" t="s">
+    <row r="42" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" s="28"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="19"/>
+    </row>
+    <row r="43" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B43" s="39"/>
+      <c r="C43" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="27" t="s">
-        <v>48</v>
-      </c>
+      <c r="D43" s="31"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="27"/>
       <c r="G43" s="28"/>
       <c r="H43" s="38"/>
       <c r="I43" s="38"/>
       <c r="J43" s="19"/>
     </row>
-    <row r="44" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="39"/>
-      <c r="C44" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="D44" s="31"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="28"/>
+    <row r="44" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B44" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="G44" s="38"/>
       <c r="H44" s="38"/>
       <c r="I44" s="38"/>
       <c r="J44" s="19"/>
     </row>
-    <row r="45" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
+    <row r="45" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="164" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="165"/>
+      <c r="D45" s="165"/>
+      <c r="E45" s="166"/>
+      <c r="F45" s="164" t="s">
+        <v>50</v>
+      </c>
+      <c r="G45" s="165"/>
+      <c r="H45" s="165"/>
+      <c r="I45" s="166"/>
       <c r="J45" s="19"/>
     </row>
-    <row r="46" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="179" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="180"/>
-      <c r="D46" s="180"/>
-      <c r="E46" s="181"/>
-      <c r="F46" s="179" t="s">
-        <v>50</v>
-      </c>
-      <c r="G46" s="180"/>
-      <c r="H46" s="180"/>
-      <c r="I46" s="181"/>
+    <row r="46" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
       <c r="J46" s="19"/>
     </row>
     <row r="47" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B47" s="27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C47" s="28"/>
       <c r="D47" s="28"/>
       <c r="E47" s="29"/>
       <c r="F47" s="28" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G47" s="38"/>
       <c r="H47" s="38"/>
@@ -2856,82 +2846,78 @@
     </row>
     <row r="48" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="27" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C48" s="28"/>
       <c r="D48" s="28"/>
       <c r="E48" s="29"/>
       <c r="F48" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
+        <v>53</v>
+      </c>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="28"/>
       <c r="J48" s="19"/>
     </row>
     <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
-      <c r="I49" s="28"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49" s="31"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H49" s="31"/>
+      <c r="I49" s="31"/>
       <c r="J49" s="19"/>
     </row>
-    <row r="50" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="19"/>
-      <c r="C50" s="36" t="s">
+    <row r="50" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="G50" s="41"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="42"/>
+      <c r="J50" s="15"/>
+    </row>
+    <row r="51" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="43"/>
+      <c r="C51" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="31"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="12" t="s">
+      <c r="D51" s="45"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="19"/>
-    </row>
-    <row r="51" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="G51" s="41"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="42"/>
+      <c r="H51" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="I51" s="46"/>
       <c r="J51" s="15"/>
     </row>
-    <row r="52" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="43"/>
-      <c r="C52" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D52" s="45"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="H52" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="I52" s="46"/>
+    <row r="52" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="15"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
       <c r="J52" s="15"/>
     </row>
-    <row r="53" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="15"/>
       <c r="C53" s="48"/>
       <c r="D53" s="48"/>
@@ -3030,77 +3016,26 @@
       <c r="I61" s="15"/>
       <c r="J61" s="15"/>
     </row>
-    <row r="62" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B62" s="15"/>
-      <c r="C62" s="48"/>
-      <c r="D62" s="48"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
-      <c r="H62" s="15"/>
-      <c r="I62" s="15"/>
-      <c r="J62" s="15"/>
-    </row>
+    <row r="62" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="63" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="64" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="65" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="66" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="67" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="68" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="76" spans="6:7" x14ac:dyDescent="0.45">
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
-    </row>
-    <row r="81" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="88" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="75" spans="6:7" x14ac:dyDescent="0.45">
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+    </row>
+    <row r="80" spans="6:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="87" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="F11:I11"/>
     <mergeCell ref="B9:E10"/>
@@ -3111,12 +3046,52 @@
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:I37"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="notContainsBlanks" dxfId="3" priority="2">
@@ -3188,7 +3163,7 @@
     <row r="2" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="89"/>
       <c r="B2" s="119" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C2" s="119"/>
       <c r="D2" s="119"/>
@@ -3196,7 +3171,7 @@
       <c r="F2" s="119"/>
       <c r="G2" s="119"/>
       <c r="H2" s="122" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I2" s="119"/>
       <c r="J2" s="119"/>
@@ -3208,7 +3183,7 @@
     <row r="3" spans="1:14" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="89"/>
       <c r="B3" s="120" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" s="120"/>
       <c r="D3" s="120"/>
@@ -3216,7 +3191,7 @@
       <c r="F3" s="121"/>
       <c r="G3" s="121"/>
       <c r="H3" s="123" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I3" s="120"/>
       <c r="J3" s="120"/>
@@ -3228,7 +3203,7 @@
     <row r="4" spans="1:14" s="86" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="88"/>
       <c r="B4" s="120" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C4" s="120"/>
       <c r="D4" s="120"/>
@@ -3236,7 +3211,7 @@
       <c r="F4" s="120"/>
       <c r="G4" s="120"/>
       <c r="H4" s="123" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I4" s="120"/>
       <c r="J4" s="120"/>
@@ -3248,7 +3223,7 @@
     <row r="5" spans="1:14" s="86" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="87"/>
       <c r="B5" s="120" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C5" s="120"/>
       <c r="D5" s="120"/>
@@ -3256,7 +3231,7 @@
       <c r="F5" s="120"/>
       <c r="G5" s="120"/>
       <c r="H5" s="123" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I5" s="120"/>
       <c r="J5" s="120"/>
@@ -3268,7 +3243,7 @@
     <row r="6" spans="1:14" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="56"/>
       <c r="B6" s="110" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C6" s="110"/>
       <c r="D6" s="110"/>
@@ -3276,7 +3251,7 @@
       <c r="F6" s="110"/>
       <c r="G6" s="110"/>
       <c r="H6" s="96" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I6" s="97"/>
       <c r="J6" s="97"/>
@@ -3288,7 +3263,7 @@
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="56"/>
       <c r="B7" s="113" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" s="124"/>
       <c r="D7" s="124"/>
@@ -3328,7 +3303,7 @@
     <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="56"/>
       <c r="B9" s="126" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C9" s="126"/>
       <c r="D9" s="126"/>
@@ -3336,7 +3311,7 @@
       <c r="F9" s="126"/>
       <c r="G9" s="126"/>
       <c r="H9" s="103" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I9" s="98"/>
       <c r="J9" s="98"/>
@@ -3388,7 +3363,7 @@
     <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="56"/>
       <c r="B12" s="126" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C12" s="126"/>
       <c r="D12" s="126"/>
@@ -3396,7 +3371,7 @@
       <c r="F12" s="126"/>
       <c r="G12" s="126"/>
       <c r="H12" s="96" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I12" s="97"/>
       <c r="J12" s="97"/>
@@ -3448,27 +3423,27 @@
     <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="85"/>
       <c r="B15" s="104" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C15" s="104"/>
       <c r="D15" s="105" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E15" s="105"/>
       <c r="F15" s="105" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G15" s="105"/>
       <c r="H15" s="106" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I15" s="105"/>
       <c r="J15" s="127" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K15" s="127"/>
       <c r="L15" s="151" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M15" s="151"/>
       <c r="N15" s="58"/>
@@ -3476,27 +3451,27 @@
     <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="56"/>
       <c r="B16" s="118" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" s="107"/>
       <c r="D16" s="156" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E16" s="108"/>
       <c r="F16" s="144" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G16" s="108"/>
       <c r="H16" s="159" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I16" s="108"/>
       <c r="J16" s="109" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K16" s="109"/>
       <c r="L16" s="152" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M16" s="152"/>
       <c r="N16" s="58"/>
@@ -3504,27 +3479,27 @@
     <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="56"/>
       <c r="B17" s="126" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C17" s="126"/>
       <c r="D17" s="126" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E17" s="130"/>
       <c r="F17" s="143" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G17" s="143"/>
       <c r="H17" s="103" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I17" s="98"/>
       <c r="J17" s="111" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K17" s="98"/>
       <c r="L17" s="153" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M17" s="154"/>
       <c r="N17" s="58"/>
@@ -3532,27 +3507,27 @@
     <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="56"/>
       <c r="B18" s="102" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C18" s="125"/>
       <c r="D18" s="157" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E18" s="109"/>
       <c r="F18" s="158" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G18" s="144"/>
       <c r="H18" s="159" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I18" s="109"/>
       <c r="J18" s="157" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K18" s="109"/>
       <c r="L18" s="152" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M18" s="152"/>
       <c r="N18" s="58"/>
@@ -3560,21 +3535,21 @@
     <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="56"/>
       <c r="B19" s="131" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C19" s="131"/>
       <c r="D19" s="131" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E19" s="131"/>
       <c r="F19" s="145"/>
       <c r="G19" s="145"/>
       <c r="H19" s="148" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I19" s="128"/>
       <c r="J19" s="126" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K19" s="126"/>
       <c r="L19" s="126"/>
@@ -3584,21 +3559,21 @@
     <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="56"/>
       <c r="B20" s="156" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="112"/>
       <c r="D20" s="129" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E20" s="129"/>
       <c r="F20" s="146"/>
       <c r="G20" s="146"/>
       <c r="H20" s="160" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I20" s="108"/>
       <c r="J20" s="113" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K20" s="114"/>
       <c r="L20" s="109"/>
@@ -3635,60 +3610,60 @@
     <row r="22" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="56"/>
       <c r="B22" s="60" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C22" s="132" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D22" s="132"/>
       <c r="E22" s="132"/>
       <c r="F22" s="150"/>
       <c r="G22" s="132"/>
       <c r="H22" s="60" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I22" s="81" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J22" s="80" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K22" s="132" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L22" s="132"/>
       <c r="M22" s="60" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N22" s="58"/>
     </row>
     <row r="23" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="56"/>
       <c r="B23" s="139" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C23" s="200" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D23" s="200"/>
       <c r="E23" s="200"/>
       <c r="F23" s="200"/>
       <c r="G23" s="140"/>
       <c r="H23" s="141" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I23" s="79" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J23" s="78">
         <v>14</v>
       </c>
       <c r="K23" s="201" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L23" s="201"/>
       <c r="M23" s="77" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N23" s="58"/>
     </row>
@@ -3700,10 +3675,10 @@
       <c r="F24" s="137"/>
       <c r="G24" s="137"/>
       <c r="H24" s="138" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I24" s="76" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J24" s="75">
         <v>14</v>
@@ -3713,7 +3688,7 @@
       </c>
       <c r="L24" s="142"/>
       <c r="M24" s="90" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N24" s="58"/>
     </row>
@@ -3925,7 +3900,7 @@
     <row r="38" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="56"/>
       <c r="B38" s="92" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C38" s="73"/>
       <c r="D38" s="73"/>
@@ -3934,7 +3909,7 @@
       <c r="G38" s="72"/>
       <c r="H38" s="71"/>
       <c r="I38" s="134" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J38" s="133"/>
       <c r="K38" s="133"/>
@@ -3945,7 +3920,7 @@
     <row r="39" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="56"/>
       <c r="B39" s="93" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C39" s="69"/>
       <c r="D39" s="69"/>
@@ -3981,7 +3956,7 @@
     <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="56"/>
       <c r="B41" s="93" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C41" s="69"/>
       <c r="D41" s="69"/>
@@ -3999,7 +3974,7 @@
     <row r="42" spans="1:14" s="64" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="68"/>
       <c r="B42" s="94" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C42" s="67"/>
       <c r="D42" s="67"/>

</xml_diff>

<commit_message>
init pictures api updated, now can set pic height + width manually
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCD2417-FEBF-4046-A164-E882B01BB09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBFC8ED-303F-4FD9-9876-C4E7EDA9BB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
     <sheet name="Invoice" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Invoice_seal_seller_start">Invoice!$J$38</definedName>
+    <definedName name="Invoice_sign_seller_end">Invoice!$K$45</definedName>
+    <definedName name="Invoice_sign_seller_start">Invoice!$J$41</definedName>
     <definedName name="MID_Contract">Export_Contract!$E$1</definedName>
     <definedName name="MID_Invoice">Invoice!$G$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$N$50</definedName>
     <definedName name="Seal_agent_end">Export_Contract!$H$51</definedName>
     <definedName name="Seal_agent_start">Export_Contract!$G$41</definedName>
     <definedName name="Seal_seller_end">Export_Contract!$C$51</definedName>
@@ -46,9 +50,9 @@
     <definedName name="Доставка_условия">Export_Contract!$B$24</definedName>
     <definedName name="Инвойс">Invoice!$B$2</definedName>
     <definedName name="Инвойс_Bl_массив">Invoice!$B$23</definedName>
-    <definedName name="Инвойс_банк_получателя">Invoice!$B$38</definedName>
-    <definedName name="Инвойс_банк_получателя_адрес">Invoice!$B$39</definedName>
-    <definedName name="Инвойс_банк_получателя_свифт">Invoice!$B$40</definedName>
+    <definedName name="Инвойс_банк_получателя">Invoice!$B$37</definedName>
+    <definedName name="Инвойс_банк_получателя_адрес">Invoice!$B$38</definedName>
+    <definedName name="Инвойс_банк_получателя_свифт">Invoice!$B$39</definedName>
     <definedName name="Инвойс_дата">Invoice!$B$5</definedName>
     <definedName name="Инвойс_дата_отправки">Invoice!$F$20</definedName>
     <definedName name="Инвойс_декларация">Invoice!$D$20</definedName>
@@ -57,13 +61,13 @@
     <definedName name="Инвойс_куда">Invoice!$D$18</definedName>
     <definedName name="Инвойс_МСЦ">Invoice!$D$16</definedName>
     <definedName name="Инвойс_откуда">Invoice!$F$18</definedName>
-    <definedName name="Инвойс_подписант">Invoice!$I$38</definedName>
+    <definedName name="Инвойс_подписант">Invoice!$I$37</definedName>
     <definedName name="Инвойс_покупатель">Invoice!$B$10</definedName>
     <definedName name="Инвойс_покупатель_адрес">Invoice!$B$11</definedName>
     <definedName name="Инвойс_получатель">Invoice!$B$13</definedName>
     <definedName name="Инвойс_получатель_адрес">Invoice!$B$14</definedName>
-    <definedName name="Инвойс_получатель_в_пользу">Invoice!$B$41</definedName>
-    <definedName name="Инвойс_получатель_счет">Invoice!$B$42</definedName>
+    <definedName name="Инвойс_получатель_в_пользу">Invoice!$B$40</definedName>
+    <definedName name="Инвойс_получатель_счет">Invoice!$B$41</definedName>
     <definedName name="Инвойс_продавец">Invoice!$B$7</definedName>
     <definedName name="Инвойс_продавец_адрес">Invoice!$B$8</definedName>
     <definedName name="Инвойс_соглашение">Invoice!$B$3</definedName>
@@ -106,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="139">
   <si>
     <t>Дополнительное соглашение № 146 от 10 марта 2023г.</t>
   </si>
@@ -858,7 +862,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1041,7 +1045,6 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1110,9 +1113,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1408,6 +1408,19 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1774,8 +1787,8 @@
   </sheetPr>
   <dimension ref="B1:AF87"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:E32"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A23" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1815,31 +1828,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="2.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
-      <c r="H1" s="162"/>
-      <c r="I1" s="162"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
     </row>
     <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="194" t="s">
+      <c r="B2" s="192" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="194" t="s">
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="194"/>
+      <c r="F2" s="192" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="163"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="161"/>
       <c r="L2" s="11"/>
       <c r="N2" s="18"/>
       <c r="AA2" s="18"/>
@@ -1848,18 +1861,18 @@
       <c r="AD2" s="18"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="195" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="199"/>
-      <c r="F3" s="197" t="s">
+      <c r="C3" s="196"/>
+      <c r="D3" s="196"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="195" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="198"/>
-      <c r="H3" s="198"/>
-      <c r="I3" s="198"/>
+      <c r="G3" s="196"/>
+      <c r="H3" s="196"/>
+      <c r="I3" s="196"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1876,18 +1889,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="197" t="s">
+      <c r="B4" s="195" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="198"/>
-      <c r="D4" s="198"/>
-      <c r="E4" s="199"/>
-      <c r="F4" s="197" t="s">
+      <c r="C4" s="196"/>
+      <c r="D4" s="196"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="195" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="198"/>
-      <c r="H4" s="198"/>
-      <c r="I4" s="198"/>
+      <c r="G4" s="196"/>
+      <c r="H4" s="196"/>
+      <c r="I4" s="196"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1908,18 +1921,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="191" t="s">
+      <c r="B5" s="189" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="192"/>
-      <c r="D5" s="192"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="191" t="s">
+      <c r="C5" s="190"/>
+      <c r="D5" s="190"/>
+      <c r="E5" s="191"/>
+      <c r="F5" s="189" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="192"/>
-      <c r="H5" s="192"/>
-      <c r="I5" s="192"/>
+      <c r="G5" s="190"/>
+      <c r="H5" s="190"/>
+      <c r="I5" s="190"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1928,18 +1941,18 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="171" t="s">
+      <c r="B6" s="169" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="172"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="171" t="s">
+      <c r="C6" s="170"/>
+      <c r="D6" s="170"/>
+      <c r="E6" s="171"/>
+      <c r="F6" s="169" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="172"/>
-      <c r="H6" s="172"/>
-      <c r="I6" s="172"/>
+      <c r="G6" s="170"/>
+      <c r="H6" s="170"/>
+      <c r="I6" s="170"/>
       <c r="J6" s="54"/>
       <c r="L6" s="55"/>
       <c r="O6" s="10"/>
@@ -1984,44 +1997,44 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="178" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="181"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="182"/>
-      <c r="F8" s="164" t="s">
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="180"/>
+      <c r="F8" s="162" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="165"/>
-      <c r="H8" s="165"/>
-      <c r="I8" s="165"/>
+      <c r="G8" s="163"/>
+      <c r="H8" s="163"/>
+      <c r="I8" s="163"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="164" t="s">
+      <c r="B9" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="165"/>
-      <c r="D9" s="165"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="164" t="s">
+      <c r="C9" s="163"/>
+      <c r="D9" s="163"/>
+      <c r="E9" s="164"/>
+      <c r="F9" s="162" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="165"/>
-      <c r="H9" s="165"/>
-      <c r="I9" s="166"/>
+      <c r="G9" s="163"/>
+      <c r="H9" s="163"/>
+      <c r="I9" s="164"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="164"/>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="166"/>
-      <c r="F10" s="164"/>
-      <c r="G10" s="165"/>
-      <c r="H10" s="165"/>
-      <c r="I10" s="166"/>
+      <c r="B10" s="162"/>
+      <c r="C10" s="163"/>
+      <c r="D10" s="163"/>
+      <c r="E10" s="164"/>
+      <c r="F10" s="162"/>
+      <c r="G10" s="163"/>
+      <c r="H10" s="163"/>
+      <c r="I10" s="164"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -2042,18 +2055,18 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="171" t="s">
+      <c r="B11" s="169" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="172"/>
-      <c r="D11" s="172"/>
-      <c r="E11" s="173"/>
-      <c r="F11" s="171" t="s">
+      <c r="C11" s="170"/>
+      <c r="D11" s="170"/>
+      <c r="E11" s="171"/>
+      <c r="F11" s="169" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="172"/>
-      <c r="H11" s="172"/>
-      <c r="I11" s="172"/>
+      <c r="G11" s="170"/>
+      <c r="H11" s="170"/>
+      <c r="I11" s="170"/>
       <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -2096,18 +2109,18 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="164" t="s">
+      <c r="B13" s="162" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="165"/>
-      <c r="E13" s="166"/>
-      <c r="F13" s="164" t="s">
+      <c r="C13" s="163"/>
+      <c r="D13" s="163"/>
+      <c r="E13" s="164"/>
+      <c r="F13" s="162" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="165"/>
-      <c r="H13" s="165"/>
-      <c r="I13" s="165"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2125,18 +2138,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="162" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="165"/>
-      <c r="E14" s="166"/>
-      <c r="F14" s="164" t="s">
+      <c r="C14" s="163"/>
+      <c r="D14" s="163"/>
+      <c r="E14" s="164"/>
+      <c r="F14" s="162" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="165"/>
-      <c r="H14" s="165"/>
-      <c r="I14" s="165"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="163"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2154,18 +2167,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="164" t="s">
+      <c r="B15" s="162" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="165"/>
-      <c r="E15" s="166"/>
-      <c r="F15" s="164" t="s">
+      <c r="C15" s="163"/>
+      <c r="D15" s="163"/>
+      <c r="E15" s="164"/>
+      <c r="F15" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="165"/>
-      <c r="H15" s="165"/>
-      <c r="I15" s="165"/>
+      <c r="G15" s="163"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="163"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2183,18 +2196,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="183" t="s">
+      <c r="B16" s="181" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="184"/>
-      <c r="D16" s="184"/>
+      <c r="C16" s="182"/>
+      <c r="D16" s="182"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="183" t="s">
+      <c r="F16" s="181" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="184"/>
-      <c r="H16" s="184"/>
-      <c r="I16" s="185"/>
+      <c r="G16" s="182"/>
+      <c r="H16" s="182"/>
+      <c r="I16" s="183"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2212,18 +2225,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="164" t="s">
+      <c r="B17" s="162" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="186"/>
-      <c r="D17" s="186"/>
-      <c r="E17" s="187"/>
-      <c r="F17" s="188" t="s">
+      <c r="C17" s="184"/>
+      <c r="D17" s="184"/>
+      <c r="E17" s="185"/>
+      <c r="F17" s="186" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="186"/>
-      <c r="H17" s="186"/>
-      <c r="I17" s="186"/>
+      <c r="G17" s="184"/>
+      <c r="H17" s="184"/>
+      <c r="I17" s="184"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2241,18 +2254,18 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="189" t="s">
+      <c r="B18" s="187" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="190"/>
+      <c r="C18" s="188"/>
       <c r="D18" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="190" t="s">
+      <c r="E18" s="188" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="190"/>
-      <c r="G18" s="190"/>
+      <c r="F18" s="188"/>
+      <c r="G18" s="188"/>
       <c r="H18" s="23" t="s">
         <v>76</v>
       </c>
@@ -2276,18 +2289,18 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="174" t="s">
+      <c r="B19" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="175"/>
+      <c r="C19" s="173"/>
       <c r="D19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="176" t="s">
+      <c r="E19" s="174" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="176"/>
-      <c r="G19" s="176"/>
+      <c r="F19" s="174"/>
+      <c r="G19" s="174"/>
       <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2421,18 +2434,18 @@
       <c r="AD23" s="10"/>
     </row>
     <row r="24" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="177" t="s">
+      <c r="B24" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="178"/>
-      <c r="D24" s="178"/>
-      <c r="E24" s="179"/>
-      <c r="F24" s="177" t="s">
+      <c r="C24" s="176"/>
+      <c r="D24" s="176"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="175" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="178"/>
-      <c r="H24" s="178"/>
-      <c r="I24" s="178"/>
+      <c r="G24" s="176"/>
+      <c r="H24" s="176"/>
+      <c r="I24" s="176"/>
       <c r="J24" s="22"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
@@ -2453,48 +2466,48 @@
       <c r="AD24" s="10"/>
     </row>
     <row r="25" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="164" t="s">
+      <c r="B25" s="162" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="165"/>
-      <c r="D25" s="165"/>
-      <c r="E25" s="166"/>
-      <c r="F25" s="164" t="s">
+      <c r="C25" s="163"/>
+      <c r="D25" s="163"/>
+      <c r="E25" s="164"/>
+      <c r="F25" s="162" t="s">
         <v>80</v>
       </c>
-      <c r="G25" s="165"/>
-      <c r="H25" s="165"/>
-      <c r="I25" s="165"/>
+      <c r="G25" s="163"/>
+      <c r="H25" s="163"/>
+      <c r="I25" s="163"/>
       <c r="J25" s="19"/>
     </row>
     <row r="26" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="180" t="s">
+      <c r="B26" s="178" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="181"/>
-      <c r="D26" s="181"/>
-      <c r="E26" s="182"/>
-      <c r="F26" s="164" t="s">
+      <c r="C26" s="179"/>
+      <c r="D26" s="179"/>
+      <c r="E26" s="180"/>
+      <c r="F26" s="162" t="s">
         <v>81</v>
       </c>
-      <c r="G26" s="165"/>
-      <c r="H26" s="165"/>
-      <c r="I26" s="166"/>
+      <c r="G26" s="163"/>
+      <c r="H26" s="163"/>
+      <c r="I26" s="164"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="171" t="s">
+      <c r="B27" s="169" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="172"/>
-      <c r="D27" s="172"/>
+      <c r="C27" s="170"/>
+      <c r="D27" s="170"/>
       <c r="E27" s="32"/>
-      <c r="F27" s="171" t="s">
+      <c r="F27" s="169" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="172"/>
-      <c r="H27" s="172"/>
-      <c r="I27" s="173"/>
+      <c r="G27" s="170"/>
+      <c r="H27" s="170"/>
+      <c r="I27" s="171"/>
       <c r="J27" s="22"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
@@ -2515,33 +2528,33 @@
       <c r="AD27" s="10"/>
     </row>
     <row r="28" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="164" t="s">
+      <c r="B28" s="162" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="165"/>
-      <c r="D28" s="165"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="164" t="s">
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="164"/>
+      <c r="F28" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="165"/>
-      <c r="H28" s="165"/>
-      <c r="I28" s="165"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
       <c r="J28" s="9"/>
     </row>
     <row r="29" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="171" t="s">
+      <c r="B29" s="169" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="172"/>
-      <c r="D29" s="172"/>
+      <c r="C29" s="170"/>
+      <c r="D29" s="170"/>
       <c r="E29" s="21"/>
-      <c r="F29" s="171" t="s">
+      <c r="F29" s="169" t="s">
         <v>37</v>
       </c>
-      <c r="G29" s="172"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="173"/>
+      <c r="G29" s="170"/>
+      <c r="H29" s="170"/>
+      <c r="I29" s="171"/>
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -2560,18 +2573,18 @@
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="167" t="s">
+      <c r="B31" s="165" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="168"/>
-      <c r="D31" s="168"/>
-      <c r="E31" s="169"/>
-      <c r="F31" s="167" t="s">
+      <c r="C31" s="166"/>
+      <c r="D31" s="166"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="165" t="s">
         <v>7</v>
       </c>
-      <c r="G31" s="168"/>
-      <c r="H31" s="168"/>
-      <c r="I31" s="168"/>
+      <c r="G31" s="166"/>
+      <c r="H31" s="166"/>
+      <c r="I31" s="166"/>
       <c r="J31" s="34"/>
       <c r="N31" s="36"/>
       <c r="O31" s="36"/>
@@ -2592,93 +2605,93 @@
       <c r="AD31" s="36"/>
     </row>
     <row r="32" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="162" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="165"/>
-      <c r="D32" s="165"/>
-      <c r="E32" s="166"/>
-      <c r="F32" s="164" t="s">
+      <c r="C32" s="163"/>
+      <c r="D32" s="163"/>
+      <c r="E32" s="164"/>
+      <c r="F32" s="162" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="165"/>
-      <c r="H32" s="165"/>
-      <c r="I32" s="165"/>
+      <c r="G32" s="163"/>
+      <c r="H32" s="163"/>
+      <c r="I32" s="163"/>
       <c r="J32" s="19"/>
     </row>
     <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="164" t="s">
+      <c r="B33" s="162" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="165"/>
-      <c r="D33" s="165"/>
-      <c r="E33" s="166"/>
-      <c r="F33" s="164" t="s">
+      <c r="C33" s="163"/>
+      <c r="D33" s="163"/>
+      <c r="E33" s="164"/>
+      <c r="F33" s="162" t="s">
         <v>40</v>
       </c>
-      <c r="G33" s="165"/>
-      <c r="H33" s="165"/>
-      <c r="I33" s="165"/>
+      <c r="G33" s="163"/>
+      <c r="H33" s="163"/>
+      <c r="I33" s="163"/>
       <c r="J33" s="19"/>
     </row>
     <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="164" t="s">
+      <c r="B34" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="165"/>
-      <c r="D34" s="165"/>
-      <c r="E34" s="166"/>
-      <c r="F34" s="164" t="s">
+      <c r="C34" s="163"/>
+      <c r="D34" s="163"/>
+      <c r="E34" s="164"/>
+      <c r="F34" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="G34" s="165"/>
-      <c r="H34" s="165"/>
-      <c r="I34" s="165"/>
+      <c r="G34" s="163"/>
+      <c r="H34" s="163"/>
+      <c r="I34" s="163"/>
       <c r="J34" s="19"/>
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="164" t="s">
+      <c r="B35" s="162" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="165"/>
-      <c r="D35" s="165"/>
-      <c r="E35" s="166"/>
-      <c r="F35" s="164" t="s">
+      <c r="C35" s="163"/>
+      <c r="D35" s="163"/>
+      <c r="E35" s="164"/>
+      <c r="F35" s="162" t="s">
         <v>42</v>
       </c>
-      <c r="G35" s="165"/>
-      <c r="H35" s="165"/>
-      <c r="I35" s="165"/>
+      <c r="G35" s="163"/>
+      <c r="H35" s="163"/>
+      <c r="I35" s="163"/>
       <c r="J35" s="19"/>
     </row>
     <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="164" t="s">
+      <c r="B36" s="162" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="165"/>
-      <c r="D36" s="165"/>
-      <c r="E36" s="166"/>
-      <c r="F36" s="164" t="s">
+      <c r="C36" s="163"/>
+      <c r="D36" s="163"/>
+      <c r="E36" s="164"/>
+      <c r="F36" s="162" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="165"/>
-      <c r="H36" s="165"/>
-      <c r="I36" s="165"/>
+      <c r="G36" s="163"/>
+      <c r="H36" s="163"/>
+      <c r="I36" s="163"/>
       <c r="J36" s="19"/>
     </row>
     <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="164" t="s">
+      <c r="B37" s="162" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="165"/>
-      <c r="D37" s="165"/>
-      <c r="E37" s="166"/>
-      <c r="F37" s="164" t="s">
+      <c r="C37" s="163"/>
+      <c r="D37" s="163"/>
+      <c r="E37" s="164"/>
+      <c r="F37" s="162" t="s">
         <v>46</v>
       </c>
-      <c r="G37" s="165"/>
-      <c r="H37" s="165"/>
-      <c r="I37" s="165"/>
+      <c r="G37" s="163"/>
+      <c r="H37" s="163"/>
+      <c r="I37" s="163"/>
       <c r="J37" s="19"/>
     </row>
     <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2697,18 +2710,18 @@
       <c r="J38" s="19"/>
     </row>
     <row r="39" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="167" t="s">
+      <c r="B39" s="165" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="168"/>
-      <c r="D39" s="168"/>
-      <c r="E39" s="169"/>
-      <c r="F39" s="167" t="s">
+      <c r="C39" s="166"/>
+      <c r="D39" s="166"/>
+      <c r="E39" s="167"/>
+      <c r="F39" s="165" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="170"/>
-      <c r="H39" s="170"/>
-      <c r="I39" s="170"/>
+      <c r="G39" s="168"/>
+      <c r="H39" s="168"/>
+      <c r="I39" s="168"/>
       <c r="J39" s="34"/>
       <c r="N39" s="36"/>
       <c r="O39" s="36"/>
@@ -2729,18 +2742,18 @@
       <c r="AD39" s="36"/>
     </row>
     <row r="40" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="164" t="s">
+      <c r="B40" s="162" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="165"/>
-      <c r="D40" s="165"/>
-      <c r="E40" s="166"/>
-      <c r="F40" s="164" t="s">
+      <c r="C40" s="163"/>
+      <c r="D40" s="163"/>
+      <c r="E40" s="164"/>
+      <c r="F40" s="162" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="165"/>
-      <c r="H40" s="165"/>
-      <c r="I40" s="165"/>
+      <c r="G40" s="163"/>
+      <c r="H40" s="163"/>
+      <c r="I40" s="163"/>
       <c r="J40" s="19"/>
     </row>
     <row r="41" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2800,18 +2813,18 @@
       <c r="J44" s="19"/>
     </row>
     <row r="45" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="164" t="s">
+      <c r="B45" s="162" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="165"/>
-      <c r="D45" s="165"/>
-      <c r="E45" s="166"/>
-      <c r="F45" s="164" t="s">
+      <c r="C45" s="163"/>
+      <c r="D45" s="163"/>
+      <c r="E45" s="164"/>
+      <c r="F45" s="162" t="s">
         <v>50</v>
       </c>
-      <c r="G45" s="165"/>
-      <c r="H45" s="165"/>
-      <c r="I45" s="166"/>
+      <c r="G45" s="163"/>
+      <c r="H45" s="163"/>
+      <c r="I45" s="164"/>
       <c r="J45" s="19"/>
     </row>
     <row r="46" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3128,10 +3141,10 @@
     <tabColor theme="8" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC52"/>
+  <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3155,446 +3168,446 @@
   <sheetData>
     <row r="1" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="56"/>
-      <c r="G1" s="161" t="s">
+      <c r="G1" s="159" t="s">
         <v>47</v>
       </c>
       <c r="N1" s="58"/>
     </row>
     <row r="2" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="89"/>
-      <c r="B2" s="119" t="s">
+      <c r="A2" s="88"/>
+      <c r="B2" s="117" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="122" t="s">
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="120" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
       <c r="N2" s="58"/>
     </row>
     <row r="3" spans="1:14" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="89"/>
-      <c r="B3" s="120" t="s">
+      <c r="A3" s="88"/>
+      <c r="B3" s="118" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="123" t="s">
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="121" t="s">
         <v>132</v>
       </c>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
       <c r="N3" s="58"/>
     </row>
-    <row r="4" spans="1:14" s="86" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="88"/>
-      <c r="B4" s="120" t="s">
+    <row r="4" spans="1:14" s="85" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="87"/>
+      <c r="B4" s="118" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="120"/>
-      <c r="H4" s="123" t="s">
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="121" t="s">
         <v>130</v>
       </c>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="120"/>
-      <c r="N4" s="84"/>
-    </row>
-    <row r="5" spans="1:14" s="86" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="87"/>
-      <c r="B5" s="120" t="s">
+      <c r="I4" s="118"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="118"/>
+      <c r="M4" s="118"/>
+      <c r="N4" s="83"/>
+    </row>
+    <row r="5" spans="1:14" s="85" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="86"/>
+      <c r="B5" s="118" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="123" t="s">
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="121" t="s">
         <v>128</v>
       </c>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="120"/>
-      <c r="N5" s="84"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="118"/>
+      <c r="K5" s="118"/>
+      <c r="L5" s="118"/>
+      <c r="M5" s="118"/>
+      <c r="N5" s="83"/>
     </row>
     <row r="6" spans="1:14" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="56"/>
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="108" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="96" t="s">
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="97"/>
-      <c r="J6" s="97"/>
-      <c r="K6" s="97"/>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="96"/>
       <c r="N6" s="58"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="56"/>
-      <c r="B7" s="113" t="s">
+      <c r="B7" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="124"/>
-      <c r="D7" s="124"/>
-      <c r="E7" s="124"/>
-      <c r="F7" s="124"/>
-      <c r="G7" s="124"/>
-      <c r="H7" s="99" t="s">
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="96"/>
       <c r="N7" s="58"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="56"/>
-      <c r="B8" s="125" t="s">
+      <c r="B8" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="125"/>
-      <c r="H8" s="101" t="s">
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
       <c r="N8" s="58"/>
     </row>
     <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="56"/>
-      <c r="B9" s="126" t="s">
+      <c r="B9" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="126"/>
-      <c r="D9" s="126"/>
-      <c r="E9" s="126"/>
-      <c r="F9" s="126"/>
-      <c r="G9" s="126"/>
-      <c r="H9" s="103" t="s">
+      <c r="C9" s="124"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="124"/>
+      <c r="F9" s="124"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="101" t="s">
         <v>136</v>
       </c>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="98"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="98"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="96"/>
+      <c r="M9" s="96"/>
       <c r="N9" s="58"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="56"/>
-      <c r="B10" s="113" t="s">
+      <c r="B10" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="113"/>
-      <c r="G10" s="113"/>
-      <c r="H10" s="99" t="s">
+      <c r="C10" s="111"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="98"/>
-      <c r="J10" s="98"/>
-      <c r="K10" s="98"/>
-      <c r="L10" s="98"/>
-      <c r="M10" s="98"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="96"/>
+      <c r="M10" s="96"/>
       <c r="N10" s="58"/>
     </row>
     <row r="11" spans="1:14" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="56"/>
-      <c r="B11" s="102" t="s">
+      <c r="B11" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="155" t="s">
+      <c r="C11" s="100"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="100"/>
+      <c r="G11" s="116"/>
+      <c r="H11" s="153" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="102"/>
-      <c r="J11" s="102"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="102"/>
-      <c r="M11" s="102"/>
+      <c r="I11" s="100"/>
+      <c r="J11" s="100"/>
+      <c r="K11" s="100"/>
+      <c r="L11" s="100"/>
+      <c r="M11" s="100"/>
       <c r="N11" s="58"/>
     </row>
     <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="56"/>
-      <c r="B12" s="126" t="s">
+      <c r="B12" s="124" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="126"/>
-      <c r="D12" s="126"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="126"/>
-      <c r="H12" s="96" t="s">
+      <c r="C12" s="124"/>
+      <c r="D12" s="124"/>
+      <c r="E12" s="124"/>
+      <c r="F12" s="124"/>
+      <c r="G12" s="124"/>
+      <c r="H12" s="94" t="s">
         <v>125</v>
       </c>
-      <c r="I12" s="97"/>
-      <c r="J12" s="97"/>
-      <c r="K12" s="97"/>
-      <c r="L12" s="98"/>
-      <c r="M12" s="98"/>
+      <c r="I12" s="95"/>
+      <c r="J12" s="95"/>
+      <c r="K12" s="95"/>
+      <c r="L12" s="96"/>
+      <c r="M12" s="96"/>
       <c r="N12" s="58"/>
     </row>
     <row r="13" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="56"/>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="113"/>
-      <c r="H13" s="99" t="s">
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100"/>
-      <c r="K13" s="100"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="98"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="96"/>
+      <c r="M13" s="96"/>
       <c r="N13" s="58"/>
     </row>
     <row r="14" spans="1:14" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="56"/>
-      <c r="B14" s="102" t="s">
+      <c r="B14" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="102"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="118"/>
-      <c r="H14" s="155" t="s">
+      <c r="C14" s="100"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="116"/>
+      <c r="H14" s="153" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="102"/>
-      <c r="J14" s="102"/>
-      <c r="K14" s="102"/>
-      <c r="L14" s="102"/>
-      <c r="M14" s="102"/>
+      <c r="I14" s="100"/>
+      <c r="J14" s="100"/>
+      <c r="K14" s="100"/>
+      <c r="L14" s="100"/>
+      <c r="M14" s="100"/>
       <c r="N14" s="58"/>
     </row>
     <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="85"/>
-      <c r="B15" s="104" t="s">
+      <c r="A15" s="84"/>
+      <c r="B15" s="102" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="105" t="s">
+      <c r="C15" s="102"/>
+      <c r="D15" s="103" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105" t="s">
+      <c r="E15" s="103"/>
+      <c r="F15" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="G15" s="105"/>
-      <c r="H15" s="106" t="s">
+      <c r="G15" s="103"/>
+      <c r="H15" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="I15" s="105"/>
-      <c r="J15" s="127" t="s">
+      <c r="I15" s="103"/>
+      <c r="J15" s="125" t="s">
         <v>109</v>
       </c>
-      <c r="K15" s="127"/>
-      <c r="L15" s="151" t="s">
+      <c r="K15" s="125"/>
+      <c r="L15" s="149" t="s">
         <v>110</v>
       </c>
-      <c r="M15" s="151"/>
+      <c r="M15" s="149"/>
       <c r="N15" s="58"/>
     </row>
     <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="56"/>
-      <c r="B16" s="118" t="s">
+      <c r="B16" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="107"/>
-      <c r="D16" s="156" t="s">
+      <c r="C16" s="105"/>
+      <c r="D16" s="154" t="s">
         <v>107</v>
       </c>
-      <c r="E16" s="108"/>
-      <c r="F16" s="144" t="s">
+      <c r="E16" s="106"/>
+      <c r="F16" s="142" t="s">
         <v>108</v>
       </c>
-      <c r="G16" s="108"/>
-      <c r="H16" s="159" t="s">
+      <c r="G16" s="106"/>
+      <c r="H16" s="157" t="s">
         <v>106</v>
       </c>
-      <c r="I16" s="108"/>
-      <c r="J16" s="109" t="s">
+      <c r="I16" s="106"/>
+      <c r="J16" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="K16" s="109"/>
-      <c r="L16" s="152" t="s">
+      <c r="K16" s="107"/>
+      <c r="L16" s="150" t="s">
         <v>105</v>
       </c>
-      <c r="M16" s="152"/>
+      <c r="M16" s="150"/>
       <c r="N16" s="58"/>
     </row>
     <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="56"/>
-      <c r="B17" s="126" t="s">
+      <c r="B17" s="124" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="126"/>
-      <c r="D17" s="126" t="s">
+      <c r="C17" s="124"/>
+      <c r="D17" s="124" t="s">
         <v>123</v>
       </c>
-      <c r="E17" s="130"/>
-      <c r="F17" s="143" t="s">
+      <c r="E17" s="128"/>
+      <c r="F17" s="141" t="s">
         <v>122</v>
       </c>
-      <c r="G17" s="143"/>
-      <c r="H17" s="103" t="s">
+      <c r="G17" s="141"/>
+      <c r="H17" s="101" t="s">
         <v>121</v>
       </c>
-      <c r="I17" s="98"/>
-      <c r="J17" s="111" t="s">
+      <c r="I17" s="96"/>
+      <c r="J17" s="109" t="s">
         <v>120</v>
       </c>
-      <c r="K17" s="98"/>
-      <c r="L17" s="153" t="s">
+      <c r="K17" s="96"/>
+      <c r="L17" s="151" t="s">
         <v>119</v>
       </c>
-      <c r="M17" s="154"/>
+      <c r="M17" s="152"/>
       <c r="N17" s="58"/>
     </row>
     <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="56"/>
-      <c r="B18" s="102" t="s">
+      <c r="B18" s="100" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="125"/>
-      <c r="D18" s="157" t="s">
+      <c r="C18" s="123"/>
+      <c r="D18" s="155" t="s">
         <v>117</v>
       </c>
-      <c r="E18" s="109"/>
-      <c r="F18" s="158" t="s">
+      <c r="E18" s="107"/>
+      <c r="F18" s="156" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="144"/>
-      <c r="H18" s="159" t="s">
+      <c r="G18" s="142"/>
+      <c r="H18" s="157" t="s">
         <v>116</v>
       </c>
-      <c r="I18" s="109"/>
-      <c r="J18" s="157" t="s">
+      <c r="I18" s="107"/>
+      <c r="J18" s="155" t="s">
         <v>115</v>
       </c>
-      <c r="K18" s="109"/>
-      <c r="L18" s="152" t="s">
+      <c r="K18" s="107"/>
+      <c r="L18" s="150" t="s">
         <v>114</v>
       </c>
-      <c r="M18" s="152"/>
+      <c r="M18" s="150"/>
       <c r="N18" s="58"/>
     </row>
     <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="56"/>
-      <c r="B19" s="131" t="s">
+      <c r="B19" s="129" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="131"/>
-      <c r="D19" s="131" t="s">
+      <c r="C19" s="129"/>
+      <c r="D19" s="129" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="131"/>
-      <c r="F19" s="145"/>
-      <c r="G19" s="145"/>
-      <c r="H19" s="148" t="s">
+      <c r="E19" s="129"/>
+      <c r="F19" s="143"/>
+      <c r="G19" s="143"/>
+      <c r="H19" s="146" t="s">
         <v>137</v>
       </c>
-      <c r="I19" s="128"/>
-      <c r="J19" s="126" t="s">
+      <c r="I19" s="126"/>
+      <c r="J19" s="124" t="s">
         <v>101</v>
       </c>
-      <c r="K19" s="126"/>
-      <c r="L19" s="126"/>
-      <c r="M19" s="126"/>
+      <c r="K19" s="124"/>
+      <c r="L19" s="124"/>
+      <c r="M19" s="124"/>
       <c r="N19" s="58"/>
     </row>
     <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="56"/>
-      <c r="B20" s="156" t="s">
+      <c r="B20" s="154" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="112"/>
-      <c r="D20" s="129" t="s">
+      <c r="C20" s="110"/>
+      <c r="D20" s="127" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="129"/>
-      <c r="F20" s="146"/>
-      <c r="G20" s="146"/>
-      <c r="H20" s="160" t="s">
+      <c r="E20" s="127"/>
+      <c r="F20" s="144"/>
+      <c r="G20" s="144"/>
+      <c r="H20" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="I20" s="108"/>
-      <c r="J20" s="113" t="s">
+      <c r="I20" s="106"/>
+      <c r="J20" s="111" t="s">
         <v>100</v>
       </c>
-      <c r="K20" s="114"/>
-      <c r="L20" s="109"/>
-      <c r="M20" s="109"/>
+      <c r="K20" s="112"/>
+      <c r="L20" s="107"/>
+      <c r="M20" s="107"/>
       <c r="N20" s="58"/>
     </row>
-    <row r="21" spans="1:29" s="82" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="95"/>
-      <c r="B21" s="115"/>
-      <c r="C21" s="115"/>
-      <c r="D21" s="115"/>
-      <c r="E21" s="115"/>
-      <c r="F21" s="115"/>
-      <c r="G21" s="147"/>
-      <c r="H21" s="149"/>
-      <c r="I21" s="116"/>
-      <c r="J21" s="116"/>
-      <c r="K21" s="116"/>
-      <c r="L21" s="116"/>
-      <c r="M21" s="117"/>
-      <c r="N21" s="83"/>
+    <row r="21" spans="1:29" s="81" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="93"/>
+      <c r="B21" s="113"/>
+      <c r="C21" s="113"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="113"/>
+      <c r="G21" s="145"/>
+      <c r="H21" s="147"/>
+      <c r="I21" s="114"/>
+      <c r="J21" s="114"/>
+      <c r="K21" s="114"/>
+      <c r="L21" s="114"/>
+      <c r="M21" s="115"/>
+      <c r="N21" s="82"/>
       <c r="S21"/>
       <c r="T21"/>
       <c r="U21"/>
@@ -3612,26 +3625,26 @@
       <c r="B22" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="132" t="s">
+      <c r="C22" s="130" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="132"/>
-      <c r="E22" s="132"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="132"/>
+      <c r="D22" s="130"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="148"/>
+      <c r="G22" s="130"/>
       <c r="H22" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="I22" s="81" t="s">
+      <c r="I22" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="J22" s="80" t="s">
+      <c r="J22" s="79" t="s">
         <v>95</v>
       </c>
-      <c r="K22" s="132" t="s">
+      <c r="K22" s="130" t="s">
         <v>94</v>
       </c>
-      <c r="L22" s="132"/>
+      <c r="L22" s="130"/>
       <c r="M22" s="60" t="s">
         <v>93</v>
       </c>
@@ -3639,366 +3652,414 @@
     </row>
     <row r="23" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="56"/>
-      <c r="B23" s="139" t="s">
+      <c r="B23" s="137" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="200" t="s">
+      <c r="C23" s="198" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="200"/>
-      <c r="E23" s="200"/>
-      <c r="F23" s="200"/>
-      <c r="G23" s="140"/>
-      <c r="H23" s="141" t="s">
+      <c r="D23" s="198"/>
+      <c r="E23" s="198"/>
+      <c r="F23" s="198"/>
+      <c r="G23" s="138"/>
+      <c r="H23" s="139" t="s">
         <v>90</v>
       </c>
-      <c r="I23" s="79" t="s">
+      <c r="I23" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="J23" s="78">
+      <c r="J23" s="77">
         <v>14</v>
       </c>
-      <c r="K23" s="201" t="s">
+      <c r="K23" s="199" t="s">
         <v>89</v>
       </c>
-      <c r="L23" s="201"/>
-      <c r="M23" s="77" t="s">
+      <c r="L23" s="199"/>
+      <c r="M23" s="76" t="s">
         <v>86</v>
       </c>
       <c r="N23" s="58"/>
     </row>
     <row r="24" spans="1:29" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="56"/>
-      <c r="C24" s="137"/>
-      <c r="D24" s="137"/>
-      <c r="E24" s="137"/>
-      <c r="F24" s="137"/>
-      <c r="G24" s="137"/>
-      <c r="H24" s="138" t="s">
+      <c r="C24" s="135"/>
+      <c r="D24" s="135"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="135"/>
+      <c r="G24" s="135"/>
+      <c r="H24" s="136" t="s">
         <v>88</v>
       </c>
-      <c r="I24" s="76" t="s">
+      <c r="I24" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="J24" s="75">
+      <c r="J24" s="74">
         <v>14</v>
       </c>
-      <c r="K24" s="142" t="s">
+      <c r="K24" s="140" t="s">
         <v>47</v>
       </c>
-      <c r="L24" s="142"/>
-      <c r="M24" s="90" t="s">
+      <c r="L24" s="140"/>
+      <c r="M24" s="89" t="s">
         <v>86</v>
       </c>
       <c r="N24" s="58"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A25" s="56"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
       <c r="F25" s="59"/>
       <c r="G25" s="59"/>
       <c r="H25" s="63"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="74"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="68"/>
+      <c r="L25" s="68"/>
+      <c r="M25" s="73"/>
       <c r="N25" s="58"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A26" s="56"/>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
       <c r="F26" s="59"/>
       <c r="G26" s="59"/>
       <c r="H26" s="63"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="69"/>
-      <c r="M26" s="74"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="68"/>
+      <c r="M26" s="73"/>
       <c r="N26" s="58"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A27" s="56"/>
-      <c r="B27" s="69"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
       <c r="F27" s="59"/>
       <c r="G27" s="59"/>
       <c r="H27" s="63"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="69"/>
-      <c r="L27" s="69"/>
-      <c r="M27" s="74"/>
+      <c r="I27" s="73"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="68"/>
+      <c r="M27" s="73"/>
       <c r="N27" s="58"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A28" s="56"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
       <c r="F28" s="59"/>
       <c r="G28" s="59"/>
       <c r="H28" s="63"/>
-      <c r="I28" s="74"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="74"/>
+      <c r="I28" s="73"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="68"/>
+      <c r="L28" s="68"/>
+      <c r="M28" s="73"/>
       <c r="N28" s="58"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A29" s="56"/>
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
       <c r="F29" s="59"/>
       <c r="G29" s="59"/>
       <c r="H29" s="63"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="69"/>
-      <c r="M29" s="74"/>
+      <c r="I29" s="73"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="68"/>
+      <c r="M29" s="73"/>
       <c r="N29" s="58"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A30" s="56"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
       <c r="F30" s="59"/>
       <c r="G30" s="59"/>
       <c r="H30" s="63"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="69"/>
-      <c r="M30" s="74"/>
+      <c r="I30" s="73"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="68"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="73"/>
       <c r="N30" s="58"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A31" s="56"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
       <c r="F31" s="59"/>
       <c r="G31" s="59"/>
       <c r="H31" s="63"/>
-      <c r="I31" s="74"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="74"/>
+      <c r="I31" s="73"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="68"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="73"/>
       <c r="N31" s="58"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A32" s="56"/>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
       <c r="F32" s="59"/>
       <c r="G32" s="59"/>
       <c r="H32" s="63"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="74"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="73"/>
       <c r="N32" s="58"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" s="56"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
       <c r="F33" s="59"/>
       <c r="G33" s="59"/>
       <c r="H33" s="63"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="74"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="68"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="73"/>
       <c r="N33" s="58"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34" s="56"/>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
       <c r="F34" s="59"/>
       <c r="G34" s="59"/>
       <c r="H34" s="63"/>
-      <c r="I34" s="74"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
-      <c r="L34" s="69"/>
-      <c r="M34" s="74"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="68"/>
+      <c r="K34" s="68"/>
+      <c r="L34" s="68"/>
+      <c r="M34" s="73"/>
       <c r="N34" s="58"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35" s="56"/>
-      <c r="B35" s="69"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
       <c r="F35" s="59"/>
       <c r="G35" s="59"/>
       <c r="H35" s="63"/>
-      <c r="I35" s="74"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="69"/>
-      <c r="L35" s="69"/>
-      <c r="M35" s="74"/>
+      <c r="I35" s="73"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="68"/>
+      <c r="L35" s="68"/>
+      <c r="M35" s="73"/>
       <c r="N35" s="58"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="56"/>
-      <c r="B36" s="69"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
       <c r="F36" s="59"/>
       <c r="G36" s="59"/>
-      <c r="H36" s="63"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="69"/>
-      <c r="K36" s="69"/>
-      <c r="L36" s="69"/>
-      <c r="M36" s="74"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="61"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="68"/>
+      <c r="M36" s="61"/>
       <c r="N36" s="58"/>
     </row>
-    <row r="37" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="56"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="61"/>
-      <c r="J37" s="57"/>
-      <c r="K37" s="57"/>
-      <c r="L37" s="69"/>
-      <c r="M37" s="61"/>
+      <c r="B37" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="132" t="s">
+        <v>85</v>
+      </c>
+      <c r="J37" s="131"/>
+      <c r="K37" s="131"/>
+      <c r="L37" s="131"/>
+      <c r="M37" s="131"/>
       <c r="N37" s="58"/>
     </row>
-    <row r="38" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="56"/>
       <c r="B38" s="92" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="73"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="72"/>
-      <c r="G38" s="72"/>
-      <c r="H38" s="71"/>
-      <c r="I38" s="134" t="s">
-        <v>85</v>
-      </c>
-      <c r="J38" s="133"/>
-      <c r="K38" s="133"/>
-      <c r="L38" s="133"/>
-      <c r="M38" s="133"/>
+        <v>84</v>
+      </c>
+      <c r="C38" s="68"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="59"/>
+      <c r="H38" s="61"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="K38" s="57"/>
+      <c r="L38" s="68"/>
+      <c r="M38" s="61"/>
       <c r="N38" s="58"/>
     </row>
     <row r="39" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="56"/>
-      <c r="B39" s="93" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
+      <c r="B39" s="92" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
       <c r="F39" s="59"/>
       <c r="G39" s="59"/>
       <c r="H39" s="61"/>
-      <c r="I39" s="70"/>
-      <c r="J39" s="57"/>
+      <c r="I39" s="58"/>
       <c r="K39" s="57"/>
-      <c r="L39" s="69"/>
+      <c r="L39" s="68"/>
       <c r="M39" s="61"/>
       <c r="N39" s="58"/>
     </row>
     <row r="40" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="56"/>
-      <c r="B40" s="93" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="69"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="69"/>
+      <c r="B40" s="92" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
       <c r="F40" s="59"/>
       <c r="G40" s="59"/>
       <c r="H40" s="61"/>
-      <c r="I40" s="70"/>
+      <c r="I40" s="69"/>
       <c r="J40" s="57"/>
       <c r="K40" s="57"/>
-      <c r="L40" s="69"/>
+      <c r="L40" s="68"/>
       <c r="M40" s="61"/>
       <c r="N40" s="58"/>
     </row>
     <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="56"/>
-      <c r="B41" s="93" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="69"/>
+      <c r="B41" s="201" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
       <c r="F41" s="59"/>
       <c r="G41" s="59"/>
       <c r="H41" s="61"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="57"/>
+      <c r="I41" s="69"/>
+      <c r="J41" s="204" t="s">
+        <v>47</v>
+      </c>
       <c r="K41" s="57"/>
-      <c r="L41" s="69"/>
+      <c r="L41" s="68"/>
       <c r="M41" s="61"/>
       <c r="N41" s="58"/>
     </row>
-    <row r="42" spans="1:14" s="64" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="68"/>
-      <c r="B42" s="94" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="67"/>
-      <c r="F42" s="66"/>
-      <c r="G42" s="66"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="135"/>
-      <c r="J42" s="136"/>
-      <c r="K42" s="136"/>
-      <c r="L42" s="136"/>
-      <c r="M42" s="136"/>
-      <c r="N42" s="91"/>
-    </row>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="49" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="50" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="51" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="52" ht="2.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="42" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="202"/>
+      <c r="B42" s="206"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="69"/>
+      <c r="K42" s="57"/>
+      <c r="L42" s="68"/>
+      <c r="M42" s="61"/>
+      <c r="N42" s="58"/>
+    </row>
+    <row r="43" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="202"/>
+      <c r="B43" s="206"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="59"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="69"/>
+      <c r="J43" s="204"/>
+      <c r="K43" s="57"/>
+      <c r="L43" s="68"/>
+      <c r="M43" s="61"/>
+      <c r="N43" s="58"/>
+    </row>
+    <row r="44" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="202"/>
+      <c r="B44" s="206"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="61"/>
+      <c r="I44" s="69"/>
+      <c r="J44" s="204"/>
+      <c r="K44" s="57"/>
+      <c r="L44" s="68"/>
+      <c r="M44" s="61"/>
+      <c r="N44" s="58"/>
+    </row>
+    <row r="45" spans="1:14" s="64" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="200"/>
+      <c r="B45" s="203"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="66"/>
+      <c r="G45" s="66"/>
+      <c r="H45" s="65"/>
+      <c r="I45" s="133"/>
+      <c r="J45" s="205"/>
+      <c r="K45" s="134"/>
+      <c r="L45" s="134"/>
+      <c r="M45" s="134"/>
+      <c r="N45" s="90"/>
+    </row>
+    <row r="46" spans="1:14" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="202"/>
+      <c r="C46" s="202"/>
+    </row>
+    <row r="47" spans="1:14" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="48" spans="1:14" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="49" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="50" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="55" ht="2.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C23:F23"/>

</xml_diff>

<commit_message>
trying to fix bug special styling
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBFC8ED-303F-4FD9-9876-C4E7EDA9BB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C928E85C-D89A-46EB-BDD3-8A568B113B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -23,31 +23,33 @@
     <definedName name="MID_Contract">Export_Contract!$E$1</definedName>
     <definedName name="MID_Invoice">Invoice!$G$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$N$50</definedName>
-    <definedName name="Seal_agent_end">Export_Contract!$H$51</definedName>
-    <definedName name="Seal_agent_start">Export_Contract!$G$41</definedName>
-    <definedName name="Seal_seller_end">Export_Contract!$C$51</definedName>
-    <definedName name="Seal_seller_start">Export_Contract!$C$43</definedName>
-    <definedName name="Sign_agent_end">Export_Contract!$G$51</definedName>
-    <definedName name="Sign_agent_start">Export_Contract!$G$49</definedName>
-    <definedName name="Sign_seller_start">Export_Contract!$C$49</definedName>
-    <definedName name="Адреса_банк_получателя">Export_Contract!$B$33</definedName>
-    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$34</definedName>
-    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$35</definedName>
-    <definedName name="Адреса_подпись">Export_Contract!$B$50</definedName>
-    <definedName name="Адреса_покупатель">Export_Contract!$B$39</definedName>
-    <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$40</definedName>
-    <definedName name="Адреса_покупатель_банк">Export_Contract!$B$42</definedName>
-    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$B$45</definedName>
-    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$B$44</definedName>
-    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$B$46</definedName>
-    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$B$47</definedName>
-    <definedName name="Адреса_покупатель_счет">Export_Contract!$B$48</definedName>
-    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$B$36</definedName>
-    <definedName name="Адреса_получатель_счет">Export_Contract!$B$37</definedName>
-    <definedName name="Адреса_продавец">Export_Contract!$B$31</definedName>
-    <definedName name="Адреса_продавец_адрес">Export_Contract!$B$32</definedName>
-    <definedName name="Доставка_порт">Export_Contract!$B$25</definedName>
-    <definedName name="Доставка_условия">Export_Contract!$B$24</definedName>
+    <definedName name="Seal_agent_end">Export_Contract!$H$54</definedName>
+    <definedName name="Seal_agent_start">Export_Contract!$G$44</definedName>
+    <definedName name="Seal_seller_end">Export_Contract!$C$54</definedName>
+    <definedName name="Seal_seller_start">Export_Contract!$C$46</definedName>
+    <definedName name="Sign_agent_end">Export_Contract!$G$54</definedName>
+    <definedName name="Sign_agent_start">Export_Contract!$G$52</definedName>
+    <definedName name="Sign_seller_start">Export_Contract!$C$52</definedName>
+    <definedName name="Адреса_банк_получателя">Export_Contract!$B$36</definedName>
+    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$37</definedName>
+    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$38</definedName>
+    <definedName name="Адреса_подпись">Export_Contract!$B$53</definedName>
+    <definedName name="Адреса_покупатель">Export_Contract!$B$42</definedName>
+    <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$43</definedName>
+    <definedName name="Адреса_покупатель_банк">Export_Contract!$B$45</definedName>
+    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$B$48</definedName>
+    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$B$47</definedName>
+    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$B$49</definedName>
+    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$B$50</definedName>
+    <definedName name="Адреса_покупатель_счет">Export_Contract!$B$51</definedName>
+    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$B$39</definedName>
+    <definedName name="Адреса_получатель_счет">Export_Contract!$B$40</definedName>
+    <definedName name="Адреса_продавец">Export_Contract!$B$34</definedName>
+    <definedName name="Адреса_продавец_адрес">Export_Contract!$B$35</definedName>
+    <definedName name="Доставка_дата">Export_Contract!$B$27</definedName>
+    <definedName name="Доставка_порт">Export_Contract!$B$28</definedName>
+    <definedName name="Доставка_приемка">Export_Contract!$B$26</definedName>
+    <definedName name="Доставка_условия">Export_Contract!$B$25</definedName>
     <definedName name="Инвойс">Invoice!$B$2</definedName>
     <definedName name="Инвойс_Bl_массив">Invoice!$B$23</definedName>
     <definedName name="Инвойс_банк_получателя">Invoice!$B$37</definedName>
@@ -75,6 +77,7 @@
     <definedName name="Инвойс_условия">Invoice!$B$20</definedName>
     <definedName name="Контракт">Export_Contract!$B$3</definedName>
     <definedName name="Контракт_дата">Export_Contract!$B$4</definedName>
+    <definedName name="Контракт_предмет_заголовки">Export_Contract!$B$18</definedName>
     <definedName name="Покупатель">Export_Contract!$B$12</definedName>
     <definedName name="Покупатель_адрес">Export_Contract!$B$13</definedName>
     <definedName name="Покупатель_представитель">Export_Contract!$B$14</definedName>
@@ -84,10 +87,11 @@
     <definedName name="Продавец_адрес">Export_Contract!$B$8</definedName>
     <definedName name="Продавец_подписант">Export_Contract!$B$10</definedName>
     <definedName name="Продавец_представитель">Export_Contract!$B$9</definedName>
-    <definedName name="Прочие_условия_описание">Export_Contract!$B$28</definedName>
-    <definedName name="Сертификаты_обязательства">Export_Contract!$B$26</definedName>
+    <definedName name="Прочие_условия_описание">Export_Contract!$B$31</definedName>
+    <definedName name="Сертификаты_обязательства">Export_Contract!$B$29</definedName>
     <definedName name="Соглашение">Export_Contract!$B$2</definedName>
-    <definedName name="Цена_всего">Export_Contract!$B$22</definedName>
+    <definedName name="Цена_всего">Export_Contract!$B$23</definedName>
+    <definedName name="Цена_неком">Export_Contract!$B$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -110,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="139">
   <si>
     <t>Дополнительное соглашение № 146 от 10 марта 2023г.</t>
   </si>
@@ -862,7 +866,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="207">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1296,131 +1300,130 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1785,10 +1788,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AF87"/>
+  <dimension ref="B1:AF90"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A23" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1840,18 +1843,18 @@
       <c r="I1" s="160"/>
     </row>
     <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="192" t="s">
+      <c r="B2" s="198" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="194"/>
-      <c r="F2" s="192" t="s">
+      <c r="C2" s="199"/>
+      <c r="D2" s="199"/>
+      <c r="E2" s="200"/>
+      <c r="F2" s="198" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="193"/>
-      <c r="H2" s="193"/>
-      <c r="I2" s="193"/>
+      <c r="G2" s="199"/>
+      <c r="H2" s="199"/>
+      <c r="I2" s="199"/>
       <c r="J2" s="161"/>
       <c r="L2" s="11"/>
       <c r="N2" s="18"/>
@@ -1861,18 +1864,18 @@
       <c r="AD2" s="18"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="195" t="s">
+      <c r="B3" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="196"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="195" t="s">
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="203"/>
+      <c r="F3" s="201" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="196"/>
-      <c r="H3" s="196"/>
-      <c r="I3" s="196"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="202"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1889,18 +1892,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="195" t="s">
+      <c r="B4" s="201" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="196"/>
-      <c r="D4" s="196"/>
-      <c r="E4" s="197"/>
-      <c r="F4" s="195" t="s">
+      <c r="C4" s="202"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="196"/>
-      <c r="H4" s="196"/>
-      <c r="I4" s="196"/>
+      <c r="G4" s="202"/>
+      <c r="H4" s="202"/>
+      <c r="I4" s="202"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1921,18 +1924,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="189" t="s">
+      <c r="B5" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="190"/>
-      <c r="D5" s="190"/>
-      <c r="E5" s="191"/>
-      <c r="F5" s="189" t="s">
+      <c r="C5" s="196"/>
+      <c r="D5" s="196"/>
+      <c r="E5" s="197"/>
+      <c r="F5" s="195" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="190"/>
-      <c r="H5" s="190"/>
-      <c r="I5" s="190"/>
+      <c r="G5" s="196"/>
+      <c r="H5" s="196"/>
+      <c r="I5" s="196"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1941,18 +1944,18 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="169" t="s">
+      <c r="B6" s="175" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="170"/>
-      <c r="D6" s="170"/>
-      <c r="E6" s="171"/>
-      <c r="F6" s="169" t="s">
+      <c r="C6" s="176"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="177"/>
+      <c r="F6" s="175" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="170"/>
-      <c r="H6" s="170"/>
-      <c r="I6" s="170"/>
+      <c r="G6" s="176"/>
+      <c r="H6" s="176"/>
+      <c r="I6" s="176"/>
       <c r="J6" s="54"/>
       <c r="L6" s="55"/>
       <c r="O6" s="10"/>
@@ -1997,44 +2000,44 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="178" t="s">
+      <c r="B8" s="184" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="179"/>
-      <c r="D8" s="179"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="162" t="s">
+      <c r="C8" s="185"/>
+      <c r="D8" s="185"/>
+      <c r="E8" s="186"/>
+      <c r="F8" s="168" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="163"/>
-      <c r="H8" s="163"/>
-      <c r="I8" s="163"/>
+      <c r="G8" s="169"/>
+      <c r="H8" s="169"/>
+      <c r="I8" s="169"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="162" t="s">
+      <c r="B9" s="168" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="164"/>
-      <c r="F9" s="162" t="s">
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="170"/>
+      <c r="F9" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="163"/>
-      <c r="H9" s="163"/>
-      <c r="I9" s="164"/>
+      <c r="G9" s="169"/>
+      <c r="H9" s="169"/>
+      <c r="I9" s="170"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="162"/>
-      <c r="C10" s="163"/>
-      <c r="D10" s="163"/>
-      <c r="E10" s="164"/>
-      <c r="F10" s="162"/>
-      <c r="G10" s="163"/>
-      <c r="H10" s="163"/>
-      <c r="I10" s="164"/>
+      <c r="B10" s="168"/>
+      <c r="C10" s="169"/>
+      <c r="D10" s="169"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="168"/>
+      <c r="G10" s="169"/>
+      <c r="H10" s="169"/>
+      <c r="I10" s="170"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -2055,18 +2058,18 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="169" t="s">
+      <c r="B11" s="175" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="170"/>
-      <c r="D11" s="170"/>
-      <c r="E11" s="171"/>
-      <c r="F11" s="169" t="s">
+      <c r="C11" s="176"/>
+      <c r="D11" s="176"/>
+      <c r="E11" s="177"/>
+      <c r="F11" s="175" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="170"/>
-      <c r="H11" s="170"/>
-      <c r="I11" s="170"/>
+      <c r="G11" s="176"/>
+      <c r="H11" s="176"/>
+      <c r="I11" s="176"/>
       <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -2109,18 +2112,18 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="162" t="s">
+      <c r="B13" s="168" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="163"/>
-      <c r="D13" s="163"/>
-      <c r="E13" s="164"/>
-      <c r="F13" s="162" t="s">
+      <c r="C13" s="169"/>
+      <c r="D13" s="169"/>
+      <c r="E13" s="170"/>
+      <c r="F13" s="168" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="163"/>
-      <c r="H13" s="163"/>
-      <c r="I13" s="163"/>
+      <c r="G13" s="169"/>
+      <c r="H13" s="169"/>
+      <c r="I13" s="169"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2138,18 +2141,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="162" t="s">
+      <c r="B14" s="168" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="163"/>
-      <c r="D14" s="163"/>
-      <c r="E14" s="164"/>
-      <c r="F14" s="162" t="s">
+      <c r="C14" s="169"/>
+      <c r="D14" s="169"/>
+      <c r="E14" s="170"/>
+      <c r="F14" s="168" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="163"/>
-      <c r="H14" s="163"/>
-      <c r="I14" s="163"/>
+      <c r="G14" s="169"/>
+      <c r="H14" s="169"/>
+      <c r="I14" s="169"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2167,18 +2170,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="162" t="s">
+      <c r="B15" s="168" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="163"/>
-      <c r="D15" s="163"/>
-      <c r="E15" s="164"/>
-      <c r="F15" s="162" t="s">
+      <c r="C15" s="169"/>
+      <c r="D15" s="169"/>
+      <c r="E15" s="170"/>
+      <c r="F15" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="163"/>
-      <c r="H15" s="163"/>
-      <c r="I15" s="163"/>
+      <c r="G15" s="169"/>
+      <c r="H15" s="169"/>
+      <c r="I15" s="169"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2196,18 +2199,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="181" t="s">
+      <c r="B16" s="187" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
+      <c r="C16" s="188"/>
+      <c r="D16" s="188"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="181" t="s">
+      <c r="F16" s="187" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="183"/>
+      <c r="G16" s="188"/>
+      <c r="H16" s="188"/>
+      <c r="I16" s="189"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2225,18 +2228,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="162" t="s">
+      <c r="B17" s="190" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="184"/>
-      <c r="D17" s="184"/>
-      <c r="E17" s="185"/>
-      <c r="F17" s="186" t="s">
+      <c r="C17" s="191"/>
+      <c r="D17" s="191"/>
+      <c r="E17" s="192"/>
+      <c r="F17" s="190" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="184"/>
-      <c r="H17" s="184"/>
-      <c r="I17" s="184"/>
+      <c r="G17" s="191"/>
+      <c r="H17" s="191"/>
+      <c r="I17" s="192"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2254,18 +2257,18 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="187" t="s">
+      <c r="B18" s="193" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="188"/>
+      <c r="C18" s="194"/>
       <c r="D18" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="188" t="s">
+      <c r="E18" s="194" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="188"/>
-      <c r="G18" s="188"/>
+      <c r="F18" s="194"/>
+      <c r="G18" s="194"/>
       <c r="H18" s="23" t="s">
         <v>76</v>
       </c>
@@ -2289,18 +2292,18 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="172" t="s">
+      <c r="B19" s="178" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="173"/>
+      <c r="C19" s="179"/>
       <c r="D19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="174" t="s">
+      <c r="E19" s="180" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="174"/>
-      <c r="G19" s="174"/>
+      <c r="F19" s="180"/>
+      <c r="G19" s="180"/>
       <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2386,66 +2389,64 @@
       <c r="AC21" s="10"/>
       <c r="AD21" s="10"/>
     </row>
-    <row r="22" spans="2:30" s="30" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="19" t="s">
+    <row r="22" spans="2:30" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="2"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="10"/>
+    </row>
+    <row r="23" spans="2:30" s="30" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="19" t="s">
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="19"/>
-    </row>
-    <row r="23" spans="2:30" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="6" t="s">
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="19"/>
+    </row>
+    <row r="24" spans="2:30" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="6" t="s">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="22"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-      <c r="W23" s="10"/>
-      <c r="X23" s="10"/>
-      <c r="Y23" s="10"/>
-      <c r="Z23" s="10"/>
-      <c r="AA23" s="10"/>
-      <c r="AB23" s="10"/>
-      <c r="AC23" s="10"/>
-      <c r="AD23" s="10"/>
-    </row>
-    <row r="24" spans="2:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="175" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="176"/>
-      <c r="D24" s="176"/>
-      <c r="E24" s="177"/>
-      <c r="F24" s="175" t="s">
-        <v>32</v>
-      </c>
-      <c r="G24" s="176"/>
-      <c r="H24" s="176"/>
-      <c r="I24" s="176"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
       <c r="J24" s="22"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
@@ -2465,49 +2466,79 @@
       <c r="AC24" s="10"/>
       <c r="AD24" s="10"/>
     </row>
-    <row r="25" spans="2:30" s="30" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="162" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="163"/>
-      <c r="D25" s="163"/>
-      <c r="E25" s="164"/>
-      <c r="F25" s="162" t="s">
-        <v>80</v>
-      </c>
-      <c r="G25" s="163"/>
-      <c r="H25" s="163"/>
-      <c r="I25" s="163"/>
-      <c r="J25" s="19"/>
-    </row>
-    <row r="26" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="178" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="179"/>
-      <c r="D26" s="179"/>
-      <c r="E26" s="180"/>
-      <c r="F26" s="162" t="s">
-        <v>81</v>
-      </c>
-      <c r="G26" s="163"/>
-      <c r="H26" s="163"/>
-      <c r="I26" s="164"/>
-      <c r="J26" s="19"/>
-    </row>
-    <row r="27" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="169" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="170"/>
-      <c r="D27" s="170"/>
+    <row r="25" spans="2:30" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="181" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="182"/>
+      <c r="D25" s="182"/>
+      <c r="E25" s="183"/>
+      <c r="F25" s="181" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="182"/>
+      <c r="H25" s="182"/>
+      <c r="I25" s="182"/>
+      <c r="J25" s="22"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="10"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="10"/>
+      <c r="AD25" s="10"/>
+    </row>
+    <row r="26" spans="2:30" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="162" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="162"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="22"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="10"/>
+      <c r="AB26" s="10"/>
+      <c r="AC26" s="10"/>
+      <c r="AD26" s="10"/>
+    </row>
+    <row r="27" spans="2:30" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="162" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="32"/>
-      <c r="F27" s="169" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="170"/>
-      <c r="H27" s="170"/>
-      <c r="I27" s="171"/>
+      <c r="F27" s="162"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
       <c r="J27" s="22"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
@@ -2527,432 +2558,461 @@
       <c r="AC27" s="10"/>
       <c r="AD27" s="10"/>
     </row>
-    <row r="28" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="162" t="s">
+    <row r="28" spans="2:30" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="168" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="169"/>
+      <c r="D28" s="169"/>
+      <c r="E28" s="170"/>
+      <c r="F28" s="168" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" s="169"/>
+      <c r="H28" s="169"/>
+      <c r="I28" s="169"/>
+      <c r="J28" s="19"/>
+    </row>
+    <row r="29" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="184" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="185"/>
+      <c r="D29" s="185"/>
+      <c r="E29" s="186"/>
+      <c r="F29" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="169"/>
+      <c r="H29" s="169"/>
+      <c r="I29" s="170"/>
+      <c r="J29" s="19"/>
+    </row>
+    <row r="30" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="175" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="176"/>
+      <c r="D30" s="176"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="175" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="176"/>
+      <c r="H30" s="176"/>
+      <c r="I30" s="177"/>
+      <c r="J30" s="22"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="10"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="10"/>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="10"/>
+      <c r="AD30" s="10"/>
+    </row>
+    <row r="31" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="168" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="164"/>
-      <c r="F28" s="162" t="s">
+      <c r="C31" s="169"/>
+      <c r="D31" s="169"/>
+      <c r="E31" s="170"/>
+      <c r="F31" s="168" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="169" t="s">
+      <c r="G31" s="169"/>
+      <c r="H31" s="169"/>
+      <c r="I31" s="169"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="170"/>
-      <c r="D29" s="170"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="169" t="s">
+      <c r="C32" s="176"/>
+      <c r="D32" s="176"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="175" t="s">
         <v>37</v>
       </c>
-      <c r="G29" s="170"/>
-      <c r="H29" s="170"/>
-      <c r="I29" s="171"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="50" t="s">
+      <c r="G32" s="176"/>
+      <c r="H32" s="176"/>
+      <c r="I32" s="177"/>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="50" t="s">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="9"/>
-    </row>
-    <row r="31" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="165" t="s">
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="171" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="166"/>
-      <c r="D31" s="166"/>
-      <c r="E31" s="167"/>
-      <c r="F31" s="165" t="s">
+      <c r="C34" s="172"/>
+      <c r="D34" s="172"/>
+      <c r="E34" s="173"/>
+      <c r="F34" s="171" t="s">
         <v>7</v>
       </c>
-      <c r="G31" s="166"/>
-      <c r="H31" s="166"/>
-      <c r="I31" s="166"/>
-      <c r="J31" s="34"/>
-      <c r="N31" s="36"/>
-      <c r="O31" s="36"/>
-      <c r="P31" s="36"/>
-      <c r="Q31" s="36"/>
-      <c r="R31" s="36"/>
-      <c r="S31" s="36"/>
-      <c r="T31" s="36"/>
-      <c r="U31" s="36"/>
-      <c r="V31" s="36"/>
-      <c r="W31" s="36"/>
-      <c r="X31" s="36"/>
-      <c r="Y31" s="36"/>
-      <c r="Z31" s="36"/>
-      <c r="AA31" s="36"/>
-      <c r="AB31" s="36"/>
-      <c r="AC31" s="36"/>
-      <c r="AD31" s="36"/>
-    </row>
-    <row r="32" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="162" t="s">
+      <c r="G34" s="172"/>
+      <c r="H34" s="172"/>
+      <c r="I34" s="172"/>
+      <c r="J34" s="34"/>
+      <c r="N34" s="36"/>
+      <c r="O34" s="36"/>
+      <c r="P34" s="36"/>
+      <c r="Q34" s="36"/>
+      <c r="R34" s="36"/>
+      <c r="S34" s="36"/>
+      <c r="T34" s="36"/>
+      <c r="U34" s="36"/>
+      <c r="V34" s="36"/>
+      <c r="W34" s="36"/>
+      <c r="X34" s="36"/>
+      <c r="Y34" s="36"/>
+      <c r="Z34" s="36"/>
+      <c r="AA34" s="36"/>
+      <c r="AB34" s="36"/>
+      <c r="AC34" s="36"/>
+      <c r="AD34" s="36"/>
+    </row>
+    <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="163"/>
-      <c r="D32" s="163"/>
-      <c r="E32" s="164"/>
-      <c r="F32" s="162" t="s">
+      <c r="C35" s="169"/>
+      <c r="D35" s="169"/>
+      <c r="E35" s="170"/>
+      <c r="F35" s="168" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="163"/>
-      <c r="H32" s="163"/>
-      <c r="I32" s="163"/>
-      <c r="J32" s="19"/>
-    </row>
-    <row r="33" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="162" t="s">
+      <c r="G35" s="169"/>
+      <c r="H35" s="169"/>
+      <c r="I35" s="169"/>
+      <c r="J35" s="19"/>
+    </row>
+    <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="168" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="163"/>
-      <c r="D33" s="163"/>
-      <c r="E33" s="164"/>
-      <c r="F33" s="162" t="s">
+      <c r="C36" s="169"/>
+      <c r="D36" s="169"/>
+      <c r="E36" s="170"/>
+      <c r="F36" s="168" t="s">
         <v>40</v>
       </c>
-      <c r="G33" s="163"/>
-      <c r="H33" s="163"/>
-      <c r="I33" s="163"/>
-      <c r="J33" s="19"/>
-    </row>
-    <row r="34" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="162" t="s">
+      <c r="G36" s="169"/>
+      <c r="H36" s="169"/>
+      <c r="I36" s="169"/>
+      <c r="J36" s="19"/>
+    </row>
+    <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="168" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="163"/>
-      <c r="D34" s="163"/>
-      <c r="E34" s="164"/>
-      <c r="F34" s="162" t="s">
+      <c r="C37" s="169"/>
+      <c r="D37" s="169"/>
+      <c r="E37" s="170"/>
+      <c r="F37" s="168" t="s">
         <v>41</v>
       </c>
-      <c r="G34" s="163"/>
-      <c r="H34" s="163"/>
-      <c r="I34" s="163"/>
-      <c r="J34" s="19"/>
-    </row>
-    <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="162" t="s">
+      <c r="G37" s="169"/>
+      <c r="H37" s="169"/>
+      <c r="I37" s="169"/>
+      <c r="J37" s="19"/>
+    </row>
+    <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="163"/>
-      <c r="D35" s="163"/>
-      <c r="E35" s="164"/>
-      <c r="F35" s="162" t="s">
+      <c r="C38" s="169"/>
+      <c r="D38" s="169"/>
+      <c r="E38" s="170"/>
+      <c r="F38" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="G35" s="163"/>
-      <c r="H35" s="163"/>
-      <c r="I35" s="163"/>
-      <c r="J35" s="19"/>
-    </row>
-    <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="162" t="s">
+      <c r="G38" s="169"/>
+      <c r="H38" s="169"/>
+      <c r="I38" s="169"/>
+      <c r="J38" s="19"/>
+    </row>
+    <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="168" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="163"/>
-      <c r="D36" s="163"/>
-      <c r="E36" s="164"/>
-      <c r="F36" s="162" t="s">
+      <c r="C39" s="169"/>
+      <c r="D39" s="169"/>
+      <c r="E39" s="170"/>
+      <c r="F39" s="168" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="163"/>
-      <c r="H36" s="163"/>
-      <c r="I36" s="163"/>
-      <c r="J36" s="19"/>
-    </row>
-    <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="162" t="s">
+      <c r="G39" s="169"/>
+      <c r="H39" s="169"/>
+      <c r="I39" s="169"/>
+      <c r="J39" s="19"/>
+    </row>
+    <row r="40" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="168" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="163"/>
-      <c r="D37" s="163"/>
-      <c r="E37" s="164"/>
-      <c r="F37" s="162" t="s">
+      <c r="C40" s="169"/>
+      <c r="D40" s="169"/>
+      <c r="E40" s="170"/>
+      <c r="F40" s="168" t="s">
         <v>46</v>
       </c>
-      <c r="G37" s="163"/>
-      <c r="H37" s="163"/>
-      <c r="I37" s="163"/>
-      <c r="J37" s="19"/>
-    </row>
-    <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="62" t="s">
+      <c r="G40" s="169"/>
+      <c r="H40" s="169"/>
+      <c r="I40" s="169"/>
+      <c r="J40" s="19"/>
+    </row>
+    <row r="41" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="62" t="s">
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="19"/>
-    </row>
-    <row r="39" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="165" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="166"/>
-      <c r="D39" s="166"/>
-      <c r="E39" s="167"/>
-      <c r="F39" s="165" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="168"/>
-      <c r="H39" s="168"/>
-      <c r="I39" s="168"/>
-      <c r="J39" s="34"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="36"/>
-      <c r="R39" s="36"/>
-      <c r="S39" s="36"/>
-      <c r="T39" s="36"/>
-      <c r="U39" s="36"/>
-      <c r="V39" s="36"/>
-      <c r="W39" s="36"/>
-      <c r="X39" s="36"/>
-      <c r="Y39" s="36"/>
-      <c r="Z39" s="36"/>
-      <c r="AA39" s="36"/>
-      <c r="AB39" s="36"/>
-      <c r="AC39" s="36"/>
-      <c r="AD39" s="36"/>
-    </row>
-    <row r="40" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="162" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" s="163"/>
-      <c r="D40" s="163"/>
-      <c r="E40" s="164"/>
-      <c r="F40" s="162" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" s="163"/>
-      <c r="H40" s="163"/>
-      <c r="I40" s="163"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="41" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="19"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="20" t="s">
-        <v>47</v>
-      </c>
+      <c r="G41" s="20"/>
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
       <c r="J41" s="19"/>
     </row>
-    <row r="42" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="27" t="s">
+    <row r="42" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="171" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="172"/>
+      <c r="D42" s="172"/>
+      <c r="E42" s="173"/>
+      <c r="F42" s="171" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="174"/>
+      <c r="H42" s="174"/>
+      <c r="I42" s="174"/>
+      <c r="J42" s="34"/>
+      <c r="N42" s="36"/>
+      <c r="O42" s="36"/>
+      <c r="P42" s="36"/>
+      <c r="Q42" s="36"/>
+      <c r="R42" s="36"/>
+      <c r="S42" s="36"/>
+      <c r="T42" s="36"/>
+      <c r="U42" s="36"/>
+      <c r="V42" s="36"/>
+      <c r="W42" s="36"/>
+      <c r="X42" s="36"/>
+      <c r="Y42" s="36"/>
+      <c r="Z42" s="36"/>
+      <c r="AA42" s="36"/>
+      <c r="AB42" s="36"/>
+      <c r="AC42" s="36"/>
+      <c r="AD42" s="36"/>
+    </row>
+    <row r="43" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B43" s="168" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="169"/>
+      <c r="D43" s="169"/>
+      <c r="E43" s="170"/>
+      <c r="F43" s="168" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="169"/>
+      <c r="H43" s="169"/>
+      <c r="I43" s="169"/>
+      <c r="J43" s="19"/>
+    </row>
+    <row r="44" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B44" s="19"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="19"/>
+    </row>
+    <row r="45" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="27" t="s">
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="G42" s="28"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="39"/>
-      <c r="C43" s="31" t="s">
+      <c r="G45" s="28"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="19"/>
+    </row>
+    <row r="46" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="39"/>
+      <c r="C46" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="31"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="19"/>
-    </row>
-    <row r="44" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="38"/>
-      <c r="J44" s="19"/>
-    </row>
-    <row r="45" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="162" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="163"/>
-      <c r="D45" s="163"/>
-      <c r="E45" s="164"/>
-      <c r="F45" s="162" t="s">
-        <v>50</v>
-      </c>
-      <c r="G45" s="163"/>
-      <c r="H45" s="163"/>
-      <c r="I45" s="164"/>
-      <c r="J45" s="19"/>
-    </row>
-    <row r="46" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="G46" s="38"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="28"/>
       <c r="H46" s="38"/>
       <c r="I46" s="38"/>
       <c r="J46" s="19"/>
     </row>
     <row r="47" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B47" s="27" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C47" s="28"/>
       <c r="D47" s="28"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="28" t="s">
-        <v>52</v>
+      <c r="E47" s="37"/>
+      <c r="F47" s="27" t="s">
+        <v>49</v>
       </c>
       <c r="G47" s="38"/>
       <c r="H47" s="38"/>
       <c r="I47" s="38"/>
       <c r="J47" s="19"/>
     </row>
-    <row r="48" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="27" t="s">
+    <row r="48" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B48" s="168" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="169"/>
+      <c r="D48" s="169"/>
+      <c r="E48" s="170"/>
+      <c r="F48" s="168" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" s="169"/>
+      <c r="H48" s="169"/>
+      <c r="I48" s="170"/>
+      <c r="J48" s="19"/>
+    </row>
+    <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="19"/>
+    </row>
+    <row r="50" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="19"/>
+    </row>
+    <row r="51" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="28" t="s">
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="19"/>
-    </row>
-    <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="19"/>
-      <c r="C49" s="36" t="s">
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="19"/>
+    </row>
+    <row r="52" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="19"/>
+      <c r="C52" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="31"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="12" t="s">
+      <c r="D52" s="31"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H49" s="31"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="19"/>
-    </row>
-    <row r="50" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="40" t="s">
+      <c r="H52" s="31"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="19"/>
+    </row>
+    <row r="53" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="41" t="s">
+      <c r="C53" s="41"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="G50" s="41"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="42"/>
-      <c r="J50" s="15"/>
-    </row>
-    <row r="51" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="43"/>
-      <c r="C51" s="44" t="s">
+      <c r="G53" s="41"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="42"/>
+      <c r="J53" s="15"/>
+    </row>
+    <row r="54" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="43"/>
+      <c r="C54" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D51" s="45"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="44" t="s">
+      <c r="D54" s="45"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="H51" s="44" t="s">
+      <c r="H54" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="I51" s="46"/>
-      <c r="J51" s="15"/>
-    </row>
-    <row r="52" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="15"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="48"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-    </row>
-    <row r="53" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="15"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-    </row>
-    <row r="54" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="15"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="48"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
+      <c r="I54" s="46"/>
       <c r="J54" s="15"/>
     </row>
-    <row r="55" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B55" s="15"/>
       <c r="C55" s="48"/>
       <c r="D55" s="48"/>
@@ -3029,18 +3089,51 @@
       <c r="I61" s="15"/>
       <c r="J61" s="15"/>
     </row>
-    <row r="62" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="63" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="64" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="62" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B62" s="15"/>
+      <c r="C62" s="48"/>
+      <c r="D62" s="48"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+    </row>
+    <row r="63" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B63" s="15"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="48"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+    </row>
+    <row r="64" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B64" s="15"/>
+      <c r="C64" s="48"/>
+      <c r="D64" s="48"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+    </row>
     <row r="65" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="66" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="67" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="75" spans="6:7" x14ac:dyDescent="0.45">
-      <c r="F75" s="10"/>
-      <c r="G75" s="10"/>
-    </row>
-    <row r="80" spans="6:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="87" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="68" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="69" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="70" spans="6:7" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="78" spans="6:7" x14ac:dyDescent="0.45">
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+    </row>
+    <row r="83" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="90" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="62">
     <mergeCell ref="B2:E2"/>
@@ -3071,40 +3164,40 @@
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="E18:G18"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:I32"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:I24"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:I27"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:I30"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="F31:I31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="F45:I45"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
     <mergeCell ref="B39:E39"/>
     <mergeCell ref="F39:I39"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F37:I37"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="notContainsBlanks" dxfId="3" priority="2">
@@ -3119,7 +3212,7 @@
       <formula>LEN(TRIM(J18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J19 D19:E20 B20:C20 I20:J21 B21 E21">
+  <conditionalFormatting sqref="J19 D19:E20 B20:C20 I20:J22 B21:B22 E21:E22">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(B19))&gt;0</formula>
     </cfRule>
@@ -3143,8 +3236,8 @@
   </sheetPr>
   <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3655,12 +3748,12 @@
       <c r="B23" s="137" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="198" t="s">
+      <c r="C23" s="204" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="198"/>
-      <c r="E23" s="198"/>
-      <c r="F23" s="198"/>
+      <c r="D23" s="204"/>
+      <c r="E23" s="204"/>
+      <c r="F23" s="204"/>
       <c r="G23" s="138"/>
       <c r="H23" s="139" t="s">
         <v>90</v>
@@ -3671,10 +3764,10 @@
       <c r="J23" s="77">
         <v>14</v>
       </c>
-      <c r="K23" s="199" t="s">
+      <c r="K23" s="205" t="s">
         <v>89</v>
       </c>
-      <c r="L23" s="199"/>
+      <c r="L23" s="205"/>
       <c r="M23" s="76" t="s">
         <v>86</v>
       </c>
@@ -3970,7 +4063,7 @@
     </row>
     <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="56"/>
-      <c r="B41" s="201" t="s">
+      <c r="B41" s="164" t="s">
         <v>82</v>
       </c>
       <c r="C41" s="68"/>
@@ -3980,7 +4073,7 @@
       <c r="G41" s="59"/>
       <c r="H41" s="61"/>
       <c r="I41" s="69"/>
-      <c r="J41" s="204" t="s">
+      <c r="J41" s="57" t="s">
         <v>47</v>
       </c>
       <c r="K41" s="57"/>
@@ -3989,8 +4082,7 @@
       <c r="N41" s="58"/>
     </row>
     <row r="42" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="202"/>
-      <c r="B42" s="206"/>
+      <c r="B42" s="167"/>
       <c r="C42" s="68"/>
       <c r="D42" s="68"/>
       <c r="E42" s="68"/>
@@ -4004,8 +4096,7 @@
       <c r="N42" s="58"/>
     </row>
     <row r="43" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="202"/>
-      <c r="B43" s="206"/>
+      <c r="B43" s="167"/>
       <c r="C43" s="68"/>
       <c r="D43" s="68"/>
       <c r="E43" s="68"/>
@@ -4013,15 +4104,14 @@
       <c r="G43" s="59"/>
       <c r="H43" s="61"/>
       <c r="I43" s="69"/>
-      <c r="J43" s="204"/>
+      <c r="J43" s="57"/>
       <c r="K43" s="57"/>
       <c r="L43" s="68"/>
       <c r="M43" s="61"/>
       <c r="N43" s="58"/>
     </row>
     <row r="44" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="202"/>
-      <c r="B44" s="206"/>
+      <c r="B44" s="167"/>
       <c r="C44" s="68"/>
       <c r="D44" s="68"/>
       <c r="E44" s="68"/>
@@ -4029,15 +4119,15 @@
       <c r="G44" s="59"/>
       <c r="H44" s="61"/>
       <c r="I44" s="69"/>
-      <c r="J44" s="204"/>
+      <c r="J44" s="57"/>
       <c r="K44" s="57"/>
       <c r="L44" s="68"/>
       <c r="M44" s="61"/>
       <c r="N44" s="58"/>
     </row>
     <row r="45" spans="1:14" s="64" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="200"/>
-      <c r="B45" s="203"/>
+      <c r="A45" s="163"/>
+      <c r="B45" s="165"/>
       <c r="C45" s="67"/>
       <c r="D45" s="67"/>
       <c r="E45" s="67"/>
@@ -4045,16 +4135,13 @@
       <c r="G45" s="66"/>
       <c r="H45" s="65"/>
       <c r="I45" s="133"/>
-      <c r="J45" s="205"/>
+      <c r="J45" s="166"/>
       <c r="K45" s="134"/>
       <c r="L45" s="134"/>
       <c r="M45" s="134"/>
       <c r="N45" s="90"/>
     </row>
-    <row r="46" spans="1:14" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="202"/>
-      <c r="C46" s="202"/>
-    </row>
+    <row r="46" spans="1:14" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="47" spans="1:14" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="48" spans="1:14" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="49" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
in progress combining templates, refactoring getExportInvoiceCells module
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C928E85C-D89A-46EB-BDD3-8A568B113B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598501A9-EAC8-4EF8-ACD7-80AA9AC82D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="132">
   <si>
     <t>Дополнительное соглашение № 146 от 10 марта 2023г.</t>
   </si>
@@ -202,22 +202,10 @@
     <t>2. Цена товара</t>
   </si>
   <si>
-    <t>USD 640 000,00</t>
-  </si>
-  <si>
-    <t>$ 640 000,00</t>
-  </si>
-  <si>
     <t>3. Delivery</t>
   </si>
   <si>
     <t>3. Доставка</t>
-  </si>
-  <si>
-    <t>3.1. The commodity should be delivered under terms of CFR Busan</t>
-  </si>
-  <si>
-    <t>3.1. Поставка осуществляется на условиях CFR Пусан</t>
   </si>
   <si>
     <t>4. Other terms</t>
@@ -359,21 +347,6 @@
 Quantity, tn</t>
   </si>
   <si>
-    <t xml:space="preserve">3.5 The delivery of goods to Buyer, mentioned in clause 1.1 of this Agreement 
-should be carried in port of destination Busan, Korea
-</t>
-  </si>
-  <si>
-    <t>Seller is obligated to issue set of sertificates for consignees, mentioned in clause 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.5. Передача Покупателю Товара, оговоренного в п.1.1. настоящего Дополнения будет производиться в порту назначения Пусан, Корея
-</t>
-  </si>
-  <si>
-    <t>Покупатель обязуется выпустить комплект сертификатов на получателей, перечисленных в пункте 1.</t>
-  </si>
-  <si>
     <t>A/C: 40702840201401167199</t>
   </si>
   <si>
@@ -550,6 +523,10 @@
   </si>
   <si>
     <t>Agreement No. 146 dated March 10, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
   </si>
 </sst>
 </file>
@@ -866,7 +843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1311,6 +1288,33 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1320,6 +1324,66 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1332,98 +1396,23 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1790,8 +1779,8 @@
   </sheetPr>
   <dimension ref="B1:AF90"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1835,7 +1824,7 @@
       <c r="C1" s="160"/>
       <c r="D1" s="160"/>
       <c r="E1" s="160" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F1" s="160"/>
       <c r="G1" s="160"/>
@@ -1843,18 +1832,18 @@
       <c r="I1" s="160"/>
     </row>
     <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="198" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="198" t="s">
+      <c r="B2" s="168" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="168" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
+      <c r="G2" s="169"/>
+      <c r="H2" s="169"/>
+      <c r="I2" s="169"/>
       <c r="J2" s="161"/>
       <c r="L2" s="11"/>
       <c r="N2" s="18"/>
@@ -1864,18 +1853,18 @@
       <c r="AD2" s="18"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="201" t="s">
+      <c r="B3" s="171" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="203"/>
-      <c r="F3" s="201" t="s">
+      <c r="C3" s="172"/>
+      <c r="D3" s="172"/>
+      <c r="E3" s="173"/>
+      <c r="F3" s="171" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="202"/>
+      <c r="G3" s="172"/>
+      <c r="H3" s="172"/>
+      <c r="I3" s="172"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1892,18 +1881,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="201" t="s">
+      <c r="B4" s="171" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="202"/>
-      <c r="D4" s="202"/>
-      <c r="E4" s="203"/>
-      <c r="F4" s="201" t="s">
+      <c r="C4" s="172"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="173"/>
+      <c r="F4" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="202"/>
-      <c r="H4" s="202"/>
-      <c r="I4" s="202"/>
+      <c r="G4" s="172"/>
+      <c r="H4" s="172"/>
+      <c r="I4" s="172"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1924,18 +1913,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="195" t="s">
+      <c r="B5" s="180" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="196"/>
-      <c r="D5" s="196"/>
-      <c r="E5" s="197"/>
-      <c r="F5" s="195" t="s">
+      <c r="C5" s="181"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="182"/>
+      <c r="F5" s="180" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="196"/>
-      <c r="H5" s="196"/>
-      <c r="I5" s="196"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1944,18 +1933,18 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="175" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="176"/>
-      <c r="D6" s="176"/>
-      <c r="E6" s="177"/>
-      <c r="F6" s="175" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" s="176"/>
-      <c r="H6" s="176"/>
-      <c r="I6" s="176"/>
+      <c r="B6" s="174" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="175"/>
+      <c r="D6" s="175"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="174" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="175"/>
+      <c r="H6" s="175"/>
+      <c r="I6" s="175"/>
       <c r="J6" s="54"/>
       <c r="L6" s="55"/>
       <c r="O6" s="10"/>
@@ -1973,7 +1962,7 @@
     </row>
     <row r="7" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
@@ -2000,44 +1989,44 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="184" t="s">
+      <c r="B8" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="185"/>
-      <c r="D8" s="185"/>
-      <c r="E8" s="186"/>
-      <c r="F8" s="168" t="s">
+      <c r="C8" s="184"/>
+      <c r="D8" s="184"/>
+      <c r="E8" s="185"/>
+      <c r="F8" s="177" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="169"/>
-      <c r="H8" s="169"/>
-      <c r="I8" s="169"/>
+      <c r="G8" s="178"/>
+      <c r="H8" s="178"/>
+      <c r="I8" s="178"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="168" t="s">
+      <c r="B9" s="177" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="169"/>
-      <c r="D9" s="169"/>
-      <c r="E9" s="170"/>
-      <c r="F9" s="168" t="s">
+      <c r="C9" s="178"/>
+      <c r="D9" s="178"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="169"/>
-      <c r="H9" s="169"/>
-      <c r="I9" s="170"/>
+      <c r="G9" s="178"/>
+      <c r="H9" s="178"/>
+      <c r="I9" s="179"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="168"/>
-      <c r="C10" s="169"/>
-      <c r="D10" s="169"/>
-      <c r="E10" s="170"/>
-      <c r="F10" s="168"/>
-      <c r="G10" s="169"/>
-      <c r="H10" s="169"/>
-      <c r="I10" s="170"/>
+      <c r="B10" s="177"/>
+      <c r="C10" s="178"/>
+      <c r="D10" s="178"/>
+      <c r="E10" s="179"/>
+      <c r="F10" s="177"/>
+      <c r="G10" s="178"/>
+      <c r="H10" s="178"/>
+      <c r="I10" s="179"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -2058,18 +2047,18 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="175" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="176"/>
-      <c r="D11" s="176"/>
-      <c r="E11" s="177"/>
-      <c r="F11" s="175" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="176"/>
-      <c r="H11" s="176"/>
-      <c r="I11" s="176"/>
+      <c r="B11" s="174" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="175"/>
+      <c r="D11" s="175"/>
+      <c r="E11" s="176"/>
+      <c r="F11" s="174" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="175"/>
+      <c r="H11" s="175"/>
+      <c r="I11" s="175"/>
       <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -2112,18 +2101,18 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="168" t="s">
+      <c r="B13" s="177" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="169"/>
-      <c r="D13" s="169"/>
-      <c r="E13" s="170"/>
-      <c r="F13" s="168" t="s">
+      <c r="C13" s="178"/>
+      <c r="D13" s="178"/>
+      <c r="E13" s="179"/>
+      <c r="F13" s="177" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="169"/>
-      <c r="H13" s="169"/>
-      <c r="I13" s="169"/>
+      <c r="G13" s="178"/>
+      <c r="H13" s="178"/>
+      <c r="I13" s="178"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2141,18 +2130,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="168" t="s">
+      <c r="B14" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="169"/>
-      <c r="D14" s="169"/>
-      <c r="E14" s="170"/>
-      <c r="F14" s="168" t="s">
+      <c r="C14" s="178"/>
+      <c r="D14" s="178"/>
+      <c r="E14" s="179"/>
+      <c r="F14" s="177" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="169"/>
-      <c r="H14" s="169"/>
-      <c r="I14" s="169"/>
+      <c r="G14" s="178"/>
+      <c r="H14" s="178"/>
+      <c r="I14" s="178"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2170,18 +2159,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="168" t="s">
+      <c r="B15" s="177" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="169"/>
-      <c r="D15" s="169"/>
-      <c r="E15" s="170"/>
-      <c r="F15" s="168" t="s">
+      <c r="C15" s="178"/>
+      <c r="D15" s="178"/>
+      <c r="E15" s="179"/>
+      <c r="F15" s="177" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="169"/>
-      <c r="H15" s="169"/>
-      <c r="I15" s="169"/>
+      <c r="G15" s="178"/>
+      <c r="H15" s="178"/>
+      <c r="I15" s="178"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2199,18 +2188,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="187" t="s">
+      <c r="B16" s="186" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="188"/>
-      <c r="D16" s="188"/>
+      <c r="C16" s="187"/>
+      <c r="D16" s="187"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="187" t="s">
+      <c r="F16" s="186" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="188"/>
-      <c r="H16" s="188"/>
-      <c r="I16" s="189"/>
+      <c r="G16" s="187"/>
+      <c r="H16" s="187"/>
+      <c r="I16" s="188"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2228,18 +2217,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="190" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="191"/>
-      <c r="D17" s="191"/>
-      <c r="E17" s="192"/>
-      <c r="F17" s="190" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="191"/>
-      <c r="H17" s="191"/>
-      <c r="I17" s="192"/>
+      <c r="B17" s="189" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="190"/>
+      <c r="D17" s="190"/>
+      <c r="E17" s="191"/>
+      <c r="F17" s="189" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="190"/>
+      <c r="H17" s="190"/>
+      <c r="I17" s="191"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2257,23 +2246,23 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="193" t="s">
+      <c r="B18" s="192" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="193"/>
+      <c r="D18" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="193" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="193"/>
+      <c r="G18" s="193"/>
+      <c r="H18" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="23" t="s">
         <v>73</v>
-      </c>
-      <c r="C18" s="194"/>
-      <c r="D18" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="194" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="194"/>
-      <c r="G18" s="194"/>
-      <c r="H18" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>77</v>
       </c>
       <c r="J18" s="24"/>
       <c r="N18" s="10"/>
@@ -2292,18 +2281,18 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="178" t="s">
+      <c r="B19" s="194" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="179"/>
+      <c r="C19" s="195"/>
       <c r="D19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="180" t="s">
+      <c r="E19" s="196" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="180"/>
-      <c r="G19" s="180"/>
+      <c r="F19" s="196"/>
+      <c r="G19" s="196"/>
       <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2389,14 +2378,16 @@
       <c r="AC21" s="10"/>
       <c r="AD21" s="10"/>
     </row>
-    <row r="22" spans="2:30" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="6" t="s">
-        <v>47</v>
+    <row r="22" spans="2:30" ht="9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="206" t="s">
+        <v>43</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="6"/>
+      <c r="F22" s="206" t="s">
+        <v>43</v>
+      </c>
       <c r="G22" s="8"/>
       <c r="H22" s="26"/>
       <c r="I22" s="5"/>
@@ -2419,15 +2410,15 @@
       <c r="AC22" s="10"/>
       <c r="AD22" s="10"/>
     </row>
-    <row r="23" spans="2:30" s="30" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:30" s="30" customFormat="1" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="19" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
       <c r="E23" s="21"/>
       <c r="F23" s="19" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -2436,13 +2427,13 @@
     </row>
     <row r="24" spans="2:30" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="32"/>
       <c r="F24" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="33"/>
@@ -2466,19 +2457,19 @@
       <c r="AC24" s="10"/>
       <c r="AD24" s="10"/>
     </row>
-    <row r="25" spans="2:30" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="181" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="182"/>
-      <c r="D25" s="182"/>
-      <c r="E25" s="183"/>
-      <c r="F25" s="181" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="182"/>
-      <c r="H25" s="182"/>
-      <c r="I25" s="182"/>
+    <row r="25" spans="2:30" ht="7.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="197" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="198"/>
+      <c r="D25" s="198"/>
+      <c r="E25" s="199"/>
+      <c r="F25" s="197" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="198"/>
+      <c r="H25" s="198"/>
+      <c r="I25" s="198"/>
       <c r="J25" s="22"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
@@ -2498,9 +2489,9 @@
       <c r="AC25" s="10"/>
       <c r="AD25" s="10"/>
     </row>
-    <row r="26" spans="2:30" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:30" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="162" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
@@ -2528,9 +2519,9 @@
       <c r="AC26" s="10"/>
       <c r="AD26" s="10"/>
     </row>
-    <row r="27" spans="2:30" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:30" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="162" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
@@ -2558,49 +2549,49 @@
       <c r="AC27" s="10"/>
       <c r="AD27" s="10"/>
     </row>
-    <row r="28" spans="2:30" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="168" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="169"/>
-      <c r="D28" s="169"/>
-      <c r="E28" s="170"/>
-      <c r="F28" s="168" t="s">
-        <v>80</v>
-      </c>
-      <c r="G28" s="169"/>
-      <c r="H28" s="169"/>
-      <c r="I28" s="169"/>
+    <row r="28" spans="2:30" s="30" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="207" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" s="208"/>
+      <c r="D28" s="208"/>
+      <c r="E28" s="209"/>
+      <c r="F28" s="207" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" s="208"/>
+      <c r="H28" s="208"/>
+      <c r="I28" s="208"/>
       <c r="J28" s="19"/>
     </row>
-    <row r="29" spans="2:30" s="30" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="184" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="185"/>
-      <c r="D29" s="185"/>
-      <c r="E29" s="186"/>
-      <c r="F29" s="168" t="s">
-        <v>81</v>
-      </c>
-      <c r="G29" s="169"/>
-      <c r="H29" s="169"/>
-      <c r="I29" s="170"/>
+    <row r="29" spans="2:30" s="30" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="183" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="184"/>
+      <c r="D29" s="184"/>
+      <c r="E29" s="185"/>
+      <c r="F29" s="177" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="178"/>
+      <c r="H29" s="178"/>
+      <c r="I29" s="179"/>
       <c r="J29" s="19"/>
     </row>
     <row r="30" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="175" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="176"/>
-      <c r="D30" s="176"/>
+      <c r="B30" s="174" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="175"/>
+      <c r="D30" s="175"/>
       <c r="E30" s="32"/>
-      <c r="F30" s="175" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" s="176"/>
-      <c r="H30" s="176"/>
-      <c r="I30" s="177"/>
+      <c r="F30" s="174" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="175"/>
+      <c r="H30" s="175"/>
+      <c r="I30" s="176"/>
       <c r="J30" s="22"/>
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
@@ -2621,44 +2612,44 @@
       <c r="AD30" s="10"/>
     </row>
     <row r="31" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="168" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="169"/>
-      <c r="D31" s="169"/>
-      <c r="E31" s="170"/>
-      <c r="F31" s="168" t="s">
-        <v>35</v>
-      </c>
-      <c r="G31" s="169"/>
-      <c r="H31" s="169"/>
-      <c r="I31" s="169"/>
+      <c r="B31" s="177" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="178"/>
+      <c r="D31" s="178"/>
+      <c r="E31" s="179"/>
+      <c r="F31" s="177" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" s="178"/>
+      <c r="H31" s="178"/>
+      <c r="I31" s="178"/>
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="175" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="176"/>
-      <c r="D32" s="176"/>
+      <c r="B32" s="174" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="175"/>
+      <c r="D32" s="175"/>
       <c r="E32" s="21"/>
-      <c r="F32" s="175" t="s">
-        <v>37</v>
-      </c>
-      <c r="G32" s="176"/>
-      <c r="H32" s="176"/>
-      <c r="I32" s="177"/>
+      <c r="F32" s="174" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="175"/>
+      <c r="H32" s="175"/>
+      <c r="I32" s="176"/>
       <c r="J32" s="9"/>
     </row>
     <row r="33" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="50" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="21"/>
       <c r="F33" s="50" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
@@ -2666,18 +2657,18 @@
       <c r="J33" s="9"/>
     </row>
     <row r="34" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="171" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="172"/>
-      <c r="D34" s="172"/>
-      <c r="E34" s="173"/>
-      <c r="F34" s="171" t="s">
+      <c r="B34" s="200" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="201"/>
+      <c r="D34" s="201"/>
+      <c r="E34" s="202"/>
+      <c r="F34" s="200" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="172"/>
-      <c r="H34" s="172"/>
-      <c r="I34" s="172"/>
+      <c r="G34" s="201"/>
+      <c r="H34" s="201"/>
+      <c r="I34" s="201"/>
       <c r="J34" s="34"/>
       <c r="N34" s="36"/>
       <c r="O34" s="36"/>
@@ -2698,104 +2689,104 @@
       <c r="AD34" s="36"/>
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="168" t="s">
+      <c r="B35" s="177" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="178"/>
+      <c r="D35" s="178"/>
+      <c r="E35" s="179"/>
+      <c r="F35" s="177" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="178"/>
+      <c r="H35" s="178"/>
+      <c r="I35" s="178"/>
+      <c r="J35" s="19"/>
+    </row>
+    <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="177" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="178"/>
+      <c r="D36" s="178"/>
+      <c r="E36" s="179"/>
+      <c r="F36" s="177" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" s="178"/>
+      <c r="H36" s="178"/>
+      <c r="I36" s="178"/>
+      <c r="J36" s="19"/>
+    </row>
+    <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="177" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="178"/>
+      <c r="D37" s="178"/>
+      <c r="E37" s="179"/>
+      <c r="F37" s="177" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" s="178"/>
+      <c r="H37" s="178"/>
+      <c r="I37" s="178"/>
+      <c r="J37" s="19"/>
+    </row>
+    <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="177" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="169"/>
-      <c r="D35" s="169"/>
-      <c r="E35" s="170"/>
-      <c r="F35" s="168" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="169"/>
-      <c r="H35" s="169"/>
-      <c r="I35" s="169"/>
-      <c r="J35" s="19"/>
-    </row>
-    <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="168" t="s">
+      <c r="C38" s="178"/>
+      <c r="D38" s="178"/>
+      <c r="E38" s="179"/>
+      <c r="F38" s="177" t="s">
+        <v>38</v>
+      </c>
+      <c r="G38" s="178"/>
+      <c r="H38" s="178"/>
+      <c r="I38" s="178"/>
+      <c r="J38" s="19"/>
+    </row>
+    <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="177" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="169"/>
-      <c r="D36" s="169"/>
-      <c r="E36" s="170"/>
-      <c r="F36" s="168" t="s">
+      <c r="C39" s="178"/>
+      <c r="D39" s="178"/>
+      <c r="E39" s="179"/>
+      <c r="F39" s="177" t="s">
         <v>40</v>
       </c>
-      <c r="G36" s="169"/>
-      <c r="H36" s="169"/>
-      <c r="I36" s="169"/>
-      <c r="J36" s="19"/>
-    </row>
-    <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="168" t="s">
+      <c r="G39" s="178"/>
+      <c r="H39" s="178"/>
+      <c r="I39" s="178"/>
+      <c r="J39" s="19"/>
+    </row>
+    <row r="40" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="177" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="169"/>
-      <c r="D37" s="169"/>
-      <c r="E37" s="170"/>
-      <c r="F37" s="168" t="s">
-        <v>41</v>
-      </c>
-      <c r="G37" s="169"/>
-      <c r="H37" s="169"/>
-      <c r="I37" s="169"/>
-      <c r="J37" s="19"/>
-    </row>
-    <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="168" t="s">
+      <c r="C40" s="178"/>
+      <c r="D40" s="178"/>
+      <c r="E40" s="179"/>
+      <c r="F40" s="177" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="169"/>
-      <c r="D38" s="169"/>
-      <c r="E38" s="170"/>
-      <c r="F38" s="168" t="s">
-        <v>42</v>
-      </c>
-      <c r="G38" s="169"/>
-      <c r="H38" s="169"/>
-      <c r="I38" s="169"/>
-      <c r="J38" s="19"/>
-    </row>
-    <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="168" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="169"/>
-      <c r="D39" s="169"/>
-      <c r="E39" s="170"/>
-      <c r="F39" s="168" t="s">
-        <v>44</v>
-      </c>
-      <c r="G39" s="169"/>
-      <c r="H39" s="169"/>
-      <c r="I39" s="169"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="168" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="169"/>
-      <c r="D40" s="169"/>
-      <c r="E40" s="170"/>
-      <c r="F40" s="168" t="s">
-        <v>46</v>
-      </c>
-      <c r="G40" s="169"/>
-      <c r="H40" s="169"/>
-      <c r="I40" s="169"/>
+      <c r="G40" s="178"/>
+      <c r="H40" s="178"/>
+      <c r="I40" s="178"/>
       <c r="J40" s="19"/>
     </row>
     <row r="41" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B41" s="62" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C41" s="20"/>
       <c r="D41" s="20"/>
       <c r="E41" s="21"/>
       <c r="F41" s="62" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
@@ -2803,18 +2794,18 @@
       <c r="J41" s="19"/>
     </row>
     <row r="42" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="171" t="s">
+      <c r="B42" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="172"/>
-      <c r="D42" s="172"/>
-      <c r="E42" s="173"/>
-      <c r="F42" s="171" t="s">
+      <c r="C42" s="201"/>
+      <c r="D42" s="201"/>
+      <c r="E42" s="202"/>
+      <c r="F42" s="200" t="s">
         <v>12</v>
       </c>
-      <c r="G42" s="174"/>
-      <c r="H42" s="174"/>
-      <c r="I42" s="174"/>
+      <c r="G42" s="203"/>
+      <c r="H42" s="203"/>
+      <c r="I42" s="203"/>
       <c r="J42" s="34"/>
       <c r="N42" s="36"/>
       <c r="O42" s="36"/>
@@ -2835,18 +2826,18 @@
       <c r="AD42" s="36"/>
     </row>
     <row r="43" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="168" t="s">
+      <c r="B43" s="177" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="169"/>
-      <c r="D43" s="169"/>
-      <c r="E43" s="170"/>
-      <c r="F43" s="168" t="s">
+      <c r="C43" s="178"/>
+      <c r="D43" s="178"/>
+      <c r="E43" s="179"/>
+      <c r="F43" s="177" t="s">
         <v>13</v>
       </c>
-      <c r="G43" s="169"/>
-      <c r="H43" s="169"/>
-      <c r="I43" s="169"/>
+      <c r="G43" s="178"/>
+      <c r="H43" s="178"/>
+      <c r="I43" s="178"/>
       <c r="J43" s="19"/>
     </row>
     <row r="44" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2856,7 +2847,7 @@
       <c r="E44" s="21"/>
       <c r="F44" s="19"/>
       <c r="G44" s="20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H44" s="20"/>
       <c r="I44" s="20"/>
@@ -2864,13 +2855,13 @@
     </row>
     <row r="45" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B45" s="27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C45" s="28"/>
       <c r="D45" s="28"/>
       <c r="E45" s="37"/>
       <c r="F45" s="27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G45" s="28"/>
       <c r="H45" s="38"/>
@@ -2880,7 +2871,7 @@
     <row r="46" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B46" s="39"/>
       <c r="C46" s="31" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D46" s="31"/>
       <c r="E46" s="21"/>
@@ -2892,13 +2883,13 @@
     </row>
     <row r="47" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B47" s="27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C47" s="28"/>
       <c r="D47" s="28"/>
       <c r="E47" s="37"/>
       <c r="F47" s="27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G47" s="38"/>
       <c r="H47" s="38"/>
@@ -2906,29 +2897,29 @@
       <c r="J47" s="19"/>
     </row>
     <row r="48" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="168" t="s">
-        <v>50</v>
-      </c>
-      <c r="C48" s="169"/>
-      <c r="D48" s="169"/>
-      <c r="E48" s="170"/>
-      <c r="F48" s="168" t="s">
-        <v>50</v>
-      </c>
-      <c r="G48" s="169"/>
-      <c r="H48" s="169"/>
-      <c r="I48" s="170"/>
+      <c r="B48" s="177" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="178"/>
+      <c r="D48" s="178"/>
+      <c r="E48" s="179"/>
+      <c r="F48" s="177" t="s">
+        <v>46</v>
+      </c>
+      <c r="G48" s="178"/>
+      <c r="H48" s="178"/>
+      <c r="I48" s="179"/>
       <c r="J48" s="19"/>
     </row>
     <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="27" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C49" s="28"/>
       <c r="D49" s="28"/>
       <c r="E49" s="29"/>
       <c r="F49" s="28" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G49" s="38"/>
       <c r="H49" s="38"/>
@@ -2937,13 +2928,13 @@
     </row>
     <row r="50" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50" s="27" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C50" s="28"/>
       <c r="D50" s="28"/>
       <c r="E50" s="29"/>
       <c r="F50" s="28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G50" s="38"/>
       <c r="H50" s="38"/>
@@ -2952,13 +2943,13 @@
     </row>
     <row r="51" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B51" s="27" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C51" s="28"/>
       <c r="D51" s="28"/>
       <c r="E51" s="29"/>
       <c r="F51" s="28" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
@@ -2968,13 +2959,13 @@
     <row r="52" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="19"/>
       <c r="C52" s="36" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D52" s="31"/>
       <c r="E52" s="21"/>
       <c r="F52" s="31"/>
       <c r="G52" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H52" s="31"/>
       <c r="I52" s="31"/>
@@ -2982,13 +2973,13 @@
     </row>
     <row r="53" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="40" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C53" s="41"/>
       <c r="D53" s="41"/>
       <c r="E53" s="42"/>
       <c r="F53" s="41" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G53" s="41"/>
       <c r="H53" s="41"/>
@@ -2998,16 +2989,16 @@
     <row r="54" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B54" s="43"/>
       <c r="C54" s="44" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D54" s="45"/>
       <c r="E54" s="46"/>
       <c r="F54" s="47"/>
       <c r="G54" s="44" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H54" s="44" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I54" s="46"/>
       <c r="J54" s="15"/>
@@ -3136,34 +3127,26 @@
     <row r="90" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="F9:I10"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="B19:C19"/>
@@ -3178,26 +3161,34 @@
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="F31:I31"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="F9:I10"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="notContainsBlanks" dxfId="3" priority="2">
@@ -3236,8 +3227,8 @@
   </sheetPr>
   <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3262,14 +3253,14 @@
     <row r="1" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="56"/>
       <c r="G1" s="159" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="N1" s="58"/>
     </row>
     <row r="2" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="88"/>
       <c r="B2" s="117" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C2" s="117"/>
       <c r="D2" s="117"/>
@@ -3277,7 +3268,7 @@
       <c r="F2" s="117"/>
       <c r="G2" s="117"/>
       <c r="H2" s="120" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="I2" s="117"/>
       <c r="J2" s="117"/>
@@ -3289,7 +3280,7 @@
     <row r="3" spans="1:14" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="88"/>
       <c r="B3" s="118" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C3" s="118"/>
       <c r="D3" s="118"/>
@@ -3297,7 +3288,7 @@
       <c r="F3" s="119"/>
       <c r="G3" s="119"/>
       <c r="H3" s="121" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I3" s="118"/>
       <c r="J3" s="118"/>
@@ -3309,7 +3300,7 @@
     <row r="4" spans="1:14" s="85" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="87"/>
       <c r="B4" s="118" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C4" s="118"/>
       <c r="D4" s="118"/>
@@ -3317,7 +3308,7 @@
       <c r="F4" s="118"/>
       <c r="G4" s="118"/>
       <c r="H4" s="121" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="I4" s="118"/>
       <c r="J4" s="118"/>
@@ -3329,7 +3320,7 @@
     <row r="5" spans="1:14" s="85" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="86"/>
       <c r="B5" s="118" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C5" s="118"/>
       <c r="D5" s="118"/>
@@ -3337,7 +3328,7 @@
       <c r="F5" s="118"/>
       <c r="G5" s="118"/>
       <c r="H5" s="121" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="I5" s="118"/>
       <c r="J5" s="118"/>
@@ -3349,7 +3340,7 @@
     <row r="6" spans="1:14" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="56"/>
       <c r="B6" s="108" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C6" s="108"/>
       <c r="D6" s="108"/>
@@ -3357,7 +3348,7 @@
       <c r="F6" s="108"/>
       <c r="G6" s="108"/>
       <c r="H6" s="94" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I6" s="95"/>
       <c r="J6" s="95"/>
@@ -3369,7 +3360,7 @@
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="56"/>
       <c r="B7" s="111" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C7" s="122"/>
       <c r="D7" s="122"/>
@@ -3409,7 +3400,7 @@
     <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="56"/>
       <c r="B9" s="124" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C9" s="124"/>
       <c r="D9" s="124"/>
@@ -3417,7 +3408,7 @@
       <c r="F9" s="124"/>
       <c r="G9" s="124"/>
       <c r="H9" s="101" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I9" s="96"/>
       <c r="J9" s="96"/>
@@ -3469,7 +3460,7 @@
     <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="56"/>
       <c r="B12" s="124" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C12" s="124"/>
       <c r="D12" s="124"/>
@@ -3477,7 +3468,7 @@
       <c r="F12" s="124"/>
       <c r="G12" s="124"/>
       <c r="H12" s="94" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I12" s="95"/>
       <c r="J12" s="95"/>
@@ -3529,27 +3520,27 @@
     <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="84"/>
       <c r="B15" s="102" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C15" s="102"/>
       <c r="D15" s="103" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E15" s="103"/>
       <c r="F15" s="103" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G15" s="103"/>
       <c r="H15" s="104" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="I15" s="103"/>
       <c r="J15" s="125" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="K15" s="125"/>
       <c r="L15" s="149" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="M15" s="149"/>
       <c r="N15" s="58"/>
@@ -3557,27 +3548,27 @@
     <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="56"/>
       <c r="B16" s="116" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C16" s="105"/>
       <c r="D16" s="154" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E16" s="106"/>
       <c r="F16" s="142" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="G16" s="106"/>
       <c r="H16" s="157" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="I16" s="106"/>
       <c r="J16" s="107" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="K16" s="107"/>
       <c r="L16" s="150" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="M16" s="150"/>
       <c r="N16" s="58"/>
@@ -3585,27 +3576,27 @@
     <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="56"/>
       <c r="B17" s="124" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C17" s="124"/>
       <c r="D17" s="124" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E17" s="128"/>
       <c r="F17" s="141" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G17" s="141"/>
       <c r="H17" s="101" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I17" s="96"/>
       <c r="J17" s="109" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="K17" s="96"/>
       <c r="L17" s="151" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="M17" s="152"/>
       <c r="N17" s="58"/>
@@ -3613,27 +3604,27 @@
     <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="56"/>
       <c r="B18" s="100" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C18" s="123"/>
       <c r="D18" s="155" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E18" s="107"/>
       <c r="F18" s="156" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G18" s="142"/>
       <c r="H18" s="157" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="I18" s="107"/>
       <c r="J18" s="155" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="K18" s="107"/>
       <c r="L18" s="150" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="M18" s="150"/>
       <c r="N18" s="58"/>
@@ -3641,21 +3632,21 @@
     <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="56"/>
       <c r="B19" s="129" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C19" s="129"/>
       <c r="D19" s="129" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E19" s="129"/>
       <c r="F19" s="143"/>
       <c r="G19" s="143"/>
       <c r="H19" s="146" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="I19" s="126"/>
       <c r="J19" s="124" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="K19" s="124"/>
       <c r="L19" s="124"/>
@@ -3665,21 +3656,21 @@
     <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="56"/>
       <c r="B20" s="154" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C20" s="110"/>
       <c r="D20" s="127" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E20" s="127"/>
       <c r="F20" s="144"/>
       <c r="G20" s="144"/>
       <c r="H20" s="158" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I20" s="106"/>
       <c r="J20" s="111" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="K20" s="112"/>
       <c r="L20" s="107"/>
@@ -3716,60 +3707,60 @@
     <row r="22" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="56"/>
       <c r="B22" s="60" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C22" s="130" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D22" s="130"/>
       <c r="E22" s="130"/>
       <c r="F22" s="148"/>
       <c r="G22" s="130"/>
       <c r="H22" s="60" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="I22" s="80" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="J22" s="79" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="K22" s="130" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="L22" s="130"/>
       <c r="M22" s="60" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="N22" s="58"/>
     </row>
     <row r="23" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="56"/>
       <c r="B23" s="137" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C23" s="204" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D23" s="204"/>
       <c r="E23" s="204"/>
       <c r="F23" s="204"/>
       <c r="G23" s="138"/>
       <c r="H23" s="139" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I23" s="78" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="J23" s="77">
         <v>14</v>
       </c>
       <c r="K23" s="205" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="L23" s="205"/>
       <c r="M23" s="76" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="N23" s="58"/>
     </row>
@@ -3781,20 +3772,20 @@
       <c r="F24" s="135"/>
       <c r="G24" s="135"/>
       <c r="H24" s="136" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I24" s="75" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="J24" s="74">
         <v>14</v>
       </c>
       <c r="K24" s="140" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L24" s="140"/>
       <c r="M24" s="89" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="N24" s="58"/>
     </row>
@@ -3989,7 +3980,7 @@
     <row r="37" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="56"/>
       <c r="B37" s="91" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C37" s="72"/>
       <c r="D37" s="72"/>
@@ -3998,7 +3989,7 @@
       <c r="G37" s="71"/>
       <c r="H37" s="70"/>
       <c r="I37" s="132" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J37" s="131"/>
       <c r="K37" s="131"/>
@@ -4009,7 +4000,7 @@
     <row r="38" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="56"/>
       <c r="B38" s="92" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C38" s="68"/>
       <c r="D38" s="68"/>
@@ -4019,7 +4010,7 @@
       <c r="H38" s="61"/>
       <c r="I38" s="69"/>
       <c r="J38" s="57" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K38" s="57"/>
       <c r="L38" s="68"/>
@@ -4029,7 +4020,7 @@
     <row r="39" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="56"/>
       <c r="B39" s="92" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C39" s="68"/>
       <c r="D39" s="68"/>
@@ -4046,7 +4037,7 @@
     <row r="40" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="56"/>
       <c r="B40" s="92" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C40" s="68"/>
       <c r="D40" s="68"/>
@@ -4064,7 +4055,7 @@
     <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="56"/>
       <c r="B41" s="164" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C41" s="68"/>
       <c r="D41" s="68"/>
@@ -4074,7 +4065,7 @@
       <c r="H41" s="61"/>
       <c r="I41" s="69"/>
       <c r="J41" s="57" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K41" s="57"/>
       <c r="L41" s="68"/>

</xml_diff>

<commit_message>
refactoring getExportContractCell, defineCell api beta implemented
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598501A9-EAC8-4EF8-ACD7-80AA9AC82D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA29F611-7618-46E5-BE7B-F672530DBAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="119">
   <si>
     <t>Дополнительное соглашение № 146 от 10 марта 2023г.</t>
   </si>
@@ -277,19 +277,7 @@
     <t>Покупатель/Buyer ________________________SE JI YOUNG</t>
   </si>
   <si>
-    <t>VLADIVOSTOK, RUSSIA</t>
-  </si>
-  <si>
-    <t>CFR, Busan</t>
-  </si>
-  <si>
-    <t>f/v "Morskoy Volk"</t>
-  </si>
-  <si>
     <t>Beneficiary Bank: "ASIAN-PACIFIC BANK" (OJSC)</t>
-  </si>
-  <si>
-    <t>CFR, Пусан</t>
   </si>
   <si>
     <t>Copies of present agreement corresponded by fax are also valid.</t>
@@ -408,9 +396,6 @@
 Номер BL</t>
   </si>
   <si>
-    <t>10702070/180923/3382666</t>
-  </si>
-  <si>
     <t>№ временной декларации на товары:</t>
   </si>
   <si>
@@ -420,18 +405,9 @@
     <t>Temporary Customs Declaration:</t>
   </si>
   <si>
-    <t>Не сертифицирован</t>
-  </si>
-  <si>
     <t>РОССИЯ</t>
   </si>
   <si>
-    <t>СРТМ "Морской Волк"</t>
-  </si>
-  <si>
-    <t>Non-MSC certified</t>
-  </si>
-  <si>
     <t>RUSSIA</t>
   </si>
   <si>
@@ -448,21 +424,6 @@
   </si>
   <si>
     <t>Fishing vessel:</t>
-  </si>
-  <si>
-    <t>Владивосток</t>
-  </si>
-  <si>
-    <t>Пусан, Южная Корея</t>
-  </si>
-  <si>
-    <t>ТР "Бухта Нагаева"</t>
-  </si>
-  <si>
-    <t>Busan, Korea</t>
-  </si>
-  <si>
-    <t>m/v "Bukhta Nagaeva"</t>
   </si>
   <si>
     <t>Порт отправления:</t>
@@ -843,7 +804,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="210">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1116,9 +1077,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1259,16 +1217,10 @@
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1288,6 +1240,108 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1306,113 +1360,32 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1820,31 +1793,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="2.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160" t="s">
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
-      <c r="I1" s="160"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="157"/>
     </row>
     <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="168" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="168" t="s">
+      <c r="B2" s="199" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="201"/>
+      <c r="F2" s="199" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="161"/>
+      <c r="G2" s="200"/>
+      <c r="H2" s="200"/>
+      <c r="I2" s="200"/>
+      <c r="J2" s="158"/>
       <c r="L2" s="11"/>
       <c r="N2" s="18"/>
       <c r="AA2" s="18"/>
@@ -1853,18 +1826,18 @@
       <c r="AD2" s="18"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="202" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="172"/>
-      <c r="D3" s="172"/>
-      <c r="E3" s="173"/>
-      <c r="F3" s="171" t="s">
+      <c r="C3" s="203"/>
+      <c r="D3" s="203"/>
+      <c r="E3" s="204"/>
+      <c r="F3" s="202" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="172"/>
-      <c r="H3" s="172"/>
-      <c r="I3" s="172"/>
+      <c r="G3" s="203"/>
+      <c r="H3" s="203"/>
+      <c r="I3" s="203"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1881,18 +1854,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="202" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="172"/>
-      <c r="D4" s="172"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="171" t="s">
+      <c r="C4" s="203"/>
+      <c r="D4" s="203"/>
+      <c r="E4" s="204"/>
+      <c r="F4" s="202" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="172"/>
-      <c r="H4" s="172"/>
-      <c r="I4" s="172"/>
+      <c r="G4" s="203"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="203"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1913,18 +1886,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="180" t="s">
+      <c r="B5" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="181"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="182"/>
-      <c r="F5" s="180" t="s">
+      <c r="C5" s="197"/>
+      <c r="D5" s="197"/>
+      <c r="E5" s="198"/>
+      <c r="F5" s="196" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="181"/>
-      <c r="H5" s="181"/>
-      <c r="I5" s="181"/>
+      <c r="G5" s="197"/>
+      <c r="H5" s="197"/>
+      <c r="I5" s="197"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1933,18 +1906,18 @@
       <c r="AD5" s="18"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="174" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="175"/>
-      <c r="D6" s="175"/>
-      <c r="E6" s="176"/>
-      <c r="F6" s="174" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="175"/>
-      <c r="H6" s="175"/>
-      <c r="I6" s="175"/>
+      <c r="B6" s="173" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="174"/>
+      <c r="D6" s="174"/>
+      <c r="E6" s="175"/>
+      <c r="F6" s="173" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="174"/>
+      <c r="H6" s="174"/>
+      <c r="I6" s="174"/>
       <c r="J6" s="54"/>
       <c r="L6" s="55"/>
       <c r="O6" s="10"/>
@@ -1962,7 +1935,7 @@
     </row>
     <row r="7" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
@@ -1989,44 +1962,44 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="183" t="s">
+      <c r="B8" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="184"/>
-      <c r="D8" s="184"/>
-      <c r="E8" s="185"/>
-      <c r="F8" s="177" t="s">
+      <c r="C8" s="186"/>
+      <c r="D8" s="186"/>
+      <c r="E8" s="187"/>
+      <c r="F8" s="166" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="178"/>
-      <c r="H8" s="178"/>
-      <c r="I8" s="178"/>
+      <c r="G8" s="167"/>
+      <c r="H8" s="167"/>
+      <c r="I8" s="167"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="177" t="s">
+      <c r="B9" s="166" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="178"/>
-      <c r="D9" s="178"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="177" t="s">
+      <c r="C9" s="167"/>
+      <c r="D9" s="167"/>
+      <c r="E9" s="168"/>
+      <c r="F9" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="178"/>
-      <c r="H9" s="178"/>
-      <c r="I9" s="179"/>
+      <c r="G9" s="167"/>
+      <c r="H9" s="167"/>
+      <c r="I9" s="168"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="177"/>
-      <c r="C10" s="178"/>
-      <c r="D10" s="178"/>
-      <c r="E10" s="179"/>
-      <c r="F10" s="177"/>
-      <c r="G10" s="178"/>
-      <c r="H10" s="178"/>
-      <c r="I10" s="179"/>
+      <c r="B10" s="166"/>
+      <c r="C10" s="167"/>
+      <c r="D10" s="167"/>
+      <c r="E10" s="168"/>
+      <c r="F10" s="166"/>
+      <c r="G10" s="167"/>
+      <c r="H10" s="167"/>
+      <c r="I10" s="168"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -2047,18 +2020,18 @@
       <c r="AD10" s="18"/>
     </row>
     <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="174" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="175"/>
-      <c r="D11" s="175"/>
-      <c r="E11" s="176"/>
-      <c r="F11" s="174" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="175"/>
-      <c r="H11" s="175"/>
-      <c r="I11" s="175"/>
+      <c r="B11" s="173" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="174"/>
+      <c r="D11" s="174"/>
+      <c r="E11" s="175"/>
+      <c r="F11" s="173" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="174"/>
+      <c r="H11" s="174"/>
+      <c r="I11" s="174"/>
       <c r="J11" s="54"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -2101,18 +2074,18 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="177" t="s">
+      <c r="B13" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="178"/>
-      <c r="D13" s="178"/>
-      <c r="E13" s="179"/>
-      <c r="F13" s="177" t="s">
+      <c r="C13" s="167"/>
+      <c r="D13" s="167"/>
+      <c r="E13" s="168"/>
+      <c r="F13" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="178"/>
-      <c r="H13" s="178"/>
-      <c r="I13" s="178"/>
+      <c r="G13" s="167"/>
+      <c r="H13" s="167"/>
+      <c r="I13" s="167"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2130,18 +2103,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="177" t="s">
+      <c r="B14" s="166" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="178"/>
-      <c r="D14" s="178"/>
-      <c r="E14" s="179"/>
-      <c r="F14" s="177" t="s">
+      <c r="C14" s="167"/>
+      <c r="D14" s="167"/>
+      <c r="E14" s="168"/>
+      <c r="F14" s="166" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="178"/>
-      <c r="H14" s="178"/>
-      <c r="I14" s="178"/>
+      <c r="G14" s="167"/>
+      <c r="H14" s="167"/>
+      <c r="I14" s="167"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2159,18 +2132,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="177" t="s">
+      <c r="B15" s="166" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="178"/>
-      <c r="D15" s="178"/>
-      <c r="E15" s="179"/>
-      <c r="F15" s="177" t="s">
+      <c r="C15" s="167"/>
+      <c r="D15" s="167"/>
+      <c r="E15" s="168"/>
+      <c r="F15" s="166" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="178"/>
-      <c r="H15" s="178"/>
-      <c r="I15" s="178"/>
+      <c r="G15" s="167"/>
+      <c r="H15" s="167"/>
+      <c r="I15" s="167"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2188,18 +2161,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="186" t="s">
+      <c r="B16" s="188" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="187"/>
-      <c r="D16" s="187"/>
+      <c r="C16" s="189"/>
+      <c r="D16" s="189"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="186" t="s">
+      <c r="F16" s="188" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="187"/>
-      <c r="H16" s="187"/>
-      <c r="I16" s="188"/>
+      <c r="G16" s="189"/>
+      <c r="H16" s="189"/>
+      <c r="I16" s="190"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2217,18 +2190,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="189" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="190"/>
-      <c r="D17" s="190"/>
-      <c r="E17" s="191"/>
-      <c r="F17" s="189" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="190"/>
-      <c r="H17" s="190"/>
-      <c r="I17" s="191"/>
+      <c r="B17" s="191" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="192"/>
+      <c r="D17" s="192"/>
+      <c r="E17" s="193"/>
+      <c r="F17" s="191" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="192"/>
+      <c r="H17" s="192"/>
+      <c r="I17" s="193"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2246,23 +2219,23 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="192" t="s">
+      <c r="B18" s="194" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="195"/>
+      <c r="D18" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="195" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="195"/>
+      <c r="G18" s="195"/>
+      <c r="H18" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18" s="23" t="s">
         <v>69</v>
-      </c>
-      <c r="C18" s="193"/>
-      <c r="D18" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="193" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="193"/>
-      <c r="G18" s="193"/>
-      <c r="H18" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>73</v>
       </c>
       <c r="J18" s="24"/>
       <c r="N18" s="10"/>
@@ -2281,18 +2254,18 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="194" t="s">
+      <c r="B19" s="176" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="195"/>
+      <c r="C19" s="177"/>
       <c r="D19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="196" t="s">
+      <c r="E19" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="196"/>
-      <c r="G19" s="196"/>
+      <c r="F19" s="178"/>
+      <c r="G19" s="178"/>
       <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2379,13 +2352,13 @@
       <c r="AD21" s="10"/>
     </row>
     <row r="22" spans="2:30" ht="9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="206" t="s">
+      <c r="B22" s="165" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="206" t="s">
+      <c r="F22" s="165" t="s">
         <v>43</v>
       </c>
       <c r="G22" s="8"/>
@@ -2458,18 +2431,18 @@
       <c r="AD24" s="10"/>
     </row>
     <row r="25" spans="2:30" ht="7.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="197" t="s">
+      <c r="B25" s="179" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="198"/>
-      <c r="D25" s="198"/>
-      <c r="E25" s="199"/>
-      <c r="F25" s="197" t="s">
+      <c r="C25" s="180"/>
+      <c r="D25" s="180"/>
+      <c r="E25" s="181"/>
+      <c r="F25" s="179" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="198"/>
-      <c r="H25" s="198"/>
-      <c r="I25" s="198"/>
+      <c r="G25" s="180"/>
+      <c r="H25" s="180"/>
+      <c r="I25" s="180"/>
       <c r="J25" s="22"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
@@ -2490,13 +2463,13 @@
       <c r="AD25" s="10"/>
     </row>
     <row r="26" spans="2:30" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="162" t="s">
+      <c r="B26" s="159" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
       <c r="E26" s="32"/>
-      <c r="F26" s="162"/>
+      <c r="F26" s="159"/>
       <c r="G26" s="33"/>
       <c r="H26" s="33"/>
       <c r="I26" s="33"/>
@@ -2520,13 +2493,13 @@
       <c r="AD26" s="10"/>
     </row>
     <row r="27" spans="2:30" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="162" t="s">
+      <c r="B27" s="159" t="s">
         <v>43</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
       <c r="E27" s="32"/>
-      <c r="F27" s="162"/>
+      <c r="F27" s="159"/>
       <c r="G27" s="33"/>
       <c r="H27" s="33"/>
       <c r="I27" s="33"/>
@@ -2550,48 +2523,48 @@
       <c r="AD27" s="10"/>
     </row>
     <row r="28" spans="2:30" s="30" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="207" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="208"/>
-      <c r="D28" s="208"/>
-      <c r="E28" s="209"/>
-      <c r="F28" s="207" t="s">
-        <v>131</v>
-      </c>
-      <c r="G28" s="208"/>
-      <c r="H28" s="208"/>
-      <c r="I28" s="208"/>
+      <c r="B28" s="182" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="183"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="184"/>
+      <c r="F28" s="182" t="s">
+        <v>118</v>
+      </c>
+      <c r="G28" s="183"/>
+      <c r="H28" s="183"/>
+      <c r="I28" s="183"/>
       <c r="J28" s="19"/>
     </row>
     <row r="29" spans="2:30" s="30" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="183" t="s">
+      <c r="B29" s="185" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="184"/>
-      <c r="D29" s="184"/>
-      <c r="E29" s="185"/>
-      <c r="F29" s="177" t="s">
+      <c r="C29" s="186"/>
+      <c r="D29" s="186"/>
+      <c r="E29" s="187"/>
+      <c r="F29" s="166" t="s">
         <v>43</v>
       </c>
-      <c r="G29" s="178"/>
-      <c r="H29" s="178"/>
-      <c r="I29" s="179"/>
+      <c r="G29" s="167"/>
+      <c r="H29" s="167"/>
+      <c r="I29" s="168"/>
       <c r="J29" s="19"/>
     </row>
     <row r="30" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="174" t="s">
+      <c r="B30" s="173" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="175"/>
-      <c r="D30" s="175"/>
+      <c r="C30" s="174"/>
+      <c r="D30" s="174"/>
       <c r="E30" s="32"/>
-      <c r="F30" s="174" t="s">
+      <c r="F30" s="173" t="s">
         <v>30</v>
       </c>
-      <c r="G30" s="175"/>
-      <c r="H30" s="175"/>
-      <c r="I30" s="176"/>
+      <c r="G30" s="174"/>
+      <c r="H30" s="174"/>
+      <c r="I30" s="175"/>
       <c r="J30" s="22"/>
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
@@ -2612,44 +2585,44 @@
       <c r="AD30" s="10"/>
     </row>
     <row r="31" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="177" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="178"/>
-      <c r="D31" s="178"/>
-      <c r="E31" s="179"/>
-      <c r="F31" s="177" t="s">
+      <c r="B31" s="166" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="167"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="168"/>
+      <c r="F31" s="166" t="s">
         <v>31</v>
       </c>
-      <c r="G31" s="178"/>
-      <c r="H31" s="178"/>
-      <c r="I31" s="178"/>
+      <c r="G31" s="167"/>
+      <c r="H31" s="167"/>
+      <c r="I31" s="167"/>
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="174" t="s">
+      <c r="B32" s="173" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="175"/>
-      <c r="D32" s="175"/>
+      <c r="C32" s="174"/>
+      <c r="D32" s="174"/>
       <c r="E32" s="21"/>
-      <c r="F32" s="174" t="s">
+      <c r="F32" s="173" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="175"/>
-      <c r="H32" s="175"/>
-      <c r="I32" s="176"/>
+      <c r="G32" s="174"/>
+      <c r="H32" s="174"/>
+      <c r="I32" s="175"/>
       <c r="J32" s="9"/>
     </row>
     <row r="33" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="50" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="21"/>
       <c r="F33" s="50" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
@@ -2657,18 +2630,18 @@
       <c r="J33" s="9"/>
     </row>
     <row r="34" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="200" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="201"/>
-      <c r="D34" s="201"/>
-      <c r="E34" s="202"/>
-      <c r="F34" s="200" t="s">
+      <c r="B34" s="169" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="170"/>
+      <c r="D34" s="170"/>
+      <c r="E34" s="171"/>
+      <c r="F34" s="169" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="201"/>
-      <c r="H34" s="201"/>
-      <c r="I34" s="201"/>
+      <c r="G34" s="170"/>
+      <c r="H34" s="170"/>
+      <c r="I34" s="170"/>
       <c r="J34" s="34"/>
       <c r="N34" s="36"/>
       <c r="O34" s="36"/>
@@ -2689,104 +2662,104 @@
       <c r="AD34" s="36"/>
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="177" t="s">
+      <c r="B35" s="166" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="178"/>
-      <c r="D35" s="178"/>
-      <c r="E35" s="179"/>
-      <c r="F35" s="177" t="s">
+      <c r="C35" s="167"/>
+      <c r="D35" s="167"/>
+      <c r="E35" s="168"/>
+      <c r="F35" s="166" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="178"/>
-      <c r="H35" s="178"/>
-      <c r="I35" s="178"/>
+      <c r="G35" s="167"/>
+      <c r="H35" s="167"/>
+      <c r="I35" s="167"/>
       <c r="J35" s="19"/>
     </row>
     <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="177" t="s">
+      <c r="B36" s="166" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="178"/>
-      <c r="D36" s="178"/>
-      <c r="E36" s="179"/>
-      <c r="F36" s="177" t="s">
+      <c r="C36" s="167"/>
+      <c r="D36" s="167"/>
+      <c r="E36" s="168"/>
+      <c r="F36" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="G36" s="178"/>
-      <c r="H36" s="178"/>
-      <c r="I36" s="178"/>
+      <c r="G36" s="167"/>
+      <c r="H36" s="167"/>
+      <c r="I36" s="167"/>
       <c r="J36" s="19"/>
     </row>
     <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="177" t="s">
+      <c r="B37" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="178"/>
-      <c r="D37" s="178"/>
-      <c r="E37" s="179"/>
-      <c r="F37" s="177" t="s">
+      <c r="C37" s="167"/>
+      <c r="D37" s="167"/>
+      <c r="E37" s="168"/>
+      <c r="F37" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="G37" s="178"/>
-      <c r="H37" s="178"/>
-      <c r="I37" s="178"/>
+      <c r="G37" s="167"/>
+      <c r="H37" s="167"/>
+      <c r="I37" s="167"/>
       <c r="J37" s="19"/>
     </row>
     <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="177" t="s">
+      <c r="B38" s="166" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="178"/>
-      <c r="D38" s="178"/>
-      <c r="E38" s="179"/>
-      <c r="F38" s="177" t="s">
+      <c r="C38" s="167"/>
+      <c r="D38" s="167"/>
+      <c r="E38" s="168"/>
+      <c r="F38" s="166" t="s">
         <v>38</v>
       </c>
-      <c r="G38" s="178"/>
-      <c r="H38" s="178"/>
-      <c r="I38" s="178"/>
+      <c r="G38" s="167"/>
+      <c r="H38" s="167"/>
+      <c r="I38" s="167"/>
       <c r="J38" s="19"/>
     </row>
     <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="177" t="s">
+      <c r="B39" s="166" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="178"/>
-      <c r="D39" s="178"/>
-      <c r="E39" s="179"/>
-      <c r="F39" s="177" t="s">
+      <c r="C39" s="167"/>
+      <c r="D39" s="167"/>
+      <c r="E39" s="168"/>
+      <c r="F39" s="166" t="s">
         <v>40</v>
       </c>
-      <c r="G39" s="178"/>
-      <c r="H39" s="178"/>
-      <c r="I39" s="178"/>
+      <c r="G39" s="167"/>
+      <c r="H39" s="167"/>
+      <c r="I39" s="167"/>
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="177" t="s">
+      <c r="B40" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="178"/>
-      <c r="D40" s="178"/>
-      <c r="E40" s="179"/>
-      <c r="F40" s="177" t="s">
+      <c r="C40" s="167"/>
+      <c r="D40" s="167"/>
+      <c r="E40" s="168"/>
+      <c r="F40" s="166" t="s">
         <v>42</v>
       </c>
-      <c r="G40" s="178"/>
-      <c r="H40" s="178"/>
-      <c r="I40" s="178"/>
+      <c r="G40" s="167"/>
+      <c r="H40" s="167"/>
+      <c r="I40" s="167"/>
       <c r="J40" s="19"/>
     </row>
     <row r="41" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B41" s="62" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C41" s="20"/>
       <c r="D41" s="20"/>
       <c r="E41" s="21"/>
       <c r="F41" s="62" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
@@ -2794,18 +2767,18 @@
       <c r="J41" s="19"/>
     </row>
     <row r="42" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="200" t="s">
+      <c r="B42" s="169" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="201"/>
-      <c r="D42" s="201"/>
-      <c r="E42" s="202"/>
-      <c r="F42" s="200" t="s">
+      <c r="C42" s="170"/>
+      <c r="D42" s="170"/>
+      <c r="E42" s="171"/>
+      <c r="F42" s="169" t="s">
         <v>12</v>
       </c>
-      <c r="G42" s="203"/>
-      <c r="H42" s="203"/>
-      <c r="I42" s="203"/>
+      <c r="G42" s="172"/>
+      <c r="H42" s="172"/>
+      <c r="I42" s="172"/>
       <c r="J42" s="34"/>
       <c r="N42" s="36"/>
       <c r="O42" s="36"/>
@@ -2826,18 +2799,18 @@
       <c r="AD42" s="36"/>
     </row>
     <row r="43" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="177" t="s">
+      <c r="B43" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="178"/>
-      <c r="D43" s="178"/>
-      <c r="E43" s="179"/>
-      <c r="F43" s="177" t="s">
+      <c r="C43" s="167"/>
+      <c r="D43" s="167"/>
+      <c r="E43" s="168"/>
+      <c r="F43" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="G43" s="178"/>
-      <c r="H43" s="178"/>
-      <c r="I43" s="178"/>
+      <c r="G43" s="167"/>
+      <c r="H43" s="167"/>
+      <c r="I43" s="167"/>
       <c r="J43" s="19"/>
     </row>
     <row r="44" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2897,18 +2870,18 @@
       <c r="J47" s="19"/>
     </row>
     <row r="48" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="177" t="s">
+      <c r="B48" s="166" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="178"/>
-      <c r="D48" s="178"/>
-      <c r="E48" s="179"/>
-      <c r="F48" s="177" t="s">
+      <c r="C48" s="167"/>
+      <c r="D48" s="167"/>
+      <c r="E48" s="168"/>
+      <c r="F48" s="166" t="s">
         <v>46</v>
       </c>
-      <c r="G48" s="178"/>
-      <c r="H48" s="178"/>
-      <c r="I48" s="179"/>
+      <c r="G48" s="167"/>
+      <c r="H48" s="167"/>
+      <c r="I48" s="168"/>
       <c r="J48" s="19"/>
     </row>
     <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3127,6 +3100,54 @@
     <row r="90" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="F9:I10"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
     <mergeCell ref="B48:E48"/>
     <mergeCell ref="F48:I48"/>
     <mergeCell ref="B37:E37"/>
@@ -3141,54 +3162,6 @@
     <mergeCell ref="F39:I39"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="F9:I10"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="notContainsBlanks" dxfId="3" priority="2">
@@ -3227,8 +3200,8 @@
   </sheetPr>
   <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3252,103 +3225,103 @@
   <sheetData>
     <row r="1" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="56"/>
-      <c r="G1" s="159" t="s">
+      <c r="G1" s="156" t="s">
         <v>43</v>
       </c>
       <c r="N1" s="58"/>
     </row>
     <row r="2" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="88"/>
-      <c r="B2" s="117" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="120" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
+      <c r="B2" s="116" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="119" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
       <c r="N2" s="58"/>
     </row>
     <row r="3" spans="1:14" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="88"/>
-      <c r="B3" s="118" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="121" t="s">
-        <v>124</v>
-      </c>
-      <c r="I3" s="118"/>
-      <c r="J3" s="118"/>
-      <c r="K3" s="118"/>
-      <c r="L3" s="118"/>
-      <c r="M3" s="118"/>
+      <c r="B3" s="117" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="120" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="117"/>
       <c r="N3" s="58"/>
     </row>
     <row r="4" spans="1:14" s="85" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="87"/>
-      <c r="B4" s="118" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="118"/>
-      <c r="H4" s="121" t="s">
-        <v>122</v>
-      </c>
-      <c r="I4" s="118"/>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="118"/>
-      <c r="M4" s="118"/>
+      <c r="B4" s="117" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="120" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" s="117"/>
+      <c r="J4" s="117"/>
+      <c r="K4" s="117"/>
+      <c r="L4" s="117"/>
+      <c r="M4" s="117"/>
       <c r="N4" s="83"/>
     </row>
     <row r="5" spans="1:14" s="85" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="86"/>
-      <c r="B5" s="118" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="121" t="s">
-        <v>120</v>
-      </c>
-      <c r="I5" s="118"/>
-      <c r="J5" s="118"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="118"/>
-      <c r="M5" s="118"/>
+      <c r="B5" s="117" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="120" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
       <c r="N5" s="83"/>
     </row>
     <row r="6" spans="1:14" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="56"/>
-      <c r="B6" s="108" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
+      <c r="B6" s="107" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="107"/>
       <c r="H6" s="94" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I6" s="95"/>
       <c r="J6" s="95"/>
@@ -3359,14 +3332,14 @@
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="56"/>
-      <c r="B7" s="111" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="122"/>
-      <c r="F7" s="122"/>
-      <c r="G7" s="122"/>
+      <c r="B7" s="110" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="121"/>
+      <c r="D7" s="121"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
       <c r="H7" s="97" t="s">
         <v>7</v>
       </c>
@@ -3379,14 +3352,14 @@
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="56"/>
-      <c r="B8" s="123" t="s">
+      <c r="B8" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="123"/>
-      <c r="G8" s="123"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="122"/>
       <c r="H8" s="99" t="s">
         <v>9</v>
       </c>
@@ -3399,16 +3372,16 @@
     </row>
     <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="56"/>
-      <c r="B9" s="124" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="124"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
+      <c r="B9" s="123" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="123"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="123"/>
       <c r="H9" s="101" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="I9" s="96"/>
       <c r="J9" s="96"/>
@@ -3419,14 +3392,14 @@
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="56"/>
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="111"/>
-      <c r="F10" s="111"/>
-      <c r="G10" s="111"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
       <c r="H10" s="97" t="s">
         <v>12</v>
       </c>
@@ -3446,8 +3419,8 @@
       <c r="D11" s="100"/>
       <c r="E11" s="100"/>
       <c r="F11" s="100"/>
-      <c r="G11" s="116"/>
-      <c r="H11" s="153" t="s">
+      <c r="G11" s="115"/>
+      <c r="H11" s="152" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="100"/>
@@ -3459,16 +3432,16 @@
     </row>
     <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="56"/>
-      <c r="B12" s="124" t="s">
-        <v>118</v>
-      </c>
-      <c r="C12" s="124"/>
-      <c r="D12" s="124"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="124"/>
-      <c r="G12" s="124"/>
+      <c r="B12" s="123" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="123"/>
       <c r="H12" s="94" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="I12" s="95"/>
       <c r="J12" s="95"/>
@@ -3479,14 +3452,14 @@
     </row>
     <row r="13" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="56"/>
-      <c r="B13" s="111" t="s">
+      <c r="B13" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
       <c r="H13" s="97" t="s">
         <v>12</v>
       </c>
@@ -3497,17 +3470,17 @@
       <c r="M13" s="96"/>
       <c r="N13" s="58"/>
     </row>
-    <row r="14" spans="1:14" ht="39.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" ht="44.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="56"/>
-      <c r="B14" s="100" t="s">
+      <c r="B14" s="211" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="116"/>
-      <c r="H14" s="153" t="s">
+      <c r="C14" s="212"/>
+      <c r="D14" s="212"/>
+      <c r="E14" s="212"/>
+      <c r="F14" s="212"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="152" t="s">
         <v>13</v>
       </c>
       <c r="I14" s="100"/>
@@ -3519,178 +3492,178 @@
     </row>
     <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="84"/>
-      <c r="B15" s="102" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="103" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="103"/>
-      <c r="F15" s="103" t="s">
-        <v>104</v>
-      </c>
-      <c r="G15" s="103"/>
-      <c r="H15" s="104" t="s">
-        <v>103</v>
-      </c>
-      <c r="I15" s="103"/>
-      <c r="J15" s="125" t="s">
-        <v>101</v>
-      </c>
-      <c r="K15" s="125"/>
-      <c r="L15" s="149" t="s">
-        <v>102</v>
-      </c>
-      <c r="M15" s="149"/>
+      <c r="B15" s="207" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="208"/>
+      <c r="D15" s="102" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="102"/>
+      <c r="F15" s="102" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="102"/>
+      <c r="H15" s="103" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15" s="102"/>
+      <c r="J15" s="124" t="s">
+        <v>93</v>
+      </c>
+      <c r="K15" s="124"/>
+      <c r="L15" s="148" t="s">
+        <v>94</v>
+      </c>
+      <c r="M15" s="148"/>
       <c r="N15" s="58"/>
     </row>
     <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="56"/>
-      <c r="B16" s="116" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="154" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="106"/>
-      <c r="F16" s="142" t="s">
-        <v>100</v>
-      </c>
-      <c r="G16" s="106"/>
-      <c r="H16" s="157" t="s">
-        <v>98</v>
-      </c>
-      <c r="I16" s="106"/>
-      <c r="J16" s="107" t="s">
-        <v>96</v>
-      </c>
-      <c r="K16" s="107"/>
-      <c r="L16" s="150" t="s">
-        <v>97</v>
-      </c>
-      <c r="M16" s="150"/>
+      <c r="B16" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="104"/>
+      <c r="D16" s="153" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="105"/>
+      <c r="F16" s="141" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="105"/>
+      <c r="H16" s="155" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="105"/>
+      <c r="J16" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="106"/>
+      <c r="L16" s="149" t="s">
+        <v>91</v>
+      </c>
+      <c r="M16" s="149"/>
       <c r="N16" s="58"/>
     </row>
     <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="56"/>
-      <c r="B17" s="124" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="124"/>
-      <c r="D17" s="124" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" s="128"/>
-      <c r="F17" s="141" t="s">
-        <v>114</v>
-      </c>
-      <c r="G17" s="141"/>
+      <c r="B17" s="123" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="127"/>
+      <c r="F17" s="140" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="140"/>
       <c r="H17" s="101" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="I17" s="96"/>
-      <c r="J17" s="109" t="s">
-        <v>112</v>
+      <c r="J17" s="108" t="s">
+        <v>99</v>
       </c>
       <c r="K17" s="96"/>
-      <c r="L17" s="151" t="s">
-        <v>111</v>
-      </c>
-      <c r="M17" s="152"/>
+      <c r="L17" s="150" t="s">
+        <v>98</v>
+      </c>
+      <c r="M17" s="151"/>
       <c r="N17" s="58"/>
     </row>
     <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="56"/>
-      <c r="B18" s="100" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" s="123"/>
-      <c r="D18" s="155" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" s="107"/>
-      <c r="F18" s="156" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="142"/>
-      <c r="H18" s="157" t="s">
-        <v>108</v>
-      </c>
-      <c r="I18" s="107"/>
-      <c r="J18" s="155" t="s">
-        <v>107</v>
-      </c>
-      <c r="K18" s="107"/>
-      <c r="L18" s="150" t="s">
-        <v>106</v>
-      </c>
-      <c r="M18" s="150"/>
+      <c r="B18" s="122" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="122"/>
+      <c r="D18" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="106"/>
+      <c r="F18" s="154" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="141"/>
+      <c r="H18" s="213" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="106"/>
+      <c r="J18" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="106"/>
+      <c r="L18" s="149" t="s">
+        <v>43</v>
+      </c>
+      <c r="M18" s="149"/>
       <c r="N18" s="58"/>
     </row>
     <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="56"/>
-      <c r="B19" s="129" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="129"/>
-      <c r="D19" s="129" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" s="129"/>
-      <c r="F19" s="143"/>
-      <c r="G19" s="143"/>
-      <c r="H19" s="146" t="s">
-        <v>129</v>
-      </c>
-      <c r="I19" s="126"/>
-      <c r="J19" s="124" t="s">
-        <v>93</v>
-      </c>
-      <c r="K19" s="124"/>
-      <c r="L19" s="124"/>
-      <c r="M19" s="124"/>
+      <c r="B19" s="210" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="209"/>
+      <c r="D19" s="128" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="128"/>
+      <c r="F19" s="128"/>
+      <c r="G19" s="142"/>
+      <c r="H19" s="145" t="s">
+        <v>116</v>
+      </c>
+      <c r="I19" s="125"/>
+      <c r="J19" s="123" t="s">
+        <v>88</v>
+      </c>
+      <c r="K19" s="123"/>
+      <c r="L19" s="123"/>
+      <c r="M19" s="123"/>
       <c r="N19" s="58"/>
     </row>
     <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="56"/>
-      <c r="B20" s="154" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="110"/>
-      <c r="D20" s="127" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="127"/>
-      <c r="F20" s="144"/>
-      <c r="G20" s="144"/>
-      <c r="H20" s="158" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="106"/>
-      <c r="J20" s="111" t="s">
-        <v>92</v>
-      </c>
-      <c r="K20" s="112"/>
-      <c r="L20" s="107"/>
-      <c r="M20" s="107"/>
+      <c r="B20" s="105" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="109"/>
+      <c r="D20" s="126" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="126"/>
+      <c r="F20" s="143"/>
+      <c r="G20" s="143"/>
+      <c r="H20" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="105"/>
+      <c r="J20" s="110" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="111"/>
+      <c r="L20" s="106"/>
+      <c r="M20" s="106"/>
       <c r="N20" s="58"/>
     </row>
     <row r="21" spans="1:29" s="81" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="93"/>
-      <c r="B21" s="113"/>
-      <c r="C21" s="113"/>
-      <c r="D21" s="113"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="113"/>
-      <c r="G21" s="145"/>
-      <c r="H21" s="147"/>
-      <c r="I21" s="114"/>
-      <c r="J21" s="114"/>
-      <c r="K21" s="114"/>
-      <c r="L21" s="114"/>
-      <c r="M21" s="115"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="144"/>
+      <c r="H21" s="146"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="113"/>
+      <c r="L21" s="113"/>
+      <c r="M21" s="114"/>
       <c r="N21" s="82"/>
       <c r="S21"/>
       <c r="T21"/>
@@ -3707,85 +3680,85 @@
     <row r="22" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="56"/>
       <c r="B22" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" s="130" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="130"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="148"/>
-      <c r="G22" s="130"/>
+        <v>87</v>
+      </c>
+      <c r="C22" s="129" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="129"/>
+      <c r="E22" s="129"/>
+      <c r="F22" s="147"/>
+      <c r="G22" s="129"/>
       <c r="H22" s="60" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I22" s="80" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J22" s="79" t="s">
-        <v>87</v>
-      </c>
-      <c r="K22" s="130" t="s">
-        <v>86</v>
-      </c>
-      <c r="L22" s="130"/>
+        <v>83</v>
+      </c>
+      <c r="K22" s="129" t="s">
+        <v>82</v>
+      </c>
+      <c r="L22" s="129"/>
       <c r="M22" s="60" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="N22" s="58"/>
     </row>
     <row r="23" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="56"/>
-      <c r="B23" s="137" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="204" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="204"/>
-      <c r="E23" s="204"/>
-      <c r="F23" s="204"/>
-      <c r="G23" s="138"/>
-      <c r="H23" s="139" t="s">
-        <v>82</v>
+      <c r="B23" s="136" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="205" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="205"/>
+      <c r="E23" s="205"/>
+      <c r="F23" s="205"/>
+      <c r="G23" s="137"/>
+      <c r="H23" s="138" t="s">
+        <v>78</v>
       </c>
       <c r="I23" s="78" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J23" s="77">
         <v>14</v>
       </c>
-      <c r="K23" s="205" t="s">
-        <v>81</v>
-      </c>
-      <c r="L23" s="205"/>
+      <c r="K23" s="206" t="s">
+        <v>77</v>
+      </c>
+      <c r="L23" s="206"/>
       <c r="M23" s="76" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="N23" s="58"/>
     </row>
     <row r="24" spans="1:29" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="56"/>
-      <c r="C24" s="135"/>
-      <c r="D24" s="135"/>
-      <c r="E24" s="135"/>
-      <c r="F24" s="135"/>
-      <c r="G24" s="135"/>
-      <c r="H24" s="136" t="s">
-        <v>80</v>
+      <c r="C24" s="134"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="134"/>
+      <c r="F24" s="134"/>
+      <c r="G24" s="134"/>
+      <c r="H24" s="135" t="s">
+        <v>76</v>
       </c>
       <c r="I24" s="75" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J24" s="74">
         <v>14</v>
       </c>
-      <c r="K24" s="140" t="s">
+      <c r="K24" s="139" t="s">
         <v>43</v>
       </c>
-      <c r="L24" s="140"/>
+      <c r="L24" s="139"/>
       <c r="M24" s="89" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="N24" s="58"/>
     </row>
@@ -3980,7 +3953,7 @@
     <row r="37" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="56"/>
       <c r="B37" s="91" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C37" s="72"/>
       <c r="D37" s="72"/>
@@ -3988,19 +3961,19 @@
       <c r="F37" s="71"/>
       <c r="G37" s="71"/>
       <c r="H37" s="70"/>
-      <c r="I37" s="132" t="s">
-        <v>77</v>
-      </c>
-      <c r="J37" s="131"/>
-      <c r="K37" s="131"/>
-      <c r="L37" s="131"/>
-      <c r="M37" s="131"/>
+      <c r="I37" s="131" t="s">
+        <v>73</v>
+      </c>
+      <c r="J37" s="130"/>
+      <c r="K37" s="130"/>
+      <c r="L37" s="130"/>
+      <c r="M37" s="130"/>
       <c r="N37" s="58"/>
     </row>
     <row r="38" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="56"/>
       <c r="B38" s="92" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C38" s="68"/>
       <c r="D38" s="68"/>
@@ -4037,7 +4010,7 @@
     <row r="40" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="56"/>
       <c r="B40" s="92" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C40" s="68"/>
       <c r="D40" s="68"/>
@@ -4054,8 +4027,8 @@
     </row>
     <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="56"/>
-      <c r="B41" s="164" t="s">
-        <v>74</v>
+      <c r="B41" s="161" t="s">
+        <v>70</v>
       </c>
       <c r="C41" s="68"/>
       <c r="D41" s="68"/>
@@ -4073,7 +4046,7 @@
       <c r="N41" s="58"/>
     </row>
     <row r="42" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="167"/>
+      <c r="B42" s="164"/>
       <c r="C42" s="68"/>
       <c r="D42" s="68"/>
       <c r="E42" s="68"/>
@@ -4087,7 +4060,7 @@
       <c r="N42" s="58"/>
     </row>
     <row r="43" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="167"/>
+      <c r="B43" s="164"/>
       <c r="C43" s="68"/>
       <c r="D43" s="68"/>
       <c r="E43" s="68"/>
@@ -4102,7 +4075,7 @@
       <c r="N43" s="58"/>
     </row>
     <row r="44" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="167"/>
+      <c r="B44" s="164"/>
       <c r="C44" s="68"/>
       <c r="D44" s="68"/>
       <c r="E44" s="68"/>
@@ -4117,19 +4090,19 @@
       <c r="N44" s="58"/>
     </row>
     <row r="45" spans="1:14" s="64" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="163"/>
-      <c r="B45" s="165"/>
+      <c r="A45" s="160"/>
+      <c r="B45" s="162"/>
       <c r="C45" s="67"/>
       <c r="D45" s="67"/>
       <c r="E45" s="67"/>
       <c r="F45" s="66"/>
       <c r="G45" s="66"/>
       <c r="H45" s="65"/>
-      <c r="I45" s="133"/>
-      <c r="J45" s="166"/>
-      <c r="K45" s="134"/>
-      <c r="L45" s="134"/>
-      <c r="M45" s="134"/>
+      <c r="I45" s="132"/>
+      <c r="J45" s="163"/>
+      <c r="K45" s="133"/>
+      <c r="L45" s="133"/>
+      <c r="M45" s="133"/>
       <c r="N45" s="90"/>
     </row>
     <row r="46" spans="1:14" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4139,9 +4112,11 @@
     <row r="50" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="55" ht="2.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="K23:L23"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
fixed fca invoice tmp
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA29F611-7618-46E5-BE7B-F672530DBAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574DAE29-78B6-4B28-B1FB-23F0E5741120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -804,7 +804,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1214,14 +1214,8 @@
     <xf numFmtId="9" fontId="18" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1243,6 +1237,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1252,6 +1282,75 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1264,102 +1363,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1371,21 +1374,6 @@
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1752,8 +1740,8 @@
   </sheetPr>
   <dimension ref="B1:AF90"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:E36"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="91" zoomScaleNormal="100" zoomScaleSheetLayoutView="91" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1793,31 +1781,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="2.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157" t="s">
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="157"/>
-      <c r="I1" s="157"/>
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
+      <c r="H1" s="155"/>
+      <c r="I1" s="155"/>
     </row>
     <row r="2" spans="2:30" s="17" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="199" t="s">
+      <c r="B2" s="167" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="201"/>
-      <c r="F2" s="199" t="s">
+      <c r="C2" s="168"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="169"/>
+      <c r="F2" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
-      <c r="I2" s="200"/>
-      <c r="J2" s="158"/>
+      <c r="G2" s="168"/>
+      <c r="H2" s="168"/>
+      <c r="I2" s="168"/>
+      <c r="J2" s="156"/>
       <c r="L2" s="11"/>
       <c r="N2" s="18"/>
       <c r="AA2" s="18"/>
@@ -1826,18 +1814,18 @@
       <c r="AD2" s="18"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="202" t="s">
+      <c r="B3" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="204"/>
-      <c r="F3" s="202" t="s">
+      <c r="C3" s="171"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="172"/>
+      <c r="F3" s="170" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="203"/>
-      <c r="H3" s="203"/>
-      <c r="I3" s="203"/>
+      <c r="G3" s="171"/>
+      <c r="H3" s="171"/>
+      <c r="I3" s="171"/>
       <c r="J3" s="9"/>
       <c r="L3" s="11"/>
       <c r="O3" s="10"/>
@@ -1854,18 +1842,18 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="202" t="s">
+      <c r="B4" s="170" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="203"/>
-      <c r="D4" s="203"/>
-      <c r="E4" s="204"/>
-      <c r="F4" s="202" t="s">
+      <c r="C4" s="171"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="172"/>
+      <c r="F4" s="170" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="203"/>
-      <c r="H4" s="203"/>
-      <c r="I4" s="203"/>
+      <c r="G4" s="171"/>
+      <c r="H4" s="171"/>
+      <c r="I4" s="171"/>
       <c r="J4" s="9"/>
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
@@ -1886,18 +1874,18 @@
       <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" s="17" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="196" t="s">
+      <c r="B5" s="179" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="197"/>
-      <c r="D5" s="197"/>
-      <c r="E5" s="198"/>
-      <c r="F5" s="196" t="s">
+      <c r="C5" s="180"/>
+      <c r="D5" s="180"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="179" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="197"/>
-      <c r="H5" s="197"/>
-      <c r="I5" s="197"/>
+      <c r="G5" s="180"/>
+      <c r="H5" s="180"/>
+      <c r="I5" s="180"/>
       <c r="J5" s="16"/>
       <c r="N5" s="18"/>
       <c r="AA5" s="18"/>
@@ -1962,44 +1950,44 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="185" t="s">
+      <c r="B8" s="182" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="186"/>
-      <c r="D8" s="186"/>
-      <c r="E8" s="187"/>
-      <c r="F8" s="166" t="s">
+      <c r="C8" s="183"/>
+      <c r="D8" s="183"/>
+      <c r="E8" s="184"/>
+      <c r="F8" s="176" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="167"/>
-      <c r="H8" s="167"/>
-      <c r="I8" s="167"/>
+      <c r="G8" s="177"/>
+      <c r="H8" s="177"/>
+      <c r="I8" s="177"/>
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="166" t="s">
+      <c r="B9" s="176" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="167"/>
-      <c r="D9" s="167"/>
-      <c r="E9" s="168"/>
-      <c r="F9" s="166" t="s">
+      <c r="C9" s="177"/>
+      <c r="D9" s="177"/>
+      <c r="E9" s="178"/>
+      <c r="F9" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="167"/>
-      <c r="H9" s="167"/>
-      <c r="I9" s="168"/>
+      <c r="G9" s="177"/>
+      <c r="H9" s="177"/>
+      <c r="I9" s="178"/>
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="166"/>
-      <c r="C10" s="167"/>
-      <c r="D10" s="167"/>
-      <c r="E10" s="168"/>
-      <c r="F10" s="166"/>
-      <c r="G10" s="167"/>
-      <c r="H10" s="167"/>
-      <c r="I10" s="168"/>
+      <c r="B10" s="176"/>
+      <c r="C10" s="177"/>
+      <c r="D10" s="177"/>
+      <c r="E10" s="178"/>
+      <c r="F10" s="176"/>
+      <c r="G10" s="177"/>
+      <c r="H10" s="177"/>
+      <c r="I10" s="178"/>
       <c r="J10" s="22"/>
       <c r="N10" s="18"/>
       <c r="O10" s="10"/>
@@ -2074,18 +2062,18 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="166" t="s">
+      <c r="B13" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="167"/>
-      <c r="D13" s="167"/>
-      <c r="E13" s="168"/>
-      <c r="F13" s="166" t="s">
+      <c r="C13" s="177"/>
+      <c r="D13" s="177"/>
+      <c r="E13" s="178"/>
+      <c r="F13" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="167"/>
-      <c r="H13" s="167"/>
-      <c r="I13" s="167"/>
+      <c r="G13" s="177"/>
+      <c r="H13" s="177"/>
+      <c r="I13" s="177"/>
       <c r="J13" s="22"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2103,18 +2091,18 @@
       <c r="AA13" s="10"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="166" t="s">
+      <c r="B14" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="167"/>
-      <c r="D14" s="167"/>
-      <c r="E14" s="168"/>
-      <c r="F14" s="166" t="s">
+      <c r="C14" s="177"/>
+      <c r="D14" s="177"/>
+      <c r="E14" s="178"/>
+      <c r="F14" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="167"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="167"/>
+      <c r="G14" s="177"/>
+      <c r="H14" s="177"/>
+      <c r="I14" s="177"/>
       <c r="J14" s="22"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -2132,18 +2120,18 @@
       <c r="AA14" s="10"/>
     </row>
     <row r="15" spans="2:30" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="166" t="s">
+      <c r="B15" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="167"/>
-      <c r="D15" s="167"/>
-      <c r="E15" s="168"/>
-      <c r="F15" s="166" t="s">
+      <c r="C15" s="177"/>
+      <c r="D15" s="177"/>
+      <c r="E15" s="178"/>
+      <c r="F15" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="167"/>
+      <c r="G15" s="177"/>
+      <c r="H15" s="177"/>
+      <c r="I15" s="177"/>
       <c r="J15" s="22"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2161,18 +2149,18 @@
       <c r="AA15" s="10"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="188" t="s">
+      <c r="B16" s="185" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="189"/>
-      <c r="D16" s="189"/>
+      <c r="C16" s="186"/>
+      <c r="D16" s="186"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="188" t="s">
+      <c r="F16" s="185" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="189"/>
-      <c r="H16" s="189"/>
-      <c r="I16" s="190"/>
+      <c r="G16" s="186"/>
+      <c r="H16" s="186"/>
+      <c r="I16" s="187"/>
       <c r="J16" s="22"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2190,18 +2178,18 @@
       <c r="AA16" s="10"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="191" t="s">
+      <c r="B17" s="188" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="192"/>
-      <c r="D17" s="192"/>
-      <c r="E17" s="193"/>
-      <c r="F17" s="191" t="s">
+      <c r="C17" s="189"/>
+      <c r="D17" s="189"/>
+      <c r="E17" s="190"/>
+      <c r="F17" s="188" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="192"/>
-      <c r="H17" s="192"/>
-      <c r="I17" s="193"/>
+      <c r="G17" s="189"/>
+      <c r="H17" s="189"/>
+      <c r="I17" s="190"/>
       <c r="J17" s="22"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2219,18 +2207,18 @@
       <c r="AA17" s="10"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="194" t="s">
+      <c r="B18" s="191" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="195"/>
+      <c r="C18" s="192"/>
       <c r="D18" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="195" t="s">
+      <c r="E18" s="192" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="195"/>
-      <c r="G18" s="195"/>
+      <c r="F18" s="192"/>
+      <c r="G18" s="192"/>
       <c r="H18" s="23" t="s">
         <v>68</v>
       </c>
@@ -2254,18 +2242,18 @@
       <c r="AA18" s="10"/>
     </row>
     <row r="19" spans="2:30" ht="54.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="176" t="s">
+      <c r="B19" s="193" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="177"/>
+      <c r="C19" s="194"/>
       <c r="D19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="178" t="s">
+      <c r="E19" s="195" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="178"/>
-      <c r="G19" s="178"/>
+      <c r="F19" s="195"/>
+      <c r="G19" s="195"/>
       <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2352,13 +2340,13 @@
       <c r="AD21" s="10"/>
     </row>
     <row r="22" spans="2:30" ht="9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="165" t="s">
+      <c r="B22" s="163" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="165" t="s">
+      <c r="F22" s="163" t="s">
         <v>43</v>
       </c>
       <c r="G22" s="8"/>
@@ -2431,18 +2419,18 @@
       <c r="AD24" s="10"/>
     </row>
     <row r="25" spans="2:30" ht="7.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="179" t="s">
+      <c r="B25" s="196" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="180"/>
-      <c r="D25" s="180"/>
-      <c r="E25" s="181"/>
-      <c r="F25" s="179" t="s">
+      <c r="C25" s="197"/>
+      <c r="D25" s="197"/>
+      <c r="E25" s="198"/>
+      <c r="F25" s="196" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="180"/>
-      <c r="H25" s="180"/>
-      <c r="I25" s="180"/>
+      <c r="G25" s="197"/>
+      <c r="H25" s="197"/>
+      <c r="I25" s="197"/>
       <c r="J25" s="22"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
@@ -2463,13 +2451,13 @@
       <c r="AD25" s="10"/>
     </row>
     <row r="26" spans="2:30" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="159" t="s">
+      <c r="B26" s="157" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
       <c r="E26" s="32"/>
-      <c r="F26" s="159"/>
+      <c r="F26" s="157"/>
       <c r="G26" s="33"/>
       <c r="H26" s="33"/>
       <c r="I26" s="33"/>
@@ -2493,13 +2481,13 @@
       <c r="AD26" s="10"/>
     </row>
     <row r="27" spans="2:30" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="159" t="s">
+      <c r="B27" s="157" t="s">
         <v>43</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
       <c r="E27" s="32"/>
-      <c r="F27" s="159"/>
+      <c r="F27" s="157"/>
       <c r="G27" s="33"/>
       <c r="H27" s="33"/>
       <c r="I27" s="33"/>
@@ -2523,33 +2511,33 @@
       <c r="AD27" s="10"/>
     </row>
     <row r="28" spans="2:30" s="30" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="182" t="s">
+      <c r="B28" s="199" t="s">
         <v>118</v>
       </c>
-      <c r="C28" s="183"/>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
-      <c r="F28" s="182" t="s">
+      <c r="C28" s="200"/>
+      <c r="D28" s="200"/>
+      <c r="E28" s="201"/>
+      <c r="F28" s="199" t="s">
         <v>118</v>
       </c>
-      <c r="G28" s="183"/>
-      <c r="H28" s="183"/>
-      <c r="I28" s="183"/>
+      <c r="G28" s="200"/>
+      <c r="H28" s="200"/>
+      <c r="I28" s="200"/>
       <c r="J28" s="19"/>
     </row>
     <row r="29" spans="2:30" s="30" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="185" t="s">
+      <c r="B29" s="182" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="186"/>
-      <c r="D29" s="186"/>
-      <c r="E29" s="187"/>
-      <c r="F29" s="166" t="s">
+      <c r="C29" s="183"/>
+      <c r="D29" s="183"/>
+      <c r="E29" s="184"/>
+      <c r="F29" s="176" t="s">
         <v>43</v>
       </c>
-      <c r="G29" s="167"/>
-      <c r="H29" s="167"/>
-      <c r="I29" s="168"/>
+      <c r="G29" s="177"/>
+      <c r="H29" s="177"/>
+      <c r="I29" s="178"/>
       <c r="J29" s="19"/>
     </row>
     <row r="30" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2585,18 +2573,18 @@
       <c r="AD30" s="10"/>
     </row>
     <row r="31" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="166" t="s">
+      <c r="B31" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="167"/>
-      <c r="D31" s="167"/>
-      <c r="E31" s="168"/>
-      <c r="F31" s="166" t="s">
+      <c r="C31" s="177"/>
+      <c r="D31" s="177"/>
+      <c r="E31" s="178"/>
+      <c r="F31" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="G31" s="167"/>
-      <c r="H31" s="167"/>
-      <c r="I31" s="167"/>
+      <c r="G31" s="177"/>
+      <c r="H31" s="177"/>
+      <c r="I31" s="177"/>
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:30" ht="20.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -2630,18 +2618,18 @@
       <c r="J33" s="9"/>
     </row>
     <row r="34" spans="2:30" s="35" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="169" t="s">
+      <c r="B34" s="202" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="170"/>
-      <c r="D34" s="170"/>
-      <c r="E34" s="171"/>
-      <c r="F34" s="169" t="s">
+      <c r="C34" s="203"/>
+      <c r="D34" s="203"/>
+      <c r="E34" s="204"/>
+      <c r="F34" s="202" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="170"/>
-      <c r="H34" s="170"/>
-      <c r="I34" s="170"/>
+      <c r="G34" s="203"/>
+      <c r="H34" s="203"/>
+      <c r="I34" s="203"/>
       <c r="J34" s="34"/>
       <c r="N34" s="36"/>
       <c r="O34" s="36"/>
@@ -2662,93 +2650,93 @@
       <c r="AD34" s="36"/>
     </row>
     <row r="35" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="166" t="s">
+      <c r="B35" s="176" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="167"/>
-      <c r="D35" s="167"/>
-      <c r="E35" s="168"/>
-      <c r="F35" s="166" t="s">
+      <c r="C35" s="177"/>
+      <c r="D35" s="177"/>
+      <c r="E35" s="178"/>
+      <c r="F35" s="176" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="167"/>
-      <c r="H35" s="167"/>
-      <c r="I35" s="167"/>
+      <c r="G35" s="177"/>
+      <c r="H35" s="177"/>
+      <c r="I35" s="177"/>
       <c r="J35" s="19"/>
     </row>
     <row r="36" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="166" t="s">
+      <c r="B36" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="167"/>
-      <c r="D36" s="167"/>
-      <c r="E36" s="168"/>
-      <c r="F36" s="166" t="s">
+      <c r="C36" s="177"/>
+      <c r="D36" s="177"/>
+      <c r="E36" s="178"/>
+      <c r="F36" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="G36" s="167"/>
-      <c r="H36" s="167"/>
-      <c r="I36" s="167"/>
+      <c r="G36" s="177"/>
+      <c r="H36" s="177"/>
+      <c r="I36" s="177"/>
       <c r="J36" s="19"/>
     </row>
     <row r="37" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="166" t="s">
+      <c r="B37" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="167"/>
-      <c r="D37" s="167"/>
-      <c r="E37" s="168"/>
-      <c r="F37" s="166" t="s">
+      <c r="C37" s="177"/>
+      <c r="D37" s="177"/>
+      <c r="E37" s="178"/>
+      <c r="F37" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="G37" s="167"/>
-      <c r="H37" s="167"/>
-      <c r="I37" s="167"/>
+      <c r="G37" s="177"/>
+      <c r="H37" s="177"/>
+      <c r="I37" s="177"/>
       <c r="J37" s="19"/>
     </row>
     <row r="38" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="166" t="s">
+      <c r="B38" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="167"/>
-      <c r="D38" s="167"/>
-      <c r="E38" s="168"/>
-      <c r="F38" s="166" t="s">
+      <c r="C38" s="177"/>
+      <c r="D38" s="177"/>
+      <c r="E38" s="178"/>
+      <c r="F38" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="G38" s="167"/>
-      <c r="H38" s="167"/>
-      <c r="I38" s="167"/>
+      <c r="G38" s="177"/>
+      <c r="H38" s="177"/>
+      <c r="I38" s="177"/>
       <c r="J38" s="19"/>
     </row>
     <row r="39" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="166" t="s">
+      <c r="B39" s="176" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="167"/>
-      <c r="D39" s="167"/>
-      <c r="E39" s="168"/>
-      <c r="F39" s="166" t="s">
+      <c r="C39" s="177"/>
+      <c r="D39" s="177"/>
+      <c r="E39" s="178"/>
+      <c r="F39" s="176" t="s">
         <v>40</v>
       </c>
-      <c r="G39" s="167"/>
-      <c r="H39" s="167"/>
-      <c r="I39" s="167"/>
+      <c r="G39" s="177"/>
+      <c r="H39" s="177"/>
+      <c r="I39" s="177"/>
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="166" t="s">
+      <c r="B40" s="176" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="167"/>
-      <c r="D40" s="167"/>
-      <c r="E40" s="168"/>
-      <c r="F40" s="166" t="s">
+      <c r="C40" s="177"/>
+      <c r="D40" s="177"/>
+      <c r="E40" s="178"/>
+      <c r="F40" s="176" t="s">
         <v>42</v>
       </c>
-      <c r="G40" s="167"/>
-      <c r="H40" s="167"/>
-      <c r="I40" s="167"/>
+      <c r="G40" s="177"/>
+      <c r="H40" s="177"/>
+      <c r="I40" s="177"/>
       <c r="J40" s="19"/>
     </row>
     <row r="41" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2767,18 +2755,18 @@
       <c r="J41" s="19"/>
     </row>
     <row r="42" spans="2:30" s="35" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="169" t="s">
+      <c r="B42" s="202" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="170"/>
-      <c r="D42" s="170"/>
-      <c r="E42" s="171"/>
-      <c r="F42" s="169" t="s">
+      <c r="C42" s="203"/>
+      <c r="D42" s="203"/>
+      <c r="E42" s="204"/>
+      <c r="F42" s="202" t="s">
         <v>12</v>
       </c>
-      <c r="G42" s="172"/>
-      <c r="H42" s="172"/>
-      <c r="I42" s="172"/>
+      <c r="G42" s="205"/>
+      <c r="H42" s="205"/>
+      <c r="I42" s="205"/>
       <c r="J42" s="34"/>
       <c r="N42" s="36"/>
       <c r="O42" s="36"/>
@@ -2799,18 +2787,18 @@
       <c r="AD42" s="36"/>
     </row>
     <row r="43" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="166" t="s">
+      <c r="B43" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="167"/>
-      <c r="D43" s="167"/>
-      <c r="E43" s="168"/>
-      <c r="F43" s="166" t="s">
+      <c r="C43" s="177"/>
+      <c r="D43" s="177"/>
+      <c r="E43" s="178"/>
+      <c r="F43" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="G43" s="167"/>
-      <c r="H43" s="167"/>
-      <c r="I43" s="167"/>
+      <c r="G43" s="177"/>
+      <c r="H43" s="177"/>
+      <c r="I43" s="177"/>
       <c r="J43" s="19"/>
     </row>
     <row r="44" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2870,18 +2858,18 @@
       <c r="J47" s="19"/>
     </row>
     <row r="48" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="166" t="s">
+      <c r="B48" s="176" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="167"/>
-      <c r="D48" s="167"/>
-      <c r="E48" s="168"/>
-      <c r="F48" s="166" t="s">
+      <c r="C48" s="177"/>
+      <c r="D48" s="177"/>
+      <c r="E48" s="178"/>
+      <c r="F48" s="176" t="s">
         <v>46</v>
       </c>
-      <c r="G48" s="167"/>
-      <c r="H48" s="167"/>
-      <c r="I48" s="168"/>
+      <c r="G48" s="177"/>
+      <c r="H48" s="177"/>
+      <c r="I48" s="178"/>
       <c r="J48" s="19"/>
     </row>
     <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3100,34 +3088,26 @@
     <row r="90" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="F9:I10"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="B19:C19"/>
@@ -3142,26 +3122,34 @@
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="F31:I31"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="F9:I10"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <conditionalFormatting sqref="H19">
     <cfRule type="notContainsBlanks" dxfId="3" priority="2">
@@ -3200,8 +3188,8 @@
   </sheetPr>
   <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3225,7 +3213,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="56"/>
-      <c r="G1" s="156" t="s">
+      <c r="G1" s="154" t="s">
         <v>43</v>
       </c>
       <c r="N1" s="58"/>
@@ -3472,13 +3460,13 @@
     </row>
     <row r="14" spans="1:14" ht="44.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="56"/>
-      <c r="B14" s="211" t="s">
+      <c r="B14" s="164" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="212"/>
-      <c r="D14" s="212"/>
-      <c r="E14" s="212"/>
-      <c r="F14" s="212"/>
+      <c r="C14" s="165"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="165"/>
+      <c r="F14" s="165"/>
       <c r="G14" s="115"/>
       <c r="H14" s="152" t="s">
         <v>13</v>
@@ -3492,10 +3480,10 @@
     </row>
     <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="84"/>
-      <c r="B15" s="207" t="s">
+      <c r="B15" s="208" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="208"/>
+      <c r="C15" s="209"/>
       <c r="D15" s="102" t="s">
         <v>93</v>
       </c>
@@ -3520,11 +3508,11 @@
     </row>
     <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="56"/>
-      <c r="B16" s="115" t="s">
+      <c r="B16" s="104" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="104"/>
-      <c r="D16" s="153" t="s">
+      <c r="D16" s="105" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="105"/>
@@ -3532,7 +3520,7 @@
         <v>92</v>
       </c>
       <c r="G16" s="105"/>
-      <c r="H16" s="155" t="s">
+      <c r="H16" s="166" t="s">
         <v>43</v>
       </c>
       <c r="I16" s="105"/>
@@ -3584,11 +3572,11 @@
         <v>43</v>
       </c>
       <c r="E18" s="106"/>
-      <c r="F18" s="154" t="s">
+      <c r="F18" s="153" t="s">
         <v>43</v>
       </c>
       <c r="G18" s="141"/>
-      <c r="H18" s="213" t="s">
+      <c r="H18" s="166" t="s">
         <v>43</v>
       </c>
       <c r="I18" s="106"/>
@@ -3604,10 +3592,10 @@
     </row>
     <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="56"/>
-      <c r="B19" s="210" t="s">
+      <c r="B19" s="145" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="209"/>
+      <c r="C19" s="128"/>
       <c r="D19" s="128" t="s">
         <v>90</v>
       </c>
@@ -3712,12 +3700,12 @@
       <c r="B23" s="136" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="205" t="s">
+      <c r="C23" s="206" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="205"/>
-      <c r="E23" s="205"/>
-      <c r="F23" s="205"/>
+      <c r="D23" s="206"/>
+      <c r="E23" s="206"/>
+      <c r="F23" s="206"/>
       <c r="G23" s="137"/>
       <c r="H23" s="138" t="s">
         <v>78</v>
@@ -3728,10 +3716,10 @@
       <c r="J23" s="77">
         <v>14</v>
       </c>
-      <c r="K23" s="206" t="s">
+      <c r="K23" s="207" t="s">
         <v>77</v>
       </c>
-      <c r="L23" s="206"/>
+      <c r="L23" s="207"/>
       <c r="M23" s="76" t="s">
         <v>74</v>
       </c>
@@ -4027,7 +4015,7 @@
     </row>
     <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="56"/>
-      <c r="B41" s="161" t="s">
+      <c r="B41" s="159" t="s">
         <v>70</v>
       </c>
       <c r="C41" s="68"/>
@@ -4046,7 +4034,7 @@
       <c r="N41" s="58"/>
     </row>
     <row r="42" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="164"/>
+      <c r="B42" s="162"/>
       <c r="C42" s="68"/>
       <c r="D42" s="68"/>
       <c r="E42" s="68"/>
@@ -4060,7 +4048,7 @@
       <c r="N42" s="58"/>
     </row>
     <row r="43" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="164"/>
+      <c r="B43" s="162"/>
       <c r="C43" s="68"/>
       <c r="D43" s="68"/>
       <c r="E43" s="68"/>
@@ -4075,7 +4063,7 @@
       <c r="N43" s="58"/>
     </row>
     <row r="44" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="164"/>
+      <c r="B44" s="162"/>
       <c r="C44" s="68"/>
       <c r="D44" s="68"/>
       <c r="E44" s="68"/>
@@ -4090,8 +4078,8 @@
       <c r="N44" s="58"/>
     </row>
     <row r="45" spans="1:14" s="64" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="160"/>
-      <c r="B45" s="162"/>
+      <c r="A45" s="158"/>
+      <c r="B45" s="160"/>
       <c r="C45" s="67"/>
       <c r="D45" s="67"/>
       <c r="E45" s="67"/>
@@ -4099,7 +4087,7 @@
       <c r="G45" s="66"/>
       <c r="H45" s="65"/>
       <c r="I45" s="132"/>
-      <c r="J45" s="163"/>
+      <c r="J45" s="161"/>
       <c r="K45" s="133"/>
       <c r="L45" s="133"/>
       <c r="M45" s="133"/>
@@ -4112,11 +4100,10 @@
     <row r="50" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="55" ht="2.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
export contract tmps united, minor bugs fixed
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB32BAD-9EFA-49A8-A7B2-63E9571974E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694D6459-DB75-48EC-9D6A-12B676D157AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="117">
   <si>
     <t xml:space="preserve">Parties of Contract: </t>
   </si>
@@ -496,9 +496,6 @@
   </si>
   <si>
     <t>A/C:</t>
-  </si>
-  <si>
-    <t>ы</t>
   </si>
 </sst>
 </file>
@@ -815,7 +812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1254,35 +1251,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1357,24 +1333,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1398,6 +1356,63 @@
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1764,8 +1779,8 @@
   </sheetPr>
   <dimension ref="A1:AF94"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScale="91" zoomScaleNormal="100" zoomScaleSheetLayoutView="91" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="91" zoomScaleNormal="100" zoomScaleSheetLayoutView="91" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1817,18 +1832,18 @@
       <c r="I1" s="145"/>
     </row>
     <row r="2" spans="2:30" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="180" t="s">
+      <c r="B2" s="173" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="181"/>
-      <c r="D2" s="181"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="180" t="s">
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="173" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="181"/>
-      <c r="H2" s="181"/>
-      <c r="I2" s="181"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
+      <c r="I2" s="174"/>
       <c r="J2" s="146"/>
       <c r="L2" s="8"/>
       <c r="N2" s="15"/>
@@ -1838,18 +1853,18 @@
       <c r="AD2" s="15"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="183" t="s">
+      <c r="B3" s="176" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="184"/>
-      <c r="D3" s="184"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="183" t="s">
+      <c r="C3" s="177"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="178"/>
+      <c r="F3" s="176" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="184"/>
-      <c r="H3" s="184"/>
-      <c r="I3" s="184"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="177"/>
+      <c r="I3" s="177"/>
       <c r="J3" s="6"/>
       <c r="L3" s="8"/>
       <c r="O3" s="7"/>
@@ -1866,18 +1881,18 @@
       <c r="Z3" s="7"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="183" t="s">
+      <c r="B4" s="176" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="185"/>
-      <c r="F4" s="183" t="s">
+      <c r="C4" s="177"/>
+      <c r="D4" s="177"/>
+      <c r="E4" s="178"/>
+      <c r="F4" s="176" t="s">
         <v>90</v>
       </c>
-      <c r="G4" s="184"/>
-      <c r="H4" s="184"/>
-      <c r="I4" s="184"/>
+      <c r="G4" s="177"/>
+      <c r="H4" s="177"/>
+      <c r="I4" s="177"/>
       <c r="J4" s="6"/>
       <c r="N4" s="10"/>
       <c r="O4" s="11"/>
@@ -1898,18 +1913,18 @@
       <c r="AD4" s="10"/>
     </row>
     <row r="5" spans="2:30" s="14" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="189" t="s">
+      <c r="B5" s="182" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="190"/>
-      <c r="D5" s="190"/>
-      <c r="E5" s="191"/>
-      <c r="F5" s="189" t="s">
+      <c r="C5" s="183"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="184"/>
+      <c r="F5" s="182" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="190"/>
-      <c r="H5" s="190"/>
-      <c r="I5" s="190"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
       <c r="J5" s="13"/>
       <c r="N5" s="15"/>
       <c r="AA5" s="15"/>
@@ -1974,44 +1989,44 @@
       <c r="Z7" s="7"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="192" t="s">
+      <c r="B8" s="185" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="193"/>
-      <c r="D8" s="193"/>
-      <c r="E8" s="194"/>
-      <c r="F8" s="192" t="s">
+      <c r="C8" s="186"/>
+      <c r="D8" s="186"/>
+      <c r="E8" s="187"/>
+      <c r="F8" s="185" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="193"/>
-      <c r="H8" s="193"/>
-      <c r="I8" s="193"/>
+      <c r="G8" s="186"/>
+      <c r="H8" s="186"/>
+      <c r="I8" s="186"/>
       <c r="J8" s="19"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="186" t="s">
+      <c r="B9" s="179" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="187"/>
-      <c r="D9" s="187"/>
-      <c r="E9" s="188"/>
-      <c r="F9" s="186" t="s">
+      <c r="C9" s="180"/>
+      <c r="D9" s="180"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="179" t="s">
         <v>96</v>
       </c>
-      <c r="G9" s="187"/>
-      <c r="H9" s="187"/>
-      <c r="I9" s="188"/>
+      <c r="G9" s="180"/>
+      <c r="H9" s="180"/>
+      <c r="I9" s="181"/>
       <c r="J9" s="19"/>
     </row>
     <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="186"/>
-      <c r="C10" s="187"/>
-      <c r="D10" s="187"/>
-      <c r="E10" s="188"/>
-      <c r="F10" s="186"/>
-      <c r="G10" s="187"/>
-      <c r="H10" s="187"/>
-      <c r="I10" s="188"/>
+      <c r="B10" s="179"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="180"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="179"/>
+      <c r="G10" s="180"/>
+      <c r="H10" s="180"/>
+      <c r="I10" s="181"/>
       <c r="J10" s="19"/>
       <c r="N10" s="15"/>
       <c r="O10" s="7"/>
@@ -2086,18 +2101,18 @@
       <c r="Z12" s="7"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="186" t="s">
+      <c r="B13" s="179" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="187"/>
-      <c r="D13" s="187"/>
-      <c r="E13" s="188"/>
-      <c r="F13" s="186" t="s">
+      <c r="C13" s="180"/>
+      <c r="D13" s="180"/>
+      <c r="E13" s="181"/>
+      <c r="F13" s="179" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="187"/>
-      <c r="H13" s="187"/>
-      <c r="I13" s="187"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
       <c r="J13" s="19"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
@@ -2115,18 +2130,18 @@
       <c r="AA13" s="7"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="186" t="s">
+      <c r="B14" s="179" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="187"/>
-      <c r="D14" s="187"/>
-      <c r="E14" s="188"/>
-      <c r="F14" s="186" t="s">
+      <c r="C14" s="180"/>
+      <c r="D14" s="180"/>
+      <c r="E14" s="181"/>
+      <c r="F14" s="179" t="s">
         <v>100</v>
       </c>
-      <c r="G14" s="187"/>
-      <c r="H14" s="187"/>
-      <c r="I14" s="187"/>
+      <c r="G14" s="180"/>
+      <c r="H14" s="180"/>
+      <c r="I14" s="180"/>
       <c r="J14" s="19"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
@@ -2144,18 +2159,18 @@
       <c r="AA14" s="7"/>
     </row>
     <row r="15" spans="2:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="186" t="s">
+      <c r="B15" s="179" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="187"/>
-      <c r="D15" s="187"/>
-      <c r="E15" s="188"/>
-      <c r="F15" s="186" t="s">
+      <c r="C15" s="180"/>
+      <c r="D15" s="180"/>
+      <c r="E15" s="181"/>
+      <c r="F15" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="187"/>
-      <c r="H15" s="187"/>
-      <c r="I15" s="187"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="180"/>
+      <c r="I15" s="180"/>
       <c r="J15" s="19"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
@@ -2202,18 +2217,18 @@
       <c r="AA16" s="7"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="195" t="s">
+      <c r="B17" s="188" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="196"/>
-      <c r="D17" s="196"/>
-      <c r="E17" s="197"/>
-      <c r="F17" s="195" t="s">
+      <c r="C17" s="189"/>
+      <c r="D17" s="189"/>
+      <c r="E17" s="190"/>
+      <c r="F17" s="188" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="196"/>
-      <c r="H17" s="196"/>
-      <c r="I17" s="196"/>
+      <c r="G17" s="189"/>
+      <c r="H17" s="189"/>
+      <c r="I17" s="189"/>
       <c r="J17" s="19"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
@@ -2231,18 +2246,18 @@
       <c r="AA17" s="7"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="198" t="s">
+      <c r="B18" s="191" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="199"/>
+      <c r="C18" s="192"/>
       <c r="D18" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="199" t="s">
+      <c r="E18" s="192" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="199"/>
-      <c r="G18" s="199"/>
+      <c r="F18" s="192"/>
+      <c r="G18" s="192"/>
       <c r="H18" s="20" t="s">
         <v>35</v>
       </c>
@@ -2266,18 +2281,18 @@
       <c r="AA18" s="7"/>
     </row>
     <row r="19" spans="2:30" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="200" t="s">
+      <c r="B19" s="193" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="201"/>
+      <c r="C19" s="194"/>
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="202" t="s">
+      <c r="E19" s="195" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="202"/>
-      <c r="G19" s="202"/>
+      <c r="F19" s="195"/>
+      <c r="G19" s="195"/>
       <c r="H19" s="1" t="s">
         <v>12</v>
       </c>
@@ -2307,15 +2322,15 @@
       <c r="B20" s="152" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="172"/>
-      <c r="D20" s="172"/>
-      <c r="E20" s="173"/>
-      <c r="F20" s="168" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="169"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="171"/>
+      <c r="C20" s="168"/>
+      <c r="D20" s="168"/>
+      <c r="E20" s="169"/>
+      <c r="F20" s="219" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="220"/>
+      <c r="H20" s="221"/>
+      <c r="I20" s="222"/>
       <c r="J20" s="2"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
@@ -2336,19 +2351,19 @@
       <c r="AD20" s="7"/>
     </row>
     <row r="21" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="152" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="172"/>
-      <c r="D21" s="172"/>
-      <c r="E21" s="173"/>
-      <c r="F21" s="152" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="173"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="174"/>
-      <c r="J21" s="175"/>
+      <c r="B21" s="204" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="205"/>
+      <c r="D21" s="205"/>
+      <c r="E21" s="206"/>
+      <c r="F21" s="204" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="206"/>
+      <c r="H21" s="205"/>
+      <c r="I21" s="207"/>
+      <c r="J21" s="170"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
@@ -2368,19 +2383,19 @@
       <c r="AD21" s="7"/>
     </row>
     <row r="22" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="152" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="173"/>
-      <c r="D22" s="173"/>
-      <c r="E22" s="173"/>
-      <c r="F22" s="152" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="173"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="174"/>
-      <c r="J22" s="175"/>
+      <c r="B22" s="204" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="206"/>
+      <c r="D22" s="206"/>
+      <c r="E22" s="206"/>
+      <c r="F22" s="204" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="206"/>
+      <c r="H22" s="205"/>
+      <c r="I22" s="207"/>
+      <c r="J22" s="170"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
@@ -2400,19 +2415,19 @@
       <c r="AD22" s="7"/>
     </row>
     <row r="23" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="152" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="173"/>
-      <c r="D23" s="173"/>
-      <c r="E23" s="173"/>
-      <c r="F23" s="152" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="173"/>
-      <c r="H23" s="172"/>
-      <c r="I23" s="174"/>
-      <c r="J23" s="175"/>
+      <c r="B23" s="204" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="206"/>
+      <c r="D23" s="206"/>
+      <c r="E23" s="206"/>
+      <c r="F23" s="204" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="206"/>
+      <c r="H23" s="205"/>
+      <c r="I23" s="207"/>
+      <c r="J23" s="170"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
@@ -2432,19 +2447,19 @@
       <c r="AD23" s="7"/>
     </row>
     <row r="24" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="173"/>
-      <c r="F24" s="160" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="176"/>
-      <c r="I24" s="177"/>
-      <c r="J24" s="175"/>
+      <c r="B24" s="208" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="209"/>
+      <c r="D24" s="209"/>
+      <c r="E24" s="206"/>
+      <c r="F24" s="210" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="211"/>
+      <c r="H24" s="212"/>
+      <c r="I24" s="213"/>
+      <c r="J24" s="170"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
@@ -2464,19 +2479,19 @@
       <c r="AD24" s="7"/>
     </row>
     <row r="25" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="152" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="173"/>
-      <c r="F25" s="152" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="176"/>
-      <c r="I25" s="177"/>
-      <c r="J25" s="175"/>
+      <c r="B25" s="204" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="209"/>
+      <c r="D25" s="209"/>
+      <c r="E25" s="206"/>
+      <c r="F25" s="204" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="211"/>
+      <c r="H25" s="212"/>
+      <c r="I25" s="213"/>
+      <c r="J25" s="170"/>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
@@ -2496,33 +2511,33 @@
       <c r="AD25" s="7"/>
     </row>
     <row r="26" spans="2:30" s="28" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="156" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="156" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="157"/>
+      <c r="B26" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="18"/>
       <c r="J26" s="156"/>
     </row>
     <row r="27" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="178" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="160" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="157"/>
+      <c r="B27" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="209"/>
+      <c r="D27" s="209"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="210" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="211"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="18"/>
       <c r="J27" s="13"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
@@ -2543,18 +2558,18 @@
       <c r="AD27" s="7"/>
     </row>
     <row r="28" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="203" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="204"/>
-      <c r="D28" s="204"/>
-      <c r="E28" s="204"/>
-      <c r="F28" s="203" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="204"/>
-      <c r="H28" s="204"/>
-      <c r="I28" s="205"/>
+      <c r="B28" s="179" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="180"/>
+      <c r="D28" s="180"/>
+      <c r="E28" s="180"/>
+      <c r="F28" s="179" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="180"/>
+      <c r="H28" s="180"/>
+      <c r="I28" s="181"/>
       <c r="J28" s="13"/>
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
@@ -2575,18 +2590,18 @@
       <c r="AD28" s="7"/>
     </row>
     <row r="29" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="156" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="156" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="157"/>
+      <c r="B29" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="18"/>
       <c r="J29" s="13"/>
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
@@ -2607,18 +2622,18 @@
       <c r="AD29" s="7"/>
     </row>
     <row r="30" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="156" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="156" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="157"/>
+      <c r="B30" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="18"/>
       <c r="J30" s="13"/>
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
@@ -2639,48 +2654,48 @@
       <c r="AD30" s="7"/>
     </row>
     <row r="31" spans="2:30" s="28" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="206" t="s">
+      <c r="B31" s="214" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="207"/>
-      <c r="D31" s="207"/>
-      <c r="E31" s="207"/>
-      <c r="F31" s="206" t="s">
+      <c r="C31" s="215"/>
+      <c r="D31" s="215"/>
+      <c r="E31" s="215"/>
+      <c r="F31" s="214" t="s">
         <v>84</v>
       </c>
-      <c r="G31" s="207"/>
-      <c r="H31" s="207"/>
-      <c r="I31" s="208"/>
+      <c r="G31" s="215"/>
+      <c r="H31" s="215"/>
+      <c r="I31" s="216"/>
       <c r="J31" s="156"/>
     </row>
     <row r="32" spans="2:30" s="28" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="189" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="190"/>
-      <c r="D32" s="190"/>
-      <c r="E32" s="190"/>
-      <c r="F32" s="203" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="204"/>
-      <c r="H32" s="204"/>
-      <c r="I32" s="205"/>
+      <c r="B32" s="185" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="186"/>
+      <c r="D32" s="186"/>
+      <c r="E32" s="186"/>
+      <c r="F32" s="179" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="180"/>
+      <c r="H32" s="180"/>
+      <c r="I32" s="181"/>
       <c r="J32" s="156"/>
     </row>
     <row r="33" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="178" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="160" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="161"/>
-      <c r="H33" s="161"/>
-      <c r="I33" s="162"/>
+      <c r="B33" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="211"/>
+      <c r="D33" s="211"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="210" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="217"/>
+      <c r="H33" s="217"/>
+      <c r="I33" s="218"/>
       <c r="J33" s="13"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
@@ -2701,18 +2716,18 @@
       <c r="AD33" s="7"/>
     </row>
     <row r="34" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="203" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="204"/>
-      <c r="D34" s="204"/>
-      <c r="E34" s="204"/>
-      <c r="F34" s="203" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="204"/>
-      <c r="H34" s="204"/>
-      <c r="I34" s="205"/>
+      <c r="B34" s="179" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="180"/>
+      <c r="D34" s="180"/>
+      <c r="E34" s="180"/>
+      <c r="F34" s="179" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="180"/>
+      <c r="H34" s="180"/>
+      <c r="I34" s="181"/>
       <c r="J34" s="6"/>
     </row>
     <row r="35" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
@@ -2730,19 +2745,19 @@
       <c r="I35" s="159"/>
       <c r="J35" s="6"/>
     </row>
-    <row r="36" spans="1:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="179"/>
-      <c r="B36" s="178"/>
+    <row r="36" spans="1:30" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="172"/>
+      <c r="B36" s="171"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-      <c r="F36" s="178"/>
+      <c r="F36" s="171"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="43"/>
       <c r="J36" s="6"/>
     </row>
-    <row r="37" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:30" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="160" t="s">
         <v>22</v>
       </c>
@@ -2758,18 +2773,18 @@
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:30" s="28" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="209" t="s">
+      <c r="B38" s="196" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="210"/>
-      <c r="D38" s="210"/>
-      <c r="E38" s="210"/>
-      <c r="F38" s="209" t="s">
+      <c r="C38" s="197"/>
+      <c r="D38" s="197"/>
+      <c r="E38" s="197"/>
+      <c r="F38" s="196" t="s">
         <v>101</v>
       </c>
-      <c r="G38" s="210"/>
-      <c r="H38" s="210"/>
-      <c r="I38" s="211"/>
+      <c r="G38" s="197"/>
+      <c r="H38" s="197"/>
+      <c r="I38" s="198"/>
       <c r="J38" s="27"/>
       <c r="N38" s="29"/>
       <c r="O38" s="29"/>
@@ -2790,103 +2805,103 @@
       <c r="AD38" s="29"/>
     </row>
     <row r="39" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="186" t="s">
+      <c r="B39" s="179" t="s">
         <v>98</v>
       </c>
-      <c r="C39" s="187"/>
-      <c r="D39" s="187"/>
-      <c r="E39" s="187"/>
-      <c r="F39" s="186" t="s">
+      <c r="C39" s="180"/>
+      <c r="D39" s="180"/>
+      <c r="E39" s="180"/>
+      <c r="F39" s="179" t="s">
         <v>102</v>
       </c>
-      <c r="G39" s="187"/>
-      <c r="H39" s="187"/>
-      <c r="I39" s="188"/>
+      <c r="G39" s="180"/>
+      <c r="H39" s="180"/>
+      <c r="I39" s="181"/>
       <c r="J39" s="16"/>
     </row>
     <row r="40" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="186" t="s">
+      <c r="B40" s="179" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="187"/>
-      <c r="D40" s="187"/>
-      <c r="E40" s="188"/>
-      <c r="F40" s="186" t="s">
+      <c r="C40" s="180"/>
+      <c r="D40" s="180"/>
+      <c r="E40" s="181"/>
+      <c r="F40" s="179" t="s">
         <v>103</v>
       </c>
-      <c r="G40" s="187"/>
-      <c r="H40" s="187"/>
-      <c r="I40" s="187"/>
+      <c r="G40" s="180"/>
+      <c r="H40" s="180"/>
+      <c r="I40" s="180"/>
       <c r="J40" s="16"/>
     </row>
     <row r="41" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="186" t="s">
+      <c r="B41" s="179" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="187"/>
-      <c r="D41" s="187"/>
-      <c r="E41" s="188"/>
-      <c r="F41" s="186" t="s">
+      <c r="C41" s="180"/>
+      <c r="D41" s="180"/>
+      <c r="E41" s="181"/>
+      <c r="F41" s="179" t="s">
         <v>106</v>
       </c>
-      <c r="G41" s="187"/>
-      <c r="H41" s="187"/>
-      <c r="I41" s="187"/>
+      <c r="G41" s="180"/>
+      <c r="H41" s="180"/>
+      <c r="I41" s="180"/>
       <c r="J41" s="16"/>
     </row>
     <row r="42" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="186" t="s">
+      <c r="B42" s="179" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="187"/>
-      <c r="D42" s="187"/>
-      <c r="E42" s="188"/>
-      <c r="F42" s="186" t="s">
+      <c r="C42" s="180"/>
+      <c r="D42" s="180"/>
+      <c r="E42" s="181"/>
+      <c r="F42" s="179" t="s">
         <v>107</v>
       </c>
-      <c r="G42" s="187"/>
-      <c r="H42" s="187"/>
-      <c r="I42" s="187"/>
+      <c r="G42" s="180"/>
+      <c r="H42" s="180"/>
+      <c r="I42" s="180"/>
       <c r="J42" s="16"/>
     </row>
     <row r="43" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="186" t="s">
+      <c r="B43" s="179" t="s">
         <v>108</v>
       </c>
-      <c r="C43" s="187"/>
-      <c r="D43" s="187"/>
-      <c r="E43" s="188"/>
-      <c r="F43" s="186" t="s">
+      <c r="C43" s="180"/>
+      <c r="D43" s="180"/>
+      <c r="E43" s="181"/>
+      <c r="F43" s="179" t="s">
         <v>109</v>
       </c>
-      <c r="G43" s="187"/>
-      <c r="H43" s="187"/>
-      <c r="I43" s="187"/>
+      <c r="G43" s="180"/>
+      <c r="H43" s="180"/>
+      <c r="I43" s="180"/>
       <c r="J43" s="16"/>
     </row>
     <row r="44" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="186" t="s">
+      <c r="B44" s="179" t="s">
         <v>110</v>
       </c>
-      <c r="C44" s="187"/>
-      <c r="D44" s="187"/>
-      <c r="E44" s="188"/>
-      <c r="F44" s="186" t="s">
+      <c r="C44" s="180"/>
+      <c r="D44" s="180"/>
+      <c r="E44" s="181"/>
+      <c r="F44" s="179" t="s">
         <v>111</v>
       </c>
-      <c r="G44" s="187"/>
-      <c r="H44" s="187"/>
-      <c r="I44" s="187"/>
+      <c r="G44" s="180"/>
+      <c r="H44" s="180"/>
+      <c r="I44" s="180"/>
       <c r="J44" s="16"/>
     </row>
-    <row r="45" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="52" t="s">
+    <row r="45" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="171" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="52" t="s">
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="157"/>
+      <c r="F45" s="171" t="s">
         <v>29</v>
       </c>
       <c r="G45" s="17"/>
@@ -2895,18 +2910,18 @@
       <c r="J45" s="16"/>
     </row>
     <row r="46" spans="1:30" s="28" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="209" t="s">
+      <c r="B46" s="196" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="210"/>
-      <c r="D46" s="210"/>
-      <c r="E46" s="211"/>
-      <c r="F46" s="209" t="s">
+      <c r="C46" s="197"/>
+      <c r="D46" s="197"/>
+      <c r="E46" s="198"/>
+      <c r="F46" s="196" t="s">
         <v>97</v>
       </c>
-      <c r="G46" s="212"/>
-      <c r="H46" s="212"/>
-      <c r="I46" s="212"/>
+      <c r="G46" s="199"/>
+      <c r="H46" s="199"/>
+      <c r="I46" s="199"/>
       <c r="J46" s="27"/>
       <c r="N46" s="29"/>
       <c r="O46" s="29"/>
@@ -2927,18 +2942,18 @@
       <c r="AD46" s="29"/>
     </row>
     <row r="47" spans="1:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="186" t="s">
+      <c r="B47" s="179" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="187"/>
-      <c r="D47" s="187"/>
-      <c r="E47" s="188"/>
-      <c r="F47" s="186" t="s">
+      <c r="C47" s="180"/>
+      <c r="D47" s="180"/>
+      <c r="E47" s="181"/>
+      <c r="F47" s="179" t="s">
         <v>112</v>
       </c>
-      <c r="G47" s="187"/>
-      <c r="H47" s="187"/>
-      <c r="I47" s="187"/>
+      <c r="G47" s="180"/>
+      <c r="H47" s="180"/>
+      <c r="I47" s="180"/>
       <c r="J47" s="16"/>
     </row>
     <row r="48" spans="1:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2998,18 +3013,18 @@
       <c r="J51" s="16"/>
     </row>
     <row r="52" spans="2:10" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="186" t="s">
+      <c r="B52" s="179" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="187"/>
-      <c r="D52" s="187"/>
-      <c r="E52" s="188"/>
-      <c r="F52" s="186" t="s">
+      <c r="C52" s="180"/>
+      <c r="D52" s="180"/>
+      <c r="E52" s="181"/>
+      <c r="F52" s="179" t="s">
         <v>105</v>
       </c>
-      <c r="G52" s="187"/>
-      <c r="H52" s="187"/>
-      <c r="I52" s="188"/>
+      <c r="G52" s="180"/>
+      <c r="H52" s="180"/>
+      <c r="I52" s="181"/>
       <c r="J52" s="16"/>
     </row>
     <row r="53" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3076,9 +3091,7 @@
       <c r="B57" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="34" t="s">
-        <v>117</v>
-      </c>
+      <c r="C57" s="34"/>
       <c r="D57" s="34"/>
       <c r="E57" s="35"/>
       <c r="F57" s="34" t="s">
@@ -3320,7 +3333,7 @@
   </sheetPr>
   <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -3612,10 +3625,10 @@
     </row>
     <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="74"/>
-      <c r="B15" s="215" t="s">
+      <c r="B15" s="202" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="216"/>
+      <c r="C15" s="203"/>
       <c r="D15" s="92" t="s">
         <v>60</v>
       </c>
@@ -3832,12 +3845,12 @@
       <c r="B23" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="213" t="s">
+      <c r="C23" s="200" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="213"/>
-      <c r="E23" s="213"/>
-      <c r="F23" s="213"/>
+      <c r="D23" s="200"/>
+      <c r="E23" s="200"/>
+      <c r="F23" s="200"/>
       <c r="G23" s="127"/>
       <c r="H23" s="128" t="s">
         <v>45</v>
@@ -3848,10 +3861,10 @@
       <c r="J23" s="67">
         <v>14</v>
       </c>
-      <c r="K23" s="214" t="s">
+      <c r="K23" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="L23" s="214"/>
+      <c r="L23" s="201"/>
       <c r="M23" s="66" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
rows logic export contract tmp now in single module
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694D6459-DB75-48EC-9D6A-12B676D157AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EAE096-025D-456A-875B-19EA5E9A86B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
@@ -23,36 +23,36 @@
     <definedName name="MID_Contract">Export_Contract!$E$1</definedName>
     <definedName name="MID_Invoice">Invoice!$G$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$N$50</definedName>
-    <definedName name="Seal_agent_end">Export_Contract!$H$58</definedName>
-    <definedName name="Seal_agent_start">Export_Contract!$G$48</definedName>
-    <definedName name="Seal_seller_end">Export_Contract!$C$58</definedName>
-    <definedName name="Seal_seller_start">Export_Contract!$C$50</definedName>
-    <definedName name="Sign_agent_end">Export_Contract!$G$58</definedName>
-    <definedName name="Sign_agent_start">Export_Contract!$G$56</definedName>
-    <definedName name="Sign_seller_start">Export_Contract!$C$56</definedName>
-    <definedName name="Адреса_банк_получателя">Export_Contract!$B$40</definedName>
-    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$41</definedName>
-    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$42</definedName>
-    <definedName name="Адреса_подпись">Export_Contract!$B$57</definedName>
-    <definedName name="Адреса_покупатель">Export_Contract!$B$46</definedName>
-    <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$47</definedName>
-    <definedName name="Адреса_покупатель_банк">Export_Contract!$B$49</definedName>
-    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$B$52</definedName>
-    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$B$51</definedName>
-    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$B$53</definedName>
-    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$B$54</definedName>
-    <definedName name="Адреса_покупатель_счет">Export_Contract!$B$55</definedName>
-    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$B$43</definedName>
-    <definedName name="Адреса_получатель_счет">Export_Contract!$B$44</definedName>
-    <definedName name="Адреса_продавец">Export_Contract!$B$38</definedName>
-    <definedName name="Адреса_продавец_адрес">Export_Contract!$B$39</definedName>
-    <definedName name="Адреса_сторон_заголовок">Export_Contract!$B$35</definedName>
-    <definedName name="Доставка_дата">Export_Contract!$B$30</definedName>
-    <definedName name="Доставка_заголовок">Export_Contract!$B$27</definedName>
-    <definedName name="Доставка_порт">Export_Contract!$B$31</definedName>
-    <definedName name="Доставка_приемка">Export_Contract!$B$29</definedName>
-    <definedName name="Доставка_транспорт">Export_Contract!$B$20</definedName>
-    <definedName name="Доставка_условия">Export_Contract!$B$28</definedName>
+    <definedName name="Seal_agent_end">Export_Contract!$H$59</definedName>
+    <definedName name="Seal_agent_start">Export_Contract!$G$49</definedName>
+    <definedName name="Seal_seller_end">Export_Contract!$C$59</definedName>
+    <definedName name="Seal_seller_start">Export_Contract!$C$51</definedName>
+    <definedName name="Sign_agent_end">Export_Contract!$G$59</definedName>
+    <definedName name="Sign_agent_start">Export_Contract!$G$57</definedName>
+    <definedName name="Sign_seller_start">Export_Contract!$C$57</definedName>
+    <definedName name="Адреса_банк_получателя">Export_Contract!$B$41</definedName>
+    <definedName name="Адреса_банк_получателя_адрес">Export_Contract!$B$42</definedName>
+    <definedName name="Адреса_банк_получателя_свифт">Export_Contract!$B$43</definedName>
+    <definedName name="Адреса_подпись">Export_Contract!$B$58</definedName>
+    <definedName name="Адреса_покупатель">Export_Contract!$B$47</definedName>
+    <definedName name="Адреса_покупатель_адрес">Export_Contract!$B$48</definedName>
+    <definedName name="Адреса_покупатель_банк">Export_Contract!$B$50</definedName>
+    <definedName name="Адреса_покупатель_банк_адрес">Export_Contract!$B$53</definedName>
+    <definedName name="Адреса_покупатель_банк_ветвь">Export_Contract!$B$52</definedName>
+    <definedName name="Адреса_покупатель_банк_свифт">Export_Contract!$B$54</definedName>
+    <definedName name="Адреса_покупатель_бенефициар">Export_Contract!$B$55</definedName>
+    <definedName name="Адреса_покупатель_счет">Export_Contract!$B$56</definedName>
+    <definedName name="Адреса_получатель_в_пользу">Export_Contract!$B$44</definedName>
+    <definedName name="Адреса_получатель_счет">Export_Contract!$B$45</definedName>
+    <definedName name="Адреса_продавец">Export_Contract!$B$39</definedName>
+    <definedName name="Адреса_продавец_адрес">Export_Contract!$B$40</definedName>
+    <definedName name="Адреса_сторон_заголовок">Export_Contract!$B$36</definedName>
+    <definedName name="Доставка_дата">Export_Contract!$B$31</definedName>
+    <definedName name="Доставка_заголовок">Export_Contract!$B$28</definedName>
+    <definedName name="Доставка_порт">Export_Contract!$B$32</definedName>
+    <definedName name="Доставка_приемка">Export_Contract!$B$30</definedName>
+    <definedName name="Доставка_транспорт">Export_Contract!$B$21</definedName>
+    <definedName name="Доставка_условия">Export_Contract!$B$29</definedName>
     <definedName name="Инвойс">Invoice!$B$2</definedName>
     <definedName name="Инвойс_Bl_массив">Invoice!$B$23</definedName>
     <definedName name="Инвойс_банк_получателя">Invoice!$B$37</definedName>
@@ -81,10 +81,10 @@
     <definedName name="Контракт">Export_Contract!$B$3</definedName>
     <definedName name="Контракт_дата">Export_Contract!$B$4</definedName>
     <definedName name="Контракт_предмет_заголовки">Export_Contract!$B$18</definedName>
-    <definedName name="Остальное_контракт">Export_Contract!$B$21</definedName>
+    <definedName name="Остальное_контракт">Export_Contract!$B$22</definedName>
     <definedName name="Покупатель">Export_Contract!$B$12</definedName>
     <definedName name="Покупатель_адрес">Export_Contract!$B$13</definedName>
-    <definedName name="Покупатель_заголовок">Export_Contract!$B$45</definedName>
+    <definedName name="Покупатель_заголовок">Export_Contract!$B$46</definedName>
     <definedName name="Покупатель_представитель">Export_Contract!$B$14</definedName>
     <definedName name="Покупатель_представитель_подробно">Export_Contract!$B$15</definedName>
     <definedName name="Покупатель_шапка_заголовок">Export_Contract!$B$11</definedName>
@@ -93,19 +93,19 @@
     <definedName name="Предмет_массив">Export_Contract!$B$19</definedName>
     <definedName name="Продавец">Export_Contract!$B$7</definedName>
     <definedName name="Продавец_адрес">Export_Contract!$B$8</definedName>
-    <definedName name="Продавец_заголовок">Export_Contract!$B$37</definedName>
+    <definedName name="Продавец_заголовок">Export_Contract!$B$38</definedName>
     <definedName name="Продавец_подписант">Export_Contract!$B$10</definedName>
     <definedName name="Продавец_представитель">Export_Contract!$B$9</definedName>
     <definedName name="Продавец_шапка_заголовок">Export_Contract!$B$6</definedName>
-    <definedName name="Прочие_условия_заголовок">Export_Contract!$B$33</definedName>
-    <definedName name="Прочие_условия_описание">Export_Contract!$B$34</definedName>
-    <definedName name="Сертификаты_обязательства">Export_Contract!$B$32</definedName>
+    <definedName name="Прочие_условия_заголовок">Export_Contract!$B$34</definedName>
+    <definedName name="Прочие_условия_описание">Export_Contract!$B$35</definedName>
+    <definedName name="Сертификаты_обязательства">Export_Contract!$B$33</definedName>
     <definedName name="Соглашение">Export_Contract!$B$2</definedName>
-    <definedName name="Соглашение_вступление">Export_Contract!$B$22</definedName>
-    <definedName name="Цена_всего">Export_Contract!$B$26</definedName>
-    <definedName name="Цена_заголовок">Export_Contract!$B$24</definedName>
-    <definedName name="Цена_неком">Export_Contract!$B$25</definedName>
-    <definedName name="Юридикция">Export_Contract!$B$23</definedName>
+    <definedName name="Соглашение_вступление">Export_Contract!$B$23</definedName>
+    <definedName name="Цена_всего">Export_Contract!$B$27</definedName>
+    <definedName name="Цена_заголовок">Export_Contract!$B$25</definedName>
+    <definedName name="Цена_неком">Export_Contract!$B$26</definedName>
+    <definedName name="Юридикция">Export_Contract!$B$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -506,7 +506,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -674,6 +674,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -812,7 +820,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -870,9 +878,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -949,9 +954,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1264,6 +1266,108 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1282,69 +1386,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1357,62 +1398,63 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1777,24 +1819,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AF94"/>
+  <dimension ref="A1:AF95"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="91" zoomScaleNormal="100" zoomScaleSheetLayoutView="91" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="91" zoomScaleNormal="100" zoomScaleSheetLayoutView="91" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="1.06640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="42" customWidth="1"/>
-    <col min="3" max="3" width="23.59765625" style="42" customWidth="1"/>
-    <col min="4" max="4" width="18" style="42" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="42" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="42" customWidth="1"/>
-    <col min="7" max="7" width="21.53125" style="42" customWidth="1"/>
-    <col min="8" max="8" width="12.265625" style="42" customWidth="1"/>
-    <col min="9" max="9" width="15.06640625" style="42" customWidth="1"/>
-    <col min="10" max="10" width="1.06640625" style="42" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="41" customWidth="1"/>
+    <col min="3" max="3" width="23.59765625" style="41" customWidth="1"/>
+    <col min="4" max="4" width="18" style="41" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="41" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="41" customWidth="1"/>
+    <col min="7" max="7" width="21.53125" style="41" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" style="41" customWidth="1"/>
+    <col min="9" max="9" width="15.06640625" style="41" customWidth="1"/>
+    <col min="10" max="10" width="1.06640625" style="41" customWidth="1"/>
     <col min="11" max="11" width="8.796875" style="7"/>
     <col min="12" max="12" width="13" style="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.796875" style="7"/>
@@ -1820,31 +1862,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="2.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="143"/>
     </row>
     <row r="2" spans="2:30" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="205" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="173" t="s">
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="205" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
-      <c r="I2" s="174"/>
-      <c r="J2" s="146"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="206"/>
+      <c r="I2" s="206"/>
+      <c r="J2" s="144"/>
       <c r="L2" s="8"/>
       <c r="N2" s="15"/>
       <c r="AA2" s="15"/>
@@ -1853,18 +1895,18 @@
       <c r="AD2" s="15"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="176" t="s">
+      <c r="B3" s="208" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="178"/>
-      <c r="F3" s="176" t="s">
+      <c r="C3" s="209"/>
+      <c r="D3" s="209"/>
+      <c r="E3" s="210"/>
+      <c r="F3" s="208" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="177"/>
-      <c r="H3" s="177"/>
-      <c r="I3" s="177"/>
+      <c r="G3" s="209"/>
+      <c r="H3" s="209"/>
+      <c r="I3" s="209"/>
       <c r="J3" s="6"/>
       <c r="L3" s="8"/>
       <c r="O3" s="7"/>
@@ -1881,18 +1923,18 @@
       <c r="Z3" s="7"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="176" t="s">
+      <c r="B4" s="208" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="177"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="178"/>
-      <c r="F4" s="176" t="s">
+      <c r="C4" s="209"/>
+      <c r="D4" s="209"/>
+      <c r="E4" s="210"/>
+      <c r="F4" s="208" t="s">
         <v>90</v>
       </c>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="177"/>
+      <c r="G4" s="209"/>
+      <c r="H4" s="209"/>
+      <c r="I4" s="209"/>
       <c r="J4" s="6"/>
       <c r="N4" s="10"/>
       <c r="O4" s="11"/>
@@ -1913,18 +1955,18 @@
       <c r="AD4" s="10"/>
     </row>
     <row r="5" spans="2:30" s="14" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="182" t="s">
+      <c r="B5" s="201" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="183"/>
-      <c r="D5" s="183"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="182" t="s">
+      <c r="C5" s="202"/>
+      <c r="D5" s="202"/>
+      <c r="E5" s="203"/>
+      <c r="F5" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="183"/>
-      <c r="H5" s="183"/>
-      <c r="I5" s="183"/>
+      <c r="G5" s="202"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="202"/>
       <c r="J5" s="13"/>
       <c r="N5" s="15"/>
       <c r="AA5" s="15"/>
@@ -1933,20 +1975,20 @@
       <c r="AD5" s="15"/>
     </row>
     <row r="6" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="163" t="s">
+      <c r="B6" s="161" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="164"/>
-      <c r="D6" s="164"/>
-      <c r="E6" s="165"/>
-      <c r="F6" s="163" t="s">
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="161" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="164"/>
-      <c r="H6" s="164"/>
-      <c r="I6" s="164"/>
-      <c r="J6" s="44"/>
-      <c r="L6" s="45"/>
+      <c r="G6" s="162"/>
+      <c r="H6" s="162"/>
+      <c r="I6" s="162"/>
+      <c r="J6" s="43"/>
+      <c r="L6" s="44"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
@@ -1961,20 +2003,20 @@
       <c r="Z6" s="7"/>
     </row>
     <row r="7" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="163" t="s">
+      <c r="B7" s="161" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="167"/>
-      <c r="F7" s="163" t="s">
+      <c r="C7" s="164"/>
+      <c r="D7" s="164"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="161" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="166"/>
-      <c r="H7" s="166"/>
-      <c r="I7" s="166"/>
-      <c r="J7" s="44"/>
-      <c r="L7" s="45"/>
+      <c r="G7" s="164"/>
+      <c r="H7" s="164"/>
+      <c r="I7" s="164"/>
+      <c r="J7" s="43"/>
+      <c r="L7" s="44"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
@@ -1989,44 +2031,44 @@
       <c r="Z7" s="7"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="185" t="s">
+      <c r="B8" s="191" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="186"/>
-      <c r="D8" s="186"/>
-      <c r="E8" s="187"/>
-      <c r="F8" s="185" t="s">
+      <c r="C8" s="192"/>
+      <c r="D8" s="192"/>
+      <c r="E8" s="204"/>
+      <c r="F8" s="191" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="186"/>
-      <c r="H8" s="186"/>
-      <c r="I8" s="186"/>
+      <c r="G8" s="192"/>
+      <c r="H8" s="192"/>
+      <c r="I8" s="192"/>
       <c r="J8" s="19"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="179" t="s">
+      <c r="B9" s="181" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="180"/>
-      <c r="D9" s="180"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="179" t="s">
+      <c r="C9" s="182"/>
+      <c r="D9" s="182"/>
+      <c r="E9" s="183"/>
+      <c r="F9" s="181" t="s">
         <v>96</v>
       </c>
-      <c r="G9" s="180"/>
-      <c r="H9" s="180"/>
-      <c r="I9" s="181"/>
+      <c r="G9" s="182"/>
+      <c r="H9" s="182"/>
+      <c r="I9" s="183"/>
       <c r="J9" s="19"/>
     </row>
-    <row r="10" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="179"/>
-      <c r="C10" s="180"/>
-      <c r="D10" s="180"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="179"/>
-      <c r="G10" s="180"/>
-      <c r="H10" s="180"/>
-      <c r="I10" s="181"/>
+    <row r="10" spans="2:30" ht="8.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="181"/>
+      <c r="C10" s="182"/>
+      <c r="D10" s="182"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="182"/>
+      <c r="H10" s="182"/>
+      <c r="I10" s="183"/>
       <c r="J10" s="19"/>
       <c r="N10" s="15"/>
       <c r="O10" s="7"/>
@@ -2047,19 +2089,19 @@
       <c r="AD10" s="15"/>
     </row>
     <row r="11" spans="2:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="160" t="s">
+      <c r="B11" s="158" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="161"/>
-      <c r="D11" s="161"/>
-      <c r="E11" s="162"/>
-      <c r="F11" s="160" t="s">
+      <c r="C11" s="159"/>
+      <c r="D11" s="159"/>
+      <c r="E11" s="160"/>
+      <c r="F11" s="158" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="161"/>
-      <c r="H11" s="161"/>
-      <c r="I11" s="161"/>
-      <c r="J11" s="44"/>
+      <c r="G11" s="159"/>
+      <c r="H11" s="159"/>
+      <c r="I11" s="159"/>
+      <c r="J11" s="43"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
@@ -2074,19 +2116,19 @@
       <c r="Z11" s="7"/>
     </row>
     <row r="12" spans="2:30" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="163" t="s">
+      <c r="B12" s="161" t="s">
         <v>97</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="159"/>
-      <c r="F12" s="163" t="s">
+      <c r="E12" s="157"/>
+      <c r="F12" s="161" t="s">
         <v>97</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="166"/>
-      <c r="I12" s="166"/>
-      <c r="J12" s="44"/>
+      <c r="H12" s="164"/>
+      <c r="I12" s="164"/>
+      <c r="J12" s="43"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
@@ -2101,18 +2143,18 @@
       <c r="Z12" s="7"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="179" t="s">
+      <c r="B13" s="181" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="180"/>
-      <c r="D13" s="180"/>
-      <c r="E13" s="181"/>
-      <c r="F13" s="179" t="s">
+      <c r="C13" s="182"/>
+      <c r="D13" s="182"/>
+      <c r="E13" s="183"/>
+      <c r="F13" s="181" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="180"/>
-      <c r="H13" s="180"/>
-      <c r="I13" s="180"/>
+      <c r="G13" s="182"/>
+      <c r="H13" s="182"/>
+      <c r="I13" s="182"/>
       <c r="J13" s="19"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
@@ -2130,18 +2172,18 @@
       <c r="AA13" s="7"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="179" t="s">
+      <c r="B14" s="181" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="180"/>
-      <c r="D14" s="180"/>
-      <c r="E14" s="181"/>
-      <c r="F14" s="179" t="s">
+      <c r="C14" s="182"/>
+      <c r="D14" s="182"/>
+      <c r="E14" s="183"/>
+      <c r="F14" s="181" t="s">
         <v>100</v>
       </c>
-      <c r="G14" s="180"/>
-      <c r="H14" s="180"/>
-      <c r="I14" s="180"/>
+      <c r="G14" s="182"/>
+      <c r="H14" s="182"/>
+      <c r="I14" s="182"/>
       <c r="J14" s="19"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
@@ -2159,18 +2201,18 @@
       <c r="AA14" s="7"/>
     </row>
     <row r="15" spans="2:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="179" t="s">
+      <c r="B15" s="181" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="180"/>
-      <c r="D15" s="180"/>
-      <c r="E15" s="181"/>
-      <c r="F15" s="179" t="s">
+      <c r="C15" s="182"/>
+      <c r="D15" s="182"/>
+      <c r="E15" s="183"/>
+      <c r="F15" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="180"/>
-      <c r="H15" s="180"/>
-      <c r="I15" s="180"/>
+      <c r="G15" s="182"/>
+      <c r="H15" s="182"/>
+      <c r="I15" s="182"/>
       <c r="J15" s="19"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
@@ -2188,18 +2230,18 @@
       <c r="AA15" s="7"/>
     </row>
     <row r="16" spans="2:30" ht="1.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="163" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="164"/>
-      <c r="D16" s="164"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="163" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="164"/>
-      <c r="H16" s="164"/>
-      <c r="I16" s="165"/>
+      <c r="B16" s="161" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="162"/>
+      <c r="D16" s="162"/>
+      <c r="E16" s="156"/>
+      <c r="F16" s="161" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="162"/>
+      <c r="H16" s="162"/>
+      <c r="I16" s="163"/>
       <c r="J16" s="19"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
@@ -2217,18 +2259,18 @@
       <c r="AA16" s="7"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="188" t="s">
+      <c r="B17" s="193" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="189"/>
-      <c r="D17" s="189"/>
-      <c r="E17" s="190"/>
-      <c r="F17" s="188" t="s">
+      <c r="C17" s="194"/>
+      <c r="D17" s="194"/>
+      <c r="E17" s="195"/>
+      <c r="F17" s="193" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="189"/>
-      <c r="H17" s="189"/>
-      <c r="I17" s="189"/>
+      <c r="G17" s="194"/>
+      <c r="H17" s="194"/>
+      <c r="I17" s="194"/>
       <c r="J17" s="19"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
@@ -2246,18 +2288,18 @@
       <c r="AA17" s="7"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="191" t="s">
+      <c r="B18" s="196" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="192"/>
+      <c r="C18" s="197"/>
       <c r="D18" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="192" t="s">
+      <c r="E18" s="197" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="192"/>
-      <c r="G18" s="192"/>
+      <c r="F18" s="197"/>
+      <c r="G18" s="197"/>
       <c r="H18" s="20" t="s">
         <v>35</v>
       </c>
@@ -2281,22 +2323,22 @@
       <c r="AA18" s="7"/>
     </row>
     <row r="19" spans="2:30" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="193" t="s">
+      <c r="B19" s="198" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="194"/>
+      <c r="C19" s="199"/>
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="195" t="s">
+      <c r="E19" s="200" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="195"/>
-      <c r="G19" s="195"/>
-      <c r="H19" s="1" t="s">
+      <c r="F19" s="223"/>
+      <c r="G19" s="223"/>
+      <c r="H19" s="221" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="222" t="s">
         <v>13</v>
       </c>
       <c r="J19" s="2"/>
@@ -2318,19 +2360,15 @@
       <c r="AC19" s="7"/>
       <c r="AD19" s="7"/>
     </row>
-    <row r="20" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="152" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="168"/>
-      <c r="D20" s="168"/>
-      <c r="E20" s="169"/>
-      <c r="F20" s="219" t="s">
-        <v>17</v>
-      </c>
+    <row r="20" spans="2:30" ht="3.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="217"/>
+      <c r="C20" s="218"/>
+      <c r="D20" s="218"/>
+      <c r="E20" s="219"/>
+      <c r="F20" s="227"/>
       <c r="G20" s="220"/>
       <c r="H20" s="221"/>
-      <c r="I20" s="222"/>
+      <c r="I20" s="228"/>
       <c r="J20" s="2"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
@@ -2351,19 +2389,19 @@
       <c r="AD20" s="7"/>
     </row>
     <row r="21" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="204" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="205"/>
-      <c r="D21" s="205"/>
-      <c r="E21" s="206"/>
-      <c r="F21" s="204" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="206"/>
-      <c r="H21" s="205"/>
-      <c r="I21" s="207"/>
-      <c r="J21" s="170"/>
+      <c r="B21" s="150" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="166"/>
+      <c r="D21" s="166"/>
+      <c r="E21" s="167"/>
+      <c r="F21" s="150" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="224"/>
+      <c r="H21" s="225"/>
+      <c r="I21" s="229"/>
+      <c r="J21" s="2"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
@@ -2383,19 +2421,19 @@
       <c r="AD21" s="7"/>
     </row>
     <row r="22" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="204" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="206"/>
-      <c r="D22" s="206"/>
-      <c r="E22" s="206"/>
-      <c r="F22" s="204" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="206"/>
-      <c r="H22" s="205"/>
-      <c r="I22" s="207"/>
-      <c r="J22" s="170"/>
+      <c r="B22" s="226" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="230"/>
+      <c r="D22" s="230"/>
+      <c r="E22" s="231"/>
+      <c r="F22" s="226" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="231"/>
+      <c r="H22" s="230"/>
+      <c r="I22" s="232"/>
+      <c r="J22" s="168"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
@@ -2415,19 +2453,19 @@
       <c r="AD22" s="7"/>
     </row>
     <row r="23" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="204" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="206"/>
-      <c r="D23" s="206"/>
-      <c r="E23" s="206"/>
-      <c r="F23" s="204" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="206"/>
-      <c r="H23" s="205"/>
-      <c r="I23" s="207"/>
-      <c r="J23" s="170"/>
+      <c r="B23" s="171" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="173"/>
+      <c r="D23" s="173"/>
+      <c r="E23" s="173"/>
+      <c r="F23" s="171" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="173"/>
+      <c r="H23" s="172"/>
+      <c r="I23" s="174"/>
+      <c r="J23" s="168"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
@@ -2447,19 +2485,19 @@
       <c r="AD23" s="7"/>
     </row>
     <row r="24" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="208" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="209"/>
-      <c r="D24" s="209"/>
-      <c r="E24" s="206"/>
-      <c r="F24" s="210" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="211"/>
-      <c r="H24" s="212"/>
-      <c r="I24" s="213"/>
-      <c r="J24" s="170"/>
+      <c r="B24" s="171" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="173"/>
+      <c r="D24" s="173"/>
+      <c r="E24" s="173"/>
+      <c r="F24" s="171" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="173"/>
+      <c r="H24" s="172"/>
+      <c r="I24" s="174"/>
+      <c r="J24" s="168"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
@@ -2479,19 +2517,19 @@
       <c r="AD24" s="7"/>
     </row>
     <row r="25" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="204" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="209"/>
-      <c r="D25" s="209"/>
-      <c r="E25" s="206"/>
-      <c r="F25" s="204" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="211"/>
-      <c r="H25" s="212"/>
-      <c r="I25" s="213"/>
-      <c r="J25" s="170"/>
+      <c r="B25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="158" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="215"/>
+      <c r="I25" s="216"/>
+      <c r="J25" s="168"/>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
@@ -2510,66 +2548,66 @@
       <c r="AC25" s="7"/>
       <c r="AD25" s="7"/>
     </row>
-    <row r="26" spans="2:30" s="28" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="156"/>
-    </row>
-    <row r="27" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="209"/>
-      <c r="D27" s="209"/>
+    <row r="26" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="171" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="175"/>
+      <c r="D26" s="175"/>
+      <c r="E26" s="173"/>
+      <c r="F26" s="171" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="176"/>
+      <c r="H26" s="177"/>
+      <c r="I26" s="178"/>
+      <c r="J26" s="168"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7"/>
+      <c r="AB26" s="7"/>
+      <c r="AC26" s="7"/>
+      <c r="AD26" s="7"/>
+    </row>
+    <row r="27" spans="2:30" s="27" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="210" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="211"/>
+      <c r="F27" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="17"/>
       <c r="H27" s="17"/>
       <c r="I27" s="18"/>
-      <c r="J27" s="13"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
-      <c r="V27" s="7"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="7"/>
-      <c r="Y27" s="7"/>
-      <c r="Z27" s="7"/>
-      <c r="AA27" s="7"/>
-      <c r="AB27" s="7"/>
-      <c r="AC27" s="7"/>
-      <c r="AD27" s="7"/>
+      <c r="J27" s="154"/>
     </row>
     <row r="28" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="179" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="180"/>
-      <c r="D28" s="180"/>
-      <c r="E28" s="180"/>
-      <c r="F28" s="179" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="180"/>
-      <c r="H28" s="180"/>
-      <c r="I28" s="181"/>
+      <c r="B28" s="169" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="158" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="155"/>
       <c r="J28" s="13"/>
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
@@ -2590,18 +2628,18 @@
       <c r="AD28" s="7"/>
     </row>
     <row r="29" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="18"/>
+      <c r="B29" s="181" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="182"/>
+      <c r="D29" s="182"/>
+      <c r="E29" s="182"/>
+      <c r="F29" s="181" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="182"/>
+      <c r="H29" s="182"/>
+      <c r="I29" s="183"/>
       <c r="J29" s="13"/>
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
@@ -2653,487 +2691,508 @@
       <c r="AC30" s="7"/>
       <c r="AD30" s="7"/>
     </row>
-    <row r="31" spans="2:30" s="28" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="214" t="s">
+    <row r="31" spans="2:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="13"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7"/>
+      <c r="AC31" s="7"/>
+      <c r="AD31" s="7"/>
+    </row>
+    <row r="32" spans="2:30" s="27" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="188" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="215"/>
-      <c r="D31" s="215"/>
-      <c r="E31" s="215"/>
-      <c r="F31" s="214" t="s">
+      <c r="C32" s="189"/>
+      <c r="D32" s="189"/>
+      <c r="E32" s="189"/>
+      <c r="F32" s="188" t="s">
         <v>84</v>
       </c>
-      <c r="G31" s="215"/>
-      <c r="H31" s="215"/>
-      <c r="I31" s="216"/>
-      <c r="J31" s="156"/>
-    </row>
-    <row r="32" spans="2:30" s="28" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="185" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="186"/>
-      <c r="D32" s="186"/>
-      <c r="E32" s="186"/>
-      <c r="F32" s="179" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="180"/>
-      <c r="H32" s="180"/>
-      <c r="I32" s="181"/>
-      <c r="J32" s="156"/>
-    </row>
-    <row r="33" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="211"/>
-      <c r="D33" s="211"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="210" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="217"/>
-      <c r="H33" s="217"/>
-      <c r="I33" s="218"/>
-      <c r="J33" s="13"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
-      <c r="V33" s="7"/>
-      <c r="W33" s="7"/>
-      <c r="X33" s="7"/>
-      <c r="Y33" s="7"/>
-      <c r="Z33" s="7"/>
-      <c r="AA33" s="7"/>
-      <c r="AB33" s="7"/>
-      <c r="AC33" s="7"/>
-      <c r="AD33" s="7"/>
+      <c r="G32" s="189"/>
+      <c r="H32" s="189"/>
+      <c r="I32" s="190"/>
+      <c r="J32" s="154"/>
+    </row>
+    <row r="33" spans="1:30" s="27" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="191" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="192"/>
+      <c r="D33" s="192"/>
+      <c r="E33" s="192"/>
+      <c r="F33" s="181" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="182"/>
+      <c r="H33" s="182"/>
+      <c r="I33" s="183"/>
+      <c r="J33" s="154"/>
     </row>
     <row r="34" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="179" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="180"/>
-      <c r="D34" s="180"/>
-      <c r="E34" s="180"/>
-      <c r="F34" s="179" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="180"/>
-      <c r="H34" s="180"/>
-      <c r="I34" s="181"/>
-      <c r="J34" s="6"/>
+      <c r="B34" s="169" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="158" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="159"/>
+      <c r="H34" s="179"/>
+      <c r="I34" s="180"/>
+      <c r="J34" s="13"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="7"/>
     </row>
     <row r="35" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="181" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="182"/>
+      <c r="D35" s="182"/>
+      <c r="E35" s="182"/>
+      <c r="F35" s="181" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="182"/>
+      <c r="H35" s="182"/>
+      <c r="I35" s="183"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="233" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="159"/>
-      <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="1:30" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="172"/>
-      <c r="B36" s="171"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="171"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="43"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="234" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="157"/>
       <c r="J36" s="6"/>
     </row>
-    <row r="37" spans="1:30" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="160" t="s">
-        <v>22</v>
-      </c>
+    <row r="37" spans="1:30" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="170"/>
+      <c r="B37" s="169"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="160" t="s">
-        <v>27</v>
-      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="169"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="43"/>
+      <c r="I37" s="42"/>
       <c r="J37" s="6"/>
     </row>
-    <row r="38" spans="1:30" s="28" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="196" t="s">
+    <row r="38" spans="1:30" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="158" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="158" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="1:30" s="27" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="184" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="197"/>
-      <c r="D38" s="197"/>
-      <c r="E38" s="197"/>
-      <c r="F38" s="196" t="s">
+      <c r="C39" s="185"/>
+      <c r="D39" s="185"/>
+      <c r="E39" s="185"/>
+      <c r="F39" s="184" t="s">
         <v>101</v>
       </c>
-      <c r="G38" s="197"/>
-      <c r="H38" s="197"/>
-      <c r="I38" s="198"/>
-      <c r="J38" s="27"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="29"/>
-      <c r="AB38" s="29"/>
-      <c r="AC38" s="29"/>
-      <c r="AD38" s="29"/>
-    </row>
-    <row r="39" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="179" t="s">
+      <c r="G39" s="185"/>
+      <c r="H39" s="185"/>
+      <c r="I39" s="186"/>
+      <c r="J39" s="26"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="28"/>
+      <c r="P39" s="28"/>
+      <c r="Q39" s="28"/>
+      <c r="R39" s="28"/>
+      <c r="S39" s="28"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="28"/>
+      <c r="V39" s="28"/>
+      <c r="W39" s="28"/>
+      <c r="X39" s="28"/>
+      <c r="Y39" s="28"/>
+      <c r="Z39" s="28"/>
+      <c r="AA39" s="28"/>
+      <c r="AB39" s="28"/>
+      <c r="AC39" s="28"/>
+      <c r="AD39" s="28"/>
+    </row>
+    <row r="40" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="181" t="s">
         <v>98</v>
       </c>
-      <c r="C39" s="180"/>
-      <c r="D39" s="180"/>
-      <c r="E39" s="180"/>
-      <c r="F39" s="179" t="s">
+      <c r="C40" s="182"/>
+      <c r="D40" s="182"/>
+      <c r="E40" s="182"/>
+      <c r="F40" s="181" t="s">
         <v>102</v>
       </c>
-      <c r="G39" s="180"/>
-      <c r="H39" s="180"/>
-      <c r="I39" s="181"/>
-      <c r="J39" s="16"/>
-    </row>
-    <row r="40" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="179" t="s">
+      <c r="G40" s="182"/>
+      <c r="H40" s="182"/>
+      <c r="I40" s="183"/>
+      <c r="J40" s="16"/>
+    </row>
+    <row r="41" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="181" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="180"/>
-      <c r="D40" s="180"/>
-      <c r="E40" s="181"/>
-      <c r="F40" s="179" t="s">
+      <c r="C41" s="182"/>
+      <c r="D41" s="182"/>
+      <c r="E41" s="183"/>
+      <c r="F41" s="181" t="s">
         <v>103</v>
       </c>
-      <c r="G40" s="180"/>
-      <c r="H40" s="180"/>
-      <c r="I40" s="180"/>
-      <c r="J40" s="16"/>
-    </row>
-    <row r="41" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="179" t="s">
+      <c r="G41" s="182"/>
+      <c r="H41" s="182"/>
+      <c r="I41" s="182"/>
+      <c r="J41" s="16"/>
+    </row>
+    <row r="42" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="181" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="180"/>
-      <c r="D41" s="180"/>
-      <c r="E41" s="181"/>
-      <c r="F41" s="179" t="s">
+      <c r="C42" s="182"/>
+      <c r="D42" s="182"/>
+      <c r="E42" s="183"/>
+      <c r="F42" s="181" t="s">
         <v>106</v>
       </c>
-      <c r="G41" s="180"/>
-      <c r="H41" s="180"/>
-      <c r="I41" s="180"/>
-      <c r="J41" s="16"/>
-    </row>
-    <row r="42" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="179" t="s">
+      <c r="G42" s="182"/>
+      <c r="H42" s="182"/>
+      <c r="I42" s="182"/>
+      <c r="J42" s="16"/>
+    </row>
+    <row r="43" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B43" s="181" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="180"/>
-      <c r="D42" s="180"/>
-      <c r="E42" s="181"/>
-      <c r="F42" s="179" t="s">
+      <c r="C43" s="182"/>
+      <c r="D43" s="182"/>
+      <c r="E43" s="183"/>
+      <c r="F43" s="181" t="s">
         <v>107</v>
       </c>
-      <c r="G42" s="180"/>
-      <c r="H42" s="180"/>
-      <c r="I42" s="180"/>
-      <c r="J42" s="16"/>
-    </row>
-    <row r="43" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="179" t="s">
+      <c r="G43" s="182"/>
+      <c r="H43" s="182"/>
+      <c r="I43" s="182"/>
+      <c r="J43" s="16"/>
+    </row>
+    <row r="44" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B44" s="181" t="s">
         <v>108</v>
       </c>
-      <c r="C43" s="180"/>
-      <c r="D43" s="180"/>
-      <c r="E43" s="181"/>
-      <c r="F43" s="179" t="s">
+      <c r="C44" s="182"/>
+      <c r="D44" s="182"/>
+      <c r="E44" s="183"/>
+      <c r="F44" s="181" t="s">
         <v>109</v>
       </c>
-      <c r="G43" s="180"/>
-      <c r="H43" s="180"/>
-      <c r="I43" s="180"/>
-      <c r="J43" s="16"/>
-    </row>
-    <row r="44" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="179" t="s">
+      <c r="G44" s="182"/>
+      <c r="H44" s="182"/>
+      <c r="I44" s="182"/>
+      <c r="J44" s="16"/>
+    </row>
+    <row r="45" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="181" t="s">
         <v>110</v>
       </c>
-      <c r="C44" s="180"/>
-      <c r="D44" s="180"/>
-      <c r="E44" s="181"/>
-      <c r="F44" s="179" t="s">
+      <c r="C45" s="182"/>
+      <c r="D45" s="182"/>
+      <c r="E45" s="183"/>
+      <c r="F45" s="181" t="s">
         <v>111</v>
       </c>
-      <c r="G44" s="180"/>
-      <c r="H44" s="180"/>
-      <c r="I44" s="180"/>
-      <c r="J44" s="16"/>
-    </row>
-    <row r="45" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="171" t="s">
+      <c r="G45" s="182"/>
+      <c r="H45" s="182"/>
+      <c r="I45" s="182"/>
+      <c r="J45" s="16"/>
+    </row>
+    <row r="46" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="169" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="157"/>
-      <c r="F45" s="171" t="s">
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="155"/>
+      <c r="F46" s="169" t="s">
         <v>29</v>
       </c>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="16"/>
-    </row>
-    <row r="46" spans="1:30" s="28" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="196" t="s">
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="16"/>
+    </row>
+    <row r="47" spans="1:30" s="27" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B47" s="184" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="197"/>
-      <c r="D46" s="197"/>
-      <c r="E46" s="198"/>
-      <c r="F46" s="196" t="s">
+      <c r="C47" s="185"/>
+      <c r="D47" s="185"/>
+      <c r="E47" s="186"/>
+      <c r="F47" s="184" t="s">
         <v>97</v>
       </c>
-      <c r="G46" s="199"/>
-      <c r="H46" s="199"/>
-      <c r="I46" s="199"/>
-      <c r="J46" s="27"/>
-      <c r="N46" s="29"/>
-      <c r="O46" s="29"/>
-      <c r="P46" s="29"/>
-      <c r="Q46" s="29"/>
-      <c r="R46" s="29"/>
-      <c r="S46" s="29"/>
-      <c r="T46" s="29"/>
-      <c r="U46" s="29"/>
-      <c r="V46" s="29"/>
-      <c r="W46" s="29"/>
-      <c r="X46" s="29"/>
-      <c r="Y46" s="29"/>
-      <c r="Z46" s="29"/>
-      <c r="AA46" s="29"/>
-      <c r="AB46" s="29"/>
-      <c r="AC46" s="29"/>
-      <c r="AD46" s="29"/>
-    </row>
-    <row r="47" spans="1:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="179" t="s">
+      <c r="G47" s="187"/>
+      <c r="H47" s="187"/>
+      <c r="I47" s="187"/>
+      <c r="J47" s="26"/>
+      <c r="N47" s="28"/>
+      <c r="O47" s="28"/>
+      <c r="P47" s="28"/>
+      <c r="Q47" s="28"/>
+      <c r="R47" s="28"/>
+      <c r="S47" s="28"/>
+      <c r="T47" s="28"/>
+      <c r="U47" s="28"/>
+      <c r="V47" s="28"/>
+      <c r="W47" s="28"/>
+      <c r="X47" s="28"/>
+      <c r="Y47" s="28"/>
+      <c r="Z47" s="28"/>
+      <c r="AA47" s="28"/>
+      <c r="AB47" s="28"/>
+      <c r="AC47" s="28"/>
+      <c r="AD47" s="28"/>
+    </row>
+    <row r="48" spans="1:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B48" s="181" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="180"/>
-      <c r="D47" s="180"/>
-      <c r="E47" s="181"/>
-      <c r="F47" s="179" t="s">
+      <c r="C48" s="182"/>
+      <c r="D48" s="182"/>
+      <c r="E48" s="183"/>
+      <c r="F48" s="181" t="s">
         <v>112</v>
       </c>
-      <c r="G47" s="180"/>
-      <c r="H47" s="180"/>
-      <c r="I47" s="180"/>
-      <c r="J47" s="16"/>
-    </row>
-    <row r="48" spans="1:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="16"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
+      <c r="G48" s="182"/>
+      <c r="H48" s="182"/>
+      <c r="I48" s="182"/>
       <c r="J48" s="16"/>
     </row>
-    <row r="49" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="23" t="s">
+    <row r="49" spans="2:10" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="16"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="16"/>
+    </row>
+    <row r="50" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="23" t="s">
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="G49" s="24"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="16"/>
-    </row>
-    <row r="50" spans="2:10" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="32"/>
-      <c r="C50" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" s="26"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
       <c r="J50" s="16"/>
     </row>
-    <row r="51" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="23" t="s">
+    <row r="51" spans="2:10" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="31"/>
+      <c r="C51" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="25"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="16"/>
+    </row>
+    <row r="52" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="23" t="s">
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="G51" s="31"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="31"/>
-      <c r="J51" s="16"/>
-    </row>
-    <row r="52" spans="2:10" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="179" t="s">
+      <c r="G52" s="30"/>
+      <c r="H52" s="30"/>
+      <c r="I52" s="30"/>
+      <c r="J52" s="16"/>
+    </row>
+    <row r="53" spans="2:10" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="181" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="180"/>
-      <c r="D52" s="180"/>
-      <c r="E52" s="181"/>
-      <c r="F52" s="179" t="s">
+      <c r="C53" s="182"/>
+      <c r="D53" s="182"/>
+      <c r="E53" s="183"/>
+      <c r="F53" s="181" t="s">
         <v>105</v>
       </c>
-      <c r="G52" s="180"/>
-      <c r="H52" s="180"/>
-      <c r="I52" s="181"/>
-      <c r="J52" s="16"/>
-    </row>
-    <row r="53" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="23" t="s">
+      <c r="G53" s="182"/>
+      <c r="H53" s="182"/>
+      <c r="I53" s="183"/>
+      <c r="J53" s="16"/>
+    </row>
+    <row r="54" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="24" t="s">
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="G53" s="31"/>
-      <c r="H53" s="31"/>
-      <c r="I53" s="31"/>
-      <c r="J53" s="16"/>
-    </row>
-    <row r="54" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="23" t="s">
+      <c r="G54" s="30"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="30"/>
+      <c r="J54" s="16"/>
+    </row>
+    <row r="55" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B55" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="24" t="s">
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
-      <c r="J54" s="16"/>
-    </row>
-    <row r="55" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B55" s="23" t="s">
+      <c r="G55" s="30"/>
+      <c r="H55" s="30"/>
+      <c r="I55" s="30"/>
+      <c r="J55" s="16"/>
+    </row>
+    <row r="56" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B56" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="24" t="s">
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24"/>
-      <c r="J55" s="16"/>
-    </row>
-    <row r="56" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B56" s="16"/>
-      <c r="C56" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="26"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H56" s="26"/>
-      <c r="I56" s="26"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
       <c r="J56" s="16"/>
     </row>
-    <row r="57" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="33" t="s">
+    <row r="57" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B57" s="16"/>
+      <c r="C57" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="25"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" s="25"/>
+      <c r="I57" s="25"/>
+      <c r="J57" s="16"/>
+    </row>
+    <row r="58" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B58" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="34"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="34" t="s">
+      <c r="C58" s="33"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="G57" s="34"/>
-      <c r="H57" s="34"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="12"/>
-    </row>
-    <row r="58" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="36"/>
-      <c r="C58" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" s="38"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="H58" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="I58" s="39"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="34"/>
       <c r="J58" s="12"/>
     </row>
-    <row r="59" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B59" s="12"/>
-      <c r="C59" s="41"/>
-      <c r="D59" s="41"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
+    <row r="59" spans="2:10" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B59" s="35"/>
+      <c r="C59" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="37"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="I59" s="38"/>
       <c r="J59" s="12"/>
     </row>
-    <row r="60" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:10" ht="7.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B60" s="12"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="41"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
@@ -3143,8 +3202,8 @@
     </row>
     <row r="61" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B61" s="12"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="41"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
@@ -3154,8 +3213,8 @@
     </row>
     <row r="62" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B62" s="12"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="41"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
@@ -3165,8 +3224,8 @@
     </row>
     <row r="63" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B63" s="12"/>
-      <c r="C63" s="41"/>
-      <c r="D63" s="41"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="40"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
@@ -3176,8 +3235,8 @@
     </row>
     <row r="64" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B64" s="12"/>
-      <c r="C64" s="41"/>
-      <c r="D64" s="41"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
@@ -3187,8 +3246,8 @@
     </row>
     <row r="65" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B65" s="12"/>
-      <c r="C65" s="41"/>
-      <c r="D65" s="41"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="40"/>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
@@ -3198,8 +3257,8 @@
     </row>
     <row r="66" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B66" s="12"/>
-      <c r="C66" s="41"/>
-      <c r="D66" s="41"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
       <c r="E66" s="12"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
@@ -3209,8 +3268,8 @@
     </row>
     <row r="67" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B67" s="12"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="41"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="40"/>
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
       <c r="G67" s="12"/>
@@ -3220,8 +3279,8 @@
     </row>
     <row r="68" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B68" s="12"/>
-      <c r="C68" s="41"/>
-      <c r="D68" s="41"/>
+      <c r="C68" s="40"/>
+      <c r="D68" s="40"/>
       <c r="E68" s="12"/>
       <c r="F68" s="12"/>
       <c r="G68" s="12"/>
@@ -3229,79 +3288,90 @@
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
     </row>
-    <row r="69" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="69" spans="2:10" ht="7.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B69" s="12"/>
+      <c r="C69" s="40"/>
+      <c r="D69" s="40"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+    </row>
     <row r="70" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="71" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="72" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="73" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="74" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="82" spans="6:7" x14ac:dyDescent="0.45">
-      <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
-    </row>
-    <row r="87" spans="6:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="94" spans="6:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="75" spans="2:10" ht="3.4" hidden="1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="83" spans="6:7" x14ac:dyDescent="0.45">
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+    </row>
+    <row r="88" spans="6:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="95" spans="6:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="F9:I10"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="F9:I10"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="F45:I45"/>
   </mergeCells>
-  <conditionalFormatting sqref="D19:E23 J19:J23 E24:E25 B25">
+  <conditionalFormatting sqref="D19:E24 J19:J24 E25:E26 B26">
     <cfRule type="notContainsBlanks" dxfId="3" priority="2">
       <formula>LEN(TRIM(B19))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H19:H23 I24:J25">
+  <conditionalFormatting sqref="H19:H24 I25:J26">
     <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(H19))&gt;0</formula>
     </cfRule>
@@ -3357,447 +3427,447 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="46"/>
-      <c r="G1" s="144" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="48"/>
+      <c r="A1" s="45"/>
+      <c r="G1" s="142" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="47"/>
     </row>
     <row r="2" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="78"/>
-      <c r="B2" s="106" t="s">
+      <c r="A2" s="76"/>
+      <c r="B2" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="109" t="s">
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
-      <c r="N2" s="48"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="47"/>
     </row>
     <row r="3" spans="1:14" ht="33.4" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="78"/>
-      <c r="B3" s="107" t="s">
+      <c r="A3" s="76"/>
+      <c r="B3" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="110" t="s">
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="48"/>
-    </row>
-    <row r="4" spans="1:14" s="75" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="77"/>
-      <c r="B4" s="107" t="s">
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
+      <c r="N3" s="47"/>
+    </row>
+    <row r="4" spans="1:14" s="73" customFormat="1" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="75"/>
+      <c r="B4" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="110" t="s">
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="107"/>
-      <c r="J4" s="107"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="107"/>
-      <c r="M4" s="107"/>
-      <c r="N4" s="73"/>
-    </row>
-    <row r="5" spans="1:14" s="75" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="76"/>
-      <c r="B5" s="107" t="s">
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
+      <c r="N4" s="71"/>
+    </row>
+    <row r="5" spans="1:14" s="73" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="74"/>
+      <c r="B5" s="105" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="110" t="s">
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="107"/>
-      <c r="M5" s="107"/>
-      <c r="N5" s="73"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="105"/>
+      <c r="N5" s="71"/>
     </row>
     <row r="6" spans="1:14" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="46"/>
-      <c r="B6" s="97" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97"/>
-      <c r="H6" s="84" t="s">
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
-      <c r="L6" s="86"/>
-      <c r="M6" s="86"/>
-      <c r="N6" s="48"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="46"/>
-      <c r="B7" s="100" t="s">
+      <c r="A7" s="45"/>
+      <c r="B7" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="87" t="s">
+      <c r="C7" s="109"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="88"/>
-      <c r="L7" s="86"/>
-      <c r="M7" s="86"/>
-      <c r="N7" s="48"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="84"/>
+      <c r="M7" s="84"/>
+      <c r="N7" s="47"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="46"/>
-      <c r="B8" s="112" t="s">
+      <c r="A8" s="45"/>
+      <c r="B8" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="89" t="s">
+      <c r="C8" s="110"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="86"/>
-      <c r="M8" s="86"/>
-      <c r="N8" s="48"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="84"/>
+      <c r="M8" s="84"/>
+      <c r="N8" s="47"/>
     </row>
     <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="46"/>
-      <c r="B9" s="113" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="111" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="113"/>
-      <c r="D9" s="113"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="113"/>
-      <c r="G9" s="113"/>
-      <c r="H9" s="91" t="s">
+      <c r="C9" s="111"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="48"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="84"/>
+      <c r="N9" s="47"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="46"/>
-      <c r="B10" s="100" t="s">
+      <c r="A10" s="45"/>
+      <c r="B10" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="100"/>
-      <c r="F10" s="100"/>
-      <c r="G10" s="100"/>
-      <c r="H10" s="87" t="s">
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="48"/>
+      <c r="I10" s="84"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="84"/>
+      <c r="N10" s="47"/>
     </row>
     <row r="11" spans="1:14" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="46"/>
-      <c r="B11" s="90" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="142" t="s">
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="140" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="90"/>
-      <c r="J11" s="90"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="48"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="88"/>
+      <c r="M11" s="88"/>
+      <c r="N11" s="47"/>
     </row>
     <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="46"/>
-      <c r="B12" s="113" t="s">
+      <c r="A12" s="45"/>
+      <c r="B12" s="111" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="113"/>
-      <c r="D12" s="113"/>
-      <c r="E12" s="113"/>
-      <c r="F12" s="113"/>
-      <c r="G12" s="113"/>
-      <c r="H12" s="84" t="s">
+      <c r="C12" s="111"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="85"/>
-      <c r="J12" s="85"/>
-      <c r="K12" s="85"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="86"/>
-      <c r="N12" s="48"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="84"/>
+      <c r="M12" s="84"/>
+      <c r="N12" s="47"/>
     </row>
     <row r="13" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="46"/>
-      <c r="B13" s="100" t="s">
+      <c r="A13" s="45"/>
+      <c r="B13" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="87" t="s">
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="48"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="84"/>
+      <c r="M13" s="84"/>
+      <c r="N13" s="47"/>
     </row>
     <row r="14" spans="1:14" ht="44.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="46"/>
-      <c r="B14" s="153" t="s">
+      <c r="A14" s="45"/>
+      <c r="B14" s="151" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="154"/>
-      <c r="D14" s="154"/>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="142" t="s">
+      <c r="C14" s="152"/>
+      <c r="D14" s="152"/>
+      <c r="E14" s="152"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="140" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
-      <c r="K14" s="90"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="48"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="47"/>
     </row>
     <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="74"/>
-      <c r="B15" s="202" t="s">
+      <c r="A15" s="72"/>
+      <c r="B15" s="213" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="203"/>
-      <c r="D15" s="92" t="s">
+      <c r="C15" s="214"/>
+      <c r="D15" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="92"/>
-      <c r="F15" s="92" t="s">
+      <c r="E15" s="90"/>
+      <c r="F15" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="92"/>
-      <c r="H15" s="93" t="s">
+      <c r="G15" s="90"/>
+      <c r="H15" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="92"/>
-      <c r="J15" s="114" t="s">
+      <c r="I15" s="90"/>
+      <c r="J15" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="K15" s="114"/>
-      <c r="L15" s="138" t="s">
+      <c r="K15" s="112"/>
+      <c r="L15" s="136" t="s">
         <v>61</v>
       </c>
-      <c r="M15" s="138"/>
-      <c r="N15" s="48"/>
+      <c r="M15" s="136"/>
+      <c r="N15" s="47"/>
     </row>
     <row r="16" spans="1:14" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="46"/>
-      <c r="B16" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="94"/>
-      <c r="D16" s="95" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="95"/>
-      <c r="F16" s="131" t="s">
+      <c r="A16" s="45"/>
+      <c r="B16" s="92" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="92"/>
+      <c r="D16" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="93"/>
+      <c r="F16" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="95"/>
-      <c r="H16" s="155" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="95"/>
-      <c r="J16" s="96" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="96"/>
-      <c r="L16" s="139" t="s">
+      <c r="G16" s="93"/>
+      <c r="H16" s="153" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="93"/>
+      <c r="J16" s="94" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="94"/>
+      <c r="L16" s="137" t="s">
         <v>58</v>
       </c>
-      <c r="M16" s="139"/>
-      <c r="N16" s="48"/>
+      <c r="M16" s="137"/>
+      <c r="N16" s="47"/>
     </row>
     <row r="17" spans="1:29" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="46"/>
-      <c r="B17" s="135" t="s">
+      <c r="A17" s="45"/>
+      <c r="B17" s="133" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="113"/>
-      <c r="D17" s="132" t="s">
+      <c r="C17" s="111"/>
+      <c r="D17" s="130" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="117"/>
-      <c r="F17" s="130" t="s">
+      <c r="E17" s="115"/>
+      <c r="F17" s="128" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="130"/>
-      <c r="H17" s="91" t="s">
+      <c r="G17" s="128"/>
+      <c r="H17" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="I17" s="86"/>
-      <c r="J17" s="98" t="s">
+      <c r="I17" s="84"/>
+      <c r="J17" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K17" s="86"/>
-      <c r="L17" s="140" t="s">
+      <c r="K17" s="84"/>
+      <c r="L17" s="138" t="s">
         <v>65</v>
       </c>
-      <c r="M17" s="141"/>
-      <c r="N17" s="48"/>
+      <c r="M17" s="139"/>
+      <c r="N17" s="47"/>
     </row>
     <row r="18" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="46"/>
-      <c r="B18" s="112" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="112"/>
-      <c r="D18" s="96" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="96"/>
-      <c r="F18" s="143" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="131"/>
-      <c r="H18" s="155" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="96"/>
-      <c r="J18" s="96" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="96"/>
-      <c r="L18" s="139" t="s">
-        <v>17</v>
-      </c>
-      <c r="M18" s="139"/>
-      <c r="N18" s="48"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="110" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="110"/>
+      <c r="D18" s="94" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="94"/>
+      <c r="F18" s="141" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="129"/>
+      <c r="H18" s="153" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="94"/>
+      <c r="L18" s="137" t="s">
+        <v>17</v>
+      </c>
+      <c r="M18" s="137"/>
+      <c r="N18" s="47"/>
     </row>
     <row r="19" spans="1:29" ht="27.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="46"/>
-      <c r="B19" s="135" t="s">
+      <c r="A19" s="45"/>
+      <c r="B19" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="118"/>
-      <c r="D19" s="118" t="s">
+      <c r="C19" s="116"/>
+      <c r="D19" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="118"/>
-      <c r="F19" s="118"/>
-      <c r="G19" s="132"/>
-      <c r="H19" s="135" t="s">
+      <c r="E19" s="116"/>
+      <c r="F19" s="116"/>
+      <c r="G19" s="130"/>
+      <c r="H19" s="133" t="s">
         <v>83</v>
       </c>
-      <c r="I19" s="115"/>
-      <c r="J19" s="113" t="s">
+      <c r="I19" s="113"/>
+      <c r="J19" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="K19" s="113"/>
-      <c r="L19" s="113"/>
-      <c r="M19" s="113"/>
-      <c r="N19" s="48"/>
+      <c r="K19" s="111"/>
+      <c r="L19" s="111"/>
+      <c r="M19" s="111"/>
+      <c r="N19" s="47"/>
     </row>
     <row r="20" spans="1:29" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="46"/>
-      <c r="B20" s="95" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="99"/>
-      <c r="D20" s="116" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="116"/>
-      <c r="F20" s="133"/>
-      <c r="G20" s="133"/>
-      <c r="H20" s="87" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="95"/>
-      <c r="J20" s="100" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" s="101"/>
-      <c r="L20" s="96"/>
-      <c r="M20" s="96"/>
-      <c r="N20" s="48"/>
-    </row>
-    <row r="21" spans="1:29" s="71" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="83"/>
-      <c r="B21" s="102"/>
-      <c r="C21" s="102"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="102"/>
-      <c r="F21" s="102"/>
-      <c r="G21" s="134"/>
-      <c r="H21" s="136"/>
-      <c r="I21" s="103"/>
-      <c r="J21" s="103"/>
-      <c r="K21" s="103"/>
-      <c r="L21" s="103"/>
-      <c r="M21" s="104"/>
-      <c r="N21" s="72"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="97"/>
+      <c r="D20" s="114" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="114"/>
+      <c r="F20" s="131"/>
+      <c r="G20" s="131"/>
+      <c r="H20" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="93"/>
+      <c r="J20" s="98" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="99"/>
+      <c r="L20" s="94"/>
+      <c r="M20" s="94"/>
+      <c r="N20" s="47"/>
+    </row>
+    <row r="21" spans="1:29" s="69" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="81"/>
+      <c r="B21" s="100"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="100"/>
+      <c r="F21" s="100"/>
+      <c r="G21" s="132"/>
+      <c r="H21" s="134"/>
+      <c r="I21" s="101"/>
+      <c r="J21" s="101"/>
+      <c r="K21" s="101"/>
+      <c r="L21" s="101"/>
+      <c r="M21" s="102"/>
+      <c r="N21" s="70"/>
       <c r="S21"/>
       <c r="T21"/>
       <c r="U21"/>
@@ -3811,432 +3881,432 @@
       <c r="AC21"/>
     </row>
     <row r="22" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="46"/>
-      <c r="B22" s="50" t="s">
+      <c r="A22" s="45"/>
+      <c r="B22" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="119" t="s">
+      <c r="C22" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
-      <c r="F22" s="137"/>
-      <c r="G22" s="119"/>
-      <c r="H22" s="50" t="s">
+      <c r="D22" s="117"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="135"/>
+      <c r="G22" s="117"/>
+      <c r="H22" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="I22" s="70" t="s">
+      <c r="I22" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="69" t="s">
+      <c r="J22" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="K22" s="119" t="s">
+      <c r="K22" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="L22" s="119"/>
-      <c r="M22" s="50" t="s">
+      <c r="L22" s="117"/>
+      <c r="M22" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="N22" s="48"/>
+      <c r="N22" s="47"/>
     </row>
     <row r="23" spans="1:29" ht="52.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="46"/>
-      <c r="B23" s="126" t="s">
+      <c r="A23" s="45"/>
+      <c r="B23" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="200" t="s">
+      <c r="C23" s="211" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="200"/>
-      <c r="E23" s="200"/>
-      <c r="F23" s="200"/>
-      <c r="G23" s="127"/>
-      <c r="H23" s="128" t="s">
+      <c r="D23" s="211"/>
+      <c r="E23" s="211"/>
+      <c r="F23" s="211"/>
+      <c r="G23" s="125"/>
+      <c r="H23" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="I23" s="68" t="s">
+      <c r="I23" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="J23" s="67">
+      <c r="J23" s="65">
         <v>14</v>
       </c>
-      <c r="K23" s="201" t="s">
+      <c r="K23" s="212" t="s">
         <v>44</v>
       </c>
-      <c r="L23" s="201"/>
-      <c r="M23" s="66" t="s">
+      <c r="L23" s="212"/>
+      <c r="M23" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="N23" s="48"/>
+      <c r="N23" s="47"/>
     </row>
     <row r="24" spans="1:29" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="46"/>
-      <c r="C24" s="124"/>
-      <c r="D24" s="124"/>
-      <c r="E24" s="124"/>
-      <c r="F24" s="124"/>
-      <c r="G24" s="124"/>
-      <c r="H24" s="125" t="s">
+      <c r="A24" s="45"/>
+      <c r="C24" s="122"/>
+      <c r="D24" s="122"/>
+      <c r="E24" s="122"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="122"/>
+      <c r="H24" s="123" t="s">
         <v>43</v>
       </c>
-      <c r="I24" s="65" t="s">
+      <c r="I24" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="J24" s="64">
+      <c r="J24" s="62">
         <v>14</v>
       </c>
-      <c r="K24" s="129" t="s">
-        <v>17</v>
-      </c>
-      <c r="L24" s="129"/>
-      <c r="M24" s="79" t="s">
+      <c r="K24" s="127" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" s="127"/>
+      <c r="M24" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="N24" s="48"/>
+      <c r="N24" s="47"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A25" s="46"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="63"/>
-      <c r="N25" s="48"/>
+      <c r="A25" s="45"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="47"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A26" s="46"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="63"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="63"/>
-      <c r="N26" s="48"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="47"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A27" s="46"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="58"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="63"/>
-      <c r="N27" s="48"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="47"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A28" s="46"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="63"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="63"/>
-      <c r="N28" s="48"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="61"/>
+      <c r="N28" s="47"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A29" s="46"/>
-      <c r="B29" s="58"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="63"/>
-      <c r="K29" s="58"/>
-      <c r="L29" s="58"/>
-      <c r="M29" s="63"/>
-      <c r="N29" s="48"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="61"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="61"/>
+      <c r="N29" s="47"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A30" s="46"/>
-      <c r="B30" s="58"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="63"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="63"/>
-      <c r="N30" s="48"/>
+      <c r="A30" s="45"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="61"/>
+      <c r="N30" s="47"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A31" s="46"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="63"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="63"/>
-      <c r="N31" s="48"/>
+      <c r="A31" s="45"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="61"/>
+      <c r="N31" s="47"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A32" s="46"/>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="48"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="47"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A33" s="46"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="63"/>
-      <c r="N33" s="48"/>
+      <c r="A33" s="45"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="61"/>
+      <c r="N33" s="47"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A34" s="46"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="63"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="63"/>
-      <c r="N34" s="48"/>
+      <c r="A34" s="45"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="56"/>
+      <c r="L34" s="56"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="47"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A35" s="46"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="63"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="63"/>
-      <c r="N35" s="48"/>
+      <c r="A35" s="45"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="61"/>
+      <c r="N35" s="47"/>
     </row>
     <row r="36" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="46"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="51"/>
-      <c r="I36" s="51"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="58"/>
-      <c r="M36" s="51"/>
-      <c r="N36" s="48"/>
+      <c r="A36" s="45"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="56"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="47"/>
     </row>
     <row r="37" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="46"/>
-      <c r="B37" s="81" t="s">
+      <c r="A37" s="45"/>
+      <c r="B37" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="60"/>
-      <c r="I37" s="121" t="s">
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="J37" s="120"/>
-      <c r="K37" s="120"/>
-      <c r="L37" s="120"/>
-      <c r="M37" s="120"/>
-      <c r="N37" s="48"/>
+      <c r="J37" s="118"/>
+      <c r="K37" s="118"/>
+      <c r="L37" s="118"/>
+      <c r="M37" s="118"/>
+      <c r="N37" s="47"/>
     </row>
     <row r="38" spans="1:14" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="46"/>
-      <c r="B38" s="82" t="s">
+      <c r="A38" s="45"/>
+      <c r="B38" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="51"/>
-      <c r="I38" s="59"/>
-      <c r="J38" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="47"/>
-      <c r="L38" s="58"/>
-      <c r="M38" s="51"/>
-      <c r="N38" s="48"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="K38" s="46"/>
+      <c r="L38" s="56"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="47"/>
     </row>
     <row r="39" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="46"/>
-      <c r="B39" s="82" t="s">
+      <c r="A39" s="45"/>
+      <c r="B39" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="58"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="58"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="48"/>
-      <c r="K39" s="47"/>
-      <c r="L39" s="58"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="48"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="47"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="56"/>
+      <c r="M39" s="50"/>
+      <c r="N39" s="47"/>
     </row>
     <row r="40" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="46"/>
-      <c r="B40" s="82" t="s">
+      <c r="A40" s="45"/>
+      <c r="B40" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="49"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47"/>
-      <c r="L40" s="58"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="48"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="50"/>
+      <c r="I40" s="57"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="56"/>
+      <c r="M40" s="50"/>
+      <c r="N40" s="47"/>
     </row>
     <row r="41" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="46"/>
-      <c r="B41" s="148" t="s">
+      <c r="A41" s="45"/>
+      <c r="B41" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="49"/>
-      <c r="H41" s="51"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="47"/>
-      <c r="L41" s="58"/>
-      <c r="M41" s="51"/>
-      <c r="N41" s="48"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="K41" s="46"/>
+      <c r="L41" s="56"/>
+      <c r="M41" s="50"/>
+      <c r="N41" s="47"/>
     </row>
     <row r="42" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="151"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="59"/>
-      <c r="K42" s="47"/>
-      <c r="L42" s="58"/>
-      <c r="M42" s="51"/>
-      <c r="N42" s="48"/>
+      <c r="B42" s="149"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="57"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="56"/>
+      <c r="M42" s="50"/>
+      <c r="N42" s="47"/>
     </row>
     <row r="43" spans="1:14" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="151"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="51"/>
-      <c r="I43" s="59"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="47"/>
-      <c r="L43" s="58"/>
-      <c r="M43" s="51"/>
-      <c r="N43" s="48"/>
+      <c r="B43" s="149"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="56"/>
+      <c r="E43" s="56"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="56"/>
+      <c r="M43" s="50"/>
+      <c r="N43" s="47"/>
     </row>
     <row r="44" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="151"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="49"/>
-      <c r="H44" s="51"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="47"/>
-      <c r="K44" s="47"/>
-      <c r="L44" s="58"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="48"/>
-    </row>
-    <row r="45" spans="1:14" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="147"/>
-      <c r="B45" s="149"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="122"/>
-      <c r="J45" s="150"/>
-      <c r="K45" s="123"/>
-      <c r="L45" s="123"/>
-      <c r="M45" s="123"/>
-      <c r="N45" s="80"/>
+      <c r="B44" s="149"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="46"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="47"/>
+    </row>
+    <row r="45" spans="1:14" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="145"/>
+      <c r="B45" s="147"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="120"/>
+      <c r="J45" s="148"/>
+      <c r="K45" s="121"/>
+      <c r="L45" s="121"/>
+      <c r="M45" s="121"/>
+      <c r="N45" s="78"/>
     </row>
     <row r="46" spans="1:14" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="47" spans="1:14" ht="0.85" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
init rows dynamic headers bug fixed + minor tmp fix + port letter indexation fixed
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED4D783-FDB6-42A1-BF95-5E7F638CD273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7031575-59AA-4537-9D40-B0D3E17B7834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -820,7 +820,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="234">
+  <cellXfs count="232">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1339,6 +1339,84 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1357,81 +1435,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1443,15 +1446,6 @@
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1818,8 +1812,8 @@
   </sheetPr>
   <dimension ref="A1:AF102"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="91" zoomScaleNormal="100" zoomScaleSheetLayoutView="91" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScale="91" zoomScaleNormal="100" zoomScaleSheetLayoutView="91" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1871,18 +1865,18 @@
       <c r="I1" s="143"/>
     </row>
     <row r="2" spans="2:30" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="222" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="196" t="s">
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="224"/>
+      <c r="F2" s="222" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
-      <c r="I2" s="197"/>
+      <c r="G2" s="223"/>
+      <c r="H2" s="223"/>
+      <c r="I2" s="223"/>
       <c r="J2" s="144"/>
       <c r="L2" s="8"/>
       <c r="N2" s="15"/>
@@ -1892,18 +1886,18 @@
       <c r="AD2" s="15"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="199" t="s">
+      <c r="B3" s="225" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="201"/>
-      <c r="F3" s="199" t="s">
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="227"/>
+      <c r="F3" s="225" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="200"/>
-      <c r="H3" s="200"/>
-      <c r="I3" s="200"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="226"/>
+      <c r="I3" s="226"/>
       <c r="J3" s="6"/>
       <c r="L3" s="8"/>
       <c r="O3" s="7"/>
@@ -1920,18 +1914,18 @@
       <c r="Z3" s="7"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="199" t="s">
+      <c r="B4" s="225" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="200"/>
-      <c r="D4" s="200"/>
-      <c r="E4" s="201"/>
-      <c r="F4" s="199" t="s">
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="227"/>
+      <c r="F4" s="225" t="s">
         <v>90</v>
       </c>
-      <c r="G4" s="200"/>
-      <c r="H4" s="200"/>
-      <c r="I4" s="200"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
       <c r="J4" s="6"/>
       <c r="N4" s="10"/>
       <c r="O4" s="11"/>
@@ -1952,18 +1946,18 @@
       <c r="AD4" s="10"/>
     </row>
     <row r="5" spans="2:30" s="14" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="205" t="s">
+      <c r="B5" s="218" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="206"/>
-      <c r="D5" s="206"/>
-      <c r="E5" s="207"/>
-      <c r="F5" s="205" t="s">
+      <c r="C5" s="219"/>
+      <c r="D5" s="219"/>
+      <c r="E5" s="220"/>
+      <c r="F5" s="218" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="206"/>
-      <c r="H5" s="206"/>
-      <c r="I5" s="206"/>
+      <c r="G5" s="219"/>
+      <c r="H5" s="219"/>
+      <c r="I5" s="219"/>
       <c r="J5" s="13"/>
       <c r="N5" s="15"/>
       <c r="AA5" s="15"/>
@@ -2028,44 +2022,44 @@
       <c r="Z7" s="7"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="208" t="s">
+      <c r="B8" s="207" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="209"/>
-      <c r="D8" s="209"/>
-      <c r="E8" s="210"/>
-      <c r="F8" s="208" t="s">
+      <c r="C8" s="208"/>
+      <c r="D8" s="208"/>
+      <c r="E8" s="221"/>
+      <c r="F8" s="207" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="209"/>
-      <c r="H8" s="209"/>
-      <c r="I8" s="209"/>
+      <c r="G8" s="208"/>
+      <c r="H8" s="208"/>
+      <c r="I8" s="208"/>
       <c r="J8" s="19"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="202" t="s">
+      <c r="B9" s="197" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="203"/>
-      <c r="D9" s="203"/>
-      <c r="E9" s="204"/>
-      <c r="F9" s="202" t="s">
+      <c r="C9" s="198"/>
+      <c r="D9" s="198"/>
+      <c r="E9" s="199"/>
+      <c r="F9" s="197" t="s">
         <v>96</v>
       </c>
-      <c r="G9" s="203"/>
-      <c r="H9" s="203"/>
-      <c r="I9" s="204"/>
+      <c r="G9" s="198"/>
+      <c r="H9" s="198"/>
+      <c r="I9" s="199"/>
       <c r="J9" s="19"/>
     </row>
-    <row r="10" spans="2:30" ht="8.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="202"/>
-      <c r="C10" s="203"/>
-      <c r="D10" s="203"/>
-      <c r="E10" s="204"/>
-      <c r="F10" s="202"/>
-      <c r="G10" s="203"/>
-      <c r="H10" s="203"/>
-      <c r="I10" s="204"/>
+    <row r="10" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="197"/>
+      <c r="C10" s="198"/>
+      <c r="D10" s="198"/>
+      <c r="E10" s="199"/>
+      <c r="F10" s="197"/>
+      <c r="G10" s="198"/>
+      <c r="H10" s="198"/>
+      <c r="I10" s="199"/>
       <c r="J10" s="19"/>
       <c r="N10" s="15"/>
       <c r="O10" s="7"/>
@@ -2140,18 +2134,18 @@
       <c r="Z12" s="7"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="202" t="s">
+      <c r="B13" s="197" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="203"/>
-      <c r="D13" s="203"/>
-      <c r="E13" s="204"/>
-      <c r="F13" s="202" t="s">
+      <c r="C13" s="198"/>
+      <c r="D13" s="198"/>
+      <c r="E13" s="199"/>
+      <c r="F13" s="197" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="203"/>
-      <c r="H13" s="203"/>
-      <c r="I13" s="203"/>
+      <c r="G13" s="198"/>
+      <c r="H13" s="198"/>
+      <c r="I13" s="198"/>
       <c r="J13" s="19"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
@@ -2169,18 +2163,18 @@
       <c r="AA13" s="7"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="202" t="s">
+      <c r="B14" s="197" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="203"/>
-      <c r="D14" s="203"/>
-      <c r="E14" s="204"/>
-      <c r="F14" s="202" t="s">
+      <c r="C14" s="198"/>
+      <c r="D14" s="198"/>
+      <c r="E14" s="199"/>
+      <c r="F14" s="197" t="s">
         <v>100</v>
       </c>
-      <c r="G14" s="203"/>
-      <c r="H14" s="203"/>
-      <c r="I14" s="203"/>
+      <c r="G14" s="198"/>
+      <c r="H14" s="198"/>
+      <c r="I14" s="198"/>
       <c r="J14" s="19"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
@@ -2198,18 +2192,18 @@
       <c r="AA14" s="7"/>
     </row>
     <row r="15" spans="2:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="202" t="s">
+      <c r="B15" s="197" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="203"/>
-      <c r="D15" s="203"/>
-      <c r="E15" s="204"/>
-      <c r="F15" s="202" t="s">
+      <c r="C15" s="198"/>
+      <c r="D15" s="198"/>
+      <c r="E15" s="199"/>
+      <c r="F15" s="197" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="203"/>
-      <c r="H15" s="203"/>
-      <c r="I15" s="203"/>
+      <c r="G15" s="198"/>
+      <c r="H15" s="198"/>
+      <c r="I15" s="198"/>
       <c r="J15" s="19"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
@@ -2256,18 +2250,18 @@
       <c r="AA16" s="7"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="211" t="s">
+      <c r="B17" s="209" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="212"/>
-      <c r="D17" s="212"/>
-      <c r="E17" s="213"/>
-      <c r="F17" s="211" t="s">
+      <c r="C17" s="210"/>
+      <c r="D17" s="210"/>
+      <c r="E17" s="211"/>
+      <c r="F17" s="209" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="212"/>
-      <c r="H17" s="212"/>
-      <c r="I17" s="212"/>
+      <c r="G17" s="210"/>
+      <c r="H17" s="210"/>
+      <c r="I17" s="210"/>
       <c r="J17" s="19"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
@@ -2285,18 +2279,18 @@
       <c r="AA17" s="7"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="214" t="s">
+      <c r="B18" s="212" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="215"/>
+      <c r="C18" s="213"/>
       <c r="D18" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="215" t="s">
+      <c r="E18" s="213" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="215"/>
-      <c r="G18" s="215"/>
+      <c r="F18" s="213"/>
+      <c r="G18" s="213"/>
       <c r="H18" s="20" t="s">
         <v>35</v>
       </c>
@@ -2320,18 +2314,18 @@
       <c r="AA18" s="7"/>
     </row>
     <row r="19" spans="2:30" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="216" t="s">
+      <c r="B19" s="214" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="217"/>
+      <c r="C19" s="215"/>
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="218" t="s">
+      <c r="E19" s="216" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="219"/>
-      <c r="G19" s="219"/>
+      <c r="F19" s="217"/>
+      <c r="G19" s="217"/>
       <c r="H19" s="187" t="s">
         <v>12</v>
       </c>
@@ -2359,14 +2353,14 @@
     </row>
     <row r="20" spans="2:30" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="183"/>
-      <c r="C20" s="231"/>
-      <c r="D20" s="231"/>
-      <c r="E20" s="232"/>
+      <c r="C20" s="184"/>
+      <c r="D20" s="184"/>
+      <c r="E20" s="185"/>
       <c r="F20" s="190"/>
       <c r="G20" s="186"/>
       <c r="H20" s="187"/>
       <c r="I20" s="191"/>
-      <c r="J20" s="233"/>
+      <c r="J20" s="196"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
@@ -2387,14 +2381,14 @@
     </row>
     <row r="21" spans="2:30" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="183"/>
-      <c r="C21" s="231"/>
-      <c r="D21" s="231"/>
-      <c r="E21" s="232"/>
+      <c r="C21" s="184"/>
+      <c r="D21" s="184"/>
+      <c r="E21" s="185"/>
       <c r="F21" s="189"/>
-      <c r="G21" s="232"/>
-      <c r="H21" s="231"/>
+      <c r="G21" s="185"/>
+      <c r="H21" s="184"/>
       <c r="I21" s="193"/>
-      <c r="J21" s="233"/>
+      <c r="J21" s="196"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
@@ -2415,14 +2409,14 @@
     </row>
     <row r="22" spans="2:30" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="183"/>
-      <c r="C22" s="231"/>
-      <c r="D22" s="231"/>
-      <c r="E22" s="232"/>
+      <c r="C22" s="184"/>
+      <c r="D22" s="184"/>
+      <c r="E22" s="185"/>
       <c r="F22" s="189"/>
-      <c r="G22" s="232"/>
-      <c r="H22" s="231"/>
+      <c r="G22" s="185"/>
+      <c r="H22" s="184"/>
       <c r="I22" s="193"/>
-      <c r="J22" s="233"/>
+      <c r="J22" s="196"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
@@ -2443,14 +2437,14 @@
     </row>
     <row r="23" spans="2:30" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="183"/>
-      <c r="C23" s="231"/>
-      <c r="D23" s="231"/>
-      <c r="E23" s="232"/>
+      <c r="C23" s="184"/>
+      <c r="D23" s="184"/>
+      <c r="E23" s="185"/>
       <c r="F23" s="189"/>
-      <c r="G23" s="232"/>
-      <c r="H23" s="231"/>
+      <c r="G23" s="185"/>
+      <c r="H23" s="184"/>
       <c r="I23" s="193"/>
-      <c r="J23" s="233"/>
+      <c r="J23" s="196"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
@@ -2471,14 +2465,14 @@
     </row>
     <row r="24" spans="2:30" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="183"/>
-      <c r="C24" s="231"/>
-      <c r="D24" s="231"/>
-      <c r="E24" s="232"/>
+      <c r="C24" s="184"/>
+      <c r="D24" s="184"/>
+      <c r="E24" s="185"/>
       <c r="F24" s="189"/>
-      <c r="G24" s="232"/>
-      <c r="H24" s="231"/>
+      <c r="G24" s="185"/>
+      <c r="H24" s="184"/>
       <c r="I24" s="193"/>
-      <c r="J24" s="233"/>
+      <c r="J24" s="196"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
@@ -2499,14 +2493,14 @@
     </row>
     <row r="25" spans="2:30" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="183"/>
-      <c r="C25" s="231"/>
-      <c r="D25" s="231"/>
-      <c r="E25" s="232"/>
+      <c r="C25" s="184"/>
+      <c r="D25" s="184"/>
+      <c r="E25" s="185"/>
       <c r="F25" s="189"/>
-      <c r="G25" s="232"/>
-      <c r="H25" s="231"/>
+      <c r="G25" s="185"/>
+      <c r="H25" s="184"/>
       <c r="I25" s="193"/>
-      <c r="J25" s="233"/>
+      <c r="J25" s="196"/>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
@@ -2527,14 +2521,14 @@
     </row>
     <row r="26" spans="2:30" ht="0.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="183"/>
-      <c r="C26" s="231"/>
-      <c r="D26" s="231"/>
-      <c r="E26" s="232"/>
+      <c r="C26" s="184"/>
+      <c r="D26" s="184"/>
+      <c r="E26" s="185"/>
       <c r="F26" s="189"/>
-      <c r="G26" s="232"/>
-      <c r="H26" s="231"/>
+      <c r="G26" s="185"/>
+      <c r="H26" s="184"/>
       <c r="I26" s="193"/>
-      <c r="J26" s="233"/>
+      <c r="J26" s="196"/>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
@@ -2559,8 +2553,8 @@
       <c r="D27" s="184"/>
       <c r="E27" s="185"/>
       <c r="F27" s="189"/>
-      <c r="G27" s="232"/>
-      <c r="H27" s="231"/>
+      <c r="G27" s="185"/>
+      <c r="H27" s="184"/>
       <c r="I27" s="193"/>
       <c r="J27" s="2"/>
       <c r="N27" s="7"/>
@@ -2821,18 +2815,18 @@
       <c r="AD35" s="7"/>
     </row>
     <row r="36" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="202" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="203"/>
-      <c r="D36" s="203"/>
-      <c r="E36" s="203"/>
-      <c r="F36" s="202" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="203"/>
-      <c r="H36" s="203"/>
-      <c r="I36" s="204"/>
+      <c r="B36" s="197" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="198"/>
+      <c r="D36" s="198"/>
+      <c r="E36" s="198"/>
+      <c r="F36" s="197" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="198"/>
+      <c r="H36" s="198"/>
+      <c r="I36" s="199"/>
       <c r="J36" s="13"/>
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
@@ -2917,33 +2911,33 @@
       <c r="AD38" s="7"/>
     </row>
     <row r="39" spans="1:30" s="27" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="220" t="s">
+      <c r="B39" s="204" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="221"/>
-      <c r="D39" s="221"/>
-      <c r="E39" s="221"/>
-      <c r="F39" s="220" t="s">
+      <c r="C39" s="205"/>
+      <c r="D39" s="205"/>
+      <c r="E39" s="205"/>
+      <c r="F39" s="204" t="s">
         <v>84</v>
       </c>
-      <c r="G39" s="221"/>
-      <c r="H39" s="221"/>
-      <c r="I39" s="222"/>
+      <c r="G39" s="205"/>
+      <c r="H39" s="205"/>
+      <c r="I39" s="206"/>
       <c r="J39" s="154"/>
     </row>
     <row r="40" spans="1:30" s="27" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="208" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="209"/>
-      <c r="D40" s="209"/>
-      <c r="E40" s="209"/>
-      <c r="F40" s="202" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" s="203"/>
-      <c r="H40" s="203"/>
-      <c r="I40" s="204"/>
+      <c r="B40" s="207" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="208"/>
+      <c r="D40" s="208"/>
+      <c r="E40" s="208"/>
+      <c r="F40" s="197" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="198"/>
+      <c r="H40" s="198"/>
+      <c r="I40" s="199"/>
       <c r="J40" s="154"/>
     </row>
     <row r="41" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
@@ -2979,18 +2973,18 @@
       <c r="AD41" s="7"/>
     </row>
     <row r="42" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="202" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="203"/>
-      <c r="D42" s="203"/>
-      <c r="E42" s="203"/>
-      <c r="F42" s="202" t="s">
-        <v>17</v>
-      </c>
-      <c r="G42" s="203"/>
-      <c r="H42" s="203"/>
-      <c r="I42" s="204"/>
+      <c r="B42" s="197" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="198"/>
+      <c r="D42" s="198"/>
+      <c r="E42" s="198"/>
+      <c r="F42" s="197" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" s="198"/>
+      <c r="H42" s="198"/>
+      <c r="I42" s="199"/>
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
@@ -3008,7 +3002,7 @@
       <c r="I43" s="157"/>
       <c r="J43" s="6"/>
     </row>
-    <row r="44" spans="1:30" ht="9.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:30" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="170"/>
       <c r="B44" s="169"/>
       <c r="C44" s="5"/>
@@ -3036,18 +3030,18 @@
       <c r="J45" s="6"/>
     </row>
     <row r="46" spans="1:30" s="27" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="223" t="s">
+      <c r="B46" s="200" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="224"/>
-      <c r="D46" s="224"/>
-      <c r="E46" s="224"/>
-      <c r="F46" s="223" t="s">
+      <c r="C46" s="201"/>
+      <c r="D46" s="201"/>
+      <c r="E46" s="201"/>
+      <c r="F46" s="200" t="s">
         <v>101</v>
       </c>
-      <c r="G46" s="224"/>
-      <c r="H46" s="224"/>
-      <c r="I46" s="225"/>
+      <c r="G46" s="201"/>
+      <c r="H46" s="201"/>
+      <c r="I46" s="202"/>
       <c r="J46" s="26"/>
       <c r="N46" s="28"/>
       <c r="O46" s="28"/>
@@ -3068,93 +3062,93 @@
       <c r="AD46" s="28"/>
     </row>
     <row r="47" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="202" t="s">
+      <c r="B47" s="197" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="203"/>
-      <c r="D47" s="203"/>
-      <c r="E47" s="203"/>
-      <c r="F47" s="202" t="s">
+      <c r="C47" s="198"/>
+      <c r="D47" s="198"/>
+      <c r="E47" s="198"/>
+      <c r="F47" s="197" t="s">
         <v>102</v>
       </c>
-      <c r="G47" s="203"/>
-      <c r="H47" s="203"/>
-      <c r="I47" s="204"/>
+      <c r="G47" s="198"/>
+      <c r="H47" s="198"/>
+      <c r="I47" s="199"/>
       <c r="J47" s="16"/>
     </row>
     <row r="48" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="202" t="s">
+      <c r="B48" s="197" t="s">
         <v>104</v>
       </c>
-      <c r="C48" s="203"/>
-      <c r="D48" s="203"/>
-      <c r="E48" s="204"/>
-      <c r="F48" s="202" t="s">
+      <c r="C48" s="198"/>
+      <c r="D48" s="198"/>
+      <c r="E48" s="199"/>
+      <c r="F48" s="197" t="s">
         <v>103</v>
       </c>
-      <c r="G48" s="203"/>
-      <c r="H48" s="203"/>
-      <c r="I48" s="203"/>
+      <c r="G48" s="198"/>
+      <c r="H48" s="198"/>
+      <c r="I48" s="198"/>
       <c r="J48" s="16"/>
     </row>
     <row r="49" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="202" t="s">
+      <c r="B49" s="197" t="s">
         <v>105</v>
       </c>
-      <c r="C49" s="203"/>
-      <c r="D49" s="203"/>
-      <c r="E49" s="204"/>
-      <c r="F49" s="202" t="s">
+      <c r="C49" s="198"/>
+      <c r="D49" s="198"/>
+      <c r="E49" s="199"/>
+      <c r="F49" s="197" t="s">
         <v>106</v>
       </c>
-      <c r="G49" s="203"/>
-      <c r="H49" s="203"/>
-      <c r="I49" s="203"/>
+      <c r="G49" s="198"/>
+      <c r="H49" s="198"/>
+      <c r="I49" s="198"/>
       <c r="J49" s="16"/>
     </row>
     <row r="50" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="202" t="s">
+      <c r="B50" s="197" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="203"/>
-      <c r="D50" s="203"/>
-      <c r="E50" s="204"/>
-      <c r="F50" s="202" t="s">
+      <c r="C50" s="198"/>
+      <c r="D50" s="198"/>
+      <c r="E50" s="199"/>
+      <c r="F50" s="197" t="s">
         <v>107</v>
       </c>
-      <c r="G50" s="203"/>
-      <c r="H50" s="203"/>
-      <c r="I50" s="203"/>
+      <c r="G50" s="198"/>
+      <c r="H50" s="198"/>
+      <c r="I50" s="198"/>
       <c r="J50" s="16"/>
     </row>
     <row r="51" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="202" t="s">
+      <c r="B51" s="197" t="s">
         <v>108</v>
       </c>
-      <c r="C51" s="203"/>
-      <c r="D51" s="203"/>
-      <c r="E51" s="204"/>
-      <c r="F51" s="202" t="s">
+      <c r="C51" s="198"/>
+      <c r="D51" s="198"/>
+      <c r="E51" s="199"/>
+      <c r="F51" s="197" t="s">
         <v>109</v>
       </c>
-      <c r="G51" s="203"/>
-      <c r="H51" s="203"/>
-      <c r="I51" s="203"/>
+      <c r="G51" s="198"/>
+      <c r="H51" s="198"/>
+      <c r="I51" s="198"/>
       <c r="J51" s="16"/>
     </row>
     <row r="52" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="202" t="s">
+      <c r="B52" s="197" t="s">
         <v>110</v>
       </c>
-      <c r="C52" s="203"/>
-      <c r="D52" s="203"/>
-      <c r="E52" s="204"/>
-      <c r="F52" s="202" t="s">
+      <c r="C52" s="198"/>
+      <c r="D52" s="198"/>
+      <c r="E52" s="199"/>
+      <c r="F52" s="197" t="s">
         <v>111</v>
       </c>
-      <c r="G52" s="203"/>
-      <c r="H52" s="203"/>
-      <c r="I52" s="203"/>
+      <c r="G52" s="198"/>
+      <c r="H52" s="198"/>
+      <c r="I52" s="198"/>
       <c r="J52" s="16"/>
     </row>
     <row r="53" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3173,18 +3167,18 @@
       <c r="J53" s="16"/>
     </row>
     <row r="54" spans="2:30" s="27" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="223" t="s">
+      <c r="B54" s="200" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="224"/>
-      <c r="D54" s="224"/>
-      <c r="E54" s="225"/>
-      <c r="F54" s="223" t="s">
+      <c r="C54" s="201"/>
+      <c r="D54" s="201"/>
+      <c r="E54" s="202"/>
+      <c r="F54" s="200" t="s">
         <v>97</v>
       </c>
-      <c r="G54" s="226"/>
-      <c r="H54" s="226"/>
-      <c r="I54" s="226"/>
+      <c r="G54" s="203"/>
+      <c r="H54" s="203"/>
+      <c r="I54" s="203"/>
       <c r="J54" s="26"/>
       <c r="N54" s="28"/>
       <c r="O54" s="28"/>
@@ -3205,18 +3199,18 @@
       <c r="AD54" s="28"/>
     </row>
     <row r="55" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B55" s="202" t="s">
+      <c r="B55" s="197" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="203"/>
-      <c r="D55" s="203"/>
-      <c r="E55" s="204"/>
-      <c r="F55" s="202" t="s">
+      <c r="C55" s="198"/>
+      <c r="D55" s="198"/>
+      <c r="E55" s="199"/>
+      <c r="F55" s="197" t="s">
         <v>112</v>
       </c>
-      <c r="G55" s="203"/>
-      <c r="H55" s="203"/>
-      <c r="I55" s="203"/>
+      <c r="G55" s="198"/>
+      <c r="H55" s="198"/>
+      <c r="I55" s="198"/>
       <c r="J55" s="16"/>
     </row>
     <row r="56" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3276,18 +3270,18 @@
       <c r="J59" s="16"/>
     </row>
     <row r="60" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B60" s="202" t="s">
+      <c r="B60" s="197" t="s">
         <v>105</v>
       </c>
-      <c r="C60" s="203"/>
-      <c r="D60" s="203"/>
-      <c r="E60" s="204"/>
-      <c r="F60" s="202" t="s">
+      <c r="C60" s="198"/>
+      <c r="D60" s="198"/>
+      <c r="E60" s="199"/>
+      <c r="F60" s="197" t="s">
         <v>105</v>
       </c>
-      <c r="G60" s="203"/>
-      <c r="H60" s="203"/>
-      <c r="I60" s="204"/>
+      <c r="G60" s="198"/>
+      <c r="H60" s="198"/>
+      <c r="I60" s="199"/>
       <c r="J60" s="16"/>
     </row>
     <row r="61" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3506,6 +3500,42 @@
     <row r="102" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="F9:I10"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="F47:I47"/>
     <mergeCell ref="B48:E48"/>
     <mergeCell ref="F48:I48"/>
     <mergeCell ref="B60:E60"/>
@@ -3522,42 +3552,6 @@
     <mergeCell ref="F51:I51"/>
     <mergeCell ref="B52:E52"/>
     <mergeCell ref="F52:I52"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="F9:I10"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <conditionalFormatting sqref="D19:E31 J19:J31 E32:E33 B33">
     <cfRule type="notContainsBlanks" dxfId="3" priority="2">
@@ -3596,8 +3590,8 @@
   </sheetPr>
   <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3866,7 +3860,7 @@
       <c r="M13" s="84"/>
       <c r="N13" s="47"/>
     </row>
-    <row r="14" spans="1:14" ht="44.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="45"/>
       <c r="B14" s="151" t="s">
         <v>6</v>
@@ -3888,10 +3882,10 @@
     </row>
     <row r="15" spans="1:14" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="72"/>
-      <c r="B15" s="229" t="s">
+      <c r="B15" s="230" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="230"/>
+      <c r="C15" s="231"/>
       <c r="D15" s="90" t="s">
         <v>60</v>
       </c>
@@ -4108,12 +4102,12 @@
       <c r="B23" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="227" t="s">
+      <c r="C23" s="228" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="227"/>
-      <c r="E23" s="227"/>
-      <c r="F23" s="227"/>
+      <c r="D23" s="228"/>
+      <c r="E23" s="228"/>
+      <c r="F23" s="228"/>
       <c r="G23" s="125"/>
       <c r="H23" s="126" t="s">
         <v>45</v>
@@ -4124,10 +4118,10 @@
       <c r="J23" s="65">
         <v>14</v>
       </c>
-      <c r="K23" s="228" t="s">
+      <c r="K23" s="229" t="s">
         <v>44</v>
       </c>
-      <c r="L23" s="228"/>
+      <c r="L23" s="229"/>
       <c r="M23" s="64" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
tmp export storage invoice updated, fixing bug with redefineCell prop fn
</commit_message>
<xml_diff>
--- a/templates/Export_Agreement.xlsx
+++ b/templates/Export_Agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7031575-59AA-4537-9D40-B0D3E17B7834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81A8488-1D39-4C17-8275-0379DD0D10B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
+    <workbookView xWindow="1837" yWindow="4230" windowWidth="21600" windowHeight="11423" activeTab="1" xr2:uid="{B6FC3AD6-F63C-4057-BD0B-525C27FA51AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Export_Contract" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,11 @@
     <definedName name="Инвойс_подписант">Invoice!$I$37</definedName>
     <definedName name="Инвойс_покупатель">Invoice!$B$10</definedName>
     <definedName name="Инвойс_покупатель_адрес">Invoice!$B$11</definedName>
+    <definedName name="Инвойс_покупатель_заголовок">Invoice!$B$9</definedName>
     <definedName name="Инвойс_получатель">Invoice!$B$13</definedName>
     <definedName name="Инвойс_получатель_адрес">Invoice!$B$14</definedName>
     <definedName name="Инвойс_получатель_в_пользу">Invoice!$B$40</definedName>
+    <definedName name="Инвойс_получатель_заголовок">Invoice!$B$12</definedName>
     <definedName name="Инвойс_получатель_счет">Invoice!$B$41</definedName>
     <definedName name="Инвойс_продавец">Invoice!$B$7</definedName>
     <definedName name="Инвойс_продавец_адрес">Invoice!$B$8</definedName>
@@ -1342,6 +1344,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1351,6 +1371,60 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1362,78 +1436,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1805,6 +1807,24 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="700" row="5">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{194B85D8-D21E-44BE-839F-C25D13EC1DF3}">
+  <we:reference id="5dbca137-d02b-4283-adec-e6f28aeb3ed7" version="1.0.0.0" store="developer" storeType="Registry"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BF4CFE-C418-488F-8DFD-13F601FB1BC8}">
   <sheetPr>
@@ -1812,8 +1832,8 @@
   </sheetPr>
   <dimension ref="A1:AF102"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScale="91" zoomScaleNormal="100" zoomScaleSheetLayoutView="91" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView view="pageBreakPreview" zoomScale="91" zoomScaleNormal="100" zoomScaleSheetLayoutView="91" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1865,18 +1885,18 @@
       <c r="I1" s="143"/>
     </row>
     <row r="2" spans="2:30" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="197" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="222" t="s">
+      <c r="C2" s="198"/>
+      <c r="D2" s="198"/>
+      <c r="E2" s="199"/>
+      <c r="F2" s="197" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
-      <c r="I2" s="223"/>
+      <c r="G2" s="198"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="198"/>
       <c r="J2" s="144"/>
       <c r="L2" s="8"/>
       <c r="N2" s="15"/>
@@ -1886,18 +1906,18 @@
       <c r="AD2" s="15"/>
     </row>
     <row r="3" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="225" t="s">
+      <c r="B3" s="200" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="226"/>
-      <c r="D3" s="226"/>
-      <c r="E3" s="227"/>
-      <c r="F3" s="225" t="s">
+      <c r="C3" s="201"/>
+      <c r="D3" s="201"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="200" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="226"/>
-      <c r="H3" s="226"/>
-      <c r="I3" s="226"/>
+      <c r="G3" s="201"/>
+      <c r="H3" s="201"/>
+      <c r="I3" s="201"/>
       <c r="J3" s="6"/>
       <c r="L3" s="8"/>
       <c r="O3" s="7"/>
@@ -1914,18 +1934,18 @@
       <c r="Z3" s="7"/>
     </row>
     <row r="4" spans="2:30" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="225" t="s">
+      <c r="B4" s="200" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="226"/>
-      <c r="D4" s="226"/>
-      <c r="E4" s="227"/>
-      <c r="F4" s="225" t="s">
+      <c r="C4" s="201"/>
+      <c r="D4" s="201"/>
+      <c r="E4" s="202"/>
+      <c r="F4" s="200" t="s">
         <v>90</v>
       </c>
-      <c r="G4" s="226"/>
-      <c r="H4" s="226"/>
-      <c r="I4" s="226"/>
+      <c r="G4" s="201"/>
+      <c r="H4" s="201"/>
+      <c r="I4" s="201"/>
       <c r="J4" s="6"/>
       <c r="N4" s="10"/>
       <c r="O4" s="11"/>
@@ -1946,18 +1966,18 @@
       <c r="AD4" s="10"/>
     </row>
     <row r="5" spans="2:30" s="14" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="218" t="s">
+      <c r="B5" s="206" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="219"/>
-      <c r="D5" s="219"/>
-      <c r="E5" s="220"/>
-      <c r="F5" s="218" t="s">
+      <c r="C5" s="207"/>
+      <c r="D5" s="207"/>
+      <c r="E5" s="208"/>
+      <c r="F5" s="206" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="219"/>
-      <c r="H5" s="219"/>
-      <c r="I5" s="219"/>
+      <c r="G5" s="207"/>
+      <c r="H5" s="207"/>
+      <c r="I5" s="207"/>
       <c r="J5" s="13"/>
       <c r="N5" s="15"/>
       <c r="AA5" s="15"/>
@@ -2022,44 +2042,44 @@
       <c r="Z7" s="7"/>
     </row>
     <row r="8" spans="2:30" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="207" t="s">
+      <c r="B8" s="209" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="208"/>
-      <c r="D8" s="208"/>
-      <c r="E8" s="221"/>
-      <c r="F8" s="207" t="s">
+      <c r="C8" s="210"/>
+      <c r="D8" s="210"/>
+      <c r="E8" s="211"/>
+      <c r="F8" s="209" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="208"/>
-      <c r="H8" s="208"/>
-      <c r="I8" s="208"/>
+      <c r="G8" s="210"/>
+      <c r="H8" s="210"/>
+      <c r="I8" s="210"/>
       <c r="J8" s="19"/>
     </row>
     <row r="9" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="197" t="s">
+      <c r="B9" s="203" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="198"/>
-      <c r="D9" s="198"/>
-      <c r="E9" s="199"/>
-      <c r="F9" s="197" t="s">
+      <c r="C9" s="204"/>
+      <c r="D9" s="204"/>
+      <c r="E9" s="205"/>
+      <c r="F9" s="203" t="s">
         <v>96</v>
       </c>
-      <c r="G9" s="198"/>
-      <c r="H9" s="198"/>
-      <c r="I9" s="199"/>
+      <c r="G9" s="204"/>
+      <c r="H9" s="204"/>
+      <c r="I9" s="205"/>
       <c r="J9" s="19"/>
     </row>
     <row r="10" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="197"/>
-      <c r="C10" s="198"/>
-      <c r="D10" s="198"/>
-      <c r="E10" s="199"/>
-      <c r="F10" s="197"/>
-      <c r="G10" s="198"/>
-      <c r="H10" s="198"/>
-      <c r="I10" s="199"/>
+      <c r="B10" s="203"/>
+      <c r="C10" s="204"/>
+      <c r="D10" s="204"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="203"/>
+      <c r="G10" s="204"/>
+      <c r="H10" s="204"/>
+      <c r="I10" s="205"/>
       <c r="J10" s="19"/>
       <c r="N10" s="15"/>
       <c r="O10" s="7"/>
@@ -2134,18 +2154,18 @@
       <c r="Z12" s="7"/>
     </row>
     <row r="13" spans="2:30" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="197" t="s">
+      <c r="B13" s="203" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="198"/>
-      <c r="D13" s="198"/>
-      <c r="E13" s="199"/>
-      <c r="F13" s="197" t="s">
+      <c r="C13" s="204"/>
+      <c r="D13" s="204"/>
+      <c r="E13" s="205"/>
+      <c r="F13" s="203" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="198"/>
-      <c r="H13" s="198"/>
-      <c r="I13" s="198"/>
+      <c r="G13" s="204"/>
+      <c r="H13" s="204"/>
+      <c r="I13" s="204"/>
       <c r="J13" s="19"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
@@ -2163,18 +2183,18 @@
       <c r="AA13" s="7"/>
     </row>
     <row r="14" spans="2:30" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="197" t="s">
+      <c r="B14" s="203" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="198"/>
-      <c r="D14" s="198"/>
-      <c r="E14" s="199"/>
-      <c r="F14" s="197" t="s">
+      <c r="C14" s="204"/>
+      <c r="D14" s="204"/>
+      <c r="E14" s="205"/>
+      <c r="F14" s="203" t="s">
         <v>100</v>
       </c>
-      <c r="G14" s="198"/>
-      <c r="H14" s="198"/>
-      <c r="I14" s="198"/>
+      <c r="G14" s="204"/>
+      <c r="H14" s="204"/>
+      <c r="I14" s="204"/>
       <c r="J14" s="19"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
@@ -2192,18 +2212,18 @@
       <c r="AA14" s="7"/>
     </row>
     <row r="15" spans="2:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="197" t="s">
+      <c r="B15" s="203" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="198"/>
-      <c r="D15" s="198"/>
-      <c r="E15" s="199"/>
-      <c r="F15" s="197" t="s">
+      <c r="C15" s="204"/>
+      <c r="D15" s="204"/>
+      <c r="E15" s="205"/>
+      <c r="F15" s="203" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="198"/>
-      <c r="H15" s="198"/>
-      <c r="I15" s="198"/>
+      <c r="G15" s="204"/>
+      <c r="H15" s="204"/>
+      <c r="I15" s="204"/>
       <c r="J15" s="19"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
@@ -2250,18 +2270,18 @@
       <c r="AA16" s="7"/>
     </row>
     <row r="17" spans="2:30" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="209" t="s">
+      <c r="B17" s="212" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="210"/>
-      <c r="D17" s="210"/>
-      <c r="E17" s="211"/>
-      <c r="F17" s="209" t="s">
+      <c r="C17" s="213"/>
+      <c r="D17" s="213"/>
+      <c r="E17" s="214"/>
+      <c r="F17" s="212" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="210"/>
-      <c r="H17" s="210"/>
-      <c r="I17" s="210"/>
+      <c r="G17" s="213"/>
+      <c r="H17" s="213"/>
+      <c r="I17" s="213"/>
       <c r="J17" s="19"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
@@ -2279,18 +2299,18 @@
       <c r="AA17" s="7"/>
     </row>
     <row r="18" spans="2:30" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="212" t="s">
+      <c r="B18" s="215" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="213"/>
+      <c r="C18" s="216"/>
       <c r="D18" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="213" t="s">
+      <c r="E18" s="216" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="213"/>
-      <c r="G18" s="213"/>
+      <c r="F18" s="216"/>
+      <c r="G18" s="216"/>
       <c r="H18" s="20" t="s">
         <v>35</v>
       </c>
@@ -2314,18 +2334,18 @@
       <c r="AA18" s="7"/>
     </row>
     <row r="19" spans="2:30" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="214" t="s">
+      <c r="B19" s="217" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="215"/>
+      <c r="C19" s="218"/>
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="216" t="s">
+      <c r="E19" s="219" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="217"/>
-      <c r="G19" s="217"/>
+      <c r="F19" s="220"/>
+      <c r="G19" s="220"/>
       <c r="H19" s="187" t="s">
         <v>12</v>
       </c>
@@ -2815,18 +2835,18 @@
       <c r="AD35" s="7"/>
     </row>
     <row r="36" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="197" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="198"/>
-      <c r="D36" s="198"/>
-      <c r="E36" s="198"/>
-      <c r="F36" s="197" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="198"/>
-      <c r="H36" s="198"/>
-      <c r="I36" s="199"/>
+      <c r="B36" s="203" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="204"/>
+      <c r="D36" s="204"/>
+      <c r="E36" s="204"/>
+      <c r="F36" s="203" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="204"/>
+      <c r="H36" s="204"/>
+      <c r="I36" s="205"/>
       <c r="J36" s="13"/>
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
@@ -2911,33 +2931,33 @@
       <c r="AD38" s="7"/>
     </row>
     <row r="39" spans="1:30" s="27" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="204" t="s">
+      <c r="B39" s="221" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="205"/>
-      <c r="D39" s="205"/>
-      <c r="E39" s="205"/>
-      <c r="F39" s="204" t="s">
+      <c r="C39" s="222"/>
+      <c r="D39" s="222"/>
+      <c r="E39" s="222"/>
+      <c r="F39" s="221" t="s">
         <v>84</v>
       </c>
-      <c r="G39" s="205"/>
-      <c r="H39" s="205"/>
-      <c r="I39" s="206"/>
+      <c r="G39" s="222"/>
+      <c r="H39" s="222"/>
+      <c r="I39" s="223"/>
       <c r="J39" s="154"/>
     </row>
     <row r="40" spans="1:30" s="27" customFormat="1" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="207" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="208"/>
-      <c r="D40" s="208"/>
-      <c r="E40" s="208"/>
-      <c r="F40" s="197" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" s="198"/>
-      <c r="H40" s="198"/>
-      <c r="I40" s="199"/>
+      <c r="B40" s="209" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="210"/>
+      <c r="D40" s="210"/>
+      <c r="E40" s="210"/>
+      <c r="F40" s="203" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="204"/>
+      <c r="H40" s="204"/>
+      <c r="I40" s="205"/>
       <c r="J40" s="154"/>
     </row>
     <row r="41" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
@@ -2973,18 +2993,18 @@
       <c r="AD41" s="7"/>
     </row>
     <row r="42" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="197" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="198"/>
-      <c r="D42" s="198"/>
-      <c r="E42" s="198"/>
-      <c r="F42" s="197" t="s">
-        <v>17</v>
-      </c>
-      <c r="G42" s="198"/>
-      <c r="H42" s="198"/>
-      <c r="I42" s="199"/>
+      <c r="B42" s="203" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="204"/>
+      <c r="D42" s="204"/>
+      <c r="E42" s="204"/>
+      <c r="F42" s="203" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" s="204"/>
+      <c r="H42" s="204"/>
+      <c r="I42" s="205"/>
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:30" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
@@ -3030,18 +3050,18 @@
       <c r="J45" s="6"/>
     </row>
     <row r="46" spans="1:30" s="27" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="200" t="s">
+      <c r="B46" s="224" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="201"/>
-      <c r="D46" s="201"/>
-      <c r="E46" s="201"/>
-      <c r="F46" s="200" t="s">
+      <c r="C46" s="225"/>
+      <c r="D46" s="225"/>
+      <c r="E46" s="225"/>
+      <c r="F46" s="224" t="s">
         <v>101</v>
       </c>
-      <c r="G46" s="201"/>
-      <c r="H46" s="201"/>
-      <c r="I46" s="202"/>
+      <c r="G46" s="225"/>
+      <c r="H46" s="225"/>
+      <c r="I46" s="226"/>
       <c r="J46" s="26"/>
       <c r="N46" s="28"/>
       <c r="O46" s="28"/>
@@ -3062,93 +3082,93 @@
       <c r="AD46" s="28"/>
     </row>
     <row r="47" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="197" t="s">
+      <c r="B47" s="203" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="198"/>
-      <c r="D47" s="198"/>
-      <c r="E47" s="198"/>
-      <c r="F47" s="197" t="s">
+      <c r="C47" s="204"/>
+      <c r="D47" s="204"/>
+      <c r="E47" s="204"/>
+      <c r="F47" s="203" t="s">
         <v>102</v>
       </c>
-      <c r="G47" s="198"/>
-      <c r="H47" s="198"/>
-      <c r="I47" s="199"/>
+      <c r="G47" s="204"/>
+      <c r="H47" s="204"/>
+      <c r="I47" s="205"/>
       <c r="J47" s="16"/>
     </row>
     <row r="48" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="197" t="s">
+      <c r="B48" s="203" t="s">
         <v>104</v>
       </c>
-      <c r="C48" s="198"/>
-      <c r="D48" s="198"/>
-      <c r="E48" s="199"/>
-      <c r="F48" s="197" t="s">
+      <c r="C48" s="204"/>
+      <c r="D48" s="204"/>
+      <c r="E48" s="205"/>
+      <c r="F48" s="203" t="s">
         <v>103</v>
       </c>
-      <c r="G48" s="198"/>
-      <c r="H48" s="198"/>
-      <c r="I48" s="198"/>
+      <c r="G48" s="204"/>
+      <c r="H48" s="204"/>
+      <c r="I48" s="204"/>
       <c r="J48" s="16"/>
     </row>
     <row r="49" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="197" t="s">
+      <c r="B49" s="203" t="s">
         <v>105</v>
       </c>
-      <c r="C49" s="198"/>
-      <c r="D49" s="198"/>
-      <c r="E49" s="199"/>
-      <c r="F49" s="197" t="s">
+      <c r="C49" s="204"/>
+      <c r="D49" s="204"/>
+      <c r="E49" s="205"/>
+      <c r="F49" s="203" t="s">
         <v>106</v>
       </c>
-      <c r="G49" s="198"/>
-      <c r="H49" s="198"/>
-      <c r="I49" s="198"/>
+      <c r="G49" s="204"/>
+      <c r="H49" s="204"/>
+      <c r="I49" s="204"/>
       <c r="J49" s="16"/>
     </row>
     <row r="50" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="197" t="s">
+      <c r="B50" s="203" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="198"/>
-      <c r="D50" s="198"/>
-      <c r="E50" s="199"/>
-      <c r="F50" s="197" t="s">
+      <c r="C50" s="204"/>
+      <c r="D50" s="204"/>
+      <c r="E50" s="205"/>
+      <c r="F50" s="203" t="s">
         <v>107</v>
       </c>
-      <c r="G50" s="198"/>
-      <c r="H50" s="198"/>
-      <c r="I50" s="198"/>
+      <c r="G50" s="204"/>
+      <c r="H50" s="204"/>
+      <c r="I50" s="204"/>
       <c r="J50" s="16"/>
     </row>
     <row r="51" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="197" t="s">
+      <c r="B51" s="203" t="s">
         <v>108</v>
       </c>
-      <c r="C51" s="198"/>
-      <c r="D51" s="198"/>
-      <c r="E51" s="199"/>
-      <c r="F51" s="197" t="s">
+      <c r="C51" s="204"/>
+      <c r="D51" s="204"/>
+      <c r="E51" s="205"/>
+      <c r="F51" s="203" t="s">
         <v>109</v>
       </c>
-      <c r="G51" s="198"/>
-      <c r="H51" s="198"/>
-      <c r="I51" s="198"/>
+      <c r="G51" s="204"/>
+      <c r="H51" s="204"/>
+      <c r="I51" s="204"/>
       <c r="J51" s="16"/>
     </row>
     <row r="52" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="197" t="s">
+      <c r="B52" s="203" t="s">
         <v>110</v>
       </c>
-      <c r="C52" s="198"/>
-      <c r="D52" s="198"/>
-      <c r="E52" s="199"/>
-      <c r="F52" s="197" t="s">
+      <c r="C52" s="204"/>
+      <c r="D52" s="204"/>
+      <c r="E52" s="205"/>
+      <c r="F52" s="203" t="s">
         <v>111</v>
       </c>
-      <c r="G52" s="198"/>
-      <c r="H52" s="198"/>
-      <c r="I52" s="198"/>
+      <c r="G52" s="204"/>
+      <c r="H52" s="204"/>
+      <c r="I52" s="204"/>
       <c r="J52" s="16"/>
     </row>
     <row r="53" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3167,18 +3187,18 @@
       <c r="J53" s="16"/>
     </row>
     <row r="54" spans="2:30" s="27" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="200" t="s">
+      <c r="B54" s="224" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="201"/>
-      <c r="D54" s="201"/>
-      <c r="E54" s="202"/>
-      <c r="F54" s="200" t="s">
+      <c r="C54" s="225"/>
+      <c r="D54" s="225"/>
+      <c r="E54" s="226"/>
+      <c r="F54" s="224" t="s">
         <v>97</v>
       </c>
-      <c r="G54" s="203"/>
-      <c r="H54" s="203"/>
-      <c r="I54" s="203"/>
+      <c r="G54" s="227"/>
+      <c r="H54" s="227"/>
+      <c r="I54" s="227"/>
       <c r="J54" s="26"/>
       <c r="N54" s="28"/>
       <c r="O54" s="28"/>
@@ -3199,18 +3219,18 @@
       <c r="AD54" s="28"/>
     </row>
     <row r="55" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B55" s="197" t="s">
+      <c r="B55" s="203" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="198"/>
-      <c r="D55" s="198"/>
-      <c r="E55" s="199"/>
-      <c r="F55" s="197" t="s">
+      <c r="C55" s="204"/>
+      <c r="D55" s="204"/>
+      <c r="E55" s="205"/>
+      <c r="F55" s="203" t="s">
         <v>112</v>
       </c>
-      <c r="G55" s="198"/>
-      <c r="H55" s="198"/>
-      <c r="I55" s="198"/>
+      <c r="G55" s="204"/>
+      <c r="H55" s="204"/>
+      <c r="I55" s="204"/>
       <c r="J55" s="16"/>
     </row>
     <row r="56" spans="2:30" ht="1.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3270,18 +3290,18 @@
       <c r="J59" s="16"/>
     </row>
     <row r="60" spans="2:30" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B60" s="197" t="s">
+      <c r="B60" s="203" t="s">
         <v>105</v>
       </c>
-      <c r="C60" s="198"/>
-      <c r="D60" s="198"/>
-      <c r="E60" s="199"/>
-      <c r="F60" s="197" t="s">
+      <c r="C60" s="204"/>
+      <c r="D60" s="204"/>
+      <c r="E60" s="205"/>
+      <c r="F60" s="203" t="s">
         <v>105</v>
       </c>
-      <c r="G60" s="198"/>
-      <c r="H60" s="198"/>
-      <c r="I60" s="199"/>
+      <c r="G60" s="204"/>
+      <c r="H60" s="204"/>
+      <c r="I60" s="205"/>
       <c r="J60" s="16"/>
     </row>
     <row r="61" spans="2:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -3500,42 +3520,6 @@
     <row r="102" ht="43.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="F9:I10"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="F47:I47"/>
     <mergeCell ref="B48:E48"/>
     <mergeCell ref="F48:I48"/>
     <mergeCell ref="B60:E60"/>
@@ -3552,6 +3536,42 @@
     <mergeCell ref="F51:I51"/>
     <mergeCell ref="B52:E52"/>
     <mergeCell ref="F52:I52"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="F9:I10"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <conditionalFormatting sqref="D19:E31 J19:J31 E32:E33 B33">
     <cfRule type="notContainsBlanks" dxfId="3" priority="2">
@@ -3590,8 +3610,8 @@
   </sheetPr>
   <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>